<commit_message>
MEDS_SERD first version finalized
</commit_message>
<xml_diff>
--- a/analysis/MEDS_Tables.xlsx
+++ b/analysis/MEDS_Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27525"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="330" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A82BA9F-FBC3-441F-8899-A39896B91DFB}"/>
+  <xr:revisionPtr revIDLastSave="359" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E42C8A57-3149-41D6-9F08-0E4BF250E10B}"/>
   <bookViews>
-    <workbookView xWindow="-16005" yWindow="-21705" windowWidth="38625" windowHeight="21825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meds_tables" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2093" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2094" uniqueCount="549">
   <si>
     <t>Table</t>
   </si>
@@ -372,6 +372,7 @@
   </si>
   <si>
     <t>Does the field DATA_TYPE_INDEX refer to JOB_LOOKUPS?
+Relationship with FIELD_LOOKUP???????
 It seems that the key has multiple columns
 There is one record with a data_type_index in field_lookup that is not in job_lookups (99)</t>
   </si>
@@ -690,7 +691,7 @@
 It seems to contain two different kinds of data (definition &amp; display)
 Confirm key (not found), multiple keys
 Seems to have plenty of other foreign keys
-Many tables have columns as "data_require" and it is probably a boolean. Decide what to do with the modeland use of switches (implemented)</t>
+Many tables have columns as "data_require" and it is probably a boolean. Decide what to do with the model and use of switches (implemented)</t>
   </si>
   <si>
     <t>GEOLOGY_PARAM_DATA</t>
@@ -1695,13 +1696,22 @@
   </si>
   <si>
     <t>1180/1181</t>
+  </si>
+  <si>
+    <t>Retain for mapping, but no requirement to load</t>
+  </si>
+  <si>
+    <t>obsolescent</t>
+  </si>
+  <si>
+    <t>Not required</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2203,7 +2213,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2223,6 +2233,18 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2375,9 +2397,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2415,7 +2437,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2521,7 +2543,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2663,7 +2685,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2673,12 +2695,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W194"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W88" sqref="W88"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A87" sqref="A87:XFD90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" customWidth="1"/>
@@ -2691,7 +2713,7 @@
     <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="51.5703125" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="38.5703125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" style="7" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="10" style="7" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
@@ -2706,7 +2728,7 @@
     <col min="24" max="24" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2777,8 +2799,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
-      <c r="A2" t="s">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B2" t="s">
@@ -2831,7 +2853,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:23" hidden="1">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -2880,7 +2902,7 @@
       <c r="V3" s="7"/>
       <c r="W3"/>
     </row>
-    <row r="4" spans="1:23" hidden="1">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -2929,7 +2951,7 @@
       <c r="V4" s="7"/>
       <c r="W4"/>
     </row>
-    <row r="5" spans="1:23" hidden="1">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -2978,7 +3000,7 @@
       <c r="V5" s="7"/>
       <c r="W5"/>
     </row>
-    <row r="6" spans="1:23" hidden="1">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -3021,7 +3043,7 @@
       <c r="V6" s="7"/>
       <c r="W6"/>
     </row>
-    <row r="7" spans="1:23" hidden="1">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -3064,7 +3086,7 @@
       <c r="V7" s="7"/>
       <c r="W7"/>
     </row>
-    <row r="8" spans="1:23" hidden="1">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -3113,7 +3135,7 @@
       <c r="V8" s="7"/>
       <c r="W8"/>
     </row>
-    <row r="9" spans="1:23" hidden="1">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -3162,7 +3184,7 @@
       <c r="V9" s="7"/>
       <c r="W9"/>
     </row>
-    <row r="10" spans="1:23" hidden="1">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -3203,7 +3225,7 @@
       <c r="V10" s="7"/>
       <c r="W10"/>
     </row>
-    <row r="11" spans="1:23" hidden="1">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -3244,7 +3266,7 @@
       <c r="V11" s="7"/>
       <c r="W11"/>
     </row>
-    <row r="12" spans="1:23" hidden="1">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -3285,7 +3307,7 @@
       <c r="V12" s="7"/>
       <c r="W12"/>
     </row>
-    <row r="13" spans="1:23" hidden="1">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -3326,7 +3348,7 @@
       <c r="V13" s="7"/>
       <c r="W13"/>
     </row>
-    <row r="14" spans="1:23" hidden="1">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -3367,7 +3389,7 @@
       <c r="V14" s="7"/>
       <c r="W14"/>
     </row>
-    <row r="15" spans="1:23" hidden="1">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -3408,7 +3430,7 @@
       <c r="V15" s="7"/>
       <c r="W15"/>
     </row>
-    <row r="16" spans="1:23" hidden="1">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -3458,7 +3480,7 @@
       <c r="V16" s="7"/>
       <c r="W16"/>
     </row>
-    <row r="17" spans="1:23" hidden="1">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -3508,7 +3530,7 @@
       <c r="V17" s="7"/>
       <c r="W17"/>
     </row>
-    <row r="18" spans="1:23" hidden="1">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>74</v>
       </c>
@@ -3557,7 +3579,7 @@
       <c r="V18" s="7"/>
       <c r="W18"/>
     </row>
-    <row r="19" spans="1:23" hidden="1">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -3606,7 +3628,7 @@
       <c r="V19" s="7"/>
       <c r="W19"/>
     </row>
-    <row r="20" spans="1:23" hidden="1">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -3652,7 +3674,7 @@
       <c r="V20" s="7"/>
       <c r="W20"/>
     </row>
-    <row r="21" spans="1:23" hidden="1">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>84</v>
       </c>
@@ -3698,7 +3720,7 @@
       <c r="V21" s="7"/>
       <c r="W21"/>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>86</v>
       </c>
@@ -3716,7 +3738,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:23" hidden="1">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>90</v>
       </c>
@@ -3759,7 +3781,7 @@
       <c r="V23" s="7"/>
       <c r="W23"/>
     </row>
-    <row r="24" spans="1:23" ht="30">
+    <row r="24" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -3813,7 +3835,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>101</v>
       </c>
@@ -3867,61 +3889,66 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="60">
-      <c r="A26" t="s">
+    <row r="26" spans="1:23" s="11" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C26" t="s">
         <v>102</v>
       </c>
+      <c r="D26"/>
+      <c r="E26"/>
       <c r="F26" t="s">
         <v>107</v>
       </c>
       <c r="G26" t="s">
         <v>27</v>
       </c>
-      <c r="I26">
+      <c r="H26"/>
+      <c r="I26" s="11">
         <v>1173</v>
       </c>
+      <c r="J26"/>
+      <c r="K26"/>
       <c r="L26" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="M26" s="7" t="s">
+      <c r="M26" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="N26" s="7" t="s">
+      <c r="N26" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="O26" s="7" t="s">
+      <c r="O26" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="P26" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q26" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="R26" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="S26" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="T26" t="s">
+      <c r="P26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="R26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="S26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="T26" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="U26" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V26" s="7"/>
-      <c r="W26" s="2" t="s">
+      <c r="U26" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V26" s="12"/>
+      <c r="W26" s="13" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:23" hidden="1">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>110</v>
       </c>
@@ -3970,7 +3997,7 @@
       <c r="V27" s="7"/>
       <c r="W27"/>
     </row>
-    <row r="28" spans="1:23" hidden="1">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>114</v>
       </c>
@@ -4019,7 +4046,7 @@
       <c r="V28" s="7"/>
       <c r="W28"/>
     </row>
-    <row r="29" spans="1:23" hidden="1">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>116</v>
       </c>
@@ -4067,7 +4094,7 @@
       <c r="V29" s="7"/>
       <c r="W29"/>
     </row>
-    <row r="30" spans="1:23" hidden="1">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>120</v>
       </c>
@@ -4115,7 +4142,7 @@
       <c r="V30" s="7"/>
       <c r="W30"/>
     </row>
-    <row r="31" spans="1:23" hidden="1">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>122</v>
       </c>
@@ -4163,7 +4190,7 @@
       <c r="V31" s="7"/>
       <c r="W31"/>
     </row>
-    <row r="32" spans="1:23" hidden="1">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>124</v>
       </c>
@@ -4201,7 +4228,7 @@
       <c r="V32" s="7"/>
       <c r="W32"/>
     </row>
-    <row r="33" spans="1:23" hidden="1">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>126</v>
       </c>
@@ -4247,7 +4274,7 @@
       <c r="V33" s="7"/>
       <c r="W33"/>
     </row>
-    <row r="34" spans="1:23" hidden="1">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>130</v>
       </c>
@@ -4293,7 +4320,7 @@
       <c r="V34" s="7"/>
       <c r="W34"/>
     </row>
-    <row r="35" spans="1:23" hidden="1">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>132</v>
       </c>
@@ -4339,7 +4366,7 @@
       <c r="V35" s="7"/>
       <c r="W35"/>
     </row>
-    <row r="36" spans="1:23" hidden="1">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>136</v>
       </c>
@@ -4385,7 +4412,7 @@
       <c r="V36" s="7"/>
       <c r="W36"/>
     </row>
-    <row r="37" spans="1:23" hidden="1">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>138</v>
       </c>
@@ -4431,7 +4458,7 @@
       <c r="V37" s="7"/>
       <c r="W37"/>
     </row>
-    <row r="38" spans="1:23" hidden="1">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>140</v>
       </c>
@@ -4477,7 +4504,7 @@
       <c r="V38" s="7"/>
       <c r="W38"/>
     </row>
-    <row r="39" spans="1:23" hidden="1">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>144</v>
       </c>
@@ -4523,7 +4550,7 @@
       <c r="V39" s="7"/>
       <c r="W39"/>
     </row>
-    <row r="40" spans="1:23" hidden="1">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>146</v>
       </c>
@@ -4569,7 +4596,7 @@
       <c r="V40" s="7"/>
       <c r="W40"/>
     </row>
-    <row r="41" spans="1:23">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>148</v>
       </c>
@@ -4587,7 +4614,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:23">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>150</v>
       </c>
@@ -4605,7 +4632,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:23">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>151</v>
       </c>
@@ -4659,7 +4686,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="30">
+    <row r="44" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>156</v>
       </c>
@@ -4713,7 +4740,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="45" spans="1:23" ht="75">
+    <row r="45" spans="1:23" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>161</v>
       </c>
@@ -4767,61 +4794,66 @@
         <v>164</v>
       </c>
     </row>
-    <row r="46" spans="1:23" ht="45">
-      <c r="A46" t="s">
+    <row r="46" spans="1:23" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C46" t="s">
         <v>95</v>
       </c>
+      <c r="D46"/>
+      <c r="E46"/>
       <c r="F46" t="s">
         <v>166</v>
       </c>
       <c r="G46" t="s">
         <v>27</v>
       </c>
-      <c r="I46">
+      <c r="H46"/>
+      <c r="I46" s="11">
         <v>1422</v>
       </c>
+      <c r="J46"/>
+      <c r="K46"/>
       <c r="L46" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="M46" s="7" t="s">
+      <c r="M46" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="N46" s="7" t="s">
+      <c r="N46" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="O46" s="7" t="s">
+      <c r="O46" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="P46" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q46" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="R46" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="S46" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="T46" t="s">
+      <c r="P46" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q46" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="R46" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="S46" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="T46" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="U46" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V46" s="7"/>
-      <c r="W46" s="2" t="s">
+      <c r="U46" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V46" s="12"/>
+      <c r="W46" s="13" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="47" spans="1:23" hidden="1">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>169</v>
       </c>
@@ -4867,7 +4899,7 @@
       <c r="V47" s="7"/>
       <c r="W47"/>
     </row>
-    <row r="48" spans="1:23" hidden="1">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>173</v>
       </c>
@@ -4913,7 +4945,7 @@
       <c r="V48" s="7"/>
       <c r="W48"/>
     </row>
-    <row r="49" spans="1:23" hidden="1">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>175</v>
       </c>
@@ -4959,7 +4991,7 @@
       <c r="V49" s="7"/>
       <c r="W49"/>
     </row>
-    <row r="50" spans="1:23" hidden="1">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>179</v>
       </c>
@@ -5005,7 +5037,7 @@
       <c r="V50" s="7"/>
       <c r="W50"/>
     </row>
-    <row r="51" spans="1:23" hidden="1">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>181</v>
       </c>
@@ -5051,7 +5083,7 @@
       <c r="V51" s="7"/>
       <c r="W51"/>
     </row>
-    <row r="52" spans="1:23" hidden="1">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>183</v>
       </c>
@@ -5103,7 +5135,7 @@
       <c r="V52" s="7"/>
       <c r="W52"/>
     </row>
-    <row r="53" spans="1:23" hidden="1">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>188</v>
       </c>
@@ -5155,7 +5187,7 @@
       <c r="V53" s="7"/>
       <c r="W53"/>
     </row>
-    <row r="54" spans="1:23" hidden="1">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>190</v>
       </c>
@@ -5207,7 +5239,7 @@
       <c r="V54" s="7"/>
       <c r="W54"/>
     </row>
-    <row r="55" spans="1:23" hidden="1">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>193</v>
       </c>
@@ -5253,7 +5285,7 @@
       <c r="V55" s="7"/>
       <c r="W55"/>
     </row>
-    <row r="56" spans="1:23" hidden="1">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>197</v>
       </c>
@@ -5299,7 +5331,7 @@
       <c r="V56" s="7"/>
       <c r="W56"/>
     </row>
-    <row r="57" spans="1:23" hidden="1">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>199</v>
       </c>
@@ -5345,7 +5377,7 @@
       <c r="V57" s="7"/>
       <c r="W57"/>
     </row>
-    <row r="58" spans="1:23" hidden="1">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>201</v>
       </c>
@@ -5391,7 +5423,7 @@
       <c r="V58" s="7"/>
       <c r="W58"/>
     </row>
-    <row r="59" spans="1:23" hidden="1">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>205</v>
       </c>
@@ -5437,61 +5469,65 @@
       <c r="V59" s="7"/>
       <c r="W59"/>
     </row>
-    <row r="60" spans="1:23" ht="120">
-      <c r="A60" t="s">
+    <row r="60" spans="1:23" s="14" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C60" t="s">
         <v>208</v>
       </c>
+      <c r="D60"/>
+      <c r="E60"/>
       <c r="F60" t="s">
         <v>209</v>
       </c>
       <c r="G60" t="s">
         <v>27</v>
       </c>
-      <c r="I60">
+      <c r="H60"/>
+      <c r="I60" s="14">
         <v>178</v>
       </c>
+      <c r="J60"/>
+      <c r="K60"/>
       <c r="L60" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="M60" s="7" t="s">
+      <c r="M60" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="N60" s="7" t="s">
+      <c r="N60" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="O60" s="7" t="s">
+      <c r="O60" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="P60" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q60" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="R60" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="S60" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="T60" t="s">
+      <c r="P60" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q60" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="R60" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="S60" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="T60" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="U60" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V60" s="7"/>
-      <c r="W60" s="2" t="s">
+      <c r="U60" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="W60" s="14" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="61" spans="1:23" hidden="1">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>212</v>
       </c>
@@ -5537,7 +5573,7 @@
       <c r="V61" s="7"/>
       <c r="W61"/>
     </row>
-    <row r="62" spans="1:23" hidden="1">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>216</v>
       </c>
@@ -5583,7 +5619,7 @@
       <c r="V62" s="7"/>
       <c r="W62"/>
     </row>
-    <row r="63" spans="1:23" hidden="1">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>218</v>
       </c>
@@ -5629,7 +5665,7 @@
       <c r="V63" s="7"/>
       <c r="W63"/>
     </row>
-    <row r="64" spans="1:23" hidden="1">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>222</v>
       </c>
@@ -5675,7 +5711,7 @@
       <c r="V64" s="7"/>
       <c r="W64"/>
     </row>
-    <row r="65" spans="1:23" hidden="1">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>223</v>
       </c>
@@ -5724,7 +5760,7 @@
       <c r="V65" s="7"/>
       <c r="W65"/>
     </row>
-    <row r="66" spans="1:23" hidden="1">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>227</v>
       </c>
@@ -5773,7 +5809,7 @@
       <c r="V66" s="7"/>
       <c r="W66"/>
     </row>
-    <row r="67" spans="1:23" hidden="1">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>229</v>
       </c>
@@ -5810,7 +5846,7 @@
       <c r="V67" s="7"/>
       <c r="W67"/>
     </row>
-    <row r="68" spans="1:23" hidden="1">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>231</v>
       </c>
@@ -5856,7 +5892,7 @@
       <c r="V68" s="7"/>
       <c r="W68"/>
     </row>
-    <row r="69" spans="1:23" hidden="1">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>235</v>
       </c>
@@ -5902,7 +5938,7 @@
       <c r="V69" s="7"/>
       <c r="W69"/>
     </row>
-    <row r="70" spans="1:23" hidden="1">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>237</v>
       </c>
@@ -5948,7 +5984,7 @@
       <c r="V70" s="7"/>
       <c r="W70"/>
     </row>
-    <row r="71" spans="1:23" hidden="1">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>239</v>
       </c>
@@ -5986,7 +6022,7 @@
       <c r="V71" s="7"/>
       <c r="W71"/>
     </row>
-    <row r="72" spans="1:23" hidden="1">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>241</v>
       </c>
@@ -6023,7 +6059,7 @@
       <c r="V72" s="7"/>
       <c r="W72"/>
     </row>
-    <row r="73" spans="1:23" hidden="1">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>243</v>
       </c>
@@ -6060,7 +6096,7 @@
       <c r="V73" s="7"/>
       <c r="W73"/>
     </row>
-    <row r="74" spans="1:23" hidden="1">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>244</v>
       </c>
@@ -6106,7 +6142,7 @@
       <c r="V74" s="7"/>
       <c r="W74"/>
     </row>
-    <row r="75" spans="1:23" hidden="1">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>248</v>
       </c>
@@ -6152,7 +6188,7 @@
       <c r="V75" s="7"/>
       <c r="W75"/>
     </row>
-    <row r="76" spans="1:23" hidden="1">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>250</v>
       </c>
@@ -6198,7 +6234,7 @@
       <c r="V76" s="7"/>
       <c r="W76"/>
     </row>
-    <row r="77" spans="1:23" hidden="1">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>253</v>
       </c>
@@ -6244,7 +6280,7 @@
       <c r="V77" s="7"/>
       <c r="W77"/>
     </row>
-    <row r="78" spans="1:23" hidden="1">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>255</v>
       </c>
@@ -6290,7 +6326,7 @@
       <c r="V78" s="7"/>
       <c r="W78"/>
     </row>
-    <row r="79" spans="1:23">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>257</v>
       </c>
@@ -6344,7 +6380,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="80" spans="1:23" hidden="1">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>262</v>
       </c>
@@ -6387,7 +6423,7 @@
       <c r="V80" s="7"/>
       <c r="W80"/>
     </row>
-    <row r="81" spans="1:23" hidden="1">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>267</v>
       </c>
@@ -6430,7 +6466,7 @@
       <c r="V81" s="7"/>
       <c r="W81"/>
     </row>
-    <row r="82" spans="1:23" hidden="1">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>270</v>
       </c>
@@ -6467,7 +6503,7 @@
       <c r="V82" s="7"/>
       <c r="W82"/>
     </row>
-    <row r="83" spans="1:23">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>275</v>
       </c>
@@ -6521,59 +6557,66 @@
         <v>155</v>
       </c>
     </row>
-    <row r="84" spans="1:23" hidden="1">
-      <c r="A84" t="s">
+    <row r="84" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="B84" t="s">
-        <v>37</v>
+      <c r="B84" s="9" t="s">
+        <v>548</v>
       </c>
       <c r="C84" t="s">
         <v>276</v>
       </c>
+      <c r="D84"/>
+      <c r="E84"/>
       <c r="F84" t="s">
         <v>280</v>
       </c>
       <c r="G84" t="s">
         <v>27</v>
       </c>
-      <c r="I84">
+      <c r="H84"/>
+      <c r="I84" s="9">
         <v>16</v>
       </c>
+      <c r="J84"/>
+      <c r="K84"/>
       <c r="L84" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="M84" s="7" t="s">
+      <c r="M84" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="N84" s="7" t="s">
+      <c r="N84" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="O84" s="7" t="s">
+      <c r="O84" s="10" t="s">
         <v>281</v>
       </c>
-      <c r="P84" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q84" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="R84" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="S84" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="T84" t="s">
+      <c r="P84" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q84" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R84" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="S84" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="T84" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="U84" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V84" s="7"/>
-      <c r="W84"/>
-    </row>
-    <row r="85" spans="1:23" hidden="1">
+      <c r="U84" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="V84" s="10"/>
+      <c r="W84" s="9" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>282</v>
       </c>
@@ -6625,7 +6668,7 @@
       <c r="V85" s="7"/>
       <c r="W85"/>
     </row>
-    <row r="86" spans="1:23" ht="15" customHeight="1">
+    <row r="86" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>285</v>
       </c>
@@ -6676,124 +6719,170 @@
         <v>155</v>
       </c>
     </row>
-    <row r="87" spans="1:23">
-      <c r="A87" t="s">
+    <row r="87" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C87" t="s">
         <v>291</v>
       </c>
+      <c r="D87"/>
+      <c r="E87"/>
       <c r="F87" t="s">
         <v>292</v>
       </c>
       <c r="G87" t="s">
         <v>27</v>
       </c>
+      <c r="H87"/>
       <c r="J87" t="s">
         <v>293</v>
       </c>
       <c r="K87" t="s">
         <v>289</v>
       </c>
-      <c r="U87" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V87" s="7"/>
-      <c r="W87" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="88" spans="1:23">
-      <c r="A88" t="s">
+      <c r="L87" s="7"/>
+      <c r="M87" s="12"/>
+      <c r="N87" s="12"/>
+      <c r="O87" s="12"/>
+      <c r="P87" s="12"/>
+      <c r="Q87" s="12"/>
+      <c r="R87" s="12"/>
+      <c r="S87" s="12"/>
+      <c r="U87" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V87" s="12"/>
+      <c r="W87" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="88" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="11" t="s">
         <v>294</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C88" t="s">
         <v>295</v>
       </c>
+      <c r="D88"/>
+      <c r="E88"/>
       <c r="F88" t="s">
         <v>296</v>
       </c>
       <c r="G88" t="s">
         <v>27</v>
       </c>
+      <c r="H88"/>
       <c r="J88" t="s">
         <v>297</v>
       </c>
       <c r="K88" t="s">
         <v>289</v>
       </c>
-      <c r="U88" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V88" s="7"/>
-      <c r="W88" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="89" spans="1:23">
-      <c r="A89" t="s">
+      <c r="L88" s="7"/>
+      <c r="M88" s="12"/>
+      <c r="N88" s="12"/>
+      <c r="O88" s="12"/>
+      <c r="P88" s="12"/>
+      <c r="Q88" s="12"/>
+      <c r="R88" s="12"/>
+      <c r="S88" s="12"/>
+      <c r="U88" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V88" s="12"/>
+      <c r="W88" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="89" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C89" t="s">
         <v>299</v>
       </c>
+      <c r="D89"/>
+      <c r="E89"/>
       <c r="F89" t="s">
         <v>300</v>
       </c>
       <c r="G89" t="s">
         <v>27</v>
       </c>
+      <c r="H89"/>
       <c r="J89" t="s">
         <v>301</v>
       </c>
       <c r="K89" t="s">
         <v>289</v>
       </c>
-      <c r="U89" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V89" s="7"/>
-      <c r="W89" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="90" spans="1:23">
-      <c r="A90" t="s">
+      <c r="L89" s="7"/>
+      <c r="M89" s="12"/>
+      <c r="N89" s="12"/>
+      <c r="O89" s="12"/>
+      <c r="P89" s="12"/>
+      <c r="Q89" s="12"/>
+      <c r="R89" s="12"/>
+      <c r="S89" s="12"/>
+      <c r="U89" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V89" s="12"/>
+      <c r="W89" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="90" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C90" t="s">
         <v>303</v>
       </c>
+      <c r="D90"/>
+      <c r="E90"/>
       <c r="F90" t="s">
         <v>304</v>
       </c>
       <c r="G90" t="s">
         <v>27</v>
       </c>
-      <c r="I90">
+      <c r="H90"/>
+      <c r="I90" s="11">
         <v>1681</v>
       </c>
-      <c r="U90" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V90" s="7"/>
-      <c r="W90" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="91" spans="1:23" hidden="1">
+      <c r="J90"/>
+      <c r="K90"/>
+      <c r="L90" s="7"/>
+      <c r="M90" s="12"/>
+      <c r="N90" s="12"/>
+      <c r="O90" s="12"/>
+      <c r="P90" s="12"/>
+      <c r="Q90" s="12"/>
+      <c r="R90" s="12"/>
+      <c r="S90" s="12"/>
+      <c r="U90" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V90" s="12"/>
+      <c r="W90" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>305</v>
       </c>
@@ -6836,7 +6925,7 @@
       <c r="V91" s="7"/>
       <c r="W91"/>
     </row>
-    <row r="92" spans="1:23" hidden="1">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>308</v>
       </c>
@@ -6879,7 +6968,7 @@
       <c r="V92" s="7"/>
       <c r="W92"/>
     </row>
-    <row r="93" spans="1:23" hidden="1">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>311</v>
       </c>
@@ -6913,7 +7002,7 @@
       <c r="V93" s="7"/>
       <c r="W93"/>
     </row>
-    <row r="94" spans="1:23" hidden="1">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>312</v>
       </c>
@@ -6956,7 +7045,7 @@
       <c r="V94" s="7"/>
       <c r="W94"/>
     </row>
-    <row r="95" spans="1:23" hidden="1">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>315</v>
       </c>
@@ -7008,7 +7097,7 @@
       <c r="V95" s="7"/>
       <c r="W95"/>
     </row>
-    <row r="96" spans="1:23" hidden="1">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>319</v>
       </c>
@@ -7039,7 +7128,7 @@
       <c r="V96" s="7"/>
       <c r="W96"/>
     </row>
-    <row r="97" spans="1:23" hidden="1">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>322</v>
       </c>
@@ -7088,7 +7177,7 @@
       <c r="V97" s="7"/>
       <c r="W97"/>
     </row>
-    <row r="98" spans="1:23" hidden="1">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>326</v>
       </c>
@@ -7137,7 +7226,7 @@
       <c r="V98" s="7"/>
       <c r="W98"/>
     </row>
-    <row r="99" spans="1:23" hidden="1">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>328</v>
       </c>
@@ -7186,7 +7275,7 @@
       <c r="V99" s="7"/>
       <c r="W99"/>
     </row>
-    <row r="100" spans="1:23" hidden="1">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>332</v>
       </c>
@@ -7235,7 +7324,7 @@
       <c r="V100" s="7"/>
       <c r="W100"/>
     </row>
-    <row r="101" spans="1:23" hidden="1">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>334</v>
       </c>
@@ -7284,7 +7373,7 @@
       <c r="V101" s="7"/>
       <c r="W101"/>
     </row>
-    <row r="102" spans="1:23" hidden="1">
+    <row r="102" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>336</v>
       </c>
@@ -7333,49 +7422,57 @@
       <c r="V102" s="7"/>
       <c r="W102"/>
     </row>
-    <row r="103" spans="1:23">
-      <c r="A103" t="s">
+    <row r="103" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="11" t="s">
         <v>338</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C103" t="s">
         <v>339</v>
       </c>
+      <c r="D103"/>
+      <c r="E103"/>
+      <c r="F103"/>
+      <c r="G103"/>
       <c r="H103" t="s">
         <v>340</v>
       </c>
+      <c r="J103"/>
+      <c r="K103"/>
       <c r="L103" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="M103" s="7" t="s">
+      <c r="M103" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="P103" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q103" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="R103" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="S103" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="T103" t="s">
+      <c r="N103" s="12"/>
+      <c r="O103" s="12"/>
+      <c r="P103" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q103" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="R103" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="S103" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="T103" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="U103" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V103" s="7"/>
-      <c r="W103" t="s">
+      <c r="U103" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V103" s="12"/>
+      <c r="W103" s="11" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="104" spans="1:23">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>341</v>
       </c>
@@ -7417,7 +7514,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="105" spans="1:23" hidden="1">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>342</v>
       </c>
@@ -7466,7 +7563,7 @@
       <c r="V105" s="7"/>
       <c r="W105"/>
     </row>
-    <row r="106" spans="1:23" hidden="1">
+    <row r="106" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>346</v>
       </c>
@@ -7515,7 +7612,7 @@
       <c r="V106" s="7"/>
       <c r="W106"/>
     </row>
-    <row r="107" spans="1:23" hidden="1">
+    <row r="107" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>348</v>
       </c>
@@ -7564,7 +7661,7 @@
       <c r="V107" s="7"/>
       <c r="W107"/>
     </row>
-    <row r="108" spans="1:23" hidden="1">
+    <row r="108" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>352</v>
       </c>
@@ -7613,7 +7710,7 @@
       <c r="V108" s="7"/>
       <c r="W108"/>
     </row>
-    <row r="109" spans="1:23" hidden="1">
+    <row r="109" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>354</v>
       </c>
@@ -7662,7 +7759,7 @@
       <c r="V109" s="7"/>
       <c r="W109"/>
     </row>
-    <row r="110" spans="1:23" hidden="1">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>358</v>
       </c>
@@ -7711,7 +7808,7 @@
       <c r="V110" s="7"/>
       <c r="W110"/>
     </row>
-    <row r="111" spans="1:23" hidden="1">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>360</v>
       </c>
@@ -7760,7 +7857,7 @@
       <c r="V111" s="7"/>
       <c r="W111"/>
     </row>
-    <row r="112" spans="1:23" hidden="1">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>364</v>
       </c>
@@ -7809,7 +7906,7 @@
       <c r="V112" s="7"/>
       <c r="W112"/>
     </row>
-    <row r="113" spans="1:23" hidden="1">
+    <row r="113" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>366</v>
       </c>
@@ -7858,7 +7955,7 @@
       <c r="V113" s="7"/>
       <c r="W113"/>
     </row>
-    <row r="114" spans="1:23" hidden="1">
+    <row r="114" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>370</v>
       </c>
@@ -7907,7 +8004,7 @@
       <c r="V114" s="7"/>
       <c r="W114"/>
     </row>
-    <row r="115" spans="1:23" hidden="1">
+    <row r="115" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>372</v>
       </c>
@@ -7957,7 +8054,7 @@
       <c r="V115" s="7"/>
       <c r="W115"/>
     </row>
-    <row r="116" spans="1:23" hidden="1">
+    <row r="116" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>376</v>
       </c>
@@ -8007,7 +8104,7 @@
       <c r="V116" s="7"/>
       <c r="W116"/>
     </row>
-    <row r="117" spans="1:23" hidden="1">
+    <row r="117" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>378</v>
       </c>
@@ -8056,7 +8153,7 @@
       <c r="V117" s="7"/>
       <c r="W117"/>
     </row>
-    <row r="118" spans="1:23" hidden="1">
+    <row r="118" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>382</v>
       </c>
@@ -8105,7 +8202,7 @@
       <c r="V118" s="7"/>
       <c r="W118"/>
     </row>
-    <row r="119" spans="1:23" hidden="1">
+    <row r="119" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>384</v>
       </c>
@@ -8139,7 +8236,7 @@
       <c r="V119" s="7"/>
       <c r="W119"/>
     </row>
-    <row r="120" spans="1:23" hidden="1">
+    <row r="120" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>387</v>
       </c>
@@ -8173,7 +8270,7 @@
       <c r="V120" s="7"/>
       <c r="W120"/>
     </row>
-    <row r="121" spans="1:23" hidden="1">
+    <row r="121" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>388</v>
       </c>
@@ -8219,7 +8316,7 @@
       <c r="V121" s="7"/>
       <c r="W121"/>
     </row>
-    <row r="122" spans="1:23">
+    <row r="122" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>390</v>
       </c>
@@ -8264,7 +8361,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="123" spans="1:23" hidden="1">
+    <row r="123" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>393</v>
       </c>
@@ -8314,7 +8411,7 @@
       <c r="V123" s="7"/>
       <c r="W123"/>
     </row>
-    <row r="124" spans="1:23" hidden="1">
+    <row r="124" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>397</v>
       </c>
@@ -8364,7 +8461,7 @@
       <c r="V124" s="7"/>
       <c r="W124"/>
     </row>
-    <row r="125" spans="1:23" hidden="1">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>399</v>
       </c>
@@ -8416,7 +8513,7 @@
       <c r="V125" s="7"/>
       <c r="W125"/>
     </row>
-    <row r="126" spans="1:23" hidden="1">
+    <row r="126" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>404</v>
       </c>
@@ -8468,7 +8565,7 @@
       <c r="V126" s="7"/>
       <c r="W126"/>
     </row>
-    <row r="127" spans="1:23" hidden="1">
+    <row r="127" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>407</v>
       </c>
@@ -8520,7 +8617,7 @@
       <c r="V127" s="7"/>
       <c r="W127"/>
     </row>
-    <row r="128" spans="1:23" hidden="1">
+    <row r="128" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>410</v>
       </c>
@@ -8572,7 +8669,7 @@
       <c r="V128" s="7"/>
       <c r="W128"/>
     </row>
-    <row r="129" spans="1:23" hidden="1">
+    <row r="129" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>412</v>
       </c>
@@ -8624,7 +8721,7 @@
       <c r="V129" s="7"/>
       <c r="W129"/>
     </row>
-    <row r="130" spans="1:23" hidden="1">
+    <row r="130" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>414</v>
       </c>
@@ -8676,7 +8773,7 @@
       <c r="V130" s="7"/>
       <c r="W130"/>
     </row>
-    <row r="131" spans="1:23" hidden="1">
+    <row r="131" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>416</v>
       </c>
@@ -8728,7 +8825,7 @@
       <c r="V131" s="7"/>
       <c r="W131"/>
     </row>
-    <row r="132" spans="1:23" hidden="1">
+    <row r="132" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>418</v>
       </c>
@@ -8780,7 +8877,7 @@
       <c r="V132" s="7"/>
       <c r="W132"/>
     </row>
-    <row r="133" spans="1:23" hidden="1">
+    <row r="133" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>420</v>
       </c>
@@ -8832,7 +8929,7 @@
       <c r="V133" s="7"/>
       <c r="W133"/>
     </row>
-    <row r="134" spans="1:23" hidden="1">
+    <row r="134" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>422</v>
       </c>
@@ -8869,596 +8966,1032 @@
       <c r="V134" s="7"/>
       <c r="W134"/>
     </row>
-    <row r="135" spans="1:23">
-      <c r="A135" t="s">
+    <row r="135" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="11" t="s">
         <v>424</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B135" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C135" t="s">
         <v>425</v>
       </c>
+      <c r="D135"/>
+      <c r="E135"/>
       <c r="F135" t="s">
         <v>426</v>
       </c>
       <c r="G135" t="s">
         <v>27</v>
       </c>
-      <c r="I135">
+      <c r="H135"/>
+      <c r="I135" s="11">
         <v>4686</v>
       </c>
-      <c r="U135" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V135" s="7"/>
-      <c r="W135" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="136" spans="1:23">
-      <c r="A136" t="s">
+      <c r="J135"/>
+      <c r="K135"/>
+      <c r="L135" s="7"/>
+      <c r="M135" s="12"/>
+      <c r="N135" s="12"/>
+      <c r="O135" s="12"/>
+      <c r="P135" s="12"/>
+      <c r="Q135" s="12"/>
+      <c r="R135" s="12"/>
+      <c r="S135" s="12"/>
+      <c r="U135" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V135" s="12"/>
+      <c r="W135" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="136" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="11" t="s">
         <v>427</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B136" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C136" t="s">
         <v>428</v>
       </c>
+      <c r="D136"/>
+      <c r="E136"/>
       <c r="F136" t="s">
         <v>429</v>
       </c>
       <c r="G136" t="s">
         <v>27</v>
       </c>
+      <c r="H136"/>
       <c r="J136" t="s">
         <v>430</v>
       </c>
       <c r="K136" t="s">
         <v>289</v>
       </c>
-      <c r="U136" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V136" s="7"/>
-      <c r="W136" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="137" spans="1:23">
-      <c r="A137" t="s">
+      <c r="L136" s="7"/>
+      <c r="M136" s="12"/>
+      <c r="N136" s="12"/>
+      <c r="O136" s="12"/>
+      <c r="P136" s="12"/>
+      <c r="Q136" s="12"/>
+      <c r="R136" s="12"/>
+      <c r="S136" s="12"/>
+      <c r="U136" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V136" s="12"/>
+      <c r="W136" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="137" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="11" t="s">
         <v>431</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B137" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C137" t="s">
         <v>432</v>
       </c>
-      <c r="U137" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V137" s="7"/>
-      <c r="W137" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="138" spans="1:23">
-      <c r="A138" t="s">
+      <c r="D137"/>
+      <c r="E137"/>
+      <c r="F137"/>
+      <c r="G137"/>
+      <c r="H137"/>
+      <c r="J137"/>
+      <c r="K137"/>
+      <c r="L137" s="7"/>
+      <c r="M137" s="12"/>
+      <c r="N137" s="12"/>
+      <c r="O137" s="12"/>
+      <c r="P137" s="12"/>
+      <c r="Q137" s="12"/>
+      <c r="R137" s="12"/>
+      <c r="S137" s="12"/>
+      <c r="U137" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V137" s="12"/>
+      <c r="W137" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="138" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="11" t="s">
         <v>433</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B138" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C138" t="s">
         <v>432</v>
       </c>
-      <c r="U138" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V138" s="7"/>
-      <c r="W138" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="139" spans="1:23">
-      <c r="A139" t="s">
+      <c r="D138"/>
+      <c r="E138"/>
+      <c r="F138"/>
+      <c r="G138"/>
+      <c r="H138"/>
+      <c r="J138"/>
+      <c r="K138"/>
+      <c r="L138" s="7"/>
+      <c r="M138" s="12"/>
+      <c r="N138" s="12"/>
+      <c r="O138" s="12"/>
+      <c r="P138" s="12"/>
+      <c r="Q138" s="12"/>
+      <c r="R138" s="12"/>
+      <c r="S138" s="12"/>
+      <c r="U138" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V138" s="12"/>
+      <c r="W138" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="139" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="11" t="s">
         <v>434</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B139" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C139" t="s">
         <v>432</v>
       </c>
-      <c r="U139" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V139" s="7"/>
-      <c r="W139" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="140" spans="1:23">
-      <c r="A140" t="s">
+      <c r="D139"/>
+      <c r="E139"/>
+      <c r="F139"/>
+      <c r="G139"/>
+      <c r="H139"/>
+      <c r="J139"/>
+      <c r="K139"/>
+      <c r="L139" s="7"/>
+      <c r="M139" s="12"/>
+      <c r="N139" s="12"/>
+      <c r="O139" s="12"/>
+      <c r="P139" s="12"/>
+      <c r="Q139" s="12"/>
+      <c r="R139" s="12"/>
+      <c r="S139" s="12"/>
+      <c r="U139" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V139" s="12"/>
+      <c r="W139" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="140" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="11" t="s">
         <v>435</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C140" t="s">
         <v>432</v>
       </c>
-      <c r="U140" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V140" s="7"/>
-      <c r="W140" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="141" spans="1:23">
-      <c r="A141" t="s">
+      <c r="D140"/>
+      <c r="E140"/>
+      <c r="F140"/>
+      <c r="G140"/>
+      <c r="H140"/>
+      <c r="J140"/>
+      <c r="K140"/>
+      <c r="L140" s="7"/>
+      <c r="M140" s="12"/>
+      <c r="N140" s="12"/>
+      <c r="O140" s="12"/>
+      <c r="P140" s="12"/>
+      <c r="Q140" s="12"/>
+      <c r="R140" s="12"/>
+      <c r="S140" s="12"/>
+      <c r="U140" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V140" s="12"/>
+      <c r="W140" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="141" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="11" t="s">
         <v>436</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B141" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C141" t="s">
         <v>437</v>
       </c>
+      <c r="D141"/>
+      <c r="E141"/>
       <c r="F141" t="s">
         <v>438</v>
       </c>
       <c r="G141" t="s">
         <v>27</v>
       </c>
+      <c r="H141"/>
       <c r="J141" t="s">
         <v>439</v>
       </c>
       <c r="K141" t="s">
         <v>289</v>
       </c>
-      <c r="U141" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V141" s="7"/>
-      <c r="W141" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="142" spans="1:23">
-      <c r="A142" t="s">
+      <c r="L141" s="7"/>
+      <c r="M141" s="12"/>
+      <c r="N141" s="12"/>
+      <c r="O141" s="12"/>
+      <c r="P141" s="12"/>
+      <c r="Q141" s="12"/>
+      <c r="R141" s="12"/>
+      <c r="S141" s="12"/>
+      <c r="U141" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V141" s="12"/>
+      <c r="W141" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="142" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="11" t="s">
         <v>440</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B142" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C142" t="s">
         <v>432</v>
       </c>
-      <c r="U142" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V142" s="7"/>
-      <c r="W142" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="143" spans="1:23">
-      <c r="A143" t="s">
+      <c r="D142"/>
+      <c r="E142"/>
+      <c r="F142"/>
+      <c r="G142"/>
+      <c r="H142"/>
+      <c r="J142"/>
+      <c r="K142"/>
+      <c r="L142" s="7"/>
+      <c r="M142" s="12"/>
+      <c r="N142" s="12"/>
+      <c r="O142" s="12"/>
+      <c r="P142" s="12"/>
+      <c r="Q142" s="12"/>
+      <c r="R142" s="12"/>
+      <c r="S142" s="12"/>
+      <c r="U142" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V142" s="12"/>
+      <c r="W142" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="143" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="11" t="s">
         <v>441</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B143" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C143" t="s">
         <v>432</v>
       </c>
-      <c r="U143" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V143" s="7"/>
-      <c r="W143" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="144" spans="1:23">
-      <c r="A144" t="s">
+      <c r="D143"/>
+      <c r="E143"/>
+      <c r="F143"/>
+      <c r="G143"/>
+      <c r="H143"/>
+      <c r="J143"/>
+      <c r="K143"/>
+      <c r="L143" s="7"/>
+      <c r="M143" s="12"/>
+      <c r="N143" s="12"/>
+      <c r="O143" s="12"/>
+      <c r="P143" s="12"/>
+      <c r="Q143" s="12"/>
+      <c r="R143" s="12"/>
+      <c r="S143" s="12"/>
+      <c r="U143" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V143" s="12"/>
+      <c r="W143" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="144" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="11" t="s">
         <v>442</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B144" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C144" t="s">
         <v>432</v>
       </c>
-      <c r="U144" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V144" s="7"/>
-      <c r="W144" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="145" spans="1:23">
-      <c r="A145" t="s">
+      <c r="D144"/>
+      <c r="E144"/>
+      <c r="F144"/>
+      <c r="G144"/>
+      <c r="H144"/>
+      <c r="J144"/>
+      <c r="K144"/>
+      <c r="L144" s="7"/>
+      <c r="M144" s="12"/>
+      <c r="N144" s="12"/>
+      <c r="O144" s="12"/>
+      <c r="P144" s="12"/>
+      <c r="Q144" s="12"/>
+      <c r="R144" s="12"/>
+      <c r="S144" s="12"/>
+      <c r="U144" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V144" s="12"/>
+      <c r="W144" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="145" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="11" t="s">
         <v>443</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B145" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C145" t="s">
         <v>432</v>
       </c>
-      <c r="U145" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V145" s="7"/>
-      <c r="W145" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="146" spans="1:23">
-      <c r="A146" t="s">
+      <c r="D145"/>
+      <c r="E145"/>
+      <c r="F145"/>
+      <c r="G145"/>
+      <c r="H145"/>
+      <c r="J145"/>
+      <c r="K145"/>
+      <c r="L145" s="7"/>
+      <c r="M145" s="12"/>
+      <c r="N145" s="12"/>
+      <c r="O145" s="12"/>
+      <c r="P145" s="12"/>
+      <c r="Q145" s="12"/>
+      <c r="R145" s="12"/>
+      <c r="S145" s="12"/>
+      <c r="U145" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V145" s="12"/>
+      <c r="W145" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="146" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="11" t="s">
         <v>444</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B146" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C146" t="s">
         <v>432</v>
       </c>
-      <c r="U146" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V146" s="7"/>
-      <c r="W146" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="147" spans="1:23">
-      <c r="A147" t="s">
+      <c r="D146"/>
+      <c r="E146"/>
+      <c r="F146"/>
+      <c r="G146"/>
+      <c r="H146"/>
+      <c r="J146"/>
+      <c r="K146"/>
+      <c r="L146" s="7"/>
+      <c r="M146" s="12"/>
+      <c r="N146" s="12"/>
+      <c r="O146" s="12"/>
+      <c r="P146" s="12"/>
+      <c r="Q146" s="12"/>
+      <c r="R146" s="12"/>
+      <c r="S146" s="12"/>
+      <c r="U146" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V146" s="12"/>
+      <c r="W146" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="147" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="11" t="s">
         <v>445</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B147" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C147" t="s">
         <v>432</v>
       </c>
-      <c r="U147" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V147" s="7"/>
-      <c r="W147" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="148" spans="1:23">
-      <c r="A148" t="s">
+      <c r="D147"/>
+      <c r="E147"/>
+      <c r="F147"/>
+      <c r="G147"/>
+      <c r="H147"/>
+      <c r="J147"/>
+      <c r="K147"/>
+      <c r="L147" s="7"/>
+      <c r="M147" s="12"/>
+      <c r="N147" s="12"/>
+      <c r="O147" s="12"/>
+      <c r="P147" s="12"/>
+      <c r="Q147" s="12"/>
+      <c r="R147" s="12"/>
+      <c r="S147" s="12"/>
+      <c r="U147" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V147" s="12"/>
+      <c r="W147" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="148" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="11" t="s">
         <v>446</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B148" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C148" t="s">
         <v>432</v>
       </c>
-      <c r="U148" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V148" s="7"/>
-      <c r="W148" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="149" spans="1:23">
-      <c r="A149" t="s">
+      <c r="D148"/>
+      <c r="E148"/>
+      <c r="F148"/>
+      <c r="G148"/>
+      <c r="H148"/>
+      <c r="J148"/>
+      <c r="K148"/>
+      <c r="L148" s="7"/>
+      <c r="M148" s="12"/>
+      <c r="N148" s="12"/>
+      <c r="O148" s="12"/>
+      <c r="P148" s="12"/>
+      <c r="Q148" s="12"/>
+      <c r="R148" s="12"/>
+      <c r="S148" s="12"/>
+      <c r="U148" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V148" s="12"/>
+      <c r="W148" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="149" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="11" t="s">
         <v>447</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B149" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C149" t="s">
         <v>432</v>
       </c>
-      <c r="U149" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V149" s="7"/>
-      <c r="W149" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="150" spans="1:23">
-      <c r="A150" t="s">
+      <c r="D149"/>
+      <c r="E149"/>
+      <c r="F149"/>
+      <c r="G149"/>
+      <c r="H149"/>
+      <c r="J149"/>
+      <c r="K149"/>
+      <c r="L149" s="7"/>
+      <c r="M149" s="12"/>
+      <c r="N149" s="12"/>
+      <c r="O149" s="12"/>
+      <c r="P149" s="12"/>
+      <c r="Q149" s="12"/>
+      <c r="R149" s="12"/>
+      <c r="S149" s="12"/>
+      <c r="U149" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V149" s="12"/>
+      <c r="W149" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="150" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="11" t="s">
         <v>448</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B150" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C150" t="s">
         <v>432</v>
       </c>
-      <c r="U150" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V150" s="7"/>
-      <c r="W150" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="151" spans="1:23">
-      <c r="A151" t="s">
+      <c r="D150"/>
+      <c r="E150"/>
+      <c r="F150"/>
+      <c r="G150"/>
+      <c r="H150"/>
+      <c r="J150"/>
+      <c r="K150"/>
+      <c r="L150" s="7"/>
+      <c r="M150" s="12"/>
+      <c r="N150" s="12"/>
+      <c r="O150" s="12"/>
+      <c r="P150" s="12"/>
+      <c r="Q150" s="12"/>
+      <c r="R150" s="12"/>
+      <c r="S150" s="12"/>
+      <c r="U150" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V150" s="12"/>
+      <c r="W150" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="151" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="11" t="s">
         <v>449</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B151" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C151" t="s">
         <v>432</v>
       </c>
-      <c r="U151" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V151" s="7"/>
-      <c r="W151" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="152" spans="1:23">
-      <c r="A152" t="s">
+      <c r="D151"/>
+      <c r="E151"/>
+      <c r="F151"/>
+      <c r="G151"/>
+      <c r="H151"/>
+      <c r="J151"/>
+      <c r="K151"/>
+      <c r="L151" s="7"/>
+      <c r="M151" s="12"/>
+      <c r="N151" s="12"/>
+      <c r="O151" s="12"/>
+      <c r="P151" s="12"/>
+      <c r="Q151" s="12"/>
+      <c r="R151" s="12"/>
+      <c r="S151" s="12"/>
+      <c r="U151" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V151" s="12"/>
+      <c r="W151" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="152" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="11" t="s">
         <v>450</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B152" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C152" t="s">
         <v>432</v>
       </c>
-      <c r="U152" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V152" s="7"/>
-      <c r="W152" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="153" spans="1:23">
-      <c r="A153" t="s">
+      <c r="D152"/>
+      <c r="E152"/>
+      <c r="F152"/>
+      <c r="G152"/>
+      <c r="H152"/>
+      <c r="J152"/>
+      <c r="K152"/>
+      <c r="L152" s="7"/>
+      <c r="M152" s="12"/>
+      <c r="N152" s="12"/>
+      <c r="O152" s="12"/>
+      <c r="P152" s="12"/>
+      <c r="Q152" s="12"/>
+      <c r="R152" s="12"/>
+      <c r="S152" s="12"/>
+      <c r="U152" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V152" s="12"/>
+      <c r="W152" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="153" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="11" t="s">
         <v>451</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B153" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C153" t="s">
         <v>452</v>
       </c>
+      <c r="D153"/>
+      <c r="E153"/>
       <c r="F153" t="s">
         <v>453</v>
       </c>
       <c r="G153" t="s">
         <v>27</v>
       </c>
+      <c r="H153"/>
       <c r="J153" t="s">
         <v>301</v>
       </c>
       <c r="K153" t="s">
         <v>289</v>
       </c>
-      <c r="U153" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V153" s="7"/>
-      <c r="W153" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="154" spans="1:23">
-      <c r="A154" t="s">
+      <c r="L153" s="7"/>
+      <c r="M153" s="12"/>
+      <c r="N153" s="12"/>
+      <c r="O153" s="12"/>
+      <c r="P153" s="12"/>
+      <c r="Q153" s="12"/>
+      <c r="R153" s="12"/>
+      <c r="S153" s="12"/>
+      <c r="U153" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V153" s="12"/>
+      <c r="W153" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="154" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="11" t="s">
         <v>454</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B154" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C154" t="s">
         <v>432</v>
       </c>
-      <c r="U154" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V154" s="7"/>
-      <c r="W154" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="155" spans="1:23">
-      <c r="A155" t="s">
+      <c r="D154"/>
+      <c r="E154"/>
+      <c r="F154"/>
+      <c r="G154"/>
+      <c r="H154"/>
+      <c r="J154"/>
+      <c r="K154"/>
+      <c r="L154" s="7"/>
+      <c r="M154" s="12"/>
+      <c r="N154" s="12"/>
+      <c r="O154" s="12"/>
+      <c r="P154" s="12"/>
+      <c r="Q154" s="12"/>
+      <c r="R154" s="12"/>
+      <c r="S154" s="12"/>
+      <c r="U154" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V154" s="12"/>
+      <c r="W154" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="155" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="11" t="s">
         <v>455</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B155" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C155" t="s">
         <v>432</v>
       </c>
-      <c r="U155" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V155" s="7"/>
-      <c r="W155" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="156" spans="1:23">
-      <c r="A156" t="s">
+      <c r="D155"/>
+      <c r="E155"/>
+      <c r="F155"/>
+      <c r="G155"/>
+      <c r="H155"/>
+      <c r="J155"/>
+      <c r="K155"/>
+      <c r="L155" s="7"/>
+      <c r="M155" s="12"/>
+      <c r="N155" s="12"/>
+      <c r="O155" s="12"/>
+      <c r="P155" s="12"/>
+      <c r="Q155" s="12"/>
+      <c r="R155" s="12"/>
+      <c r="S155" s="12"/>
+      <c r="U155" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V155" s="12"/>
+      <c r="W155" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="156" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="11" t="s">
         <v>456</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B156" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C156" t="s">
         <v>432</v>
       </c>
-      <c r="U156" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V156" s="7"/>
-      <c r="W156" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="157" spans="1:23">
-      <c r="A157" t="s">
+      <c r="D156"/>
+      <c r="E156"/>
+      <c r="F156"/>
+      <c r="G156"/>
+      <c r="H156"/>
+      <c r="J156"/>
+      <c r="K156"/>
+      <c r="L156" s="7"/>
+      <c r="M156" s="12"/>
+      <c r="N156" s="12"/>
+      <c r="O156" s="12"/>
+      <c r="P156" s="12"/>
+      <c r="Q156" s="12"/>
+      <c r="R156" s="12"/>
+      <c r="S156" s="12"/>
+      <c r="U156" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V156" s="12"/>
+      <c r="W156" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="157" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B157" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C157" t="s">
         <v>432</v>
       </c>
-      <c r="U157" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V157" s="7"/>
-      <c r="W157" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="158" spans="1:23">
-      <c r="A158" t="s">
+      <c r="D157"/>
+      <c r="E157"/>
+      <c r="F157"/>
+      <c r="G157"/>
+      <c r="H157"/>
+      <c r="J157"/>
+      <c r="K157"/>
+      <c r="L157" s="7"/>
+      <c r="M157" s="12"/>
+      <c r="N157" s="12"/>
+      <c r="O157" s="12"/>
+      <c r="P157" s="12"/>
+      <c r="Q157" s="12"/>
+      <c r="R157" s="12"/>
+      <c r="S157" s="12"/>
+      <c r="U157" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V157" s="12"/>
+      <c r="W157" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="158" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="11" t="s">
         <v>458</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B158" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C158" t="s">
         <v>432</v>
       </c>
-      <c r="U158" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V158" s="7"/>
-      <c r="W158" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="159" spans="1:23">
-      <c r="A159" t="s">
+      <c r="D158"/>
+      <c r="E158"/>
+      <c r="F158"/>
+      <c r="G158"/>
+      <c r="H158"/>
+      <c r="J158"/>
+      <c r="K158"/>
+      <c r="L158" s="7"/>
+      <c r="M158" s="12"/>
+      <c r="N158" s="12"/>
+      <c r="O158" s="12"/>
+      <c r="P158" s="12"/>
+      <c r="Q158" s="12"/>
+      <c r="R158" s="12"/>
+      <c r="S158" s="12"/>
+      <c r="U158" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V158" s="12"/>
+      <c r="W158" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="159" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="11" t="s">
         <v>459</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B159" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C159" t="s">
         <v>432</v>
       </c>
-      <c r="U159" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V159" s="7"/>
-      <c r="W159" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="160" spans="1:23">
-      <c r="A160" t="s">
+      <c r="D159"/>
+      <c r="E159"/>
+      <c r="F159"/>
+      <c r="G159"/>
+      <c r="H159"/>
+      <c r="J159"/>
+      <c r="K159"/>
+      <c r="L159" s="7"/>
+      <c r="M159" s="12"/>
+      <c r="N159" s="12"/>
+      <c r="O159" s="12"/>
+      <c r="P159" s="12"/>
+      <c r="Q159" s="12"/>
+      <c r="R159" s="12"/>
+      <c r="S159" s="12"/>
+      <c r="U159" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V159" s="12"/>
+      <c r="W159" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="160" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="11" t="s">
         <v>460</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B160" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C160" t="s">
         <v>432</v>
       </c>
-      <c r="U160" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V160" s="7"/>
-      <c r="W160" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="161" spans="1:23">
-      <c r="A161" t="s">
+      <c r="D160"/>
+      <c r="E160"/>
+      <c r="F160"/>
+      <c r="G160"/>
+      <c r="H160"/>
+      <c r="J160"/>
+      <c r="K160"/>
+      <c r="L160" s="7"/>
+      <c r="M160" s="12"/>
+      <c r="N160" s="12"/>
+      <c r="O160" s="12"/>
+      <c r="P160" s="12"/>
+      <c r="Q160" s="12"/>
+      <c r="R160" s="12"/>
+      <c r="S160" s="12"/>
+      <c r="U160" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V160" s="12"/>
+      <c r="W160" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="161" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="11" t="s">
         <v>461</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B161" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C161" t="s">
         <v>432</v>
       </c>
-      <c r="U161" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V161" s="7"/>
-      <c r="W161" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="162" spans="1:23">
-      <c r="A162" t="s">
+      <c r="D161"/>
+      <c r="E161"/>
+      <c r="F161"/>
+      <c r="G161"/>
+      <c r="H161"/>
+      <c r="J161"/>
+      <c r="K161"/>
+      <c r="L161" s="7"/>
+      <c r="M161" s="12"/>
+      <c r="N161" s="12"/>
+      <c r="O161" s="12"/>
+      <c r="P161" s="12"/>
+      <c r="Q161" s="12"/>
+      <c r="R161" s="12"/>
+      <c r="S161" s="12"/>
+      <c r="U161" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V161" s="12"/>
+      <c r="W161" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="162" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="11" t="s">
         <v>462</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B162" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C162" t="s">
         <v>432</v>
       </c>
-      <c r="U162" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V162" s="7"/>
-      <c r="W162" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="163" spans="1:23">
-      <c r="A163" t="s">
+      <c r="D162"/>
+      <c r="E162"/>
+      <c r="F162"/>
+      <c r="G162"/>
+      <c r="H162"/>
+      <c r="J162"/>
+      <c r="K162"/>
+      <c r="L162" s="7"/>
+      <c r="M162" s="12"/>
+      <c r="N162" s="12"/>
+      <c r="O162" s="12"/>
+      <c r="P162" s="12"/>
+      <c r="Q162" s="12"/>
+      <c r="R162" s="12"/>
+      <c r="S162" s="12"/>
+      <c r="U162" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V162" s="12"/>
+      <c r="W162" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="163" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="11" t="s">
         <v>463</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B163" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C163" t="s">
         <v>432</v>
       </c>
-      <c r="U163" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V163" s="7"/>
-      <c r="W163" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="164" spans="1:23">
-      <c r="A164" t="s">
+      <c r="D163"/>
+      <c r="E163"/>
+      <c r="F163"/>
+      <c r="G163"/>
+      <c r="H163"/>
+      <c r="J163"/>
+      <c r="K163"/>
+      <c r="L163" s="7"/>
+      <c r="M163" s="12"/>
+      <c r="N163" s="12"/>
+      <c r="O163" s="12"/>
+      <c r="P163" s="12"/>
+      <c r="Q163" s="12"/>
+      <c r="R163" s="12"/>
+      <c r="S163" s="12"/>
+      <c r="U163" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V163" s="12"/>
+      <c r="W163" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="164" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="11" t="s">
         <v>464</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B164" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C164" t="s">
         <v>432</v>
       </c>
-      <c r="U164" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V164" s="7"/>
-      <c r="W164" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="165" spans="1:23">
-      <c r="A165" t="s">
+      <c r="D164"/>
+      <c r="E164"/>
+      <c r="F164"/>
+      <c r="G164"/>
+      <c r="H164"/>
+      <c r="J164"/>
+      <c r="K164"/>
+      <c r="L164" s="7"/>
+      <c r="M164" s="12"/>
+      <c r="N164" s="12"/>
+      <c r="O164" s="12"/>
+      <c r="P164" s="12"/>
+      <c r="Q164" s="12"/>
+      <c r="R164" s="12"/>
+      <c r="S164" s="12"/>
+      <c r="U164" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V164" s="12"/>
+      <c r="W164" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="165" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B165" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C165" s="4" t="s">
@@ -9479,231 +10012,377 @@
       <c r="K165" t="s">
         <v>289</v>
       </c>
-      <c r="U165" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V165" s="7"/>
-      <c r="W165" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="166" spans="1:23">
-      <c r="A166" t="s">
+      <c r="L165" s="7"/>
+      <c r="M165" s="12"/>
+      <c r="N165" s="12"/>
+      <c r="O165" s="12"/>
+      <c r="P165" s="12"/>
+      <c r="Q165" s="12"/>
+      <c r="R165" s="12"/>
+      <c r="S165" s="12"/>
+      <c r="U165" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V165" s="12"/>
+      <c r="W165" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="166" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="11" t="s">
         <v>469</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B166" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C166" t="s">
         <v>432</v>
       </c>
-      <c r="U166" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V166" s="7"/>
-      <c r="W166" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="167" spans="1:23">
-      <c r="A167" t="s">
+      <c r="D166"/>
+      <c r="E166"/>
+      <c r="F166"/>
+      <c r="G166"/>
+      <c r="H166"/>
+      <c r="J166"/>
+      <c r="K166"/>
+      <c r="L166" s="7"/>
+      <c r="M166" s="12"/>
+      <c r="N166" s="12"/>
+      <c r="O166" s="12"/>
+      <c r="P166" s="12"/>
+      <c r="Q166" s="12"/>
+      <c r="R166" s="12"/>
+      <c r="S166" s="12"/>
+      <c r="U166" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V166" s="12"/>
+      <c r="W166" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="167" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="11" t="s">
         <v>470</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B167" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C167" t="s">
         <v>432</v>
       </c>
-      <c r="U167" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V167" s="7"/>
-      <c r="W167" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="168" spans="1:23">
-      <c r="A168" t="s">
+      <c r="D167"/>
+      <c r="E167"/>
+      <c r="F167"/>
+      <c r="G167"/>
+      <c r="H167"/>
+      <c r="J167"/>
+      <c r="K167"/>
+      <c r="L167" s="7"/>
+      <c r="M167" s="12"/>
+      <c r="N167" s="12"/>
+      <c r="O167" s="12"/>
+      <c r="P167" s="12"/>
+      <c r="Q167" s="12"/>
+      <c r="R167" s="12"/>
+      <c r="S167" s="12"/>
+      <c r="U167" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V167" s="12"/>
+      <c r="W167" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="168" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="11" t="s">
         <v>471</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B168" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C168" t="s">
         <v>432</v>
       </c>
-      <c r="U168" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V168" s="7"/>
-      <c r="W168" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="169" spans="1:23">
-      <c r="A169" t="s">
+      <c r="D168"/>
+      <c r="E168"/>
+      <c r="F168"/>
+      <c r="G168"/>
+      <c r="H168"/>
+      <c r="J168"/>
+      <c r="K168"/>
+      <c r="L168" s="7"/>
+      <c r="M168" s="12"/>
+      <c r="N168" s="12"/>
+      <c r="O168" s="12"/>
+      <c r="P168" s="12"/>
+      <c r="Q168" s="12"/>
+      <c r="R168" s="12"/>
+      <c r="S168" s="12"/>
+      <c r="U168" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V168" s="12"/>
+      <c r="W168" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="169" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="11" t="s">
         <v>472</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B169" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C169" t="s">
         <v>432</v>
       </c>
-      <c r="U169" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V169" s="7"/>
-      <c r="W169" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="170" spans="1:23">
-      <c r="A170" t="s">
+      <c r="D169"/>
+      <c r="E169"/>
+      <c r="F169"/>
+      <c r="G169"/>
+      <c r="H169"/>
+      <c r="J169"/>
+      <c r="K169"/>
+      <c r="L169" s="7"/>
+      <c r="M169" s="12"/>
+      <c r="N169" s="12"/>
+      <c r="O169" s="12"/>
+      <c r="P169" s="12"/>
+      <c r="Q169" s="12"/>
+      <c r="R169" s="12"/>
+      <c r="S169" s="12"/>
+      <c r="U169" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V169" s="12"/>
+      <c r="W169" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="170" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="11" t="s">
         <v>473</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B170" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C170" t="s">
         <v>432</v>
       </c>
-      <c r="U170" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V170" s="7"/>
-      <c r="W170" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="171" spans="1:23">
-      <c r="A171" t="s">
+      <c r="D170"/>
+      <c r="E170"/>
+      <c r="F170"/>
+      <c r="G170"/>
+      <c r="H170"/>
+      <c r="J170"/>
+      <c r="K170"/>
+      <c r="L170" s="7"/>
+      <c r="M170" s="12"/>
+      <c r="N170" s="12"/>
+      <c r="O170" s="12"/>
+      <c r="P170" s="12"/>
+      <c r="Q170" s="12"/>
+      <c r="R170" s="12"/>
+      <c r="S170" s="12"/>
+      <c r="U170" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V170" s="12"/>
+      <c r="W170" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="171" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="11" t="s">
         <v>474</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B171" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C171" t="s">
         <v>432</v>
       </c>
-      <c r="U171" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V171" s="7"/>
-      <c r="W171" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="172" spans="1:23">
-      <c r="A172" t="s">
+      <c r="D171"/>
+      <c r="E171"/>
+      <c r="F171"/>
+      <c r="G171"/>
+      <c r="H171"/>
+      <c r="J171"/>
+      <c r="K171"/>
+      <c r="L171" s="7"/>
+      <c r="M171" s="12"/>
+      <c r="N171" s="12"/>
+      <c r="O171" s="12"/>
+      <c r="P171" s="12"/>
+      <c r="Q171" s="12"/>
+      <c r="R171" s="12"/>
+      <c r="S171" s="12"/>
+      <c r="U171" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V171" s="12"/>
+      <c r="W171" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="172" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="11" t="s">
         <v>475</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B172" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C172" t="s">
         <v>432</v>
       </c>
-      <c r="U172" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V172" s="7"/>
-      <c r="W172" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="173" spans="1:23">
-      <c r="A173" t="s">
+      <c r="D172"/>
+      <c r="E172"/>
+      <c r="F172"/>
+      <c r="G172"/>
+      <c r="H172"/>
+      <c r="J172"/>
+      <c r="K172"/>
+      <c r="L172" s="7"/>
+      <c r="M172" s="12"/>
+      <c r="N172" s="12"/>
+      <c r="O172" s="12"/>
+      <c r="P172" s="12"/>
+      <c r="Q172" s="12"/>
+      <c r="R172" s="12"/>
+      <c r="S172" s="12"/>
+      <c r="U172" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V172" s="12"/>
+      <c r="W172" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="173" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="11" t="s">
         <v>476</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B173" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C173" t="s">
         <v>477</v>
       </c>
+      <c r="D173"/>
+      <c r="E173"/>
       <c r="F173" t="s">
         <v>478</v>
       </c>
       <c r="G173" t="s">
         <v>27</v>
       </c>
+      <c r="H173"/>
       <c r="J173" t="s">
         <v>479</v>
       </c>
       <c r="K173" t="s">
         <v>289</v>
       </c>
-      <c r="U173" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V173" s="7"/>
-      <c r="W173" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="174" spans="1:23">
-      <c r="A174" t="s">
+      <c r="L173" s="7"/>
+      <c r="M173" s="12"/>
+      <c r="N173" s="12"/>
+      <c r="O173" s="12"/>
+      <c r="P173" s="12"/>
+      <c r="Q173" s="12"/>
+      <c r="R173" s="12"/>
+      <c r="S173" s="12"/>
+      <c r="U173" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V173" s="12"/>
+      <c r="W173" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="174" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="11" t="s">
         <v>480</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B174" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C174" t="s">
         <v>481</v>
       </c>
+      <c r="D174"/>
+      <c r="E174"/>
       <c r="F174" t="s">
         <v>482</v>
       </c>
       <c r="G174" t="s">
         <v>27</v>
       </c>
+      <c r="H174"/>
       <c r="J174" t="s">
         <v>483</v>
       </c>
       <c r="K174" t="s">
         <v>289</v>
       </c>
-      <c r="U174" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V174" s="7"/>
-      <c r="W174" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="175" spans="1:23">
-      <c r="A175" t="s">
+      <c r="L174" s="7"/>
+      <c r="M174" s="12"/>
+      <c r="N174" s="12"/>
+      <c r="O174" s="12"/>
+      <c r="P174" s="12"/>
+      <c r="Q174" s="12"/>
+      <c r="R174" s="12"/>
+      <c r="S174" s="12"/>
+      <c r="U174" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V174" s="12"/>
+      <c r="W174" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="175" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="11" t="s">
         <v>484</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B175" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C175" t="s">
         <v>485</v>
       </c>
+      <c r="D175"/>
+      <c r="E175"/>
       <c r="F175" t="s">
         <v>486</v>
       </c>
       <c r="G175" t="s">
         <v>27</v>
       </c>
+      <c r="H175"/>
       <c r="J175" t="s">
         <v>487</v>
       </c>
       <c r="K175" t="s">
         <v>289</v>
       </c>
-      <c r="U175" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V175" s="7"/>
-      <c r="W175" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="176" spans="1:23" hidden="1">
+      <c r="L175" s="7"/>
+      <c r="M175" s="12"/>
+      <c r="N175" s="12"/>
+      <c r="O175" s="12"/>
+      <c r="P175" s="12"/>
+      <c r="Q175" s="12"/>
+      <c r="R175" s="12"/>
+      <c r="S175" s="12"/>
+      <c r="U175" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="V175" s="12"/>
+      <c r="W175" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="176" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>488</v>
       </c>
@@ -9752,7 +10431,7 @@
       <c r="V176" s="7"/>
       <c r="W176"/>
     </row>
-    <row r="177" spans="1:23" hidden="1">
+    <row r="177" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>492</v>
       </c>
@@ -9801,7 +10480,7 @@
       <c r="V177" s="7"/>
       <c r="W177"/>
     </row>
-    <row r="178" spans="1:23" hidden="1">
+    <row r="178" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>494</v>
       </c>
@@ -9850,7 +10529,7 @@
       <c r="V178" s="7"/>
       <c r="W178"/>
     </row>
-    <row r="179" spans="1:23" hidden="1">
+    <row r="179" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>497</v>
       </c>
@@ -9899,7 +10578,7 @@
       <c r="V179" s="7"/>
       <c r="W179"/>
     </row>
-    <row r="180" spans="1:23" hidden="1">
+    <row r="180" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>499</v>
       </c>
@@ -9948,7 +10627,7 @@
       <c r="V180" s="7"/>
       <c r="W180"/>
     </row>
-    <row r="181" spans="1:23" hidden="1">
+    <row r="181" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>503</v>
       </c>
@@ -9997,7 +10676,7 @@
       <c r="V181" s="7"/>
       <c r="W181"/>
     </row>
-    <row r="182" spans="1:23" ht="30">
+    <row r="182" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>505</v>
       </c>
@@ -10051,7 +10730,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="183" spans="1:23">
+    <row r="183" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>510</v>
       </c>
@@ -10078,7 +10757,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="184" spans="1:23" hidden="1">
+    <row r="184" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>514</v>
       </c>
@@ -10128,7 +10807,7 @@
       <c r="V184" s="7"/>
       <c r="W184"/>
     </row>
-    <row r="185" spans="1:23" hidden="1">
+    <row r="185" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>517</v>
       </c>
@@ -10175,7 +10854,7 @@
       <c r="V185" s="7"/>
       <c r="W185"/>
     </row>
-    <row r="186" spans="1:23">
+    <row r="186" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>519</v>
       </c>
@@ -10229,7 +10908,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="187" spans="1:23">
+    <row r="187" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>523</v>
       </c>
@@ -10265,7 +10944,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="188" spans="1:23">
+    <row r="188" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>525</v>
       </c>
@@ -10286,7 +10965,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="189" spans="1:23">
+    <row r="189" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>526</v>
       </c>
@@ -10313,7 +10992,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="190" spans="1:23" hidden="1">
+    <row r="190" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>529</v>
       </c>
@@ -10359,7 +11038,7 @@
       <c r="V190" s="7"/>
       <c r="W190"/>
     </row>
-    <row r="191" spans="1:23" hidden="1">
+    <row r="191" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>532</v>
       </c>
@@ -10402,7 +11081,7 @@
       <c r="V191" s="7"/>
       <c r="W191"/>
     </row>
-    <row r="192" spans="1:23" hidden="1">
+    <row r="192" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>536</v>
       </c>
@@ -10445,7 +11124,7 @@
       <c r="V192" s="7"/>
       <c r="W192"/>
     </row>
-    <row r="193" spans="1:23">
+    <row r="193" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>538</v>
       </c>
@@ -10499,7 +11178,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="194" spans="1:23" ht="30">
+    <row r="194" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>543</v>
       </c>
@@ -10571,294 +11250,294 @@
       <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>2552</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2552</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3055</v>
       </c>
     </row>
-    <row r="4" spans="1:1" hidden="1">
+    <row r="4" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3055</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3201</v>
       </c>
     </row>
-    <row r="6" spans="1:1" hidden="1">
+    <row r="6" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3201</v>
       </c>
     </row>
-    <row r="7" spans="1:1" hidden="1">
+    <row r="7" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3201</v>
       </c>
     </row>
-    <row r="8" spans="1:1" hidden="1">
+    <row r="8" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3201</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5031</v>
       </c>
     </row>
-    <row r="10" spans="1:1" hidden="1">
+    <row r="10" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5031</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5664</v>
       </c>
     </row>
-    <row r="12" spans="1:1" hidden="1">
+    <row r="12" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5664</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5676</v>
       </c>
     </row>
-    <row r="14" spans="1:1" hidden="1">
+    <row r="14" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5676</v>
       </c>
     </row>
-    <row r="15" spans="1:1" hidden="1">
+    <row r="15" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5676</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6183</v>
       </c>
     </row>
-    <row r="17" spans="1:1" hidden="1">
+    <row r="17" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6183</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6242</v>
       </c>
     </row>
-    <row r="19" spans="1:1" hidden="1">
+    <row r="19" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6242</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6347</v>
       </c>
     </row>
-    <row r="21" spans="1:1" hidden="1">
+    <row r="21" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6347</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6362</v>
       </c>
     </row>
-    <row r="23" spans="1:1" hidden="1">
+    <row r="23" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6362</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6371</v>
       </c>
     </row>
-    <row r="25" spans="1:1" hidden="1">
+    <row r="25" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6371</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6485</v>
       </c>
     </row>
-    <row r="27" spans="1:1" hidden="1">
+    <row r="27" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>6485</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6571</v>
       </c>
     </row>
-    <row r="29" spans="1:1" hidden="1">
+    <row r="29" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6571</v>
       </c>
     </row>
-    <row r="30" spans="1:1" hidden="1">
+    <row r="30" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6571</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>6692</v>
       </c>
     </row>
-    <row r="32" spans="1:1" hidden="1">
+    <row r="32" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6692</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>6734</v>
       </c>
     </row>
-    <row r="34" spans="1:1" hidden="1">
+    <row r="34" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>6734</v>
       </c>
     </row>
-    <row r="35" spans="1:1" hidden="1">
+    <row r="35" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>6734</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>6830</v>
       </c>
     </row>
-    <row r="37" spans="1:1" hidden="1">
+    <row r="37" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>6830</v>
       </c>
     </row>
-    <row r="38" spans="1:1" hidden="1">
+    <row r="38" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>6830</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>7114</v>
       </c>
     </row>
-    <row r="40" spans="1:1" hidden="1">
+    <row r="40" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>7114</v>
       </c>
     </row>
-    <row r="41" spans="1:1" hidden="1">
+    <row r="41" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>7114</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>7235</v>
       </c>
     </row>
-    <row r="43" spans="1:1" hidden="1">
+    <row r="43" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>7235</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>7236</v>
       </c>
     </row>
-    <row r="45" spans="1:1" hidden="1">
+    <row r="45" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>7236</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>7237</v>
       </c>
     </row>
-    <row r="47" spans="1:1" hidden="1">
+    <row r="47" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>7237</v>
       </c>
     </row>
-    <row r="48" spans="1:1" hidden="1">
+    <row r="48" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>7237</v>
       </c>
     </row>
-    <row r="49" spans="1:1" hidden="1">
+    <row r="49" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>7237</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>7258</v>
       </c>
     </row>
-    <row r="51" spans="1:1" hidden="1">
+    <row r="51" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>7258</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>7282</v>
       </c>
     </row>
-    <row r="53" spans="1:1" hidden="1">
+    <row r="53" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>7282</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>7283</v>
       </c>
     </row>
-    <row r="55" spans="1:1" hidden="1">
+    <row r="55" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>7283</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>7294</v>
       </c>
     </row>
-    <row r="57" spans="1:1" hidden="1">
+    <row r="57" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>7294</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>4</v>
       </c>
@@ -10872,6 +11551,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEAE28352B96D64C95AA0D5E2FA62FAD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed183881d36ac1b5d7d67982eda510d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d161086-4829-409f-9f75-5bde88dcb151" xmlns:ns3="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="685f4fda20cf913d28bf77c13cd653dd" ns2:_="" ns3:_="">
     <xsd:import namespace="3d161086-4829-409f-9f75-5bde88dcb151"/>
@@ -11094,15 +11782,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -11115,13 +11794,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C74AB5E7-5C87-4FF7-BF80-AB0EB6BD1D32}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C74AB5E7-5C87-4FF7-BF80-AB0EB6BD1D32}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
V_STG_SERD_ROW_CONTINUATION and V_STG_SERD_ROW_MAIN modified
All scripts consolidated in one folder under 'ddl'
</commit_message>
<xml_diff>
--- a/analysis/MEDS_Tables.xlsx
+++ b/analysis/MEDS_Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.arboittedossantos\Shield Reply\UKHO - MEDS Replacement - Documents\MEDS DB\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="451" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{9430AA97-1569-418E-8D34-29C52C4B43A0}"/>
+  <xr:revisionPtr revIDLastSave="466" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8326922-C663-4164-93A2-66C044B6436F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meds_tables" sheetId="1" r:id="rId1"/>
@@ -1670,9 +1670,6 @@
     <t>Glider_threaded 92</t>
   </si>
   <si>
-    <t>Glider_threaded 93</t>
-  </si>
-  <si>
     <t>OMNI_AMBIENT 16 ?</t>
   </si>
   <si>
@@ -1724,13 +1721,16 @@
     <t>MLO_SHIP 23</t>
   </si>
   <si>
-    <t>PROFILE_HEADER_SV 75</t>
-  </si>
-  <si>
-    <t>PROFILE_HEADER_TS 74</t>
-  </si>
-  <si>
-    <t>PROFILE_INDEX_TONLY 70</t>
+    <t>Field Index</t>
+  </si>
+  <si>
+    <t>82 ?</t>
+  </si>
+  <si>
+    <t>16 ?</t>
+  </si>
+  <si>
+    <t>JD027_A_sta.dat, JD027_A_sta.hdr, JD028_A_sta.dat, JD028_A_sta.hdr</t>
   </si>
 </sst>
 </file>
@@ -2319,7 +2319,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2372,6 +2372,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2419,6 +2428,20 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2441,20 +2464,6 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2555,7 +2564,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{272C22F9-909F-4469-A1D3-BB727D8CFD47}" name="Table2" displayName="Table2" ref="A1:C42" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{272C22F9-909F-4469-A1D3-BB727D8CFD47}" name="Table2" displayName="Table2" ref="A1:C42" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:C42" xr:uid="{A0B33C19-2877-43DA-A8B5-1F8EC96E5D8B}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A80168AA-523D-45E3-8F4C-4204320BF4B2}" name="Table"/>
@@ -10093,284 +10102,295 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76451C41-9738-4BC1-978E-20A0DA8744C6}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43" style="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.28515625" style="29" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="22"/>
     <col min="7" max="7" width="11.28515625" style="22" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="30" t="s">
+        <v>561</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>535</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="31">
+        <v>88</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="27"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="16" t="s">
+        <v>564</v>
+      </c>
+      <c r="F2" s="27"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>536</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="32">
+        <v>89</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="28"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="14" t="s">
+        <v>564</v>
+      </c>
+      <c r="F3" s="28"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>45</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>537</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="31">
+        <v>90</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="27"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="16" t="s">
+        <v>564</v>
+      </c>
+      <c r="F4" s="27"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>52</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>534</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="32">
+        <v>94</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="E5" s="14" t="s">
         <v>519</v>
       </c>
-      <c r="E5" s="28"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="28"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>55</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>534</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="31">
+        <v>94</v>
+      </c>
+      <c r="D6" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="E6" s="16" t="s">
         <v>519</v>
       </c>
-      <c r="E6" s="27"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="27"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>77</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="32">
+        <v>89</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="E7" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="E7" s="28" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="28"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>83</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="31">
+        <v>89</v>
+      </c>
+      <c r="D8" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="E8" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="27" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="27"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>104</v>
+        <v>170</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>540</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>105</v>
+        <v>542</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>562</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>524</v>
-      </c>
-      <c r="E9" s="28"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>523</v>
+      </c>
+      <c r="F9" s="28"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>107</v>
+        <v>174</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>541</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>105</v>
+        <v>542</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>562</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>524</v>
-      </c>
-      <c r="E10" s="27"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>523</v>
+      </c>
+      <c r="F10" s="27"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>542</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="32" t="s">
+        <v>562</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="E11" s="14" t="s">
         <v>523</v>
       </c>
-      <c r="E11" s="28"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="28"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>174</v>
+        <v>203</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>542</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>171</v>
+        <v>543</v>
+      </c>
+      <c r="C12" s="31">
+        <v>92</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>523</v>
-      </c>
-      <c r="E12" s="27"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>515</v>
+      </c>
+      <c r="F12" s="27"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>542</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>171</v>
+        <v>543</v>
+      </c>
+      <c r="C13" s="32">
+        <v>92</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>523</v>
-      </c>
-      <c r="E13" s="28"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>515</v>
+      </c>
+      <c r="F13" s="28"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>203</v>
+        <v>360</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>543</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>204</v>
+        <v>544</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>563</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>515</v>
-      </c>
-      <c r="E14" s="27"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>518</v>
+      </c>
+      <c r="F14" s="27"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>206</v>
+        <v>363</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>544</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>204</v>
+      <c r="C15" s="32" t="s">
+        <v>563</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>515</v>
-      </c>
-      <c r="E15" s="28"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>360</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>545</v>
-      </c>
-      <c r="C16" s="16" t="s">
         <v>361</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="E15" s="14" t="s">
         <v>518</v>
       </c>
-      <c r="E16" s="27"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>363</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>545</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>361</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>518</v>
-      </c>
-      <c r="E17" s="28"/>
+      <c r="F15" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10380,10 +10400,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA06BA7C-CD17-4C21-9F28-C604AE25C8B9}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10395,7 +10415,7 @@
     <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -10412,12 +10432,12 @@
         <v>539</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>70</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>71</v>
@@ -10427,12 +10447,12 @@
       </c>
       <c r="E2" s="20"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>75</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>71</v>
@@ -10442,72 +10462,72 @@
       </c>
       <c r="E3" s="21"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>540</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>524</v>
+      </c>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>541</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>524</v>
+      </c>
+      <c r="E5" s="21"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>299</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B6" s="16" t="s">
+        <v>547</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>516</v>
+      </c>
+      <c r="E6" s="20"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>547</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>516</v>
+      </c>
+      <c r="E7" s="21"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>548</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>300</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>516</v>
-      </c>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>302</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>548</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>516</v>
-      </c>
-      <c r="E5" s="21"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>304</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>549</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>305</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>521</v>
-      </c>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>309</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>550</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>305</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>521</v>
-      </c>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>551</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>305</v>
@@ -10517,12 +10537,12 @@
       </c>
       <c r="E8" s="20"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>305</v>
@@ -10532,215 +10552,246 @@
       </c>
       <c r="E9" s="21"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>550</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>305</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>521</v>
+      </c>
+      <c r="E10" s="20"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>551</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>521</v>
+      </c>
+      <c r="E11" s="21"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>317</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B12" s="16" t="s">
+        <v>552</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>512</v>
+      </c>
+      <c r="E12" s="20"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>320</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>552</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>512</v>
+      </c>
+      <c r="E13" s="21"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="B14" s="17" t="s">
         <v>553</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>318</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>512</v>
-      </c>
-      <c r="E10" s="20"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>320</v>
-      </c>
-      <c r="B11" s="14" t="s">
+      <c r="C14" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>517</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="21"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>325</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>553</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>318</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>512</v>
-      </c>
-      <c r="E11" s="21"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>322</v>
-      </c>
-      <c r="B12" s="16" t="s">
+      <c r="C15" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>517</v>
+      </c>
+      <c r="E15" s="21"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="B16" s="16" t="s">
         <v>554</v>
       </c>
-      <c r="C12" s="16" t="s">
-        <v>323</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>517</v>
-      </c>
-      <c r="E12" s="20"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>325</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>554</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>323</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>517</v>
-      </c>
-      <c r="E13" s="21"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>327</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>555</v>
-      </c>
-      <c r="C14" s="16" t="s">
+      <c r="C16" s="16" t="s">
         <v>328</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D16" s="16" t="s">
         <v>508</v>
-      </c>
-      <c r="E14" s="20"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>330</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>556</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>328</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>508</v>
-      </c>
-      <c r="E15" s="21"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>332</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>557</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>333</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>510</v>
       </c>
       <c r="E16" s="20"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E17" s="21"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E18" s="20"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E19" s="21"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="E20" s="20"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="E21" s="21"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>520</v>
+        <v>509</v>
       </c>
       <c r="E22" s="20"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
+        <v>345</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>559</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>509</v>
+      </c>
+      <c r="E23" s="21"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>560</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>348</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>520</v>
+      </c>
+      <c r="E24" s="20"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="B23" s="14" t="s">
-        <v>561</v>
-      </c>
-      <c r="C23" s="14" t="s">
+      <c r="B25" s="14" t="s">
+        <v>560</v>
+      </c>
+      <c r="C25" s="14" t="s">
         <v>348</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D25" s="14" t="s">
         <v>520</v>
       </c>
-      <c r="E23" s="21"/>
+      <c r="E25" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10749,160 +10800,141 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A026136A-3463-4F46-9920-D2EEED3E1AFC}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>365</v>
       </c>
-      <c r="B2" s="16"/>
+      <c r="B2" s="16" t="s">
+        <v>366</v>
+      </c>
       <c r="C2" s="16" t="s">
-        <v>366</v>
-      </c>
-      <c r="D2" s="16" t="s">
         <v>514</v>
       </c>
-      <c r="E2" s="20"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" s="20"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>370</v>
       </c>
-      <c r="B3" s="14"/>
+      <c r="B3" s="14" t="s">
+        <v>371</v>
+      </c>
       <c r="C3" s="14" t="s">
-        <v>371</v>
-      </c>
-      <c r="D3" s="14" t="s">
         <v>513</v>
       </c>
-      <c r="E3" s="21"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>373</v>
       </c>
-      <c r="B4" s="16"/>
+      <c r="B4" s="16" t="s">
+        <v>374</v>
+      </c>
       <c r="C4" s="16" t="s">
-        <v>374</v>
-      </c>
-      <c r="D4" s="16" t="s">
         <v>522</v>
       </c>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="20"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>376</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>562</v>
+        <v>366</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>366</v>
-      </c>
-      <c r="D5" s="14" t="s">
         <v>514</v>
       </c>
-      <c r="E5" s="21"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="21"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>378</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="16" t="s">
+        <v>371</v>
+      </c>
       <c r="C6" s="16" t="s">
-        <v>371</v>
-      </c>
-      <c r="D6" s="16" t="s">
         <v>513</v>
       </c>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" s="20"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>380</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>563</v>
+        <v>374</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="D7" s="14" t="s">
         <v>522</v>
       </c>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="21"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>382</v>
       </c>
-      <c r="B8" s="16"/>
+      <c r="B8" s="16" t="s">
+        <v>366</v>
+      </c>
       <c r="C8" s="16" t="s">
-        <v>366</v>
-      </c>
-      <c r="D8" s="16" t="s">
         <v>514</v>
       </c>
-      <c r="E8" s="20"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" s="20"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>384</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>564</v>
+        <v>371</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>371</v>
-      </c>
-      <c r="D9" s="14" t="s">
         <v>513</v>
       </c>
-      <c r="E9" s="21"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="21"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>386</v>
       </c>
-      <c r="B10" s="16"/>
+      <c r="B10" s="16" t="s">
+        <v>374</v>
+      </c>
       <c r="C10" s="16" t="s">
-        <v>374</v>
-      </c>
-      <c r="D10" s="16" t="s">
         <v>522</v>
       </c>
-      <c r="E10" s="20"/>
+      <c r="D10" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11333,6 +11365,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEAE28352B96D64C95AA0D5E2FA62FAD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed183881d36ac1b5d7d67982eda510d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d161086-4829-409f-9f75-5bde88dcb151" xmlns:ns3="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="685f4fda20cf913d28bf77c13cd653dd" ns2:_="" ns3:_="">
     <xsd:import namespace="3d161086-4829-409f-9f75-5bde88dcb151"/>
@@ -11555,33 +11596,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C74AB5E7-5C87-4FF7-BF80-AB0EB6BD1D32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11598,12 +11638,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Data types 89 and 94 done
</commit_message>
<xml_diff>
--- a/analysis/MEDS_Tables.xlsx
+++ b/analysis/MEDS_Tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.arboittedossantos\Shield Reply\UKHO - MEDS Replacement - Documents\MEDS DB\analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="466" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8326922-C663-4164-93A2-66C044B6436F}"/>
+  <xr:revisionPtr revIDLastSave="488" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{644EC829-0B7A-482D-B99F-F4E2D2021820}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meds_tables" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2259" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2264" uniqueCount="566">
   <si>
     <t>Table</t>
   </si>
@@ -1731,6 +1731,9 @@
   </si>
   <si>
     <t>JD027_A_sta.dat, JD027_A_sta.hdr, JD028_A_sta.dat, JD028_A_sta.hdr</t>
+  </si>
+  <si>
+    <t>Job</t>
   </si>
 </sst>
 </file>
@@ -2564,8 +2567,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{272C22F9-909F-4469-A1D3-BB727D8CFD47}" name="Table2" displayName="Table2" ref="A1:C42" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:C42" xr:uid="{A0B33C19-2877-43DA-A8B5-1F8EC96E5D8B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{272C22F9-909F-4469-A1D3-BB727D8CFD47}" name="Table2" displayName="Table2" ref="A1:C44" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:C44" xr:uid="{A0B33C19-2877-43DA-A8B5-1F8EC96E5D8B}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A80168AA-523D-45E3-8F4C-4204320BF4B2}" name="Table"/>
     <tableColumn id="2" xr3:uid="{09BF1769-12E6-46DF-9C9C-263B496390D2}" name="State/Use"/>
@@ -10104,8 +10107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76451C41-9738-4BC1-978E-20A0DA8744C6}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10403,7 +10406,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="D2" sqref="D2:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10800,10 +10803,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A026136A-3463-4F46-9920-D2EEED3E1AFC}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10811,10 +10814,11 @@
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.85546875" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -10824,11 +10828,14 @@
       <c r="C1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="30" t="s">
+        <v>565</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>365</v>
       </c>
@@ -10838,9 +10845,12 @@
       <c r="C2" s="16" t="s">
         <v>514</v>
       </c>
-      <c r="D2" s="20"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="16">
+        <v>101901</v>
+      </c>
+      <c r="E2" s="20"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>370</v>
       </c>
@@ -10850,9 +10860,12 @@
       <c r="C3" s="14" t="s">
         <v>513</v>
       </c>
-      <c r="D3" s="21"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="14">
+        <v>100167</v>
+      </c>
+      <c r="E3" s="21"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>373</v>
       </c>
@@ -10862,9 +10875,12 @@
       <c r="C4" s="16" t="s">
         <v>522</v>
       </c>
-      <c r="D4" s="20"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="16">
+        <v>102341</v>
+      </c>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>376</v>
       </c>
@@ -10874,9 +10890,12 @@
       <c r="C5" s="14" t="s">
         <v>514</v>
       </c>
-      <c r="D5" s="21"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="14">
+        <v>101901</v>
+      </c>
+      <c r="E5" s="21"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>378</v>
       </c>
@@ -10886,9 +10905,12 @@
       <c r="C6" s="16" t="s">
         <v>513</v>
       </c>
-      <c r="D6" s="20"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="16">
+        <v>100167</v>
+      </c>
+      <c r="E6" s="20"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>380</v>
       </c>
@@ -10898,9 +10920,12 @@
       <c r="C7" s="14" t="s">
         <v>522</v>
       </c>
-      <c r="D7" s="21"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="14">
+        <v>102341</v>
+      </c>
+      <c r="E7" s="21"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>382</v>
       </c>
@@ -10910,9 +10935,12 @@
       <c r="C8" s="16" t="s">
         <v>514</v>
       </c>
-      <c r="D8" s="20"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="16">
+        <v>101901</v>
+      </c>
+      <c r="E8" s="20"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>384</v>
       </c>
@@ -10922,9 +10950,12 @@
       <c r="C9" s="14" t="s">
         <v>513</v>
       </c>
-      <c r="D9" s="21"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="14">
+        <v>100167</v>
+      </c>
+      <c r="E9" s="21"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>386</v>
       </c>
@@ -10934,19 +10965,23 @@
       <c r="C10" s="16" t="s">
         <v>522</v>
       </c>
-      <c r="D10" s="20"/>
+      <c r="D10" s="16">
+        <v>102341</v>
+      </c>
+      <c r="E10" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6DDA247-F6AE-445A-B41C-F6181C9C037C}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10968,39 +11003,39 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
         <v>110</v>
@@ -11008,39 +11043,39 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B9" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B11" t="s">
         <v>124</v>
@@ -11048,23 +11083,23 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B13" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B14" t="s">
         <v>131</v>
@@ -11072,39 +11107,39 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="B16" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B17" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B19" t="s">
         <v>164</v>
@@ -11112,23 +11147,23 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>178</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>179</v>
+        <v>166</v>
+      </c>
+      <c r="B20" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>181</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>179</v>
+        <v>168</v>
+      </c>
+      <c r="B21" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>179</v>
@@ -11136,71 +11171,71 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>194</v>
-      </c>
-      <c r="B25" t="s">
-        <v>195</v>
+        <v>185</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>197</v>
-      </c>
-      <c r="B26" t="s">
-        <v>195</v>
+        <v>188</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B27" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B28" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="B29" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="B30" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B31" t="s">
         <v>211</v>
@@ -11208,39 +11243,39 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="B32" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B33" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B34" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B35" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B36" t="s">
         <v>228</v>
@@ -11248,49 +11283,65 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>267</v>
+        <v>230</v>
       </c>
       <c r="B37" t="s">
-        <v>268</v>
+        <v>228</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>271</v>
+        <v>232</v>
       </c>
       <c r="B38" t="s">
-        <v>272</v>
+        <v>228</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="B39" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B40" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>477</v>
+        <v>275</v>
       </c>
       <c r="B41" t="s">
-        <v>478</v>
+        <v>276</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>279</v>
+      </c>
+      <c r="B42" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>477</v>
+      </c>
+      <c r="B43" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>480</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B44" t="s">
         <v>478</v>
       </c>
     </row>
@@ -11354,17 +11405,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -11373,7 +11413,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEAE28352B96D64C95AA0D5E2FA62FAD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed183881d36ac1b5d7d67982eda510d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d161086-4829-409f-9f75-5bde88dcb151" xmlns:ns3="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="685f4fda20cf913d28bf77c13cd653dd" ns2:_="" ns3:_="">
     <xsd:import namespace="3d161086-4829-409f-9f75-5bde88dcb151"/>
@@ -11596,24 +11636,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -11621,7 +11655,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C74AB5E7-5C87-4FF7-BF80-AB0EB6BD1D32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11638,4 +11672,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
UPLOAD_UTIL.parse_datatype_adcp hdr file done
</commit_message>
<xml_diff>
--- a/analysis/MEDS_Tables.xlsx
+++ b/analysis/MEDS_Tables.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="496" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AB7862E-602B-4D38-AC6E-E593ED46C186}"/>
+  <xr:revisionPtr revIDLastSave="501" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{5628A49D-3B55-489F-9BEB-596FCDE9380C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meds_tables" sheetId="1" r:id="rId1"/>
     <sheet name="csv" sheetId="6" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="10" r:id="rId3"/>
+    <sheet name="tasks" sheetId="10" r:id="rId3"/>
     <sheet name="form" sheetId="7" r:id="rId4"/>
     <sheet name="serd" sheetId="8" r:id="rId5"/>
     <sheet name="output" sheetId="9" r:id="rId6"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2522" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2524" uniqueCount="568">
   <si>
     <t>Table</t>
   </si>
@@ -2538,47 +2538,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="19" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2602,6 +2563,45 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -10328,7 +10328,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10388,8 +10388,8 @@
       <c r="B3" s="14" t="s">
         <v>536</v>
       </c>
-      <c r="C3" s="32">
-        <v>89</v>
+      <c r="C3" s="31">
+        <v>88</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>38</v>
@@ -10407,7 +10407,7 @@
         <v>537</v>
       </c>
       <c r="C4" s="31">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>38</v>
@@ -10638,14 +10638,14 @@
   <dimension ref="A1:I94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+      <selection activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" style="63" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="50" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="63.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -10678,581 +10678,585 @@
       <c r="A2" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39" t="s">
+      <c r="C2" s="57"/>
+      <c r="D2" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="61" t="s">
         <v>564</v>
       </c>
-      <c r="G2" s="41">
+      <c r="G2" s="62">
         <f>C94/C93</f>
-        <v>2.2727272727272728E-2</v>
-      </c>
-      <c r="H2" s="42" t="s">
+        <v>4.6511627906976744E-2</v>
+      </c>
+      <c r="H2" s="63" t="s">
         <v>566</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="46"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="42"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="55"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="46"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="42"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="55"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="63"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="55" t="s">
         <v>519</v>
       </c>
-      <c r="G5" s="41"/>
-      <c r="H5" s="42"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="63"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="46"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="55"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="46" t="s">
+      <c r="E7" s="55" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="46"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="55"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="51" t="s">
         <v>171</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45" t="s">
+      <c r="C9" s="53"/>
+      <c r="D9" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="46" t="s">
+      <c r="E9" s="55" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="46"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="55"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="46"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="55"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="38" t="s">
         <v>203</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="51" t="s">
         <v>204</v>
       </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45" t="s">
+      <c r="C12" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="46" t="s">
+      <c r="E12" s="55" t="s">
         <v>515</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="46"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="55"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="38" t="s">
         <v>360</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="51" t="s">
         <v>361</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45" t="s">
+      <c r="C14" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="46" t="s">
+      <c r="E14" s="55" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="39" t="s">
         <v>363</v>
       </c>
-      <c r="B15" s="48"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="50"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="56"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39" t="s">
+      <c r="C16" s="57"/>
+      <c r="D16" s="57" t="s">
         <v>567</v>
       </c>
-      <c r="E16" s="40" t="s">
+      <c r="E16" s="61" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="46"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="55"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45" t="s">
+      <c r="C18" s="53"/>
+      <c r="D18" s="53" t="s">
         <v>567</v>
       </c>
-      <c r="E18" s="46" t="s">
+      <c r="E18" s="55" t="s">
         <v>524</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="46"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="55"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="38" t="s">
         <v>299</v>
       </c>
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="51" t="s">
         <v>300</v>
       </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45" t="s">
+      <c r="C20" s="53"/>
+      <c r="D20" s="53" t="s">
         <v>567</v>
       </c>
-      <c r="E20" s="46" t="s">
+      <c r="E20" s="55" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="38" t="s">
         <v>302</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="46"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="55"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="38" t="s">
         <v>304</v>
       </c>
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="51" t="s">
         <v>305</v>
       </c>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45" t="s">
+      <c r="C22" s="53"/>
+      <c r="D22" s="53" t="s">
         <v>567</v>
       </c>
-      <c r="E22" s="46" t="s">
+      <c r="E22" s="55" t="s">
         <v>521</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="38" t="s">
         <v>309</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="46"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="55"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="38" t="s">
         <v>307</v>
       </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45" t="s">
+      <c r="B24" s="51"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53" t="s">
         <v>567</v>
       </c>
-      <c r="E24" s="46"/>
+      <c r="E24" s="55"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="38" t="s">
         <v>311</v>
       </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="46"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="55"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="43" t="s">
+      <c r="A26" s="38" t="s">
         <v>317</v>
       </c>
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="51" t="s">
         <v>318</v>
       </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45" t="s">
+      <c r="C26" s="53"/>
+      <c r="D26" s="53" t="s">
         <v>567</v>
       </c>
-      <c r="E26" s="46" t="s">
+      <c r="E26" s="55" t="s">
         <v>512</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="43" t="s">
+      <c r="A27" s="38" t="s">
         <v>320</v>
       </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="46"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="55"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="38" t="s">
         <v>322</v>
       </c>
-      <c r="B28" s="51" t="s">
+      <c r="B28" s="59" t="s">
         <v>323</v>
       </c>
-      <c r="C28" s="52"/>
-      <c r="D28" s="45" t="s">
+      <c r="C28" s="60"/>
+      <c r="D28" s="53" t="s">
         <v>567</v>
       </c>
-      <c r="E28" s="46" t="s">
+      <c r="E28" s="55" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="38" t="s">
         <v>325</v>
       </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="46"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="55"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="43" t="s">
+      <c r="A30" s="38" t="s">
         <v>327</v>
       </c>
-      <c r="B30" s="44" t="s">
+      <c r="B30" s="51" t="s">
         <v>328</v>
       </c>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45" t="s">
+      <c r="C30" s="53"/>
+      <c r="D30" s="53" t="s">
         <v>567</v>
       </c>
-      <c r="E30" s="46" t="s">
+      <c r="E30" s="55" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="38" t="s">
         <v>330</v>
       </c>
-      <c r="B31" s="44"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="46"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="55"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="38" t="s">
         <v>332</v>
       </c>
-      <c r="B32" s="44" t="s">
+      <c r="B32" s="51" t="s">
         <v>333</v>
       </c>
-      <c r="C32" s="45"/>
-      <c r="D32" s="45" t="s">
+      <c r="C32" s="53"/>
+      <c r="D32" s="53" t="s">
         <v>567</v>
       </c>
-      <c r="E32" s="46" t="s">
+      <c r="E32" s="55" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="43" t="s">
+      <c r="A33" s="38" t="s">
         <v>335</v>
       </c>
-      <c r="B33" s="44"/>
-      <c r="C33" s="45"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="46"/>
+      <c r="B33" s="51"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="55"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="43" t="s">
+      <c r="A34" s="38" t="s">
         <v>337</v>
       </c>
-      <c r="B34" s="44" t="s">
+      <c r="B34" s="51" t="s">
         <v>338</v>
       </c>
-      <c r="C34" s="45"/>
-      <c r="D34" s="45" t="s">
+      <c r="C34" s="53"/>
+      <c r="D34" s="53" t="s">
         <v>567</v>
       </c>
-      <c r="E34" s="46" t="s">
+      <c r="E34" s="55" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="43" t="s">
+      <c r="A35" s="38" t="s">
         <v>340</v>
       </c>
-      <c r="B35" s="44"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="46"/>
+      <c r="B35" s="51"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="55"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="38" t="s">
         <v>342</v>
       </c>
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="51" t="s">
         <v>343</v>
       </c>
-      <c r="C36" s="45"/>
-      <c r="D36" s="45" t="s">
+      <c r="C36" s="53"/>
+      <c r="D36" s="53" t="s">
         <v>567</v>
       </c>
-      <c r="E36" s="46" t="s">
+      <c r="E36" s="55" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="43" t="s">
+      <c r="A37" s="38" t="s">
         <v>345</v>
       </c>
-      <c r="B37" s="44"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="46"/>
+      <c r="B37" s="51"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="55"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="43" t="s">
+      <c r="A38" s="38" t="s">
         <v>347</v>
       </c>
-      <c r="B38" s="44" t="s">
+      <c r="B38" s="51" t="s">
         <v>348</v>
       </c>
-      <c r="C38" s="45"/>
-      <c r="D38" s="45" t="s">
+      <c r="C38" s="53"/>
+      <c r="D38" s="53" t="s">
         <v>567</v>
       </c>
-      <c r="E38" s="46" t="s">
+      <c r="E38" s="55" t="s">
         <v>520</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="47" t="s">
+      <c r="A39" s="39" t="s">
         <v>350</v>
       </c>
-      <c r="B39" s="48"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="50"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="56"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="37" t="s">
         <v>365</v>
       </c>
-      <c r="B40" s="53" t="s">
+      <c r="B40" s="40" t="s">
         <v>366</v>
       </c>
-      <c r="C40" s="54"/>
-      <c r="D40" s="39" t="s">
+      <c r="C40" s="41"/>
+      <c r="D40" s="57" t="s">
         <v>369</v>
       </c>
-      <c r="E40" s="55" t="s">
+      <c r="E40" s="42" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="43" t="s">
+      <c r="A41" s="38" t="s">
         <v>370</v>
       </c>
-      <c r="B41" s="56" t="s">
+      <c r="B41" s="43" t="s">
         <v>371</v>
       </c>
-      <c r="C41" s="57"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="58" t="s">
+      <c r="C41" s="44"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="45" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="38" t="s">
         <v>373</v>
       </c>
-      <c r="B42" s="56" t="s">
+      <c r="B42" s="43" t="s">
         <v>374</v>
       </c>
-      <c r="C42" s="57"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="58" t="s">
+      <c r="C42" s="44"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="45" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="38" t="s">
         <v>376</v>
       </c>
-      <c r="B43" s="56" t="s">
+      <c r="B43" s="43" t="s">
         <v>366</v>
       </c>
-      <c r="C43" s="57"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="58" t="s">
+      <c r="C43" s="44"/>
+      <c r="D43" s="53"/>
+      <c r="E43" s="45" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="43" t="s">
+      <c r="A44" s="38" t="s">
         <v>378</v>
       </c>
-      <c r="B44" s="56" t="s">
+      <c r="B44" s="43" t="s">
         <v>371</v>
       </c>
-      <c r="C44" s="57"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="58" t="s">
+      <c r="C44" s="44"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="45" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="43" t="s">
+      <c r="A45" s="38" t="s">
         <v>380</v>
       </c>
-      <c r="B45" s="56" t="s">
+      <c r="B45" s="43" t="s">
         <v>374</v>
       </c>
-      <c r="C45" s="57"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="58" t="s">
+      <c r="C45" s="44"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="45" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="43" t="s">
+      <c r="A46" s="38" t="s">
         <v>382</v>
       </c>
-      <c r="B46" s="56" t="s">
+      <c r="B46" s="43" t="s">
         <v>366</v>
       </c>
-      <c r="C46" s="57"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="58" t="s">
+      <c r="C46" s="44"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="45" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="43" t="s">
+      <c r="A47" s="38" t="s">
         <v>384</v>
       </c>
-      <c r="B47" s="56" t="s">
+      <c r="B47" s="43" t="s">
         <v>371</v>
       </c>
-      <c r="C47" s="57"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="58" t="s">
+      <c r="C47" s="44"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="45" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="43" t="s">
+      <c r="A48" s="38" t="s">
         <v>386</v>
       </c>
-      <c r="B48" s="56" t="s">
+      <c r="B48" s="43" t="s">
         <v>374</v>
       </c>
-      <c r="C48" s="57"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="58" t="s">
+      <c r="C48" s="44"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="45" t="s">
         <v>522</v>
       </c>
     </row>
@@ -11260,614 +11264,628 @@
       <c r="A49" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="38" t="s">
+      <c r="B49" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="C49" s="39"/>
-      <c r="D49" s="39" t="s">
+      <c r="C49" s="57"/>
+      <c r="D49" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="E49" s="59" t="s">
+      <c r="E49" s="46" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="43" t="s">
+      <c r="A50" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="44"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="60" t="s">
+      <c r="B50" s="51"/>
+      <c r="C50" s="53"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="43" t="s">
+      <c r="A51" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="B51" s="44" t="s">
+      <c r="B51" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="C51" s="45"/>
-      <c r="D51" s="45" t="s">
+      <c r="C51" s="53"/>
+      <c r="D51" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="E51" s="60" t="s">
+      <c r="E51" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="43" t="s">
+      <c r="A52" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B52" s="44"/>
-      <c r="C52" s="45"/>
-      <c r="D52" s="45"/>
-      <c r="E52" s="60" t="s">
+      <c r="B52" s="51"/>
+      <c r="C52" s="53"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="43" t="s">
+      <c r="A53" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="B53" s="44" t="s">
+      <c r="B53" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="C53" s="45"/>
-      <c r="D53" s="45" t="s">
+      <c r="C53" s="53"/>
+      <c r="D53" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="E53" s="60" t="s">
+      <c r="E53" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="43" t="s">
+      <c r="A54" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="B54" s="44"/>
-      <c r="C54" s="45"/>
-      <c r="D54" s="45"/>
-      <c r="E54" s="60" t="s">
+      <c r="B54" s="51"/>
+      <c r="C54" s="53"/>
+      <c r="D54" s="53"/>
+      <c r="E54" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="43" t="s">
+      <c r="A55" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="B55" s="44"/>
-      <c r="C55" s="45"/>
-      <c r="D55" s="45"/>
-      <c r="E55" s="60" t="s">
+      <c r="B55" s="51"/>
+      <c r="C55" s="53"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="43" t="s">
+      <c r="A56" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="B56" s="44" t="s">
+      <c r="B56" s="51" t="s">
         <v>119</v>
       </c>
-      <c r="C56" s="45"/>
-      <c r="D56" s="45" t="s">
+      <c r="C56" s="53"/>
+      <c r="D56" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="E56" s="60" t="s">
+      <c r="E56" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="43" t="s">
+      <c r="A57" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="B57" s="44"/>
-      <c r="C57" s="45"/>
-      <c r="D57" s="45"/>
-      <c r="E57" s="60" t="s">
+      <c r="B57" s="51"/>
+      <c r="C57" s="53"/>
+      <c r="D57" s="53"/>
+      <c r="E57" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="43" t="s">
+      <c r="A58" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="B58" s="44" t="s">
+      <c r="B58" s="51" t="s">
         <v>124</v>
       </c>
-      <c r="C58" s="45"/>
-      <c r="D58" s="45" t="s">
+      <c r="C58" s="53"/>
+      <c r="D58" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="60" t="s">
+      <c r="E58" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="43" t="s">
+      <c r="A59" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="B59" s="44"/>
-      <c r="C59" s="45"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="60" t="s">
+      <c r="B59" s="51"/>
+      <c r="C59" s="53"/>
+      <c r="D59" s="53"/>
+      <c r="E59" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="43" t="s">
+      <c r="A60" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="B60" s="44"/>
-      <c r="C60" s="45"/>
-      <c r="D60" s="45"/>
-      <c r="E60" s="60" t="s">
+      <c r="B60" s="51"/>
+      <c r="C60" s="53"/>
+      <c r="D60" s="53"/>
+      <c r="E60" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="43" t="s">
+      <c r="A61" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="B61" s="44" t="s">
+      <c r="B61" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="C61" s="45"/>
-      <c r="D61" s="45" t="s">
+      <c r="C61" s="53"/>
+      <c r="D61" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="E61" s="60" t="s">
+      <c r="E61" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="43" t="s">
+      <c r="A62" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="B62" s="44"/>
-      <c r="C62" s="45"/>
-      <c r="D62" s="45"/>
-      <c r="E62" s="60" t="s">
+      <c r="B62" s="51"/>
+      <c r="C62" s="53"/>
+      <c r="D62" s="53"/>
+      <c r="E62" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="43" t="s">
+      <c r="A63" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="B63" s="44"/>
-      <c r="C63" s="45"/>
-      <c r="D63" s="45"/>
-      <c r="E63" s="60" t="s">
+      <c r="B63" s="51"/>
+      <c r="C63" s="53"/>
+      <c r="D63" s="53"/>
+      <c r="E63" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="43" t="s">
+      <c r="A64" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="B64" s="44" t="s">
+      <c r="B64" s="51" t="s">
         <v>159</v>
       </c>
-      <c r="C64" s="45"/>
-      <c r="D64" s="45" t="s">
+      <c r="C64" s="53"/>
+      <c r="D64" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="E64" s="60" t="s">
+      <c r="E64" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="43" t="s">
+      <c r="A65" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="B65" s="44"/>
-      <c r="C65" s="45"/>
-      <c r="D65" s="45"/>
-      <c r="E65" s="60" t="s">
+      <c r="B65" s="51"/>
+      <c r="C65" s="53"/>
+      <c r="D65" s="53"/>
+      <c r="E65" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="43" t="s">
+      <c r="A66" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="B66" s="44" t="s">
+      <c r="B66" s="51" t="s">
         <v>164</v>
       </c>
-      <c r="C66" s="45"/>
-      <c r="D66" s="45" t="s">
+      <c r="C66" s="53"/>
+      <c r="D66" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="E66" s="60" t="s">
+      <c r="E66" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="43" t="s">
+      <c r="A67" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="B67" s="44"/>
-      <c r="C67" s="45"/>
-      <c r="D67" s="45"/>
-      <c r="E67" s="60" t="s">
+      <c r="B67" s="51"/>
+      <c r="C67" s="53"/>
+      <c r="D67" s="53"/>
+      <c r="E67" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="43" t="s">
+      <c r="A68" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="B68" s="44"/>
-      <c r="C68" s="45"/>
-      <c r="D68" s="45"/>
-      <c r="E68" s="60" t="s">
+      <c r="B68" s="51"/>
+      <c r="C68" s="53"/>
+      <c r="D68" s="53"/>
+      <c r="E68" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="43" t="s">
+      <c r="A69" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="B69" s="44" t="s">
+      <c r="B69" s="51" t="s">
         <v>179</v>
       </c>
-      <c r="C69" s="45"/>
-      <c r="D69" s="45" t="s">
+      <c r="C69" s="53"/>
+      <c r="D69" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="E69" s="60" t="s">
+      <c r="E69" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="43" t="s">
+      <c r="A70" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="B70" s="44"/>
-      <c r="C70" s="45"/>
-      <c r="D70" s="45"/>
-      <c r="E70" s="60" t="s">
+      <c r="B70" s="51"/>
+      <c r="C70" s="53"/>
+      <c r="D70" s="53"/>
+      <c r="E70" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="43" t="s">
+      <c r="A71" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="B71" s="44"/>
-      <c r="C71" s="45"/>
-      <c r="D71" s="45"/>
-      <c r="E71" s="60" t="s">
+      <c r="B71" s="51"/>
+      <c r="C71" s="53"/>
+      <c r="D71" s="53"/>
+      <c r="E71" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="43" t="s">
+      <c r="A72" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="B72" s="44" t="s">
+      <c r="B72" s="51" t="s">
         <v>186</v>
       </c>
-      <c r="C72" s="45"/>
-      <c r="D72" s="45" t="s">
+      <c r="C72" s="53"/>
+      <c r="D72" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="E72" s="60" t="s">
+      <c r="E72" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="43" t="s">
+      <c r="A73" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="B73" s="44"/>
-      <c r="C73" s="45"/>
-      <c r="D73" s="45"/>
-      <c r="E73" s="60" t="s">
+      <c r="B73" s="51"/>
+      <c r="C73" s="53"/>
+      <c r="D73" s="53"/>
+      <c r="E73" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="43" t="s">
+      <c r="A74" s="38" t="s">
         <v>194</v>
       </c>
-      <c r="B74" s="44" t="s">
+      <c r="B74" s="51" t="s">
         <v>195</v>
       </c>
-      <c r="C74" s="45"/>
-      <c r="D74" s="45" t="s">
+      <c r="C74" s="53"/>
+      <c r="D74" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="E74" s="60" t="s">
+      <c r="E74" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="43" t="s">
+      <c r="A75" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="B75" s="44"/>
-      <c r="C75" s="45"/>
-      <c r="D75" s="45"/>
-      <c r="E75" s="60" t="s">
+      <c r="B75" s="51"/>
+      <c r="C75" s="53"/>
+      <c r="D75" s="53"/>
+      <c r="E75" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="43" t="s">
+      <c r="A76" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="B76" s="44" t="s">
+      <c r="B76" s="51" t="s">
         <v>200</v>
       </c>
-      <c r="C76" s="45"/>
-      <c r="D76" s="45" t="s">
+      <c r="C76" s="53"/>
+      <c r="D76" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="E76" s="60" t="s">
+      <c r="E76" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="43" t="s">
+      <c r="A77" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="B77" s="44"/>
-      <c r="C77" s="45"/>
-      <c r="D77" s="45"/>
-      <c r="E77" s="60" t="s">
+      <c r="B77" s="51"/>
+      <c r="C77" s="53"/>
+      <c r="D77" s="53"/>
+      <c r="E77" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="43" t="s">
+      <c r="A78" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="B78" s="44" t="s">
+      <c r="B78" s="51" t="s">
         <v>211</v>
       </c>
-      <c r="C78" s="45"/>
-      <c r="D78" s="45" t="s">
+      <c r="C78" s="53"/>
+      <c r="D78" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="E78" s="60" t="s">
+      <c r="E78" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="43" t="s">
+      <c r="A79" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="B79" s="44"/>
-      <c r="C79" s="45"/>
-      <c r="D79" s="45"/>
-      <c r="E79" s="60" t="s">
+      <c r="B79" s="51"/>
+      <c r="C79" s="53"/>
+      <c r="D79" s="53"/>
+      <c r="E79" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="43" t="s">
+      <c r="A80" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="B80" s="44"/>
-      <c r="C80" s="45"/>
-      <c r="D80" s="45"/>
-      <c r="E80" s="60" t="s">
+      <c r="B80" s="51"/>
+      <c r="C80" s="53"/>
+      <c r="D80" s="53"/>
+      <c r="E80" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="43" t="s">
+      <c r="A81" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="B81" s="44" t="s">
+      <c r="B81" s="51" t="s">
         <v>223</v>
       </c>
-      <c r="C81" s="45"/>
-      <c r="D81" s="45" t="s">
+      <c r="C81" s="53"/>
+      <c r="D81" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="E81" s="60" t="s">
+      <c r="E81" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="43" t="s">
+      <c r="A82" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="B82" s="44"/>
-      <c r="C82" s="45"/>
-      <c r="D82" s="45"/>
-      <c r="E82" s="60" t="s">
+      <c r="B82" s="51"/>
+      <c r="C82" s="53"/>
+      <c r="D82" s="53"/>
+      <c r="E82" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="43" t="s">
+      <c r="A83" s="38" t="s">
         <v>227</v>
       </c>
-      <c r="B83" s="44" t="s">
+      <c r="B83" s="51" t="s">
         <v>228</v>
       </c>
-      <c r="C83" s="45"/>
-      <c r="D83" s="45" t="s">
+      <c r="C83" s="53"/>
+      <c r="D83" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="E83" s="60" t="s">
+      <c r="E83" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="43" t="s">
+      <c r="A84" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="B84" s="44"/>
-      <c r="C84" s="45"/>
-      <c r="D84" s="45"/>
-      <c r="E84" s="60" t="s">
+      <c r="B84" s="51"/>
+      <c r="C84" s="53"/>
+      <c r="D84" s="53"/>
+      <c r="E84" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="43" t="s">
+      <c r="A85" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="B85" s="44"/>
-      <c r="C85" s="45"/>
-      <c r="D85" s="45"/>
-      <c r="E85" s="60" t="s">
+      <c r="B85" s="51"/>
+      <c r="C85" s="53"/>
+      <c r="D85" s="53"/>
+      <c r="E85" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="43" t="s">
+      <c r="A86" s="38" t="s">
         <v>267</v>
       </c>
-      <c r="B86" s="61" t="s">
+      <c r="B86" s="48" t="s">
         <v>268</v>
       </c>
-      <c r="C86" s="57"/>
-      <c r="D86" s="57" t="s">
+      <c r="C86" s="44"/>
+      <c r="D86" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="E86" s="60" t="s">
+      <c r="E86" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="43" t="s">
+      <c r="A87" s="38" t="s">
         <v>271</v>
       </c>
-      <c r="B87" s="61" t="s">
+      <c r="B87" s="48" t="s">
         <v>272</v>
       </c>
-      <c r="C87" s="57"/>
-      <c r="D87" s="57" t="s">
+      <c r="C87" s="44"/>
+      <c r="D87" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="E87" s="60" t="s">
+      <c r="E87" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="43" t="s">
+      <c r="A88" s="38" t="s">
         <v>275</v>
       </c>
-      <c r="B88" s="61" t="s">
+      <c r="B88" s="48" t="s">
         <v>276</v>
       </c>
-      <c r="C88" s="57"/>
-      <c r="D88" s="57" t="s">
+      <c r="C88" s="44"/>
+      <c r="D88" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="E88" s="60" t="s">
+      <c r="E88" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="43" t="s">
+      <c r="A89" s="38" t="s">
         <v>279</v>
       </c>
-      <c r="B89" s="61" t="s">
+      <c r="B89" s="48" t="s">
         <v>280</v>
       </c>
-      <c r="C89" s="57"/>
-      <c r="D89" s="57" t="s">
+      <c r="C89" s="44"/>
+      <c r="D89" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="E89" s="60" t="s">
+      <c r="E89" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="43" t="s">
+      <c r="A90" s="38" t="s">
         <v>477</v>
       </c>
-      <c r="B90" s="44" t="s">
+      <c r="B90" s="51" t="s">
         <v>478</v>
       </c>
-      <c r="C90" s="45"/>
-      <c r="D90" s="45" t="s">
+      <c r="C90" s="53"/>
+      <c r="D90" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="E90" s="60" t="s">
+      <c r="E90" s="47" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="47" t="s">
+      <c r="A91" s="39" t="s">
         <v>480</v>
       </c>
-      <c r="B91" s="48"/>
-      <c r="C91" s="49"/>
-      <c r="D91" s="49"/>
-      <c r="E91" s="62" t="s">
+      <c r="B91" s="52"/>
+      <c r="C91" s="54"/>
+      <c r="D91" s="54"/>
+      <c r="E91" s="49" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C93" s="63">
+      <c r="C93" s="50">
         <f>COUNTBLANK(C2:C91)</f>
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C94" s="63">
+      <c r="C94" s="50">
         <f>COUNTA(C2:C91)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="120">
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="D90:D91"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="D83:D85"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="C78:C80"/>
-    <mergeCell ref="D78:D80"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="C66:C68"/>
-    <mergeCell ref="D66:D68"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="C69:C71"/>
-    <mergeCell ref="D69:D71"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="C61:C63"/>
-    <mergeCell ref="D61:D63"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="D58:D60"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="D38:D39"/>
@@ -11884,65 +11902,51 @@
     <mergeCell ref="C36:C37"/>
     <mergeCell ref="D36:D37"/>
     <mergeCell ref="E36:E37"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="D58:D60"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="C66:C68"/>
+    <mergeCell ref="D66:D68"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="C69:C71"/>
+    <mergeCell ref="D69:D71"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="C61:C63"/>
+    <mergeCell ref="D61:D63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="C78:C80"/>
+    <mergeCell ref="D78:D80"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="D90:D91"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="D83:D85"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12952,14 +12956,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13186,27 +13188,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
-    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13231,9 +13226,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Front satellite observation done
</commit_message>
<xml_diff>
--- a/analysis/MEDS_Tables.xlsx
+++ b/analysis/MEDS_Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="501" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{5628A49D-3B55-489F-9BEB-596FCDE9380C}"/>
+  <xr:revisionPtr revIDLastSave="502" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3E0A762-8083-4E80-A748-BE7F4F206F70}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meds_tables" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2524" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2525" uniqueCount="568">
   <si>
     <t>Table</t>
   </si>
@@ -2565,43 +2565,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="19" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="19" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -10327,7 +10327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76451C41-9738-4BC1-978E-20A0DA8744C6}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -10637,8 +10637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8FA477-9B46-4053-B7AD-310B8B9F2B30}">
   <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10678,21 +10678,23 @@
       <c r="A2" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="57"/>
+      <c r="C2" s="57" t="s">
+        <v>81</v>
+      </c>
       <c r="D2" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="61" t="s">
+      <c r="E2" s="58" t="s">
         <v>564</v>
       </c>
-      <c r="G2" s="62">
+      <c r="G2" s="51">
         <f>C94/C93</f>
-        <v>4.6511627906976744E-2</v>
-      </c>
-      <c r="H2" s="63" t="s">
+        <v>5.8823529411764705E-2</v>
+      </c>
+      <c r="H2" s="52" t="s">
         <v>566</v>
       </c>
     </row>
@@ -10700,63 +10702,63 @@
       <c r="A3" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
       <c r="E3" s="55"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="52"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
       <c r="E4" s="55"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="63"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="52"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="54" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="55" t="s">
         <v>519</v>
       </c>
-      <c r="G5" s="62"/>
-      <c r="H5" s="63"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="52"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
       <c r="E6" s="55"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="53" t="s">
+      <c r="D7" s="54" t="s">
         <v>42</v>
       </c>
       <c r="E7" s="55" t="s">
@@ -10767,20 +10769,20 @@
       <c r="A8" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="51"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
       <c r="E8" s="55"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="53" t="s">
         <v>171</v>
       </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53" t="s">
+      <c r="C9" s="54"/>
+      <c r="D9" s="54" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="55" t="s">
@@ -10791,31 +10793,31 @@
       <c r="A10" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
       <c r="E10" s="55"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
       <c r="E11" s="55"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
         <v>203</v>
       </c>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="53" t="s">
         <v>204</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="53" t="s">
+      <c r="D12" s="54" t="s">
         <v>42</v>
       </c>
       <c r="E12" s="55" t="s">
@@ -10826,22 +10828,22 @@
       <c r="A13" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
       <c r="E13" s="55"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
         <v>360</v>
       </c>
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="53" t="s">
         <v>361</v>
       </c>
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="53" t="s">
+      <c r="D14" s="54" t="s">
         <v>42</v>
       </c>
       <c r="E14" s="55" t="s">
@@ -10852,23 +10854,23 @@
       <c r="A15" s="39" t="s">
         <v>363</v>
       </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="56"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="61"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="56" t="s">
         <v>71</v>
       </c>
       <c r="C16" s="57"/>
       <c r="D16" s="57" t="s">
         <v>567</v>
       </c>
-      <c r="E16" s="61" t="s">
+      <c r="E16" s="58" t="s">
         <v>73</v>
       </c>
     </row>
@@ -10876,20 +10878,20 @@
       <c r="A17" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
       <c r="E17" s="55"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53" t="s">
+      <c r="C18" s="54"/>
+      <c r="D18" s="54" t="s">
         <v>567</v>
       </c>
       <c r="E18" s="55" t="s">
@@ -10900,20 +10902,20 @@
       <c r="A19" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="B19" s="51"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
       <c r="E19" s="55"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
         <v>299</v>
       </c>
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="53" t="s">
         <v>300</v>
       </c>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53" t="s">
+      <c r="C20" s="54"/>
+      <c r="D20" s="54" t="s">
         <v>567</v>
       </c>
       <c r="E20" s="55" t="s">
@@ -10924,20 +10926,20 @@
       <c r="A21" s="38" t="s">
         <v>302</v>
       </c>
-      <c r="B21" s="51"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
       <c r="E21" s="55"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="38" t="s">
         <v>304</v>
       </c>
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="53" t="s">
         <v>305</v>
       </c>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53" t="s">
+      <c r="C22" s="54"/>
+      <c r="D22" s="54" t="s">
         <v>567</v>
       </c>
       <c r="E22" s="55" t="s">
@@ -10948,18 +10950,18 @@
       <c r="A23" s="38" t="s">
         <v>309</v>
       </c>
-      <c r="B23" s="51"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
       <c r="E23" s="55"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="38" t="s">
         <v>307</v>
       </c>
-      <c r="B24" s="51"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53" t="s">
+      <c r="B24" s="53"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54" t="s">
         <v>567</v>
       </c>
       <c r="E24" s="55"/>
@@ -10968,20 +10970,20 @@
       <c r="A25" s="38" t="s">
         <v>311</v>
       </c>
-      <c r="B25" s="51"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
       <c r="E25" s="55"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="38" t="s">
         <v>317</v>
       </c>
-      <c r="B26" s="51" t="s">
+      <c r="B26" s="53" t="s">
         <v>318</v>
       </c>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53" t="s">
+      <c r="C26" s="54"/>
+      <c r="D26" s="54" t="s">
         <v>567</v>
       </c>
       <c r="E26" s="55" t="s">
@@ -10992,20 +10994,20 @@
       <c r="A27" s="38" t="s">
         <v>320</v>
       </c>
-      <c r="B27" s="51"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
       <c r="E27" s="55"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="38" t="s">
         <v>322</v>
       </c>
-      <c r="B28" s="59" t="s">
+      <c r="B28" s="62" t="s">
         <v>323</v>
       </c>
-      <c r="C28" s="60"/>
-      <c r="D28" s="53" t="s">
+      <c r="C28" s="63"/>
+      <c r="D28" s="54" t="s">
         <v>567</v>
       </c>
       <c r="E28" s="55" t="s">
@@ -11016,20 +11018,20 @@
       <c r="A29" s="38" t="s">
         <v>325</v>
       </c>
-      <c r="B29" s="59"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="53"/>
+      <c r="B29" s="62"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="54"/>
       <c r="E29" s="55"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="38" t="s">
         <v>327</v>
       </c>
-      <c r="B30" s="51" t="s">
+      <c r="B30" s="53" t="s">
         <v>328</v>
       </c>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53" t="s">
+      <c r="C30" s="54"/>
+      <c r="D30" s="54" t="s">
         <v>567</v>
       </c>
       <c r="E30" s="55" t="s">
@@ -11040,20 +11042,20 @@
       <c r="A31" s="38" t="s">
         <v>330</v>
       </c>
-      <c r="B31" s="51"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
       <c r="E31" s="55"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="38" t="s">
         <v>332</v>
       </c>
-      <c r="B32" s="51" t="s">
+      <c r="B32" s="53" t="s">
         <v>333</v>
       </c>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53" t="s">
+      <c r="C32" s="54"/>
+      <c r="D32" s="54" t="s">
         <v>567</v>
       </c>
       <c r="E32" s="55" t="s">
@@ -11064,20 +11066,20 @@
       <c r="A33" s="38" t="s">
         <v>335</v>
       </c>
-      <c r="B33" s="51"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
       <c r="E33" s="55"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="38" t="s">
         <v>337</v>
       </c>
-      <c r="B34" s="51" t="s">
+      <c r="B34" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="C34" s="53"/>
-      <c r="D34" s="53" t="s">
+      <c r="C34" s="54"/>
+      <c r="D34" s="54" t="s">
         <v>567</v>
       </c>
       <c r="E34" s="55" t="s">
@@ -11088,20 +11090,20 @@
       <c r="A35" s="38" t="s">
         <v>340</v>
       </c>
-      <c r="B35" s="51"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
+      <c r="B35" s="53"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
       <c r="E35" s="55"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="38" t="s">
         <v>342</v>
       </c>
-      <c r="B36" s="51" t="s">
+      <c r="B36" s="53" t="s">
         <v>343</v>
       </c>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53" t="s">
+      <c r="C36" s="54"/>
+      <c r="D36" s="54" t="s">
         <v>567</v>
       </c>
       <c r="E36" s="55" t="s">
@@ -11112,20 +11114,20 @@
       <c r="A37" s="38" t="s">
         <v>345</v>
       </c>
-      <c r="B37" s="51"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
+      <c r="B37" s="53"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
       <c r="E37" s="55"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="38" t="s">
         <v>347</v>
       </c>
-      <c r="B38" s="51" t="s">
+      <c r="B38" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53" t="s">
+      <c r="C38" s="54"/>
+      <c r="D38" s="54" t="s">
         <v>567</v>
       </c>
       <c r="E38" s="55" t="s">
@@ -11136,10 +11138,10 @@
       <c r="A39" s="39" t="s">
         <v>350</v>
       </c>
-      <c r="B39" s="52"/>
-      <c r="C39" s="54"/>
-      <c r="D39" s="54"/>
-      <c r="E39" s="56"/>
+      <c r="B39" s="59"/>
+      <c r="C39" s="60"/>
+      <c r="D39" s="60"/>
+      <c r="E39" s="61"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="37" t="s">
@@ -11164,7 +11166,7 @@
         <v>371</v>
       </c>
       <c r="C41" s="44"/>
-      <c r="D41" s="53"/>
+      <c r="D41" s="54"/>
       <c r="E41" s="45" t="s">
         <v>513</v>
       </c>
@@ -11177,7 +11179,7 @@
         <v>374</v>
       </c>
       <c r="C42" s="44"/>
-      <c r="D42" s="53"/>
+      <c r="D42" s="54"/>
       <c r="E42" s="45" t="s">
         <v>522</v>
       </c>
@@ -11190,7 +11192,7 @@
         <v>366</v>
       </c>
       <c r="C43" s="44"/>
-      <c r="D43" s="53"/>
+      <c r="D43" s="54"/>
       <c r="E43" s="45" t="s">
         <v>514</v>
       </c>
@@ -11203,7 +11205,7 @@
         <v>371</v>
       </c>
       <c r="C44" s="44"/>
-      <c r="D44" s="53"/>
+      <c r="D44" s="54"/>
       <c r="E44" s="45" t="s">
         <v>513</v>
       </c>
@@ -11216,7 +11218,7 @@
         <v>374</v>
       </c>
       <c r="C45" s="44"/>
-      <c r="D45" s="53"/>
+      <c r="D45" s="54"/>
       <c r="E45" s="45" t="s">
         <v>522</v>
       </c>
@@ -11229,7 +11231,7 @@
         <v>366</v>
       </c>
       <c r="C46" s="44"/>
-      <c r="D46" s="53"/>
+      <c r="D46" s="54"/>
       <c r="E46" s="45" t="s">
         <v>514</v>
       </c>
@@ -11242,7 +11244,7 @@
         <v>371</v>
       </c>
       <c r="C47" s="44"/>
-      <c r="D47" s="53"/>
+      <c r="D47" s="54"/>
       <c r="E47" s="45" t="s">
         <v>513</v>
       </c>
@@ -11255,7 +11257,7 @@
         <v>374</v>
       </c>
       <c r="C48" s="44"/>
-      <c r="D48" s="53"/>
+      <c r="D48" s="54"/>
       <c r="E48" s="45" t="s">
         <v>522</v>
       </c>
@@ -11264,7 +11266,7 @@
       <c r="A49" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="58" t="s">
+      <c r="B49" s="56" t="s">
         <v>48</v>
       </c>
       <c r="C49" s="57"/>
@@ -11279,9 +11281,9 @@
       <c r="A50" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="51"/>
-      <c r="C50" s="53"/>
-      <c r="D50" s="53"/>
+      <c r="B50" s="53"/>
+      <c r="C50" s="54"/>
+      <c r="D50" s="54"/>
       <c r="E50" s="47" t="s">
         <v>33</v>
       </c>
@@ -11290,11 +11292,11 @@
       <c r="A51" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="B51" s="51" t="s">
+      <c r="B51" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="C51" s="53"/>
-      <c r="D51" s="53" t="s">
+      <c r="C51" s="54"/>
+      <c r="D51" s="54" t="s">
         <v>18</v>
       </c>
       <c r="E51" s="47" t="s">
@@ -11305,9 +11307,9 @@
       <c r="A52" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B52" s="51"/>
-      <c r="C52" s="53"/>
-      <c r="D52" s="53"/>
+      <c r="B52" s="53"/>
+      <c r="C52" s="54"/>
+      <c r="D52" s="54"/>
       <c r="E52" s="47" t="s">
         <v>33</v>
       </c>
@@ -11316,11 +11318,11 @@
       <c r="A53" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="B53" s="51" t="s">
+      <c r="B53" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="C53" s="53"/>
-      <c r="D53" s="53" t="s">
+      <c r="C53" s="54"/>
+      <c r="D53" s="54" t="s">
         <v>18</v>
       </c>
       <c r="E53" s="47" t="s">
@@ -11331,9 +11333,9 @@
       <c r="A54" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="B54" s="51"/>
-      <c r="C54" s="53"/>
-      <c r="D54" s="53"/>
+      <c r="B54" s="53"/>
+      <c r="C54" s="54"/>
+      <c r="D54" s="54"/>
       <c r="E54" s="47" t="s">
         <v>33</v>
       </c>
@@ -11342,9 +11344,9 @@
       <c r="A55" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="B55" s="51"/>
-      <c r="C55" s="53"/>
-      <c r="D55" s="53"/>
+      <c r="B55" s="53"/>
+      <c r="C55" s="54"/>
+      <c r="D55" s="54"/>
       <c r="E55" s="47" t="s">
         <v>33</v>
       </c>
@@ -11353,11 +11355,11 @@
       <c r="A56" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="B56" s="51" t="s">
+      <c r="B56" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="C56" s="53"/>
-      <c r="D56" s="53" t="s">
+      <c r="C56" s="54"/>
+      <c r="D56" s="54" t="s">
         <v>18</v>
       </c>
       <c r="E56" s="47" t="s">
@@ -11368,9 +11370,9 @@
       <c r="A57" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="B57" s="51"/>
-      <c r="C57" s="53"/>
-      <c r="D57" s="53"/>
+      <c r="B57" s="53"/>
+      <c r="C57" s="54"/>
+      <c r="D57" s="54"/>
       <c r="E57" s="47" t="s">
         <v>33</v>
       </c>
@@ -11379,11 +11381,11 @@
       <c r="A58" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="B58" s="51" t="s">
+      <c r="B58" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="C58" s="53"/>
-      <c r="D58" s="53" t="s">
+      <c r="C58" s="54"/>
+      <c r="D58" s="54" t="s">
         <v>18</v>
       </c>
       <c r="E58" s="47" t="s">
@@ -11394,9 +11396,9 @@
       <c r="A59" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="B59" s="51"/>
-      <c r="C59" s="53"/>
-      <c r="D59" s="53"/>
+      <c r="B59" s="53"/>
+      <c r="C59" s="54"/>
+      <c r="D59" s="54"/>
       <c r="E59" s="47" t="s">
         <v>33</v>
       </c>
@@ -11405,9 +11407,9 @@
       <c r="A60" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="B60" s="51"/>
-      <c r="C60" s="53"/>
-      <c r="D60" s="53"/>
+      <c r="B60" s="53"/>
+      <c r="C60" s="54"/>
+      <c r="D60" s="54"/>
       <c r="E60" s="47" t="s">
         <v>33</v>
       </c>
@@ -11416,11 +11418,11 @@
       <c r="A61" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="B61" s="51" t="s">
+      <c r="B61" s="53" t="s">
         <v>131</v>
       </c>
-      <c r="C61" s="53"/>
-      <c r="D61" s="53" t="s">
+      <c r="C61" s="54"/>
+      <c r="D61" s="54" t="s">
         <v>18</v>
       </c>
       <c r="E61" s="47" t="s">
@@ -11431,9 +11433,9 @@
       <c r="A62" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="B62" s="51"/>
-      <c r="C62" s="53"/>
-      <c r="D62" s="53"/>
+      <c r="B62" s="53"/>
+      <c r="C62" s="54"/>
+      <c r="D62" s="54"/>
       <c r="E62" s="47" t="s">
         <v>33</v>
       </c>
@@ -11442,9 +11444,9 @@
       <c r="A63" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="B63" s="51"/>
-      <c r="C63" s="53"/>
-      <c r="D63" s="53"/>
+      <c r="B63" s="53"/>
+      <c r="C63" s="54"/>
+      <c r="D63" s="54"/>
       <c r="E63" s="47" t="s">
         <v>33</v>
       </c>
@@ -11453,11 +11455,11 @@
       <c r="A64" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="B64" s="51" t="s">
+      <c r="B64" s="53" t="s">
         <v>159</v>
       </c>
-      <c r="C64" s="53"/>
-      <c r="D64" s="53" t="s">
+      <c r="C64" s="54"/>
+      <c r="D64" s="54" t="s">
         <v>18</v>
       </c>
       <c r="E64" s="47" t="s">
@@ -11468,9 +11470,9 @@
       <c r="A65" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="B65" s="51"/>
-      <c r="C65" s="53"/>
-      <c r="D65" s="53"/>
+      <c r="B65" s="53"/>
+      <c r="C65" s="54"/>
+      <c r="D65" s="54"/>
       <c r="E65" s="47" t="s">
         <v>33</v>
       </c>
@@ -11479,11 +11481,11 @@
       <c r="A66" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="B66" s="51" t="s">
+      <c r="B66" s="53" t="s">
         <v>164</v>
       </c>
-      <c r="C66" s="53"/>
-      <c r="D66" s="53" t="s">
+      <c r="C66" s="54"/>
+      <c r="D66" s="54" t="s">
         <v>18</v>
       </c>
       <c r="E66" s="47" t="s">
@@ -11494,9 +11496,9 @@
       <c r="A67" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="B67" s="51"/>
-      <c r="C67" s="53"/>
-      <c r="D67" s="53"/>
+      <c r="B67" s="53"/>
+      <c r="C67" s="54"/>
+      <c r="D67" s="54"/>
       <c r="E67" s="47" t="s">
         <v>33</v>
       </c>
@@ -11505,9 +11507,9 @@
       <c r="A68" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="B68" s="51"/>
-      <c r="C68" s="53"/>
-      <c r="D68" s="53"/>
+      <c r="B68" s="53"/>
+      <c r="C68" s="54"/>
+      <c r="D68" s="54"/>
       <c r="E68" s="47" t="s">
         <v>33</v>
       </c>
@@ -11516,11 +11518,11 @@
       <c r="A69" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="B69" s="51" t="s">
+      <c r="B69" s="53" t="s">
         <v>179</v>
       </c>
-      <c r="C69" s="53"/>
-      <c r="D69" s="53" t="s">
+      <c r="C69" s="54"/>
+      <c r="D69" s="54" t="s">
         <v>18</v>
       </c>
       <c r="E69" s="47" t="s">
@@ -11531,9 +11533,9 @@
       <c r="A70" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="B70" s="51"/>
-      <c r="C70" s="53"/>
-      <c r="D70" s="53"/>
+      <c r="B70" s="53"/>
+      <c r="C70" s="54"/>
+      <c r="D70" s="54"/>
       <c r="E70" s="47" t="s">
         <v>33</v>
       </c>
@@ -11542,9 +11544,9 @@
       <c r="A71" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="B71" s="51"/>
-      <c r="C71" s="53"/>
-      <c r="D71" s="53"/>
+      <c r="B71" s="53"/>
+      <c r="C71" s="54"/>
+      <c r="D71" s="54"/>
       <c r="E71" s="47" t="s">
         <v>33</v>
       </c>
@@ -11553,11 +11555,11 @@
       <c r="A72" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="B72" s="51" t="s">
+      <c r="B72" s="53" t="s">
         <v>186</v>
       </c>
-      <c r="C72" s="53"/>
-      <c r="D72" s="53" t="s">
+      <c r="C72" s="54"/>
+      <c r="D72" s="54" t="s">
         <v>18</v>
       </c>
       <c r="E72" s="47" t="s">
@@ -11568,9 +11570,9 @@
       <c r="A73" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="B73" s="51"/>
-      <c r="C73" s="53"/>
-      <c r="D73" s="53"/>
+      <c r="B73" s="53"/>
+      <c r="C73" s="54"/>
+      <c r="D73" s="54"/>
       <c r="E73" s="47" t="s">
         <v>33</v>
       </c>
@@ -11579,11 +11581,11 @@
       <c r="A74" s="38" t="s">
         <v>194</v>
       </c>
-      <c r="B74" s="51" t="s">
+      <c r="B74" s="53" t="s">
         <v>195</v>
       </c>
-      <c r="C74" s="53"/>
-      <c r="D74" s="53" t="s">
+      <c r="C74" s="54"/>
+      <c r="D74" s="54" t="s">
         <v>18</v>
       </c>
       <c r="E74" s="47" t="s">
@@ -11594,9 +11596,9 @@
       <c r="A75" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="B75" s="51"/>
-      <c r="C75" s="53"/>
-      <c r="D75" s="53"/>
+      <c r="B75" s="53"/>
+      <c r="C75" s="54"/>
+      <c r="D75" s="54"/>
       <c r="E75" s="47" t="s">
         <v>33</v>
       </c>
@@ -11605,11 +11607,11 @@
       <c r="A76" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="B76" s="51" t="s">
+      <c r="B76" s="53" t="s">
         <v>200</v>
       </c>
-      <c r="C76" s="53"/>
-      <c r="D76" s="53" t="s">
+      <c r="C76" s="54"/>
+      <c r="D76" s="54" t="s">
         <v>18</v>
       </c>
       <c r="E76" s="47" t="s">
@@ -11620,9 +11622,9 @@
       <c r="A77" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="B77" s="51"/>
-      <c r="C77" s="53"/>
-      <c r="D77" s="53"/>
+      <c r="B77" s="53"/>
+      <c r="C77" s="54"/>
+      <c r="D77" s="54"/>
       <c r="E77" s="47" t="s">
         <v>33</v>
       </c>
@@ -11631,11 +11633,11 @@
       <c r="A78" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="B78" s="51" t="s">
+      <c r="B78" s="53" t="s">
         <v>211</v>
       </c>
-      <c r="C78" s="53"/>
-      <c r="D78" s="53" t="s">
+      <c r="C78" s="54"/>
+      <c r="D78" s="54" t="s">
         <v>18</v>
       </c>
       <c r="E78" s="47" t="s">
@@ -11646,9 +11648,9 @@
       <c r="A79" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="B79" s="51"/>
-      <c r="C79" s="53"/>
-      <c r="D79" s="53"/>
+      <c r="B79" s="53"/>
+      <c r="C79" s="54"/>
+      <c r="D79" s="54"/>
       <c r="E79" s="47" t="s">
         <v>33</v>
       </c>
@@ -11657,9 +11659,9 @@
       <c r="A80" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="B80" s="51"/>
-      <c r="C80" s="53"/>
-      <c r="D80" s="53"/>
+      <c r="B80" s="53"/>
+      <c r="C80" s="54"/>
+      <c r="D80" s="54"/>
       <c r="E80" s="47" t="s">
         <v>33</v>
       </c>
@@ -11668,11 +11670,11 @@
       <c r="A81" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="B81" s="51" t="s">
+      <c r="B81" s="53" t="s">
         <v>223</v>
       </c>
-      <c r="C81" s="53"/>
-      <c r="D81" s="53" t="s">
+      <c r="C81" s="54"/>
+      <c r="D81" s="54" t="s">
         <v>18</v>
       </c>
       <c r="E81" s="47" t="s">
@@ -11683,9 +11685,9 @@
       <c r="A82" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="B82" s="51"/>
-      <c r="C82" s="53"/>
-      <c r="D82" s="53"/>
+      <c r="B82" s="53"/>
+      <c r="C82" s="54"/>
+      <c r="D82" s="54"/>
       <c r="E82" s="47" t="s">
         <v>33</v>
       </c>
@@ -11694,11 +11696,11 @@
       <c r="A83" s="38" t="s">
         <v>227</v>
       </c>
-      <c r="B83" s="51" t="s">
+      <c r="B83" s="53" t="s">
         <v>228</v>
       </c>
-      <c r="C83" s="53"/>
-      <c r="D83" s="53" t="s">
+      <c r="C83" s="54"/>
+      <c r="D83" s="54" t="s">
         <v>18</v>
       </c>
       <c r="E83" s="47" t="s">
@@ -11709,9 +11711,9 @@
       <c r="A84" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="B84" s="51"/>
-      <c r="C84" s="53"/>
-      <c r="D84" s="53"/>
+      <c r="B84" s="53"/>
+      <c r="C84" s="54"/>
+      <c r="D84" s="54"/>
       <c r="E84" s="47" t="s">
         <v>33</v>
       </c>
@@ -11720,9 +11722,9 @@
       <c r="A85" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="B85" s="51"/>
-      <c r="C85" s="53"/>
-      <c r="D85" s="53"/>
+      <c r="B85" s="53"/>
+      <c r="C85" s="54"/>
+      <c r="D85" s="54"/>
       <c r="E85" s="47" t="s">
         <v>33</v>
       </c>
@@ -11791,11 +11793,11 @@
       <c r="A90" s="38" t="s">
         <v>477</v>
       </c>
-      <c r="B90" s="51" t="s">
+      <c r="B90" s="53" t="s">
         <v>478</v>
       </c>
-      <c r="C90" s="53"/>
-      <c r="D90" s="53" t="s">
+      <c r="C90" s="54"/>
+      <c r="D90" s="54" t="s">
         <v>18</v>
       </c>
       <c r="E90" s="47" t="s">
@@ -11806,9 +11808,9 @@
       <c r="A91" s="39" t="s">
         <v>480</v>
       </c>
-      <c r="B91" s="52"/>
-      <c r="C91" s="54"/>
-      <c r="D91" s="54"/>
+      <c r="B91" s="59"/>
+      <c r="C91" s="60"/>
+      <c r="D91" s="60"/>
       <c r="E91" s="49" t="s">
         <v>33</v>
       </c>
@@ -11816,60 +11818,78 @@
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C93" s="50">
         <f>COUNTBLANK(C2:C91)</f>
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C94" s="50">
         <f>COUNTA(C2:C91)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="120">
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="D90:D91"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="D83:D85"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="C78:C80"/>
+    <mergeCell ref="D78:D80"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="C66:C68"/>
+    <mergeCell ref="D66:D68"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="C69:C71"/>
+    <mergeCell ref="D69:D71"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="C61:C63"/>
+    <mergeCell ref="D61:D63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="D58:D60"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="D40:D48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="D30:D31"/>
@@ -11886,67 +11906,49 @@
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="E28:E29"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="D40:D48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="D58:D60"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="C66:C68"/>
-    <mergeCell ref="D66:D68"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="C69:C71"/>
-    <mergeCell ref="D69:D71"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="C61:C63"/>
-    <mergeCell ref="D61:D63"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="C78:C80"/>
-    <mergeCell ref="D78:D80"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="D90:D91"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="D83:D85"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12956,12 +12958,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13188,20 +13192,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13226,18 +13237,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Function fn_check_job_type_upload added to UPLOAD_UTIL
</commit_message>
<xml_diff>
--- a/analysis/MEDS_Tables.xlsx
+++ b/analysis/MEDS_Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="502" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3E0A762-8083-4E80-A748-BE7F4F206F70}"/>
+  <xr:revisionPtr revIDLastSave="503" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E64BEDE-DC1A-4AA5-9338-E723D3A5F07D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2525" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2526" uniqueCount="568">
   <si>
     <t>Table</t>
   </si>
@@ -2565,43 +2565,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="19" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -10637,8 +10637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8FA477-9B46-4053-B7AD-310B8B9F2B30}">
   <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A11"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10678,7 +10678,7 @@
       <c r="A2" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="58" t="s">
         <v>38</v>
       </c>
       <c r="C2" s="57" t="s">
@@ -10687,14 +10687,14 @@
       <c r="D2" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="61" t="s">
         <v>564</v>
       </c>
-      <c r="G2" s="51">
+      <c r="G2" s="62">
         <f>C94/C93</f>
-        <v>5.8823529411764705E-2</v>
-      </c>
-      <c r="H2" s="52" t="s">
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="H2" s="63" t="s">
         <v>566</v>
       </c>
     </row>
@@ -10702,63 +10702,63 @@
       <c r="A3" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
       <c r="E3" s="55"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
       <c r="E4" s="55"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="52"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="63"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="53" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="55" t="s">
         <v>519</v>
       </c>
-      <c r="G5" s="51"/>
-      <c r="H5" s="52"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="63"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="53"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
       <c r="E6" s="55"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="54" t="s">
+      <c r="D7" s="53" t="s">
         <v>42</v>
       </c>
       <c r="E7" s="55" t="s">
@@ -10769,20 +10769,22 @@
       <c r="A8" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="53"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
       <c r="E8" s="55"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="51" t="s">
         <v>171</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54" t="s">
+      <c r="C9" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="53" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="55" t="s">
@@ -10793,31 +10795,31 @@
       <c r="A10" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
       <c r="E10" s="55"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
       <c r="E11" s="55"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
         <v>203</v>
       </c>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="51" t="s">
         <v>204</v>
       </c>
-      <c r="C12" s="54" t="s">
+      <c r="C12" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="54" t="s">
+      <c r="D12" s="53" t="s">
         <v>42</v>
       </c>
       <c r="E12" s="55" t="s">
@@ -10828,22 +10830,22 @@
       <c r="A13" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
       <c r="E13" s="55"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
         <v>360</v>
       </c>
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="51" t="s">
         <v>361</v>
       </c>
-      <c r="C14" s="54" t="s">
+      <c r="C14" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="D14" s="53" t="s">
         <v>42</v>
       </c>
       <c r="E14" s="55" t="s">
@@ -10854,23 +10856,23 @@
       <c r="A15" s="39" t="s">
         <v>363</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="61"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="56"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="58" t="s">
         <v>71</v>
       </c>
       <c r="C16" s="57"/>
       <c r="D16" s="57" t="s">
         <v>567</v>
       </c>
-      <c r="E16" s="58" t="s">
+      <c r="E16" s="61" t="s">
         <v>73</v>
       </c>
     </row>
@@ -10878,20 +10880,20 @@
       <c r="A17" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="53"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
       <c r="E17" s="55"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="53" t="s">
+      <c r="B18" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54" t="s">
+      <c r="C18" s="53"/>
+      <c r="D18" s="53" t="s">
         <v>567</v>
       </c>
       <c r="E18" s="55" t="s">
@@ -10902,20 +10904,20 @@
       <c r="A19" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="B19" s="53"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
       <c r="E19" s="55"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
         <v>299</v>
       </c>
-      <c r="B20" s="53" t="s">
+      <c r="B20" s="51" t="s">
         <v>300</v>
       </c>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54" t="s">
+      <c r="C20" s="53"/>
+      <c r="D20" s="53" t="s">
         <v>567</v>
       </c>
       <c r="E20" s="55" t="s">
@@ -10926,20 +10928,20 @@
       <c r="A21" s="38" t="s">
         <v>302</v>
       </c>
-      <c r="B21" s="53"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
       <c r="E21" s="55"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="38" t="s">
         <v>304</v>
       </c>
-      <c r="B22" s="53" t="s">
+      <c r="B22" s="51" t="s">
         <v>305</v>
       </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="54" t="s">
+      <c r="C22" s="53"/>
+      <c r="D22" s="53" t="s">
         <v>567</v>
       </c>
       <c r="E22" s="55" t="s">
@@ -10950,18 +10952,18 @@
       <c r="A23" s="38" t="s">
         <v>309</v>
       </c>
-      <c r="B23" s="53"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
       <c r="E23" s="55"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="38" t="s">
         <v>307</v>
       </c>
-      <c r="B24" s="53"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54" t="s">
+      <c r="B24" s="51"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53" t="s">
         <v>567</v>
       </c>
       <c r="E24" s="55"/>
@@ -10970,20 +10972,20 @@
       <c r="A25" s="38" t="s">
         <v>311</v>
       </c>
-      <c r="B25" s="53"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
       <c r="E25" s="55"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="38" t="s">
         <v>317</v>
       </c>
-      <c r="B26" s="53" t="s">
+      <c r="B26" s="51" t="s">
         <v>318</v>
       </c>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54" t="s">
+      <c r="C26" s="53"/>
+      <c r="D26" s="53" t="s">
         <v>567</v>
       </c>
       <c r="E26" s="55" t="s">
@@ -10994,20 +10996,20 @@
       <c r="A27" s="38" t="s">
         <v>320</v>
       </c>
-      <c r="B27" s="53"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
       <c r="E27" s="55"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="38" t="s">
         <v>322</v>
       </c>
-      <c r="B28" s="62" t="s">
+      <c r="B28" s="59" t="s">
         <v>323</v>
       </c>
-      <c r="C28" s="63"/>
-      <c r="D28" s="54" t="s">
+      <c r="C28" s="60"/>
+      <c r="D28" s="53" t="s">
         <v>567</v>
       </c>
       <c r="E28" s="55" t="s">
@@ -11018,20 +11020,20 @@
       <c r="A29" s="38" t="s">
         <v>325</v>
       </c>
-      <c r="B29" s="62"/>
-      <c r="C29" s="63"/>
-      <c r="D29" s="54"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="53"/>
       <c r="E29" s="55"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="38" t="s">
         <v>327</v>
       </c>
-      <c r="B30" s="53" t="s">
+      <c r="B30" s="51" t="s">
         <v>328</v>
       </c>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54" t="s">
+      <c r="C30" s="53"/>
+      <c r="D30" s="53" t="s">
         <v>567</v>
       </c>
       <c r="E30" s="55" t="s">
@@ -11042,20 +11044,20 @@
       <c r="A31" s="38" t="s">
         <v>330</v>
       </c>
-      <c r="B31" s="53"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
       <c r="E31" s="55"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="38" t="s">
         <v>332</v>
       </c>
-      <c r="B32" s="53" t="s">
+      <c r="B32" s="51" t="s">
         <v>333</v>
       </c>
-      <c r="C32" s="54"/>
-      <c r="D32" s="54" t="s">
+      <c r="C32" s="53"/>
+      <c r="D32" s="53" t="s">
         <v>567</v>
       </c>
       <c r="E32" s="55" t="s">
@@ -11066,20 +11068,20 @@
       <c r="A33" s="38" t="s">
         <v>335</v>
       </c>
-      <c r="B33" s="53"/>
-      <c r="C33" s="54"/>
-      <c r="D33" s="54"/>
+      <c r="B33" s="51"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
       <c r="E33" s="55"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="38" t="s">
         <v>337</v>
       </c>
-      <c r="B34" s="53" t="s">
+      <c r="B34" s="51" t="s">
         <v>338</v>
       </c>
-      <c r="C34" s="54"/>
-      <c r="D34" s="54" t="s">
+      <c r="C34" s="53"/>
+      <c r="D34" s="53" t="s">
         <v>567</v>
       </c>
       <c r="E34" s="55" t="s">
@@ -11090,20 +11092,20 @@
       <c r="A35" s="38" t="s">
         <v>340</v>
       </c>
-      <c r="B35" s="53"/>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
+      <c r="B35" s="51"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
       <c r="E35" s="55"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="38" t="s">
         <v>342</v>
       </c>
-      <c r="B36" s="53" t="s">
+      <c r="B36" s="51" t="s">
         <v>343</v>
       </c>
-      <c r="C36" s="54"/>
-      <c r="D36" s="54" t="s">
+      <c r="C36" s="53"/>
+      <c r="D36" s="53" t="s">
         <v>567</v>
       </c>
       <c r="E36" s="55" t="s">
@@ -11114,20 +11116,20 @@
       <c r="A37" s="38" t="s">
         <v>345</v>
       </c>
-      <c r="B37" s="53"/>
-      <c r="C37" s="54"/>
-      <c r="D37" s="54"/>
+      <c r="B37" s="51"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
       <c r="E37" s="55"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="38" t="s">
         <v>347</v>
       </c>
-      <c r="B38" s="53" t="s">
+      <c r="B38" s="51" t="s">
         <v>348</v>
       </c>
-      <c r="C38" s="54"/>
-      <c r="D38" s="54" t="s">
+      <c r="C38" s="53"/>
+      <c r="D38" s="53" t="s">
         <v>567</v>
       </c>
       <c r="E38" s="55" t="s">
@@ -11138,10 +11140,10 @@
       <c r="A39" s="39" t="s">
         <v>350</v>
       </c>
-      <c r="B39" s="59"/>
-      <c r="C39" s="60"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="61"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="56"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="37" t="s">
@@ -11166,7 +11168,7 @@
         <v>371</v>
       </c>
       <c r="C41" s="44"/>
-      <c r="D41" s="54"/>
+      <c r="D41" s="53"/>
       <c r="E41" s="45" t="s">
         <v>513</v>
       </c>
@@ -11179,7 +11181,7 @@
         <v>374</v>
       </c>
       <c r="C42" s="44"/>
-      <c r="D42" s="54"/>
+      <c r="D42" s="53"/>
       <c r="E42" s="45" t="s">
         <v>522</v>
       </c>
@@ -11192,7 +11194,7 @@
         <v>366</v>
       </c>
       <c r="C43" s="44"/>
-      <c r="D43" s="54"/>
+      <c r="D43" s="53"/>
       <c r="E43" s="45" t="s">
         <v>514</v>
       </c>
@@ -11205,7 +11207,7 @@
         <v>371</v>
       </c>
       <c r="C44" s="44"/>
-      <c r="D44" s="54"/>
+      <c r="D44" s="53"/>
       <c r="E44" s="45" t="s">
         <v>513</v>
       </c>
@@ -11218,7 +11220,7 @@
         <v>374</v>
       </c>
       <c r="C45" s="44"/>
-      <c r="D45" s="54"/>
+      <c r="D45" s="53"/>
       <c r="E45" s="45" t="s">
         <v>522</v>
       </c>
@@ -11231,7 +11233,7 @@
         <v>366</v>
       </c>
       <c r="C46" s="44"/>
-      <c r="D46" s="54"/>
+      <c r="D46" s="53"/>
       <c r="E46" s="45" t="s">
         <v>514</v>
       </c>
@@ -11244,7 +11246,7 @@
         <v>371</v>
       </c>
       <c r="C47" s="44"/>
-      <c r="D47" s="54"/>
+      <c r="D47" s="53"/>
       <c r="E47" s="45" t="s">
         <v>513</v>
       </c>
@@ -11257,7 +11259,7 @@
         <v>374</v>
       </c>
       <c r="C48" s="44"/>
-      <c r="D48" s="54"/>
+      <c r="D48" s="53"/>
       <c r="E48" s="45" t="s">
         <v>522</v>
       </c>
@@ -11266,7 +11268,7 @@
       <c r="A49" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="56" t="s">
+      <c r="B49" s="58" t="s">
         <v>48</v>
       </c>
       <c r="C49" s="57"/>
@@ -11281,9 +11283,9 @@
       <c r="A50" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="53"/>
-      <c r="C50" s="54"/>
-      <c r="D50" s="54"/>
+      <c r="B50" s="51"/>
+      <c r="C50" s="53"/>
+      <c r="D50" s="53"/>
       <c r="E50" s="47" t="s">
         <v>33</v>
       </c>
@@ -11292,11 +11294,11 @@
       <c r="A51" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="B51" s="53" t="s">
+      <c r="B51" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="C51" s="54"/>
-      <c r="D51" s="54" t="s">
+      <c r="C51" s="53"/>
+      <c r="D51" s="53" t="s">
         <v>18</v>
       </c>
       <c r="E51" s="47" t="s">
@@ -11307,9 +11309,9 @@
       <c r="A52" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B52" s="53"/>
-      <c r="C52" s="54"/>
-      <c r="D52" s="54"/>
+      <c r="B52" s="51"/>
+      <c r="C52" s="53"/>
+      <c r="D52" s="53"/>
       <c r="E52" s="47" t="s">
         <v>33</v>
       </c>
@@ -11318,11 +11320,11 @@
       <c r="A53" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="B53" s="53" t="s">
+      <c r="B53" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="C53" s="54"/>
-      <c r="D53" s="54" t="s">
+      <c r="C53" s="53"/>
+      <c r="D53" s="53" t="s">
         <v>18</v>
       </c>
       <c r="E53" s="47" t="s">
@@ -11333,9 +11335,9 @@
       <c r="A54" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="B54" s="53"/>
-      <c r="C54" s="54"/>
-      <c r="D54" s="54"/>
+      <c r="B54" s="51"/>
+      <c r="C54" s="53"/>
+      <c r="D54" s="53"/>
       <c r="E54" s="47" t="s">
         <v>33</v>
       </c>
@@ -11344,9 +11346,9 @@
       <c r="A55" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="B55" s="53"/>
-      <c r="C55" s="54"/>
-      <c r="D55" s="54"/>
+      <c r="B55" s="51"/>
+      <c r="C55" s="53"/>
+      <c r="D55" s="53"/>
       <c r="E55" s="47" t="s">
         <v>33</v>
       </c>
@@ -11355,11 +11357,11 @@
       <c r="A56" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="B56" s="53" t="s">
+      <c r="B56" s="51" t="s">
         <v>119</v>
       </c>
-      <c r="C56" s="54"/>
-      <c r="D56" s="54" t="s">
+      <c r="C56" s="53"/>
+      <c r="D56" s="53" t="s">
         <v>18</v>
       </c>
       <c r="E56" s="47" t="s">
@@ -11370,9 +11372,9 @@
       <c r="A57" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="B57" s="53"/>
-      <c r="C57" s="54"/>
-      <c r="D57" s="54"/>
+      <c r="B57" s="51"/>
+      <c r="C57" s="53"/>
+      <c r="D57" s="53"/>
       <c r="E57" s="47" t="s">
         <v>33</v>
       </c>
@@ -11381,11 +11383,11 @@
       <c r="A58" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="B58" s="53" t="s">
+      <c r="B58" s="51" t="s">
         <v>124</v>
       </c>
-      <c r="C58" s="54"/>
-      <c r="D58" s="54" t="s">
+      <c r="C58" s="53"/>
+      <c r="D58" s="53" t="s">
         <v>18</v>
       </c>
       <c r="E58" s="47" t="s">
@@ -11396,9 +11398,9 @@
       <c r="A59" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="B59" s="53"/>
-      <c r="C59" s="54"/>
-      <c r="D59" s="54"/>
+      <c r="B59" s="51"/>
+      <c r="C59" s="53"/>
+      <c r="D59" s="53"/>
       <c r="E59" s="47" t="s">
         <v>33</v>
       </c>
@@ -11407,9 +11409,9 @@
       <c r="A60" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="B60" s="53"/>
-      <c r="C60" s="54"/>
-      <c r="D60" s="54"/>
+      <c r="B60" s="51"/>
+      <c r="C60" s="53"/>
+      <c r="D60" s="53"/>
       <c r="E60" s="47" t="s">
         <v>33</v>
       </c>
@@ -11418,11 +11420,11 @@
       <c r="A61" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="B61" s="53" t="s">
+      <c r="B61" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="C61" s="54"/>
-      <c r="D61" s="54" t="s">
+      <c r="C61" s="53"/>
+      <c r="D61" s="53" t="s">
         <v>18</v>
       </c>
       <c r="E61" s="47" t="s">
@@ -11433,9 +11435,9 @@
       <c r="A62" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="B62" s="53"/>
-      <c r="C62" s="54"/>
-      <c r="D62" s="54"/>
+      <c r="B62" s="51"/>
+      <c r="C62" s="53"/>
+      <c r="D62" s="53"/>
       <c r="E62" s="47" t="s">
         <v>33</v>
       </c>
@@ -11444,9 +11446,9 @@
       <c r="A63" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="B63" s="53"/>
-      <c r="C63" s="54"/>
-      <c r="D63" s="54"/>
+      <c r="B63" s="51"/>
+      <c r="C63" s="53"/>
+      <c r="D63" s="53"/>
       <c r="E63" s="47" t="s">
         <v>33</v>
       </c>
@@ -11455,11 +11457,11 @@
       <c r="A64" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="B64" s="53" t="s">
+      <c r="B64" s="51" t="s">
         <v>159</v>
       </c>
-      <c r="C64" s="54"/>
-      <c r="D64" s="54" t="s">
+      <c r="C64" s="53"/>
+      <c r="D64" s="53" t="s">
         <v>18</v>
       </c>
       <c r="E64" s="47" t="s">
@@ -11470,9 +11472,9 @@
       <c r="A65" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="B65" s="53"/>
-      <c r="C65" s="54"/>
-      <c r="D65" s="54"/>
+      <c r="B65" s="51"/>
+      <c r="C65" s="53"/>
+      <c r="D65" s="53"/>
       <c r="E65" s="47" t="s">
         <v>33</v>
       </c>
@@ -11481,11 +11483,11 @@
       <c r="A66" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="B66" s="53" t="s">
+      <c r="B66" s="51" t="s">
         <v>164</v>
       </c>
-      <c r="C66" s="54"/>
-      <c r="D66" s="54" t="s">
+      <c r="C66" s="53"/>
+      <c r="D66" s="53" t="s">
         <v>18</v>
       </c>
       <c r="E66" s="47" t="s">
@@ -11496,9 +11498,9 @@
       <c r="A67" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="B67" s="53"/>
-      <c r="C67" s="54"/>
-      <c r="D67" s="54"/>
+      <c r="B67" s="51"/>
+      <c r="C67" s="53"/>
+      <c r="D67" s="53"/>
       <c r="E67" s="47" t="s">
         <v>33</v>
       </c>
@@ -11507,9 +11509,9 @@
       <c r="A68" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="B68" s="53"/>
-      <c r="C68" s="54"/>
-      <c r="D68" s="54"/>
+      <c r="B68" s="51"/>
+      <c r="C68" s="53"/>
+      <c r="D68" s="53"/>
       <c r="E68" s="47" t="s">
         <v>33</v>
       </c>
@@ -11518,11 +11520,11 @@
       <c r="A69" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="B69" s="53" t="s">
+      <c r="B69" s="51" t="s">
         <v>179</v>
       </c>
-      <c r="C69" s="54"/>
-      <c r="D69" s="54" t="s">
+      <c r="C69" s="53"/>
+      <c r="D69" s="53" t="s">
         <v>18</v>
       </c>
       <c r="E69" s="47" t="s">
@@ -11533,9 +11535,9 @@
       <c r="A70" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="B70" s="53"/>
-      <c r="C70" s="54"/>
-      <c r="D70" s="54"/>
+      <c r="B70" s="51"/>
+      <c r="C70" s="53"/>
+      <c r="D70" s="53"/>
       <c r="E70" s="47" t="s">
         <v>33</v>
       </c>
@@ -11544,9 +11546,9 @@
       <c r="A71" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="B71" s="53"/>
-      <c r="C71" s="54"/>
-      <c r="D71" s="54"/>
+      <c r="B71" s="51"/>
+      <c r="C71" s="53"/>
+      <c r="D71" s="53"/>
       <c r="E71" s="47" t="s">
         <v>33</v>
       </c>
@@ -11555,11 +11557,11 @@
       <c r="A72" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="B72" s="53" t="s">
+      <c r="B72" s="51" t="s">
         <v>186</v>
       </c>
-      <c r="C72" s="54"/>
-      <c r="D72" s="54" t="s">
+      <c r="C72" s="53"/>
+      <c r="D72" s="53" t="s">
         <v>18</v>
       </c>
       <c r="E72" s="47" t="s">
@@ -11570,9 +11572,9 @@
       <c r="A73" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="B73" s="53"/>
-      <c r="C73" s="54"/>
-      <c r="D73" s="54"/>
+      <c r="B73" s="51"/>
+      <c r="C73" s="53"/>
+      <c r="D73" s="53"/>
       <c r="E73" s="47" t="s">
         <v>33</v>
       </c>
@@ -11581,11 +11583,11 @@
       <c r="A74" s="38" t="s">
         <v>194</v>
       </c>
-      <c r="B74" s="53" t="s">
+      <c r="B74" s="51" t="s">
         <v>195</v>
       </c>
-      <c r="C74" s="54"/>
-      <c r="D74" s="54" t="s">
+      <c r="C74" s="53"/>
+      <c r="D74" s="53" t="s">
         <v>18</v>
       </c>
       <c r="E74" s="47" t="s">
@@ -11596,9 +11598,9 @@
       <c r="A75" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="B75" s="53"/>
-      <c r="C75" s="54"/>
-      <c r="D75" s="54"/>
+      <c r="B75" s="51"/>
+      <c r="C75" s="53"/>
+      <c r="D75" s="53"/>
       <c r="E75" s="47" t="s">
         <v>33</v>
       </c>
@@ -11607,11 +11609,11 @@
       <c r="A76" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="B76" s="53" t="s">
+      <c r="B76" s="51" t="s">
         <v>200</v>
       </c>
-      <c r="C76" s="54"/>
-      <c r="D76" s="54" t="s">
+      <c r="C76" s="53"/>
+      <c r="D76" s="53" t="s">
         <v>18</v>
       </c>
       <c r="E76" s="47" t="s">
@@ -11622,9 +11624,9 @@
       <c r="A77" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="B77" s="53"/>
-      <c r="C77" s="54"/>
-      <c r="D77" s="54"/>
+      <c r="B77" s="51"/>
+      <c r="C77" s="53"/>
+      <c r="D77" s="53"/>
       <c r="E77" s="47" t="s">
         <v>33</v>
       </c>
@@ -11633,11 +11635,11 @@
       <c r="A78" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="B78" s="53" t="s">
+      <c r="B78" s="51" t="s">
         <v>211</v>
       </c>
-      <c r="C78" s="54"/>
-      <c r="D78" s="54" t="s">
+      <c r="C78" s="53"/>
+      <c r="D78" s="53" t="s">
         <v>18</v>
       </c>
       <c r="E78" s="47" t="s">
@@ -11648,9 +11650,9 @@
       <c r="A79" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="B79" s="53"/>
-      <c r="C79" s="54"/>
-      <c r="D79" s="54"/>
+      <c r="B79" s="51"/>
+      <c r="C79" s="53"/>
+      <c r="D79" s="53"/>
       <c r="E79" s="47" t="s">
         <v>33</v>
       </c>
@@ -11659,9 +11661,9 @@
       <c r="A80" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="B80" s="53"/>
-      <c r="C80" s="54"/>
-      <c r="D80" s="54"/>
+      <c r="B80" s="51"/>
+      <c r="C80" s="53"/>
+      <c r="D80" s="53"/>
       <c r="E80" s="47" t="s">
         <v>33</v>
       </c>
@@ -11670,11 +11672,11 @@
       <c r="A81" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="B81" s="53" t="s">
+      <c r="B81" s="51" t="s">
         <v>223</v>
       </c>
-      <c r="C81" s="54"/>
-      <c r="D81" s="54" t="s">
+      <c r="C81" s="53"/>
+      <c r="D81" s="53" t="s">
         <v>18</v>
       </c>
       <c r="E81" s="47" t="s">
@@ -11685,9 +11687,9 @@
       <c r="A82" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="B82" s="53"/>
-      <c r="C82" s="54"/>
-      <c r="D82" s="54"/>
+      <c r="B82" s="51"/>
+      <c r="C82" s="53"/>
+      <c r="D82" s="53"/>
       <c r="E82" s="47" t="s">
         <v>33</v>
       </c>
@@ -11696,11 +11698,11 @@
       <c r="A83" s="38" t="s">
         <v>227</v>
       </c>
-      <c r="B83" s="53" t="s">
+      <c r="B83" s="51" t="s">
         <v>228</v>
       </c>
-      <c r="C83" s="54"/>
-      <c r="D83" s="54" t="s">
+      <c r="C83" s="53"/>
+      <c r="D83" s="53" t="s">
         <v>18</v>
       </c>
       <c r="E83" s="47" t="s">
@@ -11711,9 +11713,9 @@
       <c r="A84" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="B84" s="53"/>
-      <c r="C84" s="54"/>
-      <c r="D84" s="54"/>
+      <c r="B84" s="51"/>
+      <c r="C84" s="53"/>
+      <c r="D84" s="53"/>
       <c r="E84" s="47" t="s">
         <v>33</v>
       </c>
@@ -11722,9 +11724,9 @@
       <c r="A85" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="B85" s="53"/>
-      <c r="C85" s="54"/>
-      <c r="D85" s="54"/>
+      <c r="B85" s="51"/>
+      <c r="C85" s="53"/>
+      <c r="D85" s="53"/>
       <c r="E85" s="47" t="s">
         <v>33</v>
       </c>
@@ -11793,11 +11795,11 @@
       <c r="A90" s="38" t="s">
         <v>477</v>
       </c>
-      <c r="B90" s="53" t="s">
+      <c r="B90" s="51" t="s">
         <v>478</v>
       </c>
-      <c r="C90" s="54"/>
-      <c r="D90" s="54" t="s">
+      <c r="C90" s="53"/>
+      <c r="D90" s="53" t="s">
         <v>18</v>
       </c>
       <c r="E90" s="47" t="s">
@@ -11808,9 +11810,9 @@
       <c r="A91" s="39" t="s">
         <v>480</v>
       </c>
-      <c r="B91" s="59"/>
-      <c r="C91" s="60"/>
-      <c r="D91" s="60"/>
+      <c r="B91" s="52"/>
+      <c r="C91" s="54"/>
+      <c r="D91" s="54"/>
       <c r="E91" s="49" t="s">
         <v>33</v>
       </c>
@@ -11818,62 +11820,76 @@
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C93" s="50">
         <f>COUNTBLANK(C2:C91)</f>
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C94" s="50">
         <f>COUNTA(C2:C91)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="120">
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="D90:D91"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="D83:D85"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="C78:C80"/>
-    <mergeCell ref="D78:D80"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="C66:C68"/>
-    <mergeCell ref="D66:D68"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="C69:C71"/>
-    <mergeCell ref="D69:D71"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="C61:C63"/>
-    <mergeCell ref="D61:D63"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="D58:D60"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="D38:D39"/>
@@ -11890,65 +11906,51 @@
     <mergeCell ref="C36:C37"/>
     <mergeCell ref="D36:D37"/>
     <mergeCell ref="E36:E37"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="D58:D60"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="C66:C68"/>
+    <mergeCell ref="D66:D68"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="C69:C71"/>
+    <mergeCell ref="D69:D71"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="C61:C63"/>
+    <mergeCell ref="D61:D63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="C78:C80"/>
+    <mergeCell ref="D78:D80"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="D90:D91"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="D83:D85"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12958,14 +12960,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13192,27 +13192,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13237,9 +13230,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Before refactoring packages, dividing UPLOAD_UTIL in UPLOAD_CSV_UTIL and UPLOAD_SERD_UTIL
</commit_message>
<xml_diff>
--- a/analysis/MEDS_Tables.xlsx
+++ b/analysis/MEDS_Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="503" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E64BEDE-DC1A-4AA5-9338-E723D3A5F07D}"/>
+  <xr:revisionPtr revIDLastSave="538" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEA924F8-4B1F-4D4C-A1DB-3B68E950C3BC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meds_tables" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2526" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2546" uniqueCount="582">
   <si>
     <t>Table</t>
   </si>
@@ -1741,6 +1741,49 @@
   </si>
   <si>
     <t>Form &amp; Edit</t>
+  </si>
+  <si>
+    <t>Instrument</t>
+  </si>
+  <si>
+    <t>Data Use</t>
+  </si>
+  <si>
+    <t>MEIC Number</t>
+  </si>
+  <si>
+    <t>Job Number</t>
+  </si>
+  <si>
+    <t>Job Type</t>
+  </si>
+  <si>
+    <t>8 (XBT)</t>
+  </si>
+  <si>
+    <t>1 (SV Probes)</t>
+  </si>
+  <si>
+    <t>2 (CTD)</t>
+  </si>
+  <si>
+    <t>SERD (Observed Physical Data)</t>
+  </si>
+  <si>
+    <t>PROFILE_HEADER_TS, PROFILE_INDEX_TS, PROFILE_DATA_TS</t>
+  </si>
+  <si>
+    <t>PROFILE_HEADER_TONLY, PROFILE_INDEX_TONLY, PROFILE_DATA_TONLY</t>
+  </si>
+  <si>
+    <t>PROFILE_HEADER_SV, PROFILE_INDEX_SV, PROFILE_DATA_SV</t>
+  </si>
+  <si>
+    <t>Tables</t>
+  </si>
+  <si>
+    <t>Form &amp; Edit
+Text File (?)</t>
   </si>
 </sst>
 </file>
@@ -1750,7 +1793,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1902,6 +1945,13 @@
     <font>
       <sz val="16"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2463,7 +2513,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2565,37 +2615,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="19" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2603,6 +2647,28 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -10635,10 +10701,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8FA477-9B46-4053-B7AD-310B8B9F2B30}">
-  <dimension ref="A1:I94"/>
+  <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E46" activeCellId="2" sqref="E40 E43 E46"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10678,23 +10744,23 @@
       <c r="A2" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="62" t="s">
         <v>564</v>
       </c>
-      <c r="G2" s="51">
-        <f>C94/C93</f>
-        <v>7.1428571428571425E-2</v>
-      </c>
-      <c r="H2" s="52" t="s">
+      <c r="G2" s="63">
+        <f>C107/C106</f>
+        <v>6.1855670103092786E-2</v>
+      </c>
+      <c r="H2" s="64" t="s">
         <v>566</v>
       </c>
     </row>
@@ -10702,29 +10768,29 @@
       <c r="A3" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="53"/>
+      <c r="B3" s="52"/>
       <c r="C3" s="54"/>
       <c r="D3" s="54"/>
-      <c r="E3" s="55"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52"/>
+      <c r="E3" s="56"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="53"/>
+      <c r="B4" s="52"/>
       <c r="C4" s="54"/>
       <c r="D4" s="54"/>
-      <c r="E4" s="55"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="52"/>
+      <c r="E4" s="56"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="64"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="52" t="s">
         <v>53</v>
       </c>
       <c r="C5" s="54" t="s">
@@ -10733,26 +10799,26 @@
       <c r="D5" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="56" t="s">
         <v>519</v>
       </c>
-      <c r="G5" s="51"/>
-      <c r="H5" s="52"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="64"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="53"/>
+      <c r="B6" s="52"/>
       <c r="C6" s="54"/>
       <c r="D6" s="54"/>
-      <c r="E6" s="55"/>
+      <c r="E6" s="56"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="52" t="s">
         <v>78</v>
       </c>
       <c r="C7" s="54" t="s">
@@ -10761,7 +10827,7 @@
       <c r="D7" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="55" t="s">
+      <c r="E7" s="56" t="s">
         <v>80</v>
       </c>
     </row>
@@ -10769,16 +10835,16 @@
       <c r="A8" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="53"/>
+      <c r="B8" s="52"/>
       <c r="C8" s="54"/>
       <c r="D8" s="54"/>
-      <c r="E8" s="55"/>
+      <c r="E8" s="56"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="52" t="s">
         <v>171</v>
       </c>
       <c r="C9" s="54" t="s">
@@ -10787,7 +10853,7 @@
       <c r="D9" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="55" t="s">
+      <c r="E9" s="56" t="s">
         <v>523</v>
       </c>
     </row>
@@ -10795,25 +10861,25 @@
       <c r="A10" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="B10" s="53"/>
+      <c r="B10" s="52"/>
       <c r="C10" s="54"/>
       <c r="D10" s="54"/>
-      <c r="E10" s="55"/>
+      <c r="E10" s="56"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="B11" s="53"/>
+      <c r="B11" s="52"/>
       <c r="C11" s="54"/>
       <c r="D11" s="54"/>
-      <c r="E11" s="55"/>
+      <c r="E11" s="56"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
         <v>203</v>
       </c>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="52" t="s">
         <v>204</v>
       </c>
       <c r="C12" s="54" t="s">
@@ -10822,7 +10888,7 @@
       <c r="D12" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="55" t="s">
+      <c r="E12" s="56" t="s">
         <v>515</v>
       </c>
     </row>
@@ -10830,16 +10896,16 @@
       <c r="A13" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="B13" s="53"/>
+      <c r="B13" s="52"/>
       <c r="C13" s="54"/>
       <c r="D13" s="54"/>
-      <c r="E13" s="55"/>
+      <c r="E13" s="56"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
         <v>360</v>
       </c>
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="52" t="s">
         <v>361</v>
       </c>
       <c r="C14" s="54" t="s">
@@ -10848,7 +10914,7 @@
       <c r="D14" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="55" t="s">
+      <c r="E14" s="56" t="s">
         <v>518</v>
       </c>
     </row>
@@ -10856,23 +10922,23 @@
       <c r="A15" s="39" t="s">
         <v>363</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="61"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="57"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57" t="s">
+      <c r="C16" s="58"/>
+      <c r="D16" s="58" t="s">
         <v>567</v>
       </c>
-      <c r="E16" s="58" t="s">
+      <c r="E16" s="62" t="s">
         <v>73</v>
       </c>
     </row>
@@ -10880,23 +10946,23 @@
       <c r="A17" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="53"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="54"/>
       <c r="D17" s="54"/>
-      <c r="E17" s="55"/>
+      <c r="E17" s="56"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="53" t="s">
+      <c r="B18" s="52" t="s">
         <v>105</v>
       </c>
       <c r="C18" s="54"/>
       <c r="D18" s="54" t="s">
         <v>567</v>
       </c>
-      <c r="E18" s="55" t="s">
+      <c r="E18" s="56" t="s">
         <v>524</v>
       </c>
     </row>
@@ -10904,23 +10970,23 @@
       <c r="A19" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="B19" s="53"/>
+      <c r="B19" s="52"/>
       <c r="C19" s="54"/>
       <c r="D19" s="54"/>
-      <c r="E19" s="55"/>
+      <c r="E19" s="56"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
         <v>299</v>
       </c>
-      <c r="B20" s="53" t="s">
+      <c r="B20" s="52" t="s">
         <v>300</v>
       </c>
       <c r="C20" s="54"/>
       <c r="D20" s="54" t="s">
         <v>567</v>
       </c>
-      <c r="E20" s="55" t="s">
+      <c r="E20" s="56" t="s">
         <v>516</v>
       </c>
     </row>
@@ -10928,23 +10994,23 @@
       <c r="A21" s="38" t="s">
         <v>302</v>
       </c>
-      <c r="B21" s="53"/>
+      <c r="B21" s="52"/>
       <c r="C21" s="54"/>
       <c r="D21" s="54"/>
-      <c r="E21" s="55"/>
+      <c r="E21" s="56"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="38" t="s">
         <v>304</v>
       </c>
-      <c r="B22" s="53" t="s">
+      <c r="B22" s="52" t="s">
         <v>305</v>
       </c>
       <c r="C22" s="54"/>
       <c r="D22" s="54" t="s">
         <v>567</v>
       </c>
-      <c r="E22" s="55" t="s">
+      <c r="E22" s="56" t="s">
         <v>521</v>
       </c>
     </row>
@@ -10952,43 +11018,43 @@
       <c r="A23" s="38" t="s">
         <v>309</v>
       </c>
-      <c r="B23" s="53"/>
+      <c r="B23" s="52"/>
       <c r="C23" s="54"/>
       <c r="D23" s="54"/>
-      <c r="E23" s="55"/>
+      <c r="E23" s="56"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="38" t="s">
         <v>307</v>
       </c>
-      <c r="B24" s="53"/>
+      <c r="B24" s="52"/>
       <c r="C24" s="54"/>
       <c r="D24" s="54" t="s">
         <v>567</v>
       </c>
-      <c r="E24" s="55"/>
+      <c r="E24" s="56"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="38" t="s">
         <v>311</v>
       </c>
-      <c r="B25" s="53"/>
+      <c r="B25" s="52"/>
       <c r="C25" s="54"/>
       <c r="D25" s="54"/>
-      <c r="E25" s="55"/>
+      <c r="E25" s="56"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="38" t="s">
         <v>317</v>
       </c>
-      <c r="B26" s="53" t="s">
+      <c r="B26" s="52" t="s">
         <v>318</v>
       </c>
       <c r="C26" s="54"/>
       <c r="D26" s="54" t="s">
         <v>567</v>
       </c>
-      <c r="E26" s="55" t="s">
+      <c r="E26" s="56" t="s">
         <v>512</v>
       </c>
     </row>
@@ -10996,23 +11062,23 @@
       <c r="A27" s="38" t="s">
         <v>320</v>
       </c>
-      <c r="B27" s="53"/>
+      <c r="B27" s="52"/>
       <c r="C27" s="54"/>
       <c r="D27" s="54"/>
-      <c r="E27" s="55"/>
+      <c r="E27" s="56"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="38" t="s">
         <v>322</v>
       </c>
-      <c r="B28" s="62" t="s">
+      <c r="B28" s="60" t="s">
         <v>323</v>
       </c>
-      <c r="C28" s="63"/>
+      <c r="C28" s="61"/>
       <c r="D28" s="54" t="s">
         <v>567</v>
       </c>
-      <c r="E28" s="55" t="s">
+      <c r="E28" s="56" t="s">
         <v>517</v>
       </c>
     </row>
@@ -11020,23 +11086,23 @@
       <c r="A29" s="38" t="s">
         <v>325</v>
       </c>
-      <c r="B29" s="62"/>
-      <c r="C29" s="63"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="61"/>
       <c r="D29" s="54"/>
-      <c r="E29" s="55"/>
+      <c r="E29" s="56"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="38" t="s">
         <v>327</v>
       </c>
-      <c r="B30" s="53" t="s">
+      <c r="B30" s="52" t="s">
         <v>328</v>
       </c>
       <c r="C30" s="54"/>
       <c r="D30" s="54" t="s">
         <v>567</v>
       </c>
-      <c r="E30" s="55" t="s">
+      <c r="E30" s="56" t="s">
         <v>508</v>
       </c>
     </row>
@@ -11044,23 +11110,23 @@
       <c r="A31" s="38" t="s">
         <v>330</v>
       </c>
-      <c r="B31" s="53"/>
+      <c r="B31" s="52"/>
       <c r="C31" s="54"/>
       <c r="D31" s="54"/>
-      <c r="E31" s="55"/>
+      <c r="E31" s="56"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="38" t="s">
         <v>332</v>
       </c>
-      <c r="B32" s="53" t="s">
+      <c r="B32" s="52" t="s">
         <v>333</v>
       </c>
       <c r="C32" s="54"/>
       <c r="D32" s="54" t="s">
         <v>567</v>
       </c>
-      <c r="E32" s="55" t="s">
+      <c r="E32" s="56" t="s">
         <v>510</v>
       </c>
     </row>
@@ -11068,23 +11134,23 @@
       <c r="A33" s="38" t="s">
         <v>335</v>
       </c>
-      <c r="B33" s="53"/>
+      <c r="B33" s="52"/>
       <c r="C33" s="54"/>
       <c r="D33" s="54"/>
-      <c r="E33" s="55"/>
+      <c r="E33" s="56"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="38" t="s">
         <v>337</v>
       </c>
-      <c r="B34" s="53" t="s">
+      <c r="B34" s="52" t="s">
         <v>338</v>
       </c>
       <c r="C34" s="54"/>
       <c r="D34" s="54" t="s">
         <v>567</v>
       </c>
-      <c r="E34" s="55" t="s">
+      <c r="E34" s="56" t="s">
         <v>511</v>
       </c>
     </row>
@@ -11092,23 +11158,23 @@
       <c r="A35" s="38" t="s">
         <v>340</v>
       </c>
-      <c r="B35" s="53"/>
+      <c r="B35" s="52"/>
       <c r="C35" s="54"/>
       <c r="D35" s="54"/>
-      <c r="E35" s="55"/>
+      <c r="E35" s="56"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="38" t="s">
         <v>342</v>
       </c>
-      <c r="B36" s="53" t="s">
+      <c r="B36" s="52" t="s">
         <v>343</v>
       </c>
       <c r="C36" s="54"/>
       <c r="D36" s="54" t="s">
         <v>567</v>
       </c>
-      <c r="E36" s="55" t="s">
+      <c r="E36" s="56" t="s">
         <v>509</v>
       </c>
     </row>
@@ -11116,23 +11182,23 @@
       <c r="A37" s="38" t="s">
         <v>345</v>
       </c>
-      <c r="B37" s="53"/>
+      <c r="B37" s="52"/>
       <c r="C37" s="54"/>
       <c r="D37" s="54"/>
-      <c r="E37" s="55"/>
+      <c r="E37" s="56"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="38" t="s">
         <v>347</v>
       </c>
-      <c r="B38" s="53" t="s">
+      <c r="B38" s="52" t="s">
         <v>348</v>
       </c>
       <c r="C38" s="54"/>
       <c r="D38" s="54" t="s">
         <v>567</v>
       </c>
-      <c r="E38" s="55" t="s">
+      <c r="E38" s="56" t="s">
         <v>520</v>
       </c>
     </row>
@@ -11140,10 +11206,10 @@
       <c r="A39" s="39" t="s">
         <v>350</v>
       </c>
-      <c r="B39" s="59"/>
-      <c r="C39" s="60"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="61"/>
+      <c r="B39" s="53"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="57"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="37" t="s">
@@ -11153,7 +11219,7 @@
         <v>366</v>
       </c>
       <c r="C40" s="41"/>
-      <c r="D40" s="57" t="s">
+      <c r="D40" s="58" t="s">
         <v>369</v>
       </c>
       <c r="E40" s="42" t="s">
@@ -11268,11 +11334,11 @@
       <c r="A49" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="56" t="s">
+      <c r="B49" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="C49" s="57"/>
-      <c r="D49" s="57" t="s">
+      <c r="C49" s="58"/>
+      <c r="D49" s="58" t="s">
         <v>18</v>
       </c>
       <c r="E49" s="46" t="s">
@@ -11283,7 +11349,7 @@
       <c r="A50" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="53"/>
+      <c r="B50" s="52"/>
       <c r="C50" s="54"/>
       <c r="D50" s="54"/>
       <c r="E50" s="47" t="s">
@@ -11294,7 +11360,7 @@
       <c r="A51" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="B51" s="53" t="s">
+      <c r="B51" s="52" t="s">
         <v>65</v>
       </c>
       <c r="C51" s="54"/>
@@ -11309,7 +11375,7 @@
       <c r="A52" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B52" s="53"/>
+      <c r="B52" s="52"/>
       <c r="C52" s="54"/>
       <c r="D52" s="54"/>
       <c r="E52" s="47" t="s">
@@ -11320,7 +11386,7 @@
       <c r="A53" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="B53" s="53" t="s">
+      <c r="B53" s="52" t="s">
         <v>110</v>
       </c>
       <c r="C53" s="54"/>
@@ -11335,7 +11401,7 @@
       <c r="A54" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="B54" s="53"/>
+      <c r="B54" s="52"/>
       <c r="C54" s="54"/>
       <c r="D54" s="54"/>
       <c r="E54" s="47" t="s">
@@ -11346,7 +11412,7 @@
       <c r="A55" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="B55" s="53"/>
+      <c r="B55" s="52"/>
       <c r="C55" s="54"/>
       <c r="D55" s="54"/>
       <c r="E55" s="47" t="s">
@@ -11357,7 +11423,7 @@
       <c r="A56" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="B56" s="53" t="s">
+      <c r="B56" s="52" t="s">
         <v>119</v>
       </c>
       <c r="C56" s="54"/>
@@ -11372,7 +11438,7 @@
       <c r="A57" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="B57" s="53"/>
+      <c r="B57" s="52"/>
       <c r="C57" s="54"/>
       <c r="D57" s="54"/>
       <c r="E57" s="47" t="s">
@@ -11383,7 +11449,7 @@
       <c r="A58" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="B58" s="53" t="s">
+      <c r="B58" s="52" t="s">
         <v>124</v>
       </c>
       <c r="C58" s="54"/>
@@ -11398,7 +11464,7 @@
       <c r="A59" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="B59" s="53"/>
+      <c r="B59" s="52"/>
       <c r="C59" s="54"/>
       <c r="D59" s="54"/>
       <c r="E59" s="47" t="s">
@@ -11409,7 +11475,7 @@
       <c r="A60" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="B60" s="53"/>
+      <c r="B60" s="52"/>
       <c r="C60" s="54"/>
       <c r="D60" s="54"/>
       <c r="E60" s="47" t="s">
@@ -11420,7 +11486,7 @@
       <c r="A61" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="B61" s="53" t="s">
+      <c r="B61" s="52" t="s">
         <v>131</v>
       </c>
       <c r="C61" s="54"/>
@@ -11435,7 +11501,7 @@
       <c r="A62" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="B62" s="53"/>
+      <c r="B62" s="52"/>
       <c r="C62" s="54"/>
       <c r="D62" s="54"/>
       <c r="E62" s="47" t="s">
@@ -11446,7 +11512,7 @@
       <c r="A63" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="B63" s="53"/>
+      <c r="B63" s="52"/>
       <c r="C63" s="54"/>
       <c r="D63" s="54"/>
       <c r="E63" s="47" t="s">
@@ -11457,7 +11523,7 @@
       <c r="A64" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="B64" s="53" t="s">
+      <c r="B64" s="52" t="s">
         <v>159</v>
       </c>
       <c r="C64" s="54"/>
@@ -11472,7 +11538,7 @@
       <c r="A65" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="B65" s="53"/>
+      <c r="B65" s="52"/>
       <c r="C65" s="54"/>
       <c r="D65" s="54"/>
       <c r="E65" s="47" t="s">
@@ -11483,7 +11549,7 @@
       <c r="A66" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="B66" s="53" t="s">
+      <c r="B66" s="52" t="s">
         <v>164</v>
       </c>
       <c r="C66" s="54"/>
@@ -11498,7 +11564,7 @@
       <c r="A67" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="B67" s="53"/>
+      <c r="B67" s="52"/>
       <c r="C67" s="54"/>
       <c r="D67" s="54"/>
       <c r="E67" s="47" t="s">
@@ -11509,7 +11575,7 @@
       <c r="A68" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="B68" s="53"/>
+      <c r="B68" s="52"/>
       <c r="C68" s="54"/>
       <c r="D68" s="54"/>
       <c r="E68" s="47" t="s">
@@ -11520,7 +11586,7 @@
       <c r="A69" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="B69" s="53" t="s">
+      <c r="B69" s="52" t="s">
         <v>179</v>
       </c>
       <c r="C69" s="54"/>
@@ -11535,7 +11601,7 @@
       <c r="A70" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="B70" s="53"/>
+      <c r="B70" s="52"/>
       <c r="C70" s="54"/>
       <c r="D70" s="54"/>
       <c r="E70" s="47" t="s">
@@ -11546,7 +11612,7 @@
       <c r="A71" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="B71" s="53"/>
+      <c r="B71" s="52"/>
       <c r="C71" s="54"/>
       <c r="D71" s="54"/>
       <c r="E71" s="47" t="s">
@@ -11557,7 +11623,7 @@
       <c r="A72" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="B72" s="53" t="s">
+      <c r="B72" s="52" t="s">
         <v>186</v>
       </c>
       <c r="C72" s="54"/>
@@ -11572,7 +11638,7 @@
       <c r="A73" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="B73" s="53"/>
+      <c r="B73" s="52"/>
       <c r="C73" s="54"/>
       <c r="D73" s="54"/>
       <c r="E73" s="47" t="s">
@@ -11583,7 +11649,7 @@
       <c r="A74" s="38" t="s">
         <v>194</v>
       </c>
-      <c r="B74" s="53" t="s">
+      <c r="B74" s="52" t="s">
         <v>195</v>
       </c>
       <c r="C74" s="54"/>
@@ -11598,7 +11664,7 @@
       <c r="A75" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="B75" s="53"/>
+      <c r="B75" s="52"/>
       <c r="C75" s="54"/>
       <c r="D75" s="54"/>
       <c r="E75" s="47" t="s">
@@ -11609,7 +11675,7 @@
       <c r="A76" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="B76" s="53" t="s">
+      <c r="B76" s="52" t="s">
         <v>200</v>
       </c>
       <c r="C76" s="54"/>
@@ -11624,7 +11690,7 @@
       <c r="A77" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="B77" s="53"/>
+      <c r="B77" s="52"/>
       <c r="C77" s="54"/>
       <c r="D77" s="54"/>
       <c r="E77" s="47" t="s">
@@ -11635,7 +11701,7 @@
       <c r="A78" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="B78" s="53" t="s">
+      <c r="B78" s="52" t="s">
         <v>211</v>
       </c>
       <c r="C78" s="54"/>
@@ -11650,7 +11716,7 @@
       <c r="A79" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="B79" s="53"/>
+      <c r="B79" s="52"/>
       <c r="C79" s="54"/>
       <c r="D79" s="54"/>
       <c r="E79" s="47" t="s">
@@ -11661,7 +11727,7 @@
       <c r="A80" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="B80" s="53"/>
+      <c r="B80" s="52"/>
       <c r="C80" s="54"/>
       <c r="D80" s="54"/>
       <c r="E80" s="47" t="s">
@@ -11672,7 +11738,7 @@
       <c r="A81" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="B81" s="53" t="s">
+      <c r="B81" s="52" t="s">
         <v>223</v>
       </c>
       <c r="C81" s="54"/>
@@ -11687,7 +11753,7 @@
       <c r="A82" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="B82" s="53"/>
+      <c r="B82" s="52"/>
       <c r="C82" s="54"/>
       <c r="D82" s="54"/>
       <c r="E82" s="47" t="s">
@@ -11698,7 +11764,7 @@
       <c r="A83" s="38" t="s">
         <v>227</v>
       </c>
-      <c r="B83" s="53" t="s">
+      <c r="B83" s="52" t="s">
         <v>228</v>
       </c>
       <c r="C83" s="54"/>
@@ -11713,7 +11779,7 @@
       <c r="A84" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="B84" s="53"/>
+      <c r="B84" s="52"/>
       <c r="C84" s="54"/>
       <c r="D84" s="54"/>
       <c r="E84" s="47" t="s">
@@ -11724,7 +11790,7 @@
       <c r="A85" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="B85" s="53"/>
+      <c r="B85" s="52"/>
       <c r="C85" s="54"/>
       <c r="D85" s="54"/>
       <c r="E85" s="47" t="s">
@@ -11791,91 +11857,204 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="38" t="s">
+    <row r="90" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="65" t="s">
+        <v>464</v>
+      </c>
+      <c r="B90" s="68" t="s">
+        <v>465</v>
+      </c>
+      <c r="C90" s="54"/>
+      <c r="D90" s="67" t="s">
+        <v>581</v>
+      </c>
+      <c r="E90" s="47"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="65" t="s">
+        <v>467</v>
+      </c>
+      <c r="B91" s="68"/>
+      <c r="C91" s="54"/>
+      <c r="D91" s="67"/>
+      <c r="E91" s="47"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="65"/>
+      <c r="B92" s="69"/>
+      <c r="C92" s="51"/>
+      <c r="D92" s="66"/>
+      <c r="E92" s="47"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="65"/>
+      <c r="B93" s="69"/>
+      <c r="C93" s="51"/>
+      <c r="D93" s="66"/>
+      <c r="E93" s="47"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="65"/>
+      <c r="B94" s="69"/>
+      <c r="C94" s="51"/>
+      <c r="D94" s="66"/>
+      <c r="E94" s="47"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="65"/>
+      <c r="B95" s="69"/>
+      <c r="C95" s="51"/>
+      <c r="D95" s="66"/>
+      <c r="E95" s="47"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="65"/>
+      <c r="B96" s="69"/>
+      <c r="C96" s="51"/>
+      <c r="D96" s="66"/>
+      <c r="E96" s="47"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="65"/>
+      <c r="B97" s="69"/>
+      <c r="C97" s="51"/>
+      <c r="D97" s="66"/>
+      <c r="E97" s="47"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="65"/>
+      <c r="B98" s="69"/>
+      <c r="C98" s="51"/>
+      <c r="D98" s="66"/>
+      <c r="E98" s="47"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="65"/>
+      <c r="B99" s="69"/>
+      <c r="C99" s="51"/>
+      <c r="D99" s="66"/>
+      <c r="E99" s="47"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="65"/>
+      <c r="B100" s="69"/>
+      <c r="C100" s="51"/>
+      <c r="D100" s="66"/>
+      <c r="E100" s="47"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="65"/>
+      <c r="B101" s="69"/>
+      <c r="C101" s="51"/>
+      <c r="D101" s="66"/>
+      <c r="E101" s="47"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="65"/>
+      <c r="B102" s="69"/>
+      <c r="C102" s="51"/>
+      <c r="D102" s="66"/>
+      <c r="E102" s="47"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="38" t="s">
         <v>477</v>
       </c>
-      <c r="B90" s="53" t="s">
+      <c r="B103" s="52" t="s">
         <v>478</v>
       </c>
-      <c r="C90" s="54"/>
-      <c r="D90" s="54" t="s">
+      <c r="C103" s="54"/>
+      <c r="D103" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="E90" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="39" t="s">
+      <c r="E103" s="47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="39" t="s">
         <v>480</v>
       </c>
-      <c r="B91" s="59"/>
-      <c r="C91" s="60"/>
-      <c r="D91" s="60"/>
-      <c r="E91" s="49" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C93" s="50">
-        <f>COUNTBLANK(C2:C91)</f>
-        <v>84</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C94" s="50">
-        <f>COUNTA(C2:C91)</f>
+      <c r="B104" s="53"/>
+      <c r="C104" s="55"/>
+      <c r="D104" s="55"/>
+      <c r="E104" s="49" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C106" s="50">
+        <f>COUNTBLANK(C2:C104)</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C107" s="50">
+        <f>COUNTA(C2:C104)</f>
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="120">
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="D90:D91"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="D83:D85"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="C78:C80"/>
-    <mergeCell ref="D78:D80"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="C66:C68"/>
-    <mergeCell ref="D66:D68"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="C69:C71"/>
-    <mergeCell ref="D69:D71"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="C61:C63"/>
-    <mergeCell ref="D61:D63"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="D58:D60"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="D53:D55"/>
+  <mergeCells count="123">
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="D38:D39"/>
@@ -11892,65 +12071,54 @@
     <mergeCell ref="C36:C37"/>
     <mergeCell ref="D36:D37"/>
     <mergeCell ref="E36:E37"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="D58:D60"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="C66:C68"/>
+    <mergeCell ref="D66:D68"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="C69:C71"/>
+    <mergeCell ref="D69:D71"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="C61:C63"/>
+    <mergeCell ref="D61:D63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="C78:C80"/>
+    <mergeCell ref="D78:D80"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="C103:C104"/>
+    <mergeCell ref="D103:D104"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="D83:D85"/>
+    <mergeCell ref="D90:D91"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="C90:C91"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12358,10 +12526,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A026136A-3463-4F46-9920-D2EEED3E1AFC}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12371,9 +12539,17 @@
     <col min="3" max="3" width="38.85546875" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="66.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -12390,7 +12566,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>365</v>
       </c>
@@ -12404,8 +12580,29 @@
         <v>101901</v>
       </c>
       <c r="E2" s="20"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I2" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>568</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>569</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>370</v>
       </c>
@@ -12419,8 +12616,29 @@
         <v>100167</v>
       </c>
       <c r="E3" s="21"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>5676</v>
+      </c>
+      <c r="J3" t="s">
+        <v>573</v>
+      </c>
+      <c r="K3">
+        <v>100167</v>
+      </c>
+      <c r="L3" t="s">
+        <v>576</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>5</v>
+      </c>
+      <c r="O3" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>373</v>
       </c>
@@ -12434,8 +12652,29 @@
         <v>102341</v>
       </c>
       <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>6830</v>
+      </c>
+      <c r="J4" t="s">
+        <v>574</v>
+      </c>
+      <c r="K4">
+        <v>101901</v>
+      </c>
+      <c r="L4" t="s">
+        <v>576</v>
+      </c>
+      <c r="M4">
+        <v>78</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+      <c r="O4" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>376</v>
       </c>
@@ -12449,8 +12688,29 @@
         <v>101901</v>
       </c>
       <c r="E5" s="21"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>7114</v>
+      </c>
+      <c r="J5" t="s">
+        <v>575</v>
+      </c>
+      <c r="K5">
+        <v>102341</v>
+      </c>
+      <c r="L5" t="s">
+        <v>576</v>
+      </c>
+      <c r="M5">
+        <v>19</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>378</v>
       </c>
@@ -12465,7 +12725,7 @@
       </c>
       <c r="E6" s="20"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>380</v>
       </c>
@@ -12480,7 +12740,7 @@
       </c>
       <c r="E7" s="21"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>382</v>
       </c>
@@ -12495,7 +12755,7 @@
       </c>
       <c r="E8" s="20"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>384</v>
       </c>
@@ -12510,7 +12770,7 @@
       </c>
       <c r="E9" s="21"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>386</v>
       </c>
@@ -12524,6 +12784,9 @@
         <v>102341</v>
       </c>
       <c r="E10" s="20"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12960,14 +13223,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13194,27 +13455,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13239,9 +13493,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
All SERD files tested
</commit_message>
<xml_diff>
--- a/analysis/MEDS_Tables.xlsx
+++ b/analysis/MEDS_Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="542" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{2209F74E-171A-4417-98E5-6E2B3EE17EC4}"/>
+  <xr:revisionPtr revIDLastSave="550" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B40B32B-0EB6-4976-B3AE-F6D6FDE56444}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meds_tables" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2547" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2673" uniqueCount="583">
   <si>
     <t>Table</t>
   </si>
@@ -1947,15 +1947,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color rgb="FF9C5700"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
+      <sz val="20"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2172,7 +2172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -2363,43 +2363,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -2517,7 +2480,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2579,60 +2542,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="19" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2641,25 +2565,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2668,11 +2598,24 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -10705,1426 +10648,2184 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8FA477-9B46-4053-B7AD-310B8B9F2B30}">
-  <dimension ref="A1:I107"/>
+  <dimension ref="A1:P143"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G73" sqref="G73"/>
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="63.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="3:16" s="40" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="D1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="E1" s="56" t="s">
         <v>539</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="F1" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="G1" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="F1"/>
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="I1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="H1" s="60"/>
+      <c r="I1" s="41">
+        <f>E141/E140</f>
+        <v>7.03125E-2</v>
+      </c>
+      <c r="J1" s="61" t="s">
+        <v>566</v>
+      </c>
+      <c r="K1" s="60"/>
+    </row>
+    <row r="2" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="D2" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="E2" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="F2" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="62" t="s">
+      <c r="G2" s="55" t="s">
         <v>564</v>
       </c>
-      <c r="G2" s="55">
-        <f>C107/C106</f>
-        <v>6.1855670103092786E-2</v>
-      </c>
-      <c r="H2" s="56" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+    </row>
+    <row r="3" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="59"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="56"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="D3" s="44"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="49"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="36"/>
+      <c r="P3" s="36"/>
+    </row>
+    <row r="4" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="59"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="56"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="D4" s="44"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="49"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
+    </row>
+    <row r="5" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="D5" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="E5" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="F5" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="G5" s="49" t="s">
         <v>519</v>
       </c>
-      <c r="G5" s="55"/>
-      <c r="H5" s="56"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="K5" s="36"/>
+      <c r="L5" s="58" t="s">
+        <v>464</v>
+      </c>
+      <c r="M5" s="59" t="s">
+        <v>465</v>
+      </c>
+      <c r="N5" s="46"/>
+      <c r="O5" s="48" t="s">
+        <v>581</v>
+      </c>
+      <c r="P5" s="36"/>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C6" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="59"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="D6" s="44"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="49"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="58" t="s">
+        <v>467</v>
+      </c>
+      <c r="M6" s="59"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="36"/>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C7" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="D7" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="E7" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="58" t="s">
+      <c r="F7" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="G7" s="49" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="36"/>
+      <c r="O7" s="36"/>
+      <c r="P7" s="36"/>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C8" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="59"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="D8" s="44"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="49"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="36"/>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C9" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="D9" s="44" t="s">
         <v>171</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="E9" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="58" t="s">
+      <c r="F9" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="59" t="s">
+      <c r="G9" s="49" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C10" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
+      <c r="D10" s="44"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="49"/>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C11" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="59"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="D11" s="44"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="49"/>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C12" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="B12" s="57" t="s">
+      <c r="D12" s="44" t="s">
         <v>204</v>
       </c>
-      <c r="C12" s="58" t="s">
+      <c r="E12" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="58" t="s">
+      <c r="F12" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="59" t="s">
+      <c r="G12" s="49" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C13" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="59"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
+      <c r="D13" s="44"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="49"/>
+    </row>
+    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C14" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="B14" s="57" t="s">
+      <c r="D14" s="44" t="s">
         <v>361</v>
       </c>
-      <c r="C14" s="58" t="s">
+      <c r="E14" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="58" t="s">
+      <c r="F14" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="59" t="s">
+      <c r="G14" s="49" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
+    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C15" s="35" t="s">
         <v>363</v>
       </c>
-      <c r="B15" s="63"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="65"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
+      <c r="D15" s="45"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="50"/>
+    </row>
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C16" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="60" t="s">
+      <c r="D16" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="61"/>
-      <c r="D16" s="61" t="s">
+      <c r="E16" s="51"/>
+      <c r="F16" s="51" t="s">
         <v>567</v>
       </c>
-      <c r="E16" s="62" t="s">
+      <c r="G16" s="55" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="38" t="s">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="59"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="38" t="s">
+      <c r="D17" s="44"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="49"/>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="D18" s="44" t="s">
         <v>105</v>
       </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58" t="s">
+      <c r="E18" s="46"/>
+      <c r="F18" s="46" t="s">
         <v>567</v>
       </c>
-      <c r="E18" s="59" t="s">
+      <c r="G18" s="49" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="38" t="s">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="B19" s="57"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="59"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
+      <c r="D19" s="44"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="49"/>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="B20" s="57" t="s">
+      <c r="D20" s="44" t="s">
         <v>300</v>
       </c>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58" t="s">
+      <c r="E20" s="46"/>
+      <c r="F20" s="46" t="s">
         <v>567</v>
       </c>
-      <c r="E20" s="59" t="s">
+      <c r="G20" s="49" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="38" t="s">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="B21" s="57"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="59"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
+      <c r="D21" s="44"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="49"/>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="B22" s="57" t="s">
+      <c r="D22" s="44" t="s">
         <v>305</v>
       </c>
-      <c r="C22" s="58"/>
-      <c r="D22" s="58" t="s">
+      <c r="E22" s="46"/>
+      <c r="F22" s="46" t="s">
         <v>567</v>
       </c>
-      <c r="E22" s="59" t="s">
+      <c r="G22" s="49" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="s">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="B23" s="57"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="59"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
+      <c r="D23" s="44"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="49"/>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="B24" s="57"/>
-      <c r="C24" s="58"/>
-      <c r="D24" s="58" t="s">
+      <c r="D24" s="44"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="49"/>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C25" s="34" t="s">
+        <v>311</v>
+      </c>
+      <c r="D25" s="44"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="49"/>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C26" s="34" t="s">
+        <v>317</v>
+      </c>
+      <c r="D26" s="44" t="s">
+        <v>318</v>
+      </c>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46" t="s">
         <v>567</v>
       </c>
-      <c r="E24" s="59"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
+      <c r="G26" s="49" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C27" s="34" t="s">
+        <v>320</v>
+      </c>
+      <c r="D27" s="44"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="49"/>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="D28" s="53" t="s">
+        <v>323</v>
+      </c>
+      <c r="E28" s="54"/>
+      <c r="F28" s="46" t="s">
+        <v>567</v>
+      </c>
+      <c r="G28" s="49" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C29" s="34" t="s">
+        <v>325</v>
+      </c>
+      <c r="D29" s="53"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="49"/>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="34" t="s">
+        <v>327</v>
+      </c>
+      <c r="D30" s="44" t="s">
+        <v>328</v>
+      </c>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46" t="s">
+        <v>567</v>
+      </c>
+      <c r="G30" s="49" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="34" t="s">
+        <v>330</v>
+      </c>
+      <c r="D31" s="44"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="49"/>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="34" t="s">
+        <v>332</v>
+      </c>
+      <c r="D32" s="44" t="s">
+        <v>333</v>
+      </c>
+      <c r="E32" s="46"/>
+      <c r="F32" s="46" t="s">
+        <v>567</v>
+      </c>
+      <c r="G32" s="49" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="33" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C33" s="34" t="s">
+        <v>335</v>
+      </c>
+      <c r="D33" s="44"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="49"/>
+    </row>
+    <row r="34" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C34" s="34" t="s">
+        <v>337</v>
+      </c>
+      <c r="D34" s="44" t="s">
+        <v>338</v>
+      </c>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46" t="s">
+        <v>567</v>
+      </c>
+      <c r="G34" s="49" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="35" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C35" s="34" t="s">
+        <v>340</v>
+      </c>
+      <c r="D35" s="44"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="49"/>
+    </row>
+    <row r="36" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C36" s="34" t="s">
+        <v>342</v>
+      </c>
+      <c r="D36" s="44" t="s">
+        <v>343</v>
+      </c>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46" t="s">
+        <v>567</v>
+      </c>
+      <c r="G36" s="49" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="37" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C37" s="34" t="s">
+        <v>345</v>
+      </c>
+      <c r="D37" s="44"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="49"/>
+    </row>
+    <row r="38" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C38" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="D38" s="44" t="s">
+        <v>348</v>
+      </c>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46" t="s">
+        <v>567</v>
+      </c>
+      <c r="G38" s="49" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="39" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C39" s="35" t="s">
+        <v>350</v>
+      </c>
+      <c r="D39" s="45"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="50"/>
+    </row>
+    <row r="40" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C40" s="33" t="s">
+        <v>365</v>
+      </c>
+      <c r="D40" s="52" t="s">
+        <v>366</v>
+      </c>
+      <c r="E40" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" s="51" t="s">
+        <v>369</v>
+      </c>
+      <c r="G40" s="55" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="41" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C41" s="34" t="s">
+        <v>376</v>
+      </c>
+      <c r="D41" s="44"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="49"/>
+    </row>
+    <row r="42" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C42" s="34" t="s">
+        <v>382</v>
+      </c>
+      <c r="D42" s="44"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="49"/>
+    </row>
+    <row r="43" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C43" s="34" t="s">
+        <v>370</v>
+      </c>
+      <c r="D43" s="44" t="s">
+        <v>371</v>
+      </c>
+      <c r="E43" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="F43" s="46" t="s">
+        <v>369</v>
+      </c>
+      <c r="G43" s="49" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="44" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C44" s="34" t="s">
+        <v>378</v>
+      </c>
+      <c r="D44" s="44"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="49"/>
+    </row>
+    <row r="45" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C45" s="34" t="s">
+        <v>384</v>
+      </c>
+      <c r="D45" s="44"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="49"/>
+    </row>
+    <row r="46" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C46" s="34" t="s">
+        <v>373</v>
+      </c>
+      <c r="D46" s="44" t="s">
+        <v>374</v>
+      </c>
+      <c r="E46" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="F46" s="46" t="s">
+        <v>369</v>
+      </c>
+      <c r="G46" s="49" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="47" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C47" s="34" t="s">
+        <v>380</v>
+      </c>
+      <c r="D47" s="44"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="49"/>
+    </row>
+    <row r="48" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C48" s="35" t="s">
+        <v>386</v>
+      </c>
+      <c r="D48" s="45"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="50"/>
+      <c r="J48" s="36"/>
+      <c r="K48" s="36"/>
+      <c r="L48" s="36"/>
+      <c r="M48" s="36"/>
+    </row>
+    <row r="49" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C49" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D49" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="E49" s="51"/>
+      <c r="F49" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="G49" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J49" s="36"/>
+      <c r="K49" s="36"/>
+      <c r="L49" s="36"/>
+      <c r="M49" s="36"/>
+    </row>
+    <row r="50" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C50" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D50" s="44"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J50" s="36"/>
+      <c r="K50" s="36"/>
+      <c r="L50" s="36"/>
+      <c r="M50" s="36"/>
+    </row>
+    <row r="51" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C51" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D51" s="44"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="46"/>
+      <c r="G51" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J51" s="36"/>
+      <c r="K51" s="36"/>
+      <c r="L51" s="36"/>
+      <c r="M51" s="36"/>
+    </row>
+    <row r="52" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C52" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D52" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="E52" s="46"/>
+      <c r="F52" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G52" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J52" s="36"/>
+      <c r="K52" s="36"/>
+      <c r="L52" s="36"/>
+      <c r="M52" s="36"/>
+    </row>
+    <row r="53" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C53" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D53" s="44"/>
+      <c r="E53" s="46"/>
+      <c r="F53" s="46"/>
+      <c r="G53" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J53" s="36"/>
+      <c r="K53" s="36"/>
+      <c r="L53" s="36"/>
+      <c r="M53" s="36"/>
+    </row>
+    <row r="54" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C54" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D54" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E54" s="46"/>
+      <c r="F54" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G54" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J54" s="36"/>
+      <c r="K54" s="36"/>
+      <c r="L54" s="36"/>
+      <c r="M54" s="36"/>
+    </row>
+    <row r="55" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C55" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D55" s="44"/>
+      <c r="E55" s="46"/>
+      <c r="F55" s="46"/>
+      <c r="G55" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J55" s="36"/>
+      <c r="K55" s="36"/>
+      <c r="L55" s="36"/>
+      <c r="M55" s="36"/>
+    </row>
+    <row r="56" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C56" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="D56" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="E56" s="46"/>
+      <c r="F56" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G56" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J56" s="36"/>
+      <c r="K56" s="36"/>
+      <c r="L56" s="36"/>
+      <c r="M56" s="36"/>
+    </row>
+    <row r="57" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C57" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D57" s="44"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J57" s="36"/>
+      <c r="K57" s="36"/>
+      <c r="L57" s="36"/>
+      <c r="M57" s="36"/>
+    </row>
+    <row r="58" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C58" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D58" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="E58" s="46"/>
+      <c r="F58" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G58" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J58" s="36"/>
+      <c r="K58" s="36"/>
+      <c r="L58" s="36"/>
+      <c r="M58" s="36"/>
+    </row>
+    <row r="59" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C59" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="D59" s="44"/>
+      <c r="E59" s="46"/>
+      <c r="F59" s="46"/>
+      <c r="G59" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J59" s="36"/>
+      <c r="K59" s="36"/>
+      <c r="L59" s="36"/>
+      <c r="M59" s="36"/>
+    </row>
+    <row r="60" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C60" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="D60" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="E60" s="46"/>
+      <c r="F60" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G60" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J60" s="36"/>
+      <c r="K60" s="36"/>
+      <c r="L60" s="36"/>
+      <c r="M60" s="36"/>
+    </row>
+    <row r="61" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C61" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="D61" s="44"/>
+      <c r="E61" s="46"/>
+      <c r="F61" s="46"/>
+      <c r="G61" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J61" s="36"/>
+      <c r="K61" s="36"/>
+      <c r="L61" s="36"/>
+      <c r="M61" s="36"/>
+    </row>
+    <row r="62" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C62" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="D62" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="E62" s="46"/>
+      <c r="F62" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G62" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J62" s="36"/>
+      <c r="K62" s="36"/>
+      <c r="L62" s="36"/>
+      <c r="M62" s="36"/>
+    </row>
+    <row r="63" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C63" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="D63" s="44"/>
+      <c r="E63" s="46"/>
+      <c r="F63" s="46"/>
+      <c r="G63" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J63" s="36"/>
+      <c r="K63" s="36"/>
+      <c r="L63" s="36"/>
+      <c r="M63" s="36"/>
+    </row>
+    <row r="64" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C64" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="D64" s="44"/>
+      <c r="E64" s="46"/>
+      <c r="F64" s="46"/>
+      <c r="G64" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J64" s="36"/>
+      <c r="K64" s="36"/>
+      <c r="L64" s="36"/>
+      <c r="M64" s="36"/>
+    </row>
+    <row r="65" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C65" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="D65" s="44" t="s">
+        <v>204</v>
+      </c>
+      <c r="E65" s="46"/>
+      <c r="F65" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G65" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J65" s="36"/>
+      <c r="K65" s="36"/>
+      <c r="L65" s="36"/>
+      <c r="M65" s="36"/>
+    </row>
+    <row r="66" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C66" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="D66" s="44"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J66" s="36"/>
+      <c r="K66" s="36"/>
+      <c r="L66" s="36"/>
+      <c r="M66" s="36"/>
+    </row>
+    <row r="67" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C67" s="34" t="s">
+        <v>299</v>
+      </c>
+      <c r="D67" s="44" t="s">
+        <v>300</v>
+      </c>
+      <c r="E67" s="46"/>
+      <c r="F67" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G67" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J67" s="36"/>
+      <c r="K67" s="36"/>
+      <c r="L67" s="36"/>
+      <c r="M67" s="36"/>
+    </row>
+    <row r="68" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C68" s="34" t="s">
+        <v>302</v>
+      </c>
+      <c r="D68" s="44"/>
+      <c r="E68" s="46"/>
+      <c r="F68" s="46"/>
+      <c r="G68" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J68" s="36"/>
+      <c r="K68" s="36"/>
+      <c r="L68" s="36"/>
+      <c r="M68" s="36"/>
+    </row>
+    <row r="69" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C69" s="34" t="s">
+        <v>304</v>
+      </c>
+      <c r="D69" s="44" t="s">
+        <v>305</v>
+      </c>
+      <c r="E69" s="46"/>
+      <c r="F69" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G69" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J69" s="36"/>
+      <c r="K69" s="36"/>
+      <c r="L69" s="36"/>
+      <c r="M69" s="36"/>
+    </row>
+    <row r="70" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C70" s="34" t="s">
+        <v>309</v>
+      </c>
+      <c r="D70" s="44"/>
+      <c r="E70" s="46"/>
+      <c r="F70" s="46"/>
+      <c r="G70" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J70" s="36"/>
+      <c r="K70" s="36"/>
+      <c r="L70" s="36"/>
+      <c r="M70" s="36"/>
+    </row>
+    <row r="71" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C71" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="D71" s="44"/>
+      <c r="E71" s="46"/>
+      <c r="F71" s="46"/>
+      <c r="G71" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J71" s="36"/>
+      <c r="K71" s="36"/>
+      <c r="L71" s="36"/>
+      <c r="M71" s="36"/>
+    </row>
+    <row r="72" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C72" s="34" t="s">
         <v>311</v>
       </c>
-      <c r="B25" s="57"/>
-      <c r="C25" s="58"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="59"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="38" t="s">
+      <c r="D72" s="44"/>
+      <c r="E72" s="46"/>
+      <c r="F72" s="46"/>
+      <c r="G72" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J72" s="36"/>
+      <c r="K72" s="36"/>
+      <c r="L72" s="36"/>
+      <c r="M72" s="36"/>
+    </row>
+    <row r="73" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C73" s="34" t="s">
         <v>317</v>
       </c>
-      <c r="B26" s="57" t="s">
+      <c r="D73" s="44" t="s">
         <v>318</v>
       </c>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58" t="s">
-        <v>567</v>
-      </c>
-      <c r="E26" s="59" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
+      <c r="E73" s="46"/>
+      <c r="F73" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G73" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J73" s="36"/>
+      <c r="K73" s="36"/>
+      <c r="L73" s="36"/>
+      <c r="M73" s="36"/>
+    </row>
+    <row r="74" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C74" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="B27" s="57"/>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="59"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="38" t="s">
+      <c r="D74" s="44"/>
+      <c r="E74" s="46"/>
+      <c r="F74" s="46"/>
+      <c r="G74" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J74" s="36"/>
+      <c r="K74" s="36"/>
+      <c r="L74" s="36"/>
+      <c r="M74" s="36"/>
+    </row>
+    <row r="75" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C75" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="B28" s="66" t="s">
+      <c r="D75" s="53" t="s">
         <v>323</v>
       </c>
-      <c r="C28" s="67"/>
-      <c r="D28" s="58" t="s">
-        <v>567</v>
-      </c>
-      <c r="E28" s="59" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="38" t="s">
+      <c r="E75" s="46"/>
+      <c r="F75" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G75" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J75" s="36"/>
+      <c r="K75" s="36"/>
+      <c r="L75" s="36"/>
+      <c r="M75" s="36"/>
+    </row>
+    <row r="76" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C76" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="B29" s="66"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="58"/>
-      <c r="E29" s="59"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="38" t="s">
+      <c r="D76" s="53"/>
+      <c r="E76" s="46"/>
+      <c r="F76" s="46"/>
+      <c r="G76" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="77" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C77" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="B30" s="57" t="s">
+      <c r="D77" s="44" t="s">
         <v>328</v>
       </c>
-      <c r="C30" s="58"/>
-      <c r="D30" s="58" t="s">
-        <v>567</v>
-      </c>
-      <c r="E30" s="59" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="38" t="s">
+      <c r="E77" s="46"/>
+      <c r="F77" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G77" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="78" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C78" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="B31" s="57"/>
-      <c r="C31" s="58"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="59"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="38" t="s">
+      <c r="D78" s="44"/>
+      <c r="E78" s="46"/>
+      <c r="F78" s="46"/>
+      <c r="G78" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="79" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C79" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="B32" s="57" t="s">
+      <c r="D79" s="44" t="s">
         <v>333</v>
       </c>
-      <c r="C32" s="58"/>
-      <c r="D32" s="58" t="s">
-        <v>567</v>
-      </c>
-      <c r="E32" s="59" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="38" t="s">
+      <c r="E79" s="46"/>
+      <c r="F79" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G79" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="80" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C80" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="B33" s="57"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="59"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="38" t="s">
+      <c r="D80" s="44"/>
+      <c r="E80" s="46"/>
+      <c r="F80" s="46"/>
+      <c r="G80" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C81" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="B34" s="57" t="s">
+      <c r="D81" s="44" t="s">
         <v>338</v>
       </c>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58" t="s">
-        <v>567</v>
-      </c>
-      <c r="E34" s="59" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="38" t="s">
+      <c r="E81" s="46"/>
+      <c r="F81" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G81" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C82" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="B35" s="57"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="59"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="38" t="s">
+      <c r="D82" s="44"/>
+      <c r="E82" s="46"/>
+      <c r="F82" s="46"/>
+      <c r="G82" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C83" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="B36" s="57" t="s">
+      <c r="D83" s="44" t="s">
         <v>343</v>
       </c>
-      <c r="C36" s="58"/>
-      <c r="D36" s="58" t="s">
-        <v>567</v>
-      </c>
-      <c r="E36" s="59" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="38" t="s">
+      <c r="E83" s="46"/>
+      <c r="F83" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G83" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C84" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="B37" s="57"/>
-      <c r="C37" s="58"/>
-      <c r="D37" s="58"/>
-      <c r="E37" s="59"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="38" t="s">
+      <c r="D84" s="44"/>
+      <c r="E84" s="46"/>
+      <c r="F84" s="46"/>
+      <c r="G84" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C85" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="B38" s="57" t="s">
+      <c r="D85" s="44" t="s">
         <v>348</v>
       </c>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58" t="s">
-        <v>567</v>
-      </c>
-      <c r="E38" s="59" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="39" t="s">
+      <c r="E85" s="46"/>
+      <c r="F85" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G85" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C86" s="34" t="s">
         <v>350</v>
       </c>
-      <c r="B39" s="63"/>
-      <c r="C39" s="64"/>
-      <c r="D39" s="64"/>
-      <c r="E39" s="65"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="37" t="s">
+      <c r="D86" s="44"/>
+      <c r="E86" s="46"/>
+      <c r="F86" s="46"/>
+      <c r="G86" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C87" s="34" t="s">
+        <v>360</v>
+      </c>
+      <c r="D87" s="44" t="s">
+        <v>361</v>
+      </c>
+      <c r="E87" s="46"/>
+      <c r="F87" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G87" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C88" s="34" t="s">
+        <v>363</v>
+      </c>
+      <c r="D88" s="44"/>
+      <c r="E88" s="46"/>
+      <c r="F88" s="46"/>
+      <c r="G88" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C89" s="34" t="s">
         <v>365</v>
       </c>
-      <c r="B40" s="40" t="s">
+      <c r="D89" s="44" t="s">
         <v>366</v>
       </c>
-      <c r="C40" s="41"/>
-      <c r="D40" s="61" t="s">
-        <v>369</v>
-      </c>
-      <c r="E40" s="42" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="38" t="s">
+      <c r="E89" s="46"/>
+      <c r="F89" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G89" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C90" s="34" t="s">
+        <v>376</v>
+      </c>
+      <c r="D90" s="44"/>
+      <c r="E90" s="46"/>
+      <c r="F90" s="46"/>
+      <c r="G90" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C91" s="34" t="s">
+        <v>382</v>
+      </c>
+      <c r="D91" s="44"/>
+      <c r="E91" s="46"/>
+      <c r="F91" s="46"/>
+      <c r="G91" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C92" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="B41" s="43" t="s">
+      <c r="D92" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="C41" s="44"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="45" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="38" t="s">
+      <c r="E92" s="46"/>
+      <c r="F92" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G92" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C93" s="34" t="s">
+        <v>378</v>
+      </c>
+      <c r="D93" s="44"/>
+      <c r="E93" s="46"/>
+      <c r="F93" s="46"/>
+      <c r="G93" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C94" s="34" t="s">
+        <v>384</v>
+      </c>
+      <c r="D94" s="44"/>
+      <c r="E94" s="46"/>
+      <c r="F94" s="46"/>
+      <c r="G94" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B95" s="37"/>
+      <c r="C95" s="36" t="s">
         <v>373</v>
       </c>
-      <c r="B42" s="43" t="s">
+      <c r="D95" s="44" t="s">
         <v>374</v>
       </c>
-      <c r="C42" s="44"/>
-      <c r="D42" s="58"/>
-      <c r="E42" s="45" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="38" t="s">
-        <v>376</v>
-      </c>
-      <c r="B43" s="43" t="s">
-        <v>366</v>
-      </c>
-      <c r="C43" s="44"/>
-      <c r="D43" s="58"/>
-      <c r="E43" s="45" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="38" t="s">
-        <v>378</v>
-      </c>
-      <c r="B44" s="43" t="s">
-        <v>371</v>
-      </c>
-      <c r="C44" s="44"/>
-      <c r="D44" s="58"/>
-      <c r="E44" s="45" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="38" t="s">
+      <c r="E95" s="46"/>
+      <c r="F95" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G95" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B96" s="37"/>
+      <c r="C96" s="36" t="s">
         <v>380</v>
       </c>
-      <c r="B45" s="43" t="s">
-        <v>374</v>
-      </c>
-      <c r="C45" s="44"/>
-      <c r="D45" s="58"/>
-      <c r="E45" s="45" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="38" t="s">
-        <v>382</v>
-      </c>
-      <c r="B46" s="43" t="s">
-        <v>366</v>
-      </c>
-      <c r="C46" s="44"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="45" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="38" t="s">
-        <v>384</v>
-      </c>
-      <c r="B47" s="43" t="s">
-        <v>371</v>
-      </c>
-      <c r="C47" s="44"/>
-      <c r="D47" s="58"/>
-      <c r="E47" s="45" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="38" t="s">
+      <c r="D96" s="44"/>
+      <c r="E96" s="46"/>
+      <c r="F96" s="46"/>
+      <c r="G96" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="97" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B97" s="37"/>
+      <c r="C97" s="36" t="s">
         <v>386</v>
       </c>
-      <c r="B48" s="43" t="s">
-        <v>374</v>
-      </c>
-      <c r="C48" s="44"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="45" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="B49" s="60" t="s">
-        <v>48</v>
-      </c>
-      <c r="C49" s="61"/>
-      <c r="D49" s="61" t="s">
+      <c r="D97" s="44"/>
+      <c r="E97" s="46"/>
+      <c r="F97" s="46"/>
+      <c r="G97" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J97" s="36"/>
+      <c r="K97" s="36"/>
+      <c r="L97" s="36"/>
+      <c r="M97" s="36"/>
+    </row>
+    <row r="98" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C98" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="D98" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="E98" s="46"/>
+      <c r="F98" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="E49" s="46" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" s="57"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="B51" s="57" t="s">
-        <v>65</v>
-      </c>
-      <c r="C51" s="58"/>
-      <c r="D51" s="58" t="s">
+      <c r="G98" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="I98" s="36"/>
+    </row>
+    <row r="99" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C99" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D99" s="44"/>
+      <c r="E99" s="46"/>
+      <c r="F99" s="46"/>
+      <c r="G99" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="100" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C100" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="D100" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="E100" s="46"/>
+      <c r="F100" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="E51" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="B52" s="57"/>
-      <c r="C52" s="58"/>
-      <c r="D52" s="58"/>
-      <c r="E52" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="38" t="s">
-        <v>109</v>
-      </c>
-      <c r="B53" s="57" t="s">
-        <v>110</v>
-      </c>
-      <c r="C53" s="58"/>
-      <c r="D53" s="58" t="s">
+      <c r="G100" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="101" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C101" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D101" s="44"/>
+      <c r="E101" s="46"/>
+      <c r="F101" s="46"/>
+      <c r="G101" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="102" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C102" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D102" s="44"/>
+      <c r="E102" s="46"/>
+      <c r="F102" s="46"/>
+      <c r="G102" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="103" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C103" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="D103" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="E103" s="46"/>
+      <c r="F103" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="E53" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="B54" s="57"/>
-      <c r="C54" s="58"/>
-      <c r="D54" s="58"/>
-      <c r="E54" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="38" t="s">
-        <v>114</v>
-      </c>
-      <c r="B55" s="57"/>
-      <c r="C55" s="58"/>
-      <c r="D55" s="58"/>
-      <c r="E55" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="38" t="s">
-        <v>118</v>
-      </c>
-      <c r="B56" s="57" t="s">
-        <v>119</v>
-      </c>
-      <c r="C56" s="58"/>
-      <c r="D56" s="58" t="s">
+      <c r="G103" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="104" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C104" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="D104" s="44"/>
+      <c r="E104" s="46"/>
+      <c r="F104" s="46"/>
+      <c r="G104" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="105" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C105" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="D105" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="E105" s="46"/>
+      <c r="F105" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="E56" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="B57" s="57"/>
-      <c r="C57" s="58"/>
-      <c r="D57" s="58"/>
-      <c r="E57" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="B58" s="57" t="s">
-        <v>124</v>
-      </c>
-      <c r="C58" s="58"/>
-      <c r="D58" s="58" t="s">
+      <c r="G105" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="106" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C106" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="D106" s="44"/>
+      <c r="E106" s="46"/>
+      <c r="F106" s="46"/>
+      <c r="G106" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="107" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C107" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="D107" s="44"/>
+      <c r="E107" s="46"/>
+      <c r="F107" s="46"/>
+      <c r="G107" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="108" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C108" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="D108" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="E108" s="46"/>
+      <c r="F108" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="B59" s="57"/>
-      <c r="C59" s="58"/>
-      <c r="D59" s="58"/>
-      <c r="E59" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="38" t="s">
+      <c r="G108" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="109" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C109" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="D109" s="44"/>
+      <c r="E109" s="46"/>
+      <c r="F109" s="46"/>
+      <c r="G109" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="110" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C110" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="D110" s="44"/>
+      <c r="E110" s="46"/>
+      <c r="F110" s="46"/>
+      <c r="G110" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="111" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C111" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="D111" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="E111" s="46"/>
+      <c r="F111" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G111" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="112" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C112" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="D112" s="44"/>
+      <c r="E112" s="46"/>
+      <c r="F112" s="46"/>
+      <c r="G112" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="113" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C113" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="D113" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="E113" s="46"/>
+      <c r="F113" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G113" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="114" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C114" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="D114" s="44"/>
+      <c r="E114" s="46"/>
+      <c r="F114" s="46"/>
+      <c r="G114" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="115" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C115" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="D115" s="44"/>
+      <c r="E115" s="46"/>
+      <c r="F115" s="46"/>
+      <c r="G115" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="116" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C116" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="D116" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="E116" s="46"/>
+      <c r="F116" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G116" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="117" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C117" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="D117" s="44"/>
+      <c r="E117" s="46"/>
+      <c r="F117" s="46"/>
+      <c r="G117" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="118" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C118" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="D118" s="44"/>
+      <c r="E118" s="46"/>
+      <c r="F118" s="46"/>
+      <c r="G118" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="119" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C119" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="D119" s="44" t="s">
+        <v>186</v>
+      </c>
+      <c r="E119" s="46"/>
+      <c r="F119" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G119" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="120" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C120" s="34" t="s">
+        <v>188</v>
+      </c>
+      <c r="D120" s="44"/>
+      <c r="E120" s="46"/>
+      <c r="F120" s="46"/>
+      <c r="G120" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="121" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C121" s="34" t="s">
+        <v>194</v>
+      </c>
+      <c r="D121" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="E121" s="46"/>
+      <c r="F121" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G121" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="122" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C122" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="D122" s="44"/>
+      <c r="E122" s="46"/>
+      <c r="F122" s="46"/>
+      <c r="G122" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="123" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C123" s="34" t="s">
+        <v>199</v>
+      </c>
+      <c r="D123" s="44" t="s">
+        <v>200</v>
+      </c>
+      <c r="E123" s="46"/>
+      <c r="F123" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G123" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="124" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C124" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="D124" s="44"/>
+      <c r="E124" s="46"/>
+      <c r="F124" s="46"/>
+      <c r="G124" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="125" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C125" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="D125" s="44" t="s">
+        <v>211</v>
+      </c>
+      <c r="E125" s="46"/>
+      <c r="F125" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G125" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="126" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C126" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="D126" s="44"/>
+      <c r="E126" s="46"/>
+      <c r="F126" s="46"/>
+      <c r="G126" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="127" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C127" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="D127" s="44"/>
+      <c r="E127" s="46"/>
+      <c r="F127" s="46"/>
+      <c r="G127" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="128" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C128" s="34" t="s">
+        <v>222</v>
+      </c>
+      <c r="D128" s="44" t="s">
+        <v>223</v>
+      </c>
+      <c r="E128" s="46"/>
+      <c r="F128" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G128" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C129" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="D129" s="44"/>
+      <c r="E129" s="46"/>
+      <c r="F129" s="46"/>
+      <c r="G129" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C130" s="34" t="s">
+        <v>227</v>
+      </c>
+      <c r="D130" s="44" t="s">
+        <v>228</v>
+      </c>
+      <c r="E130" s="46"/>
+      <c r="F130" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G130" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C131" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="D131" s="44"/>
+      <c r="E131" s="46"/>
+      <c r="F131" s="46"/>
+      <c r="G131" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C132" s="34" t="s">
+        <v>232</v>
+      </c>
+      <c r="D132" s="44"/>
+      <c r="E132" s="46"/>
+      <c r="F132" s="46"/>
+      <c r="G132" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C133" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="D133" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="E133" s="43"/>
+      <c r="F133" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="G133" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C134" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="D134" s="42" t="s">
+        <v>272</v>
+      </c>
+      <c r="E134" s="43"/>
+      <c r="F134" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="G134" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C135" s="34" t="s">
+        <v>275</v>
+      </c>
+      <c r="D135" s="42" t="s">
+        <v>276</v>
+      </c>
+      <c r="E135" s="43"/>
+      <c r="F135" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="G135" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C136" s="34" t="s">
+        <v>279</v>
+      </c>
+      <c r="D136" s="42" t="s">
+        <v>280</v>
+      </c>
+      <c r="E136" s="43"/>
+      <c r="F136" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="G136" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" s="36"/>
+      <c r="B137" s="36"/>
+      <c r="C137" s="34" t="s">
+        <v>477</v>
+      </c>
+      <c r="D137" s="44" t="s">
+        <v>478</v>
+      </c>
+      <c r="E137" s="46"/>
+      <c r="F137" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G137" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="H137" s="36"/>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="36"/>
+      <c r="B138" s="36"/>
+      <c r="C138" s="35" t="s">
+        <v>480</v>
+      </c>
+      <c r="D138" s="45"/>
+      <c r="E138" s="47"/>
+      <c r="F138" s="47"/>
+      <c r="G138" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="H138" s="36"/>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A139" s="36"/>
+      <c r="B139" s="36"/>
+      <c r="C139" s="36"/>
+      <c r="D139" s="36"/>
+      <c r="E139" s="43"/>
+      <c r="F139" s="57"/>
+      <c r="G139" s="36"/>
+      <c r="H139" s="36"/>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" s="36"/>
+      <c r="B140" s="36"/>
+      <c r="C140" s="36"/>
+      <c r="D140" s="36"/>
+      <c r="E140" s="43">
+        <f>COUNTBLANK(E2:E138)</f>
         <v>128</v>
       </c>
-      <c r="B60" s="57"/>
-      <c r="C60" s="58"/>
-      <c r="D60" s="58"/>
-      <c r="E60" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="38" t="s">
-        <v>130</v>
-      </c>
-      <c r="B61" s="57" t="s">
-        <v>131</v>
-      </c>
-      <c r="C61" s="58"/>
-      <c r="D61" s="58" t="s">
-        <v>18</v>
-      </c>
-      <c r="E61" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="B62" s="57"/>
-      <c r="C62" s="58"/>
-      <c r="D62" s="58"/>
-      <c r="E62" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="38" t="s">
-        <v>136</v>
-      </c>
-      <c r="B63" s="57"/>
-      <c r="C63" s="58"/>
-      <c r="D63" s="58"/>
-      <c r="E63" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="38" t="s">
-        <v>158</v>
-      </c>
-      <c r="B64" s="57" t="s">
-        <v>159</v>
-      </c>
-      <c r="C64" s="58"/>
-      <c r="D64" s="58" t="s">
-        <v>18</v>
-      </c>
-      <c r="E64" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="38" t="s">
-        <v>161</v>
-      </c>
-      <c r="B65" s="57"/>
-      <c r="C65" s="58"/>
-      <c r="D65" s="58"/>
-      <c r="E65" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="38" t="s">
-        <v>163</v>
-      </c>
-      <c r="B66" s="57" t="s">
-        <v>164</v>
-      </c>
-      <c r="C66" s="58"/>
-      <c r="D66" s="58" t="s">
-        <v>18</v>
-      </c>
-      <c r="E66" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="38" t="s">
-        <v>166</v>
-      </c>
-      <c r="B67" s="57"/>
-      <c r="C67" s="58"/>
-      <c r="D67" s="58"/>
-      <c r="E67" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="38" t="s">
-        <v>168</v>
-      </c>
-      <c r="B68" s="57"/>
-      <c r="C68" s="58"/>
-      <c r="D68" s="58"/>
-      <c r="E68" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="38" t="s">
-        <v>178</v>
-      </c>
-      <c r="B69" s="57" t="s">
-        <v>179</v>
-      </c>
-      <c r="C69" s="58"/>
-      <c r="D69" s="58" t="s">
-        <v>18</v>
-      </c>
-      <c r="E69" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="B70" s="57"/>
-      <c r="C70" s="58"/>
-      <c r="D70" s="58"/>
-      <c r="E70" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="38" t="s">
-        <v>183</v>
-      </c>
-      <c r="B71" s="57"/>
-      <c r="C71" s="58"/>
-      <c r="D71" s="58"/>
-      <c r="E71" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="38" t="s">
-        <v>185</v>
-      </c>
-      <c r="B72" s="57" t="s">
-        <v>186</v>
-      </c>
-      <c r="C72" s="58"/>
-      <c r="D72" s="58" t="s">
-        <v>18</v>
-      </c>
-      <c r="E72" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="38" t="s">
-        <v>188</v>
-      </c>
-      <c r="B73" s="57"/>
-      <c r="C73" s="58"/>
-      <c r="D73" s="58"/>
-      <c r="E73" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="38" t="s">
-        <v>194</v>
-      </c>
-      <c r="B74" s="57" t="s">
-        <v>195</v>
-      </c>
-      <c r="C74" s="58"/>
-      <c r="D74" s="58" t="s">
-        <v>18</v>
-      </c>
-      <c r="E74" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="B75" s="57"/>
-      <c r="C75" s="58"/>
-      <c r="D75" s="58"/>
-      <c r="E75" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="38" t="s">
-        <v>199</v>
-      </c>
-      <c r="B76" s="57" t="s">
-        <v>200</v>
-      </c>
-      <c r="C76" s="58"/>
-      <c r="D76" s="58" t="s">
-        <v>18</v>
-      </c>
-      <c r="E76" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="38" t="s">
-        <v>202</v>
-      </c>
-      <c r="B77" s="57"/>
-      <c r="C77" s="58"/>
-      <c r="D77" s="58"/>
-      <c r="E77" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="38" t="s">
-        <v>210</v>
-      </c>
-      <c r="B78" s="57" t="s">
-        <v>211</v>
-      </c>
-      <c r="C78" s="58"/>
-      <c r="D78" s="58" t="s">
-        <v>18</v>
-      </c>
-      <c r="E78" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="38" t="s">
-        <v>213</v>
-      </c>
-      <c r="B79" s="57"/>
-      <c r="C79" s="58"/>
-      <c r="D79" s="58"/>
-      <c r="E79" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="38" t="s">
-        <v>215</v>
-      </c>
-      <c r="B80" s="57"/>
-      <c r="C80" s="58"/>
-      <c r="D80" s="58"/>
-      <c r="E80" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="38" t="s">
-        <v>222</v>
-      </c>
-      <c r="B81" s="57" t="s">
-        <v>223</v>
-      </c>
-      <c r="C81" s="58"/>
-      <c r="D81" s="58" t="s">
-        <v>18</v>
-      </c>
-      <c r="E81" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="38" t="s">
-        <v>225</v>
-      </c>
-      <c r="B82" s="57"/>
-      <c r="C82" s="58"/>
-      <c r="D82" s="58"/>
-      <c r="E82" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="38" t="s">
-        <v>227</v>
-      </c>
-      <c r="B83" s="57" t="s">
-        <v>228</v>
-      </c>
-      <c r="C83" s="58"/>
-      <c r="D83" s="58" t="s">
-        <v>18</v>
-      </c>
-      <c r="E83" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="38" t="s">
-        <v>230</v>
-      </c>
-      <c r="B84" s="57"/>
-      <c r="C84" s="58"/>
-      <c r="D84" s="58"/>
-      <c r="E84" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="38" t="s">
-        <v>232</v>
-      </c>
-      <c r="B85" s="57"/>
-      <c r="C85" s="58"/>
-      <c r="D85" s="58"/>
-      <c r="E85" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="38" t="s">
-        <v>267</v>
-      </c>
-      <c r="B86" s="48" t="s">
-        <v>268</v>
-      </c>
-      <c r="C86" s="44"/>
-      <c r="D86" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="E86" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="38" t="s">
-        <v>271</v>
-      </c>
-      <c r="B87" s="48" t="s">
-        <v>272</v>
-      </c>
-      <c r="C87" s="44"/>
-      <c r="D87" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="E87" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="38" t="s">
-        <v>275</v>
-      </c>
-      <c r="B88" s="48" t="s">
-        <v>276</v>
-      </c>
-      <c r="C88" s="44"/>
-      <c r="D88" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="E88" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="38" t="s">
-        <v>279</v>
-      </c>
-      <c r="B89" s="48" t="s">
-        <v>280</v>
-      </c>
-      <c r="C89" s="44"/>
-      <c r="D89" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="E89" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="52" t="s">
-        <v>464</v>
-      </c>
-      <c r="B90" s="69" t="s">
-        <v>465</v>
-      </c>
-      <c r="C90" s="58"/>
-      <c r="D90" s="68" t="s">
-        <v>581</v>
-      </c>
-      <c r="E90" s="47"/>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="52" t="s">
-        <v>467</v>
-      </c>
-      <c r="B91" s="69"/>
-      <c r="C91" s="58"/>
-      <c r="D91" s="68"/>
-      <c r="E91" s="47"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="52"/>
-      <c r="B92" s="54"/>
-      <c r="C92" s="51"/>
-      <c r="D92" s="53"/>
-      <c r="E92" s="47"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="52"/>
-      <c r="B93" s="54"/>
-      <c r="C93" s="51"/>
-      <c r="D93" s="53"/>
-      <c r="E93" s="47"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="52"/>
-      <c r="B94" s="54"/>
-      <c r="C94" s="51"/>
-      <c r="D94" s="53"/>
-      <c r="E94" s="47"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="52"/>
-      <c r="B95" s="54"/>
-      <c r="C95" s="51"/>
-      <c r="D95" s="53"/>
-      <c r="E95" s="47"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="52"/>
-      <c r="B96" s="54"/>
-      <c r="C96" s="51"/>
-      <c r="D96" s="53"/>
-      <c r="E96" s="47"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="52"/>
-      <c r="B97" s="54"/>
-      <c r="C97" s="51"/>
-      <c r="D97" s="53"/>
-      <c r="E97" s="47"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="52"/>
-      <c r="B98" s="54"/>
-      <c r="C98" s="51"/>
-      <c r="D98" s="53"/>
-      <c r="E98" s="47"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="52"/>
-      <c r="B99" s="54"/>
-      <c r="C99" s="51"/>
-      <c r="D99" s="53"/>
-      <c r="E99" s="47"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="52"/>
-      <c r="B100" s="54"/>
-      <c r="C100" s="51"/>
-      <c r="D100" s="53"/>
-      <c r="E100" s="47"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="52"/>
-      <c r="B101" s="54"/>
-      <c r="C101" s="51"/>
-      <c r="D101" s="53"/>
-      <c r="E101" s="47"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="52"/>
-      <c r="B102" s="54"/>
-      <c r="C102" s="51"/>
-      <c r="D102" s="53"/>
-      <c r="E102" s="47"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="38" t="s">
-        <v>477</v>
-      </c>
-      <c r="B103" s="57" t="s">
-        <v>478</v>
-      </c>
-      <c r="C103" s="58"/>
-      <c r="D103" s="58" t="s">
-        <v>18</v>
-      </c>
-      <c r="E103" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="39" t="s">
-        <v>480</v>
-      </c>
-      <c r="B104" s="63"/>
-      <c r="C104" s="64"/>
-      <c r="D104" s="64"/>
-      <c r="E104" s="49" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C106" s="50">
-        <f>COUNTBLANK(C2:C104)</f>
-        <v>97</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C107" s="50">
-        <f>COUNTA(C2:C104)</f>
-        <v>6</v>
-      </c>
+      <c r="F140" s="57"/>
+      <c r="G140" s="36"/>
+      <c r="H140" s="36"/>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" s="36"/>
+      <c r="B141" s="36"/>
+      <c r="C141" s="36"/>
+      <c r="D141" s="36"/>
+      <c r="E141" s="43">
+        <f>COUNTA(E2:E138)</f>
+        <v>9</v>
+      </c>
+      <c r="F141" s="57"/>
+      <c r="G141" s="36"/>
+      <c r="H141" s="36"/>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" s="36"/>
+      <c r="B142" s="36"/>
+      <c r="C142" s="36"/>
+      <c r="D142" s="36"/>
+      <c r="E142" s="43"/>
+      <c r="F142" s="57"/>
+      <c r="G142" s="36"/>
+      <c r="H142" s="36"/>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A143" s="36"/>
+      <c r="B143" s="36"/>
+      <c r="C143" s="36"/>
+      <c r="D143" s="36"/>
+      <c r="E143" s="43"/>
+      <c r="F143" s="57"/>
+      <c r="G143" s="36"/>
+      <c r="H143" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="123">
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="C103:C104"/>
-    <mergeCell ref="D103:D104"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="C81:C82"/>
+  <mergeCells count="191">
+    <mergeCell ref="E62:E64"/>
+    <mergeCell ref="F62:F64"/>
+    <mergeCell ref="D89:D91"/>
+    <mergeCell ref="E89:E91"/>
+    <mergeCell ref="F89:F91"/>
+    <mergeCell ref="D92:D94"/>
+    <mergeCell ref="E92:E94"/>
+    <mergeCell ref="F92:F94"/>
+    <mergeCell ref="E49:E51"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="G46:G48"/>
+    <mergeCell ref="F49:F51"/>
+    <mergeCell ref="E87:E88"/>
+    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="E83:E84"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="F73:F74"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="F77:F78"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="F81:F82"/>
+    <mergeCell ref="F83:F84"/>
+    <mergeCell ref="F85:F86"/>
+    <mergeCell ref="F87:F88"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="F67:F68"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="E69:E72"/>
+    <mergeCell ref="F69:F72"/>
+    <mergeCell ref="D69:D72"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="D79:D80"/>
     <mergeCell ref="D81:D82"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="D83:D85"/>
-    <mergeCell ref="D90:D91"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="C78:C80"/>
-    <mergeCell ref="D78:D80"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="C66:C68"/>
-    <mergeCell ref="D66:D68"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="C69:C71"/>
-    <mergeCell ref="D69:D71"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="C61:C63"/>
-    <mergeCell ref="D61:D63"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="D83:D84"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="D43:D45"/>
+    <mergeCell ref="D46:D48"/>
+    <mergeCell ref="D49:D51"/>
+    <mergeCell ref="D54:D55"/>
     <mergeCell ref="D56:D57"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="D58:D60"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D62:D64"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="D87:D88"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="F22:F25"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="E38:E39"/>
-    <mergeCell ref="D40:D48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="F52:F53"/>
     <mergeCell ref="D34:D35"/>
     <mergeCell ref="E34:E35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
     <mergeCell ref="D36:D37"/>
     <mergeCell ref="E36:E37"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="E43:E45"/>
+    <mergeCell ref="F43:F45"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="G43:G45"/>
+    <mergeCell ref="D103:D104"/>
+    <mergeCell ref="E103:E104"/>
+    <mergeCell ref="F103:F104"/>
+    <mergeCell ref="D105:D107"/>
+    <mergeCell ref="E105:E107"/>
+    <mergeCell ref="F105:F107"/>
+    <mergeCell ref="D98:D99"/>
+    <mergeCell ref="E98:E99"/>
+    <mergeCell ref="F98:F99"/>
+    <mergeCell ref="D100:D102"/>
+    <mergeCell ref="E100:E102"/>
+    <mergeCell ref="F100:F102"/>
+    <mergeCell ref="D113:D115"/>
+    <mergeCell ref="E113:E115"/>
+    <mergeCell ref="F113:F115"/>
+    <mergeCell ref="D116:D118"/>
+    <mergeCell ref="E116:E118"/>
+    <mergeCell ref="F116:F118"/>
+    <mergeCell ref="D108:D110"/>
+    <mergeCell ref="E108:E110"/>
+    <mergeCell ref="F108:F110"/>
+    <mergeCell ref="D111:D112"/>
+    <mergeCell ref="E111:E112"/>
+    <mergeCell ref="F111:F112"/>
+    <mergeCell ref="D123:D124"/>
+    <mergeCell ref="E123:E124"/>
+    <mergeCell ref="F123:F124"/>
+    <mergeCell ref="D125:D127"/>
+    <mergeCell ref="E125:E127"/>
+    <mergeCell ref="F125:F127"/>
+    <mergeCell ref="D119:D120"/>
+    <mergeCell ref="E119:E120"/>
+    <mergeCell ref="F119:F120"/>
+    <mergeCell ref="D121:D122"/>
+    <mergeCell ref="E121:E122"/>
+    <mergeCell ref="F121:F122"/>
+    <mergeCell ref="D137:D138"/>
+    <mergeCell ref="E137:E138"/>
+    <mergeCell ref="F137:F138"/>
+    <mergeCell ref="D128:D129"/>
+    <mergeCell ref="E128:E129"/>
+    <mergeCell ref="F128:F129"/>
+    <mergeCell ref="D130:D132"/>
+    <mergeCell ref="E130:E132"/>
+    <mergeCell ref="F130:F132"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="D95:D97"/>
+    <mergeCell ref="E95:E97"/>
+    <mergeCell ref="F95:F97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -12532,8 +13233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A026136A-3463-4F46-9920-D2EEED3E1AFC}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12802,7 +13503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FC052A-0F27-488A-94F5-1C9E9BC7A4D4}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15:L16"/>
     </sheetView>
   </sheetViews>
@@ -13247,14 +13948,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13481,27 +14180,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13526,9 +14218,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
UPLOAD_CSV_UTIL and UPLOAD_SERD_UTIL minor adjustments
MEDS_Tables updated with other tables sent by Steve
</commit_message>
<xml_diff>
--- a/analysis/MEDS_Tables.xlsx
+++ b/analysis/MEDS_Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="550" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B40B32B-0EB6-4976-B3AE-F6D6FDE56444}"/>
+  <xr:revisionPtr revIDLastSave="567" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{25861A14-5033-415D-B6D7-154ADEF17066}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,9 +18,8 @@
     <sheet name="tasks" sheetId="10" r:id="rId3"/>
     <sheet name="form" sheetId="7" r:id="rId4"/>
     <sheet name="serd" sheetId="8" r:id="rId5"/>
-    <sheet name="serd tests" sheetId="11" r:id="rId6"/>
-    <sheet name="output" sheetId="9" r:id="rId7"/>
-    <sheet name="enhancements" sheetId="4" r:id="rId8"/>
+    <sheet name="output" sheetId="9" r:id="rId6"/>
+    <sheet name="enhancements" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">meds_tables!$A$1:$X$1</definedName>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2673" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2709" uniqueCount="589">
   <si>
     <t>Table</t>
   </si>
@@ -1787,7 +1786,25 @@
 Text File (?)</t>
   </si>
   <si>
-    <t xml:space="preserve">when there is an ICES hip in the SERD file, and the ship exists with the same name and institute, the </t>
+    <t>Seasoar profile data</t>
+  </si>
+  <si>
+    <t>Data exports format GPPDB format</t>
+  </si>
+  <si>
+    <t>Bespoke Import</t>
+  </si>
+  <si>
+    <t>20220503_0850.hdr, 20220505_0831.hdr, 20220503_1015.hdr, 20220509_0809.hdr</t>
+  </si>
+  <si>
+    <t>[MDSYS.SDO_GEOMETRY]</t>
+  </si>
+  <si>
+    <t>0470369-005-305</t>
+  </si>
+  <si>
+    <t>0550456-009-218</t>
   </si>
 </sst>
 </file>
@@ -2172,7 +2189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -2435,6 +2452,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2480,7 +2534,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2568,28 +2622,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2598,25 +2686,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -10648,10 +10718,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8FA477-9B46-4053-B7AD-310B8B9F2B30}">
-  <dimension ref="A1:P143"/>
+  <dimension ref="A1:P152"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10659,8 +10729,8 @@
     <col min="3" max="3" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" style="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="63.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="72.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.140625" customWidth="1"/>
     <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
@@ -10668,45 +10738,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:16" s="40" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="52" t="s">
         <v>539</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="F1" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="56" t="s">
+      <c r="G1" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="60"/>
+      <c r="H1" s="48"/>
       <c r="I1" s="41">
-        <f>E141/E140</f>
-        <v>7.03125E-2</v>
-      </c>
-      <c r="J1" s="61" t="s">
+        <f>E150/E149</f>
+        <v>6.569343065693431E-2</v>
+      </c>
+      <c r="J1" s="49" t="s">
         <v>566</v>
       </c>
-      <c r="K1" s="60"/>
+      <c r="K1" s="48"/>
     </row>
     <row r="2" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="55" t="s">
+      <c r="G2" s="62" t="s">
         <v>564</v>
       </c>
     </row>
@@ -10714,10 +10784,10 @@
       <c r="C3" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="49"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="64"/>
       <c r="K3" s="36"/>
       <c r="L3" s="36"/>
       <c r="M3" s="36"/>
@@ -10729,10 +10799,10 @@
       <c r="C4" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="49"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="64"/>
       <c r="K4" s="36"/>
       <c r="L4" s="36"/>
       <c r="M4" s="36"/>
@@ -10744,27 +10814,27 @@
       <c r="C5" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="F5" s="46" t="s">
+      <c r="F5" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="49" t="s">
+      <c r="G5" s="64" t="s">
         <v>519</v>
       </c>
       <c r="K5" s="36"/>
-      <c r="L5" s="58" t="s">
+      <c r="L5" s="47" t="s">
         <v>464</v>
       </c>
-      <c r="M5" s="59" t="s">
+      <c r="M5" s="55" t="s">
         <v>465</v>
       </c>
-      <c r="N5" s="46"/>
-      <c r="O5" s="48" t="s">
+      <c r="N5" s="56"/>
+      <c r="O5" s="54" t="s">
         <v>581</v>
       </c>
       <c r="P5" s="36"/>
@@ -10773,33 +10843,33 @@
       <c r="C6" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="49"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="64"/>
       <c r="K6" s="36"/>
-      <c r="L6" s="58" t="s">
+      <c r="L6" s="47" t="s">
         <v>467</v>
       </c>
-      <c r="M6" s="59"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="48"/>
+      <c r="M6" s="55"/>
+      <c r="N6" s="56"/>
+      <c r="O6" s="54"/>
       <c r="P6" s="36"/>
     </row>
     <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C7" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="46" t="s">
+      <c r="E7" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="46" t="s">
+      <c r="F7" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="49" t="s">
+      <c r="G7" s="64" t="s">
         <v>80</v>
       </c>
       <c r="K7" s="36"/>
@@ -10813,10 +10883,10 @@
       <c r="C8" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="49"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="64"/>
       <c r="K8" s="36"/>
       <c r="L8" s="36"/>
       <c r="M8" s="36"/>
@@ -10828,16 +10898,16 @@
       <c r="C9" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="57" t="s">
         <v>171</v>
       </c>
-      <c r="E9" s="46" t="s">
+      <c r="E9" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="46" t="s">
+      <c r="F9" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="49" t="s">
+      <c r="G9" s="64" t="s">
         <v>523</v>
       </c>
     </row>
@@ -10845,34 +10915,34 @@
       <c r="C10" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="D10" s="44"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="49"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="64"/>
     </row>
     <row r="11" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C11" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="D11" s="44"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="49"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="64"/>
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C12" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="57" t="s">
         <v>204</v>
       </c>
-      <c r="E12" s="46" t="s">
+      <c r="E12" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="46" t="s">
+      <c r="F12" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="49" t="s">
+      <c r="G12" s="64" t="s">
         <v>515</v>
       </c>
     </row>
@@ -10880,25 +10950,25 @@
       <c r="C13" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="49"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="64"/>
     </row>
     <row r="14" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C14" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="57" t="s">
         <v>361</v>
       </c>
-      <c r="E14" s="46" t="s">
+      <c r="E14" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="F14" s="46" t="s">
+      <c r="F14" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="49" t="s">
+      <c r="G14" s="64" t="s">
         <v>518</v>
       </c>
     </row>
@@ -10906,23 +10976,23 @@
       <c r="C15" s="35" t="s">
         <v>363</v>
       </c>
-      <c r="D15" s="45"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="50"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="63"/>
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C16" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="52" t="s">
+      <c r="D16" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51" t="s">
+      <c r="E16" s="60"/>
+      <c r="F16" s="60" t="s">
         <v>567</v>
       </c>
-      <c r="G16" s="55" t="s">
+      <c r="G16" s="62" t="s">
         <v>73</v>
       </c>
     </row>
@@ -10930,23 +11000,23 @@
       <c r="C17" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="44"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="49"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="64"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="44" t="s">
+      <c r="D18" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46" t="s">
+      <c r="E18" s="56"/>
+      <c r="F18" s="56" t="s">
         <v>567</v>
       </c>
-      <c r="G18" s="49" t="s">
+      <c r="G18" s="64" t="s">
         <v>524</v>
       </c>
     </row>
@@ -10954,23 +11024,23 @@
       <c r="C19" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="44"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="49"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="64"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="D20" s="44" t="s">
+      <c r="D20" s="57" t="s">
         <v>300</v>
       </c>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46" t="s">
+      <c r="E20" s="56"/>
+      <c r="F20" s="56" t="s">
         <v>567</v>
       </c>
-      <c r="G20" s="49" t="s">
+      <c r="G20" s="64" t="s">
         <v>516</v>
       </c>
     </row>
@@ -10978,23 +11048,23 @@
       <c r="C21" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="D21" s="44"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="49"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="64"/>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="D22" s="44" t="s">
+      <c r="D22" s="57" t="s">
         <v>305</v>
       </c>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46" t="s">
+      <c r="E22" s="56"/>
+      <c r="F22" s="56" t="s">
         <v>567</v>
       </c>
-      <c r="G22" s="49" t="s">
+      <c r="G22" s="64" t="s">
         <v>521</v>
       </c>
     </row>
@@ -11002,41 +11072,41 @@
       <c r="C23" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="D23" s="44"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="49"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="64"/>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="D24" s="44"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="49"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="64"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="34" t="s">
         <v>311</v>
       </c>
-      <c r="D25" s="44"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="49"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="64"/>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="34" t="s">
         <v>317</v>
       </c>
-      <c r="D26" s="44" t="s">
+      <c r="D26" s="57" t="s">
         <v>318</v>
       </c>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46" t="s">
+      <c r="E26" s="56"/>
+      <c r="F26" s="56" t="s">
         <v>567</v>
       </c>
-      <c r="G26" s="49" t="s">
+      <c r="G26" s="64" t="s">
         <v>512</v>
       </c>
     </row>
@@ -11044,23 +11114,23 @@
       <c r="C27" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="D27" s="44"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="49"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="64"/>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C28" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="D28" s="53" t="s">
+      <c r="D28" s="65" t="s">
         <v>323</v>
       </c>
-      <c r="E28" s="54"/>
-      <c r="F28" s="46" t="s">
+      <c r="E28" s="66"/>
+      <c r="F28" s="56" t="s">
         <v>567</v>
       </c>
-      <c r="G28" s="49" t="s">
+      <c r="G28" s="64" t="s">
         <v>517</v>
       </c>
     </row>
@@ -11068,23 +11138,23 @@
       <c r="C29" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="D29" s="53"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="49"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="64"/>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C30" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="D30" s="44" t="s">
+      <c r="D30" s="57" t="s">
         <v>328</v>
       </c>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46" t="s">
+      <c r="E30" s="56"/>
+      <c r="F30" s="56" t="s">
         <v>567</v>
       </c>
-      <c r="G30" s="49" t="s">
+      <c r="G30" s="64" t="s">
         <v>508</v>
       </c>
     </row>
@@ -11092,23 +11162,23 @@
       <c r="C31" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="D31" s="44"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="49"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="64"/>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="D32" s="44" t="s">
+      <c r="D32" s="57" t="s">
         <v>333</v>
       </c>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46" t="s">
+      <c r="E32" s="56"/>
+      <c r="F32" s="56" t="s">
         <v>567</v>
       </c>
-      <c r="G32" s="49" t="s">
+      <c r="G32" s="64" t="s">
         <v>510</v>
       </c>
     </row>
@@ -11116,23 +11186,23 @@
       <c r="C33" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="D33" s="44"/>
-      <c r="E33" s="46"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="49"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="64"/>
     </row>
     <row r="34" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C34" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="D34" s="44" t="s">
+      <c r="D34" s="57" t="s">
         <v>338</v>
       </c>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46" t="s">
+      <c r="E34" s="56"/>
+      <c r="F34" s="56" t="s">
         <v>567</v>
       </c>
-      <c r="G34" s="49" t="s">
+      <c r="G34" s="64" t="s">
         <v>511</v>
       </c>
     </row>
@@ -11140,23 +11210,23 @@
       <c r="C35" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="D35" s="44"/>
-      <c r="E35" s="46"/>
-      <c r="F35" s="46"/>
-      <c r="G35" s="49"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="64"/>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C36" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="D36" s="44" t="s">
+      <c r="D36" s="57" t="s">
         <v>343</v>
       </c>
-      <c r="E36" s="46"/>
-      <c r="F36" s="46" t="s">
+      <c r="E36" s="56"/>
+      <c r="F36" s="56" t="s">
         <v>567</v>
       </c>
-      <c r="G36" s="49" t="s">
+      <c r="G36" s="64" t="s">
         <v>509</v>
       </c>
     </row>
@@ -11164,23 +11234,23 @@
       <c r="C37" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="D37" s="44"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="49"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="56"/>
+      <c r="G37" s="64"/>
     </row>
     <row r="38" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C38" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="D38" s="44" t="s">
+      <c r="D38" s="57" t="s">
         <v>348</v>
       </c>
-      <c r="E38" s="46"/>
-      <c r="F38" s="46" t="s">
+      <c r="E38" s="56"/>
+      <c r="F38" s="56" t="s">
         <v>567</v>
       </c>
-      <c r="G38" s="49" t="s">
+      <c r="G38" s="64" t="s">
         <v>520</v>
       </c>
     </row>
@@ -11188,25 +11258,25 @@
       <c r="C39" s="35" t="s">
         <v>350</v>
       </c>
-      <c r="D39" s="45"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="50"/>
+      <c r="D39" s="59"/>
+      <c r="E39" s="61"/>
+      <c r="F39" s="61"/>
+      <c r="G39" s="63"/>
     </row>
     <row r="40" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C40" s="33" t="s">
         <v>365</v>
       </c>
-      <c r="D40" s="52" t="s">
+      <c r="D40" s="58" t="s">
         <v>366</v>
       </c>
-      <c r="E40" s="51" t="s">
+      <c r="E40" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="F40" s="51" t="s">
+      <c r="F40" s="60" t="s">
         <v>369</v>
       </c>
-      <c r="G40" s="55" t="s">
+      <c r="G40" s="62" t="s">
         <v>514</v>
       </c>
     </row>
@@ -11214,34 +11284,34 @@
       <c r="C41" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="D41" s="44"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="46"/>
-      <c r="G41" s="49"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="56"/>
+      <c r="F41" s="56"/>
+      <c r="G41" s="64"/>
     </row>
     <row r="42" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C42" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="D42" s="44"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="49"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="56"/>
+      <c r="F42" s="56"/>
+      <c r="G42" s="64"/>
     </row>
     <row r="43" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C43" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="D43" s="44" t="s">
+      <c r="D43" s="57" t="s">
         <v>371</v>
       </c>
-      <c r="E43" s="46" t="s">
+      <c r="E43" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="F43" s="46" t="s">
+      <c r="F43" s="56" t="s">
         <v>369</v>
       </c>
-      <c r="G43" s="49" t="s">
+      <c r="G43" s="64" t="s">
         <v>513</v>
       </c>
     </row>
@@ -11249,34 +11319,34 @@
       <c r="C44" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="D44" s="44"/>
-      <c r="E44" s="46"/>
-      <c r="F44" s="46"/>
-      <c r="G44" s="49"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="56"/>
+      <c r="F44" s="56"/>
+      <c r="G44" s="64"/>
     </row>
     <row r="45" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C45" s="34" t="s">
         <v>384</v>
       </c>
-      <c r="D45" s="44"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="46"/>
-      <c r="G45" s="49"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="56"/>
+      <c r="F45" s="56"/>
+      <c r="G45" s="64"/>
     </row>
     <row r="46" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C46" s="34" t="s">
         <v>373</v>
       </c>
-      <c r="D46" s="44" t="s">
+      <c r="D46" s="57" t="s">
         <v>374</v>
       </c>
-      <c r="E46" s="46" t="s">
+      <c r="E46" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="F46" s="46" t="s">
+      <c r="F46" s="56" t="s">
         <v>369</v>
       </c>
-      <c r="G46" s="49" t="s">
+      <c r="G46" s="64" t="s">
         <v>522</v>
       </c>
     </row>
@@ -11284,19 +11354,19 @@
       <c r="C47" s="34" t="s">
         <v>380</v>
       </c>
-      <c r="D47" s="44"/>
-      <c r="E47" s="46"/>
-      <c r="F47" s="46"/>
-      <c r="G47" s="49"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="56"/>
+      <c r="G47" s="64"/>
     </row>
     <row r="48" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C48" s="35" t="s">
         <v>386</v>
       </c>
-      <c r="D48" s="45"/>
-      <c r="E48" s="47"/>
-      <c r="F48" s="47"/>
-      <c r="G48" s="50"/>
+      <c r="D48" s="59"/>
+      <c r="E48" s="61"/>
+      <c r="F48" s="61"/>
+      <c r="G48" s="63"/>
       <c r="J48" s="36"/>
       <c r="K48" s="36"/>
       <c r="L48" s="36"/>
@@ -11304,17 +11374,17 @@
     </row>
     <row r="49" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C49" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="D49" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E49" s="51"/>
-      <c r="F49" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="G49" s="38" t="s">
-        <v>33</v>
+        <v>464</v>
+      </c>
+      <c r="D49" s="58" t="s">
+        <v>465</v>
+      </c>
+      <c r="E49" s="60"/>
+      <c r="F49" s="60" t="s">
+        <v>584</v>
+      </c>
+      <c r="G49" s="62" t="s">
+        <v>585</v>
       </c>
       <c r="J49" s="36"/>
       <c r="K49" s="36"/>
@@ -11322,15 +11392,13 @@
       <c r="M49" s="36"/>
     </row>
     <row r="50" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C50" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="D50" s="44"/>
-      <c r="E50" s="46"/>
-      <c r="F50" s="46"/>
-      <c r="G50" s="38" t="s">
-        <v>33</v>
-      </c>
+      <c r="C50" s="35" t="s">
+        <v>467</v>
+      </c>
+      <c r="D50" s="59"/>
+      <c r="E50" s="61"/>
+      <c r="F50" s="61"/>
+      <c r="G50" s="63"/>
       <c r="J50" s="36"/>
       <c r="K50" s="36"/>
       <c r="L50" s="36"/>
@@ -11338,11 +11406,15 @@
     </row>
     <row r="51" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C51" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="D51" s="44"/>
-      <c r="E51" s="46"/>
-      <c r="F51" s="46"/>
+        <v>36</v>
+      </c>
+      <c r="D51" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="E51" s="56"/>
+      <c r="F51" s="56" t="s">
+        <v>18</v>
+      </c>
       <c r="G51" s="38" t="s">
         <v>33</v>
       </c>
@@ -11353,15 +11425,11 @@
     </row>
     <row r="52" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C52" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="D52" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="E52" s="46"/>
-      <c r="F52" s="46" t="s">
-        <v>18</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D52" s="57"/>
+      <c r="E52" s="56"/>
+      <c r="F52" s="56"/>
       <c r="G52" s="38" t="s">
         <v>33</v>
       </c>
@@ -11372,11 +11440,11 @@
     </row>
     <row r="53" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C53" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="D53" s="44"/>
-      <c r="E53" s="46"/>
-      <c r="F53" s="46"/>
+        <v>45</v>
+      </c>
+      <c r="D53" s="57"/>
+      <c r="E53" s="56"/>
+      <c r="F53" s="56"/>
       <c r="G53" s="38" t="s">
         <v>33</v>
       </c>
@@ -11387,13 +11455,13 @@
     </row>
     <row r="54" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C54" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="D54" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="E54" s="46"/>
-      <c r="F54" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="D54" s="57" t="s">
+        <v>48</v>
+      </c>
+      <c r="E54" s="56"/>
+      <c r="F54" s="56" t="s">
         <v>18</v>
       </c>
       <c r="G54" s="38" t="s">
@@ -11406,11 +11474,11 @@
     </row>
     <row r="55" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C55" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="D55" s="44"/>
-      <c r="E55" s="46"/>
-      <c r="F55" s="46"/>
+        <v>50</v>
+      </c>
+      <c r="D55" s="57"/>
+      <c r="E55" s="56"/>
+      <c r="F55" s="56"/>
       <c r="G55" s="38" t="s">
         <v>33</v>
       </c>
@@ -11421,13 +11489,13 @@
     </row>
     <row r="56" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C56" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="D56" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="E56" s="46"/>
-      <c r="F56" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="D56" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="E56" s="56"/>
+      <c r="F56" s="56" t="s">
         <v>18</v>
       </c>
       <c r="G56" s="38" t="s">
@@ -11440,11 +11508,11 @@
     </row>
     <row r="57" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C57" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="D57" s="44"/>
-      <c r="E57" s="46"/>
-      <c r="F57" s="46"/>
+        <v>55</v>
+      </c>
+      <c r="D57" s="57"/>
+      <c r="E57" s="56"/>
+      <c r="F57" s="56"/>
       <c r="G57" s="38" t="s">
         <v>33</v>
       </c>
@@ -11455,13 +11523,13 @@
     </row>
     <row r="58" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C58" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="D58" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="E58" s="46"/>
-      <c r="F58" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="D58" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="E58" s="56"/>
+      <c r="F58" s="56" t="s">
         <v>18</v>
       </c>
       <c r="G58" s="38" t="s">
@@ -11474,11 +11542,11 @@
     </row>
     <row r="59" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C59" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="D59" s="44"/>
-      <c r="E59" s="46"/>
-      <c r="F59" s="46"/>
+        <v>83</v>
+      </c>
+      <c r="D59" s="57"/>
+      <c r="E59" s="56"/>
+      <c r="F59" s="56"/>
       <c r="G59" s="38" t="s">
         <v>33</v>
       </c>
@@ -11489,13 +11557,13 @@
     </row>
     <row r="60" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C60" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="D60" s="44" t="s">
-        <v>105</v>
-      </c>
-      <c r="E60" s="46"/>
-      <c r="F60" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="D60" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="E60" s="56"/>
+      <c r="F60" s="56" t="s">
         <v>18</v>
       </c>
       <c r="G60" s="38" t="s">
@@ -11508,11 +11576,11 @@
     </row>
     <row r="61" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C61" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="D61" s="44"/>
-      <c r="E61" s="46"/>
-      <c r="F61" s="46"/>
+        <v>75</v>
+      </c>
+      <c r="D61" s="57"/>
+      <c r="E61" s="56"/>
+      <c r="F61" s="56"/>
       <c r="G61" s="38" t="s">
         <v>33</v>
       </c>
@@ -11523,13 +11591,13 @@
     </row>
     <row r="62" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C62" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="D62" s="44" t="s">
-        <v>171</v>
-      </c>
-      <c r="E62" s="46"/>
-      <c r="F62" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="D62" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="E62" s="56"/>
+      <c r="F62" s="56" t="s">
         <v>18</v>
       </c>
       <c r="G62" s="38" t="s">
@@ -11542,11 +11610,11 @@
     </row>
     <row r="63" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C63" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="D63" s="44"/>
-      <c r="E63" s="46"/>
-      <c r="F63" s="46"/>
+        <v>107</v>
+      </c>
+      <c r="D63" s="57"/>
+      <c r="E63" s="56"/>
+      <c r="F63" s="56"/>
       <c r="G63" s="38" t="s">
         <v>33</v>
       </c>
@@ -11557,11 +11625,15 @@
     </row>
     <row r="64" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C64" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="D64" s="44"/>
-      <c r="E64" s="46"/>
-      <c r="F64" s="46"/>
+        <v>170</v>
+      </c>
+      <c r="D64" s="57" t="s">
+        <v>171</v>
+      </c>
+      <c r="E64" s="56"/>
+      <c r="F64" s="56" t="s">
+        <v>18</v>
+      </c>
       <c r="G64" s="38" t="s">
         <v>33</v>
       </c>
@@ -11572,15 +11644,11 @@
     </row>
     <row r="65" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C65" s="34" t="s">
-        <v>203</v>
-      </c>
-      <c r="D65" s="44" t="s">
-        <v>204</v>
-      </c>
-      <c r="E65" s="46"/>
-      <c r="F65" s="46" t="s">
-        <v>18</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="D65" s="57"/>
+      <c r="E65" s="56"/>
+      <c r="F65" s="56"/>
       <c r="G65" s="38" t="s">
         <v>33</v>
       </c>
@@ -11591,11 +11659,11 @@
     </row>
     <row r="66" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C66" s="34" t="s">
-        <v>206</v>
-      </c>
-      <c r="D66" s="44"/>
-      <c r="E66" s="46"/>
-      <c r="F66" s="46"/>
+        <v>176</v>
+      </c>
+      <c r="D66" s="57"/>
+      <c r="E66" s="56"/>
+      <c r="F66" s="56"/>
       <c r="G66" s="38" t="s">
         <v>33</v>
       </c>
@@ -11606,13 +11674,13 @@
     </row>
     <row r="67" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C67" s="34" t="s">
-        <v>299</v>
-      </c>
-      <c r="D67" s="44" t="s">
-        <v>300</v>
-      </c>
-      <c r="E67" s="46"/>
-      <c r="F67" s="46" t="s">
+        <v>203</v>
+      </c>
+      <c r="D67" s="57" t="s">
+        <v>204</v>
+      </c>
+      <c r="E67" s="56"/>
+      <c r="F67" s="56" t="s">
         <v>18</v>
       </c>
       <c r="G67" s="38" t="s">
@@ -11625,11 +11693,11 @@
     </row>
     <row r="68" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C68" s="34" t="s">
-        <v>302</v>
-      </c>
-      <c r="D68" s="44"/>
-      <c r="E68" s="46"/>
-      <c r="F68" s="46"/>
+        <v>206</v>
+      </c>
+      <c r="D68" s="57"/>
+      <c r="E68" s="56"/>
+      <c r="F68" s="56"/>
       <c r="G68" s="38" t="s">
         <v>33</v>
       </c>
@@ -11640,13 +11708,13 @@
     </row>
     <row r="69" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C69" s="34" t="s">
-        <v>304</v>
-      </c>
-      <c r="D69" s="44" t="s">
-        <v>305</v>
-      </c>
-      <c r="E69" s="46"/>
-      <c r="F69" s="46" t="s">
+        <v>299</v>
+      </c>
+      <c r="D69" s="57" t="s">
+        <v>300</v>
+      </c>
+      <c r="E69" s="56"/>
+      <c r="F69" s="56" t="s">
         <v>18</v>
       </c>
       <c r="G69" s="38" t="s">
@@ -11659,11 +11727,11 @@
     </row>
     <row r="70" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C70" s="34" t="s">
-        <v>309</v>
-      </c>
-      <c r="D70" s="44"/>
-      <c r="E70" s="46"/>
-      <c r="F70" s="46"/>
+        <v>302</v>
+      </c>
+      <c r="D70" s="57"/>
+      <c r="E70" s="56"/>
+      <c r="F70" s="56"/>
       <c r="G70" s="38" t="s">
         <v>33</v>
       </c>
@@ -11674,11 +11742,15 @@
     </row>
     <row r="71" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C71" s="34" t="s">
-        <v>307</v>
-      </c>
-      <c r="D71" s="44"/>
-      <c r="E71" s="46"/>
-      <c r="F71" s="46"/>
+        <v>304</v>
+      </c>
+      <c r="D71" s="57" t="s">
+        <v>305</v>
+      </c>
+      <c r="E71" s="56"/>
+      <c r="F71" s="56" t="s">
+        <v>18</v>
+      </c>
       <c r="G71" s="38" t="s">
         <v>33</v>
       </c>
@@ -11689,11 +11761,11 @@
     </row>
     <row r="72" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C72" s="34" t="s">
-        <v>311</v>
-      </c>
-      <c r="D72" s="44"/>
-      <c r="E72" s="46"/>
-      <c r="F72" s="46"/>
+        <v>309</v>
+      </c>
+      <c r="D72" s="57"/>
+      <c r="E72" s="56"/>
+      <c r="F72" s="56"/>
       <c r="G72" s="38" t="s">
         <v>33</v>
       </c>
@@ -11704,15 +11776,11 @@
     </row>
     <row r="73" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C73" s="34" t="s">
-        <v>317</v>
-      </c>
-      <c r="D73" s="44" t="s">
-        <v>318</v>
-      </c>
-      <c r="E73" s="46"/>
-      <c r="F73" s="46" t="s">
-        <v>18</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="D73" s="57"/>
+      <c r="E73" s="56"/>
+      <c r="F73" s="56"/>
       <c r="G73" s="38" t="s">
         <v>33</v>
       </c>
@@ -11723,11 +11791,11 @@
     </row>
     <row r="74" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C74" s="34" t="s">
-        <v>320</v>
-      </c>
-      <c r="D74" s="44"/>
-      <c r="E74" s="46"/>
-      <c r="F74" s="46"/>
+        <v>311</v>
+      </c>
+      <c r="D74" s="57"/>
+      <c r="E74" s="56"/>
+      <c r="F74" s="56"/>
       <c r="G74" s="38" t="s">
         <v>33</v>
       </c>
@@ -11738,13 +11806,13 @@
     </row>
     <row r="75" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C75" s="34" t="s">
-        <v>322</v>
-      </c>
-      <c r="D75" s="53" t="s">
-        <v>323</v>
-      </c>
-      <c r="E75" s="46"/>
-      <c r="F75" s="46" t="s">
+        <v>317</v>
+      </c>
+      <c r="D75" s="57" t="s">
+        <v>318</v>
+      </c>
+      <c r="E75" s="56"/>
+      <c r="F75" s="56" t="s">
         <v>18</v>
       </c>
       <c r="G75" s="38" t="s">
@@ -11757,50 +11825,58 @@
     </row>
     <row r="76" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C76" s="34" t="s">
-        <v>325</v>
-      </c>
-      <c r="D76" s="53"/>
-      <c r="E76" s="46"/>
-      <c r="F76" s="46"/>
+        <v>320</v>
+      </c>
+      <c r="D76" s="57"/>
+      <c r="E76" s="56"/>
+      <c r="F76" s="56"/>
       <c r="G76" s="38" t="s">
         <v>33</v>
       </c>
+      <c r="J76" s="36"/>
+      <c r="K76" s="36"/>
+      <c r="L76" s="36"/>
+      <c r="M76" s="36"/>
     </row>
     <row r="77" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C77" s="34" t="s">
-        <v>327</v>
-      </c>
-      <c r="D77" s="44" t="s">
-        <v>328</v>
-      </c>
-      <c r="E77" s="46"/>
-      <c r="F77" s="46" t="s">
+        <v>322</v>
+      </c>
+      <c r="D77" s="65" t="s">
+        <v>323</v>
+      </c>
+      <c r="E77" s="56"/>
+      <c r="F77" s="56" t="s">
         <v>18</v>
       </c>
       <c r="G77" s="38" t="s">
         <v>33</v>
       </c>
+      <c r="J77" s="36"/>
+      <c r="K77" s="36"/>
+      <c r="L77" s="36"/>
+      <c r="M77" s="36"/>
     </row>
     <row r="78" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C78" s="34" t="s">
-        <v>330</v>
-      </c>
-      <c r="D78" s="44"/>
-      <c r="E78" s="46"/>
-      <c r="F78" s="46"/>
+        <v>325</v>
+      </c>
+      <c r="D78" s="65"/>
+      <c r="E78" s="56"/>
+      <c r="F78" s="56"/>
       <c r="G78" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="79" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C79" s="34" t="s">
-        <v>332</v>
-      </c>
-      <c r="D79" s="44" t="s">
-        <v>333</v>
-      </c>
-      <c r="E79" s="46"/>
-      <c r="F79" s="46" t="s">
+        <v>327</v>
+      </c>
+      <c r="D79" s="57" t="s">
+        <v>328</v>
+      </c>
+      <c r="E79" s="56"/>
+      <c r="F79" s="56" t="s">
         <v>18</v>
       </c>
       <c r="G79" s="38" t="s">
@@ -11809,217 +11885,215 @@
     </row>
     <row r="80" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C80" s="34" t="s">
+        <v>330</v>
+      </c>
+      <c r="D80" s="57"/>
+      <c r="E80" s="56"/>
+      <c r="F80" s="56"/>
+      <c r="G80" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C81" s="34" t="s">
+        <v>332</v>
+      </c>
+      <c r="D81" s="57" t="s">
+        <v>333</v>
+      </c>
+      <c r="E81" s="56"/>
+      <c r="F81" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="G81" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C82" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="D80" s="44"/>
-      <c r="E80" s="46"/>
-      <c r="F80" s="46"/>
-      <c r="G80" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C81" s="34" t="s">
+      <c r="D82" s="57"/>
+      <c r="E82" s="56"/>
+      <c r="F82" s="56"/>
+      <c r="G82" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="83" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C83" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="D81" s="44" t="s">
+      <c r="D83" s="57" t="s">
         <v>338</v>
       </c>
-      <c r="E81" s="46"/>
-      <c r="F81" s="46" t="s">
+      <c r="E83" s="56"/>
+      <c r="F83" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="G81" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C82" s="34" t="s">
+      <c r="G83" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C84" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="D82" s="44"/>
-      <c r="E82" s="46"/>
-      <c r="F82" s="46"/>
-      <c r="G82" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C83" s="34" t="s">
+      <c r="D84" s="57"/>
+      <c r="E84" s="56"/>
+      <c r="F84" s="56"/>
+      <c r="G84" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C85" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="D83" s="44" t="s">
+      <c r="D85" s="57" t="s">
         <v>343</v>
       </c>
-      <c r="E83" s="46"/>
-      <c r="F83" s="46" t="s">
+      <c r="E85" s="56"/>
+      <c r="F85" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="G83" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C84" s="34" t="s">
+      <c r="G85" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C86" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="D84" s="44"/>
-      <c r="E84" s="46"/>
-      <c r="F84" s="46"/>
-      <c r="G84" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C85" s="34" t="s">
+      <c r="D86" s="57"/>
+      <c r="E86" s="56"/>
+      <c r="F86" s="56"/>
+      <c r="G86" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C87" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="D85" s="44" t="s">
+      <c r="D87" s="57" t="s">
         <v>348</v>
       </c>
-      <c r="E85" s="46"/>
-      <c r="F85" s="46" t="s">
+      <c r="E87" s="56"/>
+      <c r="F87" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="G85" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C86" s="34" t="s">
+      <c r="G87" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C88" s="34" t="s">
         <v>350</v>
       </c>
-      <c r="D86" s="44"/>
-      <c r="E86" s="46"/>
-      <c r="F86" s="46"/>
-      <c r="G86" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C87" s="34" t="s">
+      <c r="D88" s="57"/>
+      <c r="E88" s="56"/>
+      <c r="F88" s="56"/>
+      <c r="G88" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="89" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C89" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="D87" s="44" t="s">
+      <c r="D89" s="57" t="s">
         <v>361</v>
       </c>
-      <c r="E87" s="46"/>
-      <c r="F87" s="46" t="s">
+      <c r="E89" s="56"/>
+      <c r="F89" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="G87" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C88" s="34" t="s">
+      <c r="G89" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="90" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C90" s="34" t="s">
         <v>363</v>
       </c>
-      <c r="D88" s="44"/>
-      <c r="E88" s="46"/>
-      <c r="F88" s="46"/>
-      <c r="G88" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C89" s="34" t="s">
+      <c r="D90" s="57"/>
+      <c r="E90" s="56"/>
+      <c r="F90" s="56"/>
+      <c r="G90" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="91" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C91" s="34" t="s">
         <v>365</v>
       </c>
-      <c r="D89" s="44" t="s">
+      <c r="D91" s="57" t="s">
         <v>366</v>
       </c>
-      <c r="E89" s="46"/>
-      <c r="F89" s="46" t="s">
+      <c r="E91" s="56"/>
+      <c r="F91" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="G89" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C90" s="34" t="s">
+      <c r="G91" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="92" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C92" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="D90" s="44"/>
-      <c r="E90" s="46"/>
-      <c r="F90" s="46"/>
-      <c r="G90" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C91" s="34" t="s">
+      <c r="D92" s="57"/>
+      <c r="E92" s="56"/>
+      <c r="F92" s="56"/>
+      <c r="G92" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="93" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C93" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="D91" s="44"/>
-      <c r="E91" s="46"/>
-      <c r="F91" s="46"/>
-      <c r="G91" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C92" s="34" t="s">
+      <c r="D93" s="57"/>
+      <c r="E93" s="56"/>
+      <c r="F93" s="56"/>
+      <c r="G93" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="94" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C94" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="D92" s="44" t="s">
+      <c r="D94" s="57" t="s">
         <v>371</v>
       </c>
-      <c r="E92" s="46"/>
-      <c r="F92" s="46" t="s">
+      <c r="E94" s="56"/>
+      <c r="F94" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="G92" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C93" s="34" t="s">
+      <c r="G94" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="95" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C95" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="D93" s="44"/>
-      <c r="E93" s="46"/>
-      <c r="F93" s="46"/>
-      <c r="G93" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C94" s="34" t="s">
+      <c r="D95" s="57"/>
+      <c r="E95" s="56"/>
+      <c r="F95" s="56"/>
+      <c r="G95" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="96" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C96" s="34" t="s">
         <v>384</v>
       </c>
-      <c r="D94" s="44"/>
-      <c r="E94" s="46"/>
-      <c r="F94" s="46"/>
-      <c r="G94" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B95" s="37"/>
-      <c r="C95" s="36" t="s">
-        <v>373</v>
-      </c>
-      <c r="D95" s="44" t="s">
-        <v>374</v>
-      </c>
-      <c r="E95" s="46"/>
-      <c r="F95" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="G95" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B96" s="37"/>
-      <c r="C96" s="36" t="s">
-        <v>380</v>
-      </c>
-      <c r="D96" s="44"/>
-      <c r="E96" s="46"/>
-      <c r="F96" s="46"/>
+      <c r="D96" s="57"/>
+      <c r="E96" s="56"/>
+      <c r="F96" s="56"/>
       <c r="G96" s="38" t="s">
         <v>33</v>
       </c>
@@ -12027,118 +12101,120 @@
     <row r="97" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B97" s="37"/>
       <c r="C97" s="36" t="s">
+        <v>373</v>
+      </c>
+      <c r="D97" s="57" t="s">
+        <v>374</v>
+      </c>
+      <c r="E97" s="56"/>
+      <c r="F97" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="G97" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="98" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B98" s="37"/>
+      <c r="C98" s="36" t="s">
+        <v>380</v>
+      </c>
+      <c r="D98" s="57"/>
+      <c r="E98" s="56"/>
+      <c r="F98" s="56"/>
+      <c r="G98" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="99" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B99" s="37"/>
+      <c r="C99" s="36" t="s">
         <v>386</v>
       </c>
-      <c r="D97" s="44"/>
-      <c r="E97" s="46"/>
-      <c r="F97" s="46"/>
-      <c r="G97" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="J97" s="36"/>
-      <c r="K97" s="36"/>
-      <c r="L97" s="36"/>
-      <c r="M97" s="36"/>
-    </row>
-    <row r="98" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C98" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="D98" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="E98" s="46"/>
-      <c r="F98" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="G98" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="I98" s="36"/>
-    </row>
-    <row r="99" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C99" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="D99" s="44"/>
-      <c r="E99" s="46"/>
-      <c r="F99" s="46"/>
+      <c r="D99" s="57"/>
+      <c r="E99" s="56"/>
+      <c r="F99" s="56"/>
       <c r="G99" s="38" t="s">
         <v>33</v>
       </c>
+      <c r="J99" s="36"/>
+      <c r="K99" s="36"/>
+      <c r="L99" s="36"/>
+      <c r="M99" s="36"/>
     </row>
     <row r="100" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C100" s="34" t="s">
-        <v>109</v>
-      </c>
-      <c r="D100" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="E100" s="46"/>
-      <c r="F100" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="D100" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="E100" s="56"/>
+      <c r="F100" s="56" t="s">
         <v>18</v>
       </c>
       <c r="G100" s="38" t="s">
         <v>33</v>
       </c>
+      <c r="I100" s="36"/>
     </row>
     <row r="101" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C101" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="D101" s="44"/>
-      <c r="E101" s="46"/>
-      <c r="F101" s="46"/>
+        <v>68</v>
+      </c>
+      <c r="D101" s="57"/>
+      <c r="E101" s="56"/>
+      <c r="F101" s="56"/>
       <c r="G101" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="102" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C102" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="D102" s="44"/>
-      <c r="E102" s="46"/>
-      <c r="F102" s="46"/>
+        <v>109</v>
+      </c>
+      <c r="D102" s="57" t="s">
+        <v>110</v>
+      </c>
+      <c r="E102" s="56"/>
+      <c r="F102" s="56" t="s">
+        <v>18</v>
+      </c>
       <c r="G102" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="103" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C103" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="D103" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="E103" s="46"/>
-      <c r="F103" s="46" t="s">
-        <v>18</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="D103" s="57"/>
+      <c r="E103" s="56"/>
+      <c r="F103" s="56"/>
       <c r="G103" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="104" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C104" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="D104" s="44"/>
-      <c r="E104" s="46"/>
-      <c r="F104" s="46"/>
+        <v>114</v>
+      </c>
+      <c r="D104" s="57"/>
+      <c r="E104" s="56"/>
+      <c r="F104" s="56"/>
       <c r="G104" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="105" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C105" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="D105" s="44" t="s">
-        <v>124</v>
-      </c>
-      <c r="E105" s="46"/>
-      <c r="F105" s="46" t="s">
+        <v>118</v>
+      </c>
+      <c r="D105" s="57" t="s">
+        <v>119</v>
+      </c>
+      <c r="E105" s="56"/>
+      <c r="F105" s="56" t="s">
         <v>18</v>
       </c>
       <c r="G105" s="38" t="s">
@@ -12147,98 +12223,98 @@
     </row>
     <row r="106" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C106" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="D106" s="44"/>
-      <c r="E106" s="46"/>
-      <c r="F106" s="46"/>
+        <v>121</v>
+      </c>
+      <c r="D106" s="57"/>
+      <c r="E106" s="56"/>
+      <c r="F106" s="56"/>
       <c r="G106" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="107" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C107" s="34" t="s">
-        <v>128</v>
-      </c>
-      <c r="D107" s="44"/>
-      <c r="E107" s="46"/>
-      <c r="F107" s="46"/>
+        <v>123</v>
+      </c>
+      <c r="D107" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="E107" s="56"/>
+      <c r="F107" s="56" t="s">
+        <v>18</v>
+      </c>
       <c r="G107" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="108" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C108" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="D108" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="E108" s="46"/>
-      <c r="F108" s="46" t="s">
-        <v>18</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="D108" s="57"/>
+      <c r="E108" s="56"/>
+      <c r="F108" s="56"/>
       <c r="G108" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="109" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C109" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="D109" s="44"/>
-      <c r="E109" s="46"/>
-      <c r="F109" s="46"/>
+        <v>128</v>
+      </c>
+      <c r="D109" s="57"/>
+      <c r="E109" s="56"/>
+      <c r="F109" s="56"/>
       <c r="G109" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="110" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C110" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D110" s="44"/>
-      <c r="E110" s="46"/>
-      <c r="F110" s="46"/>
+        <v>130</v>
+      </c>
+      <c r="D110" s="57" t="s">
+        <v>131</v>
+      </c>
+      <c r="E110" s="56"/>
+      <c r="F110" s="56" t="s">
+        <v>18</v>
+      </c>
       <c r="G110" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="111" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C111" s="34" t="s">
-        <v>158</v>
-      </c>
-      <c r="D111" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="E111" s="46"/>
-      <c r="F111" s="46" t="s">
-        <v>18</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="D111" s="57"/>
+      <c r="E111" s="56"/>
+      <c r="F111" s="56"/>
       <c r="G111" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="112" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C112" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="D112" s="44"/>
-      <c r="E112" s="46"/>
-      <c r="F112" s="46"/>
+        <v>136</v>
+      </c>
+      <c r="D112" s="57"/>
+      <c r="E112" s="56"/>
+      <c r="F112" s="56"/>
       <c r="G112" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="113" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C113" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="D113" s="44" t="s">
-        <v>164</v>
-      </c>
-      <c r="E113" s="46"/>
-      <c r="F113" s="46" t="s">
+        <v>158</v>
+      </c>
+      <c r="D113" s="57" t="s">
+        <v>159</v>
+      </c>
+      <c r="E113" s="56"/>
+      <c r="F113" s="56" t="s">
         <v>18</v>
       </c>
       <c r="G113" s="38" t="s">
@@ -12247,98 +12323,98 @@
     </row>
     <row r="114" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C114" s="34" t="s">
-        <v>166</v>
-      </c>
-      <c r="D114" s="44"/>
-      <c r="E114" s="46"/>
-      <c r="F114" s="46"/>
+        <v>161</v>
+      </c>
+      <c r="D114" s="57"/>
+      <c r="E114" s="56"/>
+      <c r="F114" s="56"/>
       <c r="G114" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="115" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C115" s="34" t="s">
-        <v>168</v>
-      </c>
-      <c r="D115" s="44"/>
-      <c r="E115" s="46"/>
-      <c r="F115" s="46"/>
+        <v>163</v>
+      </c>
+      <c r="D115" s="57" t="s">
+        <v>164</v>
+      </c>
+      <c r="E115" s="56"/>
+      <c r="F115" s="56" t="s">
+        <v>18</v>
+      </c>
       <c r="G115" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="116" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C116" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="D116" s="44" t="s">
-        <v>179</v>
-      </c>
-      <c r="E116" s="46"/>
-      <c r="F116" s="46" t="s">
-        <v>18</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="D116" s="57"/>
+      <c r="E116" s="56"/>
+      <c r="F116" s="56"/>
       <c r="G116" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="117" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C117" s="34" t="s">
-        <v>181</v>
-      </c>
-      <c r="D117" s="44"/>
-      <c r="E117" s="46"/>
-      <c r="F117" s="46"/>
+        <v>168</v>
+      </c>
+      <c r="D117" s="57"/>
+      <c r="E117" s="56"/>
+      <c r="F117" s="56"/>
       <c r="G117" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="118" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C118" s="34" t="s">
-        <v>183</v>
-      </c>
-      <c r="D118" s="44"/>
-      <c r="E118" s="46"/>
-      <c r="F118" s="46"/>
+        <v>178</v>
+      </c>
+      <c r="D118" s="57" t="s">
+        <v>179</v>
+      </c>
+      <c r="E118" s="56"/>
+      <c r="F118" s="56" t="s">
+        <v>18</v>
+      </c>
       <c r="G118" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="119" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C119" s="34" t="s">
-        <v>185</v>
-      </c>
-      <c r="D119" s="44" t="s">
-        <v>186</v>
-      </c>
-      <c r="E119" s="46"/>
-      <c r="F119" s="46" t="s">
-        <v>18</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="D119" s="57"/>
+      <c r="E119" s="56"/>
+      <c r="F119" s="56"/>
       <c r="G119" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="120" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C120" s="34" t="s">
-        <v>188</v>
-      </c>
-      <c r="D120" s="44"/>
-      <c r="E120" s="46"/>
-      <c r="F120" s="46"/>
+        <v>183</v>
+      </c>
+      <c r="D120" s="57"/>
+      <c r="E120" s="56"/>
+      <c r="F120" s="56"/>
       <c r="G120" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="121" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C121" s="34" t="s">
-        <v>194</v>
-      </c>
-      <c r="D121" s="44" t="s">
-        <v>195</v>
-      </c>
-      <c r="E121" s="46"/>
-      <c r="F121" s="46" t="s">
+        <v>185</v>
+      </c>
+      <c r="D121" s="57" t="s">
+        <v>186</v>
+      </c>
+      <c r="E121" s="56"/>
+      <c r="F121" s="56" t="s">
         <v>18</v>
       </c>
       <c r="G121" s="38" t="s">
@@ -12347,24 +12423,24 @@
     </row>
     <row r="122" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C122" s="34" t="s">
-        <v>197</v>
-      </c>
-      <c r="D122" s="44"/>
-      <c r="E122" s="46"/>
-      <c r="F122" s="46"/>
+        <v>188</v>
+      </c>
+      <c r="D122" s="57"/>
+      <c r="E122" s="56"/>
+      <c r="F122" s="56"/>
       <c r="G122" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="123" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C123" s="34" t="s">
-        <v>199</v>
-      </c>
-      <c r="D123" s="44" t="s">
-        <v>200</v>
-      </c>
-      <c r="E123" s="46"/>
-      <c r="F123" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="D123" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="E123" s="56"/>
+      <c r="F123" s="56" t="s">
         <v>18</v>
       </c>
       <c r="G123" s="38" t="s">
@@ -12373,24 +12449,24 @@
     </row>
     <row r="124" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C124" s="34" t="s">
-        <v>202</v>
-      </c>
-      <c r="D124" s="44"/>
-      <c r="E124" s="46"/>
-      <c r="F124" s="46"/>
+        <v>197</v>
+      </c>
+      <c r="D124" s="57"/>
+      <c r="E124" s="56"/>
+      <c r="F124" s="56"/>
       <c r="G124" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="125" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C125" s="34" t="s">
-        <v>210</v>
-      </c>
-      <c r="D125" s="44" t="s">
-        <v>211</v>
-      </c>
-      <c r="E125" s="46"/>
-      <c r="F125" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="D125" s="57" t="s">
+        <v>200</v>
+      </c>
+      <c r="E125" s="56"/>
+      <c r="F125" s="56" t="s">
         <v>18</v>
       </c>
       <c r="G125" s="38" t="s">
@@ -12399,125 +12475,121 @@
     </row>
     <row r="126" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C126" s="34" t="s">
-        <v>213</v>
-      </c>
-      <c r="D126" s="44"/>
-      <c r="E126" s="46"/>
-      <c r="F126" s="46"/>
+        <v>202</v>
+      </c>
+      <c r="D126" s="57"/>
+      <c r="E126" s="56"/>
+      <c r="F126" s="56"/>
       <c r="G126" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="127" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C127" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="D127" s="44"/>
-      <c r="E127" s="46"/>
-      <c r="F127" s="46"/>
+        <v>210</v>
+      </c>
+      <c r="D127" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="E127" s="56"/>
+      <c r="F127" s="56" t="s">
+        <v>18</v>
+      </c>
       <c r="G127" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="128" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C128" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="D128" s="57"/>
+      <c r="E128" s="56"/>
+      <c r="F128" s="56"/>
+      <c r="G128" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="129" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C129" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="D129" s="57"/>
+      <c r="E129" s="56"/>
+      <c r="F129" s="56"/>
+      <c r="G129" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="130" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C130" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="D128" s="44" t="s">
+      <c r="D130" s="57" t="s">
         <v>223</v>
       </c>
-      <c r="E128" s="46"/>
-      <c r="F128" s="46" t="s">
+      <c r="E130" s="56"/>
+      <c r="F130" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="G128" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C129" s="34" t="s">
+      <c r="G130" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="131" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C131" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="D129" s="44"/>
-      <c r="E129" s="46"/>
-      <c r="F129" s="46"/>
-      <c r="G129" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C130" s="34" t="s">
+      <c r="D131" s="57"/>
+      <c r="E131" s="56"/>
+      <c r="F131" s="56"/>
+      <c r="G131" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="132" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C132" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="D130" s="44" t="s">
+      <c r="D132" s="57" t="s">
         <v>228</v>
       </c>
-      <c r="E130" s="46"/>
-      <c r="F130" s="46" t="s">
+      <c r="E132" s="56"/>
+      <c r="F132" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="G130" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C131" s="34" t="s">
+      <c r="G132" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="133" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C133" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="D131" s="44"/>
-      <c r="E131" s="46"/>
-      <c r="F131" s="46"/>
-      <c r="G131" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C132" s="34" t="s">
+      <c r="D133" s="57"/>
+      <c r="E133" s="56"/>
+      <c r="F133" s="56"/>
+      <c r="G133" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="134" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C134" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="D132" s="44"/>
-      <c r="E132" s="46"/>
-      <c r="F132" s="46"/>
-      <c r="G132" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C133" s="34" t="s">
+      <c r="D134" s="57"/>
+      <c r="E134" s="56"/>
+      <c r="F134" s="56"/>
+      <c r="G134" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="135" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C135" s="34" t="s">
         <v>267</v>
       </c>
-      <c r="D133" s="42" t="s">
+      <c r="D135" s="42" t="s">
         <v>268</v>
-      </c>
-      <c r="E133" s="43"/>
-      <c r="F133" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="G133" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C134" s="34" t="s">
-        <v>271</v>
-      </c>
-      <c r="D134" s="42" t="s">
-        <v>272</v>
-      </c>
-      <c r="E134" s="43"/>
-      <c r="F134" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="G134" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C135" s="34" t="s">
-        <v>275</v>
-      </c>
-      <c r="D135" s="42" t="s">
-        <v>276</v>
       </c>
       <c r="E135" s="43"/>
       <c r="F135" s="43" t="s">
@@ -12527,12 +12599,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C136" s="34" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="D136" s="42" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="E136" s="43"/>
       <c r="F136" s="43" t="s">
@@ -12542,124 +12614,255 @@
         <v>33</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A137" s="36"/>
-      <c r="B137" s="36"/>
+    <row r="137" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C137" s="34" t="s">
+        <v>275</v>
+      </c>
+      <c r="D137" s="42" t="s">
+        <v>276</v>
+      </c>
+      <c r="E137" s="43"/>
+      <c r="F137" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="G137" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="138" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C138" s="34" t="s">
+        <v>279</v>
+      </c>
+      <c r="D138" s="42" t="s">
+        <v>280</v>
+      </c>
+      <c r="E138" s="43"/>
+      <c r="F138" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="G138" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="139" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C139" s="34" t="s">
+        <v>454</v>
+      </c>
+      <c r="D139" s="57" t="s">
+        <v>582</v>
+      </c>
+      <c r="E139" s="56"/>
+      <c r="F139" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="G139" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="140" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C140" s="34" t="s">
+        <v>457</v>
+      </c>
+      <c r="D140" s="57"/>
+      <c r="E140" s="56"/>
+      <c r="F140" s="56"/>
+      <c r="G140" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="141" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C141" s="34" t="s">
+        <v>459</v>
+      </c>
+      <c r="D141" s="57" t="s">
+        <v>460</v>
+      </c>
+      <c r="E141" s="56"/>
+      <c r="F141" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="G141" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="142" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C142" s="34" t="s">
+        <v>462</v>
+      </c>
+      <c r="D142" s="57"/>
+      <c r="E142" s="56"/>
+      <c r="F142" s="56"/>
+      <c r="G142" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="143" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C143" s="34" t="s">
+        <v>402</v>
+      </c>
+      <c r="D143" s="44" t="s">
+        <v>403</v>
+      </c>
+      <c r="E143" s="45"/>
+      <c r="F143" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="G143" s="50" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="144" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C144" s="34" t="s">
+        <v>417</v>
+      </c>
+      <c r="D144" s="44" t="s">
+        <v>418</v>
+      </c>
+      <c r="E144" s="45"/>
+      <c r="F144" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="G144" s="50" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C145" s="34" t="s">
+        <v>431</v>
+      </c>
+      <c r="D145" s="44" t="s">
+        <v>432</v>
+      </c>
+      <c r="E145" s="45"/>
+      <c r="F145" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="G145" s="50" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A146" s="36"/>
+      <c r="B146" s="36"/>
+      <c r="C146" s="34" t="s">
         <v>477</v>
       </c>
-      <c r="D137" s="44" t="s">
+      <c r="D146" s="57" t="s">
         <v>478</v>
       </c>
-      <c r="E137" s="46"/>
-      <c r="F137" s="46" t="s">
+      <c r="E146" s="56"/>
+      <c r="F146" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="G137" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="H137" s="36"/>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A138" s="36"/>
-      <c r="B138" s="36"/>
-      <c r="C138" s="35" t="s">
+      <c r="G146" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="H146" s="36"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A147" s="36"/>
+      <c r="B147" s="36"/>
+      <c r="C147" s="35" t="s">
         <v>480</v>
       </c>
-      <c r="D138" s="45"/>
-      <c r="E138" s="47"/>
-      <c r="F138" s="47"/>
-      <c r="G138" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="H138" s="36"/>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A139" s="36"/>
-      <c r="B139" s="36"/>
-      <c r="C139" s="36"/>
-      <c r="D139" s="36"/>
-      <c r="E139" s="43"/>
-      <c r="F139" s="57"/>
-      <c r="G139" s="36"/>
-      <c r="H139" s="36"/>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A140" s="36"/>
-      <c r="B140" s="36"/>
-      <c r="C140" s="36"/>
-      <c r="D140" s="36"/>
-      <c r="E140" s="43">
-        <f>COUNTBLANK(E2:E138)</f>
-        <v>128</v>
-      </c>
-      <c r="F140" s="57"/>
-      <c r="G140" s="36"/>
-      <c r="H140" s="36"/>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A141" s="36"/>
-      <c r="B141" s="36"/>
-      <c r="C141" s="36"/>
-      <c r="D141" s="36"/>
-      <c r="E141" s="43">
-        <f>COUNTA(E2:E138)</f>
+      <c r="D147" s="59"/>
+      <c r="E147" s="61"/>
+      <c r="F147" s="61"/>
+      <c r="G147" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="H147" s="36"/>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A148" s="36"/>
+      <c r="B148" s="36"/>
+      <c r="C148" s="36"/>
+      <c r="D148" s="36"/>
+      <c r="E148" s="43"/>
+      <c r="F148" s="46"/>
+      <c r="G148" s="36"/>
+      <c r="H148" s="36"/>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A149" s="36"/>
+      <c r="B149" s="36"/>
+      <c r="C149" s="36"/>
+      <c r="D149" s="36"/>
+      <c r="E149" s="43">
+        <f>COUNTBLANK(E2:E147)</f>
+        <v>137</v>
+      </c>
+      <c r="F149" s="46"/>
+      <c r="G149" s="36"/>
+      <c r="H149" s="36"/>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A150" s="36"/>
+      <c r="B150" s="36"/>
+      <c r="C150" s="36"/>
+      <c r="D150" s="36"/>
+      <c r="E150" s="43">
+        <f>COUNTA(E2:E147)</f>
         <v>9</v>
       </c>
-      <c r="F141" s="57"/>
-      <c r="G141" s="36"/>
-      <c r="H141" s="36"/>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A142" s="36"/>
-      <c r="B142" s="36"/>
-      <c r="C142" s="36"/>
-      <c r="D142" s="36"/>
-      <c r="E142" s="43"/>
-      <c r="F142" s="57"/>
-      <c r="G142" s="36"/>
-      <c r="H142" s="36"/>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A143" s="36"/>
-      <c r="B143" s="36"/>
-      <c r="C143" s="36"/>
-      <c r="D143" s="36"/>
-      <c r="E143" s="43"/>
-      <c r="F143" s="57"/>
-      <c r="G143" s="36"/>
-      <c r="H143" s="36"/>
+      <c r="F150" s="46"/>
+      <c r="G150" s="36"/>
+      <c r="H150" s="36"/>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A151" s="36"/>
+      <c r="B151" s="36"/>
+      <c r="C151" s="36"/>
+      <c r="D151" s="36"/>
+      <c r="E151" s="43"/>
+      <c r="F151" s="46"/>
+      <c r="G151" s="36"/>
+      <c r="H151" s="36"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A152" s="36"/>
+      <c r="B152" s="36"/>
+      <c r="C152" s="36"/>
+      <c r="D152" s="36"/>
+      <c r="E152" s="43"/>
+      <c r="F152" s="46"/>
+      <c r="G152" s="36"/>
+      <c r="H152" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="191">
-    <mergeCell ref="E62:E64"/>
-    <mergeCell ref="F62:F64"/>
-    <mergeCell ref="D89:D91"/>
-    <mergeCell ref="E89:E91"/>
-    <mergeCell ref="F89:F91"/>
-    <mergeCell ref="D92:D94"/>
-    <mergeCell ref="E92:E94"/>
-    <mergeCell ref="F92:F94"/>
-    <mergeCell ref="E49:E51"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="F54:F55"/>
+  <mergeCells count="201">
+    <mergeCell ref="F64:F66"/>
+    <mergeCell ref="D91:D93"/>
+    <mergeCell ref="E91:E93"/>
+    <mergeCell ref="F91:F93"/>
+    <mergeCell ref="D94:D96"/>
+    <mergeCell ref="E94:E96"/>
+    <mergeCell ref="F94:F96"/>
+    <mergeCell ref="E51:E53"/>
     <mergeCell ref="E56:E57"/>
     <mergeCell ref="F56:F57"/>
     <mergeCell ref="E58:E59"/>
     <mergeCell ref="F58:F59"/>
     <mergeCell ref="E60:E61"/>
     <mergeCell ref="F60:F61"/>
-    <mergeCell ref="G46:G48"/>
-    <mergeCell ref="F49:F51"/>
-    <mergeCell ref="E87:E88"/>
-    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="D71:D74"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="D83:D84"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="F51:F53"/>
+    <mergeCell ref="E89:E90"/>
     <mergeCell ref="E75:E76"/>
     <mergeCell ref="E77:E78"/>
     <mergeCell ref="E79:E80"/>
     <mergeCell ref="E81:E82"/>
     <mergeCell ref="E83:E84"/>
     <mergeCell ref="E85:E86"/>
-    <mergeCell ref="F73:F74"/>
+    <mergeCell ref="E87:E88"/>
     <mergeCell ref="F75:F76"/>
     <mergeCell ref="F77:F78"/>
     <mergeCell ref="F79:F80"/>
@@ -12667,32 +12870,27 @@
     <mergeCell ref="F83:F84"/>
     <mergeCell ref="F85:F86"/>
     <mergeCell ref="F87:F88"/>
+    <mergeCell ref="F89:F90"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:F70"/>
     <mergeCell ref="E67:E68"/>
     <mergeCell ref="F67:F68"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="E69:E72"/>
-    <mergeCell ref="F69:F72"/>
-    <mergeCell ref="D69:D72"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="D83:D84"/>
-    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="E71:E74"/>
+    <mergeCell ref="F71:F74"/>
+    <mergeCell ref="E64:E66"/>
+    <mergeCell ref="D87:D88"/>
     <mergeCell ref="D40:D42"/>
     <mergeCell ref="D43:D45"/>
     <mergeCell ref="D46:D48"/>
-    <mergeCell ref="D49:D51"/>
-    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="D51:D53"/>
     <mergeCell ref="D56:D57"/>
-    <mergeCell ref="D62:D64"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="D87:D88"/>
     <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D64:D66"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="D89:D90"/>
     <mergeCell ref="D60:D61"/>
-    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="D69:D70"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
@@ -12705,6 +12903,14 @@
     <mergeCell ref="E9:E11"/>
     <mergeCell ref="F9:F11"/>
     <mergeCell ref="G9:G11"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="F22:F25"/>
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="F2:F4"/>
@@ -12725,14 +12931,6 @@
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="G14:G15"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="F22:F25"/>
     <mergeCell ref="D30:D31"/>
     <mergeCell ref="E30:E31"/>
     <mergeCell ref="F30:F31"/>
@@ -12749,20 +12947,6 @@
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="F28:F29"/>
     <mergeCell ref="G28:G29"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
     <mergeCell ref="G36:G37"/>
     <mergeCell ref="E40:E42"/>
     <mergeCell ref="F40:F42"/>
@@ -12772,57 +12956,82 @@
     <mergeCell ref="E46:E48"/>
     <mergeCell ref="F46:F48"/>
     <mergeCell ref="G43:G45"/>
-    <mergeCell ref="D103:D104"/>
-    <mergeCell ref="E103:E104"/>
-    <mergeCell ref="F103:F104"/>
-    <mergeCell ref="D105:D107"/>
-    <mergeCell ref="E105:E107"/>
-    <mergeCell ref="F105:F107"/>
-    <mergeCell ref="D98:D99"/>
-    <mergeCell ref="E98:E99"/>
-    <mergeCell ref="F98:F99"/>
-    <mergeCell ref="D100:D102"/>
-    <mergeCell ref="E100:E102"/>
-    <mergeCell ref="F100:F102"/>
-    <mergeCell ref="D113:D115"/>
-    <mergeCell ref="E113:E115"/>
-    <mergeCell ref="F113:F115"/>
-    <mergeCell ref="D116:D118"/>
-    <mergeCell ref="E116:E118"/>
-    <mergeCell ref="F116:F118"/>
-    <mergeCell ref="D108:D110"/>
-    <mergeCell ref="E108:E110"/>
-    <mergeCell ref="F108:F110"/>
-    <mergeCell ref="D111:D112"/>
-    <mergeCell ref="E111:E112"/>
-    <mergeCell ref="F111:F112"/>
+    <mergeCell ref="G46:G48"/>
+    <mergeCell ref="D105:D106"/>
+    <mergeCell ref="E105:E106"/>
+    <mergeCell ref="F105:F106"/>
+    <mergeCell ref="D107:D109"/>
+    <mergeCell ref="E107:E109"/>
+    <mergeCell ref="F107:F109"/>
+    <mergeCell ref="D100:D101"/>
+    <mergeCell ref="E100:E101"/>
+    <mergeCell ref="F100:F101"/>
+    <mergeCell ref="D102:D104"/>
+    <mergeCell ref="E102:E104"/>
+    <mergeCell ref="F102:F104"/>
+    <mergeCell ref="D115:D117"/>
+    <mergeCell ref="E115:E117"/>
+    <mergeCell ref="F115:F117"/>
+    <mergeCell ref="D118:D120"/>
+    <mergeCell ref="E118:E120"/>
+    <mergeCell ref="F118:F120"/>
+    <mergeCell ref="D110:D112"/>
+    <mergeCell ref="E110:E112"/>
+    <mergeCell ref="F110:F112"/>
+    <mergeCell ref="D113:D114"/>
+    <mergeCell ref="E113:E114"/>
+    <mergeCell ref="F113:F114"/>
+    <mergeCell ref="D125:D126"/>
+    <mergeCell ref="E125:E126"/>
+    <mergeCell ref="F125:F126"/>
+    <mergeCell ref="D127:D129"/>
+    <mergeCell ref="E127:E129"/>
+    <mergeCell ref="F127:F129"/>
+    <mergeCell ref="D121:D122"/>
+    <mergeCell ref="E121:E122"/>
+    <mergeCell ref="F121:F122"/>
     <mergeCell ref="D123:D124"/>
     <mergeCell ref="E123:E124"/>
     <mergeCell ref="F123:F124"/>
-    <mergeCell ref="D125:D127"/>
-    <mergeCell ref="E125:E127"/>
-    <mergeCell ref="F125:F127"/>
-    <mergeCell ref="D119:D120"/>
-    <mergeCell ref="E119:E120"/>
-    <mergeCell ref="F119:F120"/>
-    <mergeCell ref="D121:D122"/>
-    <mergeCell ref="E121:E122"/>
-    <mergeCell ref="F121:F122"/>
-    <mergeCell ref="D137:D138"/>
-    <mergeCell ref="E137:E138"/>
-    <mergeCell ref="F137:F138"/>
-    <mergeCell ref="D128:D129"/>
-    <mergeCell ref="E128:E129"/>
-    <mergeCell ref="F128:F129"/>
-    <mergeCell ref="D130:D132"/>
-    <mergeCell ref="E130:E132"/>
-    <mergeCell ref="F130:F132"/>
+    <mergeCell ref="D146:D147"/>
+    <mergeCell ref="E146:E147"/>
+    <mergeCell ref="F146:F147"/>
+    <mergeCell ref="D130:D131"/>
+    <mergeCell ref="E130:E131"/>
+    <mergeCell ref="F130:F131"/>
+    <mergeCell ref="D132:D134"/>
+    <mergeCell ref="E132:E134"/>
+    <mergeCell ref="F132:F134"/>
+    <mergeCell ref="D139:D140"/>
+    <mergeCell ref="D141:D142"/>
+    <mergeCell ref="F139:F140"/>
+    <mergeCell ref="F141:F142"/>
+    <mergeCell ref="E139:E140"/>
+    <mergeCell ref="E141:E142"/>
     <mergeCell ref="O5:O6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="D95:D97"/>
-    <mergeCell ref="E95:E97"/>
-    <mergeCell ref="F95:F97"/>
+    <mergeCell ref="D97:D99"/>
+    <mergeCell ref="E97:E99"/>
+    <mergeCell ref="F97:F99"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -13231,10 +13440,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A026136A-3463-4F46-9920-D2EEED3E1AFC}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R1048576"/>
+      <selection activeCell="A17" sqref="A17:W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13242,8 +13451,7 @@
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.85546875" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -13254,7 +13462,7 @@
     <col min="17" max="17" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -13271,7 +13479,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>365</v>
       </c>
@@ -13307,7 +13515,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>370</v>
       </c>
@@ -13343,7 +13551,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>373</v>
       </c>
@@ -13379,7 +13587,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>376</v>
       </c>
@@ -13415,7 +13623,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>378</v>
       </c>
@@ -13430,7 +13638,7 @@
       </c>
       <c r="E6" s="20"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>380</v>
       </c>
@@ -13445,7 +13653,7 @@
       </c>
       <c r="E7" s="21"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>382</v>
       </c>
@@ -13460,7 +13668,7 @@
       </c>
       <c r="E8" s="20"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>384</v>
       </c>
@@ -13475,7 +13683,7 @@
       </c>
       <c r="E9" s="21"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>386</v>
       </c>
@@ -13492,6 +13700,244 @@
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B14" s="67"/>
+      <c r="C14" s="67">
+        <v>44358</v>
+      </c>
+      <c r="D14" t="s">
+        <v>586</v>
+      </c>
+      <c r="E14">
+        <v>102341</v>
+      </c>
+      <c r="F14">
+        <v>3628</v>
+      </c>
+      <c r="G14">
+        <v>19</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>3</v>
+      </c>
+      <c r="K14">
+        <v>131</v>
+      </c>
+      <c r="L14">
+        <v>129</v>
+      </c>
+      <c r="M14">
+        <v>145</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>75</v>
+      </c>
+      <c r="Q14">
+        <v>2021</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="T14" t="s">
+        <v>587</v>
+      </c>
+      <c r="U14">
+        <v>47.615000000000002</v>
+      </c>
+      <c r="V14">
+        <v>-5.5083000000000002</v>
+      </c>
+      <c r="W14">
+        <v>96304</v>
+      </c>
+      <c r="X14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B15" s="67"/>
+      <c r="C15" s="67">
+        <v>44358</v>
+      </c>
+      <c r="D15" t="s">
+        <v>586</v>
+      </c>
+      <c r="E15">
+        <v>102623</v>
+      </c>
+      <c r="F15">
+        <v>3372</v>
+      </c>
+      <c r="G15">
+        <v>19</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="K15">
+        <v>131</v>
+      </c>
+      <c r="L15">
+        <v>129</v>
+      </c>
+      <c r="M15">
+        <v>145</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>75</v>
+      </c>
+      <c r="Q15">
+        <v>2021</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="T15" t="s">
+        <v>587</v>
+      </c>
+      <c r="U15">
+        <v>47.615000000000002</v>
+      </c>
+      <c r="V15">
+        <v>-5.5083000000000002</v>
+      </c>
+      <c r="W15">
+        <v>97931</v>
+      </c>
+      <c r="X15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B16" s="67">
+        <v>44385</v>
+      </c>
+      <c r="C16" t="s">
+        <v>586</v>
+      </c>
+      <c r="D16">
+        <v>102341</v>
+      </c>
+      <c r="E16">
+        <v>3628</v>
+      </c>
+      <c r="F16">
+        <v>19</v>
+      </c>
+      <c r="G16">
+        <v>41</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <v>448</v>
+      </c>
+      <c r="K16">
+        <v>444</v>
+      </c>
+      <c r="L16">
+        <v>181</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>59</v>
+      </c>
+      <c r="P16">
+        <v>2021</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="S16" t="s">
+        <v>588</v>
+      </c>
+      <c r="T16">
+        <v>55.76</v>
+      </c>
+      <c r="U16">
+        <v>-9.3633000000000006</v>
+      </c>
+      <c r="V16">
+        <v>96304</v>
+      </c>
+      <c r="W16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B17" s="67">
+        <v>44385</v>
+      </c>
+      <c r="C17" t="s">
+        <v>586</v>
+      </c>
+      <c r="D17">
+        <v>102623</v>
+      </c>
+      <c r="E17">
+        <v>3372</v>
+      </c>
+      <c r="F17">
+        <v>19</v>
+      </c>
+      <c r="G17">
+        <v>41</v>
+      </c>
+      <c r="I17">
+        <v>3</v>
+      </c>
+      <c r="J17">
+        <v>448</v>
+      </c>
+      <c r="K17">
+        <v>444</v>
+      </c>
+      <c r="L17">
+        <v>181</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>59</v>
+      </c>
+      <c r="P17">
+        <v>2021</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="S17" t="s">
+        <v>588</v>
+      </c>
+      <c r="T17">
+        <v>55.76</v>
+      </c>
+      <c r="U17">
+        <v>-9.3633000000000006</v>
+      </c>
+      <c r="V17">
+        <v>97971</v>
+      </c>
+      <c r="W17">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13500,26 +13946,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FC052A-0F27-488A-94F5-1C9E9BC7A4D4}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L15" sqref="L15:L16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>582</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6DDA247-F6AE-445A-B41C-F6181C9C037C}">
   <dimension ref="A1:C44"/>
   <sheetViews>
@@ -13896,7 +14322,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABE3366-981D-4444-A865-F5BA56B32FED}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -14220,16 +14646,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Scripts for bioluminescence and birds analysis added
</commit_message>
<xml_diff>
--- a/analysis/MEDS_Tables.xlsx
+++ b/analysis/MEDS_Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="569" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEAA9636-4C71-4E48-BA56-51D516E5BD25}"/>
+  <xr:revisionPtr revIDLastSave="571" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D4AA51C-799E-4C6C-BACE-7A659EE3CD3C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meds_tables" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2710" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2728" uniqueCount="590">
   <si>
     <t>Table</t>
   </si>
@@ -2537,7 +2537,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2651,13 +2651,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2666,39 +2675,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -10732,8 +10733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8FA477-9B46-4053-B7AD-310B8B9F2B30}">
   <dimension ref="A1:P152"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10749,7 +10750,7 @@
     <col min="11" max="11" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:16" s="40" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" s="40" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="51" t="s">
         <v>0</v>
       </c>
@@ -10768,38 +10769,40 @@
       <c r="H1" s="48"/>
       <c r="I1" s="41">
         <f>E150/E149</f>
-        <v>6.569343065693431E-2</v>
+        <v>8.1481481481481488E-2</v>
       </c>
       <c r="J1" s="49" t="s">
         <v>566</v>
       </c>
       <c r="K1" s="48"/>
     </row>
-    <row r="2" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="71"/>
       <c r="C2" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="61" t="s">
+      <c r="E2" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="61" t="s">
+      <c r="F2" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="65" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="3" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="71"/>
       <c r="C3" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="67"/>
       <c r="K3" s="36"/>
       <c r="L3" s="36"/>
       <c r="M3" s="36"/>
@@ -10807,14 +10810,15 @@
       <c r="O3" s="36"/>
       <c r="P3" s="36"/>
     </row>
-    <row r="4" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="71"/>
       <c r="C4" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="67"/>
       <c r="K4" s="36"/>
       <c r="L4" s="36"/>
       <c r="M4" s="36"/>
@@ -10822,66 +10826,69 @@
       <c r="O4" s="36"/>
       <c r="P4" s="36"/>
     </row>
-    <row r="5" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="71"/>
       <c r="C5" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="56" t="s">
+      <c r="D5" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="60" t="s">
+      <c r="G5" s="67" t="s">
         <v>519</v>
       </c>
       <c r="K5" s="36"/>
       <c r="L5" s="47" t="s">
         <v>464</v>
       </c>
-      <c r="M5" s="67" t="s">
+      <c r="M5" s="58" t="s">
         <v>465</v>
       </c>
-      <c r="N5" s="55"/>
-      <c r="O5" s="66" t="s">
+      <c r="N5" s="59"/>
+      <c r="O5" s="57" t="s">
         <v>581</v>
       </c>
       <c r="P5" s="36"/>
     </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="71"/>
       <c r="C6" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="56"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="67"/>
       <c r="K6" s="36"/>
       <c r="L6" s="47" t="s">
         <v>467</v>
       </c>
-      <c r="M6" s="67"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="66"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="57"/>
       <c r="P6" s="36"/>
     </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="71"/>
       <c r="C7" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="56" t="s">
+      <c r="D7" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="55" t="s">
+      <c r="E7" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="55" t="s">
+      <c r="F7" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="60" t="s">
+      <c r="G7" s="67" t="s">
         <v>80</v>
       </c>
       <c r="K7" s="36"/>
@@ -10891,14 +10898,15 @@
       <c r="O7" s="36"/>
       <c r="P7" s="36"/>
     </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="71"/>
       <c r="C8" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="56"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="67"/>
       <c r="K8" s="36"/>
       <c r="L8" s="36"/>
       <c r="M8" s="36"/>
@@ -10906,291 +10914,342 @@
       <c r="O8" s="36"/>
       <c r="P8" s="36"/>
     </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="71"/>
       <c r="C9" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="D9" s="56" t="s">
+      <c r="D9" s="60" t="s">
         <v>171</v>
       </c>
-      <c r="E9" s="55" t="s">
+      <c r="E9" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="55" t="s">
+      <c r="F9" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="60" t="s">
+      <c r="G9" s="67" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="71"/>
       <c r="C10" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="D10" s="56"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="60"/>
-    </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="D10" s="60"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="67"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="71"/>
       <c r="C11" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="D11" s="56"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="60"/>
-    </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="D11" s="60"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="67"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="71"/>
       <c r="C12" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="D12" s="56" t="s">
+      <c r="D12" s="60" t="s">
         <v>204</v>
       </c>
-      <c r="E12" s="55" t="s">
+      <c r="E12" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="55" t="s">
+      <c r="F12" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="60" t="s">
+      <c r="G12" s="67" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="71"/>
       <c r="C13" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="D13" s="56"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="60"/>
-    </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="D13" s="60"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="67"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="71"/>
       <c r="C14" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="D14" s="56" t="s">
+      <c r="D14" s="60" t="s">
         <v>361</v>
       </c>
-      <c r="E14" s="55" t="s">
+      <c r="E14" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F14" s="55" t="s">
+      <c r="F14" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="60" t="s">
+      <c r="G14" s="67" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="71"/>
       <c r="C15" s="35" t="s">
         <v>363</v>
       </c>
-      <c r="D15" s="59"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="64"/>
-    </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="D15" s="62"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="66"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C16" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="58" t="s">
+      <c r="D16" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61" t="s">
+      <c r="E16" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="63" t="s">
         <v>567</v>
       </c>
-      <c r="G16" s="62" t="s">
+      <c r="G16" s="65" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C17" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="56"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="60"/>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D17" s="60"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="67"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C18" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="56" t="s">
+      <c r="D18" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55" t="s">
+      <c r="E18" s="59"/>
+      <c r="F18" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G18" s="60" t="s">
+      <c r="G18" s="67" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C19" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="56"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="60"/>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D19" s="60"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="67"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C20" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="D20" s="56" t="s">
+      <c r="D20" s="60" t="s">
         <v>300</v>
       </c>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55" t="s">
+      <c r="E20" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G20" s="60" t="s">
+      <c r="G20" s="67" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C21" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="D21" s="56"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="60"/>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D21" s="60"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="67"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C22" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="D22" s="56" t="s">
+      <c r="D22" s="60" t="s">
         <v>305</v>
       </c>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55" t="s">
+      <c r="E22" s="59"/>
+      <c r="F22" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G22" s="60" t="s">
+      <c r="G22" s="67" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C23" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="D23" s="56"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="60"/>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D23" s="60"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="67"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C24" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="D24" s="56"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="60"/>
-    </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D24" s="60"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="67"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C25" s="34" t="s">
         <v>311</v>
       </c>
-      <c r="D25" s="56"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="60"/>
-    </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D25" s="60"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="67"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C26" s="34" t="s">
         <v>317</v>
       </c>
-      <c r="D26" s="56" t="s">
+      <c r="D26" s="60" t="s">
         <v>318</v>
       </c>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55" t="s">
+      <c r="E26" s="59"/>
+      <c r="F26" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G26" s="60" t="s">
+      <c r="G26" s="67" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C27" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="D27" s="56"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="60"/>
-    </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D27" s="60"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="67"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C28" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="D28" s="57" t="s">
+      <c r="D28" s="68" t="s">
         <v>323</v>
       </c>
-      <c r="E28" s="65"/>
-      <c r="F28" s="55" t="s">
+      <c r="E28" s="69"/>
+      <c r="F28" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G28" s="60" t="s">
+      <c r="G28" s="67" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="J28" s="36"/>
+      <c r="K28" s="36"/>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C29" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="D29" s="57"/>
-      <c r="E29" s="65"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="60"/>
-    </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D29" s="68"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="67"/>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C30" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="D30" s="56" t="s">
+      <c r="D30" s="60" t="s">
         <v>328</v>
       </c>
-      <c r="E30" s="55"/>
-      <c r="F30" s="55" t="s">
+      <c r="E30" s="59"/>
+      <c r="F30" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G30" s="60" t="s">
+      <c r="G30" s="67" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C31" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="D31" s="56"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="60"/>
-    </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D31" s="60"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="67"/>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="D32" s="56" t="s">
+      <c r="D32" s="60" t="s">
         <v>333</v>
       </c>
-      <c r="E32" s="55"/>
-      <c r="F32" s="55" t="s">
+      <c r="E32" s="59"/>
+      <c r="F32" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G32" s="60" t="s">
+      <c r="G32" s="67" t="s">
         <v>510</v>
       </c>
     </row>
@@ -11198,23 +11257,23 @@
       <c r="C33" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="D33" s="56"/>
-      <c r="E33" s="55"/>
-      <c r="F33" s="55"/>
-      <c r="G33" s="60"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="67"/>
     </row>
     <row r="34" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C34" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="D34" s="56" t="s">
+      <c r="D34" s="60" t="s">
         <v>338</v>
       </c>
-      <c r="E34" s="55"/>
-      <c r="F34" s="55" t="s">
+      <c r="E34" s="59"/>
+      <c r="F34" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G34" s="60" t="s">
+      <c r="G34" s="67" t="s">
         <v>511</v>
       </c>
     </row>
@@ -11222,23 +11281,23 @@
       <c r="C35" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="D35" s="56"/>
-      <c r="E35" s="55"/>
-      <c r="F35" s="55"/>
-      <c r="G35" s="60"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="67"/>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C36" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="D36" s="56" t="s">
+      <c r="D36" s="60" t="s">
         <v>343</v>
       </c>
-      <c r="E36" s="55"/>
-      <c r="F36" s="55" t="s">
+      <c r="E36" s="59"/>
+      <c r="F36" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G36" s="60" t="s">
+      <c r="G36" s="67" t="s">
         <v>509</v>
       </c>
     </row>
@@ -11246,23 +11305,23 @@
       <c r="C37" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="D37" s="56"/>
-      <c r="E37" s="55"/>
-      <c r="F37" s="55"/>
-      <c r="G37" s="60"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="67"/>
     </row>
     <row r="38" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C38" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="D38" s="56" t="s">
+      <c r="D38" s="60" t="s">
         <v>348</v>
       </c>
-      <c r="E38" s="55"/>
-      <c r="F38" s="55" t="s">
+      <c r="E38" s="59"/>
+      <c r="F38" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G38" s="60" t="s">
+      <c r="G38" s="67" t="s">
         <v>520</v>
       </c>
     </row>
@@ -11270,25 +11329,25 @@
       <c r="C39" s="35" t="s">
         <v>350</v>
       </c>
-      <c r="D39" s="59"/>
-      <c r="E39" s="63"/>
-      <c r="F39" s="63"/>
-      <c r="G39" s="64"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="64"/>
+      <c r="F39" s="64"/>
+      <c r="G39" s="66"/>
     </row>
     <row r="40" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C40" s="33" t="s">
         <v>365</v>
       </c>
-      <c r="D40" s="58" t="s">
+      <c r="D40" s="61" t="s">
         <v>366</v>
       </c>
-      <c r="E40" s="61" t="s">
+      <c r="E40" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="F40" s="61" t="s">
+      <c r="F40" s="63" t="s">
         <v>369</v>
       </c>
-      <c r="G40" s="62" t="s">
+      <c r="G40" s="65" t="s">
         <v>514</v>
       </c>
     </row>
@@ -11296,34 +11355,34 @@
       <c r="C41" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="D41" s="56"/>
-      <c r="E41" s="55"/>
-      <c r="F41" s="55"/>
-      <c r="G41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="59"/>
+      <c r="F41" s="59"/>
+      <c r="G41" s="67"/>
     </row>
     <row r="42" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C42" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="D42" s="56"/>
-      <c r="E42" s="55"/>
-      <c r="F42" s="55"/>
-      <c r="G42" s="60"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="59"/>
+      <c r="G42" s="67"/>
     </row>
     <row r="43" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C43" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="D43" s="56" t="s">
+      <c r="D43" s="60" t="s">
         <v>371</v>
       </c>
-      <c r="E43" s="55" t="s">
+      <c r="E43" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F43" s="55" t="s">
+      <c r="F43" s="59" t="s">
         <v>369</v>
       </c>
-      <c r="G43" s="60" t="s">
+      <c r="G43" s="67" t="s">
         <v>513</v>
       </c>
     </row>
@@ -11331,34 +11390,34 @@
       <c r="C44" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="D44" s="56"/>
-      <c r="E44" s="55"/>
-      <c r="F44" s="55"/>
-      <c r="G44" s="60"/>
+      <c r="D44" s="60"/>
+      <c r="E44" s="59"/>
+      <c r="F44" s="59"/>
+      <c r="G44" s="67"/>
     </row>
     <row r="45" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C45" s="34" t="s">
         <v>384</v>
       </c>
-      <c r="D45" s="56"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="60"/>
+      <c r="D45" s="60"/>
+      <c r="E45" s="59"/>
+      <c r="F45" s="59"/>
+      <c r="G45" s="67"/>
     </row>
     <row r="46" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C46" s="34" t="s">
         <v>373</v>
       </c>
-      <c r="D46" s="56" t="s">
+      <c r="D46" s="60" t="s">
         <v>374</v>
       </c>
-      <c r="E46" s="55" t="s">
+      <c r="E46" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F46" s="55" t="s">
+      <c r="F46" s="59" t="s">
         <v>369</v>
       </c>
-      <c r="G46" s="60" t="s">
+      <c r="G46" s="67" t="s">
         <v>522</v>
       </c>
     </row>
@@ -11366,19 +11425,19 @@
       <c r="C47" s="34" t="s">
         <v>380</v>
       </c>
-      <c r="D47" s="56"/>
-      <c r="E47" s="55"/>
-      <c r="F47" s="55"/>
-      <c r="G47" s="60"/>
+      <c r="D47" s="60"/>
+      <c r="E47" s="59"/>
+      <c r="F47" s="59"/>
+      <c r="G47" s="67"/>
     </row>
     <row r="48" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C48" s="35" t="s">
         <v>386</v>
       </c>
-      <c r="D48" s="59"/>
-      <c r="E48" s="63"/>
-      <c r="F48" s="63"/>
-      <c r="G48" s="64"/>
+      <c r="D48" s="62"/>
+      <c r="E48" s="64"/>
+      <c r="F48" s="64"/>
+      <c r="G48" s="66"/>
       <c r="J48" s="36"/>
       <c r="K48" s="36"/>
       <c r="L48" s="36"/>
@@ -11388,14 +11447,14 @@
       <c r="C49" s="33" t="s">
         <v>464</v>
       </c>
-      <c r="D49" s="58" t="s">
+      <c r="D49" s="61" t="s">
         <v>465</v>
       </c>
-      <c r="E49" s="61"/>
-      <c r="F49" s="61" t="s">
+      <c r="E49" s="63"/>
+      <c r="F49" s="63" t="s">
         <v>584</v>
       </c>
-      <c r="G49" s="62" t="s">
+      <c r="G49" s="65" t="s">
         <v>585</v>
       </c>
       <c r="J49" s="36"/>
@@ -11407,10 +11466,10 @@
       <c r="C50" s="35" t="s">
         <v>467</v>
       </c>
-      <c r="D50" s="59"/>
-      <c r="E50" s="63"/>
-      <c r="F50" s="63"/>
-      <c r="G50" s="64"/>
+      <c r="D50" s="62"/>
+      <c r="E50" s="64"/>
+      <c r="F50" s="64"/>
+      <c r="G50" s="66"/>
       <c r="J50" s="36"/>
       <c r="K50" s="36"/>
       <c r="L50" s="36"/>
@@ -11420,11 +11479,11 @@
       <c r="C51" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="D51" s="56" t="s">
+      <c r="D51" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="E51" s="55"/>
-      <c r="F51" s="55" t="s">
+      <c r="E51" s="59"/>
+      <c r="F51" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G51" s="38" t="s">
@@ -11439,9 +11498,9 @@
       <c r="C52" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D52" s="56"/>
-      <c r="E52" s="55"/>
-      <c r="F52" s="55"/>
+      <c r="D52" s="60"/>
+      <c r="E52" s="59"/>
+      <c r="F52" s="59"/>
       <c r="G52" s="38" t="s">
         <v>33</v>
       </c>
@@ -11454,9 +11513,9 @@
       <c r="C53" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D53" s="56"/>
-      <c r="E53" s="55"/>
-      <c r="F53" s="55"/>
+      <c r="D53" s="60"/>
+      <c r="E53" s="59"/>
+      <c r="F53" s="59"/>
       <c r="G53" s="38" t="s">
         <v>33</v>
       </c>
@@ -11469,11 +11528,11 @@
       <c r="C54" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="D54" s="56" t="s">
+      <c r="D54" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="E54" s="55"/>
-      <c r="F54" s="55" t="s">
+      <c r="E54" s="59"/>
+      <c r="F54" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G54" s="38" t="s">
@@ -11488,9 +11547,9 @@
       <c r="C55" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D55" s="56"/>
-      <c r="E55" s="55"/>
-      <c r="F55" s="55"/>
+      <c r="D55" s="60"/>
+      <c r="E55" s="59"/>
+      <c r="F55" s="59"/>
       <c r="G55" s="38" t="s">
         <v>33</v>
       </c>
@@ -11503,11 +11562,11 @@
       <c r="C56" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D56" s="56" t="s">
+      <c r="D56" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="E56" s="55"/>
-      <c r="F56" s="55" t="s">
+      <c r="E56" s="59"/>
+      <c r="F56" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G56" s="38" t="s">
@@ -11522,9 +11581,9 @@
       <c r="C57" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D57" s="56"/>
-      <c r="E57" s="55"/>
-      <c r="F57" s="55"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="59"/>
+      <c r="F57" s="59"/>
       <c r="G57" s="38" t="s">
         <v>33</v>
       </c>
@@ -11537,11 +11596,11 @@
       <c r="C58" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D58" s="56" t="s">
+      <c r="D58" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="E58" s="55"/>
-      <c r="F58" s="55" t="s">
+      <c r="E58" s="59"/>
+      <c r="F58" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G58" s="38" t="s">
@@ -11556,9 +11615,9 @@
       <c r="C59" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D59" s="56"/>
-      <c r="E59" s="55"/>
-      <c r="F59" s="55"/>
+      <c r="D59" s="60"/>
+      <c r="E59" s="59"/>
+      <c r="F59" s="59"/>
       <c r="G59" s="38" t="s">
         <v>33</v>
       </c>
@@ -11571,11 +11630,11 @@
       <c r="C60" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="D60" s="56" t="s">
+      <c r="D60" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="E60" s="55"/>
-      <c r="F60" s="55" t="s">
+      <c r="E60" s="59"/>
+      <c r="F60" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G60" s="38" t="s">
@@ -11590,9 +11649,9 @@
       <c r="C61" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D61" s="56"/>
-      <c r="E61" s="55"/>
-      <c r="F61" s="55"/>
+      <c r="D61" s="60"/>
+      <c r="E61" s="59"/>
+      <c r="F61" s="59"/>
       <c r="G61" s="38" t="s">
         <v>33</v>
       </c>
@@ -11605,11 +11664,11 @@
       <c r="C62" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D62" s="56" t="s">
+      <c r="D62" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="E62" s="55"/>
-      <c r="F62" s="55" t="s">
+      <c r="E62" s="59"/>
+      <c r="F62" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G62" s="38" t="s">
@@ -11624,9 +11683,9 @@
       <c r="C63" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D63" s="56"/>
-      <c r="E63" s="55"/>
-      <c r="F63" s="55"/>
+      <c r="D63" s="60"/>
+      <c r="E63" s="59"/>
+      <c r="F63" s="59"/>
       <c r="G63" s="38" t="s">
         <v>33</v>
       </c>
@@ -11639,11 +11698,11 @@
       <c r="C64" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="D64" s="56" t="s">
+      <c r="D64" s="60" t="s">
         <v>171</v>
       </c>
-      <c r="E64" s="55"/>
-      <c r="F64" s="55" t="s">
+      <c r="E64" s="59"/>
+      <c r="F64" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G64" s="38" t="s">
@@ -11658,9 +11717,9 @@
       <c r="C65" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="D65" s="56"/>
-      <c r="E65" s="55"/>
-      <c r="F65" s="55"/>
+      <c r="D65" s="60"/>
+      <c r="E65" s="59"/>
+      <c r="F65" s="59"/>
       <c r="G65" s="38" t="s">
         <v>33</v>
       </c>
@@ -11673,9 +11732,9 @@
       <c r="C66" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="D66" s="56"/>
-      <c r="E66" s="55"/>
-      <c r="F66" s="55"/>
+      <c r="D66" s="60"/>
+      <c r="E66" s="59"/>
+      <c r="F66" s="59"/>
       <c r="G66" s="38" t="s">
         <v>33</v>
       </c>
@@ -11688,11 +11747,11 @@
       <c r="C67" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="D67" s="56" t="s">
+      <c r="D67" s="60" t="s">
         <v>204</v>
       </c>
-      <c r="E67" s="55"/>
-      <c r="F67" s="55" t="s">
+      <c r="E67" s="59"/>
+      <c r="F67" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G67" s="38" t="s">
@@ -11707,9 +11766,9 @@
       <c r="C68" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="D68" s="56"/>
-      <c r="E68" s="55"/>
-      <c r="F68" s="55"/>
+      <c r="D68" s="60"/>
+      <c r="E68" s="59"/>
+      <c r="F68" s="59"/>
       <c r="G68" s="38" t="s">
         <v>33</v>
       </c>
@@ -11722,11 +11781,11 @@
       <c r="C69" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="D69" s="56" t="s">
+      <c r="D69" s="60" t="s">
         <v>300</v>
       </c>
-      <c r="E69" s="55"/>
-      <c r="F69" s="55" t="s">
+      <c r="E69" s="59"/>
+      <c r="F69" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G69" s="38" t="s">
@@ -11741,9 +11800,9 @@
       <c r="C70" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="D70" s="56"/>
-      <c r="E70" s="55"/>
-      <c r="F70" s="55"/>
+      <c r="D70" s="60"/>
+      <c r="E70" s="59"/>
+      <c r="F70" s="59"/>
       <c r="G70" s="38" t="s">
         <v>33</v>
       </c>
@@ -11756,11 +11815,11 @@
       <c r="C71" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="D71" s="56" t="s">
+      <c r="D71" s="60" t="s">
         <v>305</v>
       </c>
-      <c r="E71" s="55"/>
-      <c r="F71" s="55" t="s">
+      <c r="E71" s="59"/>
+      <c r="F71" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G71" s="38" t="s">
@@ -11775,9 +11834,9 @@
       <c r="C72" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="D72" s="56"/>
-      <c r="E72" s="55"/>
-      <c r="F72" s="55"/>
+      <c r="D72" s="60"/>
+      <c r="E72" s="59"/>
+      <c r="F72" s="59"/>
       <c r="G72" s="38" t="s">
         <v>33</v>
       </c>
@@ -11790,9 +11849,9 @@
       <c r="C73" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="D73" s="56"/>
-      <c r="E73" s="55"/>
-      <c r="F73" s="55"/>
+      <c r="D73" s="60"/>
+      <c r="E73" s="59"/>
+      <c r="F73" s="59"/>
       <c r="G73" s="38" t="s">
         <v>33</v>
       </c>
@@ -11805,9 +11864,9 @@
       <c r="C74" s="34" t="s">
         <v>311</v>
       </c>
-      <c r="D74" s="56"/>
-      <c r="E74" s="55"/>
-      <c r="F74" s="55"/>
+      <c r="D74" s="60"/>
+      <c r="E74" s="59"/>
+      <c r="F74" s="59"/>
       <c r="G74" s="38" t="s">
         <v>33</v>
       </c>
@@ -11820,11 +11879,11 @@
       <c r="C75" s="34" t="s">
         <v>317</v>
       </c>
-      <c r="D75" s="56" t="s">
+      <c r="D75" s="60" t="s">
         <v>318</v>
       </c>
-      <c r="E75" s="55"/>
-      <c r="F75" s="55" t="s">
+      <c r="E75" s="59"/>
+      <c r="F75" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G75" s="38" t="s">
@@ -11839,9 +11898,9 @@
       <c r="C76" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="D76" s="56"/>
-      <c r="E76" s="55"/>
-      <c r="F76" s="55"/>
+      <c r="D76" s="60"/>
+      <c r="E76" s="59"/>
+      <c r="F76" s="59"/>
       <c r="G76" s="38" t="s">
         <v>33</v>
       </c>
@@ -11854,11 +11913,11 @@
       <c r="C77" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="D77" s="57" t="s">
+      <c r="D77" s="68" t="s">
         <v>323</v>
       </c>
-      <c r="E77" s="55"/>
-      <c r="F77" s="55" t="s">
+      <c r="E77" s="59"/>
+      <c r="F77" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G77" s="38" t="s">
@@ -11873,9 +11932,9 @@
       <c r="C78" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="D78" s="57"/>
-      <c r="E78" s="55"/>
-      <c r="F78" s="55"/>
+      <c r="D78" s="68"/>
+      <c r="E78" s="59"/>
+      <c r="F78" s="59"/>
       <c r="G78" s="38" t="s">
         <v>33</v>
       </c>
@@ -11884,11 +11943,11 @@
       <c r="C79" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="D79" s="56" t="s">
+      <c r="D79" s="60" t="s">
         <v>328</v>
       </c>
-      <c r="E79" s="55"/>
-      <c r="F79" s="55" t="s">
+      <c r="E79" s="59"/>
+      <c r="F79" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G79" s="38" t="s">
@@ -11899,9 +11958,9 @@
       <c r="C80" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="D80" s="56"/>
-      <c r="E80" s="55"/>
-      <c r="F80" s="55"/>
+      <c r="D80" s="60"/>
+      <c r="E80" s="59"/>
+      <c r="F80" s="59"/>
       <c r="G80" s="38" t="s">
         <v>33</v>
       </c>
@@ -11910,11 +11969,11 @@
       <c r="C81" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="D81" s="56" t="s">
+      <c r="D81" s="60" t="s">
         <v>333</v>
       </c>
-      <c r="E81" s="55"/>
-      <c r="F81" s="55" t="s">
+      <c r="E81" s="59"/>
+      <c r="F81" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G81" s="38" t="s">
@@ -11925,9 +11984,9 @@
       <c r="C82" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="D82" s="56"/>
-      <c r="E82" s="55"/>
-      <c r="F82" s="55"/>
+      <c r="D82" s="60"/>
+      <c r="E82" s="59"/>
+      <c r="F82" s="59"/>
       <c r="G82" s="38" t="s">
         <v>33</v>
       </c>
@@ -11936,11 +11995,11 @@
       <c r="C83" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="D83" s="56" t="s">
+      <c r="D83" s="60" t="s">
         <v>338</v>
       </c>
-      <c r="E83" s="55"/>
-      <c r="F83" s="55" t="s">
+      <c r="E83" s="59"/>
+      <c r="F83" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G83" s="38" t="s">
@@ -11951,9 +12010,9 @@
       <c r="C84" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="D84" s="56"/>
-      <c r="E84" s="55"/>
-      <c r="F84" s="55"/>
+      <c r="D84" s="60"/>
+      <c r="E84" s="59"/>
+      <c r="F84" s="59"/>
       <c r="G84" s="38" t="s">
         <v>33</v>
       </c>
@@ -11962,11 +12021,11 @@
       <c r="C85" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="D85" s="56" t="s">
+      <c r="D85" s="60" t="s">
         <v>343</v>
       </c>
-      <c r="E85" s="55"/>
-      <c r="F85" s="55" t="s">
+      <c r="E85" s="59"/>
+      <c r="F85" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G85" s="38" t="s">
@@ -11977,9 +12036,9 @@
       <c r="C86" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="D86" s="56"/>
-      <c r="E86" s="55"/>
-      <c r="F86" s="55"/>
+      <c r="D86" s="60"/>
+      <c r="E86" s="59"/>
+      <c r="F86" s="59"/>
       <c r="G86" s="38" t="s">
         <v>33</v>
       </c>
@@ -11988,11 +12047,11 @@
       <c r="C87" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="D87" s="56" t="s">
+      <c r="D87" s="60" t="s">
         <v>348</v>
       </c>
-      <c r="E87" s="55"/>
-      <c r="F87" s="55" t="s">
+      <c r="E87" s="59"/>
+      <c r="F87" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G87" s="38" t="s">
@@ -12003,9 +12062,9 @@
       <c r="C88" s="34" t="s">
         <v>350</v>
       </c>
-      <c r="D88" s="56"/>
-      <c r="E88" s="55"/>
-      <c r="F88" s="55"/>
+      <c r="D88" s="60"/>
+      <c r="E88" s="59"/>
+      <c r="F88" s="59"/>
       <c r="G88" s="38" t="s">
         <v>33</v>
       </c>
@@ -12014,11 +12073,11 @@
       <c r="C89" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="D89" s="56" t="s">
+      <c r="D89" s="60" t="s">
         <v>361</v>
       </c>
-      <c r="E89" s="55"/>
-      <c r="F89" s="55" t="s">
+      <c r="E89" s="59"/>
+      <c r="F89" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G89" s="38" t="s">
@@ -12029,9 +12088,9 @@
       <c r="C90" s="34" t="s">
         <v>363</v>
       </c>
-      <c r="D90" s="56"/>
-      <c r="E90" s="55"/>
-      <c r="F90" s="55"/>
+      <c r="D90" s="60"/>
+      <c r="E90" s="59"/>
+      <c r="F90" s="59"/>
       <c r="G90" s="38" t="s">
         <v>33</v>
       </c>
@@ -12040,11 +12099,11 @@
       <c r="C91" s="34" t="s">
         <v>365</v>
       </c>
-      <c r="D91" s="56" t="s">
+      <c r="D91" s="60" t="s">
         <v>366</v>
       </c>
-      <c r="E91" s="55"/>
-      <c r="F91" s="55" t="s">
+      <c r="E91" s="59"/>
+      <c r="F91" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G91" s="38" t="s">
@@ -12055,9 +12114,9 @@
       <c r="C92" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="D92" s="56"/>
-      <c r="E92" s="55"/>
-      <c r="F92" s="55"/>
+      <c r="D92" s="60"/>
+      <c r="E92" s="59"/>
+      <c r="F92" s="59"/>
       <c r="G92" s="38" t="s">
         <v>33</v>
       </c>
@@ -12066,9 +12125,9 @@
       <c r="C93" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="D93" s="56"/>
-      <c r="E93" s="55"/>
-      <c r="F93" s="55"/>
+      <c r="D93" s="60"/>
+      <c r="E93" s="59"/>
+      <c r="F93" s="59"/>
       <c r="G93" s="38" t="s">
         <v>33</v>
       </c>
@@ -12077,11 +12136,11 @@
       <c r="C94" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="D94" s="56" t="s">
+      <c r="D94" s="60" t="s">
         <v>371</v>
       </c>
-      <c r="E94" s="55"/>
-      <c r="F94" s="55" t="s">
+      <c r="E94" s="59"/>
+      <c r="F94" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G94" s="38" t="s">
@@ -12092,9 +12151,9 @@
       <c r="C95" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="D95" s="56"/>
-      <c r="E95" s="55"/>
-      <c r="F95" s="55"/>
+      <c r="D95" s="60"/>
+      <c r="E95" s="59"/>
+      <c r="F95" s="59"/>
       <c r="G95" s="38" t="s">
         <v>33</v>
       </c>
@@ -12103,9 +12162,9 @@
       <c r="C96" s="34" t="s">
         <v>384</v>
       </c>
-      <c r="D96" s="56"/>
-      <c r="E96" s="55"/>
-      <c r="F96" s="55"/>
+      <c r="D96" s="60"/>
+      <c r="E96" s="59"/>
+      <c r="F96" s="59"/>
       <c r="G96" s="38" t="s">
         <v>33</v>
       </c>
@@ -12115,11 +12174,11 @@
       <c r="C97" s="36" t="s">
         <v>373</v>
       </c>
-      <c r="D97" s="56" t="s">
+      <c r="D97" s="60" t="s">
         <v>374</v>
       </c>
-      <c r="E97" s="55"/>
-      <c r="F97" s="55" t="s">
+      <c r="E97" s="59"/>
+      <c r="F97" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G97" s="38" t="s">
@@ -12131,9 +12190,9 @@
       <c r="C98" s="36" t="s">
         <v>380</v>
       </c>
-      <c r="D98" s="56"/>
-      <c r="E98" s="55"/>
-      <c r="F98" s="55"/>
+      <c r="D98" s="60"/>
+      <c r="E98" s="59"/>
+      <c r="F98" s="59"/>
       <c r="G98" s="38" t="s">
         <v>33</v>
       </c>
@@ -12143,9 +12202,9 @@
       <c r="C99" s="36" t="s">
         <v>386</v>
       </c>
-      <c r="D99" s="56"/>
-      <c r="E99" s="55"/>
-      <c r="F99" s="55"/>
+      <c r="D99" s="60"/>
+      <c r="E99" s="59"/>
+      <c r="F99" s="59"/>
       <c r="G99" s="38" t="s">
         <v>33</v>
       </c>
@@ -12158,11 +12217,11 @@
       <c r="C100" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="D100" s="56" t="s">
+      <c r="D100" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="E100" s="55"/>
-      <c r="F100" s="55" t="s">
+      <c r="E100" s="59"/>
+      <c r="F100" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G100" s="38" t="s">
@@ -12174,9 +12233,9 @@
       <c r="C101" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="D101" s="56"/>
-      <c r="E101" s="55"/>
-      <c r="F101" s="55"/>
+      <c r="D101" s="60"/>
+      <c r="E101" s="59"/>
+      <c r="F101" s="59"/>
       <c r="G101" s="38" t="s">
         <v>33</v>
       </c>
@@ -12185,11 +12244,11 @@
       <c r="C102" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="D102" s="56" t="s">
+      <c r="D102" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="E102" s="55"/>
-      <c r="F102" s="55" t="s">
+      <c r="E102" s="59"/>
+      <c r="F102" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G102" s="38" t="s">
@@ -12200,9 +12259,9 @@
       <c r="C103" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="D103" s="56"/>
-      <c r="E103" s="55"/>
-      <c r="F103" s="55"/>
+      <c r="D103" s="60"/>
+      <c r="E103" s="59"/>
+      <c r="F103" s="59"/>
       <c r="G103" s="38" t="s">
         <v>33</v>
       </c>
@@ -12211,9 +12270,9 @@
       <c r="C104" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="D104" s="56"/>
-      <c r="E104" s="55"/>
-      <c r="F104" s="55"/>
+      <c r="D104" s="60"/>
+      <c r="E104" s="59"/>
+      <c r="F104" s="59"/>
       <c r="G104" s="38" t="s">
         <v>33</v>
       </c>
@@ -12222,11 +12281,11 @@
       <c r="C105" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="D105" s="56" t="s">
+      <c r="D105" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="E105" s="55"/>
-      <c r="F105" s="55" t="s">
+      <c r="E105" s="59"/>
+      <c r="F105" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G105" s="38" t="s">
@@ -12237,9 +12296,9 @@
       <c r="C106" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="D106" s="56"/>
-      <c r="E106" s="55"/>
-      <c r="F106" s="55"/>
+      <c r="D106" s="60"/>
+      <c r="E106" s="59"/>
+      <c r="F106" s="59"/>
       <c r="G106" s="38" t="s">
         <v>33</v>
       </c>
@@ -12248,11 +12307,11 @@
       <c r="C107" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="D107" s="56" t="s">
+      <c r="D107" s="60" t="s">
         <v>124</v>
       </c>
-      <c r="E107" s="55"/>
-      <c r="F107" s="55" t="s">
+      <c r="E107" s="59"/>
+      <c r="F107" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G107" s="38" t="s">
@@ -12263,9 +12322,9 @@
       <c r="C108" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="D108" s="56"/>
-      <c r="E108" s="55"/>
-      <c r="F108" s="55"/>
+      <c r="D108" s="60"/>
+      <c r="E108" s="59"/>
+      <c r="F108" s="59"/>
       <c r="G108" s="38" t="s">
         <v>33</v>
       </c>
@@ -12274,9 +12333,9 @@
       <c r="C109" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="D109" s="56"/>
-      <c r="E109" s="55"/>
-      <c r="F109" s="55"/>
+      <c r="D109" s="60"/>
+      <c r="E109" s="59"/>
+      <c r="F109" s="59"/>
       <c r="G109" s="38" t="s">
         <v>33</v>
       </c>
@@ -12285,11 +12344,11 @@
       <c r="C110" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="D110" s="56" t="s">
+      <c r="D110" s="60" t="s">
         <v>131</v>
       </c>
-      <c r="E110" s="55"/>
-      <c r="F110" s="55" t="s">
+      <c r="E110" s="59"/>
+      <c r="F110" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G110" s="38" t="s">
@@ -12300,9 +12359,9 @@
       <c r="C111" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="D111" s="56"/>
-      <c r="E111" s="55"/>
-      <c r="F111" s="55"/>
+      <c r="D111" s="60"/>
+      <c r="E111" s="59"/>
+      <c r="F111" s="59"/>
       <c r="G111" s="38" t="s">
         <v>33</v>
       </c>
@@ -12311,292 +12370,334 @@
       <c r="C112" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="D112" s="56"/>
-      <c r="E112" s="55"/>
-      <c r="F112" s="55"/>
+      <c r="D112" s="60"/>
+      <c r="E112" s="59"/>
+      <c r="F112" s="59"/>
       <c r="G112" s="38" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="113" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C113" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="D113" s="56" t="s">
+      <c r="D113" s="60" t="s">
         <v>159</v>
       </c>
-      <c r="E113" s="55"/>
-      <c r="F113" s="55" t="s">
+      <c r="E113" s="59"/>
+      <c r="F113" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G113" s="38" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="114" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C114" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="D114" s="56"/>
-      <c r="E114" s="55"/>
-      <c r="F114" s="55"/>
+      <c r="D114" s="60"/>
+      <c r="E114" s="59"/>
+      <c r="F114" s="59"/>
       <c r="G114" s="38" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="115" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C115" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="D115" s="56" t="s">
+      <c r="D115" s="60" t="s">
         <v>164</v>
       </c>
-      <c r="E115" s="55"/>
-      <c r="F115" s="55" t="s">
+      <c r="E115" s="59"/>
+      <c r="F115" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G115" s="38" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="116" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C116" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="D116" s="56"/>
-      <c r="E116" s="55"/>
-      <c r="F116" s="55"/>
+      <c r="D116" s="60"/>
+      <c r="E116" s="59"/>
+      <c r="F116" s="59"/>
       <c r="G116" s="38" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="117" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C117" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="D117" s="56"/>
-      <c r="E117" s="55"/>
-      <c r="F117" s="55"/>
+      <c r="D117" s="60"/>
+      <c r="E117" s="59"/>
+      <c r="F117" s="59"/>
       <c r="G117" s="38" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="118" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C118" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="D118" s="56" t="s">
+      <c r="D118" s="60" t="s">
         <v>179</v>
       </c>
-      <c r="E118" s="55"/>
-      <c r="F118" s="55" t="s">
+      <c r="E118" s="59"/>
+      <c r="F118" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G118" s="38" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="119" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C119" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="D119" s="56"/>
-      <c r="E119" s="55"/>
-      <c r="F119" s="55"/>
+      <c r="D119" s="60"/>
+      <c r="E119" s="59"/>
+      <c r="F119" s="59"/>
       <c r="G119" s="38" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="120" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C120" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="D120" s="56"/>
-      <c r="E120" s="55"/>
-      <c r="F120" s="55"/>
+      <c r="D120" s="60"/>
+      <c r="E120" s="59"/>
+      <c r="F120" s="59"/>
       <c r="G120" s="38" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="121" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C121" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="D121" s="56" t="s">
+      <c r="D121" s="60" t="s">
         <v>186</v>
       </c>
-      <c r="E121" s="55"/>
-      <c r="F121" s="55" t="s">
+      <c r="E121" s="59"/>
+      <c r="F121" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G121" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="122" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K121" s="34" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="122" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C122" s="34" t="s">
         <v>188</v>
       </c>
-      <c r="D122" s="56"/>
-      <c r="E122" s="55"/>
-      <c r="F122" s="55"/>
+      <c r="D122" s="60"/>
+      <c r="E122" s="59"/>
+      <c r="F122" s="59"/>
       <c r="G122" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="123" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K122" s="34" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="123" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C123" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="D123" s="56" t="s">
+      <c r="D123" s="60" t="s">
         <v>195</v>
       </c>
-      <c r="E123" s="55"/>
-      <c r="F123" s="55" t="s">
+      <c r="E123" s="59"/>
+      <c r="F123" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G123" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="124" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K123" s="34" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="124" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C124" s="34" t="s">
         <v>197</v>
       </c>
-      <c r="D124" s="56"/>
-      <c r="E124" s="55"/>
-      <c r="F124" s="55"/>
+      <c r="D124" s="60"/>
+      <c r="E124" s="59"/>
+      <c r="F124" s="59"/>
       <c r="G124" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="125" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K124" s="34" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="125" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C125" s="34" t="s">
         <v>199</v>
       </c>
-      <c r="D125" s="56" t="s">
+      <c r="D125" s="60" t="s">
         <v>200</v>
       </c>
-      <c r="E125" s="55"/>
-      <c r="F125" s="55" t="s">
+      <c r="E125" s="59"/>
+      <c r="F125" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G125" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="126" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K125" s="34" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="126" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C126" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="D126" s="56"/>
-      <c r="E126" s="55"/>
-      <c r="F126" s="55"/>
+      <c r="D126" s="60"/>
+      <c r="E126" s="59"/>
+      <c r="F126" s="59"/>
       <c r="G126" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="127" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K126" s="34" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="127" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C127" s="34" t="s">
         <v>210</v>
       </c>
-      <c r="D127" s="56" t="s">
+      <c r="D127" s="60" t="s">
         <v>211</v>
       </c>
-      <c r="E127" s="55"/>
-      <c r="F127" s="55" t="s">
+      <c r="E127" s="59"/>
+      <c r="F127" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G127" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="128" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K127" s="34" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="128" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C128" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="D128" s="56"/>
-      <c r="E128" s="55"/>
-      <c r="F128" s="55"/>
+      <c r="D128" s="60"/>
+      <c r="E128" s="59"/>
+      <c r="F128" s="59"/>
       <c r="G128" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="129" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K128" s="34" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="129" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C129" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="D129" s="56"/>
-      <c r="E129" s="55"/>
-      <c r="F129" s="55"/>
+      <c r="D129" s="60"/>
+      <c r="E129" s="59"/>
+      <c r="F129" s="59"/>
       <c r="G129" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="130" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K129" s="34" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="130" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C130" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="D130" s="56" t="s">
+      <c r="D130" s="60" t="s">
         <v>223</v>
       </c>
-      <c r="E130" s="55"/>
-      <c r="F130" s="55" t="s">
+      <c r="E130" s="59"/>
+      <c r="F130" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G130" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="131" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K130" s="34" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="131" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C131" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="D131" s="56"/>
-      <c r="E131" s="55"/>
-      <c r="F131" s="55"/>
+      <c r="D131" s="60"/>
+      <c r="E131" s="59"/>
+      <c r="F131" s="59"/>
       <c r="G131" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="132" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K131" s="34" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="132" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C132" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="D132" s="56" t="s">
+      <c r="D132" s="60" t="s">
         <v>228</v>
       </c>
-      <c r="E132" s="55"/>
-      <c r="F132" s="55" t="s">
+      <c r="E132" s="59"/>
+      <c r="F132" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G132" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="133" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K132" s="34" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="133" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C133" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="D133" s="56"/>
-      <c r="E133" s="55"/>
-      <c r="F133" s="55"/>
+      <c r="D133" s="60"/>
+      <c r="E133" s="59"/>
+      <c r="F133" s="59"/>
       <c r="G133" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="134" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K133" s="34" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="134" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C134" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="D134" s="56"/>
-      <c r="E134" s="55"/>
-      <c r="F134" s="55"/>
+      <c r="D134" s="60"/>
+      <c r="E134" s="59"/>
+      <c r="F134" s="59"/>
       <c r="G134" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="135" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K134" s="34" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="135" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C135" s="34" t="s">
         <v>267</v>
       </c>
@@ -12610,8 +12711,11 @@
       <c r="G135" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="136" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K135" s="34" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="136" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C136" s="34" t="s">
         <v>271</v>
       </c>
@@ -12625,8 +12729,11 @@
       <c r="G136" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="137" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K136" s="34" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="137" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C137" s="34" t="s">
         <v>275</v>
       </c>
@@ -12641,7 +12748,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="138" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C138" s="34" t="s">
         <v>279</v>
       </c>
@@ -12656,59 +12763,59 @@
         <v>33</v>
       </c>
     </row>
-    <row r="139" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C139" s="34" t="s">
         <v>454</v>
       </c>
-      <c r="D139" s="56" t="s">
+      <c r="D139" s="60" t="s">
         <v>582</v>
       </c>
-      <c r="E139" s="55"/>
-      <c r="F139" s="55" t="s">
+      <c r="E139" s="59"/>
+      <c r="F139" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G139" s="38" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="140" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C140" s="34" t="s">
         <v>457</v>
       </c>
-      <c r="D140" s="56"/>
-      <c r="E140" s="55"/>
-      <c r="F140" s="55"/>
+      <c r="D140" s="60"/>
+      <c r="E140" s="59"/>
+      <c r="F140" s="59"/>
       <c r="G140" s="38" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="141" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C141" s="34" t="s">
         <v>459</v>
       </c>
-      <c r="D141" s="56" t="s">
+      <c r="D141" s="60" t="s">
         <v>460</v>
       </c>
-      <c r="E141" s="55"/>
-      <c r="F141" s="55" t="s">
+      <c r="E141" s="59"/>
+      <c r="F141" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G141" s="38" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="142" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C142" s="34" t="s">
         <v>462</v>
       </c>
-      <c r="D142" s="56"/>
-      <c r="E142" s="55"/>
-      <c r="F142" s="55"/>
+      <c r="D142" s="60"/>
+      <c r="E142" s="59"/>
+      <c r="F142" s="59"/>
       <c r="G142" s="38" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="143" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C143" s="34" t="s">
         <v>402</v>
       </c>
@@ -12723,7 +12830,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="144" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C144" s="34" t="s">
         <v>417</v>
       </c>
@@ -12759,11 +12866,11 @@
       <c r="C146" s="34" t="s">
         <v>477</v>
       </c>
-      <c r="D146" s="56" t="s">
+      <c r="D146" s="60" t="s">
         <v>478</v>
       </c>
-      <c r="E146" s="55"/>
-      <c r="F146" s="55" t="s">
+      <c r="E146" s="59"/>
+      <c r="F146" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G146" s="38" t="s">
@@ -12777,9 +12884,9 @@
       <c r="C147" s="35" t="s">
         <v>480</v>
       </c>
-      <c r="D147" s="59"/>
-      <c r="E147" s="63"/>
-      <c r="F147" s="63"/>
+      <c r="D147" s="62"/>
+      <c r="E147" s="64"/>
+      <c r="F147" s="64"/>
       <c r="G147" s="39" t="s">
         <v>33</v>
       </c>
@@ -12802,7 +12909,7 @@
       <c r="D149" s="36"/>
       <c r="E149" s="43">
         <f>COUNTBLANK(E2:E147)</f>
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F149" s="46"/>
       <c r="G149" s="36"/>
@@ -12815,7 +12922,7 @@
       <c r="D150" s="36"/>
       <c r="E150" s="43">
         <f>COUNTA(E2:E147)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F150" s="46"/>
       <c r="G150" s="36"/>
@@ -12843,6 +12950,183 @@
     </row>
   </sheetData>
   <mergeCells count="201">
+    <mergeCell ref="D91:D93"/>
+    <mergeCell ref="E91:E93"/>
+    <mergeCell ref="F91:F93"/>
+    <mergeCell ref="D94:D96"/>
+    <mergeCell ref="E94:E96"/>
+    <mergeCell ref="F94:F96"/>
+    <mergeCell ref="E51:E53"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="D71:D74"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="D83:D84"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="F51:F53"/>
+    <mergeCell ref="E89:E90"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="E83:E84"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="E87:E88"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="F77:F78"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="F81:F82"/>
+    <mergeCell ref="F83:F84"/>
+    <mergeCell ref="F85:F86"/>
+    <mergeCell ref="F87:F88"/>
+    <mergeCell ref="F89:F90"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="F67:F68"/>
+    <mergeCell ref="E71:E74"/>
+    <mergeCell ref="F71:F74"/>
+    <mergeCell ref="E64:E66"/>
+    <mergeCell ref="D87:D88"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="D43:D45"/>
+    <mergeCell ref="D46:D48"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D64:D66"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="F64:F66"/>
+    <mergeCell ref="D89:D90"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="F22:F25"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="E43:E45"/>
+    <mergeCell ref="F43:F45"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="G43:G45"/>
+    <mergeCell ref="G46:G48"/>
+    <mergeCell ref="D105:D106"/>
+    <mergeCell ref="E105:E106"/>
+    <mergeCell ref="F105:F106"/>
+    <mergeCell ref="D107:D109"/>
+    <mergeCell ref="E107:E109"/>
+    <mergeCell ref="F107:F109"/>
+    <mergeCell ref="D100:D101"/>
+    <mergeCell ref="E100:E101"/>
+    <mergeCell ref="F100:F101"/>
+    <mergeCell ref="D102:D104"/>
+    <mergeCell ref="E102:E104"/>
+    <mergeCell ref="F102:F104"/>
+    <mergeCell ref="D115:D117"/>
+    <mergeCell ref="E115:E117"/>
+    <mergeCell ref="F115:F117"/>
+    <mergeCell ref="D118:D120"/>
+    <mergeCell ref="E118:E120"/>
+    <mergeCell ref="F118:F120"/>
+    <mergeCell ref="D110:D112"/>
+    <mergeCell ref="E110:E112"/>
+    <mergeCell ref="F110:F112"/>
+    <mergeCell ref="D113:D114"/>
+    <mergeCell ref="E113:E114"/>
+    <mergeCell ref="F113:F114"/>
+    <mergeCell ref="D125:D126"/>
+    <mergeCell ref="E125:E126"/>
+    <mergeCell ref="F125:F126"/>
+    <mergeCell ref="D127:D129"/>
+    <mergeCell ref="E127:E129"/>
+    <mergeCell ref="F127:F129"/>
+    <mergeCell ref="D121:D122"/>
+    <mergeCell ref="E121:E122"/>
+    <mergeCell ref="F121:F122"/>
+    <mergeCell ref="D123:D124"/>
+    <mergeCell ref="E123:E124"/>
+    <mergeCell ref="F123:F124"/>
+    <mergeCell ref="D146:D147"/>
+    <mergeCell ref="E146:E147"/>
+    <mergeCell ref="F146:F147"/>
+    <mergeCell ref="D130:D131"/>
+    <mergeCell ref="E130:E131"/>
+    <mergeCell ref="F130:F131"/>
+    <mergeCell ref="D132:D134"/>
+    <mergeCell ref="E132:E134"/>
+    <mergeCell ref="F132:F134"/>
+    <mergeCell ref="D139:D140"/>
+    <mergeCell ref="D141:D142"/>
+    <mergeCell ref="F139:F140"/>
+    <mergeCell ref="F141:F142"/>
+    <mergeCell ref="E139:E140"/>
+    <mergeCell ref="E141:E142"/>
     <mergeCell ref="O5:O6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
@@ -12867,183 +13151,6 @@
     <mergeCell ref="D36:D37"/>
     <mergeCell ref="E36:E37"/>
     <mergeCell ref="F36:F37"/>
-    <mergeCell ref="D146:D147"/>
-    <mergeCell ref="E146:E147"/>
-    <mergeCell ref="F146:F147"/>
-    <mergeCell ref="D130:D131"/>
-    <mergeCell ref="E130:E131"/>
-    <mergeCell ref="F130:F131"/>
-    <mergeCell ref="D132:D134"/>
-    <mergeCell ref="E132:E134"/>
-    <mergeCell ref="F132:F134"/>
-    <mergeCell ref="D139:D140"/>
-    <mergeCell ref="D141:D142"/>
-    <mergeCell ref="F139:F140"/>
-    <mergeCell ref="F141:F142"/>
-    <mergeCell ref="E139:E140"/>
-    <mergeCell ref="E141:E142"/>
-    <mergeCell ref="D125:D126"/>
-    <mergeCell ref="E125:E126"/>
-    <mergeCell ref="F125:F126"/>
-    <mergeCell ref="D127:D129"/>
-    <mergeCell ref="E127:E129"/>
-    <mergeCell ref="F127:F129"/>
-    <mergeCell ref="D121:D122"/>
-    <mergeCell ref="E121:E122"/>
-    <mergeCell ref="F121:F122"/>
-    <mergeCell ref="D123:D124"/>
-    <mergeCell ref="E123:E124"/>
-    <mergeCell ref="F123:F124"/>
-    <mergeCell ref="D115:D117"/>
-    <mergeCell ref="E115:E117"/>
-    <mergeCell ref="F115:F117"/>
-    <mergeCell ref="D118:D120"/>
-    <mergeCell ref="E118:E120"/>
-    <mergeCell ref="F118:F120"/>
-    <mergeCell ref="D110:D112"/>
-    <mergeCell ref="E110:E112"/>
-    <mergeCell ref="F110:F112"/>
-    <mergeCell ref="D113:D114"/>
-    <mergeCell ref="E113:E114"/>
-    <mergeCell ref="F113:F114"/>
-    <mergeCell ref="D105:D106"/>
-    <mergeCell ref="E105:E106"/>
-    <mergeCell ref="F105:F106"/>
-    <mergeCell ref="D107:D109"/>
-    <mergeCell ref="E107:E109"/>
-    <mergeCell ref="F107:F109"/>
-    <mergeCell ref="D100:D101"/>
-    <mergeCell ref="E100:E101"/>
-    <mergeCell ref="F100:F101"/>
-    <mergeCell ref="D102:D104"/>
-    <mergeCell ref="E102:E104"/>
-    <mergeCell ref="F102:F104"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="G40:G42"/>
-    <mergeCell ref="E43:E45"/>
-    <mergeCell ref="F43:F45"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="G43:G45"/>
-    <mergeCell ref="G46:G48"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="D89:D90"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="F22:F25"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="F67:F68"/>
-    <mergeCell ref="E71:E74"/>
-    <mergeCell ref="F71:F74"/>
-    <mergeCell ref="E64:E66"/>
-    <mergeCell ref="D87:D88"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="D43:D45"/>
-    <mergeCell ref="D46:D48"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="D64:D66"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E89:E90"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="E81:E82"/>
-    <mergeCell ref="E83:E84"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="E87:E88"/>
-    <mergeCell ref="F75:F76"/>
-    <mergeCell ref="F77:F78"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="F81:F82"/>
-    <mergeCell ref="F83:F84"/>
-    <mergeCell ref="F85:F86"/>
-    <mergeCell ref="F87:F88"/>
-    <mergeCell ref="F89:F90"/>
-    <mergeCell ref="F64:F66"/>
-    <mergeCell ref="D91:D93"/>
-    <mergeCell ref="E91:E93"/>
-    <mergeCell ref="F91:F93"/>
-    <mergeCell ref="D94:D96"/>
-    <mergeCell ref="E94:E96"/>
-    <mergeCell ref="F94:F96"/>
-    <mergeCell ref="E51:E53"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="F56:F57"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="D71:D74"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="D83:D84"/>
-    <mergeCell ref="D85:D86"/>
-    <mergeCell ref="F51:F53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -13054,7 +13161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA06BA7C-CD17-4C21-9F28-C604AE25C8B9}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -13068,23 +13175,23 @@
     <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="70" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:6" s="56" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="55" t="s">
         <v>589</v>
       </c>
-      <c r="F1" s="70" t="s">
+      <c r="F1" s="56" t="s">
         <v>539</v>
       </c>
     </row>
@@ -13101,7 +13208,7 @@
       <c r="D2" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="68">
+      <c r="E2" s="70">
         <v>101332</v>
       </c>
     </row>
@@ -13118,7 +13225,7 @@
       <c r="D3" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="68"/>
+      <c r="E3" s="70"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -13133,7 +13240,7 @@
       <c r="D4" t="s">
         <v>524</v>
       </c>
-      <c r="E4" s="68">
+      <c r="E4" s="70">
         <v>99343</v>
       </c>
     </row>
@@ -13150,7 +13257,7 @@
       <c r="D5" t="s">
         <v>524</v>
       </c>
-      <c r="E5" s="68"/>
+      <c r="E5" s="70"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -13165,7 +13272,7 @@
       <c r="D6" t="s">
         <v>516</v>
       </c>
-      <c r="E6" s="68">
+      <c r="E6" s="70">
         <v>102453</v>
       </c>
     </row>
@@ -13182,7 +13289,7 @@
       <c r="D7" t="s">
         <v>516</v>
       </c>
-      <c r="E7" s="68"/>
+      <c r="E7" s="70"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -13197,7 +13304,7 @@
       <c r="D8" t="s">
         <v>521</v>
       </c>
-      <c r="E8" s="68">
+      <c r="E8" s="70">
         <v>102447</v>
       </c>
     </row>
@@ -13214,7 +13321,7 @@
       <c r="D9" t="s">
         <v>521</v>
       </c>
-      <c r="E9" s="68"/>
+      <c r="E9" s="70"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -13229,7 +13336,7 @@
       <c r="D10" t="s">
         <v>521</v>
       </c>
-      <c r="E10" s="68"/>
+      <c r="E10" s="70"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -13244,7 +13351,7 @@
       <c r="D11" t="s">
         <v>521</v>
       </c>
-      <c r="E11" s="68"/>
+      <c r="E11" s="70"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -13259,7 +13366,7 @@
       <c r="D12" t="s">
         <v>512</v>
       </c>
-      <c r="E12" s="68">
+      <c r="E12" s="70">
         <v>101221</v>
       </c>
     </row>
@@ -13276,7 +13383,7 @@
       <c r="D13" t="s">
         <v>512</v>
       </c>
-      <c r="E13" s="68"/>
+      <c r="E13" s="70"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -13291,7 +13398,7 @@
       <c r="D14" t="s">
         <v>517</v>
       </c>
-      <c r="E14" s="68">
+      <c r="E14" s="70">
         <v>102455</v>
       </c>
     </row>
@@ -13308,7 +13415,7 @@
       <c r="D15" t="s">
         <v>517</v>
       </c>
-      <c r="E15" s="68"/>
+      <c r="E15" s="70"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -13323,7 +13430,7 @@
       <c r="D16" t="s">
         <v>508</v>
       </c>
-      <c r="E16" s="68">
+      <c r="E16" s="70">
         <v>1013824</v>
       </c>
     </row>
@@ -13340,7 +13447,7 @@
       <c r="D17" t="s">
         <v>508</v>
       </c>
-      <c r="E17" s="68"/>
+      <c r="E17" s="70"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -13355,7 +13462,7 @@
       <c r="D18" t="s">
         <v>510</v>
       </c>
-      <c r="E18" s="68">
+      <c r="E18" s="70">
         <v>102445</v>
       </c>
     </row>
@@ -13372,7 +13479,7 @@
       <c r="D19" t="s">
         <v>510</v>
       </c>
-      <c r="E19" s="68"/>
+      <c r="E19" s="70"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -13387,7 +13494,7 @@
       <c r="D20" t="s">
         <v>511</v>
       </c>
-      <c r="E20" s="68">
+      <c r="E20" s="70">
         <v>101557</v>
       </c>
     </row>
@@ -13404,7 +13511,7 @@
       <c r="D21" t="s">
         <v>511</v>
       </c>
-      <c r="E21" s="68"/>
+      <c r="E21" s="70"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -13419,7 +13526,7 @@
       <c r="D22" t="s">
         <v>509</v>
       </c>
-      <c r="E22" s="68">
+      <c r="E22" s="70">
         <v>101339</v>
       </c>
     </row>
@@ -13436,7 +13543,7 @@
       <c r="D23" t="s">
         <v>509</v>
       </c>
-      <c r="E23" s="68"/>
+      <c r="E23" s="70"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -13451,7 +13558,7 @@
       <c r="D24" t="s">
         <v>520</v>
       </c>
-      <c r="E24" s="68">
+      <c r="E24" s="70">
         <v>102391</v>
       </c>
     </row>
@@ -13468,21 +13575,21 @@
       <c r="D25" t="s">
         <v>520</v>
       </c>
-      <c r="E25" s="68"/>
+      <c r="E25" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E22:E23"/>
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="E8:E11"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="E22:E23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -14425,26 +14532,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEAE28352B96D64C95AA0D5E2FA62FAD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed183881d36ac1b5d7d67982eda510d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d161086-4829-409f-9f75-5bde88dcb151" xmlns:ns3="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="685f4fda20cf913d28bf77c13cd653dd" ns2:_="" ns3:_="">
     <xsd:import namespace="3d161086-4829-409f-9f75-5bde88dcb151"/>
@@ -14667,32 +14754,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C74AB5E7-5C87-4FF7-BF80-AB0EB6BD1D32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14709,4 +14791,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Scripts execute_dd_to_dms and execute_dmm_to_dd added
</commit_message>
<xml_diff>
--- a/analysis/MEDS_Tables.xlsx
+++ b/analysis/MEDS_Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="571" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D4AA51C-799E-4C6C-BACE-7A659EE3CD3C}"/>
+  <xr:revisionPtr revIDLastSave="577" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A864FF4-3463-48DB-A6CE-A3B148BE268A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2728" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2734" uniqueCount="590">
   <si>
     <t>Table</t>
   </si>
@@ -2657,16 +2657,14 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2675,31 +2673,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -10733,8 +10733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8FA477-9B46-4053-B7AD-310B8B9F2B30}">
   <dimension ref="A1:P152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22:E25"/>
+    <sheetView tabSelected="1" topLeftCell="C13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10769,7 +10769,7 @@
       <c r="H1" s="48"/>
       <c r="I1" s="41">
         <f>E150/E149</f>
-        <v>8.1481481481481488E-2</v>
+        <v>0.13178294573643412</v>
       </c>
       <c r="J1" s="49" t="s">
         <v>566</v>
@@ -10777,17 +10777,17 @@
       <c r="K1" s="48"/>
     </row>
     <row r="2" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
+      <c r="B2" s="57"/>
       <c r="C2" s="33" t="s">
         <v>36</v>
       </c>
       <c r="D2" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="63" t="s">
+      <c r="E2" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="63" t="s">
+      <c r="F2" s="64" t="s">
         <v>42</v>
       </c>
       <c r="G2" s="65" t="s">
@@ -10795,14 +10795,14 @@
       </c>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="71"/>
+      <c r="B3" s="57"/>
       <c r="C3" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="60"/>
+      <c r="D3" s="58"/>
       <c r="E3" s="59"/>
       <c r="F3" s="59"/>
-      <c r="G3" s="67"/>
+      <c r="G3" s="63"/>
       <c r="K3" s="36"/>
       <c r="L3" s="36"/>
       <c r="M3" s="36"/>
@@ -10811,14 +10811,14 @@
       <c r="P3" s="36"/>
     </row>
     <row r="4" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="71"/>
+      <c r="B4" s="57"/>
       <c r="C4" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="60"/>
+      <c r="D4" s="58"/>
       <c r="E4" s="59"/>
       <c r="F4" s="59"/>
-      <c r="G4" s="67"/>
+      <c r="G4" s="63"/>
       <c r="K4" s="36"/>
       <c r="L4" s="36"/>
       <c r="M4" s="36"/>
@@ -10827,11 +10827,11 @@
       <c r="P4" s="36"/>
     </row>
     <row r="5" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="71"/>
+      <c r="B5" s="57"/>
       <c r="C5" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="60" t="s">
+      <c r="D5" s="58" t="s">
         <v>53</v>
       </c>
       <c r="E5" s="59" t="s">
@@ -10840,46 +10840,46 @@
       <c r="F5" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="67" t="s">
+      <c r="G5" s="63" t="s">
         <v>519</v>
       </c>
       <c r="K5" s="36"/>
       <c r="L5" s="47" t="s">
         <v>464</v>
       </c>
-      <c r="M5" s="58" t="s">
+      <c r="M5" s="70" t="s">
         <v>465</v>
       </c>
       <c r="N5" s="59"/>
-      <c r="O5" s="57" t="s">
+      <c r="O5" s="69" t="s">
         <v>581</v>
       </c>
       <c r="P5" s="36"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="71"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="60"/>
+      <c r="D6" s="58"/>
       <c r="E6" s="59"/>
       <c r="F6" s="59"/>
-      <c r="G6" s="67"/>
+      <c r="G6" s="63"/>
       <c r="K6" s="36"/>
       <c r="L6" s="47" t="s">
         <v>467</v>
       </c>
-      <c r="M6" s="58"/>
+      <c r="M6" s="70"/>
       <c r="N6" s="59"/>
-      <c r="O6" s="57"/>
+      <c r="O6" s="69"/>
       <c r="P6" s="36"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="71"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="60" t="s">
+      <c r="D7" s="58" t="s">
         <v>78</v>
       </c>
       <c r="E7" s="59" t="s">
@@ -10888,7 +10888,7 @@
       <c r="F7" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="67" t="s">
+      <c r="G7" s="63" t="s">
         <v>80</v>
       </c>
       <c r="K7" s="36"/>
@@ -10899,14 +10899,14 @@
       <c r="P7" s="36"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="71"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="60"/>
+      <c r="D8" s="58"/>
       <c r="E8" s="59"/>
       <c r="F8" s="59"/>
-      <c r="G8" s="67"/>
+      <c r="G8" s="63"/>
       <c r="K8" s="36"/>
       <c r="L8" s="36"/>
       <c r="M8" s="36"/>
@@ -10915,11 +10915,11 @@
       <c r="P8" s="36"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="71"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="D9" s="60" t="s">
+      <c r="D9" s="58" t="s">
         <v>171</v>
       </c>
       <c r="E9" s="59" t="s">
@@ -10928,42 +10928,42 @@
       <c r="F9" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="67" t="s">
+      <c r="G9" s="63" t="s">
         <v>523</v>
       </c>
       <c r="J9" s="36"/>
       <c r="K9" s="36"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="71"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="D10" s="60"/>
+      <c r="D10" s="58"/>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
-      <c r="G10" s="67"/>
+      <c r="G10" s="63"/>
       <c r="J10" s="36"/>
       <c r="K10" s="36"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="71"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="D11" s="60"/>
+      <c r="D11" s="58"/>
       <c r="E11" s="59"/>
       <c r="F11" s="59"/>
-      <c r="G11" s="67"/>
+      <c r="G11" s="63"/>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="71"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="58" t="s">
         <v>204</v>
       </c>
       <c r="E12" s="59" t="s">
@@ -10972,30 +10972,30 @@
       <c r="F12" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="67" t="s">
+      <c r="G12" s="63" t="s">
         <v>515</v>
       </c>
       <c r="J12" s="36"/>
       <c r="K12" s="36"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="71"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="D13" s="60"/>
+      <c r="D13" s="58"/>
       <c r="E13" s="59"/>
       <c r="F13" s="59"/>
-      <c r="G13" s="67"/>
+      <c r="G13" s="63"/>
       <c r="J13" s="36"/>
       <c r="K13" s="36"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="71"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="D14" s="60" t="s">
+      <c r="D14" s="58" t="s">
         <v>361</v>
       </c>
       <c r="E14" s="59" t="s">
@@ -11004,21 +11004,21 @@
       <c r="F14" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="67" t="s">
+      <c r="G14" s="63" t="s">
         <v>518</v>
       </c>
       <c r="J14" s="36"/>
       <c r="K14" s="36"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="71"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="35" t="s">
         <v>363</v>
       </c>
       <c r="D15" s="62"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="67"/>
       <c r="J15" s="36"/>
       <c r="K15" s="36"/>
     </row>
@@ -11029,10 +11029,10 @@
       <c r="D16" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="63" t="s">
+      <c r="E16" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F16" s="63" t="s">
+      <c r="F16" s="64" t="s">
         <v>567</v>
       </c>
       <c r="G16" s="65" t="s">
@@ -11045,10 +11045,10 @@
       <c r="C17" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="60"/>
+      <c r="D17" s="58"/>
       <c r="E17" s="59"/>
       <c r="F17" s="59"/>
-      <c r="G17" s="67"/>
+      <c r="G17" s="63"/>
       <c r="J17" s="36"/>
       <c r="K17" s="36"/>
     </row>
@@ -11056,14 +11056,14 @@
       <c r="C18" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="60" t="s">
+      <c r="D18" s="58" t="s">
         <v>105</v>
       </c>
       <c r="E18" s="59"/>
       <c r="F18" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G18" s="67" t="s">
+      <c r="G18" s="63" t="s">
         <v>524</v>
       </c>
       <c r="J18" s="36"/>
@@ -11073,10 +11073,10 @@
       <c r="C19" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="60"/>
+      <c r="D19" s="58"/>
       <c r="E19" s="59"/>
       <c r="F19" s="59"/>
-      <c r="G19" s="67"/>
+      <c r="G19" s="63"/>
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
     </row>
@@ -11084,7 +11084,7 @@
       <c r="C20" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="D20" s="60" t="s">
+      <c r="D20" s="58" t="s">
         <v>300</v>
       </c>
       <c r="E20" s="59" t="s">
@@ -11093,7 +11093,7 @@
       <c r="F20" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G20" s="67" t="s">
+      <c r="G20" s="63" t="s">
         <v>516</v>
       </c>
       <c r="J20" s="36"/>
@@ -11103,10 +11103,10 @@
       <c r="C21" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="D21" s="60"/>
+      <c r="D21" s="58"/>
       <c r="E21" s="59"/>
       <c r="F21" s="59"/>
-      <c r="G21" s="67"/>
+      <c r="G21" s="63"/>
       <c r="J21" s="36"/>
       <c r="K21" s="36"/>
     </row>
@@ -11114,14 +11114,14 @@
       <c r="C22" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="D22" s="60" t="s">
+      <c r="D22" s="58" t="s">
         <v>305</v>
       </c>
       <c r="E22" s="59"/>
       <c r="F22" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G22" s="67" t="s">
+      <c r="G22" s="63" t="s">
         <v>521</v>
       </c>
       <c r="J22" s="36"/>
@@ -11131,10 +11131,10 @@
       <c r="C23" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="D23" s="60"/>
+      <c r="D23" s="58"/>
       <c r="E23" s="59"/>
       <c r="F23" s="59"/>
-      <c r="G23" s="67"/>
+      <c r="G23" s="63"/>
       <c r="J23" s="36"/>
       <c r="K23" s="36"/>
     </row>
@@ -11142,10 +11142,10 @@
       <c r="C24" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="D24" s="60"/>
+      <c r="D24" s="58"/>
       <c r="E24" s="59"/>
       <c r="F24" s="59"/>
-      <c r="G24" s="67"/>
+      <c r="G24" s="63"/>
       <c r="J24" s="36"/>
       <c r="K24" s="36"/>
     </row>
@@ -11153,10 +11153,10 @@
       <c r="C25" s="34" t="s">
         <v>311</v>
       </c>
-      <c r="D25" s="60"/>
+      <c r="D25" s="58"/>
       <c r="E25" s="59"/>
       <c r="F25" s="59"/>
-      <c r="G25" s="67"/>
+      <c r="G25" s="63"/>
       <c r="J25" s="36"/>
       <c r="K25" s="36"/>
     </row>
@@ -11164,14 +11164,16 @@
       <c r="C26" s="34" t="s">
         <v>317</v>
       </c>
-      <c r="D26" s="60" t="s">
+      <c r="D26" s="58" t="s">
         <v>318</v>
       </c>
-      <c r="E26" s="59"/>
+      <c r="E26" s="59" t="s">
+        <v>81</v>
+      </c>
       <c r="F26" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G26" s="67" t="s">
+      <c r="G26" s="63" t="s">
         <v>512</v>
       </c>
       <c r="J26" s="36"/>
@@ -11181,10 +11183,10 @@
       <c r="C27" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="D27" s="60"/>
+      <c r="D27" s="58"/>
       <c r="E27" s="59"/>
       <c r="F27" s="59"/>
-      <c r="G27" s="67"/>
+      <c r="G27" s="63"/>
       <c r="J27" s="36"/>
       <c r="K27" s="36"/>
     </row>
@@ -11192,14 +11194,14 @@
       <c r="C28" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="D28" s="68" t="s">
+      <c r="D28" s="60" t="s">
         <v>323</v>
       </c>
-      <c r="E28" s="69"/>
+      <c r="E28" s="68"/>
       <c r="F28" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G28" s="67" t="s">
+      <c r="G28" s="63" t="s">
         <v>517</v>
       </c>
       <c r="J28" s="36"/>
@@ -11209,23 +11211,25 @@
       <c r="C29" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="D29" s="68"/>
-      <c r="E29" s="69"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="68"/>
       <c r="F29" s="59"/>
-      <c r="G29" s="67"/>
+      <c r="G29" s="63"/>
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C30" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="D30" s="60" t="s">
+      <c r="D30" s="58" t="s">
         <v>328</v>
       </c>
-      <c r="E30" s="59"/>
+      <c r="E30" s="59" t="s">
+        <v>81</v>
+      </c>
       <c r="F30" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G30" s="67" t="s">
+      <c r="G30" s="63" t="s">
         <v>508</v>
       </c>
     </row>
@@ -11233,23 +11237,25 @@
       <c r="C31" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="D31" s="60"/>
+      <c r="D31" s="58"/>
       <c r="E31" s="59"/>
       <c r="F31" s="59"/>
-      <c r="G31" s="67"/>
+      <c r="G31" s="63"/>
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="D32" s="60" t="s">
+      <c r="D32" s="58" t="s">
         <v>333</v>
       </c>
-      <c r="E32" s="59"/>
+      <c r="E32" s="59" t="s">
+        <v>81</v>
+      </c>
       <c r="F32" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G32" s="67" t="s">
+      <c r="G32" s="63" t="s">
         <v>510</v>
       </c>
     </row>
@@ -11257,23 +11263,25 @@
       <c r="C33" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="D33" s="60"/>
+      <c r="D33" s="58"/>
       <c r="E33" s="59"/>
       <c r="F33" s="59"/>
-      <c r="G33" s="67"/>
+      <c r="G33" s="63"/>
     </row>
     <row r="34" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C34" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="D34" s="60" t="s">
+      <c r="D34" s="58" t="s">
         <v>338</v>
       </c>
-      <c r="E34" s="59"/>
+      <c r="E34" s="59" t="s">
+        <v>81</v>
+      </c>
       <c r="F34" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G34" s="67" t="s">
+      <c r="G34" s="63" t="s">
         <v>511</v>
       </c>
     </row>
@@ -11281,23 +11289,25 @@
       <c r="C35" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="D35" s="60"/>
+      <c r="D35" s="58"/>
       <c r="E35" s="59"/>
       <c r="F35" s="59"/>
-      <c r="G35" s="67"/>
+      <c r="G35" s="63"/>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C36" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="D36" s="60" t="s">
+      <c r="D36" s="58" t="s">
         <v>343</v>
       </c>
-      <c r="E36" s="59"/>
+      <c r="E36" s="59" t="s">
+        <v>81</v>
+      </c>
       <c r="F36" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G36" s="67" t="s">
+      <c r="G36" s="63" t="s">
         <v>509</v>
       </c>
     </row>
@@ -11305,23 +11315,25 @@
       <c r="C37" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="D37" s="60"/>
+      <c r="D37" s="58"/>
       <c r="E37" s="59"/>
       <c r="F37" s="59"/>
-      <c r="G37" s="67"/>
+      <c r="G37" s="63"/>
     </row>
     <row r="38" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C38" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="D38" s="60" t="s">
+      <c r="D38" s="58" t="s">
         <v>348</v>
       </c>
-      <c r="E38" s="59"/>
+      <c r="E38" s="59" t="s">
+        <v>81</v>
+      </c>
       <c r="F38" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G38" s="67" t="s">
+      <c r="G38" s="63" t="s">
         <v>520</v>
       </c>
     </row>
@@ -11330,9 +11342,9 @@
         <v>350</v>
       </c>
       <c r="D39" s="62"/>
-      <c r="E39" s="64"/>
-      <c r="F39" s="64"/>
-      <c r="G39" s="66"/>
+      <c r="E39" s="66"/>
+      <c r="F39" s="66"/>
+      <c r="G39" s="67"/>
     </row>
     <row r="40" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C40" s="33" t="s">
@@ -11341,10 +11353,10 @@
       <c r="D40" s="61" t="s">
         <v>366</v>
       </c>
-      <c r="E40" s="63" t="s">
+      <c r="E40" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F40" s="63" t="s">
+      <c r="F40" s="64" t="s">
         <v>369</v>
       </c>
       <c r="G40" s="65" t="s">
@@ -11355,25 +11367,25 @@
       <c r="C41" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="D41" s="60"/>
+      <c r="D41" s="58"/>
       <c r="E41" s="59"/>
       <c r="F41" s="59"/>
-      <c r="G41" s="67"/>
+      <c r="G41" s="63"/>
     </row>
     <row r="42" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C42" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="D42" s="60"/>
+      <c r="D42" s="58"/>
       <c r="E42" s="59"/>
       <c r="F42" s="59"/>
-      <c r="G42" s="67"/>
+      <c r="G42" s="63"/>
     </row>
     <row r="43" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C43" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="D43" s="60" t="s">
+      <c r="D43" s="58" t="s">
         <v>371</v>
       </c>
       <c r="E43" s="59" t="s">
@@ -11382,7 +11394,7 @@
       <c r="F43" s="59" t="s">
         <v>369</v>
       </c>
-      <c r="G43" s="67" t="s">
+      <c r="G43" s="63" t="s">
         <v>513</v>
       </c>
     </row>
@@ -11390,25 +11402,25 @@
       <c r="C44" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="D44" s="60"/>
+      <c r="D44" s="58"/>
       <c r="E44" s="59"/>
       <c r="F44" s="59"/>
-      <c r="G44" s="67"/>
+      <c r="G44" s="63"/>
     </row>
     <row r="45" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C45" s="34" t="s">
         <v>384</v>
       </c>
-      <c r="D45" s="60"/>
+      <c r="D45" s="58"/>
       <c r="E45" s="59"/>
       <c r="F45" s="59"/>
-      <c r="G45" s="67"/>
+      <c r="G45" s="63"/>
     </row>
     <row r="46" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C46" s="34" t="s">
         <v>373</v>
       </c>
-      <c r="D46" s="60" t="s">
+      <c r="D46" s="58" t="s">
         <v>374</v>
       </c>
       <c r="E46" s="59" t="s">
@@ -11417,7 +11429,7 @@
       <c r="F46" s="59" t="s">
         <v>369</v>
       </c>
-      <c r="G46" s="67" t="s">
+      <c r="G46" s="63" t="s">
         <v>522</v>
       </c>
     </row>
@@ -11425,19 +11437,19 @@
       <c r="C47" s="34" t="s">
         <v>380</v>
       </c>
-      <c r="D47" s="60"/>
+      <c r="D47" s="58"/>
       <c r="E47" s="59"/>
       <c r="F47" s="59"/>
-      <c r="G47" s="67"/>
+      <c r="G47" s="63"/>
     </row>
     <row r="48" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C48" s="35" t="s">
         <v>386</v>
       </c>
       <c r="D48" s="62"/>
-      <c r="E48" s="64"/>
-      <c r="F48" s="64"/>
-      <c r="G48" s="66"/>
+      <c r="E48" s="66"/>
+      <c r="F48" s="66"/>
+      <c r="G48" s="67"/>
       <c r="J48" s="36"/>
       <c r="K48" s="36"/>
       <c r="L48" s="36"/>
@@ -11450,8 +11462,8 @@
       <c r="D49" s="61" t="s">
         <v>465</v>
       </c>
-      <c r="E49" s="63"/>
-      <c r="F49" s="63" t="s">
+      <c r="E49" s="64"/>
+      <c r="F49" s="64" t="s">
         <v>584</v>
       </c>
       <c r="G49" s="65" t="s">
@@ -11467,9 +11479,9 @@
         <v>467</v>
       </c>
       <c r="D50" s="62"/>
-      <c r="E50" s="64"/>
-      <c r="F50" s="64"/>
-      <c r="G50" s="66"/>
+      <c r="E50" s="66"/>
+      <c r="F50" s="66"/>
+      <c r="G50" s="67"/>
       <c r="J50" s="36"/>
       <c r="K50" s="36"/>
       <c r="L50" s="36"/>
@@ -11479,7 +11491,7 @@
       <c r="C51" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="D51" s="60" t="s">
+      <c r="D51" s="58" t="s">
         <v>38</v>
       </c>
       <c r="E51" s="59"/>
@@ -11498,7 +11510,7 @@
       <c r="C52" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D52" s="60"/>
+      <c r="D52" s="58"/>
       <c r="E52" s="59"/>
       <c r="F52" s="59"/>
       <c r="G52" s="38" t="s">
@@ -11513,7 +11525,7 @@
       <c r="C53" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D53" s="60"/>
+      <c r="D53" s="58"/>
       <c r="E53" s="59"/>
       <c r="F53" s="59"/>
       <c r="G53" s="38" t="s">
@@ -11528,7 +11540,7 @@
       <c r="C54" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="D54" s="60" t="s">
+      <c r="D54" s="58" t="s">
         <v>48</v>
       </c>
       <c r="E54" s="59"/>
@@ -11547,7 +11559,7 @@
       <c r="C55" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D55" s="60"/>
+      <c r="D55" s="58"/>
       <c r="E55" s="59"/>
       <c r="F55" s="59"/>
       <c r="G55" s="38" t="s">
@@ -11562,7 +11574,7 @@
       <c r="C56" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D56" s="60" t="s">
+      <c r="D56" s="58" t="s">
         <v>53</v>
       </c>
       <c r="E56" s="59"/>
@@ -11581,7 +11593,7 @@
       <c r="C57" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D57" s="60"/>
+      <c r="D57" s="58"/>
       <c r="E57" s="59"/>
       <c r="F57" s="59"/>
       <c r="G57" s="38" t="s">
@@ -11596,7 +11608,7 @@
       <c r="C58" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D58" s="60" t="s">
+      <c r="D58" s="58" t="s">
         <v>78</v>
       </c>
       <c r="E58" s="59"/>
@@ -11615,7 +11627,7 @@
       <c r="C59" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D59" s="60"/>
+      <c r="D59" s="58"/>
       <c r="E59" s="59"/>
       <c r="F59" s="59"/>
       <c r="G59" s="38" t="s">
@@ -11630,7 +11642,7 @@
       <c r="C60" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="D60" s="60" t="s">
+      <c r="D60" s="58" t="s">
         <v>71</v>
       </c>
       <c r="E60" s="59"/>
@@ -11649,7 +11661,7 @@
       <c r="C61" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D61" s="60"/>
+      <c r="D61" s="58"/>
       <c r="E61" s="59"/>
       <c r="F61" s="59"/>
       <c r="G61" s="38" t="s">
@@ -11664,7 +11676,7 @@
       <c r="C62" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D62" s="60" t="s">
+      <c r="D62" s="58" t="s">
         <v>105</v>
       </c>
       <c r="E62" s="59"/>
@@ -11683,7 +11695,7 @@
       <c r="C63" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D63" s="60"/>
+      <c r="D63" s="58"/>
       <c r="E63" s="59"/>
       <c r="F63" s="59"/>
       <c r="G63" s="38" t="s">
@@ -11698,7 +11710,7 @@
       <c r="C64" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="D64" s="60" t="s">
+      <c r="D64" s="58" t="s">
         <v>171</v>
       </c>
       <c r="E64" s="59"/>
@@ -11717,7 +11729,7 @@
       <c r="C65" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="D65" s="60"/>
+      <c r="D65" s="58"/>
       <c r="E65" s="59"/>
       <c r="F65" s="59"/>
       <c r="G65" s="38" t="s">
@@ -11732,7 +11744,7 @@
       <c r="C66" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="D66" s="60"/>
+      <c r="D66" s="58"/>
       <c r="E66" s="59"/>
       <c r="F66" s="59"/>
       <c r="G66" s="38" t="s">
@@ -11747,7 +11759,7 @@
       <c r="C67" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="D67" s="60" t="s">
+      <c r="D67" s="58" t="s">
         <v>204</v>
       </c>
       <c r="E67" s="59"/>
@@ -11766,7 +11778,7 @@
       <c r="C68" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="D68" s="60"/>
+      <c r="D68" s="58"/>
       <c r="E68" s="59"/>
       <c r="F68" s="59"/>
       <c r="G68" s="38" t="s">
@@ -11781,7 +11793,7 @@
       <c r="C69" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="D69" s="60" t="s">
+      <c r="D69" s="58" t="s">
         <v>300</v>
       </c>
       <c r="E69" s="59"/>
@@ -11800,7 +11812,7 @@
       <c r="C70" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="D70" s="60"/>
+      <c r="D70" s="58"/>
       <c r="E70" s="59"/>
       <c r="F70" s="59"/>
       <c r="G70" s="38" t="s">
@@ -11815,7 +11827,7 @@
       <c r="C71" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="D71" s="60" t="s">
+      <c r="D71" s="58" t="s">
         <v>305</v>
       </c>
       <c r="E71" s="59"/>
@@ -11834,7 +11846,7 @@
       <c r="C72" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="D72" s="60"/>
+      <c r="D72" s="58"/>
       <c r="E72" s="59"/>
       <c r="F72" s="59"/>
       <c r="G72" s="38" t="s">
@@ -11849,7 +11861,7 @@
       <c r="C73" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="D73" s="60"/>
+      <c r="D73" s="58"/>
       <c r="E73" s="59"/>
       <c r="F73" s="59"/>
       <c r="G73" s="38" t="s">
@@ -11864,7 +11876,7 @@
       <c r="C74" s="34" t="s">
         <v>311</v>
       </c>
-      <c r="D74" s="60"/>
+      <c r="D74" s="58"/>
       <c r="E74" s="59"/>
       <c r="F74" s="59"/>
       <c r="G74" s="38" t="s">
@@ -11879,7 +11891,7 @@
       <c r="C75" s="34" t="s">
         <v>317</v>
       </c>
-      <c r="D75" s="60" t="s">
+      <c r="D75" s="58" t="s">
         <v>318</v>
       </c>
       <c r="E75" s="59"/>
@@ -11898,7 +11910,7 @@
       <c r="C76" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="D76" s="60"/>
+      <c r="D76" s="58"/>
       <c r="E76" s="59"/>
       <c r="F76" s="59"/>
       <c r="G76" s="38" t="s">
@@ -11913,7 +11925,7 @@
       <c r="C77" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="D77" s="68" t="s">
+      <c r="D77" s="60" t="s">
         <v>323</v>
       </c>
       <c r="E77" s="59"/>
@@ -11932,7 +11944,7 @@
       <c r="C78" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="D78" s="68"/>
+      <c r="D78" s="60"/>
       <c r="E78" s="59"/>
       <c r="F78" s="59"/>
       <c r="G78" s="38" t="s">
@@ -11943,7 +11955,7 @@
       <c r="C79" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="D79" s="60" t="s">
+      <c r="D79" s="58" t="s">
         <v>328</v>
       </c>
       <c r="E79" s="59"/>
@@ -11958,7 +11970,7 @@
       <c r="C80" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="D80" s="60"/>
+      <c r="D80" s="58"/>
       <c r="E80" s="59"/>
       <c r="F80" s="59"/>
       <c r="G80" s="38" t="s">
@@ -11969,7 +11981,7 @@
       <c r="C81" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="D81" s="60" t="s">
+      <c r="D81" s="58" t="s">
         <v>333</v>
       </c>
       <c r="E81" s="59"/>
@@ -11984,7 +11996,7 @@
       <c r="C82" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="D82" s="60"/>
+      <c r="D82" s="58"/>
       <c r="E82" s="59"/>
       <c r="F82" s="59"/>
       <c r="G82" s="38" t="s">
@@ -11995,7 +12007,7 @@
       <c r="C83" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="D83" s="60" t="s">
+      <c r="D83" s="58" t="s">
         <v>338</v>
       </c>
       <c r="E83" s="59"/>
@@ -12010,7 +12022,7 @@
       <c r="C84" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="D84" s="60"/>
+      <c r="D84" s="58"/>
       <c r="E84" s="59"/>
       <c r="F84" s="59"/>
       <c r="G84" s="38" t="s">
@@ -12021,7 +12033,7 @@
       <c r="C85" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="D85" s="60" t="s">
+      <c r="D85" s="58" t="s">
         <v>343</v>
       </c>
       <c r="E85" s="59"/>
@@ -12036,7 +12048,7 @@
       <c r="C86" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="D86" s="60"/>
+      <c r="D86" s="58"/>
       <c r="E86" s="59"/>
       <c r="F86" s="59"/>
       <c r="G86" s="38" t="s">
@@ -12047,7 +12059,7 @@
       <c r="C87" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="D87" s="60" t="s">
+      <c r="D87" s="58" t="s">
         <v>348</v>
       </c>
       <c r="E87" s="59"/>
@@ -12062,7 +12074,7 @@
       <c r="C88" s="34" t="s">
         <v>350</v>
       </c>
-      <c r="D88" s="60"/>
+      <c r="D88" s="58"/>
       <c r="E88" s="59"/>
       <c r="F88" s="59"/>
       <c r="G88" s="38" t="s">
@@ -12073,7 +12085,7 @@
       <c r="C89" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="D89" s="60" t="s">
+      <c r="D89" s="58" t="s">
         <v>361</v>
       </c>
       <c r="E89" s="59"/>
@@ -12088,7 +12100,7 @@
       <c r="C90" s="34" t="s">
         <v>363</v>
       </c>
-      <c r="D90" s="60"/>
+      <c r="D90" s="58"/>
       <c r="E90" s="59"/>
       <c r="F90" s="59"/>
       <c r="G90" s="38" t="s">
@@ -12099,7 +12111,7 @@
       <c r="C91" s="34" t="s">
         <v>365</v>
       </c>
-      <c r="D91" s="60" t="s">
+      <c r="D91" s="58" t="s">
         <v>366</v>
       </c>
       <c r="E91" s="59"/>
@@ -12114,7 +12126,7 @@
       <c r="C92" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="D92" s="60"/>
+      <c r="D92" s="58"/>
       <c r="E92" s="59"/>
       <c r="F92" s="59"/>
       <c r="G92" s="38" t="s">
@@ -12125,7 +12137,7 @@
       <c r="C93" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="D93" s="60"/>
+      <c r="D93" s="58"/>
       <c r="E93" s="59"/>
       <c r="F93" s="59"/>
       <c r="G93" s="38" t="s">
@@ -12136,7 +12148,7 @@
       <c r="C94" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="D94" s="60" t="s">
+      <c r="D94" s="58" t="s">
         <v>371</v>
       </c>
       <c r="E94" s="59"/>
@@ -12151,7 +12163,7 @@
       <c r="C95" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="D95" s="60"/>
+      <c r="D95" s="58"/>
       <c r="E95" s="59"/>
       <c r="F95" s="59"/>
       <c r="G95" s="38" t="s">
@@ -12162,7 +12174,7 @@
       <c r="C96" s="34" t="s">
         <v>384</v>
       </c>
-      <c r="D96" s="60"/>
+      <c r="D96" s="58"/>
       <c r="E96" s="59"/>
       <c r="F96" s="59"/>
       <c r="G96" s="38" t="s">
@@ -12174,7 +12186,7 @@
       <c r="C97" s="36" t="s">
         <v>373</v>
       </c>
-      <c r="D97" s="60" t="s">
+      <c r="D97" s="58" t="s">
         <v>374</v>
       </c>
       <c r="E97" s="59"/>
@@ -12190,7 +12202,7 @@
       <c r="C98" s="36" t="s">
         <v>380</v>
       </c>
-      <c r="D98" s="60"/>
+      <c r="D98" s="58"/>
       <c r="E98" s="59"/>
       <c r="F98" s="59"/>
       <c r="G98" s="38" t="s">
@@ -12202,7 +12214,7 @@
       <c r="C99" s="36" t="s">
         <v>386</v>
       </c>
-      <c r="D99" s="60"/>
+      <c r="D99" s="58"/>
       <c r="E99" s="59"/>
       <c r="F99" s="59"/>
       <c r="G99" s="38" t="s">
@@ -12217,7 +12229,7 @@
       <c r="C100" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="D100" s="60" t="s">
+      <c r="D100" s="58" t="s">
         <v>65</v>
       </c>
       <c r="E100" s="59"/>
@@ -12233,7 +12245,7 @@
       <c r="C101" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="D101" s="60"/>
+      <c r="D101" s="58"/>
       <c r="E101" s="59"/>
       <c r="F101" s="59"/>
       <c r="G101" s="38" t="s">
@@ -12244,7 +12256,7 @@
       <c r="C102" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="D102" s="60" t="s">
+      <c r="D102" s="58" t="s">
         <v>110</v>
       </c>
       <c r="E102" s="59"/>
@@ -12259,7 +12271,7 @@
       <c r="C103" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="D103" s="60"/>
+      <c r="D103" s="58"/>
       <c r="E103" s="59"/>
       <c r="F103" s="59"/>
       <c r="G103" s="38" t="s">
@@ -12270,7 +12282,7 @@
       <c r="C104" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="D104" s="60"/>
+      <c r="D104" s="58"/>
       <c r="E104" s="59"/>
       <c r="F104" s="59"/>
       <c r="G104" s="38" t="s">
@@ -12281,7 +12293,7 @@
       <c r="C105" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="D105" s="60" t="s">
+      <c r="D105" s="58" t="s">
         <v>119</v>
       </c>
       <c r="E105" s="59"/>
@@ -12296,7 +12308,7 @@
       <c r="C106" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="D106" s="60"/>
+      <c r="D106" s="58"/>
       <c r="E106" s="59"/>
       <c r="F106" s="59"/>
       <c r="G106" s="38" t="s">
@@ -12307,7 +12319,7 @@
       <c r="C107" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="D107" s="60" t="s">
+      <c r="D107" s="58" t="s">
         <v>124</v>
       </c>
       <c r="E107" s="59"/>
@@ -12322,7 +12334,7 @@
       <c r="C108" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="D108" s="60"/>
+      <c r="D108" s="58"/>
       <c r="E108" s="59"/>
       <c r="F108" s="59"/>
       <c r="G108" s="38" t="s">
@@ -12333,7 +12345,7 @@
       <c r="C109" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="D109" s="60"/>
+      <c r="D109" s="58"/>
       <c r="E109" s="59"/>
       <c r="F109" s="59"/>
       <c r="G109" s="38" t="s">
@@ -12344,7 +12356,7 @@
       <c r="C110" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="D110" s="60" t="s">
+      <c r="D110" s="58" t="s">
         <v>131</v>
       </c>
       <c r="E110" s="59"/>
@@ -12359,7 +12371,7 @@
       <c r="C111" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="D111" s="60"/>
+      <c r="D111" s="58"/>
       <c r="E111" s="59"/>
       <c r="F111" s="59"/>
       <c r="G111" s="38" t="s">
@@ -12370,7 +12382,7 @@
       <c r="C112" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="D112" s="60"/>
+      <c r="D112" s="58"/>
       <c r="E112" s="59"/>
       <c r="F112" s="59"/>
       <c r="G112" s="38" t="s">
@@ -12381,7 +12393,7 @@
       <c r="C113" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="D113" s="60" t="s">
+      <c r="D113" s="58" t="s">
         <v>159</v>
       </c>
       <c r="E113" s="59"/>
@@ -12396,7 +12408,7 @@
       <c r="C114" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="D114" s="60"/>
+      <c r="D114" s="58"/>
       <c r="E114" s="59"/>
       <c r="F114" s="59"/>
       <c r="G114" s="38" t="s">
@@ -12407,7 +12419,7 @@
       <c r="C115" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="D115" s="60" t="s">
+      <c r="D115" s="58" t="s">
         <v>164</v>
       </c>
       <c r="E115" s="59"/>
@@ -12422,7 +12434,7 @@
       <c r="C116" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="D116" s="60"/>
+      <c r="D116" s="58"/>
       <c r="E116" s="59"/>
       <c r="F116" s="59"/>
       <c r="G116" s="38" t="s">
@@ -12433,7 +12445,7 @@
       <c r="C117" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="D117" s="60"/>
+      <c r="D117" s="58"/>
       <c r="E117" s="59"/>
       <c r="F117" s="59"/>
       <c r="G117" s="38" t="s">
@@ -12444,7 +12456,7 @@
       <c r="C118" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="D118" s="60" t="s">
+      <c r="D118" s="58" t="s">
         <v>179</v>
       </c>
       <c r="E118" s="59"/>
@@ -12459,7 +12471,7 @@
       <c r="C119" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="D119" s="60"/>
+      <c r="D119" s="58"/>
       <c r="E119" s="59"/>
       <c r="F119" s="59"/>
       <c r="G119" s="38" t="s">
@@ -12470,7 +12482,7 @@
       <c r="C120" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="D120" s="60"/>
+      <c r="D120" s="58"/>
       <c r="E120" s="59"/>
       <c r="F120" s="59"/>
       <c r="G120" s="38" t="s">
@@ -12481,7 +12493,7 @@
       <c r="C121" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="D121" s="60" t="s">
+      <c r="D121" s="58" t="s">
         <v>186</v>
       </c>
       <c r="E121" s="59"/>
@@ -12499,7 +12511,7 @@
       <c r="C122" s="34" t="s">
         <v>188</v>
       </c>
-      <c r="D122" s="60"/>
+      <c r="D122" s="58"/>
       <c r="E122" s="59"/>
       <c r="F122" s="59"/>
       <c r="G122" s="38" t="s">
@@ -12513,7 +12525,7 @@
       <c r="C123" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="D123" s="60" t="s">
+      <c r="D123" s="58" t="s">
         <v>195</v>
       </c>
       <c r="E123" s="59"/>
@@ -12531,7 +12543,7 @@
       <c r="C124" s="34" t="s">
         <v>197</v>
       </c>
-      <c r="D124" s="60"/>
+      <c r="D124" s="58"/>
       <c r="E124" s="59"/>
       <c r="F124" s="59"/>
       <c r="G124" s="38" t="s">
@@ -12545,7 +12557,7 @@
       <c r="C125" s="34" t="s">
         <v>199</v>
       </c>
-      <c r="D125" s="60" t="s">
+      <c r="D125" s="58" t="s">
         <v>200</v>
       </c>
       <c r="E125" s="59"/>
@@ -12563,7 +12575,7 @@
       <c r="C126" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="D126" s="60"/>
+      <c r="D126" s="58"/>
       <c r="E126" s="59"/>
       <c r="F126" s="59"/>
       <c r="G126" s="38" t="s">
@@ -12577,7 +12589,7 @@
       <c r="C127" s="34" t="s">
         <v>210</v>
       </c>
-      <c r="D127" s="60" t="s">
+      <c r="D127" s="58" t="s">
         <v>211</v>
       </c>
       <c r="E127" s="59"/>
@@ -12595,7 +12607,7 @@
       <c r="C128" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="D128" s="60"/>
+      <c r="D128" s="58"/>
       <c r="E128" s="59"/>
       <c r="F128" s="59"/>
       <c r="G128" s="38" t="s">
@@ -12609,7 +12621,7 @@
       <c r="C129" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="D129" s="60"/>
+      <c r="D129" s="58"/>
       <c r="E129" s="59"/>
       <c r="F129" s="59"/>
       <c r="G129" s="38" t="s">
@@ -12623,7 +12635,7 @@
       <c r="C130" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="D130" s="60" t="s">
+      <c r="D130" s="58" t="s">
         <v>223</v>
       </c>
       <c r="E130" s="59"/>
@@ -12641,7 +12653,7 @@
       <c r="C131" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="D131" s="60"/>
+      <c r="D131" s="58"/>
       <c r="E131" s="59"/>
       <c r="F131" s="59"/>
       <c r="G131" s="38" t="s">
@@ -12655,7 +12667,7 @@
       <c r="C132" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="D132" s="60" t="s">
+      <c r="D132" s="58" t="s">
         <v>228</v>
       </c>
       <c r="E132" s="59"/>
@@ -12673,7 +12685,7 @@
       <c r="C133" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="D133" s="60"/>
+      <c r="D133" s="58"/>
       <c r="E133" s="59"/>
       <c r="F133" s="59"/>
       <c r="G133" s="38" t="s">
@@ -12687,7 +12699,7 @@
       <c r="C134" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="D134" s="60"/>
+      <c r="D134" s="58"/>
       <c r="E134" s="59"/>
       <c r="F134" s="59"/>
       <c r="G134" s="38" t="s">
@@ -12767,7 +12779,7 @@
       <c r="C139" s="34" t="s">
         <v>454</v>
       </c>
-      <c r="D139" s="60" t="s">
+      <c r="D139" s="58" t="s">
         <v>582</v>
       </c>
       <c r="E139" s="59"/>
@@ -12782,7 +12794,7 @@
       <c r="C140" s="34" t="s">
         <v>457</v>
       </c>
-      <c r="D140" s="60"/>
+      <c r="D140" s="58"/>
       <c r="E140" s="59"/>
       <c r="F140" s="59"/>
       <c r="G140" s="38" t="s">
@@ -12793,7 +12805,7 @@
       <c r="C141" s="34" t="s">
         <v>459</v>
       </c>
-      <c r="D141" s="60" t="s">
+      <c r="D141" s="58" t="s">
         <v>460</v>
       </c>
       <c r="E141" s="59"/>
@@ -12808,7 +12820,7 @@
       <c r="C142" s="34" t="s">
         <v>462</v>
       </c>
-      <c r="D142" s="60"/>
+      <c r="D142" s="58"/>
       <c r="E142" s="59"/>
       <c r="F142" s="59"/>
       <c r="G142" s="38" t="s">
@@ -12866,7 +12878,7 @@
       <c r="C146" s="34" t="s">
         <v>477</v>
       </c>
-      <c r="D146" s="60" t="s">
+      <c r="D146" s="58" t="s">
         <v>478</v>
       </c>
       <c r="E146" s="59"/>
@@ -12885,8 +12897,8 @@
         <v>480</v>
       </c>
       <c r="D147" s="62"/>
-      <c r="E147" s="64"/>
-      <c r="F147" s="64"/>
+      <c r="E147" s="66"/>
+      <c r="F147" s="66"/>
       <c r="G147" s="39" t="s">
         <v>33</v>
       </c>
@@ -12909,7 +12921,7 @@
       <c r="D149" s="36"/>
       <c r="E149" s="43">
         <f>COUNTBLANK(E2:E147)</f>
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F149" s="46"/>
       <c r="G149" s="36"/>
@@ -12922,7 +12934,7 @@
       <c r="D150" s="36"/>
       <c r="E150" s="43">
         <f>COUNTA(E2:E147)</f>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F150" s="46"/>
       <c r="G150" s="36"/>
@@ -12950,6 +12962,183 @@
     </row>
   </sheetData>
   <mergeCells count="201">
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="D97:D99"/>
+    <mergeCell ref="E97:E99"/>
+    <mergeCell ref="F97:F99"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="D146:D147"/>
+    <mergeCell ref="E146:E147"/>
+    <mergeCell ref="F146:F147"/>
+    <mergeCell ref="D130:D131"/>
+    <mergeCell ref="E130:E131"/>
+    <mergeCell ref="F130:F131"/>
+    <mergeCell ref="D132:D134"/>
+    <mergeCell ref="E132:E134"/>
+    <mergeCell ref="F132:F134"/>
+    <mergeCell ref="D139:D140"/>
+    <mergeCell ref="D141:D142"/>
+    <mergeCell ref="F139:F140"/>
+    <mergeCell ref="F141:F142"/>
+    <mergeCell ref="E139:E140"/>
+    <mergeCell ref="E141:E142"/>
+    <mergeCell ref="D125:D126"/>
+    <mergeCell ref="E125:E126"/>
+    <mergeCell ref="F125:F126"/>
+    <mergeCell ref="D127:D129"/>
+    <mergeCell ref="E127:E129"/>
+    <mergeCell ref="F127:F129"/>
+    <mergeCell ref="D121:D122"/>
+    <mergeCell ref="E121:E122"/>
+    <mergeCell ref="F121:F122"/>
+    <mergeCell ref="D123:D124"/>
+    <mergeCell ref="E123:E124"/>
+    <mergeCell ref="F123:F124"/>
+    <mergeCell ref="D115:D117"/>
+    <mergeCell ref="E115:E117"/>
+    <mergeCell ref="F115:F117"/>
+    <mergeCell ref="D118:D120"/>
+    <mergeCell ref="E118:E120"/>
+    <mergeCell ref="F118:F120"/>
+    <mergeCell ref="D110:D112"/>
+    <mergeCell ref="E110:E112"/>
+    <mergeCell ref="F110:F112"/>
+    <mergeCell ref="D113:D114"/>
+    <mergeCell ref="E113:E114"/>
+    <mergeCell ref="F113:F114"/>
+    <mergeCell ref="D105:D106"/>
+    <mergeCell ref="E105:E106"/>
+    <mergeCell ref="F105:F106"/>
+    <mergeCell ref="D107:D109"/>
+    <mergeCell ref="E107:E109"/>
+    <mergeCell ref="F107:F109"/>
+    <mergeCell ref="D100:D101"/>
+    <mergeCell ref="E100:E101"/>
+    <mergeCell ref="F100:F101"/>
+    <mergeCell ref="D102:D104"/>
+    <mergeCell ref="E102:E104"/>
+    <mergeCell ref="F102:F104"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="E43:E45"/>
+    <mergeCell ref="F43:F45"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="G43:G45"/>
+    <mergeCell ref="G46:G48"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="F22:F25"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="D43:D45"/>
+    <mergeCell ref="D46:D48"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D64:D66"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="F64:F66"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="F89:F90"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="F67:F68"/>
+    <mergeCell ref="E71:E74"/>
+    <mergeCell ref="F71:F74"/>
+    <mergeCell ref="E64:E66"/>
+    <mergeCell ref="D87:D88"/>
+    <mergeCell ref="D89:D90"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="E83:E84"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="E87:E88"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="F77:F78"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="F81:F82"/>
+    <mergeCell ref="F83:F84"/>
+    <mergeCell ref="F85:F86"/>
+    <mergeCell ref="F87:F88"/>
     <mergeCell ref="D91:D93"/>
     <mergeCell ref="E91:E93"/>
     <mergeCell ref="F91:F93"/>
@@ -12974,183 +13163,6 @@
     <mergeCell ref="D85:D86"/>
     <mergeCell ref="F51:F53"/>
     <mergeCell ref="E89:E90"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="E81:E82"/>
-    <mergeCell ref="E83:E84"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="E87:E88"/>
-    <mergeCell ref="F75:F76"/>
-    <mergeCell ref="F77:F78"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="F81:F82"/>
-    <mergeCell ref="F83:F84"/>
-    <mergeCell ref="F85:F86"/>
-    <mergeCell ref="F87:F88"/>
-    <mergeCell ref="F89:F90"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="F67:F68"/>
-    <mergeCell ref="E71:E74"/>
-    <mergeCell ref="F71:F74"/>
-    <mergeCell ref="E64:E66"/>
-    <mergeCell ref="D87:D88"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="D43:D45"/>
-    <mergeCell ref="D46:D48"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="D64:D66"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="F64:F66"/>
-    <mergeCell ref="D89:D90"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="F22:F25"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="G40:G42"/>
-    <mergeCell ref="E43:E45"/>
-    <mergeCell ref="F43:F45"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="G43:G45"/>
-    <mergeCell ref="G46:G48"/>
-    <mergeCell ref="D105:D106"/>
-    <mergeCell ref="E105:E106"/>
-    <mergeCell ref="F105:F106"/>
-    <mergeCell ref="D107:D109"/>
-    <mergeCell ref="E107:E109"/>
-    <mergeCell ref="F107:F109"/>
-    <mergeCell ref="D100:D101"/>
-    <mergeCell ref="E100:E101"/>
-    <mergeCell ref="F100:F101"/>
-    <mergeCell ref="D102:D104"/>
-    <mergeCell ref="E102:E104"/>
-    <mergeCell ref="F102:F104"/>
-    <mergeCell ref="D115:D117"/>
-    <mergeCell ref="E115:E117"/>
-    <mergeCell ref="F115:F117"/>
-    <mergeCell ref="D118:D120"/>
-    <mergeCell ref="E118:E120"/>
-    <mergeCell ref="F118:F120"/>
-    <mergeCell ref="D110:D112"/>
-    <mergeCell ref="E110:E112"/>
-    <mergeCell ref="F110:F112"/>
-    <mergeCell ref="D113:D114"/>
-    <mergeCell ref="E113:E114"/>
-    <mergeCell ref="F113:F114"/>
-    <mergeCell ref="D125:D126"/>
-    <mergeCell ref="E125:E126"/>
-    <mergeCell ref="F125:F126"/>
-    <mergeCell ref="D127:D129"/>
-    <mergeCell ref="E127:E129"/>
-    <mergeCell ref="F127:F129"/>
-    <mergeCell ref="D121:D122"/>
-    <mergeCell ref="E121:E122"/>
-    <mergeCell ref="F121:F122"/>
-    <mergeCell ref="D123:D124"/>
-    <mergeCell ref="E123:E124"/>
-    <mergeCell ref="F123:F124"/>
-    <mergeCell ref="D146:D147"/>
-    <mergeCell ref="E146:E147"/>
-    <mergeCell ref="F146:F147"/>
-    <mergeCell ref="D130:D131"/>
-    <mergeCell ref="E130:E131"/>
-    <mergeCell ref="F130:F131"/>
-    <mergeCell ref="D132:D134"/>
-    <mergeCell ref="E132:E134"/>
-    <mergeCell ref="F132:F134"/>
-    <mergeCell ref="D139:D140"/>
-    <mergeCell ref="D141:D142"/>
-    <mergeCell ref="F139:F140"/>
-    <mergeCell ref="F141:F142"/>
-    <mergeCell ref="E139:E140"/>
-    <mergeCell ref="E141:E142"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="D97:D99"/>
-    <mergeCell ref="E97:E99"/>
-    <mergeCell ref="F97:F99"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -13208,7 +13220,7 @@
       <c r="D2" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="70">
+      <c r="E2" s="71">
         <v>101332</v>
       </c>
     </row>
@@ -13225,7 +13237,7 @@
       <c r="D3" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="70"/>
+      <c r="E3" s="71"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -13240,7 +13252,7 @@
       <c r="D4" t="s">
         <v>524</v>
       </c>
-      <c r="E4" s="70">
+      <c r="E4" s="71">
         <v>99343</v>
       </c>
     </row>
@@ -13257,7 +13269,7 @@
       <c r="D5" t="s">
         <v>524</v>
       </c>
-      <c r="E5" s="70"/>
+      <c r="E5" s="71"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -13272,7 +13284,7 @@
       <c r="D6" t="s">
         <v>516</v>
       </c>
-      <c r="E6" s="70">
+      <c r="E6" s="71">
         <v>102453</v>
       </c>
     </row>
@@ -13289,7 +13301,7 @@
       <c r="D7" t="s">
         <v>516</v>
       </c>
-      <c r="E7" s="70"/>
+      <c r="E7" s="71"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -13304,7 +13316,7 @@
       <c r="D8" t="s">
         <v>521</v>
       </c>
-      <c r="E8" s="70">
+      <c r="E8" s="71">
         <v>102447</v>
       </c>
     </row>
@@ -13321,7 +13333,7 @@
       <c r="D9" t="s">
         <v>521</v>
       </c>
-      <c r="E9" s="70"/>
+      <c r="E9" s="71"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -13336,7 +13348,7 @@
       <c r="D10" t="s">
         <v>521</v>
       </c>
-      <c r="E10" s="70"/>
+      <c r="E10" s="71"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -13351,7 +13363,7 @@
       <c r="D11" t="s">
         <v>521</v>
       </c>
-      <c r="E11" s="70"/>
+      <c r="E11" s="71"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -13366,7 +13378,7 @@
       <c r="D12" t="s">
         <v>512</v>
       </c>
-      <c r="E12" s="70">
+      <c r="E12" s="71">
         <v>101221</v>
       </c>
     </row>
@@ -13383,7 +13395,7 @@
       <c r="D13" t="s">
         <v>512</v>
       </c>
-      <c r="E13" s="70"/>
+      <c r="E13" s="71"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -13398,7 +13410,7 @@
       <c r="D14" t="s">
         <v>517</v>
       </c>
-      <c r="E14" s="70">
+      <c r="E14" s="71">
         <v>102455</v>
       </c>
     </row>
@@ -13415,7 +13427,7 @@
       <c r="D15" t="s">
         <v>517</v>
       </c>
-      <c r="E15" s="70"/>
+      <c r="E15" s="71"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -13430,7 +13442,7 @@
       <c r="D16" t="s">
         <v>508</v>
       </c>
-      <c r="E16" s="70">
+      <c r="E16" s="71">
         <v>1013824</v>
       </c>
     </row>
@@ -13447,7 +13459,7 @@
       <c r="D17" t="s">
         <v>508</v>
       </c>
-      <c r="E17" s="70"/>
+      <c r="E17" s="71"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -13462,7 +13474,7 @@
       <c r="D18" t="s">
         <v>510</v>
       </c>
-      <c r="E18" s="70">
+      <c r="E18" s="71">
         <v>102445</v>
       </c>
     </row>
@@ -13479,7 +13491,7 @@
       <c r="D19" t="s">
         <v>510</v>
       </c>
-      <c r="E19" s="70"/>
+      <c r="E19" s="71"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -13494,7 +13506,7 @@
       <c r="D20" t="s">
         <v>511</v>
       </c>
-      <c r="E20" s="70">
+      <c r="E20" s="71">
         <v>101557</v>
       </c>
     </row>
@@ -13511,7 +13523,7 @@
       <c r="D21" t="s">
         <v>511</v>
       </c>
-      <c r="E21" s="70"/>
+      <c r="E21" s="71"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -13526,7 +13538,7 @@
       <c r="D22" t="s">
         <v>509</v>
       </c>
-      <c r="E22" s="70">
+      <c r="E22" s="71">
         <v>101339</v>
       </c>
     </row>
@@ -13543,7 +13555,7 @@
       <c r="D23" t="s">
         <v>509</v>
       </c>
-      <c r="E23" s="70"/>
+      <c r="E23" s="71"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -13558,7 +13570,7 @@
       <c r="D24" t="s">
         <v>520</v>
       </c>
-      <c r="E24" s="70">
+      <c r="E24" s="71">
         <v>102391</v>
       </c>
     </row>
@@ -13575,7 +13587,7 @@
       <c r="D25" t="s">
         <v>520</v>
       </c>
-      <c r="E25" s="70"/>
+      <c r="E25" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -14532,6 +14544,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEAE28352B96D64C95AA0D5E2FA62FAD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed183881d36ac1b5d7d67982eda510d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d161086-4829-409f-9f75-5bde88dcb151" xmlns:ns3="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="685f4fda20cf913d28bf77c13cd653dd" ns2:_="" ns3:_="">
     <xsd:import namespace="3d161086-4829-409f-9f75-5bde88dcb151"/>
@@ -14754,27 +14786,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C74AB5E7-5C87-4FF7-BF80-AB0EB6BD1D32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14791,29 +14828,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
User questions updated, MEDS_Tables updated
</commit_message>
<xml_diff>
--- a/analysis/MEDS_Tables.xlsx
+++ b/analysis/MEDS_Tables.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="577" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A864FF4-3463-48DB-A6CE-A3B148BE268A}"/>
+  <xr:revisionPtr revIDLastSave="596" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CB97B8D-766D-4129-B6D3-8810EBAD930B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meds_tables" sheetId="1" r:id="rId1"/>
     <sheet name="csv" sheetId="6" r:id="rId2"/>
     <sheet name="tasks" sheetId="10" r:id="rId3"/>
-    <sheet name="form" sheetId="7" r:id="rId4"/>
-    <sheet name="serd" sheetId="8" r:id="rId5"/>
-    <sheet name="output" sheetId="9" r:id="rId6"/>
-    <sheet name="enhancements" sheetId="4" r:id="rId7"/>
+    <sheet name="indexes candidates" sheetId="11" r:id="rId4"/>
+    <sheet name="form" sheetId="7" r:id="rId5"/>
+    <sheet name="serd" sheetId="8" r:id="rId6"/>
+    <sheet name="output" sheetId="9" r:id="rId7"/>
+    <sheet name="enhancements" sheetId="4" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">meds_tables!$A$1:$X$1</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2734" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2744" uniqueCount="596">
   <si>
     <t>Table</t>
   </si>
@@ -1808,6 +1809,24 @@
   </si>
   <si>
     <t>Jobs</t>
+  </si>
+  <si>
+    <t>Data Audit</t>
+  </si>
+  <si>
+    <t>Add audit to the application tables and funcionality to access and report on it</t>
+  </si>
+  <si>
+    <t>SOURCE</t>
+  </si>
+  <si>
+    <t>SUPPLIER</t>
+  </si>
+  <si>
+    <t>MEDS_PROCESSING_JOBS</t>
+  </si>
+  <si>
+    <t>ORIGINATOR</t>
   </si>
 </sst>
 </file>
@@ -2659,12 +2678,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2673,29 +2695,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -10733,8 +10752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8FA477-9B46-4053-B7AD-310B8B9F2B30}">
   <dimension ref="A1:P152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38:E39"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10769,7 +10788,7 @@
       <c r="H1" s="48"/>
       <c r="I1" s="41">
         <f>E150/E149</f>
-        <v>0.13178294573643412</v>
+        <v>0.14960629921259844</v>
       </c>
       <c r="J1" s="49" t="s">
         <v>566</v>
@@ -10781,7 +10800,7 @@
       <c r="C2" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="62" t="s">
         <v>38</v>
       </c>
       <c r="E2" s="64" t="s">
@@ -10790,7 +10809,7 @@
       <c r="F2" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="65" t="s">
+      <c r="G2" s="66" t="s">
         <v>564</v>
       </c>
     </row>
@@ -10799,10 +10818,10 @@
       <c r="C3" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="63"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="68"/>
       <c r="K3" s="36"/>
       <c r="L3" s="36"/>
       <c r="M3" s="36"/>
@@ -10815,10 +10834,10 @@
       <c r="C4" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="63"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="68"/>
       <c r="K4" s="36"/>
       <c r="L4" s="36"/>
       <c r="M4" s="36"/>
@@ -10831,27 +10850,27 @@
       <c r="C5" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="F5" s="59" t="s">
+      <c r="F5" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="63" t="s">
+      <c r="G5" s="68" t="s">
         <v>519</v>
       </c>
       <c r="K5" s="36"/>
       <c r="L5" s="47" t="s">
         <v>464</v>
       </c>
-      <c r="M5" s="70" t="s">
+      <c r="M5" s="59" t="s">
         <v>465</v>
       </c>
-      <c r="N5" s="59"/>
-      <c r="O5" s="69" t="s">
+      <c r="N5" s="60"/>
+      <c r="O5" s="58" t="s">
         <v>581</v>
       </c>
       <c r="P5" s="36"/>
@@ -10861,17 +10880,17 @@
       <c r="C6" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="58"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="63"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="68"/>
       <c r="K6" s="36"/>
       <c r="L6" s="47" t="s">
         <v>467</v>
       </c>
-      <c r="M6" s="70"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="69"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="58"/>
       <c r="P6" s="36"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
@@ -10879,16 +10898,16 @@
       <c r="C7" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="58" t="s">
+      <c r="D7" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="63" t="s">
+      <c r="G7" s="68" t="s">
         <v>80</v>
       </c>
       <c r="K7" s="36"/>
@@ -10903,10 +10922,10 @@
       <c r="C8" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="58"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="63"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="68"/>
       <c r="K8" s="36"/>
       <c r="L8" s="36"/>
       <c r="M8" s="36"/>
@@ -10919,16 +10938,16 @@
       <c r="C9" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="D9" s="58" t="s">
+      <c r="D9" s="61" t="s">
         <v>171</v>
       </c>
-      <c r="E9" s="59" t="s">
+      <c r="E9" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="59" t="s">
+      <c r="F9" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="63" t="s">
+      <c r="G9" s="68" t="s">
         <v>523</v>
       </c>
       <c r="J9" s="36"/>
@@ -10939,10 +10958,10 @@
       <c r="C10" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="63"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="68"/>
       <c r="J10" s="36"/>
       <c r="K10" s="36"/>
     </row>
@@ -10951,10 +10970,10 @@
       <c r="C11" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="D11" s="58"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="63"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="68"/>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
     </row>
@@ -10963,16 +10982,16 @@
       <c r="C12" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="D12" s="58" t="s">
+      <c r="D12" s="61" t="s">
         <v>204</v>
       </c>
-      <c r="E12" s="59" t="s">
+      <c r="E12" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="59" t="s">
+      <c r="F12" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="63" t="s">
+      <c r="G12" s="68" t="s">
         <v>515</v>
       </c>
       <c r="J12" s="36"/>
@@ -10983,10 +11002,10 @@
       <c r="C13" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="D13" s="58"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="63"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="68"/>
       <c r="J13" s="36"/>
       <c r="K13" s="36"/>
     </row>
@@ -10995,16 +11014,16 @@
       <c r="C14" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="D14" s="58" t="s">
+      <c r="D14" s="61" t="s">
         <v>361</v>
       </c>
-      <c r="E14" s="59" t="s">
+      <c r="E14" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="F14" s="59" t="s">
+      <c r="F14" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="63" t="s">
+      <c r="G14" s="68" t="s">
         <v>518</v>
       </c>
       <c r="J14" s="36"/>
@@ -11015,9 +11034,9 @@
       <c r="C15" s="35" t="s">
         <v>363</v>
       </c>
-      <c r="D15" s="62"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
       <c r="G15" s="67"/>
       <c r="J15" s="36"/>
       <c r="K15" s="36"/>
@@ -11026,7 +11045,7 @@
       <c r="C16" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="61" t="s">
+      <c r="D16" s="62" t="s">
         <v>71</v>
       </c>
       <c r="E16" s="64" t="s">
@@ -11035,7 +11054,7 @@
       <c r="F16" s="64" t="s">
         <v>567</v>
       </c>
-      <c r="G16" s="65" t="s">
+      <c r="G16" s="66" t="s">
         <v>73</v>
       </c>
       <c r="J16" s="36"/>
@@ -11045,10 +11064,10 @@
       <c r="C17" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="58"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="63"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="68"/>
       <c r="J17" s="36"/>
       <c r="K17" s="36"/>
     </row>
@@ -11056,14 +11075,16 @@
       <c r="C18" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="58" t="s">
+      <c r="D18" s="61" t="s">
         <v>105</v>
       </c>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59" t="s">
+      <c r="E18" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="60" t="s">
         <v>567</v>
       </c>
-      <c r="G18" s="63" t="s">
+      <c r="G18" s="68" t="s">
         <v>524</v>
       </c>
       <c r="J18" s="36"/>
@@ -11073,10 +11094,10 @@
       <c r="C19" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="58"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="63"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="68"/>
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
     </row>
@@ -11084,16 +11105,16 @@
       <c r="C20" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="D20" s="58" t="s">
+      <c r="D20" s="61" t="s">
         <v>300</v>
       </c>
-      <c r="E20" s="59" t="s">
+      <c r="E20" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="F20" s="59" t="s">
+      <c r="F20" s="60" t="s">
         <v>567</v>
       </c>
-      <c r="G20" s="63" t="s">
+      <c r="G20" s="68" t="s">
         <v>516</v>
       </c>
       <c r="J20" s="36"/>
@@ -11103,10 +11124,10 @@
       <c r="C21" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="D21" s="58"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="63"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="68"/>
       <c r="J21" s="36"/>
       <c r="K21" s="36"/>
     </row>
@@ -11114,14 +11135,14 @@
       <c r="C22" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="D22" s="58" t="s">
+      <c r="D22" s="61" t="s">
         <v>305</v>
       </c>
-      <c r="E22" s="59"/>
-      <c r="F22" s="59" t="s">
+      <c r="E22" s="60"/>
+      <c r="F22" s="60" t="s">
         <v>567</v>
       </c>
-      <c r="G22" s="63" t="s">
+      <c r="G22" s="68" t="s">
         <v>521</v>
       </c>
       <c r="J22" s="36"/>
@@ -11131,10 +11152,10 @@
       <c r="C23" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="D23" s="58"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="63"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="68"/>
       <c r="J23" s="36"/>
       <c r="K23" s="36"/>
     </row>
@@ -11142,10 +11163,10 @@
       <c r="C24" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="D24" s="58"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="63"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="68"/>
       <c r="J24" s="36"/>
       <c r="K24" s="36"/>
     </row>
@@ -11153,10 +11174,10 @@
       <c r="C25" s="34" t="s">
         <v>311</v>
       </c>
-      <c r="D25" s="58"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="63"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="68"/>
       <c r="J25" s="36"/>
       <c r="K25" s="36"/>
     </row>
@@ -11164,16 +11185,16 @@
       <c r="C26" s="34" t="s">
         <v>317</v>
       </c>
-      <c r="D26" s="58" t="s">
+      <c r="D26" s="61" t="s">
         <v>318</v>
       </c>
-      <c r="E26" s="59" t="s">
+      <c r="E26" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="F26" s="59" t="s">
+      <c r="F26" s="60" t="s">
         <v>567</v>
       </c>
-      <c r="G26" s="63" t="s">
+      <c r="G26" s="68" t="s">
         <v>512</v>
       </c>
       <c r="J26" s="36"/>
@@ -11183,10 +11204,10 @@
       <c r="C27" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="D27" s="58"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="63"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="68"/>
       <c r="J27" s="36"/>
       <c r="K27" s="36"/>
     </row>
@@ -11194,14 +11215,16 @@
       <c r="C28" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="D28" s="60" t="s">
+      <c r="D28" s="69" t="s">
         <v>323</v>
       </c>
-      <c r="E28" s="68"/>
-      <c r="F28" s="59" t="s">
+      <c r="E28" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" s="60" t="s">
         <v>567</v>
       </c>
-      <c r="G28" s="63" t="s">
+      <c r="G28" s="68" t="s">
         <v>517</v>
       </c>
       <c r="J28" s="36"/>
@@ -11211,25 +11234,25 @@
       <c r="C29" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="D29" s="60"/>
-      <c r="E29" s="68"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="63"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="70"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="68"/>
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C30" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="D30" s="58" t="s">
+      <c r="D30" s="61" t="s">
         <v>328</v>
       </c>
-      <c r="E30" s="59" t="s">
+      <c r="E30" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="F30" s="59" t="s">
+      <c r="F30" s="60" t="s">
         <v>567</v>
       </c>
-      <c r="G30" s="63" t="s">
+      <c r="G30" s="68" t="s">
         <v>508</v>
       </c>
     </row>
@@ -11237,25 +11260,25 @@
       <c r="C31" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="D31" s="58"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="63"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="68"/>
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="D32" s="58" t="s">
+      <c r="D32" s="61" t="s">
         <v>333</v>
       </c>
-      <c r="E32" s="59" t="s">
+      <c r="E32" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="F32" s="59" t="s">
+      <c r="F32" s="60" t="s">
         <v>567</v>
       </c>
-      <c r="G32" s="63" t="s">
+      <c r="G32" s="68" t="s">
         <v>510</v>
       </c>
     </row>
@@ -11263,25 +11286,25 @@
       <c r="C33" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="D33" s="58"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="59"/>
-      <c r="G33" s="63"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="68"/>
     </row>
     <row r="34" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C34" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="D34" s="58" t="s">
+      <c r="D34" s="61" t="s">
         <v>338</v>
       </c>
-      <c r="E34" s="59" t="s">
+      <c r="E34" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="F34" s="59" t="s">
+      <c r="F34" s="60" t="s">
         <v>567</v>
       </c>
-      <c r="G34" s="63" t="s">
+      <c r="G34" s="68" t="s">
         <v>511</v>
       </c>
     </row>
@@ -11289,25 +11312,25 @@
       <c r="C35" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="D35" s="58"/>
-      <c r="E35" s="59"/>
-      <c r="F35" s="59"/>
-      <c r="G35" s="63"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="68"/>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C36" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="D36" s="58" t="s">
+      <c r="D36" s="61" t="s">
         <v>343</v>
       </c>
-      <c r="E36" s="59" t="s">
+      <c r="E36" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="F36" s="59" t="s">
+      <c r="F36" s="60" t="s">
         <v>567</v>
       </c>
-      <c r="G36" s="63" t="s">
+      <c r="G36" s="68" t="s">
         <v>509</v>
       </c>
     </row>
@@ -11315,25 +11338,25 @@
       <c r="C37" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="D37" s="58"/>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
-      <c r="G37" s="63"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
+      <c r="G37" s="68"/>
     </row>
     <row r="38" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C38" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="D38" s="58" t="s">
+      <c r="D38" s="61" t="s">
         <v>348</v>
       </c>
-      <c r="E38" s="59" t="s">
+      <c r="E38" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="F38" s="59" t="s">
+      <c r="F38" s="60" t="s">
         <v>567</v>
       </c>
-      <c r="G38" s="63" t="s">
+      <c r="G38" s="68" t="s">
         <v>520</v>
       </c>
     </row>
@@ -11341,16 +11364,16 @@
       <c r="C39" s="35" t="s">
         <v>350</v>
       </c>
-      <c r="D39" s="62"/>
-      <c r="E39" s="66"/>
-      <c r="F39" s="66"/>
+      <c r="D39" s="63"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="65"/>
       <c r="G39" s="67"/>
     </row>
     <row r="40" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C40" s="33" t="s">
         <v>365</v>
       </c>
-      <c r="D40" s="61" t="s">
+      <c r="D40" s="62" t="s">
         <v>366</v>
       </c>
       <c r="E40" s="64" t="s">
@@ -11359,7 +11382,7 @@
       <c r="F40" s="64" t="s">
         <v>369</v>
       </c>
-      <c r="G40" s="65" t="s">
+      <c r="G40" s="66" t="s">
         <v>514</v>
       </c>
     </row>
@@ -11367,34 +11390,34 @@
       <c r="C41" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="D41" s="58"/>
-      <c r="E41" s="59"/>
-      <c r="F41" s="59"/>
-      <c r="G41" s="63"/>
+      <c r="D41" s="61"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="68"/>
     </row>
     <row r="42" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C42" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="D42" s="58"/>
-      <c r="E42" s="59"/>
-      <c r="F42" s="59"/>
-      <c r="G42" s="63"/>
+      <c r="D42" s="61"/>
+      <c r="E42" s="60"/>
+      <c r="F42" s="60"/>
+      <c r="G42" s="68"/>
     </row>
     <row r="43" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C43" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="D43" s="58" t="s">
+      <c r="D43" s="61" t="s">
         <v>371</v>
       </c>
-      <c r="E43" s="59" t="s">
+      <c r="E43" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="F43" s="59" t="s">
+      <c r="F43" s="60" t="s">
         <v>369</v>
       </c>
-      <c r="G43" s="63" t="s">
+      <c r="G43" s="68" t="s">
         <v>513</v>
       </c>
     </row>
@@ -11402,34 +11425,34 @@
       <c r="C44" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="D44" s="58"/>
-      <c r="E44" s="59"/>
-      <c r="F44" s="59"/>
-      <c r="G44" s="63"/>
+      <c r="D44" s="61"/>
+      <c r="E44" s="60"/>
+      <c r="F44" s="60"/>
+      <c r="G44" s="68"/>
     </row>
     <row r="45" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C45" s="34" t="s">
         <v>384</v>
       </c>
-      <c r="D45" s="58"/>
-      <c r="E45" s="59"/>
-      <c r="F45" s="59"/>
-      <c r="G45" s="63"/>
+      <c r="D45" s="61"/>
+      <c r="E45" s="60"/>
+      <c r="F45" s="60"/>
+      <c r="G45" s="68"/>
     </row>
     <row r="46" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C46" s="34" t="s">
         <v>373</v>
       </c>
-      <c r="D46" s="58" t="s">
+      <c r="D46" s="61" t="s">
         <v>374</v>
       </c>
-      <c r="E46" s="59" t="s">
+      <c r="E46" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="F46" s="59" t="s">
+      <c r="F46" s="60" t="s">
         <v>369</v>
       </c>
-      <c r="G46" s="63" t="s">
+      <c r="G46" s="68" t="s">
         <v>522</v>
       </c>
     </row>
@@ -11437,18 +11460,18 @@
       <c r="C47" s="34" t="s">
         <v>380</v>
       </c>
-      <c r="D47" s="58"/>
-      <c r="E47" s="59"/>
-      <c r="F47" s="59"/>
-      <c r="G47" s="63"/>
+      <c r="D47" s="61"/>
+      <c r="E47" s="60"/>
+      <c r="F47" s="60"/>
+      <c r="G47" s="68"/>
     </row>
     <row r="48" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C48" s="35" t="s">
         <v>386</v>
       </c>
-      <c r="D48" s="62"/>
-      <c r="E48" s="66"/>
-      <c r="F48" s="66"/>
+      <c r="D48" s="63"/>
+      <c r="E48" s="65"/>
+      <c r="F48" s="65"/>
       <c r="G48" s="67"/>
       <c r="J48" s="36"/>
       <c r="K48" s="36"/>
@@ -11459,14 +11482,14 @@
       <c r="C49" s="33" t="s">
         <v>464</v>
       </c>
-      <c r="D49" s="61" t="s">
+      <c r="D49" s="62" t="s">
         <v>465</v>
       </c>
       <c r="E49" s="64"/>
       <c r="F49" s="64" t="s">
         <v>584</v>
       </c>
-      <c r="G49" s="65" t="s">
+      <c r="G49" s="66" t="s">
         <v>585</v>
       </c>
       <c r="J49" s="36"/>
@@ -11478,9 +11501,9 @@
       <c r="C50" s="35" t="s">
         <v>467</v>
       </c>
-      <c r="D50" s="62"/>
-      <c r="E50" s="66"/>
-      <c r="F50" s="66"/>
+      <c r="D50" s="63"/>
+      <c r="E50" s="65"/>
+      <c r="F50" s="65"/>
       <c r="G50" s="67"/>
       <c r="J50" s="36"/>
       <c r="K50" s="36"/>
@@ -11491,11 +11514,11 @@
       <c r="C51" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="D51" s="58" t="s">
+      <c r="D51" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="E51" s="59"/>
-      <c r="F51" s="59" t="s">
+      <c r="E51" s="60"/>
+      <c r="F51" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G51" s="38" t="s">
@@ -11510,9 +11533,9 @@
       <c r="C52" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D52" s="58"/>
-      <c r="E52" s="59"/>
-      <c r="F52" s="59"/>
+      <c r="D52" s="61"/>
+      <c r="E52" s="60"/>
+      <c r="F52" s="60"/>
       <c r="G52" s="38" t="s">
         <v>33</v>
       </c>
@@ -11525,9 +11548,9 @@
       <c r="C53" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D53" s="58"/>
-      <c r="E53" s="59"/>
-      <c r="F53" s="59"/>
+      <c r="D53" s="61"/>
+      <c r="E53" s="60"/>
+      <c r="F53" s="60"/>
       <c r="G53" s="38" t="s">
         <v>33</v>
       </c>
@@ -11540,11 +11563,11 @@
       <c r="C54" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="D54" s="58" t="s">
+      <c r="D54" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="E54" s="59"/>
-      <c r="F54" s="59" t="s">
+      <c r="E54" s="60"/>
+      <c r="F54" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G54" s="38" t="s">
@@ -11559,9 +11582,9 @@
       <c r="C55" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D55" s="58"/>
-      <c r="E55" s="59"/>
-      <c r="F55" s="59"/>
+      <c r="D55" s="61"/>
+      <c r="E55" s="60"/>
+      <c r="F55" s="60"/>
       <c r="G55" s="38" t="s">
         <v>33</v>
       </c>
@@ -11574,11 +11597,11 @@
       <c r="C56" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D56" s="58" t="s">
+      <c r="D56" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="E56" s="59"/>
-      <c r="F56" s="59" t="s">
+      <c r="E56" s="60"/>
+      <c r="F56" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G56" s="38" t="s">
@@ -11593,9 +11616,9 @@
       <c r="C57" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D57" s="58"/>
-      <c r="E57" s="59"/>
-      <c r="F57" s="59"/>
+      <c r="D57" s="61"/>
+      <c r="E57" s="60"/>
+      <c r="F57" s="60"/>
       <c r="G57" s="38" t="s">
         <v>33</v>
       </c>
@@ -11608,11 +11631,11 @@
       <c r="C58" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D58" s="58" t="s">
+      <c r="D58" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="E58" s="59"/>
-      <c r="F58" s="59" t="s">
+      <c r="E58" s="60"/>
+      <c r="F58" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G58" s="38" t="s">
@@ -11627,9 +11650,9 @@
       <c r="C59" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D59" s="58"/>
-      <c r="E59" s="59"/>
-      <c r="F59" s="59"/>
+      <c r="D59" s="61"/>
+      <c r="E59" s="60"/>
+      <c r="F59" s="60"/>
       <c r="G59" s="38" t="s">
         <v>33</v>
       </c>
@@ -11642,11 +11665,11 @@
       <c r="C60" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="D60" s="58" t="s">
+      <c r="D60" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="E60" s="59"/>
-      <c r="F60" s="59" t="s">
+      <c r="E60" s="60"/>
+      <c r="F60" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G60" s="38" t="s">
@@ -11661,9 +11684,9 @@
       <c r="C61" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D61" s="58"/>
-      <c r="E61" s="59"/>
-      <c r="F61" s="59"/>
+      <c r="D61" s="61"/>
+      <c r="E61" s="60"/>
+      <c r="F61" s="60"/>
       <c r="G61" s="38" t="s">
         <v>33</v>
       </c>
@@ -11676,11 +11699,11 @@
       <c r="C62" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D62" s="58" t="s">
+      <c r="D62" s="61" t="s">
         <v>105</v>
       </c>
-      <c r="E62" s="59"/>
-      <c r="F62" s="59" t="s">
+      <c r="E62" s="60"/>
+      <c r="F62" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G62" s="38" t="s">
@@ -11695,9 +11718,9 @@
       <c r="C63" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D63" s="58"/>
-      <c r="E63" s="59"/>
-      <c r="F63" s="59"/>
+      <c r="D63" s="61"/>
+      <c r="E63" s="60"/>
+      <c r="F63" s="60"/>
       <c r="G63" s="38" t="s">
         <v>33</v>
       </c>
@@ -11710,11 +11733,11 @@
       <c r="C64" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="D64" s="58" t="s">
+      <c r="D64" s="61" t="s">
         <v>171</v>
       </c>
-      <c r="E64" s="59"/>
-      <c r="F64" s="59" t="s">
+      <c r="E64" s="60"/>
+      <c r="F64" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G64" s="38" t="s">
@@ -11729,9 +11752,9 @@
       <c r="C65" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="D65" s="58"/>
-      <c r="E65" s="59"/>
-      <c r="F65" s="59"/>
+      <c r="D65" s="61"/>
+      <c r="E65" s="60"/>
+      <c r="F65" s="60"/>
       <c r="G65" s="38" t="s">
         <v>33</v>
       </c>
@@ -11744,9 +11767,9 @@
       <c r="C66" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="D66" s="58"/>
-      <c r="E66" s="59"/>
-      <c r="F66" s="59"/>
+      <c r="D66" s="61"/>
+      <c r="E66" s="60"/>
+      <c r="F66" s="60"/>
       <c r="G66" s="38" t="s">
         <v>33</v>
       </c>
@@ -11759,11 +11782,11 @@
       <c r="C67" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="D67" s="58" t="s">
+      <c r="D67" s="61" t="s">
         <v>204</v>
       </c>
-      <c r="E67" s="59"/>
-      <c r="F67" s="59" t="s">
+      <c r="E67" s="60"/>
+      <c r="F67" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G67" s="38" t="s">
@@ -11778,9 +11801,9 @@
       <c r="C68" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="D68" s="58"/>
-      <c r="E68" s="59"/>
-      <c r="F68" s="59"/>
+      <c r="D68" s="61"/>
+      <c r="E68" s="60"/>
+      <c r="F68" s="60"/>
       <c r="G68" s="38" t="s">
         <v>33</v>
       </c>
@@ -11793,11 +11816,11 @@
       <c r="C69" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="D69" s="58" t="s">
+      <c r="D69" s="61" t="s">
         <v>300</v>
       </c>
-      <c r="E69" s="59"/>
-      <c r="F69" s="59" t="s">
+      <c r="E69" s="60"/>
+      <c r="F69" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G69" s="38" t="s">
@@ -11812,9 +11835,9 @@
       <c r="C70" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="D70" s="58"/>
-      <c r="E70" s="59"/>
-      <c r="F70" s="59"/>
+      <c r="D70" s="61"/>
+      <c r="E70" s="60"/>
+      <c r="F70" s="60"/>
       <c r="G70" s="38" t="s">
         <v>33</v>
       </c>
@@ -11827,11 +11850,11 @@
       <c r="C71" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="D71" s="58" t="s">
+      <c r="D71" s="61" t="s">
         <v>305</v>
       </c>
-      <c r="E71" s="59"/>
-      <c r="F71" s="59" t="s">
+      <c r="E71" s="60"/>
+      <c r="F71" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G71" s="38" t="s">
@@ -11846,9 +11869,9 @@
       <c r="C72" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="D72" s="58"/>
-      <c r="E72" s="59"/>
-      <c r="F72" s="59"/>
+      <c r="D72" s="61"/>
+      <c r="E72" s="60"/>
+      <c r="F72" s="60"/>
       <c r="G72" s="38" t="s">
         <v>33</v>
       </c>
@@ -11861,9 +11884,9 @@
       <c r="C73" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="D73" s="58"/>
-      <c r="E73" s="59"/>
-      <c r="F73" s="59"/>
+      <c r="D73" s="61"/>
+      <c r="E73" s="60"/>
+      <c r="F73" s="60"/>
       <c r="G73" s="38" t="s">
         <v>33</v>
       </c>
@@ -11876,9 +11899,9 @@
       <c r="C74" s="34" t="s">
         <v>311</v>
       </c>
-      <c r="D74" s="58"/>
-      <c r="E74" s="59"/>
-      <c r="F74" s="59"/>
+      <c r="D74" s="61"/>
+      <c r="E74" s="60"/>
+      <c r="F74" s="60"/>
       <c r="G74" s="38" t="s">
         <v>33</v>
       </c>
@@ -11891,11 +11914,11 @@
       <c r="C75" s="34" t="s">
         <v>317</v>
       </c>
-      <c r="D75" s="58" t="s">
+      <c r="D75" s="61" t="s">
         <v>318</v>
       </c>
-      <c r="E75" s="59"/>
-      <c r="F75" s="59" t="s">
+      <c r="E75" s="60"/>
+      <c r="F75" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G75" s="38" t="s">
@@ -11910,9 +11933,9 @@
       <c r="C76" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="D76" s="58"/>
-      <c r="E76" s="59"/>
-      <c r="F76" s="59"/>
+      <c r="D76" s="61"/>
+      <c r="E76" s="60"/>
+      <c r="F76" s="60"/>
       <c r="G76" s="38" t="s">
         <v>33</v>
       </c>
@@ -11925,11 +11948,11 @@
       <c r="C77" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="D77" s="60" t="s">
+      <c r="D77" s="69" t="s">
         <v>323</v>
       </c>
-      <c r="E77" s="59"/>
-      <c r="F77" s="59" t="s">
+      <c r="E77" s="60"/>
+      <c r="F77" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G77" s="38" t="s">
@@ -11944,9 +11967,9 @@
       <c r="C78" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="D78" s="60"/>
-      <c r="E78" s="59"/>
-      <c r="F78" s="59"/>
+      <c r="D78" s="69"/>
+      <c r="E78" s="60"/>
+      <c r="F78" s="60"/>
       <c r="G78" s="38" t="s">
         <v>33</v>
       </c>
@@ -11955,11 +11978,11 @@
       <c r="C79" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="D79" s="58" t="s">
+      <c r="D79" s="61" t="s">
         <v>328</v>
       </c>
-      <c r="E79" s="59"/>
-      <c r="F79" s="59" t="s">
+      <c r="E79" s="60"/>
+      <c r="F79" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G79" s="38" t="s">
@@ -11970,9 +11993,9 @@
       <c r="C80" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="D80" s="58"/>
-      <c r="E80" s="59"/>
-      <c r="F80" s="59"/>
+      <c r="D80" s="61"/>
+      <c r="E80" s="60"/>
+      <c r="F80" s="60"/>
       <c r="G80" s="38" t="s">
         <v>33</v>
       </c>
@@ -11981,11 +12004,11 @@
       <c r="C81" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="D81" s="58" t="s">
+      <c r="D81" s="61" t="s">
         <v>333</v>
       </c>
-      <c r="E81" s="59"/>
-      <c r="F81" s="59" t="s">
+      <c r="E81" s="60"/>
+      <c r="F81" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G81" s="38" t="s">
@@ -11996,9 +12019,9 @@
       <c r="C82" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="D82" s="58"/>
-      <c r="E82" s="59"/>
-      <c r="F82" s="59"/>
+      <c r="D82" s="61"/>
+      <c r="E82" s="60"/>
+      <c r="F82" s="60"/>
       <c r="G82" s="38" t="s">
         <v>33</v>
       </c>
@@ -12007,11 +12030,11 @@
       <c r="C83" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="D83" s="58" t="s">
+      <c r="D83" s="61" t="s">
         <v>338</v>
       </c>
-      <c r="E83" s="59"/>
-      <c r="F83" s="59" t="s">
+      <c r="E83" s="60"/>
+      <c r="F83" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G83" s="38" t="s">
@@ -12022,9 +12045,9 @@
       <c r="C84" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="D84" s="58"/>
-      <c r="E84" s="59"/>
-      <c r="F84" s="59"/>
+      <c r="D84" s="61"/>
+      <c r="E84" s="60"/>
+      <c r="F84" s="60"/>
       <c r="G84" s="38" t="s">
         <v>33</v>
       </c>
@@ -12033,11 +12056,11 @@
       <c r="C85" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="D85" s="58" t="s">
+      <c r="D85" s="61" t="s">
         <v>343</v>
       </c>
-      <c r="E85" s="59"/>
-      <c r="F85" s="59" t="s">
+      <c r="E85" s="60"/>
+      <c r="F85" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G85" s="38" t="s">
@@ -12048,9 +12071,9 @@
       <c r="C86" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="D86" s="58"/>
-      <c r="E86" s="59"/>
-      <c r="F86" s="59"/>
+      <c r="D86" s="61"/>
+      <c r="E86" s="60"/>
+      <c r="F86" s="60"/>
       <c r="G86" s="38" t="s">
         <v>33</v>
       </c>
@@ -12059,11 +12082,11 @@
       <c r="C87" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="D87" s="58" t="s">
+      <c r="D87" s="61" t="s">
         <v>348</v>
       </c>
-      <c r="E87" s="59"/>
-      <c r="F87" s="59" t="s">
+      <c r="E87" s="60"/>
+      <c r="F87" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G87" s="38" t="s">
@@ -12074,9 +12097,9 @@
       <c r="C88" s="34" t="s">
         <v>350</v>
       </c>
-      <c r="D88" s="58"/>
-      <c r="E88" s="59"/>
-      <c r="F88" s="59"/>
+      <c r="D88" s="61"/>
+      <c r="E88" s="60"/>
+      <c r="F88" s="60"/>
       <c r="G88" s="38" t="s">
         <v>33</v>
       </c>
@@ -12085,11 +12108,11 @@
       <c r="C89" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="D89" s="58" t="s">
+      <c r="D89" s="61" t="s">
         <v>361</v>
       </c>
-      <c r="E89" s="59"/>
-      <c r="F89" s="59" t="s">
+      <c r="E89" s="60"/>
+      <c r="F89" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G89" s="38" t="s">
@@ -12100,9 +12123,9 @@
       <c r="C90" s="34" t="s">
         <v>363</v>
       </c>
-      <c r="D90" s="58"/>
-      <c r="E90" s="59"/>
-      <c r="F90" s="59"/>
+      <c r="D90" s="61"/>
+      <c r="E90" s="60"/>
+      <c r="F90" s="60"/>
       <c r="G90" s="38" t="s">
         <v>33</v>
       </c>
@@ -12111,11 +12134,11 @@
       <c r="C91" s="34" t="s">
         <v>365</v>
       </c>
-      <c r="D91" s="58" t="s">
+      <c r="D91" s="61" t="s">
         <v>366</v>
       </c>
-      <c r="E91" s="59"/>
-      <c r="F91" s="59" t="s">
+      <c r="E91" s="60"/>
+      <c r="F91" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G91" s="38" t="s">
@@ -12126,9 +12149,9 @@
       <c r="C92" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="D92" s="58"/>
-      <c r="E92" s="59"/>
-      <c r="F92" s="59"/>
+      <c r="D92" s="61"/>
+      <c r="E92" s="60"/>
+      <c r="F92" s="60"/>
       <c r="G92" s="38" t="s">
         <v>33</v>
       </c>
@@ -12137,9 +12160,9 @@
       <c r="C93" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="D93" s="58"/>
-      <c r="E93" s="59"/>
-      <c r="F93" s="59"/>
+      <c r="D93" s="61"/>
+      <c r="E93" s="60"/>
+      <c r="F93" s="60"/>
       <c r="G93" s="38" t="s">
         <v>33</v>
       </c>
@@ -12148,11 +12171,11 @@
       <c r="C94" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="D94" s="58" t="s">
+      <c r="D94" s="61" t="s">
         <v>371</v>
       </c>
-      <c r="E94" s="59"/>
-      <c r="F94" s="59" t="s">
+      <c r="E94" s="60"/>
+      <c r="F94" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G94" s="38" t="s">
@@ -12163,9 +12186,9 @@
       <c r="C95" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="D95" s="58"/>
-      <c r="E95" s="59"/>
-      <c r="F95" s="59"/>
+      <c r="D95" s="61"/>
+      <c r="E95" s="60"/>
+      <c r="F95" s="60"/>
       <c r="G95" s="38" t="s">
         <v>33</v>
       </c>
@@ -12174,9 +12197,9 @@
       <c r="C96" s="34" t="s">
         <v>384</v>
       </c>
-      <c r="D96" s="58"/>
-      <c r="E96" s="59"/>
-      <c r="F96" s="59"/>
+      <c r="D96" s="61"/>
+      <c r="E96" s="60"/>
+      <c r="F96" s="60"/>
       <c r="G96" s="38" t="s">
         <v>33</v>
       </c>
@@ -12186,11 +12209,11 @@
       <c r="C97" s="36" t="s">
         <v>373</v>
       </c>
-      <c r="D97" s="58" t="s">
+      <c r="D97" s="61" t="s">
         <v>374</v>
       </c>
-      <c r="E97" s="59"/>
-      <c r="F97" s="59" t="s">
+      <c r="E97" s="60"/>
+      <c r="F97" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G97" s="38" t="s">
@@ -12202,9 +12225,9 @@
       <c r="C98" s="36" t="s">
         <v>380</v>
       </c>
-      <c r="D98" s="58"/>
-      <c r="E98" s="59"/>
-      <c r="F98" s="59"/>
+      <c r="D98" s="61"/>
+      <c r="E98" s="60"/>
+      <c r="F98" s="60"/>
       <c r="G98" s="38" t="s">
         <v>33</v>
       </c>
@@ -12214,9 +12237,9 @@
       <c r="C99" s="36" t="s">
         <v>386</v>
       </c>
-      <c r="D99" s="58"/>
-      <c r="E99" s="59"/>
-      <c r="F99" s="59"/>
+      <c r="D99" s="61"/>
+      <c r="E99" s="60"/>
+      <c r="F99" s="60"/>
       <c r="G99" s="38" t="s">
         <v>33</v>
       </c>
@@ -12229,11 +12252,11 @@
       <c r="C100" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="D100" s="58" t="s">
+      <c r="D100" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="E100" s="59"/>
-      <c r="F100" s="59" t="s">
+      <c r="E100" s="60"/>
+      <c r="F100" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G100" s="38" t="s">
@@ -12245,9 +12268,9 @@
       <c r="C101" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="D101" s="58"/>
-      <c r="E101" s="59"/>
-      <c r="F101" s="59"/>
+      <c r="D101" s="61"/>
+      <c r="E101" s="60"/>
+      <c r="F101" s="60"/>
       <c r="G101" s="38" t="s">
         <v>33</v>
       </c>
@@ -12256,11 +12279,11 @@
       <c r="C102" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="D102" s="58" t="s">
+      <c r="D102" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="E102" s="59"/>
-      <c r="F102" s="59" t="s">
+      <c r="E102" s="60"/>
+      <c r="F102" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G102" s="38" t="s">
@@ -12271,9 +12294,9 @@
       <c r="C103" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="D103" s="58"/>
-      <c r="E103" s="59"/>
-      <c r="F103" s="59"/>
+      <c r="D103" s="61"/>
+      <c r="E103" s="60"/>
+      <c r="F103" s="60"/>
       <c r="G103" s="38" t="s">
         <v>33</v>
       </c>
@@ -12282,9 +12305,9 @@
       <c r="C104" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="D104" s="58"/>
-      <c r="E104" s="59"/>
-      <c r="F104" s="59"/>
+      <c r="D104" s="61"/>
+      <c r="E104" s="60"/>
+      <c r="F104" s="60"/>
       <c r="G104" s="38" t="s">
         <v>33</v>
       </c>
@@ -12293,11 +12316,11 @@
       <c r="C105" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="D105" s="58" t="s">
+      <c r="D105" s="61" t="s">
         <v>119</v>
       </c>
-      <c r="E105" s="59"/>
-      <c r="F105" s="59" t="s">
+      <c r="E105" s="60"/>
+      <c r="F105" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G105" s="38" t="s">
@@ -12308,9 +12331,9 @@
       <c r="C106" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="D106" s="58"/>
-      <c r="E106" s="59"/>
-      <c r="F106" s="59"/>
+      <c r="D106" s="61"/>
+      <c r="E106" s="60"/>
+      <c r="F106" s="60"/>
       <c r="G106" s="38" t="s">
         <v>33</v>
       </c>
@@ -12319,11 +12342,11 @@
       <c r="C107" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="D107" s="58" t="s">
+      <c r="D107" s="61" t="s">
         <v>124</v>
       </c>
-      <c r="E107" s="59"/>
-      <c r="F107" s="59" t="s">
+      <c r="E107" s="60"/>
+      <c r="F107" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G107" s="38" t="s">
@@ -12334,9 +12357,9 @@
       <c r="C108" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="D108" s="58"/>
-      <c r="E108" s="59"/>
-      <c r="F108" s="59"/>
+      <c r="D108" s="61"/>
+      <c r="E108" s="60"/>
+      <c r="F108" s="60"/>
       <c r="G108" s="38" t="s">
         <v>33</v>
       </c>
@@ -12345,9 +12368,9 @@
       <c r="C109" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="D109" s="58"/>
-      <c r="E109" s="59"/>
-      <c r="F109" s="59"/>
+      <c r="D109" s="61"/>
+      <c r="E109" s="60"/>
+      <c r="F109" s="60"/>
       <c r="G109" s="38" t="s">
         <v>33</v>
       </c>
@@ -12356,11 +12379,11 @@
       <c r="C110" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="D110" s="58" t="s">
+      <c r="D110" s="61" t="s">
         <v>131</v>
       </c>
-      <c r="E110" s="59"/>
-      <c r="F110" s="59" t="s">
+      <c r="E110" s="60"/>
+      <c r="F110" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G110" s="38" t="s">
@@ -12371,9 +12394,9 @@
       <c r="C111" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="D111" s="58"/>
-      <c r="E111" s="59"/>
-      <c r="F111" s="59"/>
+      <c r="D111" s="61"/>
+      <c r="E111" s="60"/>
+      <c r="F111" s="60"/>
       <c r="G111" s="38" t="s">
         <v>33</v>
       </c>
@@ -12382,9 +12405,9 @@
       <c r="C112" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="D112" s="58"/>
-      <c r="E112" s="59"/>
-      <c r="F112" s="59"/>
+      <c r="D112" s="61"/>
+      <c r="E112" s="60"/>
+      <c r="F112" s="60"/>
       <c r="G112" s="38" t="s">
         <v>33</v>
       </c>
@@ -12393,11 +12416,11 @@
       <c r="C113" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="D113" s="58" t="s">
+      <c r="D113" s="61" t="s">
         <v>159</v>
       </c>
-      <c r="E113" s="59"/>
-      <c r="F113" s="59" t="s">
+      <c r="E113" s="60"/>
+      <c r="F113" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G113" s="38" t="s">
@@ -12408,9 +12431,9 @@
       <c r="C114" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="D114" s="58"/>
-      <c r="E114" s="59"/>
-      <c r="F114" s="59"/>
+      <c r="D114" s="61"/>
+      <c r="E114" s="60"/>
+      <c r="F114" s="60"/>
       <c r="G114" s="38" t="s">
         <v>33</v>
       </c>
@@ -12419,11 +12442,11 @@
       <c r="C115" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="D115" s="58" t="s">
+      <c r="D115" s="61" t="s">
         <v>164</v>
       </c>
-      <c r="E115" s="59"/>
-      <c r="F115" s="59" t="s">
+      <c r="E115" s="60"/>
+      <c r="F115" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G115" s="38" t="s">
@@ -12434,9 +12457,9 @@
       <c r="C116" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="D116" s="58"/>
-      <c r="E116" s="59"/>
-      <c r="F116" s="59"/>
+      <c r="D116" s="61"/>
+      <c r="E116" s="60"/>
+      <c r="F116" s="60"/>
       <c r="G116" s="38" t="s">
         <v>33</v>
       </c>
@@ -12445,9 +12468,9 @@
       <c r="C117" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="D117" s="58"/>
-      <c r="E117" s="59"/>
-      <c r="F117" s="59"/>
+      <c r="D117" s="61"/>
+      <c r="E117" s="60"/>
+      <c r="F117" s="60"/>
       <c r="G117" s="38" t="s">
         <v>33</v>
       </c>
@@ -12456,11 +12479,11 @@
       <c r="C118" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="D118" s="58" t="s">
+      <c r="D118" s="61" t="s">
         <v>179</v>
       </c>
-      <c r="E118" s="59"/>
-      <c r="F118" s="59" t="s">
+      <c r="E118" s="60"/>
+      <c r="F118" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G118" s="38" t="s">
@@ -12471,9 +12494,9 @@
       <c r="C119" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="D119" s="58"/>
-      <c r="E119" s="59"/>
-      <c r="F119" s="59"/>
+      <c r="D119" s="61"/>
+      <c r="E119" s="60"/>
+      <c r="F119" s="60"/>
       <c r="G119" s="38" t="s">
         <v>33</v>
       </c>
@@ -12482,9 +12505,9 @@
       <c r="C120" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="D120" s="58"/>
-      <c r="E120" s="59"/>
-      <c r="F120" s="59"/>
+      <c r="D120" s="61"/>
+      <c r="E120" s="60"/>
+      <c r="F120" s="60"/>
       <c r="G120" s="38" t="s">
         <v>33</v>
       </c>
@@ -12493,11 +12516,11 @@
       <c r="C121" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="D121" s="58" t="s">
+      <c r="D121" s="61" t="s">
         <v>186</v>
       </c>
-      <c r="E121" s="59"/>
-      <c r="F121" s="59" t="s">
+      <c r="E121" s="60"/>
+      <c r="F121" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G121" s="38" t="s">
@@ -12511,9 +12534,9 @@
       <c r="C122" s="34" t="s">
         <v>188</v>
       </c>
-      <c r="D122" s="58"/>
-      <c r="E122" s="59"/>
-      <c r="F122" s="59"/>
+      <c r="D122" s="61"/>
+      <c r="E122" s="60"/>
+      <c r="F122" s="60"/>
       <c r="G122" s="38" t="s">
         <v>33</v>
       </c>
@@ -12525,11 +12548,11 @@
       <c r="C123" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="D123" s="58" t="s">
+      <c r="D123" s="61" t="s">
         <v>195</v>
       </c>
-      <c r="E123" s="59"/>
-      <c r="F123" s="59" t="s">
+      <c r="E123" s="60"/>
+      <c r="F123" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G123" s="38" t="s">
@@ -12543,9 +12566,9 @@
       <c r="C124" s="34" t="s">
         <v>197</v>
       </c>
-      <c r="D124" s="58"/>
-      <c r="E124" s="59"/>
-      <c r="F124" s="59"/>
+      <c r="D124" s="61"/>
+      <c r="E124" s="60"/>
+      <c r="F124" s="60"/>
       <c r="G124" s="38" t="s">
         <v>33</v>
       </c>
@@ -12557,11 +12580,11 @@
       <c r="C125" s="34" t="s">
         <v>199</v>
       </c>
-      <c r="D125" s="58" t="s">
+      <c r="D125" s="61" t="s">
         <v>200</v>
       </c>
-      <c r="E125" s="59"/>
-      <c r="F125" s="59" t="s">
+      <c r="E125" s="60"/>
+      <c r="F125" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G125" s="38" t="s">
@@ -12575,9 +12598,9 @@
       <c r="C126" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="D126" s="58"/>
-      <c r="E126" s="59"/>
-      <c r="F126" s="59"/>
+      <c r="D126" s="61"/>
+      <c r="E126" s="60"/>
+      <c r="F126" s="60"/>
       <c r="G126" s="38" t="s">
         <v>33</v>
       </c>
@@ -12589,11 +12612,11 @@
       <c r="C127" s="34" t="s">
         <v>210</v>
       </c>
-      <c r="D127" s="58" t="s">
+      <c r="D127" s="61" t="s">
         <v>211</v>
       </c>
-      <c r="E127" s="59"/>
-      <c r="F127" s="59" t="s">
+      <c r="E127" s="60"/>
+      <c r="F127" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G127" s="38" t="s">
@@ -12607,9 +12630,9 @@
       <c r="C128" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="D128" s="58"/>
-      <c r="E128" s="59"/>
-      <c r="F128" s="59"/>
+      <c r="D128" s="61"/>
+      <c r="E128" s="60"/>
+      <c r="F128" s="60"/>
       <c r="G128" s="38" t="s">
         <v>33</v>
       </c>
@@ -12621,9 +12644,9 @@
       <c r="C129" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="D129" s="58"/>
-      <c r="E129" s="59"/>
-      <c r="F129" s="59"/>
+      <c r="D129" s="61"/>
+      <c r="E129" s="60"/>
+      <c r="F129" s="60"/>
       <c r="G129" s="38" t="s">
         <v>33</v>
       </c>
@@ -12635,11 +12658,11 @@
       <c r="C130" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="D130" s="58" t="s">
+      <c r="D130" s="61" t="s">
         <v>223</v>
       </c>
-      <c r="E130" s="59"/>
-      <c r="F130" s="59" t="s">
+      <c r="E130" s="60"/>
+      <c r="F130" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G130" s="38" t="s">
@@ -12653,9 +12676,9 @@
       <c r="C131" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="D131" s="58"/>
-      <c r="E131" s="59"/>
-      <c r="F131" s="59"/>
+      <c r="D131" s="61"/>
+      <c r="E131" s="60"/>
+      <c r="F131" s="60"/>
       <c r="G131" s="38" t="s">
         <v>33</v>
       </c>
@@ -12667,11 +12690,11 @@
       <c r="C132" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="D132" s="58" t="s">
+      <c r="D132" s="61" t="s">
         <v>228</v>
       </c>
-      <c r="E132" s="59"/>
-      <c r="F132" s="59" t="s">
+      <c r="E132" s="60"/>
+      <c r="F132" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G132" s="38" t="s">
@@ -12685,9 +12708,9 @@
       <c r="C133" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="D133" s="58"/>
-      <c r="E133" s="59"/>
-      <c r="F133" s="59"/>
+      <c r="D133" s="61"/>
+      <c r="E133" s="60"/>
+      <c r="F133" s="60"/>
       <c r="G133" s="38" t="s">
         <v>33</v>
       </c>
@@ -12699,9 +12722,9 @@
       <c r="C134" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="D134" s="58"/>
-      <c r="E134" s="59"/>
-      <c r="F134" s="59"/>
+      <c r="D134" s="61"/>
+      <c r="E134" s="60"/>
+      <c r="F134" s="60"/>
       <c r="G134" s="38" t="s">
         <v>33</v>
       </c>
@@ -12779,11 +12802,11 @@
       <c r="C139" s="34" t="s">
         <v>454</v>
       </c>
-      <c r="D139" s="58" t="s">
+      <c r="D139" s="61" t="s">
         <v>582</v>
       </c>
-      <c r="E139" s="59"/>
-      <c r="F139" s="59" t="s">
+      <c r="E139" s="60"/>
+      <c r="F139" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G139" s="38" t="s">
@@ -12794,9 +12817,9 @@
       <c r="C140" s="34" t="s">
         <v>457</v>
       </c>
-      <c r="D140" s="58"/>
-      <c r="E140" s="59"/>
-      <c r="F140" s="59"/>
+      <c r="D140" s="61"/>
+      <c r="E140" s="60"/>
+      <c r="F140" s="60"/>
       <c r="G140" s="38" t="s">
         <v>33</v>
       </c>
@@ -12805,11 +12828,11 @@
       <c r="C141" s="34" t="s">
         <v>459</v>
       </c>
-      <c r="D141" s="58" t="s">
+      <c r="D141" s="61" t="s">
         <v>460</v>
       </c>
-      <c r="E141" s="59"/>
-      <c r="F141" s="59" t="s">
+      <c r="E141" s="60"/>
+      <c r="F141" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G141" s="38" t="s">
@@ -12820,9 +12843,9 @@
       <c r="C142" s="34" t="s">
         <v>462</v>
       </c>
-      <c r="D142" s="58"/>
-      <c r="E142" s="59"/>
-      <c r="F142" s="59"/>
+      <c r="D142" s="61"/>
+      <c r="E142" s="60"/>
+      <c r="F142" s="60"/>
       <c r="G142" s="38" t="s">
         <v>33</v>
       </c>
@@ -12878,11 +12901,11 @@
       <c r="C146" s="34" t="s">
         <v>477</v>
       </c>
-      <c r="D146" s="58" t="s">
+      <c r="D146" s="61" t="s">
         <v>478</v>
       </c>
-      <c r="E146" s="59"/>
-      <c r="F146" s="59" t="s">
+      <c r="E146" s="60"/>
+      <c r="F146" s="60" t="s">
         <v>18</v>
       </c>
       <c r="G146" s="38" t="s">
@@ -12896,9 +12919,9 @@
       <c r="C147" s="35" t="s">
         <v>480</v>
       </c>
-      <c r="D147" s="62"/>
-      <c r="E147" s="66"/>
-      <c r="F147" s="66"/>
+      <c r="D147" s="63"/>
+      <c r="E147" s="65"/>
+      <c r="F147" s="65"/>
       <c r="G147" s="39" t="s">
         <v>33</v>
       </c>
@@ -12921,7 +12944,7 @@
       <c r="D149" s="36"/>
       <c r="E149" s="43">
         <f>COUNTBLANK(E2:E147)</f>
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F149" s="46"/>
       <c r="G149" s="36"/>
@@ -12934,7 +12957,7 @@
       <c r="D150" s="36"/>
       <c r="E150" s="43">
         <f>COUNTA(E2:E147)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F150" s="46"/>
       <c r="G150" s="36"/>
@@ -12962,6 +12985,183 @@
     </row>
   </sheetData>
   <mergeCells count="201">
+    <mergeCell ref="E89:E90"/>
+    <mergeCell ref="F87:F88"/>
+    <mergeCell ref="D91:D93"/>
+    <mergeCell ref="E91:E93"/>
+    <mergeCell ref="F91:F93"/>
+    <mergeCell ref="D94:D96"/>
+    <mergeCell ref="E94:E96"/>
+    <mergeCell ref="F94:F96"/>
+    <mergeCell ref="E51:E53"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="D71:D74"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="D83:D84"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="F51:F53"/>
+    <mergeCell ref="F89:F90"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="F67:F68"/>
+    <mergeCell ref="E71:E74"/>
+    <mergeCell ref="F71:F74"/>
+    <mergeCell ref="E64:E66"/>
+    <mergeCell ref="D87:D88"/>
+    <mergeCell ref="D89:D90"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="E83:E84"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="E87:E88"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="F77:F78"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="F81:F82"/>
+    <mergeCell ref="F83:F84"/>
+    <mergeCell ref="F85:F86"/>
+    <mergeCell ref="D43:D45"/>
+    <mergeCell ref="D46:D48"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D64:D66"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="F64:F66"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="F22:F25"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="E43:E45"/>
+    <mergeCell ref="F43:F45"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="G43:G45"/>
+    <mergeCell ref="G46:G48"/>
+    <mergeCell ref="D105:D106"/>
+    <mergeCell ref="E105:E106"/>
+    <mergeCell ref="F105:F106"/>
+    <mergeCell ref="D107:D109"/>
+    <mergeCell ref="E107:E109"/>
+    <mergeCell ref="F107:F109"/>
+    <mergeCell ref="D100:D101"/>
+    <mergeCell ref="E100:E101"/>
+    <mergeCell ref="F100:F101"/>
+    <mergeCell ref="D102:D104"/>
+    <mergeCell ref="E102:E104"/>
+    <mergeCell ref="F102:F104"/>
+    <mergeCell ref="D115:D117"/>
+    <mergeCell ref="E115:E117"/>
+    <mergeCell ref="F115:F117"/>
+    <mergeCell ref="D118:D120"/>
+    <mergeCell ref="E118:E120"/>
+    <mergeCell ref="F118:F120"/>
+    <mergeCell ref="D110:D112"/>
+    <mergeCell ref="E110:E112"/>
+    <mergeCell ref="F110:F112"/>
+    <mergeCell ref="D113:D114"/>
+    <mergeCell ref="E113:E114"/>
+    <mergeCell ref="F113:F114"/>
+    <mergeCell ref="D125:D126"/>
+    <mergeCell ref="E125:E126"/>
+    <mergeCell ref="F125:F126"/>
+    <mergeCell ref="D127:D129"/>
+    <mergeCell ref="E127:E129"/>
+    <mergeCell ref="F127:F129"/>
+    <mergeCell ref="D121:D122"/>
+    <mergeCell ref="E121:E122"/>
+    <mergeCell ref="F121:F122"/>
+    <mergeCell ref="D123:D124"/>
+    <mergeCell ref="E123:E124"/>
+    <mergeCell ref="F123:F124"/>
+    <mergeCell ref="D146:D147"/>
+    <mergeCell ref="E146:E147"/>
+    <mergeCell ref="F146:F147"/>
+    <mergeCell ref="D130:D131"/>
+    <mergeCell ref="E130:E131"/>
+    <mergeCell ref="F130:F131"/>
+    <mergeCell ref="D132:D134"/>
+    <mergeCell ref="E132:E134"/>
+    <mergeCell ref="F132:F134"/>
+    <mergeCell ref="D139:D140"/>
+    <mergeCell ref="D141:D142"/>
+    <mergeCell ref="F139:F140"/>
+    <mergeCell ref="F141:F142"/>
+    <mergeCell ref="E139:E140"/>
+    <mergeCell ref="E141:E142"/>
     <mergeCell ref="O5:O6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
@@ -12986,183 +13186,6 @@
     <mergeCell ref="D36:D37"/>
     <mergeCell ref="E36:E37"/>
     <mergeCell ref="F36:F37"/>
-    <mergeCell ref="D146:D147"/>
-    <mergeCell ref="E146:E147"/>
-    <mergeCell ref="F146:F147"/>
-    <mergeCell ref="D130:D131"/>
-    <mergeCell ref="E130:E131"/>
-    <mergeCell ref="F130:F131"/>
-    <mergeCell ref="D132:D134"/>
-    <mergeCell ref="E132:E134"/>
-    <mergeCell ref="F132:F134"/>
-    <mergeCell ref="D139:D140"/>
-    <mergeCell ref="D141:D142"/>
-    <mergeCell ref="F139:F140"/>
-    <mergeCell ref="F141:F142"/>
-    <mergeCell ref="E139:E140"/>
-    <mergeCell ref="E141:E142"/>
-    <mergeCell ref="D125:D126"/>
-    <mergeCell ref="E125:E126"/>
-    <mergeCell ref="F125:F126"/>
-    <mergeCell ref="D127:D129"/>
-    <mergeCell ref="E127:E129"/>
-    <mergeCell ref="F127:F129"/>
-    <mergeCell ref="D121:D122"/>
-    <mergeCell ref="E121:E122"/>
-    <mergeCell ref="F121:F122"/>
-    <mergeCell ref="D123:D124"/>
-    <mergeCell ref="E123:E124"/>
-    <mergeCell ref="F123:F124"/>
-    <mergeCell ref="D115:D117"/>
-    <mergeCell ref="E115:E117"/>
-    <mergeCell ref="F115:F117"/>
-    <mergeCell ref="D118:D120"/>
-    <mergeCell ref="E118:E120"/>
-    <mergeCell ref="F118:F120"/>
-    <mergeCell ref="D110:D112"/>
-    <mergeCell ref="E110:E112"/>
-    <mergeCell ref="F110:F112"/>
-    <mergeCell ref="D113:D114"/>
-    <mergeCell ref="E113:E114"/>
-    <mergeCell ref="F113:F114"/>
-    <mergeCell ref="D105:D106"/>
-    <mergeCell ref="E105:E106"/>
-    <mergeCell ref="F105:F106"/>
-    <mergeCell ref="D107:D109"/>
-    <mergeCell ref="E107:E109"/>
-    <mergeCell ref="F107:F109"/>
-    <mergeCell ref="D100:D101"/>
-    <mergeCell ref="E100:E101"/>
-    <mergeCell ref="F100:F101"/>
-    <mergeCell ref="D102:D104"/>
-    <mergeCell ref="E102:E104"/>
-    <mergeCell ref="F102:F104"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="G40:G42"/>
-    <mergeCell ref="E43:E45"/>
-    <mergeCell ref="F43:F45"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="G43:G45"/>
-    <mergeCell ref="G46:G48"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="F22:F25"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="D43:D45"/>
-    <mergeCell ref="D46:D48"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="D64:D66"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="F64:F66"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="F89:F90"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="F67:F68"/>
-    <mergeCell ref="E71:E74"/>
-    <mergeCell ref="F71:F74"/>
-    <mergeCell ref="E64:E66"/>
-    <mergeCell ref="D87:D88"/>
-    <mergeCell ref="D89:D90"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="E81:E82"/>
-    <mergeCell ref="E83:E84"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="E87:E88"/>
-    <mergeCell ref="F75:F76"/>
-    <mergeCell ref="F77:F78"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="F81:F82"/>
-    <mergeCell ref="F83:F84"/>
-    <mergeCell ref="F85:F86"/>
-    <mergeCell ref="F87:F88"/>
-    <mergeCell ref="D91:D93"/>
-    <mergeCell ref="E91:E93"/>
-    <mergeCell ref="F91:F93"/>
-    <mergeCell ref="D94:D96"/>
-    <mergeCell ref="E94:E96"/>
-    <mergeCell ref="F94:F96"/>
-    <mergeCell ref="E51:E53"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="F56:F57"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="D71:D74"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="D83:D84"/>
-    <mergeCell ref="D85:D86"/>
-    <mergeCell ref="F51:F53"/>
-    <mergeCell ref="E89:E90"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -13170,6 +13193,49 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C5067C9-23D2-4ADE-8DCB-648ED12E8246}">
+  <dimension ref="A2:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B3" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>594</v>
+      </c>
+      <c r="B4" t="s">
+        <v>595</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA06BA7C-CD17-4C21-9F28-C604AE25C8B9}">
   <dimension ref="A1:F25"/>
   <sheetViews>
@@ -13608,7 +13674,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A026136A-3463-4F46-9920-D2EEED3E1AFC}">
   <dimension ref="A1:X17"/>
   <sheetViews>
@@ -14115,7 +14181,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6DDA247-F6AE-445A-B41C-F6181C9C037C}">
   <dimension ref="A1:C44"/>
   <sheetViews>
@@ -14492,12 +14558,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABE3366-981D-4444-A865-F5BA56B32FED}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14538,32 +14604,20 @@
         <v>532</v>
       </c>
     </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>591</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEAE28352B96D64C95AA0D5E2FA62FAD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed183881d36ac1b5d7d67982eda510d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d161086-4829-409f-9f75-5bde88dcb151" xmlns:ns3="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="685f4fda20cf913d28bf77c13cd653dd" ns2:_="" ns3:_="">
     <xsd:import namespace="3d161086-4829-409f-9f75-5bde88dcb151"/>
@@ -14786,32 +14840,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C74AB5E7-5C87-4FF7-BF80-AB0EB6BD1D32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14828,4 +14877,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Initial structure of the forms test plan
</commit_message>
<xml_diff>
--- a/analysis/MEDS_Tables.xlsx
+++ b/analysis/MEDS_Tables.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="621" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2A0F485-AC58-4DDD-9A01-3DBB558E9E07}"/>
+  <xr:revisionPtr revIDLastSave="622" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDCA29DA-84DE-4DEF-A691-7BE442576755}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meds_tables" sheetId="1" r:id="rId1"/>
     <sheet name="csv" sheetId="6" r:id="rId2"/>
     <sheet name="tasks" sheetId="10" r:id="rId3"/>
     <sheet name="indexes candidates" sheetId="11" r:id="rId4"/>
-    <sheet name="form" sheetId="7" r:id="rId5"/>
-    <sheet name="serd" sheetId="8" r:id="rId6"/>
-    <sheet name="output" sheetId="9" r:id="rId7"/>
-    <sheet name="enhancements" sheetId="4" r:id="rId8"/>
+    <sheet name="test cases" sheetId="12" r:id="rId5"/>
+    <sheet name="test plan" sheetId="13" r:id="rId6"/>
+    <sheet name="form" sheetId="7" r:id="rId7"/>
+    <sheet name="serd" sheetId="8" r:id="rId8"/>
+    <sheet name="output" sheetId="9" r:id="rId9"/>
+    <sheet name="enhancements" sheetId="4" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">meds_tables!$A$1:$X$1</definedName>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2776" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2816" uniqueCount="637">
   <si>
     <t>Table</t>
   </si>
@@ -1845,6 +1847,270 @@
   </si>
   <si>
     <t>HI_CRUISE</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>Test Steps</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>Test case ID</t>
+  </si>
+  <si>
+    <t>Test case scenario</t>
+  </si>
+  <si>
+    <t>Test case</t>
+  </si>
+  <si>
+    <t>Pre-conditions</t>
+  </si>
+  <si>
+    <t>Test steps</t>
+  </si>
+  <si>
+    <t>Test data</t>
+  </si>
+  <si>
+    <t>Expected results</t>
+  </si>
+  <si>
+    <t>Post-condition</t>
+  </si>
+  <si>
+    <t>Actual results</t>
+  </si>
+  <si>
+    <t>Each of your test cases should have a unique identifier so that you can easily look one up (there will be many tests). Choose a naming convention and stick to it, whether you use ours or one of your own.</t>
+  </si>
+  <si>
+    <t>Here’s where you’ll choose one of the many test scenarios your developers and testers have created. A test case should only focus on one specific scenario at a time. This is where you’ll describe that test case scenario.</t>
+  </si>
+  <si>
+    <t>At this point, you’ll take the test scenario chosen and explain how it will be tested. In our example, we chose to test the login. Therefore, one test case is to use the correct user ID and correct password. Another scenario would be to use the incorrect user ID and correct password and so forth.</t>
+  </si>
+  <si>
+    <t>These are the conditions that need to be met before executing the test case. Again, in our example, the pre-conditions are having a valid user ID and password to test that functionality.</t>
+  </si>
+  <si>
+    <t>Here’s where you’ll list the actions needed for the test case scenario. Be sure to mention all the steps in as much detail as necessary and the order in which they should be executed. This should be done from the end-user’s perspective. Looking at our example on the template, those steps would be to enter the correct user ID and correct password and then click the login button.</t>
+  </si>
+  <si>
+    <t>To run the test case, you need to have the right data. In the case of our example, that’d be having the correct user ID and correct password to test the login function of the software.</t>
+  </si>
+  <si>
+    <t>This is where you note the result you expect to happen, which ideally is that the login works and the user is given access to the software. But you might not think the test will work in which case you’d write what you think will happen, perhaps an error message or nothing at all.</t>
+  </si>
+  <si>
+    <t>This is the condition that needs to happen for the case to be successfully executed. For example, the login works.</t>
+  </si>
+  <si>
+    <t>Of course, the actual results may be very different from what you expect as the post-condition of the case test. This is where you’ll put those actual results. It could be that the login worked, which is great. But if the login doesn’t work, you’ll need to detail what happened to mitigate the bug.</t>
+  </si>
+  <si>
+    <t>The test case will have one of two outcomes: pass or fail. If it passes, you can move to the next scenario. If it fails, then you’ll have to fix the problem and do another test case until it passes. Our template has a dropdown menu with a red failure or a green pass to indicate the status of the test case.</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Expected Results</t>
+  </si>
+  <si>
+    <t>Actual Results</t>
+  </si>
+  <si>
+    <t>Creating a new observation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking button </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Create and Create Another</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> should trigger form validations</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking button </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Create</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> should trigger form validations</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Button </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cancel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> should be enabled</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Button </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Create and Create Another</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> should be enabled</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Button </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Create</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> should be enabled</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicking button </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cancel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> should navigate back to </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Job Process</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page</t>
+    </r>
+  </si>
+  <si>
+    <t>A record can only be created if latitude degress, decimal minutes and cardinal point are informed</t>
+  </si>
+  <si>
+    <t>A record can only be created if longitude degress, decimal minutes and cardinal point are informed</t>
   </si>
 </sst>
 </file>
@@ -1854,7 +2120,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2013,6 +2279,14 @@
     <font>
       <sz val="20"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2574,7 +2848,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2696,46 +2970,49 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -10456,6 +10733,65 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABE3366-981D-4444-A865-F5BA56B32FED}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.42578125" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>525</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>527</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>529</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>531</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>591</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76451C41-9738-4BC1-978E-20A0DA8744C6}">
   <dimension ref="A1:F15"/>
@@ -10770,8 +11106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8FA477-9B46-4053-B7AD-310B8B9F2B30}">
   <dimension ref="A1:P150"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24:E25"/>
+    <sheetView tabSelected="1" topLeftCell="C94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G128" sqref="G128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10818,7 +11154,7 @@
       <c r="C2" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="63" t="s">
         <v>38</v>
       </c>
       <c r="E2" s="64" t="s">
@@ -10827,7 +11163,7 @@
       <c r="F2" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="66" t="s">
+      <c r="G2" s="65" t="s">
         <v>564</v>
       </c>
     </row>
@@ -10836,10 +11172,10 @@
       <c r="C3" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="61"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="68"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="62"/>
       <c r="K3" s="36"/>
       <c r="L3" s="36"/>
       <c r="M3" s="36"/>
@@ -10852,10 +11188,10 @@
       <c r="C4" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="61"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="68"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="62"/>
       <c r="K4" s="36"/>
       <c r="L4" s="36"/>
       <c r="M4" s="36"/>
@@ -10868,27 +11204,27 @@
       <c r="C5" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="61" t="s">
+      <c r="D5" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="60" t="s">
+      <c r="E5" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F5" s="60" t="s">
+      <c r="F5" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="68" t="s">
+      <c r="G5" s="62" t="s">
         <v>519</v>
       </c>
       <c r="K5" s="36"/>
       <c r="L5" s="47" t="s">
         <v>464</v>
       </c>
-      <c r="M5" s="59" t="s">
+      <c r="M5" s="70" t="s">
         <v>465</v>
       </c>
-      <c r="N5" s="60"/>
-      <c r="O5" s="58" t="s">
+      <c r="N5" s="59"/>
+      <c r="O5" s="69" t="s">
         <v>581</v>
       </c>
       <c r="P5" s="36"/>
@@ -10898,17 +11234,17 @@
       <c r="C6" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="61"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="68"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="62"/>
       <c r="K6" s="36"/>
       <c r="L6" s="47" t="s">
         <v>467</v>
       </c>
-      <c r="M6" s="59"/>
-      <c r="N6" s="60"/>
-      <c r="O6" s="58"/>
+      <c r="M6" s="70"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="69"/>
       <c r="P6" s="36"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
@@ -10916,16 +11252,16 @@
       <c r="C7" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="61" t="s">
+      <c r="D7" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="60" t="s">
+      <c r="E7" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="60" t="s">
+      <c r="F7" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="68" t="s">
+      <c r="G7" s="62" t="s">
         <v>80</v>
       </c>
       <c r="K7" s="36"/>
@@ -10940,10 +11276,10 @@
       <c r="C8" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="61"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="68"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="62"/>
       <c r="K8" s="36"/>
       <c r="L8" s="36"/>
       <c r="M8" s="36"/>
@@ -10956,16 +11292,16 @@
       <c r="C9" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="D9" s="61" t="s">
+      <c r="D9" s="58" t="s">
         <v>171</v>
       </c>
-      <c r="E9" s="60" t="s">
+      <c r="E9" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="60" t="s">
+      <c r="F9" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="68" t="s">
+      <c r="G9" s="62" t="s">
         <v>523</v>
       </c>
       <c r="J9" s="36"/>
@@ -10976,10 +11312,10 @@
       <c r="C10" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="D10" s="61"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="68"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="62"/>
       <c r="J10" s="36"/>
       <c r="K10" s="36"/>
     </row>
@@ -10988,10 +11324,10 @@
       <c r="C11" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="D11" s="61"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="68"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="62"/>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
     </row>
@@ -11000,16 +11336,16 @@
       <c r="C12" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="D12" s="61" t="s">
+      <c r="D12" s="58" t="s">
         <v>204</v>
       </c>
-      <c r="E12" s="60" t="s">
+      <c r="E12" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="60" t="s">
+      <c r="F12" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="68" t="s">
+      <c r="G12" s="62" t="s">
         <v>515</v>
       </c>
       <c r="J12" s="36"/>
@@ -11020,10 +11356,10 @@
       <c r="C13" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="D13" s="61"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="68"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="62"/>
       <c r="J13" s="36"/>
       <c r="K13" s="36"/>
     </row>
@@ -11032,16 +11368,16 @@
       <c r="C14" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="D14" s="61" t="s">
+      <c r="D14" s="58" t="s">
         <v>361</v>
       </c>
-      <c r="E14" s="60" t="s">
+      <c r="E14" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F14" s="60" t="s">
+      <c r="F14" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="68" t="s">
+      <c r="G14" s="62" t="s">
         <v>518</v>
       </c>
       <c r="J14" s="36"/>
@@ -11052,9 +11388,9 @@
       <c r="C15" s="35" t="s">
         <v>363</v>
       </c>
-      <c r="D15" s="63"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
       <c r="G15" s="67"/>
       <c r="J15" s="36"/>
       <c r="K15" s="36"/>
@@ -11063,7 +11399,7 @@
       <c r="C16" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="62" t="s">
+      <c r="D16" s="63" t="s">
         <v>71</v>
       </c>
       <c r="E16" s="64" t="s">
@@ -11072,7 +11408,7 @@
       <c r="F16" s="64" t="s">
         <v>567</v>
       </c>
-      <c r="G16" s="66" t="s">
+      <c r="G16" s="65" t="s">
         <v>73</v>
       </c>
       <c r="J16" s="36"/>
@@ -11082,10 +11418,10 @@
       <c r="C17" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="61"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="68"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="62"/>
       <c r="J17" s="36"/>
       <c r="K17" s="36"/>
     </row>
@@ -11093,16 +11429,16 @@
       <c r="C18" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="61" t="s">
+      <c r="D18" s="58" t="s">
         <v>105</v>
       </c>
-      <c r="E18" s="60" t="s">
+      <c r="E18" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F18" s="60" t="s">
+      <c r="F18" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G18" s="68" t="s">
+      <c r="G18" s="62" t="s">
         <v>524</v>
       </c>
       <c r="J18" s="36"/>
@@ -11112,10 +11448,10 @@
       <c r="C19" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="61"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="68"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="62"/>
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
     </row>
@@ -11123,16 +11459,16 @@
       <c r="C20" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="D20" s="61" t="s">
+      <c r="D20" s="58" t="s">
         <v>300</v>
       </c>
-      <c r="E20" s="60" t="s">
+      <c r="E20" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F20" s="60" t="s">
+      <c r="F20" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G20" s="68" t="s">
+      <c r="G20" s="62" t="s">
         <v>516</v>
       </c>
       <c r="J20" s="36"/>
@@ -11142,10 +11478,10 @@
       <c r="C21" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="D21" s="61"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="68"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="62"/>
       <c r="J21" s="36"/>
       <c r="K21" s="36"/>
     </row>
@@ -11153,16 +11489,16 @@
       <c r="C22" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="D22" s="61" t="s">
+      <c r="D22" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="E22" s="60" t="s">
+      <c r="E22" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F22" s="60" t="s">
+      <c r="F22" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G22" s="68" t="s">
+      <c r="G22" s="62" t="s">
         <v>521</v>
       </c>
       <c r="J22" s="36"/>
@@ -11172,10 +11508,10 @@
       <c r="C23" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="D23" s="61"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="68"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="62"/>
       <c r="J23" s="36"/>
       <c r="K23" s="36"/>
     </row>
@@ -11183,16 +11519,16 @@
       <c r="C24" s="34" t="s">
         <v>317</v>
       </c>
-      <c r="D24" s="61" t="s">
+      <c r="D24" s="58" t="s">
         <v>318</v>
       </c>
-      <c r="E24" s="60" t="s">
+      <c r="E24" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F24" s="60" t="s">
+      <c r="F24" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G24" s="68" t="s">
+      <c r="G24" s="62" t="s">
         <v>512</v>
       </c>
       <c r="J24" s="36"/>
@@ -11202,10 +11538,10 @@
       <c r="C25" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="D25" s="61"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="68"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="62"/>
       <c r="J25" s="36"/>
       <c r="K25" s="36"/>
     </row>
@@ -11213,16 +11549,16 @@
       <c r="C26" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="D26" s="69" t="s">
+      <c r="D26" s="60" t="s">
         <v>323</v>
       </c>
-      <c r="E26" s="70" t="s">
+      <c r="E26" s="68" t="s">
         <v>81</v>
       </c>
-      <c r="F26" s="60" t="s">
+      <c r="F26" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G26" s="68" t="s">
+      <c r="G26" s="62" t="s">
         <v>517</v>
       </c>
       <c r="J26" s="36"/>
@@ -11232,25 +11568,25 @@
       <c r="C27" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="D27" s="69"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="68"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="62"/>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C28" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="D28" s="61" t="s">
+      <c r="D28" s="58" t="s">
         <v>328</v>
       </c>
-      <c r="E28" s="60" t="s">
+      <c r="E28" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F28" s="60" t="s">
+      <c r="F28" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G28" s="68" t="s">
+      <c r="G28" s="62" t="s">
         <v>508</v>
       </c>
     </row>
@@ -11258,25 +11594,25 @@
       <c r="C29" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="D29" s="61"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="68"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="62"/>
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C30" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="D30" s="61" t="s">
+      <c r="D30" s="58" t="s">
         <v>333</v>
       </c>
-      <c r="E30" s="60" t="s">
+      <c r="E30" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F30" s="60" t="s">
+      <c r="F30" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G30" s="68" t="s">
+      <c r="G30" s="62" t="s">
         <v>510</v>
       </c>
     </row>
@@ -11284,25 +11620,25 @@
       <c r="C31" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="D31" s="61"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="68"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="62"/>
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="D32" s="61" t="s">
+      <c r="D32" s="58" t="s">
         <v>338</v>
       </c>
-      <c r="E32" s="60" t="s">
+      <c r="E32" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F32" s="60" t="s">
+      <c r="F32" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G32" s="68" t="s">
+      <c r="G32" s="62" t="s">
         <v>511</v>
       </c>
     </row>
@@ -11310,25 +11646,25 @@
       <c r="C33" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="D33" s="61"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="60"/>
-      <c r="G33" s="68"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="62"/>
     </row>
     <row r="34" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C34" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="D34" s="61" t="s">
+      <c r="D34" s="58" t="s">
         <v>343</v>
       </c>
-      <c r="E34" s="60" t="s">
+      <c r="E34" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F34" s="60" t="s">
+      <c r="F34" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G34" s="68" t="s">
+      <c r="G34" s="62" t="s">
         <v>509</v>
       </c>
     </row>
@@ -11336,25 +11672,25 @@
       <c r="C35" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="D35" s="61"/>
-      <c r="E35" s="60"/>
-      <c r="F35" s="60"/>
-      <c r="G35" s="68"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="62"/>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C36" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="D36" s="61" t="s">
+      <c r="D36" s="58" t="s">
         <v>348</v>
       </c>
-      <c r="E36" s="60" t="s">
+      <c r="E36" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F36" s="60" t="s">
+      <c r="F36" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="G36" s="68" t="s">
+      <c r="G36" s="62" t="s">
         <v>520</v>
       </c>
     </row>
@@ -11362,16 +11698,16 @@
       <c r="C37" s="35" t="s">
         <v>350</v>
       </c>
-      <c r="D37" s="63"/>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="67"/>
     </row>
     <row r="38" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C38" s="33" t="s">
         <v>365</v>
       </c>
-      <c r="D38" s="62" t="s">
+      <c r="D38" s="63" t="s">
         <v>366</v>
       </c>
       <c r="E38" s="64" t="s">
@@ -11380,7 +11716,7 @@
       <c r="F38" s="64" t="s">
         <v>369</v>
       </c>
-      <c r="G38" s="66" t="s">
+      <c r="G38" s="65" t="s">
         <v>514</v>
       </c>
     </row>
@@ -11388,34 +11724,34 @@
       <c r="C39" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="D39" s="61"/>
-      <c r="E39" s="60"/>
-      <c r="F39" s="60"/>
-      <c r="G39" s="68"/>
+      <c r="D39" s="58"/>
+      <c r="E39" s="59"/>
+      <c r="F39" s="59"/>
+      <c r="G39" s="62"/>
     </row>
     <row r="40" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C40" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="D40" s="61"/>
-      <c r="E40" s="60"/>
-      <c r="F40" s="60"/>
-      <c r="G40" s="68"/>
+      <c r="D40" s="58"/>
+      <c r="E40" s="59"/>
+      <c r="F40" s="59"/>
+      <c r="G40" s="62"/>
     </row>
     <row r="41" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C41" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="D41" s="61" t="s">
+      <c r="D41" s="58" t="s">
         <v>371</v>
       </c>
-      <c r="E41" s="60" t="s">
+      <c r="E41" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F41" s="60" t="s">
+      <c r="F41" s="59" t="s">
         <v>369</v>
       </c>
-      <c r="G41" s="68" t="s">
+      <c r="G41" s="62" t="s">
         <v>513</v>
       </c>
     </row>
@@ -11423,34 +11759,34 @@
       <c r="C42" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="D42" s="61"/>
-      <c r="E42" s="60"/>
-      <c r="F42" s="60"/>
-      <c r="G42" s="68"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="59"/>
+      <c r="G42" s="62"/>
     </row>
     <row r="43" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C43" s="34" t="s">
         <v>384</v>
       </c>
-      <c r="D43" s="61"/>
-      <c r="E43" s="60"/>
-      <c r="F43" s="60"/>
-      <c r="G43" s="68"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="59"/>
+      <c r="F43" s="59"/>
+      <c r="G43" s="62"/>
     </row>
     <row r="44" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C44" s="34" t="s">
         <v>373</v>
       </c>
-      <c r="D44" s="61" t="s">
+      <c r="D44" s="58" t="s">
         <v>374</v>
       </c>
-      <c r="E44" s="60" t="s">
+      <c r="E44" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F44" s="60" t="s">
+      <c r="F44" s="59" t="s">
         <v>369</v>
       </c>
-      <c r="G44" s="68" t="s">
+      <c r="G44" s="62" t="s">
         <v>522</v>
       </c>
     </row>
@@ -11458,18 +11794,18 @@
       <c r="C45" s="34" t="s">
         <v>380</v>
       </c>
-      <c r="D45" s="61"/>
-      <c r="E45" s="60"/>
-      <c r="F45" s="60"/>
-      <c r="G45" s="68"/>
+      <c r="D45" s="58"/>
+      <c r="E45" s="59"/>
+      <c r="F45" s="59"/>
+      <c r="G45" s="62"/>
     </row>
     <row r="46" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C46" s="35" t="s">
         <v>386</v>
       </c>
-      <c r="D46" s="63"/>
-      <c r="E46" s="65"/>
-      <c r="F46" s="65"/>
+      <c r="D46" s="61"/>
+      <c r="E46" s="66"/>
+      <c r="F46" s="66"/>
       <c r="G46" s="67"/>
       <c r="J46" s="36"/>
       <c r="K46" s="36"/>
@@ -11480,14 +11816,14 @@
       <c r="C47" s="33" t="s">
         <v>464</v>
       </c>
-      <c r="D47" s="62" t="s">
+      <c r="D47" s="63" t="s">
         <v>465</v>
       </c>
       <c r="E47" s="64"/>
       <c r="F47" s="64" t="s">
         <v>584</v>
       </c>
-      <c r="G47" s="66" t="s">
+      <c r="G47" s="65" t="s">
         <v>585</v>
       </c>
       <c r="J47" s="36"/>
@@ -11499,9 +11835,9 @@
       <c r="C48" s="35" t="s">
         <v>467</v>
       </c>
-      <c r="D48" s="63"/>
-      <c r="E48" s="65"/>
-      <c r="F48" s="65"/>
+      <c r="D48" s="61"/>
+      <c r="E48" s="66"/>
+      <c r="F48" s="66"/>
       <c r="G48" s="67"/>
       <c r="J48" s="36"/>
       <c r="K48" s="36"/>
@@ -11512,11 +11848,11 @@
       <c r="C49" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="D49" s="61" t="s">
+      <c r="D49" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="E49" s="60"/>
-      <c r="F49" s="60" t="s">
+      <c r="E49" s="59"/>
+      <c r="F49" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G49" s="38" t="s">
@@ -11531,9 +11867,9 @@
       <c r="C50" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D50" s="61"/>
-      <c r="E50" s="60"/>
-      <c r="F50" s="60"/>
+      <c r="D50" s="58"/>
+      <c r="E50" s="59"/>
+      <c r="F50" s="59"/>
       <c r="G50" s="38" t="s">
         <v>33</v>
       </c>
@@ -11546,9 +11882,9 @@
       <c r="C51" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D51" s="61"/>
-      <c r="E51" s="60"/>
-      <c r="F51" s="60"/>
+      <c r="D51" s="58"/>
+      <c r="E51" s="59"/>
+      <c r="F51" s="59"/>
       <c r="G51" s="38" t="s">
         <v>33</v>
       </c>
@@ -11561,11 +11897,11 @@
       <c r="C52" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="D52" s="61" t="s">
+      <c r="D52" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="E52" s="60"/>
-      <c r="F52" s="60" t="s">
+      <c r="E52" s="59"/>
+      <c r="F52" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G52" s="38" t="s">
@@ -11580,9 +11916,9 @@
       <c r="C53" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D53" s="61"/>
-      <c r="E53" s="60"/>
-      <c r="F53" s="60"/>
+      <c r="D53" s="58"/>
+      <c r="E53" s="59"/>
+      <c r="F53" s="59"/>
       <c r="G53" s="38" t="s">
         <v>33</v>
       </c>
@@ -11595,11 +11931,11 @@
       <c r="C54" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D54" s="61" t="s">
+      <c r="D54" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="E54" s="60"/>
-      <c r="F54" s="60" t="s">
+      <c r="E54" s="59"/>
+      <c r="F54" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G54" s="38" t="s">
@@ -11614,9 +11950,9 @@
       <c r="C55" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D55" s="61"/>
-      <c r="E55" s="60"/>
-      <c r="F55" s="60"/>
+      <c r="D55" s="58"/>
+      <c r="E55" s="59"/>
+      <c r="F55" s="59"/>
       <c r="G55" s="38" t="s">
         <v>33</v>
       </c>
@@ -11629,11 +11965,11 @@
       <c r="C56" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D56" s="61" t="s">
+      <c r="D56" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="E56" s="60"/>
-      <c r="F56" s="60" t="s">
+      <c r="E56" s="59"/>
+      <c r="F56" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G56" s="38" t="s">
@@ -11648,9 +11984,9 @@
       <c r="C57" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D57" s="61"/>
-      <c r="E57" s="60"/>
-      <c r="F57" s="60"/>
+      <c r="D57" s="58"/>
+      <c r="E57" s="59"/>
+      <c r="F57" s="59"/>
       <c r="G57" s="38" t="s">
         <v>33</v>
       </c>
@@ -11663,11 +11999,11 @@
       <c r="C58" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="D58" s="61" t="s">
+      <c r="D58" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="E58" s="60"/>
-      <c r="F58" s="60" t="s">
+      <c r="E58" s="59"/>
+      <c r="F58" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G58" s="38" t="s">
@@ -11682,9 +12018,9 @@
       <c r="C59" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D59" s="61"/>
-      <c r="E59" s="60"/>
-      <c r="F59" s="60"/>
+      <c r="D59" s="58"/>
+      <c r="E59" s="59"/>
+      <c r="F59" s="59"/>
       <c r="G59" s="38" t="s">
         <v>33</v>
       </c>
@@ -11697,11 +12033,11 @@
       <c r="C60" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D60" s="61" t="s">
+      <c r="D60" s="58" t="s">
         <v>105</v>
       </c>
-      <c r="E60" s="60"/>
-      <c r="F60" s="60" t="s">
+      <c r="E60" s="59"/>
+      <c r="F60" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G60" s="38" t="s">
@@ -11716,9 +12052,9 @@
       <c r="C61" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D61" s="61"/>
-      <c r="E61" s="60"/>
-      <c r="F61" s="60"/>
+      <c r="D61" s="58"/>
+      <c r="E61" s="59"/>
+      <c r="F61" s="59"/>
       <c r="G61" s="38" t="s">
         <v>33</v>
       </c>
@@ -11731,11 +12067,11 @@
       <c r="C62" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="D62" s="61" t="s">
+      <c r="D62" s="58" t="s">
         <v>171</v>
       </c>
-      <c r="E62" s="60"/>
-      <c r="F62" s="60" t="s">
+      <c r="E62" s="59"/>
+      <c r="F62" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G62" s="38" t="s">
@@ -11750,9 +12086,9 @@
       <c r="C63" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="D63" s="61"/>
-      <c r="E63" s="60"/>
-      <c r="F63" s="60"/>
+      <c r="D63" s="58"/>
+      <c r="E63" s="59"/>
+      <c r="F63" s="59"/>
       <c r="G63" s="38" t="s">
         <v>33</v>
       </c>
@@ -11765,9 +12101,9 @@
       <c r="C64" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="D64" s="61"/>
-      <c r="E64" s="60"/>
-      <c r="F64" s="60"/>
+      <c r="D64" s="58"/>
+      <c r="E64" s="59"/>
+      <c r="F64" s="59"/>
       <c r="G64" s="38" t="s">
         <v>33</v>
       </c>
@@ -11780,11 +12116,11 @@
       <c r="C65" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="D65" s="61" t="s">
+      <c r="D65" s="58" t="s">
         <v>204</v>
       </c>
-      <c r="E65" s="60"/>
-      <c r="F65" s="60" t="s">
+      <c r="E65" s="59"/>
+      <c r="F65" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G65" s="38" t="s">
@@ -11799,9 +12135,9 @@
       <c r="C66" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="D66" s="61"/>
-      <c r="E66" s="60"/>
-      <c r="F66" s="60"/>
+      <c r="D66" s="58"/>
+      <c r="E66" s="59"/>
+      <c r="F66" s="59"/>
       <c r="G66" s="38" t="s">
         <v>33</v>
       </c>
@@ -11814,11 +12150,11 @@
       <c r="C67" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="D67" s="61" t="s">
+      <c r="D67" s="58" t="s">
         <v>300</v>
       </c>
-      <c r="E67" s="60"/>
-      <c r="F67" s="60" t="s">
+      <c r="E67" s="59"/>
+      <c r="F67" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G67" s="38" t="s">
@@ -11833,9 +12169,9 @@
       <c r="C68" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="D68" s="61"/>
-      <c r="E68" s="60"/>
-      <c r="F68" s="60"/>
+      <c r="D68" s="58"/>
+      <c r="E68" s="59"/>
+      <c r="F68" s="59"/>
       <c r="G68" s="38" t="s">
         <v>33</v>
       </c>
@@ -11848,11 +12184,11 @@
       <c r="C69" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="D69" s="61" t="s">
+      <c r="D69" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="E69" s="60"/>
-      <c r="F69" s="60" t="s">
+      <c r="E69" s="59"/>
+      <c r="F69" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G69" s="38" t="s">
@@ -11867,9 +12203,9 @@
       <c r="C70" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="D70" s="61"/>
-      <c r="E70" s="60"/>
-      <c r="F70" s="60"/>
+      <c r="D70" s="58"/>
+      <c r="E70" s="59"/>
+      <c r="F70" s="59"/>
       <c r="G70" s="38" t="s">
         <v>33</v>
       </c>
@@ -11882,9 +12218,9 @@
       <c r="C71" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="D71" s="61"/>
-      <c r="E71" s="60"/>
-      <c r="F71" s="60"/>
+      <c r="D71" s="58"/>
+      <c r="E71" s="59"/>
+      <c r="F71" s="59"/>
       <c r="G71" s="38" t="s">
         <v>33</v>
       </c>
@@ -11897,9 +12233,9 @@
       <c r="C72" s="34" t="s">
         <v>311</v>
       </c>
-      <c r="D72" s="61"/>
-      <c r="E72" s="60"/>
-      <c r="F72" s="60"/>
+      <c r="D72" s="58"/>
+      <c r="E72" s="59"/>
+      <c r="F72" s="59"/>
       <c r="G72" s="38" t="s">
         <v>33</v>
       </c>
@@ -11912,11 +12248,11 @@
       <c r="C73" s="34" t="s">
         <v>317</v>
       </c>
-      <c r="D73" s="61" t="s">
+      <c r="D73" s="58" t="s">
         <v>318</v>
       </c>
-      <c r="E73" s="60"/>
-      <c r="F73" s="60" t="s">
+      <c r="E73" s="59"/>
+      <c r="F73" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G73" s="38" t="s">
@@ -11931,9 +12267,9 @@
       <c r="C74" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="D74" s="61"/>
-      <c r="E74" s="60"/>
-      <c r="F74" s="60"/>
+      <c r="D74" s="58"/>
+      <c r="E74" s="59"/>
+      <c r="F74" s="59"/>
       <c r="G74" s="38" t="s">
         <v>33</v>
       </c>
@@ -11946,11 +12282,11 @@
       <c r="C75" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="D75" s="69" t="s">
+      <c r="D75" s="60" t="s">
         <v>323</v>
       </c>
-      <c r="E75" s="60"/>
-      <c r="F75" s="60" t="s">
+      <c r="E75" s="59"/>
+      <c r="F75" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G75" s="38" t="s">
@@ -11965,9 +12301,9 @@
       <c r="C76" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="D76" s="69"/>
-      <c r="E76" s="60"/>
-      <c r="F76" s="60"/>
+      <c r="D76" s="60"/>
+      <c r="E76" s="59"/>
+      <c r="F76" s="59"/>
       <c r="G76" s="38" t="s">
         <v>33</v>
       </c>
@@ -11976,11 +12312,11 @@
       <c r="C77" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="D77" s="61" t="s">
+      <c r="D77" s="58" t="s">
         <v>328</v>
       </c>
-      <c r="E77" s="60"/>
-      <c r="F77" s="60" t="s">
+      <c r="E77" s="59"/>
+      <c r="F77" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G77" s="38" t="s">
@@ -11991,9 +12327,9 @@
       <c r="C78" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="D78" s="61"/>
-      <c r="E78" s="60"/>
-      <c r="F78" s="60"/>
+      <c r="D78" s="58"/>
+      <c r="E78" s="59"/>
+      <c r="F78" s="59"/>
       <c r="G78" s="38" t="s">
         <v>33</v>
       </c>
@@ -12002,11 +12338,11 @@
       <c r="C79" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="D79" s="61" t="s">
+      <c r="D79" s="58" t="s">
         <v>333</v>
       </c>
-      <c r="E79" s="60"/>
-      <c r="F79" s="60" t="s">
+      <c r="E79" s="59"/>
+      <c r="F79" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G79" s="38" t="s">
@@ -12017,9 +12353,9 @@
       <c r="C80" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="D80" s="61"/>
-      <c r="E80" s="60"/>
-      <c r="F80" s="60"/>
+      <c r="D80" s="58"/>
+      <c r="E80" s="59"/>
+      <c r="F80" s="59"/>
       <c r="G80" s="38" t="s">
         <v>33</v>
       </c>
@@ -12028,11 +12364,11 @@
       <c r="C81" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="D81" s="61" t="s">
+      <c r="D81" s="58" t="s">
         <v>338</v>
       </c>
-      <c r="E81" s="60"/>
-      <c r="F81" s="60" t="s">
+      <c r="E81" s="59"/>
+      <c r="F81" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G81" s="38" t="s">
@@ -12043,9 +12379,9 @@
       <c r="C82" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="D82" s="61"/>
-      <c r="E82" s="60"/>
-      <c r="F82" s="60"/>
+      <c r="D82" s="58"/>
+      <c r="E82" s="59"/>
+      <c r="F82" s="59"/>
       <c r="G82" s="38" t="s">
         <v>33</v>
       </c>
@@ -12054,11 +12390,11 @@
       <c r="C83" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="D83" s="61" t="s">
+      <c r="D83" s="58" t="s">
         <v>343</v>
       </c>
-      <c r="E83" s="60"/>
-      <c r="F83" s="60" t="s">
+      <c r="E83" s="59"/>
+      <c r="F83" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G83" s="38" t="s">
@@ -12069,9 +12405,9 @@
       <c r="C84" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="D84" s="61"/>
-      <c r="E84" s="60"/>
-      <c r="F84" s="60"/>
+      <c r="D84" s="58"/>
+      <c r="E84" s="59"/>
+      <c r="F84" s="59"/>
       <c r="G84" s="38" t="s">
         <v>33</v>
       </c>
@@ -12080,11 +12416,11 @@
       <c r="C85" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="D85" s="61" t="s">
+      <c r="D85" s="58" t="s">
         <v>348</v>
       </c>
-      <c r="E85" s="60"/>
-      <c r="F85" s="60" t="s">
+      <c r="E85" s="59"/>
+      <c r="F85" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G85" s="38" t="s">
@@ -12095,9 +12431,9 @@
       <c r="C86" s="34" t="s">
         <v>350</v>
       </c>
-      <c r="D86" s="61"/>
-      <c r="E86" s="60"/>
-      <c r="F86" s="60"/>
+      <c r="D86" s="58"/>
+      <c r="E86" s="59"/>
+      <c r="F86" s="59"/>
       <c r="G86" s="38" t="s">
         <v>33</v>
       </c>
@@ -12106,11 +12442,11 @@
       <c r="C87" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="D87" s="61" t="s">
+      <c r="D87" s="58" t="s">
         <v>361</v>
       </c>
-      <c r="E87" s="60"/>
-      <c r="F87" s="60" t="s">
+      <c r="E87" s="59"/>
+      <c r="F87" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G87" s="38" t="s">
@@ -12121,9 +12457,9 @@
       <c r="C88" s="34" t="s">
         <v>363</v>
       </c>
-      <c r="D88" s="61"/>
-      <c r="E88" s="60"/>
-      <c r="F88" s="60"/>
+      <c r="D88" s="58"/>
+      <c r="E88" s="59"/>
+      <c r="F88" s="59"/>
       <c r="G88" s="38" t="s">
         <v>33</v>
       </c>
@@ -12132,11 +12468,11 @@
       <c r="C89" s="34" t="s">
         <v>365</v>
       </c>
-      <c r="D89" s="61" t="s">
+      <c r="D89" s="58" t="s">
         <v>366</v>
       </c>
-      <c r="E89" s="60"/>
-      <c r="F89" s="60" t="s">
+      <c r="E89" s="59"/>
+      <c r="F89" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G89" s="38" t="s">
@@ -12147,9 +12483,9 @@
       <c r="C90" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="D90" s="61"/>
-      <c r="E90" s="60"/>
-      <c r="F90" s="60"/>
+      <c r="D90" s="58"/>
+      <c r="E90" s="59"/>
+      <c r="F90" s="59"/>
       <c r="G90" s="38" t="s">
         <v>33</v>
       </c>
@@ -12158,9 +12494,9 @@
       <c r="C91" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="D91" s="61"/>
-      <c r="E91" s="60"/>
-      <c r="F91" s="60"/>
+      <c r="D91" s="58"/>
+      <c r="E91" s="59"/>
+      <c r="F91" s="59"/>
       <c r="G91" s="38" t="s">
         <v>33</v>
       </c>
@@ -12169,11 +12505,11 @@
       <c r="C92" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="D92" s="61" t="s">
+      <c r="D92" s="58" t="s">
         <v>371</v>
       </c>
-      <c r="E92" s="60"/>
-      <c r="F92" s="60" t="s">
+      <c r="E92" s="59"/>
+      <c r="F92" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G92" s="38" t="s">
@@ -12184,9 +12520,9 @@
       <c r="C93" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="D93" s="61"/>
-      <c r="E93" s="60"/>
-      <c r="F93" s="60"/>
+      <c r="D93" s="58"/>
+      <c r="E93" s="59"/>
+      <c r="F93" s="59"/>
       <c r="G93" s="38" t="s">
         <v>33</v>
       </c>
@@ -12195,9 +12531,9 @@
       <c r="C94" s="34" t="s">
         <v>384</v>
       </c>
-      <c r="D94" s="61"/>
-      <c r="E94" s="60"/>
-      <c r="F94" s="60"/>
+      <c r="D94" s="58"/>
+      <c r="E94" s="59"/>
+      <c r="F94" s="59"/>
       <c r="G94" s="38" t="s">
         <v>33</v>
       </c>
@@ -12207,11 +12543,11 @@
       <c r="C95" s="36" t="s">
         <v>373</v>
       </c>
-      <c r="D95" s="61" t="s">
+      <c r="D95" s="58" t="s">
         <v>374</v>
       </c>
-      <c r="E95" s="60"/>
-      <c r="F95" s="60" t="s">
+      <c r="E95" s="59"/>
+      <c r="F95" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G95" s="38" t="s">
@@ -12223,9 +12559,9 @@
       <c r="C96" s="36" t="s">
         <v>380</v>
       </c>
-      <c r="D96" s="61"/>
-      <c r="E96" s="60"/>
-      <c r="F96" s="60"/>
+      <c r="D96" s="58"/>
+      <c r="E96" s="59"/>
+      <c r="F96" s="59"/>
       <c r="G96" s="38" t="s">
         <v>33</v>
       </c>
@@ -12235,9 +12571,9 @@
       <c r="C97" s="36" t="s">
         <v>386</v>
       </c>
-      <c r="D97" s="61"/>
-      <c r="E97" s="60"/>
-      <c r="F97" s="60"/>
+      <c r="D97" s="58"/>
+      <c r="E97" s="59"/>
+      <c r="F97" s="59"/>
       <c r="G97" s="38" t="s">
         <v>33</v>
       </c>
@@ -12250,11 +12586,11 @@
       <c r="C98" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="D98" s="61" t="s">
+      <c r="D98" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="E98" s="60"/>
-      <c r="F98" s="60" t="s">
+      <c r="E98" s="59"/>
+      <c r="F98" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G98" s="38" t="s">
@@ -12266,9 +12602,9 @@
       <c r="C99" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="D99" s="61"/>
-      <c r="E99" s="60"/>
-      <c r="F99" s="60"/>
+      <c r="D99" s="58"/>
+      <c r="E99" s="59"/>
+      <c r="F99" s="59"/>
       <c r="G99" s="38" t="s">
         <v>33</v>
       </c>
@@ -12277,11 +12613,11 @@
       <c r="C100" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="D100" s="61" t="s">
+      <c r="D100" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="E100" s="60"/>
-      <c r="F100" s="60" t="s">
+      <c r="E100" s="59"/>
+      <c r="F100" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G100" s="38" t="s">
@@ -12292,9 +12628,9 @@
       <c r="C101" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="D101" s="61"/>
-      <c r="E101" s="60"/>
-      <c r="F101" s="60"/>
+      <c r="D101" s="58"/>
+      <c r="E101" s="59"/>
+      <c r="F101" s="59"/>
       <c r="G101" s="38" t="s">
         <v>33</v>
       </c>
@@ -12303,9 +12639,9 @@
       <c r="C102" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="D102" s="61"/>
-      <c r="E102" s="60"/>
-      <c r="F102" s="60"/>
+      <c r="D102" s="58"/>
+      <c r="E102" s="59"/>
+      <c r="F102" s="59"/>
       <c r="G102" s="38" t="s">
         <v>33</v>
       </c>
@@ -12314,11 +12650,11 @@
       <c r="C103" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="D103" s="61" t="s">
+      <c r="D103" s="58" t="s">
         <v>119</v>
       </c>
-      <c r="E103" s="60"/>
-      <c r="F103" s="60" t="s">
+      <c r="E103" s="59"/>
+      <c r="F103" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G103" s="38" t="s">
@@ -12329,9 +12665,9 @@
       <c r="C104" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="D104" s="61"/>
-      <c r="E104" s="60"/>
-      <c r="F104" s="60"/>
+      <c r="D104" s="58"/>
+      <c r="E104" s="59"/>
+      <c r="F104" s="59"/>
       <c r="G104" s="38" t="s">
         <v>33</v>
       </c>
@@ -12340,11 +12676,11 @@
       <c r="C105" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="D105" s="61" t="s">
+      <c r="D105" s="58" t="s">
         <v>124</v>
       </c>
-      <c r="E105" s="60"/>
-      <c r="F105" s="60" t="s">
+      <c r="E105" s="59"/>
+      <c r="F105" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G105" s="38" t="s">
@@ -12355,9 +12691,9 @@
       <c r="C106" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="D106" s="61"/>
-      <c r="E106" s="60"/>
-      <c r="F106" s="60"/>
+      <c r="D106" s="58"/>
+      <c r="E106" s="59"/>
+      <c r="F106" s="59"/>
       <c r="G106" s="38" t="s">
         <v>33</v>
       </c>
@@ -12366,9 +12702,9 @@
       <c r="C107" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="D107" s="61"/>
-      <c r="E107" s="60"/>
-      <c r="F107" s="60"/>
+      <c r="D107" s="58"/>
+      <c r="E107" s="59"/>
+      <c r="F107" s="59"/>
       <c r="G107" s="38" t="s">
         <v>33</v>
       </c>
@@ -12377,11 +12713,11 @@
       <c r="C108" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="D108" s="61" t="s">
+      <c r="D108" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="E108" s="60"/>
-      <c r="F108" s="60" t="s">
+      <c r="E108" s="59"/>
+      <c r="F108" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G108" s="38" t="s">
@@ -12392,9 +12728,9 @@
       <c r="C109" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="D109" s="61"/>
-      <c r="E109" s="60"/>
-      <c r="F109" s="60"/>
+      <c r="D109" s="58"/>
+      <c r="E109" s="59"/>
+      <c r="F109" s="59"/>
       <c r="G109" s="38" t="s">
         <v>33</v>
       </c>
@@ -12403,9 +12739,9 @@
       <c r="C110" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="D110" s="61"/>
-      <c r="E110" s="60"/>
-      <c r="F110" s="60"/>
+      <c r="D110" s="58"/>
+      <c r="E110" s="59"/>
+      <c r="F110" s="59"/>
       <c r="G110" s="38" t="s">
         <v>33</v>
       </c>
@@ -12414,11 +12750,11 @@
       <c r="C111" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="D111" s="61" t="s">
+      <c r="D111" s="58" t="s">
         <v>159</v>
       </c>
-      <c r="E111" s="60"/>
-      <c r="F111" s="60" t="s">
+      <c r="E111" s="59"/>
+      <c r="F111" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G111" s="38" t="s">
@@ -12429,9 +12765,9 @@
       <c r="C112" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="D112" s="61"/>
-      <c r="E112" s="60"/>
-      <c r="F112" s="60"/>
+      <c r="D112" s="58"/>
+      <c r="E112" s="59"/>
+      <c r="F112" s="59"/>
       <c r="G112" s="38" t="s">
         <v>33</v>
       </c>
@@ -12440,11 +12776,11 @@
       <c r="C113" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="D113" s="61" t="s">
+      <c r="D113" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="E113" s="60"/>
-      <c r="F113" s="60" t="s">
+      <c r="E113" s="59"/>
+      <c r="F113" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G113" s="38" t="s">
@@ -12455,9 +12791,9 @@
       <c r="C114" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="D114" s="61"/>
-      <c r="E114" s="60"/>
-      <c r="F114" s="60"/>
+      <c r="D114" s="58"/>
+      <c r="E114" s="59"/>
+      <c r="F114" s="59"/>
       <c r="G114" s="38" t="s">
         <v>33</v>
       </c>
@@ -12466,9 +12802,9 @@
       <c r="C115" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="D115" s="61"/>
-      <c r="E115" s="60"/>
-      <c r="F115" s="60"/>
+      <c r="D115" s="58"/>
+      <c r="E115" s="59"/>
+      <c r="F115" s="59"/>
       <c r="G115" s="38" t="s">
         <v>33</v>
       </c>
@@ -12477,11 +12813,11 @@
       <c r="C116" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="D116" s="61" t="s">
+      <c r="D116" s="58" t="s">
         <v>179</v>
       </c>
-      <c r="E116" s="60"/>
-      <c r="F116" s="60" t="s">
+      <c r="E116" s="59"/>
+      <c r="F116" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G116" s="38" t="s">
@@ -12492,9 +12828,9 @@
       <c r="C117" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="D117" s="61"/>
-      <c r="E117" s="60"/>
-      <c r="F117" s="60"/>
+      <c r="D117" s="58"/>
+      <c r="E117" s="59"/>
+      <c r="F117" s="59"/>
       <c r="G117" s="38" t="s">
         <v>33</v>
       </c>
@@ -12503,9 +12839,9 @@
       <c r="C118" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="D118" s="61"/>
-      <c r="E118" s="60"/>
-      <c r="F118" s="60"/>
+      <c r="D118" s="58"/>
+      <c r="E118" s="59"/>
+      <c r="F118" s="59"/>
       <c r="G118" s="38" t="s">
         <v>33</v>
       </c>
@@ -12514,11 +12850,11 @@
       <c r="C119" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="D119" s="61" t="s">
+      <c r="D119" s="58" t="s">
         <v>186</v>
       </c>
-      <c r="E119" s="60"/>
-      <c r="F119" s="60" t="s">
+      <c r="E119" s="59"/>
+      <c r="F119" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G119" s="38" t="s">
@@ -12532,9 +12868,9 @@
       <c r="C120" s="34" t="s">
         <v>188</v>
       </c>
-      <c r="D120" s="61"/>
-      <c r="E120" s="60"/>
-      <c r="F120" s="60"/>
+      <c r="D120" s="58"/>
+      <c r="E120" s="59"/>
+      <c r="F120" s="59"/>
       <c r="G120" s="38" t="s">
         <v>33</v>
       </c>
@@ -12546,11 +12882,11 @@
       <c r="C121" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="D121" s="61" t="s">
+      <c r="D121" s="58" t="s">
         <v>195</v>
       </c>
-      <c r="E121" s="60"/>
-      <c r="F121" s="60" t="s">
+      <c r="E121" s="59"/>
+      <c r="F121" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G121" s="38" t="s">
@@ -12564,9 +12900,9 @@
       <c r="C122" s="34" t="s">
         <v>197</v>
       </c>
-      <c r="D122" s="61"/>
-      <c r="E122" s="60"/>
-      <c r="F122" s="60"/>
+      <c r="D122" s="58"/>
+      <c r="E122" s="59"/>
+      <c r="F122" s="59"/>
       <c r="G122" s="38" t="s">
         <v>33</v>
       </c>
@@ -12578,11 +12914,11 @@
       <c r="C123" s="34" t="s">
         <v>199</v>
       </c>
-      <c r="D123" s="61" t="s">
+      <c r="D123" s="58" t="s">
         <v>200</v>
       </c>
-      <c r="E123" s="60"/>
-      <c r="F123" s="60" t="s">
+      <c r="E123" s="59"/>
+      <c r="F123" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G123" s="38" t="s">
@@ -12596,9 +12932,9 @@
       <c r="C124" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="D124" s="61"/>
-      <c r="E124" s="60"/>
-      <c r="F124" s="60"/>
+      <c r="D124" s="58"/>
+      <c r="E124" s="59"/>
+      <c r="F124" s="59"/>
       <c r="G124" s="38" t="s">
         <v>33</v>
       </c>
@@ -12610,11 +12946,11 @@
       <c r="C125" s="34" t="s">
         <v>210</v>
       </c>
-      <c r="D125" s="61" t="s">
+      <c r="D125" s="58" t="s">
         <v>211</v>
       </c>
-      <c r="E125" s="60"/>
-      <c r="F125" s="60" t="s">
+      <c r="E125" s="59"/>
+      <c r="F125" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G125" s="38" t="s">
@@ -12628,9 +12964,9 @@
       <c r="C126" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="D126" s="61"/>
-      <c r="E126" s="60"/>
-      <c r="F126" s="60"/>
+      <c r="D126" s="58"/>
+      <c r="E126" s="59"/>
+      <c r="F126" s="59"/>
       <c r="G126" s="38" t="s">
         <v>33</v>
       </c>
@@ -12642,9 +12978,9 @@
       <c r="C127" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="D127" s="61"/>
-      <c r="E127" s="60"/>
-      <c r="F127" s="60"/>
+      <c r="D127" s="58"/>
+      <c r="E127" s="59"/>
+      <c r="F127" s="59"/>
       <c r="G127" s="38" t="s">
         <v>33</v>
       </c>
@@ -12656,11 +12992,11 @@
       <c r="C128" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="D128" s="61" t="s">
+      <c r="D128" s="58" t="s">
         <v>223</v>
       </c>
-      <c r="E128" s="60"/>
-      <c r="F128" s="60" t="s">
+      <c r="E128" s="59"/>
+      <c r="F128" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G128" s="38" t="s">
@@ -12674,9 +13010,9 @@
       <c r="C129" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="D129" s="61"/>
-      <c r="E129" s="60"/>
-      <c r="F129" s="60"/>
+      <c r="D129" s="58"/>
+      <c r="E129" s="59"/>
+      <c r="F129" s="59"/>
       <c r="G129" s="38" t="s">
         <v>33</v>
       </c>
@@ -12688,11 +13024,11 @@
       <c r="C130" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="D130" s="61" t="s">
+      <c r="D130" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="E130" s="60"/>
-      <c r="F130" s="60" t="s">
+      <c r="E130" s="59"/>
+      <c r="F130" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G130" s="38" t="s">
@@ -12706,9 +13042,9 @@
       <c r="C131" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="D131" s="61"/>
-      <c r="E131" s="60"/>
-      <c r="F131" s="60"/>
+      <c r="D131" s="58"/>
+      <c r="E131" s="59"/>
+      <c r="F131" s="59"/>
       <c r="G131" s="38" t="s">
         <v>33</v>
       </c>
@@ -12720,9 +13056,9 @@
       <c r="C132" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="D132" s="61"/>
-      <c r="E132" s="60"/>
-      <c r="F132" s="60"/>
+      <c r="D132" s="58"/>
+      <c r="E132" s="59"/>
+      <c r="F132" s="59"/>
       <c r="G132" s="38" t="s">
         <v>33</v>
       </c>
@@ -12800,11 +13136,11 @@
       <c r="C137" s="34" t="s">
         <v>454</v>
       </c>
-      <c r="D137" s="61" t="s">
+      <c r="D137" s="58" t="s">
         <v>582</v>
       </c>
-      <c r="E137" s="60"/>
-      <c r="F137" s="60" t="s">
+      <c r="E137" s="59"/>
+      <c r="F137" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G137" s="38" t="s">
@@ -12815,9 +13151,9 @@
       <c r="C138" s="34" t="s">
         <v>457</v>
       </c>
-      <c r="D138" s="61"/>
-      <c r="E138" s="60"/>
-      <c r="F138" s="60"/>
+      <c r="D138" s="58"/>
+      <c r="E138" s="59"/>
+      <c r="F138" s="59"/>
       <c r="G138" s="38" t="s">
         <v>33</v>
       </c>
@@ -12826,11 +13162,11 @@
       <c r="C139" s="34" t="s">
         <v>459</v>
       </c>
-      <c r="D139" s="61" t="s">
+      <c r="D139" s="58" t="s">
         <v>460</v>
       </c>
-      <c r="E139" s="60"/>
-      <c r="F139" s="60" t="s">
+      <c r="E139" s="59"/>
+      <c r="F139" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G139" s="38" t="s">
@@ -12841,9 +13177,9 @@
       <c r="C140" s="34" t="s">
         <v>462</v>
       </c>
-      <c r="D140" s="61"/>
-      <c r="E140" s="60"/>
-      <c r="F140" s="60"/>
+      <c r="D140" s="58"/>
+      <c r="E140" s="59"/>
+      <c r="F140" s="59"/>
       <c r="G140" s="38" t="s">
         <v>33</v>
       </c>
@@ -12899,11 +13235,11 @@
       <c r="C144" s="34" t="s">
         <v>477</v>
       </c>
-      <c r="D144" s="61" t="s">
+      <c r="D144" s="58" t="s">
         <v>478</v>
       </c>
-      <c r="E144" s="60"/>
-      <c r="F144" s="60" t="s">
+      <c r="E144" s="59"/>
+      <c r="F144" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G144" s="38" t="s">
@@ -12917,9 +13253,9 @@
       <c r="C145" s="35" t="s">
         <v>480</v>
       </c>
-      <c r="D145" s="63"/>
-      <c r="E145" s="65"/>
-      <c r="F145" s="65"/>
+      <c r="D145" s="61"/>
+      <c r="E145" s="66"/>
+      <c r="F145" s="66"/>
       <c r="G145" s="39" t="s">
         <v>33</v>
       </c>
@@ -12983,6 +13319,183 @@
     </row>
   </sheetData>
   <mergeCells count="201">
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="D95:D97"/>
+    <mergeCell ref="E95:E97"/>
+    <mergeCell ref="F95:F97"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="D144:D145"/>
+    <mergeCell ref="E144:E145"/>
+    <mergeCell ref="F144:F145"/>
+    <mergeCell ref="D128:D129"/>
+    <mergeCell ref="E128:E129"/>
+    <mergeCell ref="F128:F129"/>
+    <mergeCell ref="D130:D132"/>
+    <mergeCell ref="E130:E132"/>
+    <mergeCell ref="F130:F132"/>
+    <mergeCell ref="D137:D138"/>
+    <mergeCell ref="D139:D140"/>
+    <mergeCell ref="F137:F138"/>
+    <mergeCell ref="F139:F140"/>
+    <mergeCell ref="E137:E138"/>
+    <mergeCell ref="E139:E140"/>
+    <mergeCell ref="D123:D124"/>
+    <mergeCell ref="E123:E124"/>
+    <mergeCell ref="F123:F124"/>
+    <mergeCell ref="D125:D127"/>
+    <mergeCell ref="E125:E127"/>
+    <mergeCell ref="F125:F127"/>
+    <mergeCell ref="D119:D120"/>
+    <mergeCell ref="E119:E120"/>
+    <mergeCell ref="F119:F120"/>
+    <mergeCell ref="D121:D122"/>
+    <mergeCell ref="E121:E122"/>
+    <mergeCell ref="F121:F122"/>
+    <mergeCell ref="D113:D115"/>
+    <mergeCell ref="E113:E115"/>
+    <mergeCell ref="F113:F115"/>
+    <mergeCell ref="D116:D118"/>
+    <mergeCell ref="E116:E118"/>
+    <mergeCell ref="F116:F118"/>
+    <mergeCell ref="D108:D110"/>
+    <mergeCell ref="E108:E110"/>
+    <mergeCell ref="F108:F110"/>
+    <mergeCell ref="D111:D112"/>
+    <mergeCell ref="E111:E112"/>
+    <mergeCell ref="F111:F112"/>
+    <mergeCell ref="D103:D104"/>
+    <mergeCell ref="E103:E104"/>
+    <mergeCell ref="F103:F104"/>
+    <mergeCell ref="D105:D107"/>
+    <mergeCell ref="E105:E107"/>
+    <mergeCell ref="F105:F107"/>
+    <mergeCell ref="D98:D99"/>
+    <mergeCell ref="E98:E99"/>
+    <mergeCell ref="F98:F99"/>
+    <mergeCell ref="D100:D102"/>
+    <mergeCell ref="E100:E102"/>
+    <mergeCell ref="F100:F102"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="E41:E43"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="G41:G43"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="D49:D51"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="D62:D64"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="F62:F64"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="F49:F51"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="F81:F82"/>
+    <mergeCell ref="F83:F84"/>
+    <mergeCell ref="E87:E88"/>
+    <mergeCell ref="F85:F86"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="D87:D88"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="E83:E84"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="F67:F68"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="E69:E72"/>
+    <mergeCell ref="F69:F72"/>
+    <mergeCell ref="E62:E64"/>
+    <mergeCell ref="F73:F74"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="F77:F78"/>
     <mergeCell ref="D89:D91"/>
     <mergeCell ref="E89:E91"/>
     <mergeCell ref="F89:F91"/>
@@ -13007,183 +13520,6 @@
     <mergeCell ref="D83:D84"/>
     <mergeCell ref="F87:F88"/>
     <mergeCell ref="E67:E68"/>
-    <mergeCell ref="F67:F68"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="E69:E72"/>
-    <mergeCell ref="F69:F72"/>
-    <mergeCell ref="E62:E64"/>
-    <mergeCell ref="F73:F74"/>
-    <mergeCell ref="F75:F76"/>
-    <mergeCell ref="F77:F78"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="F81:F82"/>
-    <mergeCell ref="F83:F84"/>
-    <mergeCell ref="E87:E88"/>
-    <mergeCell ref="F85:F86"/>
-    <mergeCell ref="D85:D86"/>
-    <mergeCell ref="D87:D88"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E73:E74"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="E81:E82"/>
-    <mergeCell ref="E83:E84"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="D49:D51"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="D62:D64"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="F62:F64"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="F49:F51"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="G41:G43"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="D103:D104"/>
-    <mergeCell ref="E103:E104"/>
-    <mergeCell ref="F103:F104"/>
-    <mergeCell ref="D105:D107"/>
-    <mergeCell ref="E105:E107"/>
-    <mergeCell ref="F105:F107"/>
-    <mergeCell ref="D98:D99"/>
-    <mergeCell ref="E98:E99"/>
-    <mergeCell ref="F98:F99"/>
-    <mergeCell ref="D100:D102"/>
-    <mergeCell ref="E100:E102"/>
-    <mergeCell ref="F100:F102"/>
-    <mergeCell ref="D113:D115"/>
-    <mergeCell ref="E113:E115"/>
-    <mergeCell ref="F113:F115"/>
-    <mergeCell ref="D116:D118"/>
-    <mergeCell ref="E116:E118"/>
-    <mergeCell ref="F116:F118"/>
-    <mergeCell ref="D108:D110"/>
-    <mergeCell ref="E108:E110"/>
-    <mergeCell ref="F108:F110"/>
-    <mergeCell ref="D111:D112"/>
-    <mergeCell ref="E111:E112"/>
-    <mergeCell ref="F111:F112"/>
-    <mergeCell ref="D123:D124"/>
-    <mergeCell ref="E123:E124"/>
-    <mergeCell ref="F123:F124"/>
-    <mergeCell ref="D125:D127"/>
-    <mergeCell ref="E125:E127"/>
-    <mergeCell ref="F125:F127"/>
-    <mergeCell ref="D119:D120"/>
-    <mergeCell ref="E119:E120"/>
-    <mergeCell ref="F119:F120"/>
-    <mergeCell ref="D121:D122"/>
-    <mergeCell ref="E121:E122"/>
-    <mergeCell ref="F121:F122"/>
-    <mergeCell ref="D144:D145"/>
-    <mergeCell ref="E144:E145"/>
-    <mergeCell ref="F144:F145"/>
-    <mergeCell ref="D128:D129"/>
-    <mergeCell ref="E128:E129"/>
-    <mergeCell ref="F128:F129"/>
-    <mergeCell ref="D130:D132"/>
-    <mergeCell ref="E130:E132"/>
-    <mergeCell ref="F130:F132"/>
-    <mergeCell ref="D137:D138"/>
-    <mergeCell ref="D139:D140"/>
-    <mergeCell ref="F137:F138"/>
-    <mergeCell ref="F139:F140"/>
-    <mergeCell ref="E137:E138"/>
-    <mergeCell ref="E139:E140"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="D95:D97"/>
-    <mergeCell ref="E95:E97"/>
-    <mergeCell ref="F95:F97"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -13194,7 +13530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C5067C9-23D2-4ADE-8DCB-648ED12E8246}">
   <dimension ref="A2:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -13355,6 +13691,213 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FEA6E34-2715-4365-861D-18E53AC7F8C2}">
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" style="72" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="108.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="72" t="s">
+        <v>605</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="D1" s="72" t="s">
+        <v>624</v>
+      </c>
+      <c r="E1" s="72" t="s">
+        <v>625</v>
+      </c>
+      <c r="F1" s="72" t="s">
+        <v>602</v>
+      </c>
+      <c r="G1" s="72" t="s">
+        <v>608</v>
+      </c>
+      <c r="H1" s="72" t="s">
+        <v>603</v>
+      </c>
+      <c r="I1" s="72" t="s">
+        <v>604</v>
+      </c>
+      <c r="J1" s="72" t="s">
+        <v>626</v>
+      </c>
+      <c r="K1" s="72" t="s">
+        <v>612</v>
+      </c>
+      <c r="L1" s="72" t="s">
+        <v>627</v>
+      </c>
+      <c r="M1" s="72" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="72" t="s">
+        <v>606</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="72" t="s">
+        <v>607</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="72" t="s">
+        <v>608</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="72" t="s">
+        <v>609</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="72" t="s">
+        <v>610</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="72" t="s">
+        <v>611</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="72" t="s">
+        <v>612</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="72" t="s">
+        <v>613</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71B37C7A-27BB-4B6C-AB7C-FA91261DBC1C}">
+  <dimension ref="B2:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="89.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>628</v>
+      </c>
+      <c r="C2" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>636</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA06BA7C-CD17-4C21-9F28-C604AE25C8B9}">
   <dimension ref="A1:F25"/>
   <sheetViews>
@@ -13793,7 +14336,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A026136A-3463-4F46-9920-D2EEED3E1AFC}">
   <dimension ref="A1:X17"/>
   <sheetViews>
@@ -14300,7 +14843,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6DDA247-F6AE-445A-B41C-F6181C9C037C}">
   <dimension ref="A1:C44"/>
   <sheetViews>
@@ -14677,66 +15220,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABE3366-981D-4444-A865-F5BA56B32FED}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.42578125" style="9" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>525</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>527</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>529</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>531</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>590</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>591</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEAE28352B96D64C95AA0D5E2FA62FAD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed183881d36ac1b5d7d67982eda510d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d161086-4829-409f-9f75-5bde88dcb151" xmlns:ns3="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="685f4fda20cf913d28bf77c13cd653dd" ns2:_="" ns3:_="">
     <xsd:import namespace="3d161086-4829-409f-9f75-5bde88dcb151"/>
@@ -14959,27 +15463,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C74AB5E7-5C87-4FF7-BF80-AB0EB6BD1D32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14996,29 +15505,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Question 65 added to User_Questions
Job numbers added to the CSV list in MEDS_Tables
Before refactoring parse_datatype_biomass, removing the grouping
</commit_message>
<xml_diff>
--- a/analysis/MEDS_Tables.xlsx
+++ b/analysis/MEDS_Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="703" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AD21109-68DA-4768-A7F5-670E56CF959B}"/>
+  <xr:revisionPtr revIDLastSave="718" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{673BFC4A-AB37-4EEB-9E96-86A15051DA1C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meds_tables" sheetId="1" r:id="rId1"/>
@@ -3462,49 +3462,49 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -11678,10 +11678,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76451C41-9738-4BC1-978E-20A0DA8744C6}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11690,13 +11690,14 @@
     <col min="2" max="2" width="26.140625" style="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" style="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="22"/>
-    <col min="7" max="7" width="11.28515625" style="22" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="22"/>
+    <col min="5" max="5" width="38.5703125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="63.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="22"/>
+    <col min="8" max="8" width="11.28515625" style="22" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -11709,14 +11710,15 @@
       <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>36</v>
       </c>
@@ -11729,12 +11731,15 @@
       <c r="D2" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="16">
+        <v>102176</v>
+      </c>
+      <c r="F2" s="16" t="s">
         <v>564</v>
       </c>
-      <c r="F2" s="27"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="27"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>43</v>
       </c>
@@ -11747,12 +11752,15 @@
       <c r="D3" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="14">
+        <v>102176</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>564</v>
       </c>
-      <c r="F3" s="28"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="28"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>45</v>
       </c>
@@ -11765,12 +11773,15 @@
       <c r="D4" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="16">
+        <v>102176</v>
+      </c>
+      <c r="F4" s="16" t="s">
         <v>564</v>
       </c>
-      <c r="F4" s="27"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="27"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>52</v>
       </c>
@@ -11783,14 +11794,17 @@
       <c r="D5" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="14">
+        <v>102533</v>
+      </c>
+      <c r="F5" s="14" t="s">
         <v>519</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="G5" s="28" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>55</v>
       </c>
@@ -11803,14 +11817,17 @@
       <c r="D6" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="16">
+        <v>102533</v>
+      </c>
+      <c r="F6" s="16" t="s">
         <v>519</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="G6" s="27" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>77</v>
       </c>
@@ -11823,14 +11840,17 @@
       <c r="D7" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="14">
+        <v>68822</v>
+      </c>
+      <c r="F7" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="G7" s="28" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>83</v>
       </c>
@@ -11843,14 +11863,17 @@
       <c r="D8" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="16">
+        <v>68822</v>
+      </c>
+      <c r="F8" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="G8" s="27" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>170</v>
       </c>
@@ -11863,12 +11886,15 @@
       <c r="D9" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="14">
+        <v>101747</v>
+      </c>
+      <c r="F9" s="14" t="s">
         <v>523</v>
       </c>
-      <c r="F9" s="28"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="28"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>174</v>
       </c>
@@ -11881,12 +11907,15 @@
       <c r="D10" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="16">
+        <v>101747</v>
+      </c>
+      <c r="F10" s="16" t="s">
         <v>523</v>
       </c>
-      <c r="F10" s="27"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="27"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>176</v>
       </c>
@@ -11899,12 +11928,15 @@
       <c r="D11" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="14">
+        <v>101747</v>
+      </c>
+      <c r="F11" s="14" t="s">
         <v>523</v>
       </c>
-      <c r="F11" s="28"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="28"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>203</v>
       </c>
@@ -11917,14 +11949,17 @@
       <c r="D12" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="16">
+        <v>101607</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>515</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="G12" s="27" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>206</v>
       </c>
@@ -11937,14 +11972,17 @@
       <c r="D13" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="14">
+        <v>101607</v>
+      </c>
+      <c r="F13" s="14" t="s">
         <v>515</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="G13" s="28" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>360</v>
       </c>
@@ -11957,12 +11995,15 @@
       <c r="D14" s="16" t="s">
         <v>361</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="16">
+        <v>102460</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>518</v>
       </c>
-      <c r="F14" s="27"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="27"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>363</v>
       </c>
@@ -11975,10 +12016,13 @@
       <c r="D15" s="14" t="s">
         <v>361</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="14">
+        <v>102460</v>
+      </c>
+      <c r="F15" s="14" t="s">
         <v>518</v>
       </c>
-      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12038,7 +12082,7 @@
       <c r="C2" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="72" t="s">
+      <c r="D2" s="73" t="s">
         <v>38</v>
       </c>
       <c r="E2" s="74" t="s">
@@ -12047,7 +12091,7 @@
       <c r="F2" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="76" t="s">
+      <c r="G2" s="75" t="s">
         <v>564</v>
       </c>
     </row>
@@ -12056,10 +12100,10 @@
       <c r="C3" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="71"/>
+      <c r="D3" s="69"/>
       <c r="E3" s="70"/>
       <c r="F3" s="70"/>
-      <c r="G3" s="78"/>
+      <c r="G3" s="72"/>
       <c r="K3" s="36"/>
       <c r="L3" s="36"/>
       <c r="M3" s="36"/>
@@ -12072,10 +12116,10 @@
       <c r="C4" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="71"/>
+      <c r="D4" s="69"/>
       <c r="E4" s="70"/>
       <c r="F4" s="70"/>
-      <c r="G4" s="78"/>
+      <c r="G4" s="72"/>
       <c r="K4" s="36"/>
       <c r="L4" s="36"/>
       <c r="M4" s="36"/>
@@ -12088,7 +12132,7 @@
       <c r="C5" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="71" t="s">
+      <c r="D5" s="69" t="s">
         <v>53</v>
       </c>
       <c r="E5" s="70" t="s">
@@ -12097,18 +12141,18 @@
       <c r="F5" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="78" t="s">
+      <c r="G5" s="72" t="s">
         <v>519</v>
       </c>
       <c r="K5" s="36"/>
       <c r="L5" s="47" t="s">
         <v>464</v>
       </c>
-      <c r="M5" s="69" t="s">
+      <c r="M5" s="81" t="s">
         <v>465</v>
       </c>
       <c r="N5" s="70"/>
-      <c r="O5" s="68" t="s">
+      <c r="O5" s="80" t="s">
         <v>581</v>
       </c>
       <c r="P5" s="36"/>
@@ -12118,17 +12162,17 @@
       <c r="C6" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="71"/>
+      <c r="D6" s="69"/>
       <c r="E6" s="70"/>
       <c r="F6" s="70"/>
-      <c r="G6" s="78"/>
+      <c r="G6" s="72"/>
       <c r="K6" s="36"/>
       <c r="L6" s="47" t="s">
         <v>467</v>
       </c>
-      <c r="M6" s="69"/>
+      <c r="M6" s="81"/>
       <c r="N6" s="70"/>
-      <c r="O6" s="68"/>
+      <c r="O6" s="80"/>
       <c r="P6" s="36"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
@@ -12136,7 +12180,7 @@
       <c r="C7" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="71" t="s">
+      <c r="D7" s="69" t="s">
         <v>78</v>
       </c>
       <c r="E7" s="70" t="s">
@@ -12145,7 +12189,7 @@
       <c r="F7" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="78" t="s">
+      <c r="G7" s="72" t="s">
         <v>80</v>
       </c>
       <c r="K7" s="36"/>
@@ -12160,10 +12204,10 @@
       <c r="C8" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="71"/>
+      <c r="D8" s="69"/>
       <c r="E8" s="70"/>
       <c r="F8" s="70"/>
-      <c r="G8" s="78"/>
+      <c r="G8" s="72"/>
       <c r="K8" s="36"/>
       <c r="L8" s="36"/>
       <c r="M8" s="36"/>
@@ -12176,7 +12220,7 @@
       <c r="C9" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="D9" s="71" t="s">
+      <c r="D9" s="69" t="s">
         <v>171</v>
       </c>
       <c r="E9" s="70" t="s">
@@ -12185,7 +12229,7 @@
       <c r="F9" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="78" t="s">
+      <c r="G9" s="72" t="s">
         <v>523</v>
       </c>
       <c r="J9" s="36"/>
@@ -12196,10 +12240,10 @@
       <c r="C10" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="D10" s="71"/>
+      <c r="D10" s="69"/>
       <c r="E10" s="70"/>
       <c r="F10" s="70"/>
-      <c r="G10" s="78"/>
+      <c r="G10" s="72"/>
       <c r="J10" s="36"/>
       <c r="K10" s="36"/>
     </row>
@@ -12208,10 +12252,10 @@
       <c r="C11" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="D11" s="71"/>
+      <c r="D11" s="69"/>
       <c r="E11" s="70"/>
       <c r="F11" s="70"/>
-      <c r="G11" s="78"/>
+      <c r="G11" s="72"/>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
     </row>
@@ -12220,7 +12264,7 @@
       <c r="C12" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="D12" s="71" t="s">
+      <c r="D12" s="69" t="s">
         <v>204</v>
       </c>
       <c r="E12" s="70" t="s">
@@ -12229,7 +12273,7 @@
       <c r="F12" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="78" t="s">
+      <c r="G12" s="72" t="s">
         <v>515</v>
       </c>
       <c r="J12" s="36"/>
@@ -12240,10 +12284,10 @@
       <c r="C13" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="D13" s="71"/>
+      <c r="D13" s="69"/>
       <c r="E13" s="70"/>
       <c r="F13" s="70"/>
-      <c r="G13" s="78"/>
+      <c r="G13" s="72"/>
       <c r="J13" s="36"/>
       <c r="K13" s="36"/>
     </row>
@@ -12252,7 +12296,7 @@
       <c r="C14" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="D14" s="71" t="s">
+      <c r="D14" s="69" t="s">
         <v>361</v>
       </c>
       <c r="E14" s="70" t="s">
@@ -12261,7 +12305,7 @@
       <c r="F14" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="78" t="s">
+      <c r="G14" s="72" t="s">
         <v>518</v>
       </c>
       <c r="J14" s="36"/>
@@ -12272,10 +12316,10 @@
       <c r="C15" s="35" t="s">
         <v>363</v>
       </c>
-      <c r="D15" s="73"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="77"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="78"/>
       <c r="J15" s="36"/>
       <c r="K15" s="36"/>
     </row>
@@ -12283,7 +12327,7 @@
       <c r="C16" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="72" t="s">
+      <c r="D16" s="73" t="s">
         <v>71</v>
       </c>
       <c r="E16" s="74" t="s">
@@ -12292,7 +12336,7 @@
       <c r="F16" s="74" t="s">
         <v>567</v>
       </c>
-      <c r="G16" s="76" t="s">
+      <c r="G16" s="75" t="s">
         <v>73</v>
       </c>
       <c r="J16" s="36"/>
@@ -12302,10 +12346,10 @@
       <c r="C17" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="71"/>
+      <c r="D17" s="69"/>
       <c r="E17" s="70"/>
       <c r="F17" s="70"/>
-      <c r="G17" s="78"/>
+      <c r="G17" s="72"/>
       <c r="J17" s="36"/>
       <c r="K17" s="36"/>
     </row>
@@ -12313,7 +12357,7 @@
       <c r="C18" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="71" t="s">
+      <c r="D18" s="69" t="s">
         <v>105</v>
       </c>
       <c r="E18" s="70" t="s">
@@ -12322,7 +12366,7 @@
       <c r="F18" s="70" t="s">
         <v>567</v>
       </c>
-      <c r="G18" s="78" t="s">
+      <c r="G18" s="72" t="s">
         <v>524</v>
       </c>
       <c r="J18" s="36"/>
@@ -12332,10 +12376,10 @@
       <c r="C19" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="71"/>
+      <c r="D19" s="69"/>
       <c r="E19" s="70"/>
       <c r="F19" s="70"/>
-      <c r="G19" s="78"/>
+      <c r="G19" s="72"/>
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
     </row>
@@ -12343,7 +12387,7 @@
       <c r="C20" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="D20" s="71" t="s">
+      <c r="D20" s="69" t="s">
         <v>300</v>
       </c>
       <c r="E20" s="70" t="s">
@@ -12352,7 +12396,7 @@
       <c r="F20" s="70" t="s">
         <v>567</v>
       </c>
-      <c r="G20" s="78" t="s">
+      <c r="G20" s="72" t="s">
         <v>516</v>
       </c>
       <c r="J20" s="36"/>
@@ -12362,10 +12406,10 @@
       <c r="C21" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="D21" s="71"/>
+      <c r="D21" s="69"/>
       <c r="E21" s="70"/>
       <c r="F21" s="70"/>
-      <c r="G21" s="78"/>
+      <c r="G21" s="72"/>
       <c r="J21" s="36"/>
       <c r="K21" s="36"/>
     </row>
@@ -12373,7 +12417,7 @@
       <c r="C22" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="D22" s="71" t="s">
+      <c r="D22" s="69" t="s">
         <v>305</v>
       </c>
       <c r="E22" s="70" t="s">
@@ -12382,7 +12426,7 @@
       <c r="F22" s="70" t="s">
         <v>567</v>
       </c>
-      <c r="G22" s="78" t="s">
+      <c r="G22" s="72" t="s">
         <v>521</v>
       </c>
       <c r="J22" s="36"/>
@@ -12392,10 +12436,10 @@
       <c r="C23" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="D23" s="71"/>
+      <c r="D23" s="69"/>
       <c r="E23" s="70"/>
       <c r="F23" s="70"/>
-      <c r="G23" s="78"/>
+      <c r="G23" s="72"/>
       <c r="J23" s="36"/>
       <c r="K23" s="36"/>
     </row>
@@ -12403,7 +12447,7 @@
       <c r="C24" s="34" t="s">
         <v>317</v>
       </c>
-      <c r="D24" s="71" t="s">
+      <c r="D24" s="69" t="s">
         <v>318</v>
       </c>
       <c r="E24" s="70" t="s">
@@ -12412,7 +12456,7 @@
       <c r="F24" s="70" t="s">
         <v>567</v>
       </c>
-      <c r="G24" s="78" t="s">
+      <c r="G24" s="72" t="s">
         <v>512</v>
       </c>
       <c r="J24" s="36"/>
@@ -12422,10 +12466,10 @@
       <c r="C25" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="D25" s="71"/>
+      <c r="D25" s="69"/>
       <c r="E25" s="70"/>
       <c r="F25" s="70"/>
-      <c r="G25" s="78"/>
+      <c r="G25" s="72"/>
       <c r="J25" s="36"/>
       <c r="K25" s="36"/>
     </row>
@@ -12433,16 +12477,16 @@
       <c r="C26" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="D26" s="79" t="s">
+      <c r="D26" s="71" t="s">
         <v>323</v>
       </c>
-      <c r="E26" s="80" t="s">
+      <c r="E26" s="79" t="s">
         <v>81</v>
       </c>
       <c r="F26" s="70" t="s">
         <v>567</v>
       </c>
-      <c r="G26" s="78" t="s">
+      <c r="G26" s="72" t="s">
         <v>517</v>
       </c>
       <c r="J26" s="36"/>
@@ -12452,16 +12496,16 @@
       <c r="C27" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="D27" s="79"/>
-      <c r="E27" s="80"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="79"/>
       <c r="F27" s="70"/>
-      <c r="G27" s="78"/>
+      <c r="G27" s="72"/>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C28" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="D28" s="71" t="s">
+      <c r="D28" s="69" t="s">
         <v>328</v>
       </c>
       <c r="E28" s="70" t="s">
@@ -12470,7 +12514,7 @@
       <c r="F28" s="70" t="s">
         <v>567</v>
       </c>
-      <c r="G28" s="78" t="s">
+      <c r="G28" s="72" t="s">
         <v>508</v>
       </c>
     </row>
@@ -12478,16 +12522,16 @@
       <c r="C29" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="D29" s="71"/>
+      <c r="D29" s="69"/>
       <c r="E29" s="70"/>
       <c r="F29" s="70"/>
-      <c r="G29" s="78"/>
+      <c r="G29" s="72"/>
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C30" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="D30" s="71" t="s">
+      <c r="D30" s="69" t="s">
         <v>333</v>
       </c>
       <c r="E30" s="70" t="s">
@@ -12496,7 +12540,7 @@
       <c r="F30" s="70" t="s">
         <v>567</v>
       </c>
-      <c r="G30" s="78" t="s">
+      <c r="G30" s="72" t="s">
         <v>510</v>
       </c>
     </row>
@@ -12504,16 +12548,16 @@
       <c r="C31" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="D31" s="71"/>
+      <c r="D31" s="69"/>
       <c r="E31" s="70"/>
       <c r="F31" s="70"/>
-      <c r="G31" s="78"/>
+      <c r="G31" s="72"/>
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="D32" s="71" t="s">
+      <c r="D32" s="69" t="s">
         <v>338</v>
       </c>
       <c r="E32" s="70" t="s">
@@ -12522,7 +12566,7 @@
       <c r="F32" s="70" t="s">
         <v>567</v>
       </c>
-      <c r="G32" s="78" t="s">
+      <c r="G32" s="72" t="s">
         <v>511</v>
       </c>
     </row>
@@ -12530,16 +12574,16 @@
       <c r="C33" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="D33" s="71"/>
+      <c r="D33" s="69"/>
       <c r="E33" s="70"/>
       <c r="F33" s="70"/>
-      <c r="G33" s="78"/>
+      <c r="G33" s="72"/>
     </row>
     <row r="34" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C34" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="D34" s="71" t="s">
+      <c r="D34" s="69" t="s">
         <v>343</v>
       </c>
       <c r="E34" s="70" t="s">
@@ -12548,7 +12592,7 @@
       <c r="F34" s="70" t="s">
         <v>567</v>
       </c>
-      <c r="G34" s="78" t="s">
+      <c r="G34" s="72" t="s">
         <v>509</v>
       </c>
     </row>
@@ -12556,16 +12600,16 @@
       <c r="C35" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="D35" s="71"/>
+      <c r="D35" s="69"/>
       <c r="E35" s="70"/>
       <c r="F35" s="70"/>
-      <c r="G35" s="78"/>
+      <c r="G35" s="72"/>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C36" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="D36" s="71" t="s">
+      <c r="D36" s="69" t="s">
         <v>348</v>
       </c>
       <c r="E36" s="70" t="s">
@@ -12574,7 +12618,7 @@
       <c r="F36" s="70" t="s">
         <v>567</v>
       </c>
-      <c r="G36" s="78" t="s">
+      <c r="G36" s="72" t="s">
         <v>520</v>
       </c>
     </row>
@@ -12582,16 +12626,16 @@
       <c r="C37" s="35" t="s">
         <v>350</v>
       </c>
-      <c r="D37" s="73"/>
-      <c r="E37" s="75"/>
-      <c r="F37" s="75"/>
-      <c r="G37" s="77"/>
+      <c r="D37" s="76"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="77"/>
+      <c r="G37" s="78"/>
     </row>
     <row r="38" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C38" s="33" t="s">
         <v>365</v>
       </c>
-      <c r="D38" s="72" t="s">
+      <c r="D38" s="73" t="s">
         <v>366</v>
       </c>
       <c r="E38" s="74" t="s">
@@ -12600,7 +12644,7 @@
       <c r="F38" s="74" t="s">
         <v>369</v>
       </c>
-      <c r="G38" s="76" t="s">
+      <c r="G38" s="75" t="s">
         <v>514</v>
       </c>
     </row>
@@ -12608,25 +12652,25 @@
       <c r="C39" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="D39" s="71"/>
+      <c r="D39" s="69"/>
       <c r="E39" s="70"/>
       <c r="F39" s="70"/>
-      <c r="G39" s="78"/>
+      <c r="G39" s="72"/>
     </row>
     <row r="40" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C40" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="D40" s="71"/>
+      <c r="D40" s="69"/>
       <c r="E40" s="70"/>
       <c r="F40" s="70"/>
-      <c r="G40" s="78"/>
+      <c r="G40" s="72"/>
     </row>
     <row r="41" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C41" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="D41" s="71" t="s">
+      <c r="D41" s="69" t="s">
         <v>371</v>
       </c>
       <c r="E41" s="70" t="s">
@@ -12635,7 +12679,7 @@
       <c r="F41" s="70" t="s">
         <v>369</v>
       </c>
-      <c r="G41" s="78" t="s">
+      <c r="G41" s="72" t="s">
         <v>513</v>
       </c>
     </row>
@@ -12643,25 +12687,25 @@
       <c r="C42" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="D42" s="71"/>
+      <c r="D42" s="69"/>
       <c r="E42" s="70"/>
       <c r="F42" s="70"/>
-      <c r="G42" s="78"/>
+      <c r="G42" s="72"/>
     </row>
     <row r="43" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C43" s="34" t="s">
         <v>384</v>
       </c>
-      <c r="D43" s="71"/>
+      <c r="D43" s="69"/>
       <c r="E43" s="70"/>
       <c r="F43" s="70"/>
-      <c r="G43" s="78"/>
+      <c r="G43" s="72"/>
     </row>
     <row r="44" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C44" s="34" t="s">
         <v>373</v>
       </c>
-      <c r="D44" s="71" t="s">
+      <c r="D44" s="69" t="s">
         <v>374</v>
       </c>
       <c r="E44" s="70" t="s">
@@ -12670,7 +12714,7 @@
       <c r="F44" s="70" t="s">
         <v>369</v>
       </c>
-      <c r="G44" s="78" t="s">
+      <c r="G44" s="72" t="s">
         <v>522</v>
       </c>
     </row>
@@ -12678,19 +12722,19 @@
       <c r="C45" s="34" t="s">
         <v>380</v>
       </c>
-      <c r="D45" s="71"/>
+      <c r="D45" s="69"/>
       <c r="E45" s="70"/>
       <c r="F45" s="70"/>
-      <c r="G45" s="78"/>
+      <c r="G45" s="72"/>
     </row>
     <row r="46" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C46" s="34" t="s">
         <v>386</v>
       </c>
-      <c r="D46" s="71"/>
+      <c r="D46" s="69"/>
       <c r="E46" s="70"/>
       <c r="F46" s="70"/>
-      <c r="G46" s="78"/>
+      <c r="G46" s="72"/>
       <c r="J46" s="36"/>
       <c r="K46" s="36"/>
       <c r="L46" s="36"/>
@@ -12700,14 +12744,14 @@
       <c r="C47" s="33" t="s">
         <v>464</v>
       </c>
-      <c r="D47" s="72" t="s">
+      <c r="D47" s="73" t="s">
         <v>465</v>
       </c>
       <c r="E47" s="74"/>
       <c r="F47" s="74" t="s">
         <v>584</v>
       </c>
-      <c r="G47" s="76" t="s">
+      <c r="G47" s="75" t="s">
         <v>585</v>
       </c>
       <c r="J47" s="36"/>
@@ -12719,10 +12763,10 @@
       <c r="C48" s="35" t="s">
         <v>467</v>
       </c>
-      <c r="D48" s="73"/>
-      <c r="E48" s="75"/>
-      <c r="F48" s="75"/>
-      <c r="G48" s="77"/>
+      <c r="D48" s="76"/>
+      <c r="E48" s="77"/>
+      <c r="F48" s="77"/>
+      <c r="G48" s="78"/>
       <c r="J48" s="36"/>
       <c r="K48" s="36"/>
       <c r="L48" s="36"/>
@@ -14262,7 +14306,7 @@
       <c r="C151" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="D151" s="71" t="s">
+      <c r="D151" s="69" t="s">
         <v>38</v>
       </c>
       <c r="E151" s="70"/>
@@ -14281,7 +14325,7 @@
       <c r="C152" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D152" s="71"/>
+      <c r="D152" s="69"/>
       <c r="E152" s="70"/>
       <c r="F152" s="70"/>
       <c r="G152" s="38" t="s">
@@ -14296,7 +14340,7 @@
       <c r="C153" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D153" s="71"/>
+      <c r="D153" s="69"/>
       <c r="E153" s="70"/>
       <c r="F153" s="70"/>
       <c r="G153" s="38" t="s">
@@ -14311,7 +14355,7 @@
       <c r="C154" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="D154" s="71" t="s">
+      <c r="D154" s="69" t="s">
         <v>48</v>
       </c>
       <c r="E154" s="70"/>
@@ -14330,7 +14374,7 @@
       <c r="C155" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D155" s="71"/>
+      <c r="D155" s="69"/>
       <c r="E155" s="70"/>
       <c r="F155" s="70"/>
       <c r="G155" s="38" t="s">
@@ -14345,7 +14389,7 @@
       <c r="C156" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D156" s="71" t="s">
+      <c r="D156" s="69" t="s">
         <v>53</v>
       </c>
       <c r="E156" s="70"/>
@@ -14364,7 +14408,7 @@
       <c r="C157" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D157" s="71"/>
+      <c r="D157" s="69"/>
       <c r="E157" s="70"/>
       <c r="F157" s="70"/>
       <c r="G157" s="38" t="s">
@@ -14379,7 +14423,7 @@
       <c r="C158" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D158" s="71" t="s">
+      <c r="D158" s="69" t="s">
         <v>78</v>
       </c>
       <c r="E158" s="70"/>
@@ -14398,7 +14442,7 @@
       <c r="C159" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D159" s="71"/>
+      <c r="D159" s="69"/>
       <c r="E159" s="70"/>
       <c r="F159" s="70"/>
       <c r="G159" s="38" t="s">
@@ -14413,7 +14457,7 @@
       <c r="C160" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="D160" s="71" t="s">
+      <c r="D160" s="69" t="s">
         <v>71</v>
       </c>
       <c r="E160" s="70"/>
@@ -14432,7 +14476,7 @@
       <c r="C161" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D161" s="71"/>
+      <c r="D161" s="69"/>
       <c r="E161" s="70"/>
       <c r="F161" s="70"/>
       <c r="G161" s="38" t="s">
@@ -14447,7 +14491,7 @@
       <c r="C162" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D162" s="71" t="s">
+      <c r="D162" s="69" t="s">
         <v>105</v>
       </c>
       <c r="E162" s="70"/>
@@ -14466,7 +14510,7 @@
       <c r="C163" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D163" s="71"/>
+      <c r="D163" s="69"/>
       <c r="E163" s="70"/>
       <c r="F163" s="70"/>
       <c r="G163" s="38" t="s">
@@ -14481,7 +14525,7 @@
       <c r="C164" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="D164" s="71" t="s">
+      <c r="D164" s="69" t="s">
         <v>171</v>
       </c>
       <c r="E164" s="70"/>
@@ -14500,7 +14544,7 @@
       <c r="C165" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="D165" s="71"/>
+      <c r="D165" s="69"/>
       <c r="E165" s="70"/>
       <c r="F165" s="70"/>
       <c r="G165" s="38" t="s">
@@ -14515,7 +14559,7 @@
       <c r="C166" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="D166" s="71"/>
+      <c r="D166" s="69"/>
       <c r="E166" s="70"/>
       <c r="F166" s="70"/>
       <c r="G166" s="38" t="s">
@@ -14530,7 +14574,7 @@
       <c r="C167" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="D167" s="71" t="s">
+      <c r="D167" s="69" t="s">
         <v>204</v>
       </c>
       <c r="E167" s="70"/>
@@ -14549,7 +14593,7 @@
       <c r="C168" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="D168" s="71"/>
+      <c r="D168" s="69"/>
       <c r="E168" s="70"/>
       <c r="F168" s="70"/>
       <c r="G168" s="38" t="s">
@@ -14564,7 +14608,7 @@
       <c r="C169" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="D169" s="71" t="s">
+      <c r="D169" s="69" t="s">
         <v>300</v>
       </c>
       <c r="E169" s="70"/>
@@ -14583,7 +14627,7 @@
       <c r="C170" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="D170" s="71"/>
+      <c r="D170" s="69"/>
       <c r="E170" s="70"/>
       <c r="F170" s="70"/>
       <c r="G170" s="38" t="s">
@@ -14598,7 +14642,7 @@
       <c r="C171" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="D171" s="71" t="s">
+      <c r="D171" s="69" t="s">
         <v>305</v>
       </c>
       <c r="E171" s="70"/>
@@ -14617,7 +14661,7 @@
       <c r="C172" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="D172" s="71"/>
+      <c r="D172" s="69"/>
       <c r="E172" s="70"/>
       <c r="F172" s="70"/>
       <c r="G172" s="38" t="s">
@@ -14632,7 +14676,7 @@
       <c r="C173" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="D173" s="71"/>
+      <c r="D173" s="69"/>
       <c r="E173" s="70"/>
       <c r="F173" s="70"/>
       <c r="G173" s="38" t="s">
@@ -14647,7 +14691,7 @@
       <c r="C174" s="34" t="s">
         <v>311</v>
       </c>
-      <c r="D174" s="71"/>
+      <c r="D174" s="69"/>
       <c r="E174" s="70"/>
       <c r="F174" s="70"/>
       <c r="G174" s="38" t="s">
@@ -14662,7 +14706,7 @@
       <c r="C175" s="34" t="s">
         <v>317</v>
       </c>
-      <c r="D175" s="71" t="s">
+      <c r="D175" s="69" t="s">
         <v>318</v>
       </c>
       <c r="E175" s="70"/>
@@ -14681,7 +14725,7 @@
       <c r="C176" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="D176" s="71"/>
+      <c r="D176" s="69"/>
       <c r="E176" s="70"/>
       <c r="F176" s="70"/>
       <c r="G176" s="38" t="s">
@@ -14696,7 +14740,7 @@
       <c r="C177" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="D177" s="79" t="s">
+      <c r="D177" s="71" t="s">
         <v>323</v>
       </c>
       <c r="E177" s="70"/>
@@ -14715,7 +14759,7 @@
       <c r="C178" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="D178" s="79"/>
+      <c r="D178" s="71"/>
       <c r="E178" s="70"/>
       <c r="F178" s="70"/>
       <c r="G178" s="38" t="s">
@@ -14726,7 +14770,7 @@
       <c r="C179" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="D179" s="71" t="s">
+      <c r="D179" s="69" t="s">
         <v>328</v>
       </c>
       <c r="E179" s="70"/>
@@ -14741,7 +14785,7 @@
       <c r="C180" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="D180" s="71"/>
+      <c r="D180" s="69"/>
       <c r="E180" s="70"/>
       <c r="F180" s="70"/>
       <c r="G180" s="38" t="s">
@@ -14752,7 +14796,7 @@
       <c r="C181" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="D181" s="71" t="s">
+      <c r="D181" s="69" t="s">
         <v>333</v>
       </c>
       <c r="E181" s="70"/>
@@ -14767,7 +14811,7 @@
       <c r="C182" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="D182" s="71"/>
+      <c r="D182" s="69"/>
       <c r="E182" s="70"/>
       <c r="F182" s="70"/>
       <c r="G182" s="38" t="s">
@@ -14778,7 +14822,7 @@
       <c r="C183" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="D183" s="71" t="s">
+      <c r="D183" s="69" t="s">
         <v>338</v>
       </c>
       <c r="E183" s="70"/>
@@ -14793,7 +14837,7 @@
       <c r="C184" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="D184" s="71"/>
+      <c r="D184" s="69"/>
       <c r="E184" s="70"/>
       <c r="F184" s="70"/>
       <c r="G184" s="38" t="s">
@@ -14804,7 +14848,7 @@
       <c r="C185" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="D185" s="71" t="s">
+      <c r="D185" s="69" t="s">
         <v>343</v>
       </c>
       <c r="E185" s="70"/>
@@ -14819,7 +14863,7 @@
       <c r="C186" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="D186" s="71"/>
+      <c r="D186" s="69"/>
       <c r="E186" s="70"/>
       <c r="F186" s="70"/>
       <c r="G186" s="38" t="s">
@@ -14830,7 +14874,7 @@
       <c r="C187" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="D187" s="71" t="s">
+      <c r="D187" s="69" t="s">
         <v>348</v>
       </c>
       <c r="E187" s="70"/>
@@ -14845,7 +14889,7 @@
       <c r="C188" s="34" t="s">
         <v>350</v>
       </c>
-      <c r="D188" s="71"/>
+      <c r="D188" s="69"/>
       <c r="E188" s="70"/>
       <c r="F188" s="70"/>
       <c r="G188" s="38" t="s">
@@ -14856,7 +14900,7 @@
       <c r="C189" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="D189" s="71" t="s">
+      <c r="D189" s="69" t="s">
         <v>361</v>
       </c>
       <c r="E189" s="70"/>
@@ -14871,7 +14915,7 @@
       <c r="C190" s="34" t="s">
         <v>363</v>
       </c>
-      <c r="D190" s="71"/>
+      <c r="D190" s="69"/>
       <c r="E190" s="70"/>
       <c r="F190" s="70"/>
       <c r="G190" s="38" t="s">
@@ -14882,7 +14926,7 @@
       <c r="C191" s="34" t="s">
         <v>365</v>
       </c>
-      <c r="D191" s="71" t="s">
+      <c r="D191" s="69" t="s">
         <v>366</v>
       </c>
       <c r="E191" s="70"/>
@@ -14897,7 +14941,7 @@
       <c r="C192" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="D192" s="71"/>
+      <c r="D192" s="69"/>
       <c r="E192" s="70"/>
       <c r="F192" s="70"/>
       <c r="G192" s="38" t="s">
@@ -14908,7 +14952,7 @@
       <c r="C193" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="D193" s="71"/>
+      <c r="D193" s="69"/>
       <c r="E193" s="70"/>
       <c r="F193" s="70"/>
       <c r="G193" s="38" t="s">
@@ -14919,7 +14963,7 @@
       <c r="C194" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="D194" s="71" t="s">
+      <c r="D194" s="69" t="s">
         <v>371</v>
       </c>
       <c r="E194" s="70"/>
@@ -14934,7 +14978,7 @@
       <c r="C195" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="D195" s="71"/>
+      <c r="D195" s="69"/>
       <c r="E195" s="70"/>
       <c r="F195" s="70"/>
       <c r="G195" s="38" t="s">
@@ -14945,7 +14989,7 @@
       <c r="C196" s="34" t="s">
         <v>384</v>
       </c>
-      <c r="D196" s="71"/>
+      <c r="D196" s="69"/>
       <c r="E196" s="70"/>
       <c r="F196" s="70"/>
       <c r="G196" s="38" t="s">
@@ -14957,7 +15001,7 @@
       <c r="C197" s="36" t="s">
         <v>373</v>
       </c>
-      <c r="D197" s="71" t="s">
+      <c r="D197" s="69" t="s">
         <v>374</v>
       </c>
       <c r="E197" s="70"/>
@@ -14973,7 +15017,7 @@
       <c r="C198" s="36" t="s">
         <v>380</v>
       </c>
-      <c r="D198" s="71"/>
+      <c r="D198" s="69"/>
       <c r="E198" s="70"/>
       <c r="F198" s="70"/>
       <c r="G198" s="38" t="s">
@@ -14985,7 +15029,7 @@
       <c r="C199" s="36" t="s">
         <v>386</v>
       </c>
-      <c r="D199" s="71"/>
+      <c r="D199" s="69"/>
       <c r="E199" s="70"/>
       <c r="F199" s="70"/>
       <c r="G199" s="38" t="s">
@@ -15000,7 +15044,7 @@
       <c r="C200" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="D200" s="71" t="s">
+      <c r="D200" s="69" t="s">
         <v>65</v>
       </c>
       <c r="E200" s="70"/>
@@ -15016,7 +15060,7 @@
       <c r="C201" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="D201" s="71"/>
+      <c r="D201" s="69"/>
       <c r="E201" s="70"/>
       <c r="F201" s="70"/>
       <c r="G201" s="38" t="s">
@@ -15027,7 +15071,7 @@
       <c r="C202" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="D202" s="71" t="s">
+      <c r="D202" s="69" t="s">
         <v>110</v>
       </c>
       <c r="E202" s="70"/>
@@ -15042,7 +15086,7 @@
       <c r="C203" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="D203" s="71"/>
+      <c r="D203" s="69"/>
       <c r="E203" s="70"/>
       <c r="F203" s="70"/>
       <c r="G203" s="38" t="s">
@@ -15053,7 +15097,7 @@
       <c r="C204" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="D204" s="71"/>
+      <c r="D204" s="69"/>
       <c r="E204" s="70"/>
       <c r="F204" s="70"/>
       <c r="G204" s="38" t="s">
@@ -15064,7 +15108,7 @@
       <c r="C205" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="D205" s="71" t="s">
+      <c r="D205" s="69" t="s">
         <v>119</v>
       </c>
       <c r="E205" s="70"/>
@@ -15079,7 +15123,7 @@
       <c r="C206" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="D206" s="71"/>
+      <c r="D206" s="69"/>
       <c r="E206" s="70"/>
       <c r="F206" s="70"/>
       <c r="G206" s="38" t="s">
@@ -15090,7 +15134,7 @@
       <c r="C207" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="D207" s="71" t="s">
+      <c r="D207" s="69" t="s">
         <v>124</v>
       </c>
       <c r="E207" s="70"/>
@@ -15105,7 +15149,7 @@
       <c r="C208" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="D208" s="71"/>
+      <c r="D208" s="69"/>
       <c r="E208" s="70"/>
       <c r="F208" s="70"/>
       <c r="G208" s="38" t="s">
@@ -15116,7 +15160,7 @@
       <c r="C209" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="D209" s="71"/>
+      <c r="D209" s="69"/>
       <c r="E209" s="70"/>
       <c r="F209" s="70"/>
       <c r="G209" s="38" t="s">
@@ -15127,7 +15171,7 @@
       <c r="C210" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="D210" s="71" t="s">
+      <c r="D210" s="69" t="s">
         <v>131</v>
       </c>
       <c r="E210" s="70"/>
@@ -15142,7 +15186,7 @@
       <c r="C211" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="D211" s="71"/>
+      <c r="D211" s="69"/>
       <c r="E211" s="70"/>
       <c r="F211" s="70"/>
       <c r="G211" s="38" t="s">
@@ -15153,7 +15197,7 @@
       <c r="C212" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="D212" s="71"/>
+      <c r="D212" s="69"/>
       <c r="E212" s="70"/>
       <c r="F212" s="70"/>
       <c r="G212" s="38" t="s">
@@ -15164,7 +15208,7 @@
       <c r="C213" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="D213" s="71" t="s">
+      <c r="D213" s="69" t="s">
         <v>159</v>
       </c>
       <c r="E213" s="70"/>
@@ -15179,7 +15223,7 @@
       <c r="C214" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="D214" s="71"/>
+      <c r="D214" s="69"/>
       <c r="E214" s="70"/>
       <c r="F214" s="70"/>
       <c r="G214" s="38" t="s">
@@ -15190,7 +15234,7 @@
       <c r="C215" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="D215" s="71" t="s">
+      <c r="D215" s="69" t="s">
         <v>164</v>
       </c>
       <c r="E215" s="70"/>
@@ -15205,7 +15249,7 @@
       <c r="C216" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="D216" s="71"/>
+      <c r="D216" s="69"/>
       <c r="E216" s="70"/>
       <c r="F216" s="70"/>
       <c r="G216" s="38" t="s">
@@ -15216,7 +15260,7 @@
       <c r="C217" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="D217" s="71"/>
+      <c r="D217" s="69"/>
       <c r="E217" s="70"/>
       <c r="F217" s="70"/>
       <c r="G217" s="38" t="s">
@@ -15227,7 +15271,7 @@
       <c r="C218" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="D218" s="71" t="s">
+      <c r="D218" s="69" t="s">
         <v>179</v>
       </c>
       <c r="E218" s="70"/>
@@ -15242,7 +15286,7 @@
       <c r="C219" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="D219" s="71"/>
+      <c r="D219" s="69"/>
       <c r="E219" s="70"/>
       <c r="F219" s="70"/>
       <c r="G219" s="38" t="s">
@@ -15253,7 +15297,7 @@
       <c r="C220" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="D220" s="71"/>
+      <c r="D220" s="69"/>
       <c r="E220" s="70"/>
       <c r="F220" s="70"/>
       <c r="G220" s="38" t="s">
@@ -15264,7 +15308,7 @@
       <c r="C221" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="D221" s="71" t="s">
+      <c r="D221" s="69" t="s">
         <v>186</v>
       </c>
       <c r="E221" s="70"/>
@@ -15279,7 +15323,7 @@
       <c r="C222" s="34" t="s">
         <v>188</v>
       </c>
-      <c r="D222" s="71"/>
+      <c r="D222" s="69"/>
       <c r="E222" s="70"/>
       <c r="F222" s="70"/>
       <c r="G222" s="38" t="s">
@@ -15290,7 +15334,7 @@
       <c r="C223" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="D223" s="71" t="s">
+      <c r="D223" s="69" t="s">
         <v>195</v>
       </c>
       <c r="E223" s="70"/>
@@ -15305,7 +15349,7 @@
       <c r="C224" s="34" t="s">
         <v>197</v>
       </c>
-      <c r="D224" s="71"/>
+      <c r="D224" s="69"/>
       <c r="E224" s="70"/>
       <c r="F224" s="70"/>
       <c r="G224" s="38" t="s">
@@ -15316,7 +15360,7 @@
       <c r="C225" s="34" t="s">
         <v>199</v>
       </c>
-      <c r="D225" s="71" t="s">
+      <c r="D225" s="69" t="s">
         <v>200</v>
       </c>
       <c r="E225" s="70"/>
@@ -15331,7 +15375,7 @@
       <c r="C226" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="D226" s="71"/>
+      <c r="D226" s="69"/>
       <c r="E226" s="70"/>
       <c r="F226" s="70"/>
       <c r="G226" s="38" t="s">
@@ -15342,7 +15386,7 @@
       <c r="C227" s="34" t="s">
         <v>210</v>
       </c>
-      <c r="D227" s="71" t="s">
+      <c r="D227" s="69" t="s">
         <v>211</v>
       </c>
       <c r="E227" s="70"/>
@@ -15357,7 +15401,7 @@
       <c r="C228" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="D228" s="71"/>
+      <c r="D228" s="69"/>
       <c r="E228" s="70"/>
       <c r="F228" s="70"/>
       <c r="G228" s="38" t="s">
@@ -15368,7 +15412,7 @@
       <c r="C229" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="D229" s="71"/>
+      <c r="D229" s="69"/>
       <c r="E229" s="70"/>
       <c r="F229" s="70"/>
       <c r="G229" s="38" t="s">
@@ -15379,7 +15423,7 @@
       <c r="C230" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="D230" s="71" t="s">
+      <c r="D230" s="69" t="s">
         <v>223</v>
       </c>
       <c r="E230" s="70"/>
@@ -15394,7 +15438,7 @@
       <c r="C231" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="D231" s="71"/>
+      <c r="D231" s="69"/>
       <c r="E231" s="70"/>
       <c r="F231" s="70"/>
       <c r="G231" s="38" t="s">
@@ -15405,7 +15449,7 @@
       <c r="C232" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="D232" s="71" t="s">
+      <c r="D232" s="69" t="s">
         <v>228</v>
       </c>
       <c r="E232" s="70"/>
@@ -15420,7 +15464,7 @@
       <c r="C233" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="D233" s="71"/>
+      <c r="D233" s="69"/>
       <c r="E233" s="70"/>
       <c r="F233" s="70"/>
       <c r="G233" s="38" t="s">
@@ -15431,7 +15475,7 @@
       <c r="C234" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="D234" s="71"/>
+      <c r="D234" s="69"/>
       <c r="E234" s="70"/>
       <c r="F234" s="70"/>
       <c r="G234" s="38" t="s">
@@ -15502,7 +15546,7 @@
       <c r="C239" s="34" t="s">
         <v>454</v>
       </c>
-      <c r="D239" s="71" t="s">
+      <c r="D239" s="69" t="s">
         <v>582</v>
       </c>
       <c r="E239" s="70"/>
@@ -15517,7 +15561,7 @@
       <c r="C240" s="34" t="s">
         <v>457</v>
       </c>
-      <c r="D240" s="71"/>
+      <c r="D240" s="69"/>
       <c r="E240" s="70"/>
       <c r="F240" s="70"/>
       <c r="G240" s="38" t="s">
@@ -15528,7 +15572,7 @@
       <c r="C241" s="34" t="s">
         <v>459</v>
       </c>
-      <c r="D241" s="71" t="s">
+      <c r="D241" s="69" t="s">
         <v>460</v>
       </c>
       <c r="E241" s="70"/>
@@ -15543,7 +15587,7 @@
       <c r="C242" s="34" t="s">
         <v>462</v>
       </c>
-      <c r="D242" s="71"/>
+      <c r="D242" s="69"/>
       <c r="E242" s="70"/>
       <c r="F242" s="70"/>
       <c r="G242" s="38" t="s">
@@ -15601,7 +15645,7 @@
       <c r="C246" s="34" t="s">
         <v>477</v>
       </c>
-      <c r="D246" s="71" t="s">
+      <c r="D246" s="69" t="s">
         <v>478</v>
       </c>
       <c r="E246" s="70"/>
@@ -15619,9 +15663,9 @@
       <c r="C247" s="35" t="s">
         <v>480</v>
       </c>
-      <c r="D247" s="73"/>
-      <c r="E247" s="75"/>
-      <c r="F247" s="75"/>
+      <c r="D247" s="76"/>
+      <c r="E247" s="77"/>
+      <c r="F247" s="77"/>
       <c r="G247" s="39" t="s">
         <v>33</v>
       </c>
@@ -15685,6 +15729,183 @@
     </row>
   </sheetData>
   <mergeCells count="201">
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="D197:D199"/>
+    <mergeCell ref="E197:E199"/>
+    <mergeCell ref="F197:F199"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="D154:D155"/>
+    <mergeCell ref="E154:E155"/>
+    <mergeCell ref="F154:F155"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="D246:D247"/>
+    <mergeCell ref="E246:E247"/>
+    <mergeCell ref="F246:F247"/>
+    <mergeCell ref="D230:D231"/>
+    <mergeCell ref="E230:E231"/>
+    <mergeCell ref="F230:F231"/>
+    <mergeCell ref="D232:D234"/>
+    <mergeCell ref="E232:E234"/>
+    <mergeCell ref="F232:F234"/>
+    <mergeCell ref="D239:D240"/>
+    <mergeCell ref="D241:D242"/>
+    <mergeCell ref="F239:F240"/>
+    <mergeCell ref="F241:F242"/>
+    <mergeCell ref="E239:E240"/>
+    <mergeCell ref="E241:E242"/>
+    <mergeCell ref="D225:D226"/>
+    <mergeCell ref="E225:E226"/>
+    <mergeCell ref="F225:F226"/>
+    <mergeCell ref="D227:D229"/>
+    <mergeCell ref="E227:E229"/>
+    <mergeCell ref="F227:F229"/>
+    <mergeCell ref="D221:D222"/>
+    <mergeCell ref="E221:E222"/>
+    <mergeCell ref="F221:F222"/>
+    <mergeCell ref="D223:D224"/>
+    <mergeCell ref="E223:E224"/>
+    <mergeCell ref="F223:F224"/>
+    <mergeCell ref="D215:D217"/>
+    <mergeCell ref="E215:E217"/>
+    <mergeCell ref="F215:F217"/>
+    <mergeCell ref="D218:D220"/>
+    <mergeCell ref="E218:E220"/>
+    <mergeCell ref="F218:F220"/>
+    <mergeCell ref="D210:D212"/>
+    <mergeCell ref="E210:E212"/>
+    <mergeCell ref="F210:F212"/>
+    <mergeCell ref="D213:D214"/>
+    <mergeCell ref="E213:E214"/>
+    <mergeCell ref="F213:F214"/>
+    <mergeCell ref="D205:D206"/>
+    <mergeCell ref="E205:E206"/>
+    <mergeCell ref="F205:F206"/>
+    <mergeCell ref="D207:D209"/>
+    <mergeCell ref="E207:E209"/>
+    <mergeCell ref="F207:F209"/>
+    <mergeCell ref="D200:D201"/>
+    <mergeCell ref="E200:E201"/>
+    <mergeCell ref="F200:F201"/>
+    <mergeCell ref="D202:D204"/>
+    <mergeCell ref="E202:E204"/>
+    <mergeCell ref="F202:F204"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="E41:E43"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="G41:G43"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="D151:D153"/>
+    <mergeCell ref="D156:D157"/>
+    <mergeCell ref="D158:D159"/>
+    <mergeCell ref="D164:D166"/>
+    <mergeCell ref="D167:D168"/>
+    <mergeCell ref="F164:F166"/>
+    <mergeCell ref="D160:D161"/>
+    <mergeCell ref="D162:D163"/>
+    <mergeCell ref="F151:F153"/>
+    <mergeCell ref="E167:E168"/>
+    <mergeCell ref="F167:F168"/>
+    <mergeCell ref="E164:E166"/>
+    <mergeCell ref="F181:F182"/>
+    <mergeCell ref="F183:F184"/>
+    <mergeCell ref="F185:F186"/>
+    <mergeCell ref="E189:E190"/>
+    <mergeCell ref="F187:F188"/>
+    <mergeCell ref="D187:D188"/>
+    <mergeCell ref="D189:D190"/>
+    <mergeCell ref="D169:D170"/>
+    <mergeCell ref="E175:E176"/>
+    <mergeCell ref="E177:E178"/>
+    <mergeCell ref="E179:E180"/>
+    <mergeCell ref="E181:E182"/>
+    <mergeCell ref="E183:E184"/>
+    <mergeCell ref="E185:E186"/>
+    <mergeCell ref="E187:E188"/>
+    <mergeCell ref="F169:F170"/>
+    <mergeCell ref="E171:E174"/>
+    <mergeCell ref="F171:F174"/>
+    <mergeCell ref="F175:F176"/>
+    <mergeCell ref="F177:F178"/>
+    <mergeCell ref="F179:F180"/>
     <mergeCell ref="D191:D193"/>
     <mergeCell ref="E191:E193"/>
     <mergeCell ref="F191:F193"/>
@@ -15709,183 +15930,6 @@
     <mergeCell ref="D185:D186"/>
     <mergeCell ref="F189:F190"/>
     <mergeCell ref="E169:E170"/>
-    <mergeCell ref="F181:F182"/>
-    <mergeCell ref="F183:F184"/>
-    <mergeCell ref="F185:F186"/>
-    <mergeCell ref="E189:E190"/>
-    <mergeCell ref="F187:F188"/>
-    <mergeCell ref="D187:D188"/>
-    <mergeCell ref="D189:D190"/>
-    <mergeCell ref="D169:D170"/>
-    <mergeCell ref="E175:E176"/>
-    <mergeCell ref="E177:E178"/>
-    <mergeCell ref="E179:E180"/>
-    <mergeCell ref="E181:E182"/>
-    <mergeCell ref="E183:E184"/>
-    <mergeCell ref="E185:E186"/>
-    <mergeCell ref="E187:E188"/>
-    <mergeCell ref="F169:F170"/>
-    <mergeCell ref="E171:E174"/>
-    <mergeCell ref="F171:F174"/>
-    <mergeCell ref="F175:F176"/>
-    <mergeCell ref="F177:F178"/>
-    <mergeCell ref="F179:F180"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="D151:D153"/>
-    <mergeCell ref="D156:D157"/>
-    <mergeCell ref="D158:D159"/>
-    <mergeCell ref="D164:D166"/>
-    <mergeCell ref="D167:D168"/>
-    <mergeCell ref="F164:F166"/>
-    <mergeCell ref="D160:D161"/>
-    <mergeCell ref="D162:D163"/>
-    <mergeCell ref="F151:F153"/>
-    <mergeCell ref="E167:E168"/>
-    <mergeCell ref="F167:F168"/>
-    <mergeCell ref="E164:E166"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="G41:G43"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="D205:D206"/>
-    <mergeCell ref="E205:E206"/>
-    <mergeCell ref="F205:F206"/>
-    <mergeCell ref="D207:D209"/>
-    <mergeCell ref="E207:E209"/>
-    <mergeCell ref="F207:F209"/>
-    <mergeCell ref="D200:D201"/>
-    <mergeCell ref="E200:E201"/>
-    <mergeCell ref="F200:F201"/>
-    <mergeCell ref="D202:D204"/>
-    <mergeCell ref="E202:E204"/>
-    <mergeCell ref="F202:F204"/>
-    <mergeCell ref="D215:D217"/>
-    <mergeCell ref="E215:E217"/>
-    <mergeCell ref="F215:F217"/>
-    <mergeCell ref="D218:D220"/>
-    <mergeCell ref="E218:E220"/>
-    <mergeCell ref="F218:F220"/>
-    <mergeCell ref="D210:D212"/>
-    <mergeCell ref="E210:E212"/>
-    <mergeCell ref="F210:F212"/>
-    <mergeCell ref="D213:D214"/>
-    <mergeCell ref="E213:E214"/>
-    <mergeCell ref="F213:F214"/>
-    <mergeCell ref="D225:D226"/>
-    <mergeCell ref="E225:E226"/>
-    <mergeCell ref="F225:F226"/>
-    <mergeCell ref="D227:D229"/>
-    <mergeCell ref="E227:E229"/>
-    <mergeCell ref="F227:F229"/>
-    <mergeCell ref="D221:D222"/>
-    <mergeCell ref="E221:E222"/>
-    <mergeCell ref="F221:F222"/>
-    <mergeCell ref="D223:D224"/>
-    <mergeCell ref="E223:E224"/>
-    <mergeCell ref="F223:F224"/>
-    <mergeCell ref="D246:D247"/>
-    <mergeCell ref="E246:E247"/>
-    <mergeCell ref="F246:F247"/>
-    <mergeCell ref="D230:D231"/>
-    <mergeCell ref="E230:E231"/>
-    <mergeCell ref="F230:F231"/>
-    <mergeCell ref="D232:D234"/>
-    <mergeCell ref="E232:E234"/>
-    <mergeCell ref="F232:F234"/>
-    <mergeCell ref="D239:D240"/>
-    <mergeCell ref="D241:D242"/>
-    <mergeCell ref="F239:F240"/>
-    <mergeCell ref="F241:F242"/>
-    <mergeCell ref="E239:E240"/>
-    <mergeCell ref="E241:E242"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="D197:D199"/>
-    <mergeCell ref="E197:E199"/>
-    <mergeCell ref="F197:F199"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="D154:D155"/>
-    <mergeCell ref="E154:E155"/>
-    <mergeCell ref="F154:F155"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -16800,7 +16844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0658980E-FDBF-4B6D-A13D-5531F4808D66}">
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
@@ -16851,9 +16895,9 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="O3" s="82"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="O3" s="68"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -16865,9 +16909,9 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="L4" s="82"/>
-      <c r="M4" s="82"/>
-      <c r="O4" s="82"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="68"/>
+      <c r="O4" s="68"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -16879,9 +16923,9 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="L5" s="82"/>
-      <c r="M5" s="82"/>
-      <c r="O5" s="82"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="68"/>
+      <c r="O5" s="68"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -16893,9 +16937,9 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="L6" s="82"/>
-      <c r="M6" s="82"/>
-      <c r="O6" s="82"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="68"/>
+      <c r="O6" s="68"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -16907,9 +16951,9 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="L7" s="82"/>
-      <c r="M7" s="82"/>
-      <c r="O7" s="82"/>
+      <c r="L7" s="68"/>
+      <c r="M7" s="68"/>
+      <c r="O7" s="68"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -16921,9 +16965,9 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="L8" s="82"/>
-      <c r="M8" s="82"/>
-      <c r="O8" s="82"/>
+      <c r="L8" s="68"/>
+      <c r="M8" s="68"/>
+      <c r="O8" s="68"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -16935,9 +16979,9 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="L9" s="82"/>
-      <c r="M9" s="82"/>
-      <c r="O9" s="82"/>
+      <c r="L9" s="68"/>
+      <c r="M9" s="68"/>
+      <c r="O9" s="68"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -16949,9 +16993,9 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="L10" s="82"/>
-      <c r="M10" s="82"/>
-      <c r="O10" s="82"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="68"/>
+      <c r="O10" s="68"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -16963,9 +17007,9 @@
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="L11" s="82"/>
-      <c r="M11" s="82"/>
-      <c r="O11" s="82"/>
+      <c r="L11" s="68"/>
+      <c r="M11" s="68"/>
+      <c r="O11" s="68"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -16977,9 +17021,9 @@
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="L12" s="82"/>
-      <c r="M12" s="82"/>
-      <c r="O12" s="82"/>
+      <c r="L12" s="68"/>
+      <c r="M12" s="68"/>
+      <c r="O12" s="68"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -16991,9 +17035,9 @@
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="L13" s="82"/>
-      <c r="M13" s="82"/>
-      <c r="O13" s="82"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="68"/>
+      <c r="O13" s="68"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -17005,9 +17049,9 @@
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="L14" s="82"/>
-      <c r="M14" s="82"/>
-      <c r="O14" s="82"/>
+      <c r="L14" s="68"/>
+      <c r="M14" s="68"/>
+      <c r="O14" s="68"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -17019,9 +17063,9 @@
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="L15" s="82"/>
-      <c r="M15" s="82"/>
-      <c r="O15" s="82"/>
+      <c r="L15" s="68"/>
+      <c r="M15" s="68"/>
+      <c r="O15" s="68"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -17033,9 +17077,9 @@
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="L16" s="82"/>
-      <c r="M16" s="82"/>
-      <c r="O16" s="82"/>
+      <c r="L16" s="68"/>
+      <c r="M16" s="68"/>
+      <c r="O16" s="68"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -17047,9 +17091,9 @@
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="L17" s="82"/>
-      <c r="M17" s="82"/>
-      <c r="O17" s="82"/>
+      <c r="L17" s="68"/>
+      <c r="M17" s="68"/>
+      <c r="O17" s="68"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -17061,9 +17105,9 @@
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="L18" s="82"/>
-      <c r="M18" s="82"/>
-      <c r="O18" s="82"/>
+      <c r="L18" s="68"/>
+      <c r="M18" s="68"/>
+      <c r="O18" s="68"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -17075,9 +17119,9 @@
       <c r="C19">
         <v>1</v>
       </c>
-      <c r="L19" s="82"/>
-      <c r="M19" s="82"/>
-      <c r="O19" s="82"/>
+      <c r="L19" s="68"/>
+      <c r="M19" s="68"/>
+      <c r="O19" s="68"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -17089,9 +17133,9 @@
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="L20" s="82"/>
-      <c r="M20" s="82"/>
-      <c r="O20" s="82"/>
+      <c r="L20" s="68"/>
+      <c r="M20" s="68"/>
+      <c r="O20" s="68"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -17103,9 +17147,9 @@
       <c r="C21">
         <v>1</v>
       </c>
-      <c r="L21" s="82"/>
-      <c r="M21" s="82"/>
-      <c r="O21" s="82"/>
+      <c r="L21" s="68"/>
+      <c r="M21" s="68"/>
+      <c r="O21" s="68"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -17117,9 +17161,9 @@
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="L22" s="82"/>
-      <c r="M22" s="82"/>
-      <c r="O22" s="82"/>
+      <c r="L22" s="68"/>
+      <c r="M22" s="68"/>
+      <c r="O22" s="68"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -17131,9 +17175,9 @@
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="L23" s="82"/>
-      <c r="M23" s="82"/>
-      <c r="O23" s="82"/>
+      <c r="L23" s="68"/>
+      <c r="M23" s="68"/>
+      <c r="O23" s="68"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -17145,9 +17189,9 @@
       <c r="C24">
         <v>1</v>
       </c>
-      <c r="L24" s="82"/>
-      <c r="M24" s="82"/>
-      <c r="O24" s="82"/>
+      <c r="L24" s="68"/>
+      <c r="M24" s="68"/>
+      <c r="O24" s="68"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -17159,9 +17203,9 @@
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="L25" s="82"/>
-      <c r="M25" s="82"/>
-      <c r="O25" s="82"/>
+      <c r="L25" s="68"/>
+      <c r="M25" s="68"/>
+      <c r="O25" s="68"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -17173,9 +17217,9 @@
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="L26" s="82"/>
-      <c r="M26" s="82"/>
-      <c r="O26" s="82"/>
+      <c r="L26" s="68"/>
+      <c r="M26" s="68"/>
+      <c r="O26" s="68"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -17187,9 +17231,9 @@
       <c r="C27">
         <v>1</v>
       </c>
-      <c r="L27" s="82"/>
-      <c r="M27" s="82"/>
-      <c r="O27" s="82"/>
+      <c r="L27" s="68"/>
+      <c r="M27" s="68"/>
+      <c r="O27" s="68"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -17201,9 +17245,9 @@
       <c r="C28">
         <v>1</v>
       </c>
-      <c r="L28" s="82"/>
-      <c r="M28" s="82"/>
-      <c r="O28" s="82"/>
+      <c r="L28" s="68"/>
+      <c r="M28" s="68"/>
+      <c r="O28" s="68"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -17215,9 +17259,9 @@
       <c r="C29">
         <v>1</v>
       </c>
-      <c r="L29" s="82"/>
-      <c r="M29" s="82"/>
-      <c r="O29" s="82"/>
+      <c r="L29" s="68"/>
+      <c r="M29" s="68"/>
+      <c r="O29" s="68"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -17229,9 +17273,9 @@
       <c r="C30">
         <v>1</v>
       </c>
-      <c r="L30" s="82"/>
-      <c r="M30" s="82"/>
-      <c r="O30" s="82"/>
+      <c r="L30" s="68"/>
+      <c r="M30" s="68"/>
+      <c r="O30" s="68"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -17243,9 +17287,9 @@
       <c r="C31">
         <v>1</v>
       </c>
-      <c r="L31" s="82"/>
-      <c r="M31" s="82"/>
-      <c r="O31" s="82"/>
+      <c r="L31" s="68"/>
+      <c r="M31" s="68"/>
+      <c r="O31" s="68"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -17257,9 +17301,9 @@
       <c r="C32">
         <v>1</v>
       </c>
-      <c r="L32" s="82"/>
-      <c r="M32" s="82"/>
-      <c r="O32" s="82"/>
+      <c r="L32" s="68"/>
+      <c r="M32" s="68"/>
+      <c r="O32" s="68"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -17271,9 +17315,9 @@
       <c r="C33">
         <v>1</v>
       </c>
-      <c r="L33" s="82"/>
-      <c r="M33" s="82"/>
-      <c r="O33" s="82"/>
+      <c r="L33" s="68"/>
+      <c r="M33" s="68"/>
+      <c r="O33" s="68"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -17285,9 +17329,9 @@
       <c r="C34">
         <v>1</v>
       </c>
-      <c r="L34" s="82"/>
-      <c r="M34" s="82"/>
-      <c r="O34" s="82"/>
+      <c r="L34" s="68"/>
+      <c r="M34" s="68"/>
+      <c r="O34" s="68"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -17299,9 +17343,9 @@
       <c r="C35">
         <v>1</v>
       </c>
-      <c r="L35" s="82"/>
-      <c r="M35" s="82"/>
-      <c r="O35" s="82"/>
+      <c r="L35" s="68"/>
+      <c r="M35" s="68"/>
+      <c r="O35" s="68"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -17313,9 +17357,9 @@
       <c r="C36">
         <v>1</v>
       </c>
-      <c r="L36" s="82"/>
-      <c r="M36" s="82"/>
-      <c r="O36" s="82"/>
+      <c r="L36" s="68"/>
+      <c r="M36" s="68"/>
+      <c r="O36" s="68"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -17327,9 +17371,9 @@
       <c r="C37">
         <v>1</v>
       </c>
-      <c r="L37" s="82"/>
-      <c r="M37" s="82"/>
-      <c r="O37" s="82"/>
+      <c r="L37" s="68"/>
+      <c r="M37" s="68"/>
+      <c r="O37" s="68"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -17341,9 +17385,9 @@
       <c r="C38">
         <v>1</v>
       </c>
-      <c r="L38" s="82"/>
-      <c r="M38" s="82"/>
-      <c r="O38" s="82"/>
+      <c r="L38" s="68"/>
+      <c r="M38" s="68"/>
+      <c r="O38" s="68"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -17355,9 +17399,9 @@
       <c r="C39">
         <v>1</v>
       </c>
-      <c r="L39" s="82"/>
-      <c r="M39" s="82"/>
-      <c r="O39" s="82"/>
+      <c r="L39" s="68"/>
+      <c r="M39" s="68"/>
+      <c r="O39" s="68"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -17369,9 +17413,9 @@
       <c r="C40">
         <v>1</v>
       </c>
-      <c r="L40" s="82"/>
-      <c r="M40" s="82"/>
-      <c r="O40" s="82"/>
+      <c r="L40" s="68"/>
+      <c r="M40" s="68"/>
+      <c r="O40" s="68"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -17383,9 +17427,9 @@
       <c r="C41">
         <v>1</v>
       </c>
-      <c r="L41" s="82"/>
-      <c r="M41" s="82"/>
-      <c r="O41" s="82"/>
+      <c r="L41" s="68"/>
+      <c r="M41" s="68"/>
+      <c r="O41" s="68"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -17397,9 +17441,9 @@
       <c r="C42">
         <v>1</v>
       </c>
-      <c r="L42" s="82"/>
-      <c r="M42" s="82"/>
-      <c r="O42" s="82"/>
+      <c r="L42" s="68"/>
+      <c r="M42" s="68"/>
+      <c r="O42" s="68"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -17411,9 +17455,9 @@
       <c r="C43">
         <v>1</v>
       </c>
-      <c r="L43" s="82"/>
-      <c r="M43" s="82"/>
-      <c r="O43" s="82"/>
+      <c r="L43" s="68"/>
+      <c r="M43" s="68"/>
+      <c r="O43" s="68"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -17425,9 +17469,9 @@
       <c r="C44">
         <v>1</v>
       </c>
-      <c r="L44" s="82"/>
-      <c r="M44" s="82"/>
-      <c r="O44" s="82"/>
+      <c r="L44" s="68"/>
+      <c r="M44" s="68"/>
+      <c r="O44" s="68"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -17439,9 +17483,9 @@
       <c r="C45">
         <v>1</v>
       </c>
-      <c r="L45" s="82"/>
-      <c r="M45" s="82"/>
-      <c r="O45" s="82"/>
+      <c r="L45" s="68"/>
+      <c r="M45" s="68"/>
+      <c r="O45" s="68"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -17453,9 +17497,9 @@
       <c r="C46">
         <v>1</v>
       </c>
-      <c r="L46" s="82"/>
-      <c r="M46" s="82"/>
-      <c r="O46" s="82"/>
+      <c r="L46" s="68"/>
+      <c r="M46" s="68"/>
+      <c r="O46" s="68"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -17467,9 +17511,9 @@
       <c r="C47">
         <v>64</v>
       </c>
-      <c r="L47" s="82"/>
-      <c r="M47" s="82"/>
-      <c r="O47" s="82"/>
+      <c r="L47" s="68"/>
+      <c r="M47" s="68"/>
+      <c r="O47" s="68"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -17481,9 +17525,9 @@
       <c r="C48">
         <v>1</v>
       </c>
-      <c r="L48" s="82"/>
-      <c r="M48" s="82"/>
-      <c r="O48" s="82"/>
+      <c r="L48" s="68"/>
+      <c r="M48" s="68"/>
+      <c r="O48" s="68"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -17495,9 +17539,9 @@
       <c r="C49">
         <v>1</v>
       </c>
-      <c r="L49" s="82"/>
-      <c r="M49" s="82"/>
-      <c r="O49" s="82"/>
+      <c r="L49" s="68"/>
+      <c r="M49" s="68"/>
+      <c r="O49" s="68"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
@@ -17509,9 +17553,9 @@
       <c r="C50">
         <v>1</v>
       </c>
-      <c r="L50" s="82"/>
-      <c r="M50" s="82"/>
-      <c r="O50" s="82"/>
+      <c r="L50" s="68"/>
+      <c r="M50" s="68"/>
+      <c r="O50" s="68"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -17523,9 +17567,9 @@
       <c r="C51">
         <v>1</v>
       </c>
-      <c r="L51" s="82"/>
-      <c r="M51" s="82"/>
-      <c r="O51" s="82"/>
+      <c r="L51" s="68"/>
+      <c r="M51" s="68"/>
+      <c r="O51" s="68"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
@@ -17537,9 +17581,9 @@
       <c r="C52">
         <v>1</v>
       </c>
-      <c r="L52" s="82"/>
-      <c r="M52" s="82"/>
-      <c r="O52" s="82"/>
+      <c r="L52" s="68"/>
+      <c r="M52" s="68"/>
+      <c r="O52" s="68"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
@@ -17551,9 +17595,9 @@
       <c r="C53">
         <v>1</v>
       </c>
-      <c r="L53" s="82"/>
-      <c r="M53" s="82"/>
-      <c r="O53" s="82"/>
+      <c r="L53" s="68"/>
+      <c r="M53" s="68"/>
+      <c r="O53" s="68"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
@@ -17565,9 +17609,9 @@
       <c r="C54">
         <v>1</v>
       </c>
-      <c r="L54" s="82"/>
-      <c r="M54" s="82"/>
-      <c r="O54" s="82"/>
+      <c r="L54" s="68"/>
+      <c r="M54" s="68"/>
+      <c r="O54" s="68"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17626,7 +17670,7 @@
       <c r="D2" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="81">
+      <c r="E2" s="82">
         <v>101332</v>
       </c>
     </row>
@@ -17643,7 +17687,7 @@
       <c r="D3" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="81"/>
+      <c r="E3" s="82"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -17658,7 +17702,7 @@
       <c r="D4" t="s">
         <v>524</v>
       </c>
-      <c r="E4" s="81">
+      <c r="E4" s="82">
         <v>99343</v>
       </c>
     </row>
@@ -17675,7 +17719,7 @@
       <c r="D5" t="s">
         <v>524</v>
       </c>
-      <c r="E5" s="81"/>
+      <c r="E5" s="82"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -17690,7 +17734,7 @@
       <c r="D6" t="s">
         <v>516</v>
       </c>
-      <c r="E6" s="81">
+      <c r="E6" s="82">
         <v>102453</v>
       </c>
     </row>
@@ -17707,7 +17751,7 @@
       <c r="D7" t="s">
         <v>516</v>
       </c>
-      <c r="E7" s="81"/>
+      <c r="E7" s="82"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -17722,7 +17766,7 @@
       <c r="D8" t="s">
         <v>521</v>
       </c>
-      <c r="E8" s="81">
+      <c r="E8" s="82">
         <v>102447</v>
       </c>
     </row>
@@ -17739,7 +17783,7 @@
       <c r="D9" t="s">
         <v>521</v>
       </c>
-      <c r="E9" s="81"/>
+      <c r="E9" s="82"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -17754,7 +17798,7 @@
       <c r="D10" t="s">
         <v>521</v>
       </c>
-      <c r="E10" s="81"/>
+      <c r="E10" s="82"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -17769,7 +17813,7 @@
       <c r="D11" t="s">
         <v>521</v>
       </c>
-      <c r="E11" s="81"/>
+      <c r="E11" s="82"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -17784,7 +17828,7 @@
       <c r="D12" t="s">
         <v>512</v>
       </c>
-      <c r="E12" s="81">
+      <c r="E12" s="82">
         <v>101221</v>
       </c>
     </row>
@@ -17801,7 +17845,7 @@
       <c r="D13" t="s">
         <v>512</v>
       </c>
-      <c r="E13" s="81"/>
+      <c r="E13" s="82"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -17816,7 +17860,7 @@
       <c r="D14" t="s">
         <v>517</v>
       </c>
-      <c r="E14" s="81">
+      <c r="E14" s="82">
         <v>102455</v>
       </c>
     </row>
@@ -17833,7 +17877,7 @@
       <c r="D15" t="s">
         <v>517</v>
       </c>
-      <c r="E15" s="81"/>
+      <c r="E15" s="82"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -17848,7 +17892,7 @@
       <c r="D16" t="s">
         <v>508</v>
       </c>
-      <c r="E16" s="81">
+      <c r="E16" s="82">
         <v>1013824</v>
       </c>
     </row>
@@ -17865,7 +17909,7 @@
       <c r="D17" t="s">
         <v>508</v>
       </c>
-      <c r="E17" s="81"/>
+      <c r="E17" s="82"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -17880,7 +17924,7 @@
       <c r="D18" t="s">
         <v>510</v>
       </c>
-      <c r="E18" s="81">
+      <c r="E18" s="82">
         <v>102445</v>
       </c>
     </row>
@@ -17897,7 +17941,7 @@
       <c r="D19" t="s">
         <v>510</v>
       </c>
-      <c r="E19" s="81"/>
+      <c r="E19" s="82"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -17912,7 +17956,7 @@
       <c r="D20" t="s">
         <v>511</v>
       </c>
-      <c r="E20" s="81">
+      <c r="E20" s="82">
         <v>101557</v>
       </c>
     </row>
@@ -17929,7 +17973,7 @@
       <c r="D21" t="s">
         <v>511</v>
       </c>
-      <c r="E21" s="81"/>
+      <c r="E21" s="82"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -17944,7 +17988,7 @@
       <c r="D22" t="s">
         <v>509</v>
       </c>
-      <c r="E22" s="81">
+      <c r="E22" s="82">
         <v>101339</v>
       </c>
     </row>
@@ -17961,7 +18005,7 @@
       <c r="D23" t="s">
         <v>509</v>
       </c>
-      <c r="E23" s="81"/>
+      <c r="E23" s="82"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -17976,7 +18020,7 @@
       <c r="D24" t="s">
         <v>520</v>
       </c>
-      <c r="E24" s="81">
+      <c r="E24" s="82">
         <v>102391</v>
       </c>
     </row>
@@ -17993,7 +18037,7 @@
       <c r="D25" t="s">
         <v>520</v>
       </c>
-      <c r="E25" s="81"/>
+      <c r="E25" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -18522,6 +18566,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEAE28352B96D64C95AA0D5E2FA62FAD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed183881d36ac1b5d7d67982eda510d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d161086-4829-409f-9f75-5bde88dcb151" xmlns:ns3="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="685f4fda20cf913d28bf77c13cd653dd" ns2:_="" ns3:_="">
     <xsd:import namespace="3d161086-4829-409f-9f75-5bde88dcb151"/>
@@ -18744,17 +18799,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -18765,6 +18809,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C74AB5E7-5C87-4FF7-BF80-AB0EB6BD1D32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18783,23 +18844,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
V_MAP_BIOMASS_OBSERVATION, V_MAP_MLO_FISH_OBSERVATION, V_MAP_MLO_JELLYFISH_OBSERVATION, V_MAP_MLO_OTHERS_OBSERVATION, V_MAP_MLO_PINNIPEDS_OBSERVATION and V_MAP_MLO_REPTILES_OBSERVATION finalized
</commit_message>
<xml_diff>
--- a/analysis/MEDS_Tables.xlsx
+++ b/analysis/MEDS_Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="718" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{673BFC4A-AB37-4EEB-9E96-86A15051DA1C}"/>
+  <xr:revisionPtr revIDLastSave="726" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F9614CF-648E-4F0C-AFDA-F710D4BA5C86}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meds_tables" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3200" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3208" uniqueCount="745">
   <si>
     <t>Table</t>
   </si>
@@ -11680,7 +11680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76451C41-9738-4BC1-978E-20A0DA8744C6}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -12034,8 +12034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8FA477-9B46-4053-B7AD-310B8B9F2B30}">
   <dimension ref="A1:P252"/>
   <sheetViews>
-    <sheetView topLeftCell="C208" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M246" sqref="M246"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12070,7 +12070,7 @@
       <c r="H1" s="48"/>
       <c r="I1" s="41">
         <f>E250/E249</f>
-        <v>8.8495575221238937E-2</v>
+        <v>0.12844036697247707</v>
       </c>
       <c r="J1" s="49" t="s">
         <v>566</v>
@@ -12852,7 +12852,9 @@
         <v>640</v>
       </c>
       <c r="D54" s="58"/>
-      <c r="E54" s="59"/>
+      <c r="E54" s="59" t="s">
+        <v>81</v>
+      </c>
       <c r="F54" s="59" t="s">
         <v>685</v>
       </c>
@@ -12972,7 +12974,9 @@
         <v>648</v>
       </c>
       <c r="D62" s="58"/>
-      <c r="E62" s="59"/>
+      <c r="E62" s="59" t="s">
+        <v>81</v>
+      </c>
       <c r="F62" s="59" t="s">
         <v>685</v>
       </c>
@@ -13197,7 +13201,9 @@
         <v>663</v>
       </c>
       <c r="D77" s="58"/>
-      <c r="E77" s="59"/>
+      <c r="E77" s="59" t="s">
+        <v>81</v>
+      </c>
       <c r="F77" s="59" t="s">
         <v>685</v>
       </c>
@@ -13287,7 +13293,9 @@
         <v>669</v>
       </c>
       <c r="D83" s="58"/>
-      <c r="E83" s="59"/>
+      <c r="E83" s="59" t="s">
+        <v>81</v>
+      </c>
       <c r="F83" s="59" t="s">
         <v>685</v>
       </c>
@@ -13302,7 +13310,9 @@
         <v>670</v>
       </c>
       <c r="D84" s="58"/>
-      <c r="E84" s="59"/>
+      <c r="E84" s="59" t="s">
+        <v>81</v>
+      </c>
       <c r="F84" s="59" t="s">
         <v>685</v>
       </c>
@@ -13362,7 +13372,9 @@
         <v>674</v>
       </c>
       <c r="D88" s="58"/>
-      <c r="E88" s="59"/>
+      <c r="E88" s="59" t="s">
+        <v>81</v>
+      </c>
       <c r="F88" s="59" t="s">
         <v>685</v>
       </c>
@@ -13617,7 +13629,9 @@
         <v>640</v>
       </c>
       <c r="D105" s="58"/>
-      <c r="E105" s="59"/>
+      <c r="E105" s="59" t="s">
+        <v>81</v>
+      </c>
       <c r="F105" s="59" t="s">
         <v>686</v>
       </c>
@@ -13737,7 +13751,9 @@
         <v>648</v>
       </c>
       <c r="D113" s="58"/>
-      <c r="E113" s="59"/>
+      <c r="E113" s="59" t="s">
+        <v>81</v>
+      </c>
       <c r="F113" s="59" t="s">
         <v>686</v>
       </c>
@@ -15688,7 +15704,7 @@
       <c r="D249" s="36"/>
       <c r="E249" s="43">
         <f>COUNTBLANK(E2:E247)</f>
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="F249" s="46"/>
       <c r="G249" s="36"/>
@@ -15701,7 +15717,7 @@
       <c r="D250" s="36"/>
       <c r="E250" s="43">
         <f>COUNTA(E2:E247)</f>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F250" s="46"/>
       <c r="G250" s="36"/>
@@ -16105,7 +16121,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18811,15 +18827,15 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
V_MAP_ADCP_OBSERVATION, V_MAP_AQUAPACK_PROFILE_OBSERVATION, V_MAP_BEACH_OBSERVATION, V_MAP_MLO_CETACEANS_OBSERVATION, V_MAP_TS_OBSERVATION (v1) added
</commit_message>
<xml_diff>
--- a/analysis/MEDS_Tables.xlsx
+++ b/analysis/MEDS_Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="742" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{7692328E-F5C2-46EC-B92D-159331F800AC}"/>
+  <xr:revisionPtr revIDLastSave="746" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DE1EC85-9AD8-4F37-90BC-B1067C6CEA74}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3159" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3163" uniqueCount="744">
   <si>
     <t>Table</t>
   </si>
@@ -3442,43 +3442,43 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -12012,9 +12012,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8FA477-9B46-4053-B7AD-310B8B9F2B30}">
   <dimension ref="A1:P201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E83" sqref="E83"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12050,7 +12050,7 @@
       <c r="H1" s="45"/>
       <c r="I1" s="41">
         <f>E199/E198</f>
-        <v>0.18181818181818182</v>
+        <v>0.21118012422360249</v>
       </c>
       <c r="J1" s="46" t="s">
         <v>566</v>
@@ -12064,13 +12064,13 @@
       <c r="D2" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="64" t="s">
+      <c r="E2" s="68" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="64" t="s">
+      <c r="F2" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="68" t="s">
+      <c r="G2" s="70" t="s">
         <v>564</v>
       </c>
     </row>
@@ -12078,10 +12078,10 @@
       <c r="C3" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="62"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="67"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="72"/>
       <c r="K3" s="36"/>
       <c r="L3" s="36"/>
       <c r="M3" s="36"/>
@@ -12093,10 +12093,10 @@
       <c r="C4" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="67"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="72"/>
       <c r="K4" s="36"/>
       <c r="L4" s="36"/>
       <c r="M4" s="36"/>
@@ -12108,27 +12108,27 @@
       <c r="C5" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="62" t="s">
+      <c r="D5" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="63" t="s">
+      <c r="E5" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F5" s="63" t="s">
+      <c r="F5" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="67" t="s">
+      <c r="G5" s="72" t="s">
         <v>519</v>
       </c>
       <c r="K5" s="36"/>
       <c r="L5" s="44" t="s">
         <v>464</v>
       </c>
-      <c r="M5" s="74" t="s">
+      <c r="M5" s="63" t="s">
         <v>465</v>
       </c>
-      <c r="N5" s="63"/>
-      <c r="O5" s="73" t="s">
+      <c r="N5" s="64"/>
+      <c r="O5" s="62" t="s">
         <v>581</v>
       </c>
       <c r="P5" s="36"/>
@@ -12137,33 +12137,33 @@
       <c r="C6" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="62"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="67"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="72"/>
       <c r="K6" s="36"/>
       <c r="L6" s="44" t="s">
         <v>467</v>
       </c>
-      <c r="M6" s="74"/>
-      <c r="N6" s="63"/>
-      <c r="O6" s="73"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="64"/>
+      <c r="O6" s="62"/>
       <c r="P6" s="36"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C7" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="62" t="s">
+      <c r="D7" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="63" t="s">
+      <c r="E7" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="63" t="s">
+      <c r="F7" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="67" t="s">
+      <c r="G7" s="72" t="s">
         <v>80</v>
       </c>
       <c r="K7" s="36"/>
@@ -12177,10 +12177,10 @@
       <c r="C8" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="62"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="67"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="72"/>
       <c r="K8" s="36"/>
       <c r="L8" s="36"/>
       <c r="M8" s="36"/>
@@ -12192,16 +12192,16 @@
       <c r="C9" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="D9" s="62" t="s">
+      <c r="D9" s="65" t="s">
         <v>171</v>
       </c>
-      <c r="E9" s="63" t="s">
+      <c r="E9" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="63" t="s">
+      <c r="F9" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="67" t="s">
+      <c r="G9" s="72" t="s">
         <v>523</v>
       </c>
       <c r="J9" s="36"/>
@@ -12211,10 +12211,10 @@
       <c r="C10" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="D10" s="62"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="67"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="72"/>
       <c r="J10" s="36"/>
       <c r="K10" s="36"/>
     </row>
@@ -12222,10 +12222,10 @@
       <c r="C11" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="D11" s="62"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="67"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="72"/>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
     </row>
@@ -12233,16 +12233,16 @@
       <c r="C12" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="D12" s="62" t="s">
+      <c r="D12" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="E12" s="63" t="s">
+      <c r="E12" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="63" t="s">
+      <c r="F12" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="67" t="s">
+      <c r="G12" s="72" t="s">
         <v>515</v>
       </c>
       <c r="J12" s="36"/>
@@ -12252,10 +12252,10 @@
       <c r="C13" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="D13" s="62"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="67"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="72"/>
       <c r="J13" s="36"/>
       <c r="K13" s="36"/>
     </row>
@@ -12263,16 +12263,16 @@
       <c r="C14" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="D14" s="62" t="s">
+      <c r="D14" s="65" t="s">
         <v>361</v>
       </c>
-      <c r="E14" s="63" t="s">
+      <c r="E14" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F14" s="63" t="s">
+      <c r="F14" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="67" t="s">
+      <c r="G14" s="72" t="s">
         <v>518</v>
       </c>
       <c r="J14" s="36"/>
@@ -12282,9 +12282,9 @@
       <c r="C15" s="35" t="s">
         <v>363</v>
       </c>
-      <c r="D15" s="69"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
       <c r="G15" s="71"/>
       <c r="J15" s="36"/>
       <c r="K15" s="36"/>
@@ -12296,13 +12296,13 @@
       <c r="D16" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="64" t="s">
+      <c r="E16" s="68" t="s">
         <v>81</v>
       </c>
-      <c r="F16" s="64" t="s">
+      <c r="F16" s="68" t="s">
         <v>567</v>
       </c>
-      <c r="G16" s="68" t="s">
+      <c r="G16" s="70" t="s">
         <v>73</v>
       </c>
       <c r="J16" s="36"/>
@@ -12312,10 +12312,10 @@
       <c r="C17" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="62"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="67"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="72"/>
       <c r="J17" s="36"/>
       <c r="K17" s="36"/>
     </row>
@@ -12323,16 +12323,16 @@
       <c r="C18" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="62" t="s">
+      <c r="D18" s="65" t="s">
         <v>105</v>
       </c>
-      <c r="E18" s="63" t="s">
+      <c r="E18" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F18" s="63" t="s">
+      <c r="F18" s="64" t="s">
         <v>567</v>
       </c>
-      <c r="G18" s="67" t="s">
+      <c r="G18" s="72" t="s">
         <v>524</v>
       </c>
       <c r="J18" s="36"/>
@@ -12342,10 +12342,10 @@
       <c r="C19" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="62"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="67"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="72"/>
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
     </row>
@@ -12353,16 +12353,16 @@
       <c r="C20" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="D20" s="62" t="s">
+      <c r="D20" s="65" t="s">
         <v>300</v>
       </c>
-      <c r="E20" s="63" t="s">
+      <c r="E20" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F20" s="63" t="s">
+      <c r="F20" s="64" t="s">
         <v>567</v>
       </c>
-      <c r="G20" s="67" t="s">
+      <c r="G20" s="72" t="s">
         <v>516</v>
       </c>
       <c r="J20" s="36"/>
@@ -12372,10 +12372,10 @@
       <c r="C21" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="D21" s="62"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
-      <c r="G21" s="67"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="72"/>
       <c r="J21" s="36"/>
       <c r="K21" s="36"/>
     </row>
@@ -12383,16 +12383,16 @@
       <c r="C22" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="D22" s="62" t="s">
+      <c r="D22" s="65" t="s">
         <v>305</v>
       </c>
-      <c r="E22" s="63" t="s">
+      <c r="E22" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F22" s="63" t="s">
+      <c r="F22" s="64" t="s">
         <v>567</v>
       </c>
-      <c r="G22" s="67" t="s">
+      <c r="G22" s="72" t="s">
         <v>521</v>
       </c>
       <c r="J22" s="36"/>
@@ -12402,10 +12402,10 @@
       <c r="C23" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="D23" s="62"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="67"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="72"/>
       <c r="J23" s="36"/>
       <c r="K23" s="36"/>
     </row>
@@ -12413,16 +12413,16 @@
       <c r="C24" s="34" t="s">
         <v>317</v>
       </c>
-      <c r="D24" s="62" t="s">
+      <c r="D24" s="65" t="s">
         <v>318</v>
       </c>
-      <c r="E24" s="63" t="s">
+      <c r="E24" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F24" s="63" t="s">
+      <c r="F24" s="64" t="s">
         <v>567</v>
       </c>
-      <c r="G24" s="67" t="s">
+      <c r="G24" s="72" t="s">
         <v>512</v>
       </c>
       <c r="J24" s="36"/>
@@ -12432,10 +12432,10 @@
       <c r="C25" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="D25" s="62"/>
-      <c r="E25" s="63"/>
-      <c r="F25" s="63"/>
-      <c r="G25" s="67"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="72"/>
       <c r="J25" s="36"/>
       <c r="K25" s="36"/>
     </row>
@@ -12443,16 +12443,16 @@
       <c r="C26" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="D26" s="65" t="s">
+      <c r="D26" s="73" t="s">
         <v>323</v>
       </c>
-      <c r="E26" s="72" t="s">
+      <c r="E26" s="74" t="s">
         <v>81</v>
       </c>
-      <c r="F26" s="63" t="s">
+      <c r="F26" s="64" t="s">
         <v>567</v>
       </c>
-      <c r="G26" s="67" t="s">
+      <c r="G26" s="72" t="s">
         <v>517</v>
       </c>
       <c r="J26" s="36"/>
@@ -12462,25 +12462,25 @@
       <c r="C27" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="D27" s="65"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="67"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="72"/>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C28" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="D28" s="62" t="s">
+      <c r="D28" s="65" t="s">
         <v>328</v>
       </c>
-      <c r="E28" s="63" t="s">
+      <c r="E28" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F28" s="63" t="s">
+      <c r="F28" s="64" t="s">
         <v>567</v>
       </c>
-      <c r="G28" s="67" t="s">
+      <c r="G28" s="72" t="s">
         <v>508</v>
       </c>
     </row>
@@ -12488,25 +12488,25 @@
       <c r="C29" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="D29" s="62"/>
-      <c r="E29" s="63"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="67"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="64"/>
+      <c r="G29" s="72"/>
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C30" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="D30" s="62" t="s">
+      <c r="D30" s="65" t="s">
         <v>333</v>
       </c>
-      <c r="E30" s="63" t="s">
+      <c r="E30" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F30" s="63" t="s">
+      <c r="F30" s="64" t="s">
         <v>567</v>
       </c>
-      <c r="G30" s="67" t="s">
+      <c r="G30" s="72" t="s">
         <v>510</v>
       </c>
     </row>
@@ -12514,25 +12514,25 @@
       <c r="C31" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="D31" s="62"/>
-      <c r="E31" s="63"/>
-      <c r="F31" s="63"/>
-      <c r="G31" s="67"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="72"/>
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="D32" s="62" t="s">
+      <c r="D32" s="65" t="s">
         <v>338</v>
       </c>
-      <c r="E32" s="63" t="s">
+      <c r="E32" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F32" s="63" t="s">
+      <c r="F32" s="64" t="s">
         <v>567</v>
       </c>
-      <c r="G32" s="67" t="s">
+      <c r="G32" s="72" t="s">
         <v>511</v>
       </c>
     </row>
@@ -12540,25 +12540,25 @@
       <c r="C33" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="D33" s="62"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="67"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="64"/>
+      <c r="G33" s="72"/>
     </row>
     <row r="34" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C34" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="D34" s="62" t="s">
+      <c r="D34" s="65" t="s">
         <v>343</v>
       </c>
-      <c r="E34" s="63" t="s">
+      <c r="E34" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F34" s="63" t="s">
+      <c r="F34" s="64" t="s">
         <v>567</v>
       </c>
-      <c r="G34" s="67" t="s">
+      <c r="G34" s="72" t="s">
         <v>509</v>
       </c>
     </row>
@@ -12566,25 +12566,25 @@
       <c r="C35" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="D35" s="62"/>
-      <c r="E35" s="63"/>
-      <c r="F35" s="63"/>
-      <c r="G35" s="67"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="72"/>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C36" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="D36" s="62" t="s">
+      <c r="D36" s="65" t="s">
         <v>348</v>
       </c>
-      <c r="E36" s="63" t="s">
+      <c r="E36" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F36" s="63" t="s">
+      <c r="F36" s="64" t="s">
         <v>567</v>
       </c>
-      <c r="G36" s="67" t="s">
+      <c r="G36" s="72" t="s">
         <v>520</v>
       </c>
     </row>
@@ -12592,9 +12592,9 @@
       <c r="C37" s="35" t="s">
         <v>350</v>
       </c>
-      <c r="D37" s="69"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
+      <c r="D37" s="67"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
       <c r="G37" s="71"/>
     </row>
     <row r="38" spans="3:13" x14ac:dyDescent="0.25">
@@ -12604,13 +12604,13 @@
       <c r="D38" s="66" t="s">
         <v>366</v>
       </c>
-      <c r="E38" s="64" t="s">
+      <c r="E38" s="68" t="s">
         <v>81</v>
       </c>
-      <c r="F38" s="64" t="s">
+      <c r="F38" s="68" t="s">
         <v>369</v>
       </c>
-      <c r="G38" s="68" t="s">
+      <c r="G38" s="70" t="s">
         <v>514</v>
       </c>
     </row>
@@ -12618,34 +12618,34 @@
       <c r="C39" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="D39" s="62"/>
-      <c r="E39" s="63"/>
-      <c r="F39" s="63"/>
-      <c r="G39" s="67"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="64"/>
+      <c r="F39" s="64"/>
+      <c r="G39" s="72"/>
     </row>
     <row r="40" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C40" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="D40" s="62"/>
-      <c r="E40" s="63"/>
-      <c r="F40" s="63"/>
-      <c r="G40" s="67"/>
+      <c r="D40" s="65"/>
+      <c r="E40" s="64"/>
+      <c r="F40" s="64"/>
+      <c r="G40" s="72"/>
     </row>
     <row r="41" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C41" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="D41" s="62" t="s">
+      <c r="D41" s="65" t="s">
         <v>371</v>
       </c>
-      <c r="E41" s="63" t="s">
+      <c r="E41" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F41" s="63" t="s">
+      <c r="F41" s="64" t="s">
         <v>369</v>
       </c>
-      <c r="G41" s="67" t="s">
+      <c r="G41" s="72" t="s">
         <v>513</v>
       </c>
     </row>
@@ -12653,34 +12653,34 @@
       <c r="C42" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="D42" s="62"/>
-      <c r="E42" s="63"/>
-      <c r="F42" s="63"/>
-      <c r="G42" s="67"/>
+      <c r="D42" s="65"/>
+      <c r="E42" s="64"/>
+      <c r="F42" s="64"/>
+      <c r="G42" s="72"/>
     </row>
     <row r="43" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C43" s="34" t="s">
         <v>384</v>
       </c>
-      <c r="D43" s="62"/>
-      <c r="E43" s="63"/>
-      <c r="F43" s="63"/>
-      <c r="G43" s="67"/>
+      <c r="D43" s="65"/>
+      <c r="E43" s="64"/>
+      <c r="F43" s="64"/>
+      <c r="G43" s="72"/>
     </row>
     <row r="44" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C44" s="34" t="s">
         <v>373</v>
       </c>
-      <c r="D44" s="62" t="s">
+      <c r="D44" s="65" t="s">
         <v>374</v>
       </c>
-      <c r="E44" s="63" t="s">
+      <c r="E44" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F44" s="63" t="s">
+      <c r="F44" s="64" t="s">
         <v>369</v>
       </c>
-      <c r="G44" s="67" t="s">
+      <c r="G44" s="72" t="s">
         <v>522</v>
       </c>
     </row>
@@ -12688,19 +12688,19 @@
       <c r="C45" s="34" t="s">
         <v>380</v>
       </c>
-      <c r="D45" s="62"/>
-      <c r="E45" s="63"/>
-      <c r="F45" s="63"/>
-      <c r="G45" s="67"/>
+      <c r="D45" s="65"/>
+      <c r="E45" s="64"/>
+      <c r="F45" s="64"/>
+      <c r="G45" s="72"/>
     </row>
     <row r="46" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C46" s="34" t="s">
         <v>386</v>
       </c>
-      <c r="D46" s="62"/>
-      <c r="E46" s="63"/>
-      <c r="F46" s="63"/>
-      <c r="G46" s="67"/>
+      <c r="D46" s="65"/>
+      <c r="E46" s="64"/>
+      <c r="F46" s="64"/>
+      <c r="G46" s="72"/>
       <c r="J46" s="36"/>
       <c r="K46" s="36"/>
       <c r="L46" s="36"/>
@@ -12713,11 +12713,11 @@
       <c r="D47" s="66" t="s">
         <v>465</v>
       </c>
-      <c r="E47" s="64"/>
-      <c r="F47" s="64" t="s">
+      <c r="E47" s="68"/>
+      <c r="F47" s="68" t="s">
         <v>584</v>
       </c>
-      <c r="G47" s="68" t="s">
+      <c r="G47" s="70" t="s">
         <v>585</v>
       </c>
       <c r="J47" s="36"/>
@@ -12729,9 +12729,9 @@
       <c r="C48" s="35" t="s">
         <v>467</v>
       </c>
-      <c r="D48" s="69"/>
-      <c r="E48" s="70"/>
-      <c r="F48" s="70"/>
+      <c r="D48" s="67"/>
+      <c r="E48" s="69"/>
+      <c r="F48" s="69"/>
       <c r="G48" s="71"/>
       <c r="J48" s="36"/>
       <c r="K48" s="36"/>
@@ -12743,7 +12743,9 @@
         <v>635</v>
       </c>
       <c r="D49" s="54"/>
-      <c r="E49" s="55"/>
+      <c r="E49" s="55" t="s">
+        <v>81</v>
+      </c>
       <c r="F49" s="55" t="s">
         <v>685</v>
       </c>
@@ -12777,7 +12779,9 @@
         <v>637</v>
       </c>
       <c r="D51" s="54"/>
-      <c r="E51" s="55"/>
+      <c r="E51" s="55" t="s">
+        <v>81</v>
+      </c>
       <c r="F51" s="55" t="s">
         <v>685</v>
       </c>
@@ -12794,7 +12798,9 @@
         <v>638</v>
       </c>
       <c r="D52" s="54"/>
-      <c r="E52" s="55"/>
+      <c r="E52" s="55" t="s">
+        <v>81</v>
+      </c>
       <c r="F52" s="55" t="s">
         <v>685</v>
       </c>
@@ -12866,7 +12872,9 @@
         <v>642</v>
       </c>
       <c r="D56" s="54"/>
-      <c r="E56" s="55"/>
+      <c r="E56" s="55" t="s">
+        <v>81</v>
+      </c>
       <c r="F56" s="55" t="s">
         <v>685</v>
       </c>
@@ -13632,8 +13640,8 @@
       <c r="D100" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="E100" s="64"/>
-      <c r="F100" s="64" t="s">
+      <c r="E100" s="68"/>
+      <c r="F100" s="68" t="s">
         <v>18</v>
       </c>
       <c r="G100" s="60" t="s">
@@ -13648,9 +13656,9 @@
       <c r="C101" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D101" s="62"/>
-      <c r="E101" s="63"/>
-      <c r="F101" s="63"/>
+      <c r="D101" s="65"/>
+      <c r="E101" s="64"/>
+      <c r="F101" s="64"/>
       <c r="G101" s="38" t="s">
         <v>33</v>
       </c>
@@ -13663,9 +13671,9 @@
       <c r="C102" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D102" s="62"/>
-      <c r="E102" s="63"/>
-      <c r="F102" s="63"/>
+      <c r="D102" s="65"/>
+      <c r="E102" s="64"/>
+      <c r="F102" s="64"/>
       <c r="G102" s="38" t="s">
         <v>33</v>
       </c>
@@ -13678,11 +13686,11 @@
       <c r="C103" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="D103" s="62" t="s">
+      <c r="D103" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="E103" s="63"/>
-      <c r="F103" s="63" t="s">
+      <c r="E103" s="64"/>
+      <c r="F103" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G103" s="38" t="s">
@@ -13697,9 +13705,9 @@
       <c r="C104" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D104" s="62"/>
-      <c r="E104" s="63"/>
-      <c r="F104" s="63"/>
+      <c r="D104" s="65"/>
+      <c r="E104" s="64"/>
+      <c r="F104" s="64"/>
       <c r="G104" s="38" t="s">
         <v>33</v>
       </c>
@@ -13712,11 +13720,11 @@
       <c r="C105" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D105" s="62" t="s">
+      <c r="D105" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="E105" s="63"/>
-      <c r="F105" s="63" t="s">
+      <c r="E105" s="64"/>
+      <c r="F105" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G105" s="38" t="s">
@@ -13731,9 +13739,9 @@
       <c r="C106" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D106" s="62"/>
-      <c r="E106" s="63"/>
-      <c r="F106" s="63"/>
+      <c r="D106" s="65"/>
+      <c r="E106" s="64"/>
+      <c r="F106" s="64"/>
       <c r="G106" s="38" t="s">
         <v>33</v>
       </c>
@@ -13746,11 +13754,11 @@
       <c r="C107" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D107" s="62" t="s">
+      <c r="D107" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="E107" s="63"/>
-      <c r="F107" s="63" t="s">
+      <c r="E107" s="64"/>
+      <c r="F107" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G107" s="38" t="s">
@@ -13765,9 +13773,9 @@
       <c r="C108" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D108" s="62"/>
-      <c r="E108" s="63"/>
-      <c r="F108" s="63"/>
+      <c r="D108" s="65"/>
+      <c r="E108" s="64"/>
+      <c r="F108" s="64"/>
       <c r="G108" s="38" t="s">
         <v>33</v>
       </c>
@@ -13780,11 +13788,11 @@
       <c r="C109" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="D109" s="62" t="s">
+      <c r="D109" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="E109" s="63"/>
-      <c r="F109" s="63" t="s">
+      <c r="E109" s="64"/>
+      <c r="F109" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G109" s="38" t="s">
@@ -13799,9 +13807,9 @@
       <c r="C110" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D110" s="62"/>
-      <c r="E110" s="63"/>
-      <c r="F110" s="63"/>
+      <c r="D110" s="65"/>
+      <c r="E110" s="64"/>
+      <c r="F110" s="64"/>
       <c r="G110" s="38" t="s">
         <v>33</v>
       </c>
@@ -13814,11 +13822,11 @@
       <c r="C111" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D111" s="62" t="s">
+      <c r="D111" s="65" t="s">
         <v>105</v>
       </c>
-      <c r="E111" s="63"/>
-      <c r="F111" s="63" t="s">
+      <c r="E111" s="64"/>
+      <c r="F111" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G111" s="38" t="s">
@@ -13833,9 +13841,9 @@
       <c r="C112" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D112" s="62"/>
-      <c r="E112" s="63"/>
-      <c r="F112" s="63"/>
+      <c r="D112" s="65"/>
+      <c r="E112" s="64"/>
+      <c r="F112" s="64"/>
       <c r="G112" s="38" t="s">
         <v>33</v>
       </c>
@@ -13848,11 +13856,11 @@
       <c r="C113" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="D113" s="62" t="s">
+      <c r="D113" s="65" t="s">
         <v>171</v>
       </c>
-      <c r="E113" s="63"/>
-      <c r="F113" s="63" t="s">
+      <c r="E113" s="64"/>
+      <c r="F113" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G113" s="38" t="s">
@@ -13867,9 +13875,9 @@
       <c r="C114" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="D114" s="62"/>
-      <c r="E114" s="63"/>
-      <c r="F114" s="63"/>
+      <c r="D114" s="65"/>
+      <c r="E114" s="64"/>
+      <c r="F114" s="64"/>
       <c r="G114" s="38" t="s">
         <v>33</v>
       </c>
@@ -13882,9 +13890,9 @@
       <c r="C115" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="D115" s="62"/>
-      <c r="E115" s="63"/>
-      <c r="F115" s="63"/>
+      <c r="D115" s="65"/>
+      <c r="E115" s="64"/>
+      <c r="F115" s="64"/>
       <c r="G115" s="38" t="s">
         <v>33</v>
       </c>
@@ -13897,11 +13905,11 @@
       <c r="C116" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="D116" s="62" t="s">
+      <c r="D116" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="E116" s="63"/>
-      <c r="F116" s="63" t="s">
+      <c r="E116" s="64"/>
+      <c r="F116" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G116" s="38" t="s">
@@ -13916,9 +13924,9 @@
       <c r="C117" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="D117" s="62"/>
-      <c r="E117" s="63"/>
-      <c r="F117" s="63"/>
+      <c r="D117" s="65"/>
+      <c r="E117" s="64"/>
+      <c r="F117" s="64"/>
       <c r="G117" s="38" t="s">
         <v>33</v>
       </c>
@@ -13931,11 +13939,11 @@
       <c r="C118" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="D118" s="62" t="s">
+      <c r="D118" s="65" t="s">
         <v>300</v>
       </c>
-      <c r="E118" s="63"/>
-      <c r="F118" s="63" t="s">
+      <c r="E118" s="64"/>
+      <c r="F118" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G118" s="38" t="s">
@@ -13950,9 +13958,9 @@
       <c r="C119" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="D119" s="62"/>
-      <c r="E119" s="63"/>
-      <c r="F119" s="63"/>
+      <c r="D119" s="65"/>
+      <c r="E119" s="64"/>
+      <c r="F119" s="64"/>
       <c r="G119" s="38" t="s">
         <v>33</v>
       </c>
@@ -13965,11 +13973,11 @@
       <c r="C120" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="D120" s="62" t="s">
+      <c r="D120" s="65" t="s">
         <v>305</v>
       </c>
-      <c r="E120" s="63"/>
-      <c r="F120" s="63" t="s">
+      <c r="E120" s="64"/>
+      <c r="F120" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G120" s="38" t="s">
@@ -13984,9 +13992,9 @@
       <c r="C121" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="D121" s="62"/>
-      <c r="E121" s="63"/>
-      <c r="F121" s="63"/>
+      <c r="D121" s="65"/>
+      <c r="E121" s="64"/>
+      <c r="F121" s="64"/>
       <c r="G121" s="38" t="s">
         <v>33</v>
       </c>
@@ -13999,9 +14007,9 @@
       <c r="C122" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="D122" s="62"/>
-      <c r="E122" s="63"/>
-      <c r="F122" s="63"/>
+      <c r="D122" s="65"/>
+      <c r="E122" s="64"/>
+      <c r="F122" s="64"/>
       <c r="G122" s="38" t="s">
         <v>33</v>
       </c>
@@ -14014,9 +14022,9 @@
       <c r="C123" s="34" t="s">
         <v>311</v>
       </c>
-      <c r="D123" s="62"/>
-      <c r="E123" s="63"/>
-      <c r="F123" s="63"/>
+      <c r="D123" s="65"/>
+      <c r="E123" s="64"/>
+      <c r="F123" s="64"/>
       <c r="G123" s="38" t="s">
         <v>33</v>
       </c>
@@ -14029,11 +14037,11 @@
       <c r="C124" s="34" t="s">
         <v>317</v>
       </c>
-      <c r="D124" s="62" t="s">
+      <c r="D124" s="65" t="s">
         <v>318</v>
       </c>
-      <c r="E124" s="63"/>
-      <c r="F124" s="63" t="s">
+      <c r="E124" s="64"/>
+      <c r="F124" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G124" s="38" t="s">
@@ -14048,9 +14056,9 @@
       <c r="C125" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="D125" s="62"/>
-      <c r="E125" s="63"/>
-      <c r="F125" s="63"/>
+      <c r="D125" s="65"/>
+      <c r="E125" s="64"/>
+      <c r="F125" s="64"/>
       <c r="G125" s="38" t="s">
         <v>33</v>
       </c>
@@ -14063,11 +14071,11 @@
       <c r="C126" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="D126" s="65" t="s">
+      <c r="D126" s="73" t="s">
         <v>323</v>
       </c>
-      <c r="E126" s="63"/>
-      <c r="F126" s="63" t="s">
+      <c r="E126" s="64"/>
+      <c r="F126" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G126" s="38" t="s">
@@ -14082,9 +14090,9 @@
       <c r="C127" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="D127" s="65"/>
-      <c r="E127" s="63"/>
-      <c r="F127" s="63"/>
+      <c r="D127" s="73"/>
+      <c r="E127" s="64"/>
+      <c r="F127" s="64"/>
       <c r="G127" s="38" t="s">
         <v>33</v>
       </c>
@@ -14093,11 +14101,11 @@
       <c r="C128" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="D128" s="62" t="s">
+      <c r="D128" s="65" t="s">
         <v>328</v>
       </c>
-      <c r="E128" s="63"/>
-      <c r="F128" s="63" t="s">
+      <c r="E128" s="64"/>
+      <c r="F128" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G128" s="38" t="s">
@@ -14108,9 +14116,9 @@
       <c r="C129" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="D129" s="62"/>
-      <c r="E129" s="63"/>
-      <c r="F129" s="63"/>
+      <c r="D129" s="65"/>
+      <c r="E129" s="64"/>
+      <c r="F129" s="64"/>
       <c r="G129" s="38" t="s">
         <v>33</v>
       </c>
@@ -14119,11 +14127,11 @@
       <c r="C130" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="D130" s="62" t="s">
+      <c r="D130" s="65" t="s">
         <v>333</v>
       </c>
-      <c r="E130" s="63"/>
-      <c r="F130" s="63" t="s">
+      <c r="E130" s="64"/>
+      <c r="F130" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G130" s="38" t="s">
@@ -14134,9 +14142,9 @@
       <c r="C131" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="D131" s="62"/>
-      <c r="E131" s="63"/>
-      <c r="F131" s="63"/>
+      <c r="D131" s="65"/>
+      <c r="E131" s="64"/>
+      <c r="F131" s="64"/>
       <c r="G131" s="38" t="s">
         <v>33</v>
       </c>
@@ -14145,11 +14153,11 @@
       <c r="C132" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="D132" s="62" t="s">
+      <c r="D132" s="65" t="s">
         <v>338</v>
       </c>
-      <c r="E132" s="63"/>
-      <c r="F132" s="63" t="s">
+      <c r="E132" s="64"/>
+      <c r="F132" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G132" s="38" t="s">
@@ -14160,9 +14168,9 @@
       <c r="C133" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="D133" s="62"/>
-      <c r="E133" s="63"/>
-      <c r="F133" s="63"/>
+      <c r="D133" s="65"/>
+      <c r="E133" s="64"/>
+      <c r="F133" s="64"/>
       <c r="G133" s="38" t="s">
         <v>33</v>
       </c>
@@ -14171,11 +14179,11 @@
       <c r="C134" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="D134" s="62" t="s">
+      <c r="D134" s="65" t="s">
         <v>343</v>
       </c>
-      <c r="E134" s="63"/>
-      <c r="F134" s="63" t="s">
+      <c r="E134" s="64"/>
+      <c r="F134" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G134" s="38" t="s">
@@ -14186,9 +14194,9 @@
       <c r="C135" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="D135" s="62"/>
-      <c r="E135" s="63"/>
-      <c r="F135" s="63"/>
+      <c r="D135" s="65"/>
+      <c r="E135" s="64"/>
+      <c r="F135" s="64"/>
       <c r="G135" s="38" t="s">
         <v>33</v>
       </c>
@@ -14197,11 +14205,11 @@
       <c r="C136" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="D136" s="62" t="s">
+      <c r="D136" s="65" t="s">
         <v>348</v>
       </c>
-      <c r="E136" s="63"/>
-      <c r="F136" s="63" t="s">
+      <c r="E136" s="64"/>
+      <c r="F136" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G136" s="38" t="s">
@@ -14212,9 +14220,9 @@
       <c r="C137" s="34" t="s">
         <v>350</v>
       </c>
-      <c r="D137" s="62"/>
-      <c r="E137" s="63"/>
-      <c r="F137" s="63"/>
+      <c r="D137" s="65"/>
+      <c r="E137" s="64"/>
+      <c r="F137" s="64"/>
       <c r="G137" s="38" t="s">
         <v>33</v>
       </c>
@@ -14223,11 +14231,11 @@
       <c r="C138" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="D138" s="62" t="s">
+      <c r="D138" s="65" t="s">
         <v>361</v>
       </c>
-      <c r="E138" s="63"/>
-      <c r="F138" s="63" t="s">
+      <c r="E138" s="64"/>
+      <c r="F138" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G138" s="38" t="s">
@@ -14238,9 +14246,9 @@
       <c r="C139" s="34" t="s">
         <v>363</v>
       </c>
-      <c r="D139" s="62"/>
-      <c r="E139" s="63"/>
-      <c r="F139" s="63"/>
+      <c r="D139" s="65"/>
+      <c r="E139" s="64"/>
+      <c r="F139" s="64"/>
       <c r="G139" s="38" t="s">
         <v>33</v>
       </c>
@@ -14249,11 +14257,11 @@
       <c r="C140" s="34" t="s">
         <v>365</v>
       </c>
-      <c r="D140" s="62" t="s">
+      <c r="D140" s="65" t="s">
         <v>366</v>
       </c>
-      <c r="E140" s="63"/>
-      <c r="F140" s="63" t="s">
+      <c r="E140" s="64"/>
+      <c r="F140" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G140" s="38" t="s">
@@ -14264,9 +14272,9 @@
       <c r="C141" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="D141" s="62"/>
-      <c r="E141" s="63"/>
-      <c r="F141" s="63"/>
+      <c r="D141" s="65"/>
+      <c r="E141" s="64"/>
+      <c r="F141" s="64"/>
       <c r="G141" s="38" t="s">
         <v>33</v>
       </c>
@@ -14275,9 +14283,9 @@
       <c r="C142" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="D142" s="62"/>
-      <c r="E142" s="63"/>
-      <c r="F142" s="63"/>
+      <c r="D142" s="65"/>
+      <c r="E142" s="64"/>
+      <c r="F142" s="64"/>
       <c r="G142" s="38" t="s">
         <v>33</v>
       </c>
@@ -14286,11 +14294,11 @@
       <c r="C143" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="D143" s="62" t="s">
+      <c r="D143" s="65" t="s">
         <v>371</v>
       </c>
-      <c r="E143" s="63"/>
-      <c r="F143" s="63" t="s">
+      <c r="E143" s="64"/>
+      <c r="F143" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G143" s="38" t="s">
@@ -14301,9 +14309,9 @@
       <c r="C144" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="D144" s="62"/>
-      <c r="E144" s="63"/>
-      <c r="F144" s="63"/>
+      <c r="D144" s="65"/>
+      <c r="E144" s="64"/>
+      <c r="F144" s="64"/>
       <c r="G144" s="38" t="s">
         <v>33</v>
       </c>
@@ -14312,9 +14320,9 @@
       <c r="C145" s="34" t="s">
         <v>384</v>
       </c>
-      <c r="D145" s="62"/>
-      <c r="E145" s="63"/>
-      <c r="F145" s="63"/>
+      <c r="D145" s="65"/>
+      <c r="E145" s="64"/>
+      <c r="F145" s="64"/>
       <c r="G145" s="38" t="s">
         <v>33</v>
       </c>
@@ -14324,11 +14332,11 @@
       <c r="C146" s="34" t="s">
         <v>373</v>
       </c>
-      <c r="D146" s="62" t="s">
+      <c r="D146" s="65" t="s">
         <v>374</v>
       </c>
-      <c r="E146" s="63"/>
-      <c r="F146" s="63" t="s">
+      <c r="E146" s="64"/>
+      <c r="F146" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G146" s="38" t="s">
@@ -14340,9 +14348,9 @@
       <c r="C147" s="34" t="s">
         <v>380</v>
       </c>
-      <c r="D147" s="62"/>
-      <c r="E147" s="63"/>
-      <c r="F147" s="63"/>
+      <c r="D147" s="65"/>
+      <c r="E147" s="64"/>
+      <c r="F147" s="64"/>
       <c r="G147" s="38" t="s">
         <v>33</v>
       </c>
@@ -14352,9 +14360,9 @@
       <c r="C148" s="34" t="s">
         <v>386</v>
       </c>
-      <c r="D148" s="62"/>
-      <c r="E148" s="63"/>
-      <c r="F148" s="63"/>
+      <c r="D148" s="65"/>
+      <c r="E148" s="64"/>
+      <c r="F148" s="64"/>
       <c r="G148" s="38" t="s">
         <v>33</v>
       </c>
@@ -14367,11 +14375,11 @@
       <c r="C149" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="D149" s="62" t="s">
+      <c r="D149" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="E149" s="63"/>
-      <c r="F149" s="63" t="s">
+      <c r="E149" s="64"/>
+      <c r="F149" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G149" s="38" t="s">
@@ -14383,9 +14391,9 @@
       <c r="C150" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="D150" s="62"/>
-      <c r="E150" s="63"/>
-      <c r="F150" s="63"/>
+      <c r="D150" s="65"/>
+      <c r="E150" s="64"/>
+      <c r="F150" s="64"/>
       <c r="G150" s="38" t="s">
         <v>33</v>
       </c>
@@ -14394,11 +14402,11 @@
       <c r="C151" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="D151" s="62" t="s">
+      <c r="D151" s="65" t="s">
         <v>110</v>
       </c>
-      <c r="E151" s="63"/>
-      <c r="F151" s="63" t="s">
+      <c r="E151" s="64"/>
+      <c r="F151" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G151" s="38" t="s">
@@ -14409,9 +14417,9 @@
       <c r="C152" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="D152" s="62"/>
-      <c r="E152" s="63"/>
-      <c r="F152" s="63"/>
+      <c r="D152" s="65"/>
+      <c r="E152" s="64"/>
+      <c r="F152" s="64"/>
       <c r="G152" s="38" t="s">
         <v>33</v>
       </c>
@@ -14420,9 +14428,9 @@
       <c r="C153" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="D153" s="62"/>
-      <c r="E153" s="63"/>
-      <c r="F153" s="63"/>
+      <c r="D153" s="65"/>
+      <c r="E153" s="64"/>
+      <c r="F153" s="64"/>
       <c r="G153" s="38" t="s">
         <v>33</v>
       </c>
@@ -14431,11 +14439,11 @@
       <c r="C154" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="D154" s="62" t="s">
+      <c r="D154" s="65" t="s">
         <v>119</v>
       </c>
-      <c r="E154" s="63"/>
-      <c r="F154" s="63" t="s">
+      <c r="E154" s="64"/>
+      <c r="F154" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G154" s="38" t="s">
@@ -14446,9 +14454,9 @@
       <c r="C155" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="D155" s="62"/>
-      <c r="E155" s="63"/>
-      <c r="F155" s="63"/>
+      <c r="D155" s="65"/>
+      <c r="E155" s="64"/>
+      <c r="F155" s="64"/>
       <c r="G155" s="38" t="s">
         <v>33</v>
       </c>
@@ -14457,11 +14465,11 @@
       <c r="C156" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="D156" s="62" t="s">
+      <c r="D156" s="65" t="s">
         <v>124</v>
       </c>
-      <c r="E156" s="63"/>
-      <c r="F156" s="63" t="s">
+      <c r="E156" s="64"/>
+      <c r="F156" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G156" s="38" t="s">
@@ -14472,9 +14480,9 @@
       <c r="C157" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="D157" s="62"/>
-      <c r="E157" s="63"/>
-      <c r="F157" s="63"/>
+      <c r="D157" s="65"/>
+      <c r="E157" s="64"/>
+      <c r="F157" s="64"/>
       <c r="G157" s="38" t="s">
         <v>33</v>
       </c>
@@ -14483,9 +14491,9 @@
       <c r="C158" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="D158" s="62"/>
-      <c r="E158" s="63"/>
-      <c r="F158" s="63"/>
+      <c r="D158" s="65"/>
+      <c r="E158" s="64"/>
+      <c r="F158" s="64"/>
       <c r="G158" s="38" t="s">
         <v>33</v>
       </c>
@@ -14494,11 +14502,11 @@
       <c r="C159" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="D159" s="62" t="s">
+      <c r="D159" s="65" t="s">
         <v>131</v>
       </c>
-      <c r="E159" s="63"/>
-      <c r="F159" s="63" t="s">
+      <c r="E159" s="64"/>
+      <c r="F159" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G159" s="38" t="s">
@@ -14509,9 +14517,9 @@
       <c r="C160" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="D160" s="62"/>
-      <c r="E160" s="63"/>
-      <c r="F160" s="63"/>
+      <c r="D160" s="65"/>
+      <c r="E160" s="64"/>
+      <c r="F160" s="64"/>
       <c r="G160" s="38" t="s">
         <v>33</v>
       </c>
@@ -14520,9 +14528,9 @@
       <c r="C161" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="D161" s="62"/>
-      <c r="E161" s="63"/>
-      <c r="F161" s="63"/>
+      <c r="D161" s="65"/>
+      <c r="E161" s="64"/>
+      <c r="F161" s="64"/>
       <c r="G161" s="38" t="s">
         <v>33</v>
       </c>
@@ -14531,11 +14539,11 @@
       <c r="C162" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="D162" s="62" t="s">
+      <c r="D162" s="65" t="s">
         <v>159</v>
       </c>
-      <c r="E162" s="63"/>
-      <c r="F162" s="63" t="s">
+      <c r="E162" s="64"/>
+      <c r="F162" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G162" s="38" t="s">
@@ -14546,9 +14554,9 @@
       <c r="C163" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="D163" s="62"/>
-      <c r="E163" s="63"/>
-      <c r="F163" s="63"/>
+      <c r="D163" s="65"/>
+      <c r="E163" s="64"/>
+      <c r="F163" s="64"/>
       <c r="G163" s="38" t="s">
         <v>33</v>
       </c>
@@ -14557,11 +14565,11 @@
       <c r="C164" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="D164" s="62" t="s">
+      <c r="D164" s="65" t="s">
         <v>164</v>
       </c>
-      <c r="E164" s="63"/>
-      <c r="F164" s="63" t="s">
+      <c r="E164" s="64"/>
+      <c r="F164" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G164" s="38" t="s">
@@ -14572,9 +14580,9 @@
       <c r="C165" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="D165" s="62"/>
-      <c r="E165" s="63"/>
-      <c r="F165" s="63"/>
+      <c r="D165" s="65"/>
+      <c r="E165" s="64"/>
+      <c r="F165" s="64"/>
       <c r="G165" s="38" t="s">
         <v>33</v>
       </c>
@@ -14583,9 +14591,9 @@
       <c r="C166" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="D166" s="62"/>
-      <c r="E166" s="63"/>
-      <c r="F166" s="63"/>
+      <c r="D166" s="65"/>
+      <c r="E166" s="64"/>
+      <c r="F166" s="64"/>
       <c r="G166" s="38" t="s">
         <v>33</v>
       </c>
@@ -14594,11 +14602,11 @@
       <c r="C167" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="D167" s="62" t="s">
+      <c r="D167" s="65" t="s">
         <v>179</v>
       </c>
-      <c r="E167" s="63"/>
-      <c r="F167" s="63" t="s">
+      <c r="E167" s="64"/>
+      <c r="F167" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G167" s="38" t="s">
@@ -14609,9 +14617,9 @@
       <c r="C168" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="D168" s="62"/>
-      <c r="E168" s="63"/>
-      <c r="F168" s="63"/>
+      <c r="D168" s="65"/>
+      <c r="E168" s="64"/>
+      <c r="F168" s="64"/>
       <c r="G168" s="38" t="s">
         <v>33</v>
       </c>
@@ -14620,9 +14628,9 @@
       <c r="C169" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="D169" s="62"/>
-      <c r="E169" s="63"/>
-      <c r="F169" s="63"/>
+      <c r="D169" s="65"/>
+      <c r="E169" s="64"/>
+      <c r="F169" s="64"/>
       <c r="G169" s="38" t="s">
         <v>33</v>
       </c>
@@ -14631,11 +14639,11 @@
       <c r="C170" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="D170" s="62" t="s">
+      <c r="D170" s="65" t="s">
         <v>186</v>
       </c>
-      <c r="E170" s="63"/>
-      <c r="F170" s="63" t="s">
+      <c r="E170" s="64"/>
+      <c r="F170" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G170" s="38" t="s">
@@ -14646,9 +14654,9 @@
       <c r="C171" s="34" t="s">
         <v>188</v>
       </c>
-      <c r="D171" s="62"/>
-      <c r="E171" s="63"/>
-      <c r="F171" s="63"/>
+      <c r="D171" s="65"/>
+      <c r="E171" s="64"/>
+      <c r="F171" s="64"/>
       <c r="G171" s="38" t="s">
         <v>33</v>
       </c>
@@ -14657,11 +14665,11 @@
       <c r="C172" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="D172" s="62" t="s">
+      <c r="D172" s="65" t="s">
         <v>195</v>
       </c>
-      <c r="E172" s="63"/>
-      <c r="F172" s="63" t="s">
+      <c r="E172" s="64"/>
+      <c r="F172" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G172" s="38" t="s">
@@ -14672,9 +14680,9 @@
       <c r="C173" s="34" t="s">
         <v>197</v>
       </c>
-      <c r="D173" s="62"/>
-      <c r="E173" s="63"/>
-      <c r="F173" s="63"/>
+      <c r="D173" s="65"/>
+      <c r="E173" s="64"/>
+      <c r="F173" s="64"/>
       <c r="G173" s="38" t="s">
         <v>33</v>
       </c>
@@ -14683,11 +14691,11 @@
       <c r="C174" s="34" t="s">
         <v>199</v>
       </c>
-      <c r="D174" s="62" t="s">
+      <c r="D174" s="65" t="s">
         <v>200</v>
       </c>
-      <c r="E174" s="63"/>
-      <c r="F174" s="63" t="s">
+      <c r="E174" s="64"/>
+      <c r="F174" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G174" s="38" t="s">
@@ -14698,9 +14706,9 @@
       <c r="C175" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="D175" s="62"/>
-      <c r="E175" s="63"/>
-      <c r="F175" s="63"/>
+      <c r="D175" s="65"/>
+      <c r="E175" s="64"/>
+      <c r="F175" s="64"/>
       <c r="G175" s="38" t="s">
         <v>33</v>
       </c>
@@ -14709,11 +14717,11 @@
       <c r="C176" s="34" t="s">
         <v>210</v>
       </c>
-      <c r="D176" s="62" t="s">
+      <c r="D176" s="65" t="s">
         <v>211</v>
       </c>
-      <c r="E176" s="63"/>
-      <c r="F176" s="63" t="s">
+      <c r="E176" s="64"/>
+      <c r="F176" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G176" s="38" t="s">
@@ -14724,9 +14732,9 @@
       <c r="C177" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="D177" s="62"/>
-      <c r="E177" s="63"/>
-      <c r="F177" s="63"/>
+      <c r="D177" s="65"/>
+      <c r="E177" s="64"/>
+      <c r="F177" s="64"/>
       <c r="G177" s="38" t="s">
         <v>33</v>
       </c>
@@ -14735,9 +14743,9 @@
       <c r="C178" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="D178" s="62"/>
-      <c r="E178" s="63"/>
-      <c r="F178" s="63"/>
+      <c r="D178" s="65"/>
+      <c r="E178" s="64"/>
+      <c r="F178" s="64"/>
       <c r="G178" s="38" t="s">
         <v>33</v>
       </c>
@@ -14746,11 +14754,11 @@
       <c r="C179" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="D179" s="62" t="s">
+      <c r="D179" s="65" t="s">
         <v>223</v>
       </c>
-      <c r="E179" s="63"/>
-      <c r="F179" s="63" t="s">
+      <c r="E179" s="64"/>
+      <c r="F179" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G179" s="38" t="s">
@@ -14761,9 +14769,9 @@
       <c r="C180" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="D180" s="62"/>
-      <c r="E180" s="63"/>
-      <c r="F180" s="63"/>
+      <c r="D180" s="65"/>
+      <c r="E180" s="64"/>
+      <c r="F180" s="64"/>
       <c r="G180" s="38" t="s">
         <v>33</v>
       </c>
@@ -14772,11 +14780,11 @@
       <c r="C181" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="D181" s="62" t="s">
+      <c r="D181" s="65" t="s">
         <v>228</v>
       </c>
-      <c r="E181" s="63"/>
-      <c r="F181" s="63" t="s">
+      <c r="E181" s="64"/>
+      <c r="F181" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G181" s="38" t="s">
@@ -14787,9 +14795,9 @@
       <c r="C182" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="D182" s="62"/>
-      <c r="E182" s="63"/>
-      <c r="F182" s="63"/>
+      <c r="D182" s="65"/>
+      <c r="E182" s="64"/>
+      <c r="F182" s="64"/>
       <c r="G182" s="38" t="s">
         <v>33</v>
       </c>
@@ -14798,9 +14806,9 @@
       <c r="C183" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="D183" s="62"/>
-      <c r="E183" s="63"/>
-      <c r="F183" s="63"/>
+      <c r="D183" s="65"/>
+      <c r="E183" s="64"/>
+      <c r="F183" s="64"/>
       <c r="G183" s="38" t="s">
         <v>33</v>
       </c>
@@ -14869,11 +14877,11 @@
       <c r="C188" s="34" t="s">
         <v>454</v>
       </c>
-      <c r="D188" s="62" t="s">
+      <c r="D188" s="65" t="s">
         <v>582</v>
       </c>
-      <c r="E188" s="63"/>
-      <c r="F188" s="63" t="s">
+      <c r="E188" s="64"/>
+      <c r="F188" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G188" s="38" t="s">
@@ -14884,9 +14892,9 @@
       <c r="C189" s="34" t="s">
         <v>457</v>
       </c>
-      <c r="D189" s="62"/>
-      <c r="E189" s="63"/>
-      <c r="F189" s="63"/>
+      <c r="D189" s="65"/>
+      <c r="E189" s="64"/>
+      <c r="F189" s="64"/>
       <c r="G189" s="38" t="s">
         <v>33</v>
       </c>
@@ -14895,11 +14903,11 @@
       <c r="C190" s="34" t="s">
         <v>459</v>
       </c>
-      <c r="D190" s="62" t="s">
+      <c r="D190" s="65" t="s">
         <v>460</v>
       </c>
-      <c r="E190" s="63"/>
-      <c r="F190" s="63" t="s">
+      <c r="E190" s="64"/>
+      <c r="F190" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G190" s="38" t="s">
@@ -14910,9 +14918,9 @@
       <c r="C191" s="34" t="s">
         <v>462</v>
       </c>
-      <c r="D191" s="62"/>
-      <c r="E191" s="63"/>
-      <c r="F191" s="63"/>
+      <c r="D191" s="65"/>
+      <c r="E191" s="64"/>
+      <c r="F191" s="64"/>
       <c r="G191" s="38" t="s">
         <v>33</v>
       </c>
@@ -14968,11 +14976,11 @@
       <c r="C195" s="34" t="s">
         <v>477</v>
       </c>
-      <c r="D195" s="62" t="s">
+      <c r="D195" s="65" t="s">
         <v>478</v>
       </c>
-      <c r="E195" s="63"/>
-      <c r="F195" s="63" t="s">
+      <c r="E195" s="64"/>
+      <c r="F195" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G195" s="38" t="s">
@@ -14986,9 +14994,9 @@
       <c r="C196" s="35" t="s">
         <v>480</v>
       </c>
-      <c r="D196" s="69"/>
-      <c r="E196" s="70"/>
-      <c r="F196" s="70"/>
+      <c r="D196" s="67"/>
+      <c r="E196" s="69"/>
+      <c r="F196" s="69"/>
       <c r="G196" s="39" t="s">
         <v>33</v>
       </c>
@@ -15011,7 +15019,7 @@
       <c r="D198" s="36"/>
       <c r="E198" s="42">
         <f>COUNTBLANK(E2:E196)</f>
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F198" s="43"/>
       <c r="G198" s="36"/>
@@ -15024,7 +15032,7 @@
       <c r="D199" s="36"/>
       <c r="E199" s="42">
         <f>COUNTA(E2:E196)</f>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F199" s="43"/>
       <c r="G199" s="36"/>
@@ -15052,6 +15060,183 @@
     </row>
   </sheetData>
   <mergeCells count="201">
+    <mergeCell ref="D140:D142"/>
+    <mergeCell ref="E140:E142"/>
+    <mergeCell ref="F140:F142"/>
+    <mergeCell ref="D143:D145"/>
+    <mergeCell ref="E143:E145"/>
+    <mergeCell ref="F143:F145"/>
+    <mergeCell ref="E100:E102"/>
+    <mergeCell ref="E105:E106"/>
+    <mergeCell ref="F105:F106"/>
+    <mergeCell ref="E107:E108"/>
+    <mergeCell ref="F107:F108"/>
+    <mergeCell ref="E109:E110"/>
+    <mergeCell ref="F109:F110"/>
+    <mergeCell ref="E111:E112"/>
+    <mergeCell ref="F111:F112"/>
+    <mergeCell ref="D120:D123"/>
+    <mergeCell ref="D124:D125"/>
+    <mergeCell ref="D126:D127"/>
+    <mergeCell ref="D128:D129"/>
+    <mergeCell ref="D130:D131"/>
+    <mergeCell ref="D132:D133"/>
+    <mergeCell ref="D134:D135"/>
+    <mergeCell ref="F138:F139"/>
+    <mergeCell ref="E118:E119"/>
+    <mergeCell ref="F130:F131"/>
+    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="F134:F135"/>
+    <mergeCell ref="E138:E139"/>
+    <mergeCell ref="F136:F137"/>
+    <mergeCell ref="D136:D137"/>
+    <mergeCell ref="D138:D139"/>
+    <mergeCell ref="D118:D119"/>
+    <mergeCell ref="E124:E125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="E128:E129"/>
+    <mergeCell ref="E130:E131"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="E134:E135"/>
+    <mergeCell ref="E136:E137"/>
+    <mergeCell ref="F118:F119"/>
+    <mergeCell ref="E120:E123"/>
+    <mergeCell ref="F120:F123"/>
+    <mergeCell ref="F124:F125"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="F128:F129"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="D100:D102"/>
+    <mergeCell ref="D105:D106"/>
+    <mergeCell ref="D107:D108"/>
+    <mergeCell ref="D113:D115"/>
+    <mergeCell ref="D116:D117"/>
+    <mergeCell ref="F113:F115"/>
+    <mergeCell ref="D109:D110"/>
+    <mergeCell ref="D111:D112"/>
+    <mergeCell ref="F100:F102"/>
+    <mergeCell ref="E116:E117"/>
+    <mergeCell ref="F116:F117"/>
+    <mergeCell ref="E113:E115"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="E41:E43"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="G41:G43"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="D154:D155"/>
+    <mergeCell ref="E154:E155"/>
+    <mergeCell ref="F154:F155"/>
+    <mergeCell ref="D156:D158"/>
+    <mergeCell ref="E156:E158"/>
+    <mergeCell ref="F156:F158"/>
+    <mergeCell ref="D149:D150"/>
+    <mergeCell ref="E149:E150"/>
+    <mergeCell ref="F149:F150"/>
+    <mergeCell ref="D151:D153"/>
+    <mergeCell ref="E151:E153"/>
+    <mergeCell ref="F151:F153"/>
+    <mergeCell ref="D164:D166"/>
+    <mergeCell ref="E164:E166"/>
+    <mergeCell ref="F164:F166"/>
+    <mergeCell ref="D167:D169"/>
+    <mergeCell ref="E167:E169"/>
+    <mergeCell ref="F167:F169"/>
+    <mergeCell ref="D159:D161"/>
+    <mergeCell ref="E159:E161"/>
+    <mergeCell ref="F159:F161"/>
+    <mergeCell ref="D162:D163"/>
+    <mergeCell ref="E162:E163"/>
+    <mergeCell ref="F162:F163"/>
+    <mergeCell ref="D174:D175"/>
+    <mergeCell ref="E174:E175"/>
+    <mergeCell ref="F174:F175"/>
+    <mergeCell ref="D176:D178"/>
+    <mergeCell ref="E176:E178"/>
+    <mergeCell ref="F176:F178"/>
+    <mergeCell ref="D170:D171"/>
+    <mergeCell ref="E170:E171"/>
+    <mergeCell ref="F170:F171"/>
+    <mergeCell ref="D172:D173"/>
+    <mergeCell ref="E172:E173"/>
+    <mergeCell ref="F172:F173"/>
+    <mergeCell ref="D195:D196"/>
+    <mergeCell ref="E195:E196"/>
+    <mergeCell ref="F195:F196"/>
+    <mergeCell ref="D179:D180"/>
+    <mergeCell ref="E179:E180"/>
+    <mergeCell ref="F179:F180"/>
+    <mergeCell ref="D181:D183"/>
+    <mergeCell ref="E181:E183"/>
+    <mergeCell ref="F181:F183"/>
+    <mergeCell ref="D188:D189"/>
+    <mergeCell ref="D190:D191"/>
+    <mergeCell ref="F188:F189"/>
+    <mergeCell ref="F190:F191"/>
+    <mergeCell ref="E188:E189"/>
+    <mergeCell ref="E190:E191"/>
     <mergeCell ref="O5:O6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
@@ -15076,183 +15261,6 @@
     <mergeCell ref="D34:D35"/>
     <mergeCell ref="E34:E35"/>
     <mergeCell ref="F34:F35"/>
-    <mergeCell ref="D195:D196"/>
-    <mergeCell ref="E195:E196"/>
-    <mergeCell ref="F195:F196"/>
-    <mergeCell ref="D179:D180"/>
-    <mergeCell ref="E179:E180"/>
-    <mergeCell ref="F179:F180"/>
-    <mergeCell ref="D181:D183"/>
-    <mergeCell ref="E181:E183"/>
-    <mergeCell ref="F181:F183"/>
-    <mergeCell ref="D188:D189"/>
-    <mergeCell ref="D190:D191"/>
-    <mergeCell ref="F188:F189"/>
-    <mergeCell ref="F190:F191"/>
-    <mergeCell ref="E188:E189"/>
-    <mergeCell ref="E190:E191"/>
-    <mergeCell ref="D174:D175"/>
-    <mergeCell ref="E174:E175"/>
-    <mergeCell ref="F174:F175"/>
-    <mergeCell ref="D176:D178"/>
-    <mergeCell ref="E176:E178"/>
-    <mergeCell ref="F176:F178"/>
-    <mergeCell ref="D170:D171"/>
-    <mergeCell ref="E170:E171"/>
-    <mergeCell ref="F170:F171"/>
-    <mergeCell ref="D172:D173"/>
-    <mergeCell ref="E172:E173"/>
-    <mergeCell ref="F172:F173"/>
-    <mergeCell ref="D164:D166"/>
-    <mergeCell ref="E164:E166"/>
-    <mergeCell ref="F164:F166"/>
-    <mergeCell ref="D167:D169"/>
-    <mergeCell ref="E167:E169"/>
-    <mergeCell ref="F167:F169"/>
-    <mergeCell ref="D159:D161"/>
-    <mergeCell ref="E159:E161"/>
-    <mergeCell ref="F159:F161"/>
-    <mergeCell ref="D162:D163"/>
-    <mergeCell ref="E162:E163"/>
-    <mergeCell ref="F162:F163"/>
-    <mergeCell ref="D154:D155"/>
-    <mergeCell ref="E154:E155"/>
-    <mergeCell ref="F154:F155"/>
-    <mergeCell ref="D156:D158"/>
-    <mergeCell ref="E156:E158"/>
-    <mergeCell ref="F156:F158"/>
-    <mergeCell ref="D149:D150"/>
-    <mergeCell ref="E149:E150"/>
-    <mergeCell ref="F149:F150"/>
-    <mergeCell ref="D151:D153"/>
-    <mergeCell ref="E151:E153"/>
-    <mergeCell ref="F151:F153"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="G41:G43"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="D100:D102"/>
-    <mergeCell ref="D105:D106"/>
-    <mergeCell ref="D107:D108"/>
-    <mergeCell ref="D113:D115"/>
-    <mergeCell ref="D116:D117"/>
-    <mergeCell ref="F113:F115"/>
-    <mergeCell ref="D109:D110"/>
-    <mergeCell ref="D111:D112"/>
-    <mergeCell ref="F100:F102"/>
-    <mergeCell ref="E116:E117"/>
-    <mergeCell ref="F116:F117"/>
-    <mergeCell ref="E113:E115"/>
-    <mergeCell ref="F130:F131"/>
-    <mergeCell ref="F132:F133"/>
-    <mergeCell ref="F134:F135"/>
-    <mergeCell ref="E138:E139"/>
-    <mergeCell ref="F136:F137"/>
-    <mergeCell ref="D136:D137"/>
-    <mergeCell ref="D138:D139"/>
-    <mergeCell ref="D118:D119"/>
-    <mergeCell ref="E124:E125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="E128:E129"/>
-    <mergeCell ref="E130:E131"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="E134:E135"/>
-    <mergeCell ref="E136:E137"/>
-    <mergeCell ref="F118:F119"/>
-    <mergeCell ref="E120:E123"/>
-    <mergeCell ref="F120:F123"/>
-    <mergeCell ref="F124:F125"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="F128:F129"/>
-    <mergeCell ref="D140:D142"/>
-    <mergeCell ref="E140:E142"/>
-    <mergeCell ref="F140:F142"/>
-    <mergeCell ref="D143:D145"/>
-    <mergeCell ref="E143:E145"/>
-    <mergeCell ref="F143:F145"/>
-    <mergeCell ref="E100:E102"/>
-    <mergeCell ref="E105:E106"/>
-    <mergeCell ref="F105:F106"/>
-    <mergeCell ref="E107:E108"/>
-    <mergeCell ref="F107:F108"/>
-    <mergeCell ref="E109:E110"/>
-    <mergeCell ref="F109:F110"/>
-    <mergeCell ref="E111:E112"/>
-    <mergeCell ref="F111:F112"/>
-    <mergeCell ref="D120:D123"/>
-    <mergeCell ref="D124:D125"/>
-    <mergeCell ref="D126:D127"/>
-    <mergeCell ref="D128:D129"/>
-    <mergeCell ref="D130:D131"/>
-    <mergeCell ref="D132:D133"/>
-    <mergeCell ref="D134:D135"/>
-    <mergeCell ref="F138:F139"/>
-    <mergeCell ref="E118:E119"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -17889,17 +17897,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEAE28352B96D64C95AA0D5E2FA62FAD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed183881d36ac1b5d7d67982eda510d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d161086-4829-409f-9f75-5bde88dcb151" xmlns:ns3="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="685f4fda20cf913d28bf77c13cd653dd" ns2:_="" ns3:_="">
     <xsd:import namespace="3d161086-4829-409f-9f75-5bde88dcb151"/>
@@ -18122,6 +18119,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -18132,23 +18140,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C74AB5E7-5C87-4FF7-BF80-AB0EB6BD1D32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18167,6 +18158,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
V_MAP_SV_OBSERVATION, V_MAP_TONLY_OBSERVATION and V_MAP_TS_OBSERVATION finalized
</commit_message>
<xml_diff>
--- a/analysis/MEDS_Tables.xlsx
+++ b/analysis/MEDS_Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="746" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DE1EC85-9AD8-4F37-90BC-B1067C6CEA74}"/>
+  <xr:revisionPtr revIDLastSave="749" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{136000BB-3532-4909-A17A-756CDCE40AF9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3163" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3166" uniqueCount="744">
   <si>
     <t>Table</t>
   </si>
@@ -3442,43 +3442,43 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -12013,8 +12013,8 @@
   <dimension ref="A1:P201"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E57" sqref="E57"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12050,7 +12050,7 @@
       <c r="H1" s="45"/>
       <c r="I1" s="41">
         <f>E199/E198</f>
-        <v>0.21118012422360249</v>
+        <v>0.23417721518987342</v>
       </c>
       <c r="J1" s="46" t="s">
         <v>566</v>
@@ -12064,13 +12064,13 @@
       <c r="D2" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="E2" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="68" t="s">
+      <c r="F2" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="70" t="s">
+      <c r="G2" s="68" t="s">
         <v>564</v>
       </c>
     </row>
@@ -12078,10 +12078,10 @@
       <c r="C3" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="65"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="72"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="67"/>
       <c r="K3" s="36"/>
       <c r="L3" s="36"/>
       <c r="M3" s="36"/>
@@ -12093,10 +12093,10 @@
       <c r="C4" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="65"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="72"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="67"/>
       <c r="K4" s="36"/>
       <c r="L4" s="36"/>
       <c r="M4" s="36"/>
@@ -12108,27 +12108,27 @@
       <c r="C5" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="65" t="s">
+      <c r="D5" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="64" t="s">
+      <c r="E5" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="F5" s="64" t="s">
+      <c r="F5" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="72" t="s">
+      <c r="G5" s="67" t="s">
         <v>519</v>
       </c>
       <c r="K5" s="36"/>
       <c r="L5" s="44" t="s">
         <v>464</v>
       </c>
-      <c r="M5" s="63" t="s">
+      <c r="M5" s="74" t="s">
         <v>465</v>
       </c>
-      <c r="N5" s="64"/>
-      <c r="O5" s="62" t="s">
+      <c r="N5" s="63"/>
+      <c r="O5" s="73" t="s">
         <v>581</v>
       </c>
       <c r="P5" s="36"/>
@@ -12137,33 +12137,33 @@
       <c r="C6" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="65"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="72"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="67"/>
       <c r="K6" s="36"/>
       <c r="L6" s="44" t="s">
         <v>467</v>
       </c>
-      <c r="M6" s="63"/>
-      <c r="N6" s="64"/>
-      <c r="O6" s="62"/>
+      <c r="M6" s="74"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="73"/>
       <c r="P6" s="36"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C7" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="65" t="s">
+      <c r="D7" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="64" t="s">
+      <c r="E7" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="64" t="s">
+      <c r="F7" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="72" t="s">
+      <c r="G7" s="67" t="s">
         <v>80</v>
       </c>
       <c r="K7" s="36"/>
@@ -12177,10 +12177,10 @@
       <c r="C8" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="65"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="72"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="67"/>
       <c r="K8" s="36"/>
       <c r="L8" s="36"/>
       <c r="M8" s="36"/>
@@ -12192,16 +12192,16 @@
       <c r="C9" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="D9" s="65" t="s">
+      <c r="D9" s="62" t="s">
         <v>171</v>
       </c>
-      <c r="E9" s="64" t="s">
+      <c r="E9" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="64" t="s">
+      <c r="F9" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="72" t="s">
+      <c r="G9" s="67" t="s">
         <v>523</v>
       </c>
       <c r="J9" s="36"/>
@@ -12211,10 +12211,10 @@
       <c r="C10" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="D10" s="65"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="72"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="67"/>
       <c r="J10" s="36"/>
       <c r="K10" s="36"/>
     </row>
@@ -12222,10 +12222,10 @@
       <c r="C11" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="D11" s="65"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="72"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="67"/>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
     </row>
@@ -12233,16 +12233,16 @@
       <c r="C12" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="D12" s="65" t="s">
+      <c r="D12" s="62" t="s">
         <v>204</v>
       </c>
-      <c r="E12" s="64" t="s">
+      <c r="E12" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="64" t="s">
+      <c r="F12" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="72" t="s">
+      <c r="G12" s="67" t="s">
         <v>515</v>
       </c>
       <c r="J12" s="36"/>
@@ -12252,10 +12252,10 @@
       <c r="C13" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="D13" s="65"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="72"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="67"/>
       <c r="J13" s="36"/>
       <c r="K13" s="36"/>
     </row>
@@ -12263,16 +12263,16 @@
       <c r="C14" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="D14" s="65" t="s">
+      <c r="D14" s="62" t="s">
         <v>361</v>
       </c>
-      <c r="E14" s="64" t="s">
+      <c r="E14" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="F14" s="64" t="s">
+      <c r="F14" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="72" t="s">
+      <c r="G14" s="67" t="s">
         <v>518</v>
       </c>
       <c r="J14" s="36"/>
@@ -12282,9 +12282,9 @@
       <c r="C15" s="35" t="s">
         <v>363</v>
       </c>
-      <c r="D15" s="67"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
       <c r="G15" s="71"/>
       <c r="J15" s="36"/>
       <c r="K15" s="36"/>
@@ -12296,13 +12296,13 @@
       <c r="D16" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="68" t="s">
+      <c r="E16" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F16" s="68" t="s">
+      <c r="F16" s="64" t="s">
         <v>567</v>
       </c>
-      <c r="G16" s="70" t="s">
+      <c r="G16" s="68" t="s">
         <v>73</v>
       </c>
       <c r="J16" s="36"/>
@@ -12312,10 +12312,10 @@
       <c r="C17" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="65"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="72"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="67"/>
       <c r="J17" s="36"/>
       <c r="K17" s="36"/>
     </row>
@@ -12323,16 +12323,16 @@
       <c r="C18" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="65" t="s">
+      <c r="D18" s="62" t="s">
         <v>105</v>
       </c>
-      <c r="E18" s="64" t="s">
+      <c r="E18" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="F18" s="64" t="s">
+      <c r="F18" s="63" t="s">
         <v>567</v>
       </c>
-      <c r="G18" s="72" t="s">
+      <c r="G18" s="67" t="s">
         <v>524</v>
       </c>
       <c r="J18" s="36"/>
@@ -12342,10 +12342,10 @@
       <c r="C19" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="65"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="72"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="67"/>
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
     </row>
@@ -12353,16 +12353,16 @@
       <c r="C20" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="D20" s="65" t="s">
+      <c r="D20" s="62" t="s">
         <v>300</v>
       </c>
-      <c r="E20" s="64" t="s">
+      <c r="E20" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="F20" s="64" t="s">
+      <c r="F20" s="63" t="s">
         <v>567</v>
       </c>
-      <c r="G20" s="72" t="s">
+      <c r="G20" s="67" t="s">
         <v>516</v>
       </c>
       <c r="J20" s="36"/>
@@ -12372,10 +12372,10 @@
       <c r="C21" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="D21" s="65"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="72"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="67"/>
       <c r="J21" s="36"/>
       <c r="K21" s="36"/>
     </row>
@@ -12383,16 +12383,16 @@
       <c r="C22" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="D22" s="65" t="s">
+      <c r="D22" s="62" t="s">
         <v>305</v>
       </c>
-      <c r="E22" s="64" t="s">
+      <c r="E22" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="F22" s="64" t="s">
+      <c r="F22" s="63" t="s">
         <v>567</v>
       </c>
-      <c r="G22" s="72" t="s">
+      <c r="G22" s="67" t="s">
         <v>521</v>
       </c>
       <c r="J22" s="36"/>
@@ -12402,10 +12402,10 @@
       <c r="C23" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="D23" s="65"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="72"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="67"/>
       <c r="J23" s="36"/>
       <c r="K23" s="36"/>
     </row>
@@ -12413,16 +12413,16 @@
       <c r="C24" s="34" t="s">
         <v>317</v>
       </c>
-      <c r="D24" s="65" t="s">
+      <c r="D24" s="62" t="s">
         <v>318</v>
       </c>
-      <c r="E24" s="64" t="s">
+      <c r="E24" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="F24" s="64" t="s">
+      <c r="F24" s="63" t="s">
         <v>567</v>
       </c>
-      <c r="G24" s="72" t="s">
+      <c r="G24" s="67" t="s">
         <v>512</v>
       </c>
       <c r="J24" s="36"/>
@@ -12432,10 +12432,10 @@
       <c r="C25" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="D25" s="65"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="64"/>
-      <c r="G25" s="72"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="67"/>
       <c r="J25" s="36"/>
       <c r="K25" s="36"/>
     </row>
@@ -12443,16 +12443,16 @@
       <c r="C26" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="D26" s="73" t="s">
+      <c r="D26" s="65" t="s">
         <v>323</v>
       </c>
-      <c r="E26" s="74" t="s">
+      <c r="E26" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="F26" s="64" t="s">
+      <c r="F26" s="63" t="s">
         <v>567</v>
       </c>
-      <c r="G26" s="72" t="s">
+      <c r="G26" s="67" t="s">
         <v>517</v>
       </c>
       <c r="J26" s="36"/>
@@ -12462,25 +12462,25 @@
       <c r="C27" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="D27" s="73"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="72"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="67"/>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C28" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="D28" s="65" t="s">
+      <c r="D28" s="62" t="s">
         <v>328</v>
       </c>
-      <c r="E28" s="64" t="s">
+      <c r="E28" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="F28" s="64" t="s">
+      <c r="F28" s="63" t="s">
         <v>567</v>
       </c>
-      <c r="G28" s="72" t="s">
+      <c r="G28" s="67" t="s">
         <v>508</v>
       </c>
     </row>
@@ -12488,25 +12488,25 @@
       <c r="C29" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="D29" s="65"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="64"/>
-      <c r="G29" s="72"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="67"/>
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C30" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="D30" s="65" t="s">
+      <c r="D30" s="62" t="s">
         <v>333</v>
       </c>
-      <c r="E30" s="64" t="s">
+      <c r="E30" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="F30" s="64" t="s">
+      <c r="F30" s="63" t="s">
         <v>567</v>
       </c>
-      <c r="G30" s="72" t="s">
+      <c r="G30" s="67" t="s">
         <v>510</v>
       </c>
     </row>
@@ -12514,25 +12514,25 @@
       <c r="C31" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="D31" s="65"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="64"/>
-      <c r="G31" s="72"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="63"/>
+      <c r="G31" s="67"/>
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="D32" s="65" t="s">
+      <c r="D32" s="62" t="s">
         <v>338</v>
       </c>
-      <c r="E32" s="64" t="s">
+      <c r="E32" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="F32" s="64" t="s">
+      <c r="F32" s="63" t="s">
         <v>567</v>
       </c>
-      <c r="G32" s="72" t="s">
+      <c r="G32" s="67" t="s">
         <v>511</v>
       </c>
     </row>
@@ -12540,25 +12540,25 @@
       <c r="C33" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="D33" s="65"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64"/>
-      <c r="G33" s="72"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="67"/>
     </row>
     <row r="34" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C34" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="D34" s="65" t="s">
+      <c r="D34" s="62" t="s">
         <v>343</v>
       </c>
-      <c r="E34" s="64" t="s">
+      <c r="E34" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="F34" s="64" t="s">
+      <c r="F34" s="63" t="s">
         <v>567</v>
       </c>
-      <c r="G34" s="72" t="s">
+      <c r="G34" s="67" t="s">
         <v>509</v>
       </c>
     </row>
@@ -12566,25 +12566,25 @@
       <c r="C35" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="D35" s="65"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="64"/>
-      <c r="G35" s="72"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="67"/>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C36" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="D36" s="65" t="s">
+      <c r="D36" s="62" t="s">
         <v>348</v>
       </c>
-      <c r="E36" s="64" t="s">
+      <c r="E36" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="F36" s="64" t="s">
+      <c r="F36" s="63" t="s">
         <v>567</v>
       </c>
-      <c r="G36" s="72" t="s">
+      <c r="G36" s="67" t="s">
         <v>520</v>
       </c>
     </row>
@@ -12592,9 +12592,9 @@
       <c r="C37" s="35" t="s">
         <v>350</v>
       </c>
-      <c r="D37" s="67"/>
-      <c r="E37" s="69"/>
-      <c r="F37" s="69"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="70"/>
       <c r="G37" s="71"/>
     </row>
     <row r="38" spans="3:13" x14ac:dyDescent="0.25">
@@ -12604,13 +12604,13 @@
       <c r="D38" s="66" t="s">
         <v>366</v>
       </c>
-      <c r="E38" s="68" t="s">
+      <c r="E38" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="F38" s="68" t="s">
+      <c r="F38" s="64" t="s">
         <v>369</v>
       </c>
-      <c r="G38" s="70" t="s">
+      <c r="G38" s="68" t="s">
         <v>514</v>
       </c>
     </row>
@@ -12618,34 +12618,34 @@
       <c r="C39" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="D39" s="65"/>
-      <c r="E39" s="64"/>
-      <c r="F39" s="64"/>
-      <c r="G39" s="72"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="63"/>
+      <c r="F39" s="63"/>
+      <c r="G39" s="67"/>
     </row>
     <row r="40" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C40" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="D40" s="65"/>
-      <c r="E40" s="64"/>
-      <c r="F40" s="64"/>
-      <c r="G40" s="72"/>
+      <c r="D40" s="62"/>
+      <c r="E40" s="63"/>
+      <c r="F40" s="63"/>
+      <c r="G40" s="67"/>
     </row>
     <row r="41" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C41" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="D41" s="65" t="s">
+      <c r="D41" s="62" t="s">
         <v>371</v>
       </c>
-      <c r="E41" s="64" t="s">
+      <c r="E41" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="F41" s="64" t="s">
+      <c r="F41" s="63" t="s">
         <v>369</v>
       </c>
-      <c r="G41" s="72" t="s">
+      <c r="G41" s="67" t="s">
         <v>513</v>
       </c>
     </row>
@@ -12653,34 +12653,34 @@
       <c r="C42" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="D42" s="65"/>
-      <c r="E42" s="64"/>
-      <c r="F42" s="64"/>
-      <c r="G42" s="72"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="63"/>
+      <c r="F42" s="63"/>
+      <c r="G42" s="67"/>
     </row>
     <row r="43" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C43" s="34" t="s">
         <v>384</v>
       </c>
-      <c r="D43" s="65"/>
-      <c r="E43" s="64"/>
-      <c r="F43" s="64"/>
-      <c r="G43" s="72"/>
+      <c r="D43" s="62"/>
+      <c r="E43" s="63"/>
+      <c r="F43" s="63"/>
+      <c r="G43" s="67"/>
     </row>
     <row r="44" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C44" s="34" t="s">
         <v>373</v>
       </c>
-      <c r="D44" s="65" t="s">
+      <c r="D44" s="62" t="s">
         <v>374</v>
       </c>
-      <c r="E44" s="64" t="s">
+      <c r="E44" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="F44" s="64" t="s">
+      <c r="F44" s="63" t="s">
         <v>369</v>
       </c>
-      <c r="G44" s="72" t="s">
+      <c r="G44" s="67" t="s">
         <v>522</v>
       </c>
     </row>
@@ -12688,19 +12688,19 @@
       <c r="C45" s="34" t="s">
         <v>380</v>
       </c>
-      <c r="D45" s="65"/>
-      <c r="E45" s="64"/>
-      <c r="F45" s="64"/>
-      <c r="G45" s="72"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="63"/>
+      <c r="F45" s="63"/>
+      <c r="G45" s="67"/>
     </row>
     <row r="46" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C46" s="34" t="s">
         <v>386</v>
       </c>
-      <c r="D46" s="65"/>
-      <c r="E46" s="64"/>
-      <c r="F46" s="64"/>
-      <c r="G46" s="72"/>
+      <c r="D46" s="62"/>
+      <c r="E46" s="63"/>
+      <c r="F46" s="63"/>
+      <c r="G46" s="67"/>
       <c r="J46" s="36"/>
       <c r="K46" s="36"/>
       <c r="L46" s="36"/>
@@ -12713,11 +12713,11 @@
       <c r="D47" s="66" t="s">
         <v>465</v>
       </c>
-      <c r="E47" s="68"/>
-      <c r="F47" s="68" t="s">
+      <c r="E47" s="64"/>
+      <c r="F47" s="64" t="s">
         <v>584</v>
       </c>
-      <c r="G47" s="70" t="s">
+      <c r="G47" s="68" t="s">
         <v>585</v>
       </c>
       <c r="J47" s="36"/>
@@ -12729,9 +12729,9 @@
       <c r="C48" s="35" t="s">
         <v>467</v>
       </c>
-      <c r="D48" s="67"/>
-      <c r="E48" s="69"/>
-      <c r="F48" s="69"/>
+      <c r="D48" s="69"/>
+      <c r="E48" s="70"/>
+      <c r="F48" s="70"/>
       <c r="G48" s="71"/>
       <c r="J48" s="36"/>
       <c r="K48" s="36"/>
@@ -13570,7 +13570,9 @@
         <v>681</v>
       </c>
       <c r="D96" s="54"/>
-      <c r="E96" s="55"/>
+      <c r="E96" s="55" t="s">
+        <v>81</v>
+      </c>
       <c r="F96" s="55" t="s">
         <v>685</v>
       </c>
@@ -13587,7 +13589,9 @@
         <v>682</v>
       </c>
       <c r="D97" s="54"/>
-      <c r="E97" s="55"/>
+      <c r="E97" s="55" t="s">
+        <v>81</v>
+      </c>
       <c r="F97" s="55" t="s">
         <v>685</v>
       </c>
@@ -13604,7 +13608,9 @@
         <v>683</v>
       </c>
       <c r="D98" s="54"/>
-      <c r="E98" s="55"/>
+      <c r="E98" s="55" t="s">
+        <v>81</v>
+      </c>
       <c r="F98" s="55" t="s">
         <v>685</v>
       </c>
@@ -13640,8 +13646,8 @@
       <c r="D100" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="E100" s="68"/>
-      <c r="F100" s="68" t="s">
+      <c r="E100" s="64"/>
+      <c r="F100" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G100" s="60" t="s">
@@ -13656,9 +13662,9 @@
       <c r="C101" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D101" s="65"/>
-      <c r="E101" s="64"/>
-      <c r="F101" s="64"/>
+      <c r="D101" s="62"/>
+      <c r="E101" s="63"/>
+      <c r="F101" s="63"/>
       <c r="G101" s="38" t="s">
         <v>33</v>
       </c>
@@ -13671,9 +13677,9 @@
       <c r="C102" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D102" s="65"/>
-      <c r="E102" s="64"/>
-      <c r="F102" s="64"/>
+      <c r="D102" s="62"/>
+      <c r="E102" s="63"/>
+      <c r="F102" s="63"/>
       <c r="G102" s="38" t="s">
         <v>33</v>
       </c>
@@ -13686,11 +13692,11 @@
       <c r="C103" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="D103" s="65" t="s">
+      <c r="D103" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="E103" s="64"/>
-      <c r="F103" s="64" t="s">
+      <c r="E103" s="63"/>
+      <c r="F103" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G103" s="38" t="s">
@@ -13705,9 +13711,9 @@
       <c r="C104" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D104" s="65"/>
-      <c r="E104" s="64"/>
-      <c r="F104" s="64"/>
+      <c r="D104" s="62"/>
+      <c r="E104" s="63"/>
+      <c r="F104" s="63"/>
       <c r="G104" s="38" t="s">
         <v>33</v>
       </c>
@@ -13720,11 +13726,11 @@
       <c r="C105" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D105" s="65" t="s">
+      <c r="D105" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="E105" s="64"/>
-      <c r="F105" s="64" t="s">
+      <c r="E105" s="63"/>
+      <c r="F105" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G105" s="38" t="s">
@@ -13739,9 +13745,9 @@
       <c r="C106" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D106" s="65"/>
-      <c r="E106" s="64"/>
-      <c r="F106" s="64"/>
+      <c r="D106" s="62"/>
+      <c r="E106" s="63"/>
+      <c r="F106" s="63"/>
       <c r="G106" s="38" t="s">
         <v>33</v>
       </c>
@@ -13754,11 +13760,11 @@
       <c r="C107" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D107" s="65" t="s">
+      <c r="D107" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="E107" s="64"/>
-      <c r="F107" s="64" t="s">
+      <c r="E107" s="63"/>
+      <c r="F107" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G107" s="38" t="s">
@@ -13773,9 +13779,9 @@
       <c r="C108" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D108" s="65"/>
-      <c r="E108" s="64"/>
-      <c r="F108" s="64"/>
+      <c r="D108" s="62"/>
+      <c r="E108" s="63"/>
+      <c r="F108" s="63"/>
       <c r="G108" s="38" t="s">
         <v>33</v>
       </c>
@@ -13788,11 +13794,11 @@
       <c r="C109" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="D109" s="65" t="s">
+      <c r="D109" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="E109" s="64"/>
-      <c r="F109" s="64" t="s">
+      <c r="E109" s="63"/>
+      <c r="F109" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G109" s="38" t="s">
@@ -13807,9 +13813,9 @@
       <c r="C110" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D110" s="65"/>
-      <c r="E110" s="64"/>
-      <c r="F110" s="64"/>
+      <c r="D110" s="62"/>
+      <c r="E110" s="63"/>
+      <c r="F110" s="63"/>
       <c r="G110" s="38" t="s">
         <v>33</v>
       </c>
@@ -13822,11 +13828,11 @@
       <c r="C111" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D111" s="65" t="s">
+      <c r="D111" s="62" t="s">
         <v>105</v>
       </c>
-      <c r="E111" s="64"/>
-      <c r="F111" s="64" t="s">
+      <c r="E111" s="63"/>
+      <c r="F111" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G111" s="38" t="s">
@@ -13841,9 +13847,9 @@
       <c r="C112" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D112" s="65"/>
-      <c r="E112" s="64"/>
-      <c r="F112" s="64"/>
+      <c r="D112" s="62"/>
+      <c r="E112" s="63"/>
+      <c r="F112" s="63"/>
       <c r="G112" s="38" t="s">
         <v>33</v>
       </c>
@@ -13856,11 +13862,11 @@
       <c r="C113" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="D113" s="65" t="s">
+      <c r="D113" s="62" t="s">
         <v>171</v>
       </c>
-      <c r="E113" s="64"/>
-      <c r="F113" s="64" t="s">
+      <c r="E113" s="63"/>
+      <c r="F113" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G113" s="38" t="s">
@@ -13875,9 +13881,9 @@
       <c r="C114" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="D114" s="65"/>
-      <c r="E114" s="64"/>
-      <c r="F114" s="64"/>
+      <c r="D114" s="62"/>
+      <c r="E114" s="63"/>
+      <c r="F114" s="63"/>
       <c r="G114" s="38" t="s">
         <v>33</v>
       </c>
@@ -13890,9 +13896,9 @@
       <c r="C115" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="D115" s="65"/>
-      <c r="E115" s="64"/>
-      <c r="F115" s="64"/>
+      <c r="D115" s="62"/>
+      <c r="E115" s="63"/>
+      <c r="F115" s="63"/>
       <c r="G115" s="38" t="s">
         <v>33</v>
       </c>
@@ -13905,11 +13911,11 @@
       <c r="C116" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="D116" s="65" t="s">
+      <c r="D116" s="62" t="s">
         <v>204</v>
       </c>
-      <c r="E116" s="64"/>
-      <c r="F116" s="64" t="s">
+      <c r="E116" s="63"/>
+      <c r="F116" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G116" s="38" t="s">
@@ -13924,9 +13930,9 @@
       <c r="C117" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="D117" s="65"/>
-      <c r="E117" s="64"/>
-      <c r="F117" s="64"/>
+      <c r="D117" s="62"/>
+      <c r="E117" s="63"/>
+      <c r="F117" s="63"/>
       <c r="G117" s="38" t="s">
         <v>33</v>
       </c>
@@ -13939,11 +13945,11 @@
       <c r="C118" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="D118" s="65" t="s">
+      <c r="D118" s="62" t="s">
         <v>300</v>
       </c>
-      <c r="E118" s="64"/>
-      <c r="F118" s="64" t="s">
+      <c r="E118" s="63"/>
+      <c r="F118" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G118" s="38" t="s">
@@ -13958,9 +13964,9 @@
       <c r="C119" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="D119" s="65"/>
-      <c r="E119" s="64"/>
-      <c r="F119" s="64"/>
+      <c r="D119" s="62"/>
+      <c r="E119" s="63"/>
+      <c r="F119" s="63"/>
       <c r="G119" s="38" t="s">
         <v>33</v>
       </c>
@@ -13973,11 +13979,11 @@
       <c r="C120" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="D120" s="65" t="s">
+      <c r="D120" s="62" t="s">
         <v>305</v>
       </c>
-      <c r="E120" s="64"/>
-      <c r="F120" s="64" t="s">
+      <c r="E120" s="63"/>
+      <c r="F120" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G120" s="38" t="s">
@@ -13992,9 +13998,9 @@
       <c r="C121" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="D121" s="65"/>
-      <c r="E121" s="64"/>
-      <c r="F121" s="64"/>
+      <c r="D121" s="62"/>
+      <c r="E121" s="63"/>
+      <c r="F121" s="63"/>
       <c r="G121" s="38" t="s">
         <v>33</v>
       </c>
@@ -14007,9 +14013,9 @@
       <c r="C122" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="D122" s="65"/>
-      <c r="E122" s="64"/>
-      <c r="F122" s="64"/>
+      <c r="D122" s="62"/>
+      <c r="E122" s="63"/>
+      <c r="F122" s="63"/>
       <c r="G122" s="38" t="s">
         <v>33</v>
       </c>
@@ -14022,9 +14028,9 @@
       <c r="C123" s="34" t="s">
         <v>311</v>
       </c>
-      <c r="D123" s="65"/>
-      <c r="E123" s="64"/>
-      <c r="F123" s="64"/>
+      <c r="D123" s="62"/>
+      <c r="E123" s="63"/>
+      <c r="F123" s="63"/>
       <c r="G123" s="38" t="s">
         <v>33</v>
       </c>
@@ -14037,11 +14043,11 @@
       <c r="C124" s="34" t="s">
         <v>317</v>
       </c>
-      <c r="D124" s="65" t="s">
+      <c r="D124" s="62" t="s">
         <v>318</v>
       </c>
-      <c r="E124" s="64"/>
-      <c r="F124" s="64" t="s">
+      <c r="E124" s="63"/>
+      <c r="F124" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G124" s="38" t="s">
@@ -14056,9 +14062,9 @@
       <c r="C125" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="D125" s="65"/>
-      <c r="E125" s="64"/>
-      <c r="F125" s="64"/>
+      <c r="D125" s="62"/>
+      <c r="E125" s="63"/>
+      <c r="F125" s="63"/>
       <c r="G125" s="38" t="s">
         <v>33</v>
       </c>
@@ -14071,11 +14077,11 @@
       <c r="C126" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="D126" s="73" t="s">
+      <c r="D126" s="65" t="s">
         <v>323</v>
       </c>
-      <c r="E126" s="64"/>
-      <c r="F126" s="64" t="s">
+      <c r="E126" s="63"/>
+      <c r="F126" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G126" s="38" t="s">
@@ -14090,9 +14096,9 @@
       <c r="C127" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="D127" s="73"/>
-      <c r="E127" s="64"/>
-      <c r="F127" s="64"/>
+      <c r="D127" s="65"/>
+      <c r="E127" s="63"/>
+      <c r="F127" s="63"/>
       <c r="G127" s="38" t="s">
         <v>33</v>
       </c>
@@ -14101,11 +14107,11 @@
       <c r="C128" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="D128" s="65" t="s">
+      <c r="D128" s="62" t="s">
         <v>328</v>
       </c>
-      <c r="E128" s="64"/>
-      <c r="F128" s="64" t="s">
+      <c r="E128" s="63"/>
+      <c r="F128" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G128" s="38" t="s">
@@ -14116,9 +14122,9 @@
       <c r="C129" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="D129" s="65"/>
-      <c r="E129" s="64"/>
-      <c r="F129" s="64"/>
+      <c r="D129" s="62"/>
+      <c r="E129" s="63"/>
+      <c r="F129" s="63"/>
       <c r="G129" s="38" t="s">
         <v>33</v>
       </c>
@@ -14127,11 +14133,11 @@
       <c r="C130" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="D130" s="65" t="s">
+      <c r="D130" s="62" t="s">
         <v>333</v>
       </c>
-      <c r="E130" s="64"/>
-      <c r="F130" s="64" t="s">
+      <c r="E130" s="63"/>
+      <c r="F130" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G130" s="38" t="s">
@@ -14142,9 +14148,9 @@
       <c r="C131" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="D131" s="65"/>
-      <c r="E131" s="64"/>
-      <c r="F131" s="64"/>
+      <c r="D131" s="62"/>
+      <c r="E131" s="63"/>
+      <c r="F131" s="63"/>
       <c r="G131" s="38" t="s">
         <v>33</v>
       </c>
@@ -14153,11 +14159,11 @@
       <c r="C132" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="D132" s="65" t="s">
+      <c r="D132" s="62" t="s">
         <v>338</v>
       </c>
-      <c r="E132" s="64"/>
-      <c r="F132" s="64" t="s">
+      <c r="E132" s="63"/>
+      <c r="F132" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G132" s="38" t="s">
@@ -14168,9 +14174,9 @@
       <c r="C133" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="D133" s="65"/>
-      <c r="E133" s="64"/>
-      <c r="F133" s="64"/>
+      <c r="D133" s="62"/>
+      <c r="E133" s="63"/>
+      <c r="F133" s="63"/>
       <c r="G133" s="38" t="s">
         <v>33</v>
       </c>
@@ -14179,11 +14185,11 @@
       <c r="C134" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="D134" s="65" t="s">
+      <c r="D134" s="62" t="s">
         <v>343</v>
       </c>
-      <c r="E134" s="64"/>
-      <c r="F134" s="64" t="s">
+      <c r="E134" s="63"/>
+      <c r="F134" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G134" s="38" t="s">
@@ -14194,9 +14200,9 @@
       <c r="C135" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="D135" s="65"/>
-      <c r="E135" s="64"/>
-      <c r="F135" s="64"/>
+      <c r="D135" s="62"/>
+      <c r="E135" s="63"/>
+      <c r="F135" s="63"/>
       <c r="G135" s="38" t="s">
         <v>33</v>
       </c>
@@ -14205,11 +14211,11 @@
       <c r="C136" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="D136" s="65" t="s">
+      <c r="D136" s="62" t="s">
         <v>348</v>
       </c>
-      <c r="E136" s="64"/>
-      <c r="F136" s="64" t="s">
+      <c r="E136" s="63"/>
+      <c r="F136" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G136" s="38" t="s">
@@ -14220,9 +14226,9 @@
       <c r="C137" s="34" t="s">
         <v>350</v>
       </c>
-      <c r="D137" s="65"/>
-      <c r="E137" s="64"/>
-      <c r="F137" s="64"/>
+      <c r="D137" s="62"/>
+      <c r="E137" s="63"/>
+      <c r="F137" s="63"/>
       <c r="G137" s="38" t="s">
         <v>33</v>
       </c>
@@ -14231,11 +14237,11 @@
       <c r="C138" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="D138" s="65" t="s">
+      <c r="D138" s="62" t="s">
         <v>361</v>
       </c>
-      <c r="E138" s="64"/>
-      <c r="F138" s="64" t="s">
+      <c r="E138" s="63"/>
+      <c r="F138" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G138" s="38" t="s">
@@ -14246,9 +14252,9 @@
       <c r="C139" s="34" t="s">
         <v>363</v>
       </c>
-      <c r="D139" s="65"/>
-      <c r="E139" s="64"/>
-      <c r="F139" s="64"/>
+      <c r="D139" s="62"/>
+      <c r="E139" s="63"/>
+      <c r="F139" s="63"/>
       <c r="G139" s="38" t="s">
         <v>33</v>
       </c>
@@ -14257,11 +14263,11 @@
       <c r="C140" s="34" t="s">
         <v>365</v>
       </c>
-      <c r="D140" s="65" t="s">
+      <c r="D140" s="62" t="s">
         <v>366</v>
       </c>
-      <c r="E140" s="64"/>
-      <c r="F140" s="64" t="s">
+      <c r="E140" s="63"/>
+      <c r="F140" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G140" s="38" t="s">
@@ -14272,9 +14278,9 @@
       <c r="C141" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="D141" s="65"/>
-      <c r="E141" s="64"/>
-      <c r="F141" s="64"/>
+      <c r="D141" s="62"/>
+      <c r="E141" s="63"/>
+      <c r="F141" s="63"/>
       <c r="G141" s="38" t="s">
         <v>33</v>
       </c>
@@ -14283,9 +14289,9 @@
       <c r="C142" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="D142" s="65"/>
-      <c r="E142" s="64"/>
-      <c r="F142" s="64"/>
+      <c r="D142" s="62"/>
+      <c r="E142" s="63"/>
+      <c r="F142" s="63"/>
       <c r="G142" s="38" t="s">
         <v>33</v>
       </c>
@@ -14294,11 +14300,11 @@
       <c r="C143" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="D143" s="65" t="s">
+      <c r="D143" s="62" t="s">
         <v>371</v>
       </c>
-      <c r="E143" s="64"/>
-      <c r="F143" s="64" t="s">
+      <c r="E143" s="63"/>
+      <c r="F143" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G143" s="38" t="s">
@@ -14309,9 +14315,9 @@
       <c r="C144" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="D144" s="65"/>
-      <c r="E144" s="64"/>
-      <c r="F144" s="64"/>
+      <c r="D144" s="62"/>
+      <c r="E144" s="63"/>
+      <c r="F144" s="63"/>
       <c r="G144" s="38" t="s">
         <v>33</v>
       </c>
@@ -14320,9 +14326,9 @@
       <c r="C145" s="34" t="s">
         <v>384</v>
       </c>
-      <c r="D145" s="65"/>
-      <c r="E145" s="64"/>
-      <c r="F145" s="64"/>
+      <c r="D145" s="62"/>
+      <c r="E145" s="63"/>
+      <c r="F145" s="63"/>
       <c r="G145" s="38" t="s">
         <v>33</v>
       </c>
@@ -14332,11 +14338,11 @@
       <c r="C146" s="34" t="s">
         <v>373</v>
       </c>
-      <c r="D146" s="65" t="s">
+      <c r="D146" s="62" t="s">
         <v>374</v>
       </c>
-      <c r="E146" s="64"/>
-      <c r="F146" s="64" t="s">
+      <c r="E146" s="63"/>
+      <c r="F146" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G146" s="38" t="s">
@@ -14348,9 +14354,9 @@
       <c r="C147" s="34" t="s">
         <v>380</v>
       </c>
-      <c r="D147" s="65"/>
-      <c r="E147" s="64"/>
-      <c r="F147" s="64"/>
+      <c r="D147" s="62"/>
+      <c r="E147" s="63"/>
+      <c r="F147" s="63"/>
       <c r="G147" s="38" t="s">
         <v>33</v>
       </c>
@@ -14360,9 +14366,9 @@
       <c r="C148" s="34" t="s">
         <v>386</v>
       </c>
-      <c r="D148" s="65"/>
-      <c r="E148" s="64"/>
-      <c r="F148" s="64"/>
+      <c r="D148" s="62"/>
+      <c r="E148" s="63"/>
+      <c r="F148" s="63"/>
       <c r="G148" s="38" t="s">
         <v>33</v>
       </c>
@@ -14375,11 +14381,11 @@
       <c r="C149" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="D149" s="65" t="s">
+      <c r="D149" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="E149" s="64"/>
-      <c r="F149" s="64" t="s">
+      <c r="E149" s="63"/>
+      <c r="F149" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G149" s="38" t="s">
@@ -14391,9 +14397,9 @@
       <c r="C150" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="D150" s="65"/>
-      <c r="E150" s="64"/>
-      <c r="F150" s="64"/>
+      <c r="D150" s="62"/>
+      <c r="E150" s="63"/>
+      <c r="F150" s="63"/>
       <c r="G150" s="38" t="s">
         <v>33</v>
       </c>
@@ -14402,11 +14408,11 @@
       <c r="C151" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="D151" s="65" t="s">
+      <c r="D151" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="E151" s="64"/>
-      <c r="F151" s="64" t="s">
+      <c r="E151" s="63"/>
+      <c r="F151" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G151" s="38" t="s">
@@ -14417,9 +14423,9 @@
       <c r="C152" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="D152" s="65"/>
-      <c r="E152" s="64"/>
-      <c r="F152" s="64"/>
+      <c r="D152" s="62"/>
+      <c r="E152" s="63"/>
+      <c r="F152" s="63"/>
       <c r="G152" s="38" t="s">
         <v>33</v>
       </c>
@@ -14428,9 +14434,9 @@
       <c r="C153" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="D153" s="65"/>
-      <c r="E153" s="64"/>
-      <c r="F153" s="64"/>
+      <c r="D153" s="62"/>
+      <c r="E153" s="63"/>
+      <c r="F153" s="63"/>
       <c r="G153" s="38" t="s">
         <v>33</v>
       </c>
@@ -14439,11 +14445,11 @@
       <c r="C154" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="D154" s="65" t="s">
+      <c r="D154" s="62" t="s">
         <v>119</v>
       </c>
-      <c r="E154" s="64"/>
-      <c r="F154" s="64" t="s">
+      <c r="E154" s="63"/>
+      <c r="F154" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G154" s="38" t="s">
@@ -14454,9 +14460,9 @@
       <c r="C155" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="D155" s="65"/>
-      <c r="E155" s="64"/>
-      <c r="F155" s="64"/>
+      <c r="D155" s="62"/>
+      <c r="E155" s="63"/>
+      <c r="F155" s="63"/>
       <c r="G155" s="38" t="s">
         <v>33</v>
       </c>
@@ -14465,11 +14471,11 @@
       <c r="C156" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="D156" s="65" t="s">
+      <c r="D156" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="E156" s="64"/>
-      <c r="F156" s="64" t="s">
+      <c r="E156" s="63"/>
+      <c r="F156" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G156" s="38" t="s">
@@ -14480,9 +14486,9 @@
       <c r="C157" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="D157" s="65"/>
-      <c r="E157" s="64"/>
-      <c r="F157" s="64"/>
+      <c r="D157" s="62"/>
+      <c r="E157" s="63"/>
+      <c r="F157" s="63"/>
       <c r="G157" s="38" t="s">
         <v>33</v>
       </c>
@@ -14491,9 +14497,9 @@
       <c r="C158" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="D158" s="65"/>
-      <c r="E158" s="64"/>
-      <c r="F158" s="64"/>
+      <c r="D158" s="62"/>
+      <c r="E158" s="63"/>
+      <c r="F158" s="63"/>
       <c r="G158" s="38" t="s">
         <v>33</v>
       </c>
@@ -14502,11 +14508,11 @@
       <c r="C159" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="D159" s="65" t="s">
+      <c r="D159" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="E159" s="64"/>
-      <c r="F159" s="64" t="s">
+      <c r="E159" s="63"/>
+      <c r="F159" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G159" s="38" t="s">
@@ -14517,9 +14523,9 @@
       <c r="C160" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="D160" s="65"/>
-      <c r="E160" s="64"/>
-      <c r="F160" s="64"/>
+      <c r="D160" s="62"/>
+      <c r="E160" s="63"/>
+      <c r="F160" s="63"/>
       <c r="G160" s="38" t="s">
         <v>33</v>
       </c>
@@ -14528,9 +14534,9 @@
       <c r="C161" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="D161" s="65"/>
-      <c r="E161" s="64"/>
-      <c r="F161" s="64"/>
+      <c r="D161" s="62"/>
+      <c r="E161" s="63"/>
+      <c r="F161" s="63"/>
       <c r="G161" s="38" t="s">
         <v>33</v>
       </c>
@@ -14539,11 +14545,11 @@
       <c r="C162" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="D162" s="65" t="s">
+      <c r="D162" s="62" t="s">
         <v>159</v>
       </c>
-      <c r="E162" s="64"/>
-      <c r="F162" s="64" t="s">
+      <c r="E162" s="63"/>
+      <c r="F162" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G162" s="38" t="s">
@@ -14554,9 +14560,9 @@
       <c r="C163" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="D163" s="65"/>
-      <c r="E163" s="64"/>
-      <c r="F163" s="64"/>
+      <c r="D163" s="62"/>
+      <c r="E163" s="63"/>
+      <c r="F163" s="63"/>
       <c r="G163" s="38" t="s">
         <v>33</v>
       </c>
@@ -14565,11 +14571,11 @@
       <c r="C164" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="D164" s="65" t="s">
+      <c r="D164" s="62" t="s">
         <v>164</v>
       </c>
-      <c r="E164" s="64"/>
-      <c r="F164" s="64" t="s">
+      <c r="E164" s="63"/>
+      <c r="F164" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G164" s="38" t="s">
@@ -14580,9 +14586,9 @@
       <c r="C165" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="D165" s="65"/>
-      <c r="E165" s="64"/>
-      <c r="F165" s="64"/>
+      <c r="D165" s="62"/>
+      <c r="E165" s="63"/>
+      <c r="F165" s="63"/>
       <c r="G165" s="38" t="s">
         <v>33</v>
       </c>
@@ -14591,9 +14597,9 @@
       <c r="C166" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="D166" s="65"/>
-      <c r="E166" s="64"/>
-      <c r="F166" s="64"/>
+      <c r="D166" s="62"/>
+      <c r="E166" s="63"/>
+      <c r="F166" s="63"/>
       <c r="G166" s="38" t="s">
         <v>33</v>
       </c>
@@ -14602,11 +14608,11 @@
       <c r="C167" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="D167" s="65" t="s">
+      <c r="D167" s="62" t="s">
         <v>179</v>
       </c>
-      <c r="E167" s="64"/>
-      <c r="F167" s="64" t="s">
+      <c r="E167" s="63"/>
+      <c r="F167" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G167" s="38" t="s">
@@ -14617,9 +14623,9 @@
       <c r="C168" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="D168" s="65"/>
-      <c r="E168" s="64"/>
-      <c r="F168" s="64"/>
+      <c r="D168" s="62"/>
+      <c r="E168" s="63"/>
+      <c r="F168" s="63"/>
       <c r="G168" s="38" t="s">
         <v>33</v>
       </c>
@@ -14628,9 +14634,9 @@
       <c r="C169" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="D169" s="65"/>
-      <c r="E169" s="64"/>
-      <c r="F169" s="64"/>
+      <c r="D169" s="62"/>
+      <c r="E169" s="63"/>
+      <c r="F169" s="63"/>
       <c r="G169" s="38" t="s">
         <v>33</v>
       </c>
@@ -14639,11 +14645,11 @@
       <c r="C170" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="D170" s="65" t="s">
+      <c r="D170" s="62" t="s">
         <v>186</v>
       </c>
-      <c r="E170" s="64"/>
-      <c r="F170" s="64" t="s">
+      <c r="E170" s="63"/>
+      <c r="F170" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G170" s="38" t="s">
@@ -14654,9 +14660,9 @@
       <c r="C171" s="34" t="s">
         <v>188</v>
       </c>
-      <c r="D171" s="65"/>
-      <c r="E171" s="64"/>
-      <c r="F171" s="64"/>
+      <c r="D171" s="62"/>
+      <c r="E171" s="63"/>
+      <c r="F171" s="63"/>
       <c r="G171" s="38" t="s">
         <v>33</v>
       </c>
@@ -14665,11 +14671,11 @@
       <c r="C172" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="D172" s="65" t="s">
+      <c r="D172" s="62" t="s">
         <v>195</v>
       </c>
-      <c r="E172" s="64"/>
-      <c r="F172" s="64" t="s">
+      <c r="E172" s="63"/>
+      <c r="F172" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G172" s="38" t="s">
@@ -14680,9 +14686,9 @@
       <c r="C173" s="34" t="s">
         <v>197</v>
       </c>
-      <c r="D173" s="65"/>
-      <c r="E173" s="64"/>
-      <c r="F173" s="64"/>
+      <c r="D173" s="62"/>
+      <c r="E173" s="63"/>
+      <c r="F173" s="63"/>
       <c r="G173" s="38" t="s">
         <v>33</v>
       </c>
@@ -14691,11 +14697,11 @@
       <c r="C174" s="34" t="s">
         <v>199</v>
       </c>
-      <c r="D174" s="65" t="s">
+      <c r="D174" s="62" t="s">
         <v>200</v>
       </c>
-      <c r="E174" s="64"/>
-      <c r="F174" s="64" t="s">
+      <c r="E174" s="63"/>
+      <c r="F174" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G174" s="38" t="s">
@@ -14706,9 +14712,9 @@
       <c r="C175" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="D175" s="65"/>
-      <c r="E175" s="64"/>
-      <c r="F175" s="64"/>
+      <c r="D175" s="62"/>
+      <c r="E175" s="63"/>
+      <c r="F175" s="63"/>
       <c r="G175" s="38" t="s">
         <v>33</v>
       </c>
@@ -14717,11 +14723,11 @@
       <c r="C176" s="34" t="s">
         <v>210</v>
       </c>
-      <c r="D176" s="65" t="s">
+      <c r="D176" s="62" t="s">
         <v>211</v>
       </c>
-      <c r="E176" s="64"/>
-      <c r="F176" s="64" t="s">
+      <c r="E176" s="63"/>
+      <c r="F176" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G176" s="38" t="s">
@@ -14732,9 +14738,9 @@
       <c r="C177" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="D177" s="65"/>
-      <c r="E177" s="64"/>
-      <c r="F177" s="64"/>
+      <c r="D177" s="62"/>
+      <c r="E177" s="63"/>
+      <c r="F177" s="63"/>
       <c r="G177" s="38" t="s">
         <v>33</v>
       </c>
@@ -14743,9 +14749,9 @@
       <c r="C178" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="D178" s="65"/>
-      <c r="E178" s="64"/>
-      <c r="F178" s="64"/>
+      <c r="D178" s="62"/>
+      <c r="E178" s="63"/>
+      <c r="F178" s="63"/>
       <c r="G178" s="38" t="s">
         <v>33</v>
       </c>
@@ -14754,11 +14760,11 @@
       <c r="C179" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="D179" s="65" t="s">
+      <c r="D179" s="62" t="s">
         <v>223</v>
       </c>
-      <c r="E179" s="64"/>
-      <c r="F179" s="64" t="s">
+      <c r="E179" s="63"/>
+      <c r="F179" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G179" s="38" t="s">
@@ -14769,9 +14775,9 @@
       <c r="C180" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="D180" s="65"/>
-      <c r="E180" s="64"/>
-      <c r="F180" s="64"/>
+      <c r="D180" s="62"/>
+      <c r="E180" s="63"/>
+      <c r="F180" s="63"/>
       <c r="G180" s="38" t="s">
         <v>33</v>
       </c>
@@ -14780,11 +14786,11 @@
       <c r="C181" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="D181" s="65" t="s">
+      <c r="D181" s="62" t="s">
         <v>228</v>
       </c>
-      <c r="E181" s="64"/>
-      <c r="F181" s="64" t="s">
+      <c r="E181" s="63"/>
+      <c r="F181" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G181" s="38" t="s">
@@ -14795,9 +14801,9 @@
       <c r="C182" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="D182" s="65"/>
-      <c r="E182" s="64"/>
-      <c r="F182" s="64"/>
+      <c r="D182" s="62"/>
+      <c r="E182" s="63"/>
+      <c r="F182" s="63"/>
       <c r="G182" s="38" t="s">
         <v>33</v>
       </c>
@@ -14806,9 +14812,9 @@
       <c r="C183" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="D183" s="65"/>
-      <c r="E183" s="64"/>
-      <c r="F183" s="64"/>
+      <c r="D183" s="62"/>
+      <c r="E183" s="63"/>
+      <c r="F183" s="63"/>
       <c r="G183" s="38" t="s">
         <v>33</v>
       </c>
@@ -14877,11 +14883,11 @@
       <c r="C188" s="34" t="s">
         <v>454</v>
       </c>
-      <c r="D188" s="65" t="s">
+      <c r="D188" s="62" t="s">
         <v>582</v>
       </c>
-      <c r="E188" s="64"/>
-      <c r="F188" s="64" t="s">
+      <c r="E188" s="63"/>
+      <c r="F188" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G188" s="38" t="s">
@@ -14892,9 +14898,9 @@
       <c r="C189" s="34" t="s">
         <v>457</v>
       </c>
-      <c r="D189" s="65"/>
-      <c r="E189" s="64"/>
-      <c r="F189" s="64"/>
+      <c r="D189" s="62"/>
+      <c r="E189" s="63"/>
+      <c r="F189" s="63"/>
       <c r="G189" s="38" t="s">
         <v>33</v>
       </c>
@@ -14903,11 +14909,11 @@
       <c r="C190" s="34" t="s">
         <v>459</v>
       </c>
-      <c r="D190" s="65" t="s">
+      <c r="D190" s="62" t="s">
         <v>460</v>
       </c>
-      <c r="E190" s="64"/>
-      <c r="F190" s="64" t="s">
+      <c r="E190" s="63"/>
+      <c r="F190" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G190" s="38" t="s">
@@ -14918,9 +14924,9 @@
       <c r="C191" s="34" t="s">
         <v>462</v>
       </c>
-      <c r="D191" s="65"/>
-      <c r="E191" s="64"/>
-      <c r="F191" s="64"/>
+      <c r="D191" s="62"/>
+      <c r="E191" s="63"/>
+      <c r="F191" s="63"/>
       <c r="G191" s="38" t="s">
         <v>33</v>
       </c>
@@ -14976,11 +14982,11 @@
       <c r="C195" s="34" t="s">
         <v>477</v>
       </c>
-      <c r="D195" s="65" t="s">
+      <c r="D195" s="62" t="s">
         <v>478</v>
       </c>
-      <c r="E195" s="64"/>
-      <c r="F195" s="64" t="s">
+      <c r="E195" s="63"/>
+      <c r="F195" s="63" t="s">
         <v>18</v>
       </c>
       <c r="G195" s="38" t="s">
@@ -14994,9 +15000,9 @@
       <c r="C196" s="35" t="s">
         <v>480</v>
       </c>
-      <c r="D196" s="67"/>
-      <c r="E196" s="69"/>
-      <c r="F196" s="69"/>
+      <c r="D196" s="69"/>
+      <c r="E196" s="70"/>
+      <c r="F196" s="70"/>
       <c r="G196" s="39" t="s">
         <v>33</v>
       </c>
@@ -15019,7 +15025,7 @@
       <c r="D198" s="36"/>
       <c r="E198" s="42">
         <f>COUNTBLANK(E2:E196)</f>
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F198" s="43"/>
       <c r="G198" s="36"/>
@@ -15032,7 +15038,7 @@
       <c r="D199" s="36"/>
       <c r="E199" s="42">
         <f>COUNTA(E2:E196)</f>
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F199" s="43"/>
       <c r="G199" s="36"/>
@@ -15060,6 +15066,183 @@
     </row>
   </sheetData>
   <mergeCells count="201">
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="D146:D148"/>
+    <mergeCell ref="E146:E148"/>
+    <mergeCell ref="F146:F148"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="D103:D104"/>
+    <mergeCell ref="E103:E104"/>
+    <mergeCell ref="F103:F104"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="D195:D196"/>
+    <mergeCell ref="E195:E196"/>
+    <mergeCell ref="F195:F196"/>
+    <mergeCell ref="D179:D180"/>
+    <mergeCell ref="E179:E180"/>
+    <mergeCell ref="F179:F180"/>
+    <mergeCell ref="D181:D183"/>
+    <mergeCell ref="E181:E183"/>
+    <mergeCell ref="F181:F183"/>
+    <mergeCell ref="D188:D189"/>
+    <mergeCell ref="D190:D191"/>
+    <mergeCell ref="F188:F189"/>
+    <mergeCell ref="F190:F191"/>
+    <mergeCell ref="E188:E189"/>
+    <mergeCell ref="E190:E191"/>
+    <mergeCell ref="D174:D175"/>
+    <mergeCell ref="E174:E175"/>
+    <mergeCell ref="F174:F175"/>
+    <mergeCell ref="D176:D178"/>
+    <mergeCell ref="E176:E178"/>
+    <mergeCell ref="F176:F178"/>
+    <mergeCell ref="D170:D171"/>
+    <mergeCell ref="E170:E171"/>
+    <mergeCell ref="F170:F171"/>
+    <mergeCell ref="D172:D173"/>
+    <mergeCell ref="E172:E173"/>
+    <mergeCell ref="F172:F173"/>
+    <mergeCell ref="D164:D166"/>
+    <mergeCell ref="E164:E166"/>
+    <mergeCell ref="F164:F166"/>
+    <mergeCell ref="D167:D169"/>
+    <mergeCell ref="E167:E169"/>
+    <mergeCell ref="F167:F169"/>
+    <mergeCell ref="D159:D161"/>
+    <mergeCell ref="E159:E161"/>
+    <mergeCell ref="F159:F161"/>
+    <mergeCell ref="D162:D163"/>
+    <mergeCell ref="E162:E163"/>
+    <mergeCell ref="F162:F163"/>
+    <mergeCell ref="D154:D155"/>
+    <mergeCell ref="E154:E155"/>
+    <mergeCell ref="F154:F155"/>
+    <mergeCell ref="D156:D158"/>
+    <mergeCell ref="E156:E158"/>
+    <mergeCell ref="F156:F158"/>
+    <mergeCell ref="D149:D150"/>
+    <mergeCell ref="E149:E150"/>
+    <mergeCell ref="F149:F150"/>
+    <mergeCell ref="D151:D153"/>
+    <mergeCell ref="E151:E153"/>
+    <mergeCell ref="F151:F153"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="E41:E43"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="G41:G43"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="D100:D102"/>
+    <mergeCell ref="D105:D106"/>
+    <mergeCell ref="D107:D108"/>
+    <mergeCell ref="D113:D115"/>
+    <mergeCell ref="D116:D117"/>
+    <mergeCell ref="F113:F115"/>
+    <mergeCell ref="D109:D110"/>
+    <mergeCell ref="D111:D112"/>
+    <mergeCell ref="F100:F102"/>
+    <mergeCell ref="E116:E117"/>
+    <mergeCell ref="F116:F117"/>
+    <mergeCell ref="E113:E115"/>
+    <mergeCell ref="F130:F131"/>
+    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="F134:F135"/>
+    <mergeCell ref="E138:E139"/>
+    <mergeCell ref="F136:F137"/>
+    <mergeCell ref="D136:D137"/>
+    <mergeCell ref="D138:D139"/>
+    <mergeCell ref="D118:D119"/>
+    <mergeCell ref="E124:E125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="E128:E129"/>
+    <mergeCell ref="E130:E131"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="E134:E135"/>
+    <mergeCell ref="E136:E137"/>
+    <mergeCell ref="F118:F119"/>
+    <mergeCell ref="E120:E123"/>
+    <mergeCell ref="F120:F123"/>
+    <mergeCell ref="F124:F125"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="F128:F129"/>
     <mergeCell ref="D140:D142"/>
     <mergeCell ref="E140:E142"/>
     <mergeCell ref="F140:F142"/>
@@ -15084,183 +15267,6 @@
     <mergeCell ref="D134:D135"/>
     <mergeCell ref="F138:F139"/>
     <mergeCell ref="E118:E119"/>
-    <mergeCell ref="F130:F131"/>
-    <mergeCell ref="F132:F133"/>
-    <mergeCell ref="F134:F135"/>
-    <mergeCell ref="E138:E139"/>
-    <mergeCell ref="F136:F137"/>
-    <mergeCell ref="D136:D137"/>
-    <mergeCell ref="D138:D139"/>
-    <mergeCell ref="D118:D119"/>
-    <mergeCell ref="E124:E125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="E128:E129"/>
-    <mergeCell ref="E130:E131"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="E134:E135"/>
-    <mergeCell ref="E136:E137"/>
-    <mergeCell ref="F118:F119"/>
-    <mergeCell ref="E120:E123"/>
-    <mergeCell ref="F120:F123"/>
-    <mergeCell ref="F124:F125"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="F128:F129"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="D100:D102"/>
-    <mergeCell ref="D105:D106"/>
-    <mergeCell ref="D107:D108"/>
-    <mergeCell ref="D113:D115"/>
-    <mergeCell ref="D116:D117"/>
-    <mergeCell ref="F113:F115"/>
-    <mergeCell ref="D109:D110"/>
-    <mergeCell ref="D111:D112"/>
-    <mergeCell ref="F100:F102"/>
-    <mergeCell ref="E116:E117"/>
-    <mergeCell ref="F116:F117"/>
-    <mergeCell ref="E113:E115"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="G41:G43"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="D154:D155"/>
-    <mergeCell ref="E154:E155"/>
-    <mergeCell ref="F154:F155"/>
-    <mergeCell ref="D156:D158"/>
-    <mergeCell ref="E156:E158"/>
-    <mergeCell ref="F156:F158"/>
-    <mergeCell ref="D149:D150"/>
-    <mergeCell ref="E149:E150"/>
-    <mergeCell ref="F149:F150"/>
-    <mergeCell ref="D151:D153"/>
-    <mergeCell ref="E151:E153"/>
-    <mergeCell ref="F151:F153"/>
-    <mergeCell ref="D164:D166"/>
-    <mergeCell ref="E164:E166"/>
-    <mergeCell ref="F164:F166"/>
-    <mergeCell ref="D167:D169"/>
-    <mergeCell ref="E167:E169"/>
-    <mergeCell ref="F167:F169"/>
-    <mergeCell ref="D159:D161"/>
-    <mergeCell ref="E159:E161"/>
-    <mergeCell ref="F159:F161"/>
-    <mergeCell ref="D162:D163"/>
-    <mergeCell ref="E162:E163"/>
-    <mergeCell ref="F162:F163"/>
-    <mergeCell ref="D174:D175"/>
-    <mergeCell ref="E174:E175"/>
-    <mergeCell ref="F174:F175"/>
-    <mergeCell ref="D176:D178"/>
-    <mergeCell ref="E176:E178"/>
-    <mergeCell ref="F176:F178"/>
-    <mergeCell ref="D170:D171"/>
-    <mergeCell ref="E170:E171"/>
-    <mergeCell ref="F170:F171"/>
-    <mergeCell ref="D172:D173"/>
-    <mergeCell ref="E172:E173"/>
-    <mergeCell ref="F172:F173"/>
-    <mergeCell ref="D195:D196"/>
-    <mergeCell ref="E195:E196"/>
-    <mergeCell ref="F195:F196"/>
-    <mergeCell ref="D179:D180"/>
-    <mergeCell ref="E179:E180"/>
-    <mergeCell ref="F179:F180"/>
-    <mergeCell ref="D181:D183"/>
-    <mergeCell ref="E181:E183"/>
-    <mergeCell ref="F181:F183"/>
-    <mergeCell ref="D188:D189"/>
-    <mergeCell ref="D190:D191"/>
-    <mergeCell ref="F188:F189"/>
-    <mergeCell ref="F190:F191"/>
-    <mergeCell ref="E188:E189"/>
-    <mergeCell ref="E190:E191"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="D146:D148"/>
-    <mergeCell ref="E146:E148"/>
-    <mergeCell ref="F146:F148"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="D103:D104"/>
-    <mergeCell ref="E103:E104"/>
-    <mergeCell ref="F103:F104"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -17897,6 +17903,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEAE28352B96D64C95AA0D5E2FA62FAD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed183881d36ac1b5d7d67982eda510d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d161086-4829-409f-9f75-5bde88dcb151" xmlns:ns3="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="685f4fda20cf913d28bf77c13cd653dd" ns2:_="" ns3:_="">
     <xsd:import namespace="3d161086-4829-409f-9f75-5bde88dcb151"/>
@@ -18119,17 +18136,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -18140,6 +18146,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C74AB5E7-5C87-4FF7-BF80-AB0EB6BD1D32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18158,23 +18181,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
V_MAP_TS_OBSERVATION, V_MAP_TONLY_OBSERVATION, V_MAP_SV_OBSERVATION, V_MAP_OMNI_AMBIENT_OBSERVATION, V_MAP_AQUA2081_LINE_OBSERVATION refactored to use V_MAP_FILTER_CRITERIA
</commit_message>
<xml_diff>
--- a/analysis/MEDS_Tables.xlsx
+++ b/analysis/MEDS_Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="760" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{A11D070D-D0AB-44ED-94E6-F6B9916FF713}"/>
+  <xr:revisionPtr revIDLastSave="798" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6603979-98E9-43BC-A141-30646C4DFF65}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3167" uniqueCount="754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3168" uniqueCount="755">
   <si>
     <t>Table</t>
   </si>
@@ -2602,6 +2602,9 @@
   </si>
   <si>
     <t>fleet weather oceanographic center</t>
+  </si>
+  <si>
+    <t>Not tested, data is SENSITIVE, and as not sent by Steve</t>
   </si>
 </sst>
 </file>
@@ -3339,7 +3342,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3469,9 +3472,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3481,14 +3481,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3497,39 +3503,45 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4026,14 +4038,15 @@
   <dimension ref="A1:X194"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E109" sqref="E109"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
     <col min="4" max="4" width="62.5703125" customWidth="1"/>
     <col min="5" max="5" width="19.85546875" customWidth="1"/>
     <col min="6" max="6" width="19.140625" customWidth="1"/>
@@ -12062,8 +12075,8 @@
   <dimension ref="A1:Q201"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E146" activeCellId="17" sqref="E100:E102 E103:E104 E105:E106 E107:E108 E109:E110 E111:E112 E118:E119 E120:E123 E124:E125 E126:E127 E128:E129 E130:E131 E132:E133 E134:E135 E136:E137 E140:E142 E143:E145 E146:E148"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12073,7 +12086,7 @@
     <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" style="38" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="72.42578125" style="67" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="72.42578125" style="65" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.140625" customWidth="1"/>
     <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
@@ -12097,13 +12110,13 @@
       <c r="G1" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="63" t="s">
+      <c r="H1" s="62" t="s">
         <v>15</v>
       </c>
       <c r="I1" s="43"/>
       <c r="J1" s="39">
         <f>F199/F198</f>
-        <v>0.23417721518987342</v>
+        <v>0.24203821656050956</v>
       </c>
       <c r="K1" s="44" t="s">
         <v>566</v>
@@ -12114,17 +12127,17 @@
       <c r="C2" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="72" t="s">
+      <c r="D2" s="71" t="s">
         <v>38</v>
       </c>
       <c r="E2" s="60"/>
-      <c r="F2" s="70" t="s">
+      <c r="F2" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="70" t="s">
+      <c r="G2" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="75" t="s">
         <v>564</v>
       </c>
     </row>
@@ -12132,11 +12145,11 @@
       <c r="C3" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="69"/>
+      <c r="D3" s="70"/>
       <c r="E3" s="57"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="73"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="77"/>
       <c r="L3" s="36"/>
       <c r="M3" s="36"/>
       <c r="N3" s="36"/>
@@ -12148,11 +12161,11 @@
       <c r="C4" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="69"/>
+      <c r="D4" s="70"/>
       <c r="E4" s="57"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="73"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="77"/>
       <c r="L4" s="36"/>
       <c r="M4" s="36"/>
       <c r="N4" s="36"/>
@@ -12164,28 +12177,28 @@
       <c r="C5" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="D5" s="70" t="s">
         <v>53</v>
       </c>
       <c r="E5" s="57"/>
-      <c r="F5" s="68" t="s">
+      <c r="F5" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="68" t="s">
+      <c r="G5" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="73" t="s">
+      <c r="H5" s="77" t="s">
         <v>519</v>
       </c>
       <c r="L5" s="36"/>
       <c r="M5" s="42" t="s">
         <v>464</v>
       </c>
-      <c r="N5" s="80" t="s">
+      <c r="N5" s="68" t="s">
         <v>465</v>
       </c>
-      <c r="O5" s="68"/>
-      <c r="P5" s="79" t="s">
+      <c r="O5" s="69"/>
+      <c r="P5" s="67" t="s">
         <v>581</v>
       </c>
       <c r="Q5" s="36"/>
@@ -12194,35 +12207,35 @@
       <c r="C6" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="69"/>
+      <c r="D6" s="70"/>
       <c r="E6" s="57"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="73"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="77"/>
       <c r="L6" s="36"/>
       <c r="M6" s="42" t="s">
         <v>467</v>
       </c>
-      <c r="N6" s="80"/>
-      <c r="O6" s="68"/>
-      <c r="P6" s="79"/>
+      <c r="N6" s="68"/>
+      <c r="O6" s="69"/>
+      <c r="P6" s="67"/>
       <c r="Q6" s="36"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C7" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="69" t="s">
+      <c r="D7" s="70" t="s">
         <v>78</v>
       </c>
       <c r="E7" s="57"/>
-      <c r="F7" s="68" t="s">
+      <c r="F7" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="G7" s="68" t="s">
+      <c r="G7" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="73" t="s">
+      <c r="H7" s="77" t="s">
         <v>80</v>
       </c>
       <c r="L7" s="36"/>
@@ -12236,11 +12249,11 @@
       <c r="C8" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="69"/>
+      <c r="D8" s="70"/>
       <c r="E8" s="57"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="73"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="77"/>
       <c r="L8" s="36"/>
       <c r="M8" s="36"/>
       <c r="N8" s="36"/>
@@ -12252,17 +12265,17 @@
       <c r="C9" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="D9" s="69" t="s">
+      <c r="D9" s="70" t="s">
         <v>171</v>
       </c>
       <c r="E9" s="57"/>
-      <c r="F9" s="68" t="s">
+      <c r="F9" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="G9" s="68" t="s">
+      <c r="G9" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="H9" s="73" t="s">
+      <c r="H9" s="77" t="s">
         <v>523</v>
       </c>
       <c r="K9" s="36"/>
@@ -12272,11 +12285,11 @@
       <c r="C10" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="D10" s="69"/>
+      <c r="D10" s="70"/>
       <c r="E10" s="57"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="73"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="77"/>
       <c r="K10" s="36"/>
       <c r="L10" s="36"/>
     </row>
@@ -12284,11 +12297,11 @@
       <c r="C11" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="D11" s="69"/>
+      <c r="D11" s="70"/>
       <c r="E11" s="57"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="68"/>
-      <c r="H11" s="73"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="77"/>
       <c r="K11" s="36"/>
       <c r="L11" s="36"/>
     </row>
@@ -12296,17 +12309,17 @@
       <c r="C12" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="D12" s="69" t="s">
+      <c r="D12" s="70" t="s">
         <v>204</v>
       </c>
       <c r="E12" s="57"/>
-      <c r="F12" s="68" t="s">
+      <c r="F12" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="G12" s="68" t="s">
+      <c r="G12" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="73" t="s">
+      <c r="H12" s="77" t="s">
         <v>515</v>
       </c>
       <c r="K12" s="36"/>
@@ -12316,11 +12329,11 @@
       <c r="C13" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="D13" s="69"/>
+      <c r="D13" s="70"/>
       <c r="E13" s="57"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="73"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="77"/>
       <c r="K13" s="36"/>
       <c r="L13" s="36"/>
     </row>
@@ -12328,17 +12341,17 @@
       <c r="C14" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="D14" s="69" t="s">
+      <c r="D14" s="70" t="s">
         <v>361</v>
       </c>
       <c r="E14" s="57"/>
-      <c r="F14" s="68" t="s">
+      <c r="F14" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="G14" s="68" t="s">
+      <c r="G14" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="73" t="s">
+      <c r="H14" s="77" t="s">
         <v>518</v>
       </c>
       <c r="K14" s="36"/>
@@ -12348,11 +12361,11 @@
       <c r="C15" s="35" t="s">
         <v>363</v>
       </c>
-      <c r="D15" s="75"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="77"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="76"/>
       <c r="K15" s="36"/>
       <c r="L15" s="36"/>
     </row>
@@ -12360,17 +12373,17 @@
       <c r="C16" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="72" t="s">
+      <c r="D16" s="71" t="s">
         <v>71</v>
       </c>
       <c r="E16" s="60"/>
-      <c r="F16" s="70" t="s">
+      <c r="F16" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="G16" s="70" t="s">
+      <c r="G16" s="73" t="s">
         <v>567</v>
       </c>
-      <c r="H16" s="74" t="s">
+      <c r="H16" s="75" t="s">
         <v>73</v>
       </c>
       <c r="K16" s="36"/>
@@ -12380,11 +12393,11 @@
       <c r="C17" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="69"/>
+      <c r="D17" s="70"/>
       <c r="E17" s="57"/>
-      <c r="F17" s="68"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="73"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="77"/>
       <c r="K17" s="36"/>
       <c r="L17" s="36"/>
     </row>
@@ -12392,17 +12405,17 @@
       <c r="C18" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="69" t="s">
+      <c r="D18" s="70" t="s">
         <v>105</v>
       </c>
       <c r="E18" s="57"/>
-      <c r="F18" s="68" t="s">
+      <c r="F18" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="G18" s="68" t="s">
+      <c r="G18" s="69" t="s">
         <v>567</v>
       </c>
-      <c r="H18" s="73" t="s">
+      <c r="H18" s="77" t="s">
         <v>524</v>
       </c>
       <c r="K18" s="36"/>
@@ -12412,11 +12425,11 @@
       <c r="C19" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="69"/>
+      <c r="D19" s="70"/>
       <c r="E19" s="57"/>
-      <c r="F19" s="68"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="73"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="77"/>
       <c r="K19" s="36"/>
       <c r="L19" s="36"/>
     </row>
@@ -12424,17 +12437,17 @@
       <c r="C20" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="D20" s="69" t="s">
+      <c r="D20" s="70" t="s">
         <v>300</v>
       </c>
       <c r="E20" s="57"/>
-      <c r="F20" s="68" t="s">
+      <c r="F20" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="G20" s="68" t="s">
+      <c r="G20" s="69" t="s">
         <v>567</v>
       </c>
-      <c r="H20" s="73" t="s">
+      <c r="H20" s="77" t="s">
         <v>516</v>
       </c>
       <c r="K20" s="36"/>
@@ -12444,11 +12457,11 @@
       <c r="C21" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="D21" s="69"/>
+      <c r="D21" s="70"/>
       <c r="E21" s="57"/>
-      <c r="F21" s="68"/>
-      <c r="G21" s="68"/>
-      <c r="H21" s="73"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="77"/>
       <c r="K21" s="36"/>
       <c r="L21" s="36"/>
     </row>
@@ -12456,17 +12469,17 @@
       <c r="C22" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="D22" s="69" t="s">
+      <c r="D22" s="70" t="s">
         <v>305</v>
       </c>
       <c r="E22" s="57"/>
-      <c r="F22" s="68" t="s">
+      <c r="F22" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="G22" s="68" t="s">
+      <c r="G22" s="69" t="s">
         <v>567</v>
       </c>
-      <c r="H22" s="73" t="s">
+      <c r="H22" s="77" t="s">
         <v>521</v>
       </c>
       <c r="K22" s="36"/>
@@ -12476,11 +12489,11 @@
       <c r="C23" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="D23" s="69"/>
+      <c r="D23" s="70"/>
       <c r="E23" s="57"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="73"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="77"/>
       <c r="K23" s="36"/>
       <c r="L23" s="36"/>
     </row>
@@ -12488,17 +12501,17 @@
       <c r="C24" s="34" t="s">
         <v>317</v>
       </c>
-      <c r="D24" s="69" t="s">
+      <c r="D24" s="70" t="s">
         <v>318</v>
       </c>
       <c r="E24" s="57"/>
-      <c r="F24" s="68" t="s">
+      <c r="F24" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="G24" s="68" t="s">
+      <c r="G24" s="69" t="s">
         <v>567</v>
       </c>
-      <c r="H24" s="73" t="s">
+      <c r="H24" s="77" t="s">
         <v>512</v>
       </c>
       <c r="K24" s="36"/>
@@ -12508,11 +12521,11 @@
       <c r="C25" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="D25" s="69"/>
+      <c r="D25" s="70"/>
       <c r="E25" s="57"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="73"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="77"/>
       <c r="K25" s="36"/>
       <c r="L25" s="36"/>
     </row>
@@ -12520,17 +12533,17 @@
       <c r="C26" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="D26" s="71" t="s">
+      <c r="D26" s="78" t="s">
         <v>323</v>
       </c>
       <c r="E26" s="59"/>
-      <c r="F26" s="78" t="s">
+      <c r="F26" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="G26" s="68" t="s">
+      <c r="G26" s="69" t="s">
         <v>567</v>
       </c>
-      <c r="H26" s="73" t="s">
+      <c r="H26" s="77" t="s">
         <v>517</v>
       </c>
       <c r="K26" s="36"/>
@@ -12540,27 +12553,27 @@
       <c r="C27" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="D27" s="71"/>
+      <c r="D27" s="78"/>
       <c r="E27" s="59"/>
-      <c r="F27" s="78"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="73"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="69"/>
+      <c r="H27" s="77"/>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C28" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="D28" s="69" t="s">
+      <c r="D28" s="70" t="s">
         <v>328</v>
       </c>
       <c r="E28" s="57"/>
-      <c r="F28" s="68" t="s">
+      <c r="F28" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="G28" s="68" t="s">
+      <c r="G28" s="69" t="s">
         <v>567</v>
       </c>
-      <c r="H28" s="73" t="s">
+      <c r="H28" s="77" t="s">
         <v>508</v>
       </c>
     </row>
@@ -12568,27 +12581,27 @@
       <c r="C29" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="D29" s="69"/>
+      <c r="D29" s="70"/>
       <c r="E29" s="57"/>
-      <c r="F29" s="68"/>
-      <c r="G29" s="68"/>
-      <c r="H29" s="73"/>
+      <c r="F29" s="69"/>
+      <c r="G29" s="69"/>
+      <c r="H29" s="77"/>
     </row>
     <row r="30" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C30" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="D30" s="69" t="s">
+      <c r="D30" s="70" t="s">
         <v>333</v>
       </c>
       <c r="E30" s="57"/>
-      <c r="F30" s="68" t="s">
+      <c r="F30" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="G30" s="68" t="s">
+      <c r="G30" s="69" t="s">
         <v>567</v>
       </c>
-      <c r="H30" s="73" t="s">
+      <c r="H30" s="77" t="s">
         <v>510</v>
       </c>
     </row>
@@ -12596,27 +12609,27 @@
       <c r="C31" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="D31" s="69"/>
+      <c r="D31" s="70"/>
       <c r="E31" s="57"/>
-      <c r="F31" s="68"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="73"/>
+      <c r="F31" s="69"/>
+      <c r="G31" s="69"/>
+      <c r="H31" s="77"/>
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C32" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="D32" s="69" t="s">
+      <c r="D32" s="70" t="s">
         <v>338</v>
       </c>
       <c r="E32" s="57"/>
-      <c r="F32" s="68" t="s">
+      <c r="F32" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="G32" s="68" t="s">
+      <c r="G32" s="69" t="s">
         <v>567</v>
       </c>
-      <c r="H32" s="73" t="s">
+      <c r="H32" s="77" t="s">
         <v>511</v>
       </c>
     </row>
@@ -12624,27 +12637,27 @@
       <c r="C33" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="D33" s="69"/>
+      <c r="D33" s="70"/>
       <c r="E33" s="57"/>
-      <c r="F33" s="68"/>
-      <c r="G33" s="68"/>
-      <c r="H33" s="73"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="69"/>
+      <c r="H33" s="77"/>
     </row>
     <row r="34" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C34" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="D34" s="69" t="s">
+      <c r="D34" s="70" t="s">
         <v>343</v>
       </c>
       <c r="E34" s="57"/>
-      <c r="F34" s="68" t="s">
+      <c r="F34" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="G34" s="68" t="s">
+      <c r="G34" s="69" t="s">
         <v>567</v>
       </c>
-      <c r="H34" s="73" t="s">
+      <c r="H34" s="77" t="s">
         <v>509</v>
       </c>
     </row>
@@ -12652,27 +12665,27 @@
       <c r="C35" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="D35" s="69"/>
+      <c r="D35" s="70"/>
       <c r="E35" s="57"/>
-      <c r="F35" s="68"/>
-      <c r="G35" s="68"/>
-      <c r="H35" s="73"/>
+      <c r="F35" s="69"/>
+      <c r="G35" s="69"/>
+      <c r="H35" s="77"/>
     </row>
     <row r="36" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C36" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="D36" s="69" t="s">
+      <c r="D36" s="70" t="s">
         <v>348</v>
       </c>
       <c r="E36" s="57"/>
-      <c r="F36" s="68" t="s">
+      <c r="F36" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="G36" s="68" t="s">
+      <c r="G36" s="69" t="s">
         <v>567</v>
       </c>
-      <c r="H36" s="73" t="s">
+      <c r="H36" s="77" t="s">
         <v>520</v>
       </c>
     </row>
@@ -12680,27 +12693,27 @@
       <c r="C37" s="35" t="s">
         <v>350</v>
       </c>
-      <c r="D37" s="75"/>
-      <c r="E37" s="62"/>
-      <c r="F37" s="76"/>
-      <c r="G37" s="76"/>
-      <c r="H37" s="77"/>
+      <c r="D37" s="72"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="74"/>
+      <c r="G37" s="74"/>
+      <c r="H37" s="76"/>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C38" s="33" t="s">
         <v>365</v>
       </c>
-      <c r="D38" s="72" t="s">
+      <c r="D38" s="71" t="s">
         <v>366</v>
       </c>
       <c r="E38" s="60"/>
-      <c r="F38" s="70" t="s">
+      <c r="F38" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="G38" s="70" t="s">
+      <c r="G38" s="73" t="s">
         <v>369</v>
       </c>
-      <c r="H38" s="74" t="s">
+      <c r="H38" s="75" t="s">
         <v>514</v>
       </c>
     </row>
@@ -12708,37 +12721,37 @@
       <c r="C39" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="D39" s="69"/>
+      <c r="D39" s="70"/>
       <c r="E39" s="57"/>
-      <c r="F39" s="68"/>
-      <c r="G39" s="68"/>
-      <c r="H39" s="73"/>
+      <c r="F39" s="69"/>
+      <c r="G39" s="69"/>
+      <c r="H39" s="77"/>
     </row>
     <row r="40" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C40" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="D40" s="69"/>
+      <c r="D40" s="70"/>
       <c r="E40" s="57"/>
-      <c r="F40" s="68"/>
-      <c r="G40" s="68"/>
-      <c r="H40" s="73"/>
+      <c r="F40" s="69"/>
+      <c r="G40" s="69"/>
+      <c r="H40" s="77"/>
     </row>
     <row r="41" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C41" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="D41" s="69" t="s">
+      <c r="D41" s="70" t="s">
         <v>371</v>
       </c>
       <c r="E41" s="57"/>
-      <c r="F41" s="68" t="s">
+      <c r="F41" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="G41" s="68" t="s">
+      <c r="G41" s="69" t="s">
         <v>369</v>
       </c>
-      <c r="H41" s="73" t="s">
+      <c r="H41" s="77" t="s">
         <v>513</v>
       </c>
     </row>
@@ -12746,37 +12759,37 @@
       <c r="C42" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="D42" s="69"/>
+      <c r="D42" s="70"/>
       <c r="E42" s="57"/>
-      <c r="F42" s="68"/>
-      <c r="G42" s="68"/>
-      <c r="H42" s="73"/>
+      <c r="F42" s="69"/>
+      <c r="G42" s="69"/>
+      <c r="H42" s="77"/>
     </row>
     <row r="43" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C43" s="34" t="s">
         <v>384</v>
       </c>
-      <c r="D43" s="69"/>
+      <c r="D43" s="70"/>
       <c r="E43" s="57"/>
-      <c r="F43" s="68"/>
-      <c r="G43" s="68"/>
-      <c r="H43" s="73"/>
+      <c r="F43" s="69"/>
+      <c r="G43" s="69"/>
+      <c r="H43" s="77"/>
     </row>
     <row r="44" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C44" s="34" t="s">
         <v>373</v>
       </c>
-      <c r="D44" s="69" t="s">
+      <c r="D44" s="70" t="s">
         <v>374</v>
       </c>
       <c r="E44" s="57"/>
-      <c r="F44" s="68" t="s">
+      <c r="F44" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="G44" s="68" t="s">
+      <c r="G44" s="69" t="s">
         <v>369</v>
       </c>
-      <c r="H44" s="73" t="s">
+      <c r="H44" s="77" t="s">
         <v>522</v>
       </c>
     </row>
@@ -12784,21 +12797,21 @@
       <c r="C45" s="34" t="s">
         <v>380</v>
       </c>
-      <c r="D45" s="69"/>
+      <c r="D45" s="70"/>
       <c r="E45" s="57"/>
-      <c r="F45" s="68"/>
-      <c r="G45" s="68"/>
-      <c r="H45" s="73"/>
+      <c r="F45" s="69"/>
+      <c r="G45" s="69"/>
+      <c r="H45" s="77"/>
     </row>
     <row r="46" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C46" s="34" t="s">
         <v>386</v>
       </c>
-      <c r="D46" s="69"/>
+      <c r="D46" s="70"/>
       <c r="E46" s="57"/>
-      <c r="F46" s="68"/>
-      <c r="G46" s="68"/>
-      <c r="H46" s="73"/>
+      <c r="F46" s="69"/>
+      <c r="G46" s="69"/>
+      <c r="H46" s="77"/>
       <c r="K46" s="36"/>
       <c r="L46" s="36"/>
       <c r="M46" s="36"/>
@@ -12808,15 +12821,15 @@
       <c r="C47" s="33" t="s">
         <v>464</v>
       </c>
-      <c r="D47" s="72" t="s">
+      <c r="D47" s="71" t="s">
         <v>465</v>
       </c>
       <c r="E47" s="60"/>
-      <c r="F47" s="70"/>
-      <c r="G47" s="70" t="s">
+      <c r="F47" s="73"/>
+      <c r="G47" s="73" t="s">
         <v>584</v>
       </c>
-      <c r="H47" s="74" t="s">
+      <c r="H47" s="75" t="s">
         <v>585</v>
       </c>
       <c r="K47" s="36"/>
@@ -12828,11 +12841,11 @@
       <c r="C48" s="35" t="s">
         <v>467</v>
       </c>
-      <c r="D48" s="75"/>
-      <c r="E48" s="62"/>
-      <c r="F48" s="76"/>
-      <c r="G48" s="76"/>
-      <c r="H48" s="77"/>
+      <c r="D48" s="72"/>
+      <c r="E48" s="61"/>
+      <c r="F48" s="74"/>
+      <c r="G48" s="74"/>
+      <c r="H48" s="76"/>
       <c r="K48" s="36"/>
       <c r="L48" s="36"/>
       <c r="M48" s="36"/>
@@ -12850,7 +12863,7 @@
       <c r="G49" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H49" s="61" t="s">
+      <c r="H49" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K49" s="36"/>
@@ -12864,12 +12877,14 @@
       </c>
       <c r="D50" s="51"/>
       <c r="E50" s="57"/>
-      <c r="F50" s="52"/>
+      <c r="F50" s="52" t="s">
+        <v>81</v>
+      </c>
       <c r="G50" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H50" s="61" t="s">
-        <v>33</v>
+      <c r="H50" s="66" t="s">
+        <v>754</v>
       </c>
       <c r="K50" s="36"/>
       <c r="L50" s="36"/>
@@ -12882,13 +12897,13 @@
       </c>
       <c r="D51" s="51"/>
       <c r="E51" s="57"/>
-      <c r="F51" s="52" t="s">
+      <c r="F51" s="84" t="s">
         <v>81</v>
       </c>
       <c r="G51" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H51" s="61" t="s">
+      <c r="H51" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K51" s="36"/>
@@ -12902,13 +12917,13 @@
       </c>
       <c r="D52" s="51"/>
       <c r="E52" s="57"/>
-      <c r="F52" s="52" t="s">
+      <c r="F52" s="84" t="s">
         <v>81</v>
       </c>
       <c r="G52" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H52" s="61" t="s">
+      <c r="H52" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K52" s="36"/>
@@ -12926,7 +12941,7 @@
       <c r="G53" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H53" s="61" t="s">
+      <c r="H53" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K53" s="36"/>
@@ -12940,13 +12955,13 @@
       </c>
       <c r="D54" s="51"/>
       <c r="E54" s="57"/>
-      <c r="F54" s="52" t="s">
+      <c r="F54" s="84" t="s">
         <v>81</v>
       </c>
       <c r="G54" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H54" s="61" t="s">
+      <c r="H54" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K54" s="36"/>
@@ -12966,7 +12981,7 @@
       <c r="G55" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H55" s="61" t="s">
+      <c r="H55" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K55" s="36"/>
@@ -12980,13 +12995,13 @@
       </c>
       <c r="D56" s="51"/>
       <c r="E56" s="57"/>
-      <c r="F56" s="52" t="s">
+      <c r="F56" s="84" t="s">
         <v>81</v>
       </c>
       <c r="G56" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H56" s="61" t="s">
+      <c r="H56" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K56" s="36"/>
@@ -13004,7 +13019,7 @@
       <c r="G57" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H57" s="61" t="s">
+      <c r="H57" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K57" s="36"/>
@@ -13022,7 +13037,7 @@
       <c r="G58" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H58" s="61" t="s">
+      <c r="H58" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K58" s="36"/>
@@ -13040,7 +13055,7 @@
       <c r="G59" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H59" s="61" t="s">
+      <c r="H59" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K59" s="36"/>
@@ -13058,7 +13073,7 @@
       <c r="G60" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H60" s="61" t="s">
+      <c r="H60" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K60" s="36"/>
@@ -13076,7 +13091,7 @@
       <c r="G61" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H61" s="61" t="s">
+      <c r="H61" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K61" s="36"/>
@@ -13090,13 +13105,13 @@
       </c>
       <c r="D62" s="51"/>
       <c r="E62" s="57"/>
-      <c r="F62" s="52" t="s">
+      <c r="F62" s="84" t="s">
         <v>81</v>
       </c>
       <c r="G62" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H62" s="61" t="s">
+      <c r="H62" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K62" s="36"/>
@@ -13114,7 +13129,7 @@
       <c r="G63" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H63" s="61" t="s">
+      <c r="H63" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K63" s="36"/>
@@ -13132,7 +13147,7 @@
       <c r="G64" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H64" s="61" t="s">
+      <c r="H64" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K64" s="36"/>
@@ -13150,7 +13165,7 @@
       <c r="G65" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H65" s="61" t="s">
+      <c r="H65" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K65" s="36"/>
@@ -13168,7 +13183,7 @@
       <c r="G66" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H66" s="61" t="s">
+      <c r="H66" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K66" s="36"/>
@@ -13186,7 +13201,7 @@
       <c r="G67" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H67" s="61" t="s">
+      <c r="H67" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K67" s="36"/>
@@ -13204,7 +13219,7 @@
       <c r="G68" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H68" s="61" t="s">
+      <c r="H68" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K68" s="36"/>
@@ -13222,7 +13237,7 @@
       <c r="G69" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H69" s="61" t="s">
+      <c r="H69" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K69" s="36"/>
@@ -13240,7 +13255,7 @@
       <c r="G70" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H70" s="61" t="s">
+      <c r="H70" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K70" s="36"/>
@@ -13258,7 +13273,7 @@
       <c r="G71" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H71" s="61" t="s">
+      <c r="H71" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K71" s="36"/>
@@ -13276,7 +13291,7 @@
       <c r="G72" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H72" s="61" t="s">
+      <c r="H72" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K72" s="36"/>
@@ -13294,7 +13309,7 @@
       <c r="G73" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H73" s="61" t="s">
+      <c r="H73" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K73" s="36"/>
@@ -13312,7 +13327,7 @@
       <c r="G74" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H74" s="61" t="s">
+      <c r="H74" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K74" s="36"/>
@@ -13330,7 +13345,7 @@
       <c r="G75" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H75" s="61" t="s">
+      <c r="H75" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K75" s="36"/>
@@ -13348,7 +13363,7 @@
       <c r="G76" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H76" s="61" t="s">
+      <c r="H76" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K76" s="36"/>
@@ -13362,13 +13377,13 @@
       </c>
       <c r="D77" s="51"/>
       <c r="E77" s="57"/>
-      <c r="F77" s="52" t="s">
+      <c r="F77" s="84" t="s">
         <v>81</v>
       </c>
       <c r="G77" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H77" s="61" t="s">
+      <c r="H77" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K77" s="36"/>
@@ -13386,7 +13401,7 @@
       <c r="G78" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H78" s="61" t="s">
+      <c r="H78" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K78" s="36"/>
@@ -13404,7 +13419,7 @@
       <c r="G79" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H79" s="61" t="s">
+      <c r="H79" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K79" s="36"/>
@@ -13422,7 +13437,7 @@
       <c r="G80" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H80" s="61" t="s">
+      <c r="H80" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K80" s="36"/>
@@ -13440,7 +13455,7 @@
       <c r="G81" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H81" s="61" t="s">
+      <c r="H81" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K81" s="36"/>
@@ -13454,13 +13469,13 @@
       </c>
       <c r="D82" s="51"/>
       <c r="E82" s="57"/>
-      <c r="F82" s="52" t="s">
+      <c r="F82" s="84" t="s">
         <v>81</v>
       </c>
       <c r="G82" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H82" s="61" t="s">
+      <c r="H82" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K82" s="36"/>
@@ -13474,13 +13489,13 @@
       </c>
       <c r="D83" s="51"/>
       <c r="E83" s="57"/>
-      <c r="F83" s="52" t="s">
+      <c r="F83" s="84" t="s">
         <v>81</v>
       </c>
       <c r="G83" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H83" s="61" t="s">
+      <c r="H83" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K83" s="36"/>
@@ -13494,13 +13509,13 @@
       </c>
       <c r="D84" s="51"/>
       <c r="E84" s="57"/>
-      <c r="F84" s="52" t="s">
+      <c r="F84" s="84" t="s">
         <v>81</v>
       </c>
       <c r="G84" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H84" s="61" t="s">
+      <c r="H84" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K84" s="36"/>
@@ -13518,7 +13533,7 @@
       <c r="G85" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H85" s="61" t="s">
+      <c r="H85" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K85" s="36"/>
@@ -13536,7 +13551,7 @@
       <c r="G86" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H86" s="61" t="s">
+      <c r="H86" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K86" s="36"/>
@@ -13554,7 +13569,7 @@
       <c r="G87" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H87" s="61" t="s">
+      <c r="H87" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K87" s="36"/>
@@ -13568,13 +13583,13 @@
       </c>
       <c r="D88" s="51"/>
       <c r="E88" s="57"/>
-      <c r="F88" s="52" t="s">
+      <c r="F88" s="84" t="s">
         <v>81</v>
       </c>
       <c r="G88" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H88" s="61" t="s">
+      <c r="H88" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K88" s="36"/>
@@ -13588,13 +13603,13 @@
       </c>
       <c r="D89" s="51"/>
       <c r="E89" s="57"/>
-      <c r="F89" s="52" t="s">
+      <c r="F89" s="84" t="s">
         <v>81</v>
       </c>
       <c r="G89" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H89" s="61" t="s">
+      <c r="H89" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K89" s="36"/>
@@ -13612,7 +13627,7 @@
       <c r="G90" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H90" s="61" t="s">
+      <c r="H90" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K90" s="36"/>
@@ -13630,7 +13645,7 @@
       <c r="G91" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H91" s="61" t="s">
+      <c r="H91" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K91" s="36"/>
@@ -13648,7 +13663,7 @@
       <c r="G92" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H92" s="61" t="s">
+      <c r="H92" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K92" s="36"/>
@@ -13662,13 +13677,13 @@
       </c>
       <c r="D93" s="51"/>
       <c r="E93" s="57"/>
-      <c r="F93" s="52" t="s">
+      <c r="F93" s="84" t="s">
         <v>81</v>
       </c>
       <c r="G93" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H93" s="61" t="s">
+      <c r="H93" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K93" s="36"/>
@@ -13686,7 +13701,7 @@
       <c r="G94" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H94" s="61" t="s">
+      <c r="H94" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K94" s="36"/>
@@ -13704,7 +13719,7 @@
       <c r="G95" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H95" s="61" t="s">
+      <c r="H95" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K95" s="36"/>
@@ -13718,13 +13733,13 @@
       </c>
       <c r="D96" s="51"/>
       <c r="E96" s="57"/>
-      <c r="F96" s="52" t="s">
+      <c r="F96" s="84" t="s">
         <v>81</v>
       </c>
       <c r="G96" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H96" s="61" t="s">
+      <c r="H96" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K96" s="36"/>
@@ -13738,13 +13753,13 @@
       </c>
       <c r="D97" s="51"/>
       <c r="E97" s="57"/>
-      <c r="F97" s="52" t="s">
+      <c r="F97" s="84" t="s">
         <v>81</v>
       </c>
       <c r="G97" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H97" s="61" t="s">
+      <c r="H97" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K97" s="36"/>
@@ -13758,13 +13773,13 @@
       </c>
       <c r="D98" s="51"/>
       <c r="E98" s="57"/>
-      <c r="F98" s="52" t="s">
+      <c r="F98" s="84" t="s">
         <v>81</v>
       </c>
       <c r="G98" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H98" s="61" t="s">
+      <c r="H98" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K98" s="36"/>
@@ -13782,7 +13797,7 @@
       <c r="G99" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="H99" s="61" t="s">
+      <c r="H99" s="81" t="s">
         <v>33</v>
       </c>
       <c r="K99" s="36"/>
@@ -13794,17 +13809,17 @@
       <c r="C100" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D100" s="72" t="s">
+      <c r="D100" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="E100" s="70">
+      <c r="E100" s="73">
         <v>1</v>
       </c>
-      <c r="F100" s="70"/>
-      <c r="G100" s="70" t="s">
+      <c r="F100" s="73"/>
+      <c r="G100" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="H100" s="64" t="s">
+      <c r="H100" s="63" t="s">
         <v>751</v>
       </c>
       <c r="K100" s="36"/>
@@ -13816,11 +13831,11 @@
       <c r="C101" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D101" s="69"/>
-      <c r="E101" s="68"/>
-      <c r="F101" s="68"/>
-      <c r="G101" s="68"/>
-      <c r="H101" s="45" t="s">
+      <c r="D101" s="70"/>
+      <c r="E101" s="69"/>
+      <c r="F101" s="69"/>
+      <c r="G101" s="69"/>
+      <c r="H101" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K101" s="36"/>
@@ -13832,11 +13847,11 @@
       <c r="C102" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D102" s="69"/>
-      <c r="E102" s="68"/>
-      <c r="F102" s="68"/>
-      <c r="G102" s="68"/>
-      <c r="H102" s="45" t="s">
+      <c r="D102" s="70"/>
+      <c r="E102" s="69"/>
+      <c r="F102" s="69"/>
+      <c r="G102" s="69"/>
+      <c r="H102" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K102" s="36"/>
@@ -13848,14 +13863,14 @@
       <c r="C103" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="D103" s="69" t="s">
+      <c r="D103" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="E103" s="68">
+      <c r="E103" s="69">
         <v>1</v>
       </c>
-      <c r="F103" s="68"/>
-      <c r="G103" s="68" t="s">
+      <c r="F103" s="69"/>
+      <c r="G103" s="69" t="s">
         <v>18</v>
       </c>
       <c r="H103" s="45" t="s">
@@ -13870,11 +13885,11 @@
       <c r="C104" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D104" s="69"/>
-      <c r="E104" s="68"/>
-      <c r="F104" s="68"/>
-      <c r="G104" s="68"/>
-      <c r="H104" s="45" t="s">
+      <c r="D104" s="70"/>
+      <c r="E104" s="69"/>
+      <c r="F104" s="69"/>
+      <c r="G104" s="69"/>
+      <c r="H104" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K104" s="36"/>
@@ -13886,17 +13901,17 @@
       <c r="C105" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D105" s="69" t="s">
+      <c r="D105" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="E105" s="68">
+      <c r="E105" s="69">
         <v>1</v>
       </c>
-      <c r="F105" s="68"/>
-      <c r="G105" s="68" t="s">
+      <c r="F105" s="69"/>
+      <c r="G105" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H105" s="45" t="s">
+      <c r="H105" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K105" s="36"/>
@@ -13908,11 +13923,11 @@
       <c r="C106" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D106" s="69"/>
-      <c r="E106" s="68"/>
-      <c r="F106" s="68"/>
-      <c r="G106" s="68"/>
-      <c r="H106" s="45" t="s">
+      <c r="D106" s="70"/>
+      <c r="E106" s="69"/>
+      <c r="F106" s="69"/>
+      <c r="G106" s="69"/>
+      <c r="H106" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K106" s="36"/>
@@ -13924,17 +13939,17 @@
       <c r="C107" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D107" s="69" t="s">
+      <c r="D107" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="E107" s="68">
+      <c r="E107" s="69">
         <v>1</v>
       </c>
-      <c r="F107" s="68"/>
-      <c r="G107" s="68" t="s">
+      <c r="F107" s="69"/>
+      <c r="G107" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H107" s="45" t="s">
+      <c r="H107" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K107" s="36"/>
@@ -13946,11 +13961,11 @@
       <c r="C108" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D108" s="69"/>
-      <c r="E108" s="68"/>
-      <c r="F108" s="68"/>
-      <c r="G108" s="68"/>
-      <c r="H108" s="45" t="s">
+      <c r="D108" s="70"/>
+      <c r="E108" s="69"/>
+      <c r="F108" s="69"/>
+      <c r="G108" s="69"/>
+      <c r="H108" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K108" s="36"/>
@@ -13962,17 +13977,17 @@
       <c r="C109" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="D109" s="69" t="s">
+      <c r="D109" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="E109" s="68">
+      <c r="E109" s="69">
         <v>1</v>
       </c>
-      <c r="F109" s="68"/>
-      <c r="G109" s="68" t="s">
+      <c r="F109" s="69"/>
+      <c r="G109" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H109" s="45" t="s">
+      <c r="H109" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K109" s="36"/>
@@ -13984,11 +13999,11 @@
       <c r="C110" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D110" s="69"/>
-      <c r="E110" s="68"/>
-      <c r="F110" s="68"/>
-      <c r="G110" s="68"/>
-      <c r="H110" s="45" t="s">
+      <c r="D110" s="70"/>
+      <c r="E110" s="69"/>
+      <c r="F110" s="69"/>
+      <c r="G110" s="69"/>
+      <c r="H110" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K110" s="36"/>
@@ -14000,17 +14015,17 @@
       <c r="C111" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D111" s="69" t="s">
+      <c r="D111" s="70" t="s">
         <v>105</v>
       </c>
-      <c r="E111" s="68">
+      <c r="E111" s="69">
         <v>1</v>
       </c>
-      <c r="F111" s="68"/>
-      <c r="G111" s="68" t="s">
+      <c r="F111" s="69"/>
+      <c r="G111" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H111" s="45" t="s">
+      <c r="H111" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K111" s="36"/>
@@ -14022,11 +14037,11 @@
       <c r="C112" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D112" s="69"/>
-      <c r="E112" s="68"/>
-      <c r="F112" s="68"/>
-      <c r="G112" s="68"/>
-      <c r="H112" s="45" t="s">
+      <c r="D112" s="70"/>
+      <c r="E112" s="69"/>
+      <c r="F112" s="69"/>
+      <c r="G112" s="69"/>
+      <c r="H112" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K112" s="36"/>
@@ -14038,17 +14053,17 @@
       <c r="C113" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="D113" s="69" t="s">
+      <c r="D113" s="70" t="s">
         <v>171</v>
       </c>
-      <c r="E113" s="68">
+      <c r="E113" s="69">
         <v>3</v>
       </c>
-      <c r="F113" s="68"/>
-      <c r="G113" s="68" t="s">
+      <c r="F113" s="69"/>
+      <c r="G113" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H113" s="45" t="s">
+      <c r="H113" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K113" s="36"/>
@@ -14060,11 +14075,11 @@
       <c r="C114" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="D114" s="69"/>
-      <c r="E114" s="68"/>
-      <c r="F114" s="68"/>
-      <c r="G114" s="68"/>
-      <c r="H114" s="45" t="s">
+      <c r="D114" s="70"/>
+      <c r="E114" s="69"/>
+      <c r="F114" s="69"/>
+      <c r="G114" s="69"/>
+      <c r="H114" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K114" s="36"/>
@@ -14076,11 +14091,11 @@
       <c r="C115" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="D115" s="69"/>
-      <c r="E115" s="68"/>
-      <c r="F115" s="68"/>
-      <c r="G115" s="68"/>
-      <c r="H115" s="45" t="s">
+      <c r="D115" s="70"/>
+      <c r="E115" s="69"/>
+      <c r="F115" s="69"/>
+      <c r="G115" s="69"/>
+      <c r="H115" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K115" s="36"/>
@@ -14092,17 +14107,17 @@
       <c r="C116" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="D116" s="69" t="s">
+      <c r="D116" s="70" t="s">
         <v>204</v>
       </c>
-      <c r="E116" s="68">
+      <c r="E116" s="69">
         <v>3</v>
       </c>
-      <c r="F116" s="68"/>
-      <c r="G116" s="68" t="s">
+      <c r="F116" s="69"/>
+      <c r="G116" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H116" s="45" t="s">
+      <c r="H116" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K116" s="36"/>
@@ -14114,11 +14129,11 @@
       <c r="C117" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="D117" s="69"/>
-      <c r="E117" s="68"/>
-      <c r="F117" s="68"/>
-      <c r="G117" s="68"/>
-      <c r="H117" s="45" t="s">
+      <c r="D117" s="70"/>
+      <c r="E117" s="69"/>
+      <c r="F117" s="69"/>
+      <c r="G117" s="69"/>
+      <c r="H117" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K117" s="36"/>
@@ -14130,17 +14145,17 @@
       <c r="C118" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="D118" s="69" t="s">
+      <c r="D118" s="70" t="s">
         <v>300</v>
       </c>
-      <c r="E118" s="68">
+      <c r="E118" s="69">
         <v>1</v>
       </c>
-      <c r="F118" s="68"/>
-      <c r="G118" s="68" t="s">
+      <c r="F118" s="69"/>
+      <c r="G118" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H118" s="45" t="s">
+      <c r="H118" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K118" s="36"/>
@@ -14152,11 +14167,11 @@
       <c r="C119" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="D119" s="69"/>
-      <c r="E119" s="68"/>
-      <c r="F119" s="68"/>
-      <c r="G119" s="68"/>
-      <c r="H119" s="45" t="s">
+      <c r="D119" s="70"/>
+      <c r="E119" s="69"/>
+      <c r="F119" s="69"/>
+      <c r="G119" s="69"/>
+      <c r="H119" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K119" s="36"/>
@@ -14168,17 +14183,17 @@
       <c r="C120" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="D120" s="69" t="s">
+      <c r="D120" s="70" t="s">
         <v>305</v>
       </c>
-      <c r="E120" s="68">
+      <c r="E120" s="69">
         <v>1</v>
       </c>
-      <c r="F120" s="68"/>
-      <c r="G120" s="68" t="s">
+      <c r="F120" s="69"/>
+      <c r="G120" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H120" s="45" t="s">
+      <c r="H120" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K120" s="36"/>
@@ -14190,11 +14205,11 @@
       <c r="C121" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="D121" s="69"/>
-      <c r="E121" s="68"/>
-      <c r="F121" s="68"/>
-      <c r="G121" s="68"/>
-      <c r="H121" s="45" t="s">
+      <c r="D121" s="70"/>
+      <c r="E121" s="69"/>
+      <c r="F121" s="69"/>
+      <c r="G121" s="69"/>
+      <c r="H121" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K121" s="36"/>
@@ -14206,11 +14221,11 @@
       <c r="C122" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="D122" s="69"/>
-      <c r="E122" s="68"/>
-      <c r="F122" s="68"/>
-      <c r="G122" s="68"/>
-      <c r="H122" s="45" t="s">
+      <c r="D122" s="70"/>
+      <c r="E122" s="69"/>
+      <c r="F122" s="69"/>
+      <c r="G122" s="69"/>
+      <c r="H122" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K122" s="36"/>
@@ -14222,11 +14237,11 @@
       <c r="C123" s="34" t="s">
         <v>311</v>
       </c>
-      <c r="D123" s="69"/>
-      <c r="E123" s="68"/>
-      <c r="F123" s="68"/>
-      <c r="G123" s="68"/>
-      <c r="H123" s="45" t="s">
+      <c r="D123" s="70"/>
+      <c r="E123" s="69"/>
+      <c r="F123" s="69"/>
+      <c r="G123" s="69"/>
+      <c r="H123" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K123" s="36"/>
@@ -14238,17 +14253,17 @@
       <c r="C124" s="34" t="s">
         <v>317</v>
       </c>
-      <c r="D124" s="69" t="s">
+      <c r="D124" s="70" t="s">
         <v>318</v>
       </c>
-      <c r="E124" s="68">
+      <c r="E124" s="69">
         <v>1</v>
       </c>
-      <c r="F124" s="68"/>
-      <c r="G124" s="68" t="s">
+      <c r="F124" s="69"/>
+      <c r="G124" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H124" s="45" t="s">
+      <c r="H124" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K124" s="36"/>
@@ -14260,11 +14275,11 @@
       <c r="C125" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="D125" s="69"/>
-      <c r="E125" s="68"/>
-      <c r="F125" s="68"/>
-      <c r="G125" s="68"/>
-      <c r="H125" s="45" t="s">
+      <c r="D125" s="70"/>
+      <c r="E125" s="69"/>
+      <c r="F125" s="69"/>
+      <c r="G125" s="69"/>
+      <c r="H125" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K125" s="36"/>
@@ -14276,17 +14291,17 @@
       <c r="C126" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="D126" s="71" t="s">
+      <c r="D126" s="78" t="s">
         <v>323</v>
       </c>
-      <c r="E126" s="68">
+      <c r="E126" s="69">
         <v>1</v>
       </c>
-      <c r="F126" s="68"/>
-      <c r="G126" s="68" t="s">
+      <c r="F126" s="69"/>
+      <c r="G126" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H126" s="45" t="s">
+      <c r="H126" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K126" s="36"/>
@@ -14298,11 +14313,11 @@
       <c r="C127" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="D127" s="71"/>
-      <c r="E127" s="68"/>
-      <c r="F127" s="68"/>
-      <c r="G127" s="68"/>
-      <c r="H127" s="45" t="s">
+      <c r="D127" s="78"/>
+      <c r="E127" s="69"/>
+      <c r="F127" s="69"/>
+      <c r="G127" s="69"/>
+      <c r="H127" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14310,17 +14325,17 @@
       <c r="C128" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="D128" s="69" t="s">
+      <c r="D128" s="70" t="s">
         <v>328</v>
       </c>
-      <c r="E128" s="68">
+      <c r="E128" s="69">
         <v>1</v>
       </c>
-      <c r="F128" s="68"/>
-      <c r="G128" s="68" t="s">
+      <c r="F128" s="69"/>
+      <c r="G128" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H128" s="45" t="s">
+      <c r="H128" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14328,11 +14343,11 @@
       <c r="C129" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="D129" s="69"/>
-      <c r="E129" s="68"/>
-      <c r="F129" s="68"/>
-      <c r="G129" s="68"/>
-      <c r="H129" s="45" t="s">
+      <c r="D129" s="70"/>
+      <c r="E129" s="69"/>
+      <c r="F129" s="69"/>
+      <c r="G129" s="69"/>
+      <c r="H129" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14340,17 +14355,17 @@
       <c r="C130" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="D130" s="69" t="s">
+      <c r="D130" s="70" t="s">
         <v>333</v>
       </c>
-      <c r="E130" s="68">
+      <c r="E130" s="69">
         <v>1</v>
       </c>
-      <c r="F130" s="68"/>
-      <c r="G130" s="68" t="s">
+      <c r="F130" s="69"/>
+      <c r="G130" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H130" s="45" t="s">
+      <c r="H130" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14358,11 +14373,11 @@
       <c r="C131" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="D131" s="69"/>
-      <c r="E131" s="68"/>
-      <c r="F131" s="68"/>
-      <c r="G131" s="68"/>
-      <c r="H131" s="45" t="s">
+      <c r="D131" s="70"/>
+      <c r="E131" s="69"/>
+      <c r="F131" s="69"/>
+      <c r="G131" s="69"/>
+      <c r="H131" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14370,17 +14385,17 @@
       <c r="C132" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="D132" s="69" t="s">
+      <c r="D132" s="70" t="s">
         <v>338</v>
       </c>
-      <c r="E132" s="68">
+      <c r="E132" s="69">
         <v>1</v>
       </c>
-      <c r="F132" s="68"/>
-      <c r="G132" s="68" t="s">
+      <c r="F132" s="69"/>
+      <c r="G132" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H132" s="45" t="s">
+      <c r="H132" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14388,11 +14403,11 @@
       <c r="C133" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="D133" s="69"/>
-      <c r="E133" s="68"/>
-      <c r="F133" s="68"/>
-      <c r="G133" s="68"/>
-      <c r="H133" s="45" t="s">
+      <c r="D133" s="70"/>
+      <c r="E133" s="69"/>
+      <c r="F133" s="69"/>
+      <c r="G133" s="69"/>
+      <c r="H133" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14400,17 +14415,17 @@
       <c r="C134" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="D134" s="69" t="s">
+      <c r="D134" s="70" t="s">
         <v>343</v>
       </c>
-      <c r="E134" s="68">
+      <c r="E134" s="69">
         <v>1</v>
       </c>
-      <c r="F134" s="68"/>
-      <c r="G134" s="68" t="s">
+      <c r="F134" s="69"/>
+      <c r="G134" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H134" s="45" t="s">
+      <c r="H134" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14418,11 +14433,11 @@
       <c r="C135" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="D135" s="69"/>
-      <c r="E135" s="68"/>
-      <c r="F135" s="68"/>
-      <c r="G135" s="68"/>
-      <c r="H135" s="45" t="s">
+      <c r="D135" s="70"/>
+      <c r="E135" s="69"/>
+      <c r="F135" s="69"/>
+      <c r="G135" s="69"/>
+      <c r="H135" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14430,17 +14445,17 @@
       <c r="C136" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="D136" s="69" t="s">
+      <c r="D136" s="70" t="s">
         <v>348</v>
       </c>
-      <c r="E136" s="68">
+      <c r="E136" s="69">
         <v>1</v>
       </c>
-      <c r="F136" s="68"/>
-      <c r="G136" s="68" t="s">
+      <c r="F136" s="69"/>
+      <c r="G136" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H136" s="45" t="s">
+      <c r="H136" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14448,11 +14463,11 @@
       <c r="C137" s="34" t="s">
         <v>350</v>
       </c>
-      <c r="D137" s="69"/>
-      <c r="E137" s="68"/>
-      <c r="F137" s="68"/>
-      <c r="G137" s="68"/>
-      <c r="H137" s="45" t="s">
+      <c r="D137" s="70"/>
+      <c r="E137" s="69"/>
+      <c r="F137" s="69"/>
+      <c r="G137" s="69"/>
+      <c r="H137" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14460,17 +14475,17 @@
       <c r="C138" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="D138" s="69" t="s">
+      <c r="D138" s="70" t="s">
         <v>361</v>
       </c>
-      <c r="E138" s="68">
+      <c r="E138" s="69">
         <v>2</v>
       </c>
-      <c r="F138" s="68"/>
-      <c r="G138" s="68" t="s">
+      <c r="F138" s="69"/>
+      <c r="G138" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H138" s="45" t="s">
+      <c r="H138" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14478,11 +14493,11 @@
       <c r="C139" s="34" t="s">
         <v>363</v>
       </c>
-      <c r="D139" s="69"/>
-      <c r="E139" s="68"/>
-      <c r="F139" s="68"/>
-      <c r="G139" s="68"/>
-      <c r="H139" s="45" t="s">
+      <c r="D139" s="70"/>
+      <c r="E139" s="69"/>
+      <c r="F139" s="69"/>
+      <c r="G139" s="69"/>
+      <c r="H139" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14490,17 +14505,17 @@
       <c r="C140" s="34" t="s">
         <v>365</v>
       </c>
-      <c r="D140" s="69" t="s">
+      <c r="D140" s="70" t="s">
         <v>366</v>
       </c>
-      <c r="E140" s="68">
+      <c r="E140" s="69">
         <v>1</v>
       </c>
-      <c r="F140" s="68"/>
-      <c r="G140" s="68" t="s">
+      <c r="F140" s="69"/>
+      <c r="G140" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H140" s="45" t="s">
+      <c r="H140" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14508,11 +14523,11 @@
       <c r="C141" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="D141" s="69"/>
-      <c r="E141" s="68"/>
-      <c r="F141" s="68"/>
-      <c r="G141" s="68"/>
-      <c r="H141" s="45" t="s">
+      <c r="D141" s="70"/>
+      <c r="E141" s="69"/>
+      <c r="F141" s="69"/>
+      <c r="G141" s="69"/>
+      <c r="H141" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14520,11 +14535,11 @@
       <c r="C142" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="D142" s="69"/>
-      <c r="E142" s="68"/>
-      <c r="F142" s="68"/>
-      <c r="G142" s="68"/>
-      <c r="H142" s="45" t="s">
+      <c r="D142" s="70"/>
+      <c r="E142" s="69"/>
+      <c r="F142" s="69"/>
+      <c r="G142" s="69"/>
+      <c r="H142" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14532,17 +14547,17 @@
       <c r="C143" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="D143" s="69" t="s">
+      <c r="D143" s="70" t="s">
         <v>371</v>
       </c>
-      <c r="E143" s="68">
+      <c r="E143" s="69">
         <v>1</v>
       </c>
-      <c r="F143" s="68"/>
-      <c r="G143" s="68" t="s">
+      <c r="F143" s="69"/>
+      <c r="G143" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H143" s="45" t="s">
+      <c r="H143" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14550,11 +14565,11 @@
       <c r="C144" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="D144" s="69"/>
-      <c r="E144" s="68"/>
-      <c r="F144" s="68"/>
-      <c r="G144" s="68"/>
-      <c r="H144" s="45" t="s">
+      <c r="D144" s="70"/>
+      <c r="E144" s="69"/>
+      <c r="F144" s="69"/>
+      <c r="G144" s="69"/>
+      <c r="H144" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14562,11 +14577,11 @@
       <c r="C145" s="34" t="s">
         <v>384</v>
       </c>
-      <c r="D145" s="69"/>
-      <c r="E145" s="68"/>
-      <c r="F145" s="68"/>
-      <c r="G145" s="68"/>
-      <c r="H145" s="45" t="s">
+      <c r="D145" s="70"/>
+      <c r="E145" s="69"/>
+      <c r="F145" s="69"/>
+      <c r="G145" s="69"/>
+      <c r="H145" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14575,17 +14590,17 @@
       <c r="C146" s="34" t="s">
         <v>373</v>
       </c>
-      <c r="D146" s="69" t="s">
+      <c r="D146" s="70" t="s">
         <v>374</v>
       </c>
-      <c r="E146" s="68">
+      <c r="E146" s="69">
         <v>1</v>
       </c>
-      <c r="F146" s="68"/>
-      <c r="G146" s="68" t="s">
+      <c r="F146" s="69"/>
+      <c r="G146" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H146" s="45" t="s">
+      <c r="H146" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14594,11 +14609,11 @@
       <c r="C147" s="34" t="s">
         <v>380</v>
       </c>
-      <c r="D147" s="69"/>
-      <c r="E147" s="68"/>
-      <c r="F147" s="68"/>
-      <c r="G147" s="68"/>
-      <c r="H147" s="45" t="s">
+      <c r="D147" s="70"/>
+      <c r="E147" s="69"/>
+      <c r="F147" s="69"/>
+      <c r="G147" s="69"/>
+      <c r="H147" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14607,11 +14622,11 @@
       <c r="C148" s="34" t="s">
         <v>386</v>
       </c>
-      <c r="D148" s="69"/>
-      <c r="E148" s="68"/>
-      <c r="F148" s="68"/>
-      <c r="G148" s="68"/>
-      <c r="H148" s="45" t="s">
+      <c r="D148" s="70"/>
+      <c r="E148" s="69"/>
+      <c r="F148" s="69"/>
+      <c r="G148" s="69"/>
+      <c r="H148" s="82" t="s">
         <v>33</v>
       </c>
       <c r="K148" s="36"/>
@@ -14623,17 +14638,17 @@
       <c r="C149" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="D149" s="69" t="s">
+      <c r="D149" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="E149" s="68">
+      <c r="E149" s="69">
         <v>4</v>
       </c>
-      <c r="F149" s="68"/>
-      <c r="G149" s="68" t="s">
+      <c r="F149" s="69"/>
+      <c r="G149" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H149" s="45" t="s">
+      <c r="H149" s="82" t="s">
         <v>33</v>
       </c>
       <c r="J149" s="36"/>
@@ -14642,11 +14657,11 @@
       <c r="C150" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="D150" s="69"/>
-      <c r="E150" s="68"/>
-      <c r="F150" s="68"/>
-      <c r="G150" s="68"/>
-      <c r="H150" s="45" t="s">
+      <c r="D150" s="70"/>
+      <c r="E150" s="69"/>
+      <c r="F150" s="69"/>
+      <c r="G150" s="69"/>
+      <c r="H150" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14654,17 +14669,17 @@
       <c r="C151" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="D151" s="69" t="s">
+      <c r="D151" s="70" t="s">
         <v>110</v>
       </c>
-      <c r="E151" s="68">
+      <c r="E151" s="69">
         <v>3</v>
       </c>
-      <c r="F151" s="68"/>
-      <c r="G151" s="68" t="s">
+      <c r="F151" s="69"/>
+      <c r="G151" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H151" s="45" t="s">
+      <c r="H151" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14672,11 +14687,11 @@
       <c r="C152" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="D152" s="69"/>
-      <c r="E152" s="68"/>
-      <c r="F152" s="68"/>
-      <c r="G152" s="68"/>
-      <c r="H152" s="45" t="s">
+      <c r="D152" s="70"/>
+      <c r="E152" s="69"/>
+      <c r="F152" s="69"/>
+      <c r="G152" s="69"/>
+      <c r="H152" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14684,11 +14699,11 @@
       <c r="C153" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="D153" s="69"/>
-      <c r="E153" s="68"/>
-      <c r="F153" s="68"/>
-      <c r="G153" s="68"/>
-      <c r="H153" s="45" t="s">
+      <c r="D153" s="70"/>
+      <c r="E153" s="69"/>
+      <c r="F153" s="69"/>
+      <c r="G153" s="69"/>
+      <c r="H153" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14696,17 +14711,17 @@
       <c r="C154" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="D154" s="69" t="s">
+      <c r="D154" s="70" t="s">
         <v>119</v>
       </c>
-      <c r="E154" s="68">
+      <c r="E154" s="69">
         <v>3</v>
       </c>
-      <c r="F154" s="68"/>
-      <c r="G154" s="68" t="s">
+      <c r="F154" s="69"/>
+      <c r="G154" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H154" s="45" t="s">
+      <c r="H154" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14714,11 +14729,11 @@
       <c r="C155" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="D155" s="69"/>
-      <c r="E155" s="68"/>
-      <c r="F155" s="68"/>
-      <c r="G155" s="68"/>
-      <c r="H155" s="45" t="s">
+      <c r="D155" s="70"/>
+      <c r="E155" s="69"/>
+      <c r="F155" s="69"/>
+      <c r="G155" s="69"/>
+      <c r="H155" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14726,17 +14741,17 @@
       <c r="C156" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="D156" s="69" t="s">
+      <c r="D156" s="70" t="s">
         <v>124</v>
       </c>
-      <c r="E156" s="68">
+      <c r="E156" s="69">
         <v>3</v>
       </c>
-      <c r="F156" s="68"/>
-      <c r="G156" s="68" t="s">
+      <c r="F156" s="69"/>
+      <c r="G156" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H156" s="45" t="s">
+      <c r="H156" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14744,11 +14759,11 @@
       <c r="C157" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="D157" s="69"/>
-      <c r="E157" s="68"/>
-      <c r="F157" s="68"/>
-      <c r="G157" s="68"/>
-      <c r="H157" s="45" t="s">
+      <c r="D157" s="70"/>
+      <c r="E157" s="69"/>
+      <c r="F157" s="69"/>
+      <c r="G157" s="69"/>
+      <c r="H157" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14756,11 +14771,11 @@
       <c r="C158" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="D158" s="69"/>
-      <c r="E158" s="68"/>
-      <c r="F158" s="68"/>
-      <c r="G158" s="68"/>
-      <c r="H158" s="45" t="s">
+      <c r="D158" s="70"/>
+      <c r="E158" s="69"/>
+      <c r="F158" s="69"/>
+      <c r="G158" s="69"/>
+      <c r="H158" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14768,17 +14783,17 @@
       <c r="C159" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="D159" s="69" t="s">
+      <c r="D159" s="70" t="s">
         <v>131</v>
       </c>
-      <c r="E159" s="68">
+      <c r="E159" s="69">
         <v>3</v>
       </c>
-      <c r="F159" s="68"/>
-      <c r="G159" s="68" t="s">
+      <c r="F159" s="69"/>
+      <c r="G159" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H159" s="45" t="s">
+      <c r="H159" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14786,11 +14801,11 @@
       <c r="C160" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="D160" s="69"/>
-      <c r="E160" s="68"/>
-      <c r="F160" s="68"/>
-      <c r="G160" s="68"/>
-      <c r="H160" s="45" t="s">
+      <c r="D160" s="70"/>
+      <c r="E160" s="69"/>
+      <c r="F160" s="69"/>
+      <c r="G160" s="69"/>
+      <c r="H160" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14798,11 +14813,11 @@
       <c r="C161" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="D161" s="69"/>
-      <c r="E161" s="68"/>
-      <c r="F161" s="68"/>
-      <c r="G161" s="68"/>
-      <c r="H161" s="45" t="s">
+      <c r="D161" s="70"/>
+      <c r="E161" s="69"/>
+      <c r="F161" s="69"/>
+      <c r="G161" s="69"/>
+      <c r="H161" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14810,14 +14825,14 @@
       <c r="C162" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="D162" s="69" t="s">
+      <c r="D162" s="70" t="s">
         <v>159</v>
       </c>
-      <c r="E162" s="68">
+      <c r="E162" s="69">
         <v>5</v>
       </c>
-      <c r="F162" s="68"/>
-      <c r="G162" s="68" t="s">
+      <c r="F162" s="69"/>
+      <c r="G162" s="69" t="s">
         <v>18</v>
       </c>
       <c r="H162" s="45" t="s">
@@ -14828,11 +14843,11 @@
       <c r="C163" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="D163" s="69"/>
-      <c r="E163" s="68"/>
-      <c r="F163" s="68"/>
-      <c r="G163" s="68"/>
-      <c r="H163" s="45" t="s">
+      <c r="D163" s="70"/>
+      <c r="E163" s="69"/>
+      <c r="F163" s="69"/>
+      <c r="G163" s="69"/>
+      <c r="H163" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14840,17 +14855,17 @@
       <c r="C164" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="D164" s="69" t="s">
+      <c r="D164" s="70" t="s">
         <v>164</v>
       </c>
-      <c r="E164" s="68">
+      <c r="E164" s="69">
         <v>5</v>
       </c>
-      <c r="F164" s="68"/>
-      <c r="G164" s="68" t="s">
+      <c r="F164" s="69"/>
+      <c r="G164" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H164" s="45" t="s">
+      <c r="H164" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14858,11 +14873,11 @@
       <c r="C165" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="D165" s="69"/>
-      <c r="E165" s="68"/>
-      <c r="F165" s="68"/>
-      <c r="G165" s="68"/>
-      <c r="H165" s="45" t="s">
+      <c r="D165" s="70"/>
+      <c r="E165" s="69"/>
+      <c r="F165" s="69"/>
+      <c r="G165" s="69"/>
+      <c r="H165" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14870,11 +14885,11 @@
       <c r="C166" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="D166" s="69"/>
-      <c r="E166" s="68"/>
-      <c r="F166" s="68"/>
-      <c r="G166" s="68"/>
-      <c r="H166" s="45" t="s">
+      <c r="D166" s="70"/>
+      <c r="E166" s="69"/>
+      <c r="F166" s="69"/>
+      <c r="G166" s="69"/>
+      <c r="H166" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14882,17 +14897,17 @@
       <c r="C167" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="D167" s="69" t="s">
+      <c r="D167" s="70" t="s">
         <v>179</v>
       </c>
-      <c r="E167" s="68">
+      <c r="E167" s="69">
         <v>5</v>
       </c>
-      <c r="F167" s="68"/>
-      <c r="G167" s="68" t="s">
+      <c r="F167" s="69"/>
+      <c r="G167" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H167" s="45" t="s">
+      <c r="H167" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14900,11 +14915,11 @@
       <c r="C168" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="D168" s="69"/>
-      <c r="E168" s="68"/>
-      <c r="F168" s="68"/>
-      <c r="G168" s="68"/>
-      <c r="H168" s="45" t="s">
+      <c r="D168" s="70"/>
+      <c r="E168" s="69"/>
+      <c r="F168" s="69"/>
+      <c r="G168" s="69"/>
+      <c r="H168" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14912,11 +14927,11 @@
       <c r="C169" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="D169" s="69"/>
-      <c r="E169" s="68"/>
-      <c r="F169" s="68"/>
-      <c r="G169" s="68"/>
-      <c r="H169" s="45" t="s">
+      <c r="D169" s="70"/>
+      <c r="E169" s="69"/>
+      <c r="F169" s="69"/>
+      <c r="G169" s="69"/>
+      <c r="H169" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14924,17 +14939,17 @@
       <c r="C170" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="D170" s="69" t="s">
+      <c r="D170" s="70" t="s">
         <v>186</v>
       </c>
-      <c r="E170" s="68">
+      <c r="E170" s="69">
         <v>5</v>
       </c>
-      <c r="F170" s="68"/>
-      <c r="G170" s="68" t="s">
+      <c r="F170" s="69"/>
+      <c r="G170" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H170" s="45" t="s">
+      <c r="H170" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14942,11 +14957,11 @@
       <c r="C171" s="34" t="s">
         <v>188</v>
       </c>
-      <c r="D171" s="69"/>
-      <c r="E171" s="68"/>
-      <c r="F171" s="68"/>
-      <c r="G171" s="68"/>
-      <c r="H171" s="45" t="s">
+      <c r="D171" s="70"/>
+      <c r="E171" s="69"/>
+      <c r="F171" s="69"/>
+      <c r="G171" s="69"/>
+      <c r="H171" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14954,17 +14969,17 @@
       <c r="C172" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="D172" s="69" t="s">
+      <c r="D172" s="70" t="s">
         <v>195</v>
       </c>
-      <c r="E172" s="68">
+      <c r="E172" s="69">
         <v>5</v>
       </c>
-      <c r="F172" s="68"/>
-      <c r="G172" s="68" t="s">
+      <c r="F172" s="69"/>
+      <c r="G172" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H172" s="45" t="s">
+      <c r="H172" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14972,11 +14987,11 @@
       <c r="C173" s="34" t="s">
         <v>197</v>
       </c>
-      <c r="D173" s="69"/>
-      <c r="E173" s="68"/>
-      <c r="F173" s="68"/>
-      <c r="G173" s="68"/>
-      <c r="H173" s="45" t="s">
+      <c r="D173" s="70"/>
+      <c r="E173" s="69"/>
+      <c r="F173" s="69"/>
+      <c r="G173" s="69"/>
+      <c r="H173" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14984,17 +14999,17 @@
       <c r="C174" s="34" t="s">
         <v>199</v>
       </c>
-      <c r="D174" s="69" t="s">
+      <c r="D174" s="70" t="s">
         <v>200</v>
       </c>
-      <c r="E174" s="68">
+      <c r="E174" s="69">
         <v>5</v>
       </c>
-      <c r="F174" s="68"/>
-      <c r="G174" s="68" t="s">
+      <c r="F174" s="69"/>
+      <c r="G174" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H174" s="45" t="s">
+      <c r="H174" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -15002,11 +15017,11 @@
       <c r="C175" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="D175" s="69"/>
-      <c r="E175" s="68"/>
-      <c r="F175" s="68"/>
-      <c r="G175" s="68"/>
-      <c r="H175" s="45" t="s">
+      <c r="D175" s="70"/>
+      <c r="E175" s="69"/>
+      <c r="F175" s="69"/>
+      <c r="G175" s="69"/>
+      <c r="H175" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -15014,17 +15029,17 @@
       <c r="C176" s="34" t="s">
         <v>210</v>
       </c>
-      <c r="D176" s="69" t="s">
+      <c r="D176" s="70" t="s">
         <v>211</v>
       </c>
-      <c r="E176" s="68">
+      <c r="E176" s="69">
         <v>5</v>
       </c>
-      <c r="F176" s="68"/>
-      <c r="G176" s="68" t="s">
+      <c r="F176" s="69"/>
+      <c r="G176" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H176" s="45" t="s">
+      <c r="H176" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -15032,11 +15047,11 @@
       <c r="C177" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="D177" s="69"/>
-      <c r="E177" s="68"/>
-      <c r="F177" s="68"/>
-      <c r="G177" s="68"/>
-      <c r="H177" s="45" t="s">
+      <c r="D177" s="70"/>
+      <c r="E177" s="69"/>
+      <c r="F177" s="69"/>
+      <c r="G177" s="69"/>
+      <c r="H177" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -15044,11 +15059,11 @@
       <c r="C178" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="D178" s="69"/>
-      <c r="E178" s="68"/>
-      <c r="F178" s="68"/>
-      <c r="G178" s="68"/>
-      <c r="H178" s="45" t="s">
+      <c r="D178" s="70"/>
+      <c r="E178" s="69"/>
+      <c r="F178" s="69"/>
+      <c r="G178" s="69"/>
+      <c r="H178" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -15056,17 +15071,17 @@
       <c r="C179" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="D179" s="69" t="s">
+      <c r="D179" s="70" t="s">
         <v>223</v>
       </c>
-      <c r="E179" s="68">
+      <c r="E179" s="69">
         <v>5</v>
       </c>
-      <c r="F179" s="68"/>
-      <c r="G179" s="68" t="s">
+      <c r="F179" s="69"/>
+      <c r="G179" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H179" s="45" t="s">
+      <c r="H179" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -15074,11 +15089,11 @@
       <c r="C180" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="D180" s="69"/>
-      <c r="E180" s="68"/>
-      <c r="F180" s="68"/>
-      <c r="G180" s="68"/>
-      <c r="H180" s="45" t="s">
+      <c r="D180" s="70"/>
+      <c r="E180" s="69"/>
+      <c r="F180" s="69"/>
+      <c r="G180" s="69"/>
+      <c r="H180" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -15086,17 +15101,17 @@
       <c r="C181" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="D181" s="69" t="s">
+      <c r="D181" s="70" t="s">
         <v>228</v>
       </c>
-      <c r="E181" s="68">
+      <c r="E181" s="69">
         <v>5</v>
       </c>
-      <c r="F181" s="68"/>
-      <c r="G181" s="68" t="s">
+      <c r="F181" s="69"/>
+      <c r="G181" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H181" s="45" t="s">
+      <c r="H181" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -15104,11 +15119,11 @@
       <c r="C182" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="D182" s="69"/>
-      <c r="E182" s="68"/>
-      <c r="F182" s="68"/>
-      <c r="G182" s="68"/>
-      <c r="H182" s="45" t="s">
+      <c r="D182" s="70"/>
+      <c r="E182" s="69"/>
+      <c r="F182" s="69"/>
+      <c r="G182" s="69"/>
+      <c r="H182" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -15116,11 +15131,11 @@
       <c r="C183" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="D183" s="69"/>
-      <c r="E183" s="68"/>
-      <c r="F183" s="68"/>
-      <c r="G183" s="68"/>
-      <c r="H183" s="45" t="s">
+      <c r="D183" s="70"/>
+      <c r="E183" s="69"/>
+      <c r="F183" s="69"/>
+      <c r="G183" s="69"/>
+      <c r="H183" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -15138,7 +15153,7 @@
       <c r="G184" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="H184" s="45" t="s">
+      <c r="H184" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -15156,7 +15171,7 @@
       <c r="G185" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="H185" s="45" t="s">
+      <c r="H185" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -15174,7 +15189,7 @@
       <c r="G186" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="H186" s="45" t="s">
+      <c r="H186" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -15192,7 +15207,7 @@
       <c r="G187" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="H187" s="45" t="s">
+      <c r="H187" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -15200,17 +15215,17 @@
       <c r="C188" s="34" t="s">
         <v>454</v>
       </c>
-      <c r="D188" s="69" t="s">
+      <c r="D188" s="70" t="s">
         <v>582</v>
       </c>
-      <c r="E188" s="68">
+      <c r="E188" s="69">
         <v>3</v>
       </c>
-      <c r="F188" s="68"/>
-      <c r="G188" s="68" t="s">
+      <c r="F188" s="69"/>
+      <c r="G188" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H188" s="45" t="s">
+      <c r="H188" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -15218,11 +15233,11 @@
       <c r="C189" s="34" t="s">
         <v>457</v>
       </c>
-      <c r="D189" s="69"/>
-      <c r="E189" s="68"/>
-      <c r="F189" s="68"/>
-      <c r="G189" s="68"/>
-      <c r="H189" s="45" t="s">
+      <c r="D189" s="70"/>
+      <c r="E189" s="69"/>
+      <c r="F189" s="69"/>
+      <c r="G189" s="69"/>
+      <c r="H189" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -15230,17 +15245,17 @@
       <c r="C190" s="34" t="s">
         <v>459</v>
       </c>
-      <c r="D190" s="69" t="s">
+      <c r="D190" s="70" t="s">
         <v>460</v>
       </c>
-      <c r="E190" s="68">
+      <c r="E190" s="69">
         <v>3</v>
       </c>
-      <c r="F190" s="68"/>
-      <c r="G190" s="68" t="s">
+      <c r="F190" s="69"/>
+      <c r="G190" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H190" s="45" t="s">
+      <c r="H190" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -15248,11 +15263,11 @@
       <c r="C191" s="34" t="s">
         <v>462</v>
       </c>
-      <c r="D191" s="69"/>
-      <c r="E191" s="68"/>
-      <c r="F191" s="68"/>
-      <c r="G191" s="68"/>
-      <c r="H191" s="45" t="s">
+      <c r="D191" s="70"/>
+      <c r="E191" s="69"/>
+      <c r="F191" s="69"/>
+      <c r="G191" s="69"/>
+      <c r="H191" s="82" t="s">
         <v>33</v>
       </c>
     </row>
@@ -15316,17 +15331,17 @@
       <c r="C195" s="34" t="s">
         <v>477</v>
       </c>
-      <c r="D195" s="69" t="s">
+      <c r="D195" s="70" t="s">
         <v>478</v>
       </c>
-      <c r="E195" s="68">
+      <c r="E195" s="69">
         <v>5</v>
       </c>
-      <c r="F195" s="68"/>
-      <c r="G195" s="68" t="s">
+      <c r="F195" s="69"/>
+      <c r="G195" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H195" s="45" t="s">
+      <c r="H195" s="82" t="s">
         <v>33</v>
       </c>
       <c r="I195" s="36"/>
@@ -15337,11 +15352,11 @@
       <c r="C196" s="35" t="s">
         <v>480</v>
       </c>
-      <c r="D196" s="75"/>
-      <c r="E196" s="76"/>
-      <c r="F196" s="76"/>
-      <c r="G196" s="76"/>
-      <c r="H196" s="65" t="s">
+      <c r="D196" s="72"/>
+      <c r="E196" s="74"/>
+      <c r="F196" s="74"/>
+      <c r="G196" s="74"/>
+      <c r="H196" s="83" t="s">
         <v>33</v>
       </c>
       <c r="I196" s="36"/>
@@ -15354,7 +15369,7 @@
       <c r="E197" s="36"/>
       <c r="F197" s="40"/>
       <c r="G197" s="41"/>
-      <c r="H197" s="66"/>
+      <c r="H197" s="64"/>
       <c r="I197" s="36"/>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.25">
@@ -15365,10 +15380,10 @@
       <c r="E198" s="36"/>
       <c r="F198" s="40">
         <f>COUNTBLANK(F2:F196)</f>
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G198" s="41"/>
-      <c r="H198" s="66"/>
+      <c r="H198" s="64"/>
       <c r="I198" s="36"/>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
@@ -15379,10 +15394,10 @@
       <c r="E199" s="36"/>
       <c r="F199" s="40">
         <f>COUNTA(F2:F196)</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G199" s="41"/>
-      <c r="H199" s="66"/>
+      <c r="H199" s="64"/>
       <c r="I199" s="36"/>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
@@ -15393,7 +15408,7 @@
       <c r="E200" s="36"/>
       <c r="F200" s="40"/>
       <c r="G200" s="41"/>
-      <c r="H200" s="66"/>
+      <c r="H200" s="64"/>
       <c r="I200" s="36"/>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
@@ -15404,12 +15419,227 @@
       <c r="E201" s="36"/>
       <c r="F201" s="40"/>
       <c r="G201" s="41"/>
-      <c r="H201" s="66"/>
+      <c r="H201" s="64"/>
       <c r="I201" s="36"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q1" xr:uid="{20647E0C-146B-49B2-BC4C-D733C2BD2881}"/>
   <mergeCells count="239">
+    <mergeCell ref="E146:E148"/>
+    <mergeCell ref="E149:E150"/>
+    <mergeCell ref="E151:E153"/>
+    <mergeCell ref="E154:E155"/>
+    <mergeCell ref="E156:E158"/>
+    <mergeCell ref="E159:E161"/>
+    <mergeCell ref="E162:E163"/>
+    <mergeCell ref="E164:E166"/>
+    <mergeCell ref="E167:E169"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="E128:E129"/>
+    <mergeCell ref="E130:E131"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="E134:E135"/>
+    <mergeCell ref="E136:E137"/>
+    <mergeCell ref="E138:E139"/>
+    <mergeCell ref="E140:E142"/>
+    <mergeCell ref="E143:E145"/>
+    <mergeCell ref="D140:D142"/>
+    <mergeCell ref="F140:F142"/>
+    <mergeCell ref="G140:G142"/>
+    <mergeCell ref="D143:D145"/>
+    <mergeCell ref="F143:F145"/>
+    <mergeCell ref="G143:G145"/>
+    <mergeCell ref="F100:F102"/>
+    <mergeCell ref="F105:F106"/>
+    <mergeCell ref="G105:G106"/>
+    <mergeCell ref="F107:F108"/>
+    <mergeCell ref="G107:G108"/>
+    <mergeCell ref="F109:F110"/>
+    <mergeCell ref="G109:G110"/>
+    <mergeCell ref="F111:F112"/>
+    <mergeCell ref="G111:G112"/>
+    <mergeCell ref="D120:D123"/>
+    <mergeCell ref="D124:D125"/>
+    <mergeCell ref="D126:D127"/>
+    <mergeCell ref="D128:D129"/>
+    <mergeCell ref="D130:D131"/>
+    <mergeCell ref="D132:D133"/>
+    <mergeCell ref="D134:D135"/>
+    <mergeCell ref="G138:G139"/>
+    <mergeCell ref="F118:F119"/>
+    <mergeCell ref="G130:G131"/>
+    <mergeCell ref="G132:G133"/>
+    <mergeCell ref="G134:G135"/>
+    <mergeCell ref="F138:F139"/>
+    <mergeCell ref="G136:G137"/>
+    <mergeCell ref="D136:D137"/>
+    <mergeCell ref="D138:D139"/>
+    <mergeCell ref="D118:D119"/>
+    <mergeCell ref="F124:F125"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="F128:F129"/>
+    <mergeCell ref="F130:F131"/>
+    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="F134:F135"/>
+    <mergeCell ref="F136:F137"/>
+    <mergeCell ref="G118:G119"/>
+    <mergeCell ref="F120:F123"/>
+    <mergeCell ref="G120:G123"/>
+    <mergeCell ref="G124:G125"/>
+    <mergeCell ref="G126:G127"/>
+    <mergeCell ref="G128:G129"/>
+    <mergeCell ref="E118:E119"/>
+    <mergeCell ref="E120:E123"/>
+    <mergeCell ref="E124:E125"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="D100:D102"/>
+    <mergeCell ref="D105:D106"/>
+    <mergeCell ref="D107:D108"/>
+    <mergeCell ref="D113:D115"/>
+    <mergeCell ref="D116:D117"/>
+    <mergeCell ref="G113:G115"/>
+    <mergeCell ref="D109:D110"/>
+    <mergeCell ref="D111:D112"/>
+    <mergeCell ref="G100:G102"/>
+    <mergeCell ref="F116:F117"/>
+    <mergeCell ref="G116:G117"/>
+    <mergeCell ref="F113:F115"/>
+    <mergeCell ref="E100:E102"/>
+    <mergeCell ref="E103:E104"/>
+    <mergeCell ref="E105:E106"/>
+    <mergeCell ref="E107:E108"/>
+    <mergeCell ref="E109:E110"/>
+    <mergeCell ref="E111:E112"/>
+    <mergeCell ref="E113:E115"/>
+    <mergeCell ref="E116:E117"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="G41:G43"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="D154:D155"/>
+    <mergeCell ref="F154:F155"/>
+    <mergeCell ref="G154:G155"/>
+    <mergeCell ref="D156:D158"/>
+    <mergeCell ref="F156:F158"/>
+    <mergeCell ref="G156:G158"/>
+    <mergeCell ref="D149:D150"/>
+    <mergeCell ref="F149:F150"/>
+    <mergeCell ref="G149:G150"/>
+    <mergeCell ref="D151:D153"/>
+    <mergeCell ref="F151:F153"/>
+    <mergeCell ref="G151:G153"/>
+    <mergeCell ref="D164:D166"/>
+    <mergeCell ref="F164:F166"/>
+    <mergeCell ref="G164:G166"/>
+    <mergeCell ref="D167:D169"/>
+    <mergeCell ref="F167:F169"/>
+    <mergeCell ref="G167:G169"/>
+    <mergeCell ref="D159:D161"/>
+    <mergeCell ref="F159:F161"/>
+    <mergeCell ref="G159:G161"/>
+    <mergeCell ref="D162:D163"/>
+    <mergeCell ref="F162:F163"/>
+    <mergeCell ref="G162:G163"/>
+    <mergeCell ref="D174:D175"/>
+    <mergeCell ref="F174:F175"/>
+    <mergeCell ref="G174:G175"/>
+    <mergeCell ref="D176:D178"/>
+    <mergeCell ref="F176:F178"/>
+    <mergeCell ref="G176:G178"/>
+    <mergeCell ref="D170:D171"/>
+    <mergeCell ref="F170:F171"/>
+    <mergeCell ref="G170:G171"/>
+    <mergeCell ref="D172:D173"/>
+    <mergeCell ref="F172:F173"/>
+    <mergeCell ref="G172:G173"/>
+    <mergeCell ref="E170:E171"/>
+    <mergeCell ref="E172:E173"/>
+    <mergeCell ref="E174:E175"/>
+    <mergeCell ref="E176:E178"/>
+    <mergeCell ref="D195:D196"/>
+    <mergeCell ref="F195:F196"/>
+    <mergeCell ref="G195:G196"/>
+    <mergeCell ref="D179:D180"/>
+    <mergeCell ref="F179:F180"/>
+    <mergeCell ref="G179:G180"/>
+    <mergeCell ref="D181:D183"/>
+    <mergeCell ref="F181:F183"/>
+    <mergeCell ref="G181:G183"/>
+    <mergeCell ref="D188:D189"/>
+    <mergeCell ref="D190:D191"/>
+    <mergeCell ref="G188:G189"/>
+    <mergeCell ref="G190:G191"/>
+    <mergeCell ref="F188:F189"/>
+    <mergeCell ref="F190:F191"/>
+    <mergeCell ref="E179:E180"/>
+    <mergeCell ref="E181:E183"/>
+    <mergeCell ref="E188:E189"/>
+    <mergeCell ref="E190:E191"/>
+    <mergeCell ref="E195:E196"/>
     <mergeCell ref="P5:P6"/>
     <mergeCell ref="N5:N6"/>
     <mergeCell ref="O5:O6"/>
@@ -15434,221 +15664,6 @@
     <mergeCell ref="D34:D35"/>
     <mergeCell ref="F34:F35"/>
     <mergeCell ref="G34:G35"/>
-    <mergeCell ref="D195:D196"/>
-    <mergeCell ref="F195:F196"/>
-    <mergeCell ref="G195:G196"/>
-    <mergeCell ref="D179:D180"/>
-    <mergeCell ref="F179:F180"/>
-    <mergeCell ref="G179:G180"/>
-    <mergeCell ref="D181:D183"/>
-    <mergeCell ref="F181:F183"/>
-    <mergeCell ref="G181:G183"/>
-    <mergeCell ref="D188:D189"/>
-    <mergeCell ref="D190:D191"/>
-    <mergeCell ref="G188:G189"/>
-    <mergeCell ref="G190:G191"/>
-    <mergeCell ref="F188:F189"/>
-    <mergeCell ref="F190:F191"/>
-    <mergeCell ref="E179:E180"/>
-    <mergeCell ref="E181:E183"/>
-    <mergeCell ref="E188:E189"/>
-    <mergeCell ref="E190:E191"/>
-    <mergeCell ref="E195:E196"/>
-    <mergeCell ref="D174:D175"/>
-    <mergeCell ref="F174:F175"/>
-    <mergeCell ref="G174:G175"/>
-    <mergeCell ref="D176:D178"/>
-    <mergeCell ref="F176:F178"/>
-    <mergeCell ref="G176:G178"/>
-    <mergeCell ref="D170:D171"/>
-    <mergeCell ref="F170:F171"/>
-    <mergeCell ref="G170:G171"/>
-    <mergeCell ref="D172:D173"/>
-    <mergeCell ref="F172:F173"/>
-    <mergeCell ref="G172:G173"/>
-    <mergeCell ref="E170:E171"/>
-    <mergeCell ref="E172:E173"/>
-    <mergeCell ref="E174:E175"/>
-    <mergeCell ref="E176:E178"/>
-    <mergeCell ref="D164:D166"/>
-    <mergeCell ref="F164:F166"/>
-    <mergeCell ref="G164:G166"/>
-    <mergeCell ref="D167:D169"/>
-    <mergeCell ref="F167:F169"/>
-    <mergeCell ref="G167:G169"/>
-    <mergeCell ref="D159:D161"/>
-    <mergeCell ref="F159:F161"/>
-    <mergeCell ref="G159:G161"/>
-    <mergeCell ref="D162:D163"/>
-    <mergeCell ref="F162:F163"/>
-    <mergeCell ref="G162:G163"/>
-    <mergeCell ref="D154:D155"/>
-    <mergeCell ref="F154:F155"/>
-    <mergeCell ref="G154:G155"/>
-    <mergeCell ref="D156:D158"/>
-    <mergeCell ref="F156:F158"/>
-    <mergeCell ref="G156:G158"/>
-    <mergeCell ref="D149:D150"/>
-    <mergeCell ref="F149:F150"/>
-    <mergeCell ref="G149:G150"/>
-    <mergeCell ref="D151:D153"/>
-    <mergeCell ref="F151:F153"/>
-    <mergeCell ref="G151:G153"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="G41:G43"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="D100:D102"/>
-    <mergeCell ref="D105:D106"/>
-    <mergeCell ref="D107:D108"/>
-    <mergeCell ref="D113:D115"/>
-    <mergeCell ref="D116:D117"/>
-    <mergeCell ref="G113:G115"/>
-    <mergeCell ref="D109:D110"/>
-    <mergeCell ref="D111:D112"/>
-    <mergeCell ref="G100:G102"/>
-    <mergeCell ref="F116:F117"/>
-    <mergeCell ref="G116:G117"/>
-    <mergeCell ref="F113:F115"/>
-    <mergeCell ref="E100:E102"/>
-    <mergeCell ref="E103:E104"/>
-    <mergeCell ref="E105:E106"/>
-    <mergeCell ref="E107:E108"/>
-    <mergeCell ref="E109:E110"/>
-    <mergeCell ref="E111:E112"/>
-    <mergeCell ref="E113:E115"/>
-    <mergeCell ref="E116:E117"/>
-    <mergeCell ref="G130:G131"/>
-    <mergeCell ref="G132:G133"/>
-    <mergeCell ref="G134:G135"/>
-    <mergeCell ref="F138:F139"/>
-    <mergeCell ref="G136:G137"/>
-    <mergeCell ref="D136:D137"/>
-    <mergeCell ref="D138:D139"/>
-    <mergeCell ref="D118:D119"/>
-    <mergeCell ref="F124:F125"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="F128:F129"/>
-    <mergeCell ref="F130:F131"/>
-    <mergeCell ref="F132:F133"/>
-    <mergeCell ref="F134:F135"/>
-    <mergeCell ref="F136:F137"/>
-    <mergeCell ref="G118:G119"/>
-    <mergeCell ref="F120:F123"/>
-    <mergeCell ref="G120:G123"/>
-    <mergeCell ref="G124:G125"/>
-    <mergeCell ref="G126:G127"/>
-    <mergeCell ref="G128:G129"/>
-    <mergeCell ref="E118:E119"/>
-    <mergeCell ref="E120:E123"/>
-    <mergeCell ref="E124:E125"/>
-    <mergeCell ref="D140:D142"/>
-    <mergeCell ref="F140:F142"/>
-    <mergeCell ref="G140:G142"/>
-    <mergeCell ref="D143:D145"/>
-    <mergeCell ref="F143:F145"/>
-    <mergeCell ref="G143:G145"/>
-    <mergeCell ref="F100:F102"/>
-    <mergeCell ref="F105:F106"/>
-    <mergeCell ref="G105:G106"/>
-    <mergeCell ref="F107:F108"/>
-    <mergeCell ref="G107:G108"/>
-    <mergeCell ref="F109:F110"/>
-    <mergeCell ref="G109:G110"/>
-    <mergeCell ref="F111:F112"/>
-    <mergeCell ref="G111:G112"/>
-    <mergeCell ref="D120:D123"/>
-    <mergeCell ref="D124:D125"/>
-    <mergeCell ref="D126:D127"/>
-    <mergeCell ref="D128:D129"/>
-    <mergeCell ref="D130:D131"/>
-    <mergeCell ref="D132:D133"/>
-    <mergeCell ref="D134:D135"/>
-    <mergeCell ref="G138:G139"/>
-    <mergeCell ref="F118:F119"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="E128:E129"/>
-    <mergeCell ref="E130:E131"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="E134:E135"/>
-    <mergeCell ref="E136:E137"/>
-    <mergeCell ref="E138:E139"/>
-    <mergeCell ref="E140:E142"/>
-    <mergeCell ref="E143:E145"/>
-    <mergeCell ref="E146:E148"/>
-    <mergeCell ref="E149:E150"/>
-    <mergeCell ref="E151:E153"/>
-    <mergeCell ref="E154:E155"/>
-    <mergeCell ref="E156:E158"/>
-    <mergeCell ref="E159:E161"/>
-    <mergeCell ref="E162:E163"/>
-    <mergeCell ref="E164:E166"/>
-    <mergeCell ref="E167:E169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -17389,7 +17404,7 @@
       <c r="D2" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="81">
+      <c r="E2" s="80">
         <v>101332</v>
       </c>
     </row>
@@ -17406,7 +17421,7 @@
       <c r="D3" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="81"/>
+      <c r="E3" s="80"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -17421,7 +17436,7 @@
       <c r="D4" t="s">
         <v>524</v>
       </c>
-      <c r="E4" s="81">
+      <c r="E4" s="80">
         <v>99343</v>
       </c>
     </row>
@@ -17438,7 +17453,7 @@
       <c r="D5" t="s">
         <v>524</v>
       </c>
-      <c r="E5" s="81"/>
+      <c r="E5" s="80"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -17453,7 +17468,7 @@
       <c r="D6" t="s">
         <v>516</v>
       </c>
-      <c r="E6" s="81">
+      <c r="E6" s="80">
         <v>102453</v>
       </c>
     </row>
@@ -17470,7 +17485,7 @@
       <c r="D7" t="s">
         <v>516</v>
       </c>
-      <c r="E7" s="81"/>
+      <c r="E7" s="80"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -17485,7 +17500,7 @@
       <c r="D8" t="s">
         <v>521</v>
       </c>
-      <c r="E8" s="81">
+      <c r="E8" s="80">
         <v>102447</v>
       </c>
     </row>
@@ -17502,7 +17517,7 @@
       <c r="D9" t="s">
         <v>521</v>
       </c>
-      <c r="E9" s="81"/>
+      <c r="E9" s="80"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -17517,7 +17532,7 @@
       <c r="D10" t="s">
         <v>521</v>
       </c>
-      <c r="E10" s="81"/>
+      <c r="E10" s="80"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -17532,7 +17547,7 @@
       <c r="D11" t="s">
         <v>521</v>
       </c>
-      <c r="E11" s="81"/>
+      <c r="E11" s="80"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -17547,7 +17562,7 @@
       <c r="D12" t="s">
         <v>512</v>
       </c>
-      <c r="E12" s="81">
+      <c r="E12" s="80">
         <v>101221</v>
       </c>
     </row>
@@ -17564,7 +17579,7 @@
       <c r="D13" t="s">
         <v>512</v>
       </c>
-      <c r="E13" s="81"/>
+      <c r="E13" s="80"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -17579,7 +17594,7 @@
       <c r="D14" t="s">
         <v>517</v>
       </c>
-      <c r="E14" s="81">
+      <c r="E14" s="80">
         <v>102455</v>
       </c>
     </row>
@@ -17596,7 +17611,7 @@
       <c r="D15" t="s">
         <v>517</v>
       </c>
-      <c r="E15" s="81"/>
+      <c r="E15" s="80"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -17611,7 +17626,7 @@
       <c r="D16" t="s">
         <v>508</v>
       </c>
-      <c r="E16" s="81">
+      <c r="E16" s="80">
         <v>1013824</v>
       </c>
     </row>
@@ -17628,7 +17643,7 @@
       <c r="D17" t="s">
         <v>508</v>
       </c>
-      <c r="E17" s="81"/>
+      <c r="E17" s="80"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -17643,7 +17658,7 @@
       <c r="D18" t="s">
         <v>510</v>
       </c>
-      <c r="E18" s="81">
+      <c r="E18" s="80">
         <v>102445</v>
       </c>
     </row>
@@ -17660,7 +17675,7 @@
       <c r="D19" t="s">
         <v>510</v>
       </c>
-      <c r="E19" s="81"/>
+      <c r="E19" s="80"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -17675,7 +17690,7 @@
       <c r="D20" t="s">
         <v>511</v>
       </c>
-      <c r="E20" s="81">
+      <c r="E20" s="80">
         <v>101557</v>
       </c>
     </row>
@@ -17692,7 +17707,7 @@
       <c r="D21" t="s">
         <v>511</v>
       </c>
-      <c r="E21" s="81"/>
+      <c r="E21" s="80"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -17707,7 +17722,7 @@
       <c r="D22" t="s">
         <v>509</v>
       </c>
-      <c r="E22" s="81">
+      <c r="E22" s="80">
         <v>101339</v>
       </c>
     </row>
@@ -17724,7 +17739,7 @@
       <c r="D23" t="s">
         <v>509</v>
       </c>
-      <c r="E23" s="81"/>
+      <c r="E23" s="80"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -17739,7 +17754,7 @@
       <c r="D24" t="s">
         <v>520</v>
       </c>
-      <c r="E24" s="81">
+      <c r="E24" s="80">
         <v>102391</v>
       </c>
     </row>
@@ -17756,7 +17771,7 @@
       <c r="D25" t="s">
         <v>520</v>
       </c>
-      <c r="E25" s="81"/>
+      <c r="E25" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -18285,15 +18300,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
@@ -18302,6 +18308,15 @@
     <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18528,26 +18543,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
V_MAP_SECCHI_DISK_OBSERVATION,V_D_MLO_SHIP, V_D_MLO_SEABED_CONTACT, V_D_MLO_REPTILES, V_D_MLO_JELLYFISH, V_D_MLO_JELLYFISH, V_D_MLO_JELLYFISH, V_D_MLO_FISH, V_D_MLO_CETACEANS, V_D_AQUAPACK_PROFILE, V_D_ADCP added
</commit_message>
<xml_diff>
--- a/analysis/MEDS_Tables.xlsx
+++ b/analysis/MEDS_Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="851" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8479C32D-1A68-4355-A574-738AE10B8AC7}"/>
+  <xr:revisionPtr revIDLastSave="859" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{565F4BB3-9C22-4E6B-B2F6-C3962A84E0B8}"/>
   <bookViews>
-    <workbookView xWindow="-16000" yWindow="-21710" windowWidth="38620" windowHeight="21820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16005" yWindow="-21705" windowWidth="38625" windowHeight="21825" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meds_tables" sheetId="1" r:id="rId1"/>
@@ -34,23 +34,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3183" uniqueCount="756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3190" uniqueCount="755">
   <si>
     <t>Table</t>
   </si>
@@ -2600,9 +2589,6 @@
     <t xml:space="preserve">Profile climatology 0.25 degree </t>
   </si>
   <si>
-    <t>1file</t>
-  </si>
-  <si>
     <t xml:space="preserve"> to be buit, 1 file ouput</t>
   </si>
   <si>
@@ -2612,13 +2598,13 @@
     <t>Not tested, data is SENSITIVE, and as not sent by Steve</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Unified secchi data</t>
   </si>
   <si>
     <t>Secchi data</t>
+  </si>
+  <si>
+    <t>1 file</t>
   </si>
 </sst>
 </file>
@@ -3485,34 +3471,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3520,14 +3500,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -3724,9 +3710,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3764,7 +3750,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3870,7 +3856,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4012,7 +3998,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -12058,8 +12044,8 @@
   <dimension ref="B1:P201"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L121" sqref="L121"/>
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F105" sqref="F105:F106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12099,7 +12085,7 @@
       <c r="I1" s="37"/>
       <c r="J1" s="35">
         <f>F201/F200</f>
-        <v>0.55645161290322576</v>
+        <v>0.96938775510204078</v>
       </c>
       <c r="K1" s="38" t="s">
         <v>566</v>
@@ -12110,7 +12096,7 @@
       <c r="C2" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="63" t="s">
         <v>38</v>
       </c>
       <c r="E2" s="49"/>
@@ -12120,7 +12106,7 @@
       <c r="G2" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="69" t="s">
+      <c r="H2" s="67" t="s">
         <v>564</v>
       </c>
     </row>
@@ -12128,27 +12114,27 @@
       <c r="C3" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="59"/>
+      <c r="D3" s="62"/>
       <c r="E3" s="45"/>
       <c r="F3" s="61"/>
       <c r="G3" s="61"/>
-      <c r="H3" s="68"/>
+      <c r="H3" s="69"/>
     </row>
     <row r="4" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="59"/>
+      <c r="D4" s="62"/>
       <c r="E4" s="45"/>
       <c r="F4" s="61"/>
       <c r="G4" s="61"/>
-      <c r="H4" s="68"/>
+      <c r="H4" s="69"/>
     </row>
     <row r="5" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="62" t="s">
         <v>53</v>
       </c>
       <c r="E5" s="45"/>
@@ -12158,17 +12144,17 @@
       <c r="G5" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="68" t="s">
+      <c r="H5" s="69" t="s">
         <v>519</v>
       </c>
       <c r="M5" s="36" t="s">
         <v>464</v>
       </c>
-      <c r="N5" s="73" t="s">
+      <c r="N5" s="60" t="s">
         <v>465</v>
       </c>
       <c r="O5" s="61"/>
-      <c r="P5" s="72" t="s">
+      <c r="P5" s="59" t="s">
         <v>581</v>
       </c>
     </row>
@@ -12176,23 +12162,23 @@
       <c r="C6" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="59"/>
+      <c r="D6" s="62"/>
       <c r="E6" s="45"/>
       <c r="F6" s="61"/>
       <c r="G6" s="61"/>
-      <c r="H6" s="68"/>
+      <c r="H6" s="69"/>
       <c r="M6" s="36" t="s">
         <v>467</v>
       </c>
-      <c r="N6" s="73"/>
+      <c r="N6" s="60"/>
       <c r="O6" s="61"/>
-      <c r="P6" s="72"/>
+      <c r="P6" s="59"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C7" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="62" t="s">
         <v>78</v>
       </c>
       <c r="E7" s="45"/>
@@ -12202,7 +12188,7 @@
       <c r="G7" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="68" t="s">
+      <c r="H7" s="69" t="s">
         <v>80</v>
       </c>
     </row>
@@ -12210,17 +12196,17 @@
       <c r="C8" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="59"/>
+      <c r="D8" s="62"/>
       <c r="E8" s="45"/>
       <c r="F8" s="61"/>
       <c r="G8" s="61"/>
-      <c r="H8" s="68"/>
+      <c r="H8" s="69"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C9" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="62" t="s">
         <v>171</v>
       </c>
       <c r="E9" s="45"/>
@@ -12230,7 +12216,7 @@
       <c r="G9" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="H9" s="68" t="s">
+      <c r="H9" s="69" t="s">
         <v>523</v>
       </c>
     </row>
@@ -12238,27 +12224,27 @@
       <c r="C10" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="D10" s="59"/>
+      <c r="D10" s="62"/>
       <c r="E10" s="45"/>
       <c r="F10" s="61"/>
       <c r="G10" s="61"/>
-      <c r="H10" s="68"/>
+      <c r="H10" s="69"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C11" s="31" t="s">
         <v>176</v>
       </c>
-      <c r="D11" s="59"/>
+      <c r="D11" s="62"/>
       <c r="E11" s="45"/>
       <c r="F11" s="61"/>
       <c r="G11" s="61"/>
-      <c r="H11" s="68"/>
+      <c r="H11" s="69"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C12" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="D12" s="59" t="s">
+      <c r="D12" s="62" t="s">
         <v>204</v>
       </c>
       <c r="E12" s="45"/>
@@ -12268,7 +12254,7 @@
       <c r="G12" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="68" t="s">
+      <c r="H12" s="69" t="s">
         <v>515</v>
       </c>
     </row>
@@ -12276,17 +12262,17 @@
       <c r="C13" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="D13" s="59"/>
+      <c r="D13" s="62"/>
       <c r="E13" s="45"/>
       <c r="F13" s="61"/>
       <c r="G13" s="61"/>
-      <c r="H13" s="68"/>
+      <c r="H13" s="69"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C14" s="31" t="s">
         <v>360</v>
       </c>
-      <c r="D14" s="59" t="s">
+      <c r="D14" s="62" t="s">
         <v>361</v>
       </c>
       <c r="E14" s="45"/>
@@ -12296,7 +12282,7 @@
       <c r="G14" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="68" t="s">
+      <c r="H14" s="69" t="s">
         <v>518</v>
       </c>
     </row>
@@ -12304,17 +12290,17 @@
       <c r="C15" s="32" t="s">
         <v>363</v>
       </c>
-      <c r="D15" s="62"/>
+      <c r="D15" s="64"/>
       <c r="E15" s="50"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="70"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="68"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C16" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="67" t="s">
+      <c r="D16" s="63" t="s">
         <v>71</v>
       </c>
       <c r="E16" s="49"/>
@@ -12324,7 +12310,7 @@
       <c r="G16" s="65" t="s">
         <v>567</v>
       </c>
-      <c r="H16" s="69" t="s">
+      <c r="H16" s="67" t="s">
         <v>73</v>
       </c>
     </row>
@@ -12332,17 +12318,17 @@
       <c r="C17" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="59"/>
+      <c r="D17" s="62"/>
       <c r="E17" s="45"/>
       <c r="F17" s="61"/>
       <c r="G17" s="61"/>
-      <c r="H17" s="68"/>
+      <c r="H17" s="69"/>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C18" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="59" t="s">
+      <c r="D18" s="62" t="s">
         <v>105</v>
       </c>
       <c r="E18" s="45"/>
@@ -12352,7 +12338,7 @@
       <c r="G18" s="61" t="s">
         <v>567</v>
       </c>
-      <c r="H18" s="68" t="s">
+      <c r="H18" s="69" t="s">
         <v>524</v>
       </c>
     </row>
@@ -12360,17 +12346,17 @@
       <c r="C19" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="59"/>
+      <c r="D19" s="62"/>
       <c r="E19" s="45"/>
       <c r="F19" s="61"/>
       <c r="G19" s="61"/>
-      <c r="H19" s="68"/>
+      <c r="H19" s="69"/>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C20" s="31" t="s">
         <v>299</v>
       </c>
-      <c r="D20" s="59" t="s">
+      <c r="D20" s="62" t="s">
         <v>300</v>
       </c>
       <c r="E20" s="45"/>
@@ -12380,7 +12366,7 @@
       <c r="G20" s="61" t="s">
         <v>567</v>
       </c>
-      <c r="H20" s="68" t="s">
+      <c r="H20" s="69" t="s">
         <v>516</v>
       </c>
     </row>
@@ -12388,17 +12374,17 @@
       <c r="C21" s="31" t="s">
         <v>302</v>
       </c>
-      <c r="D21" s="59"/>
+      <c r="D21" s="62"/>
       <c r="E21" s="45"/>
       <c r="F21" s="61"/>
       <c r="G21" s="61"/>
-      <c r="H21" s="68"/>
+      <c r="H21" s="69"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C22" s="31" t="s">
         <v>304</v>
       </c>
-      <c r="D22" s="59" t="s">
+      <c r="D22" s="62" t="s">
         <v>305</v>
       </c>
       <c r="E22" s="45"/>
@@ -12408,7 +12394,7 @@
       <c r="G22" s="61" t="s">
         <v>567</v>
       </c>
-      <c r="H22" s="68" t="s">
+      <c r="H22" s="69" t="s">
         <v>521</v>
       </c>
     </row>
@@ -12416,17 +12402,17 @@
       <c r="C23" s="31" t="s">
         <v>309</v>
       </c>
-      <c r="D23" s="59"/>
+      <c r="D23" s="62"/>
       <c r="E23" s="45"/>
       <c r="F23" s="61"/>
       <c r="G23" s="61"/>
-      <c r="H23" s="68"/>
+      <c r="H23" s="69"/>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C24" s="31" t="s">
         <v>317</v>
       </c>
-      <c r="D24" s="59" t="s">
+      <c r="D24" s="62" t="s">
         <v>318</v>
       </c>
       <c r="E24" s="45"/>
@@ -12436,7 +12422,7 @@
       <c r="G24" s="61" t="s">
         <v>567</v>
       </c>
-      <c r="H24" s="68" t="s">
+      <c r="H24" s="69" t="s">
         <v>512</v>
       </c>
     </row>
@@ -12444,17 +12430,17 @@
       <c r="C25" s="31" t="s">
         <v>320</v>
       </c>
-      <c r="D25" s="59"/>
+      <c r="D25" s="62"/>
       <c r="E25" s="45"/>
       <c r="F25" s="61"/>
       <c r="G25" s="61"/>
-      <c r="H25" s="68"/>
+      <c r="H25" s="69"/>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C26" s="31" t="s">
         <v>322</v>
       </c>
-      <c r="D26" s="66" t="s">
+      <c r="D26" s="70" t="s">
         <v>323</v>
       </c>
       <c r="E26" s="48"/>
@@ -12464,7 +12450,7 @@
       <c r="G26" s="61" t="s">
         <v>567</v>
       </c>
-      <c r="H26" s="68" t="s">
+      <c r="H26" s="69" t="s">
         <v>517</v>
       </c>
     </row>
@@ -12472,17 +12458,17 @@
       <c r="C27" s="31" t="s">
         <v>325</v>
       </c>
-      <c r="D27" s="66"/>
+      <c r="D27" s="70"/>
       <c r="E27" s="48"/>
       <c r="F27" s="71"/>
       <c r="G27" s="61"/>
-      <c r="H27" s="68"/>
+      <c r="H27" s="69"/>
     </row>
     <row r="28" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C28" s="31" t="s">
         <v>327</v>
       </c>
-      <c r="D28" s="59" t="s">
+      <c r="D28" s="62" t="s">
         <v>328</v>
       </c>
       <c r="E28" s="45"/>
@@ -12492,7 +12478,7 @@
       <c r="G28" s="61" t="s">
         <v>567</v>
       </c>
-      <c r="H28" s="68" t="s">
+      <c r="H28" s="69" t="s">
         <v>508</v>
       </c>
     </row>
@@ -12500,17 +12486,17 @@
       <c r="C29" s="31" t="s">
         <v>330</v>
       </c>
-      <c r="D29" s="59"/>
+      <c r="D29" s="62"/>
       <c r="E29" s="45"/>
       <c r="F29" s="61"/>
       <c r="G29" s="61"/>
-      <c r="H29" s="68"/>
+      <c r="H29" s="69"/>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C30" s="31" t="s">
         <v>332</v>
       </c>
-      <c r="D30" s="59" t="s">
+      <c r="D30" s="62" t="s">
         <v>333</v>
       </c>
       <c r="E30" s="45"/>
@@ -12520,7 +12506,7 @@
       <c r="G30" s="61" t="s">
         <v>567</v>
       </c>
-      <c r="H30" s="68" t="s">
+      <c r="H30" s="69" t="s">
         <v>510</v>
       </c>
     </row>
@@ -12528,17 +12514,17 @@
       <c r="C31" s="31" t="s">
         <v>335</v>
       </c>
-      <c r="D31" s="59"/>
+      <c r="D31" s="62"/>
       <c r="E31" s="45"/>
       <c r="F31" s="61"/>
       <c r="G31" s="61"/>
-      <c r="H31" s="68"/>
+      <c r="H31" s="69"/>
     </row>
     <row r="32" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C32" s="31" t="s">
         <v>337</v>
       </c>
-      <c r="D32" s="59" t="s">
+      <c r="D32" s="62" t="s">
         <v>338</v>
       </c>
       <c r="E32" s="45"/>
@@ -12548,7 +12534,7 @@
       <c r="G32" s="61" t="s">
         <v>567</v>
       </c>
-      <c r="H32" s="68" t="s">
+      <c r="H32" s="69" t="s">
         <v>511</v>
       </c>
     </row>
@@ -12556,17 +12542,17 @@
       <c r="C33" s="31" t="s">
         <v>340</v>
       </c>
-      <c r="D33" s="59"/>
+      <c r="D33" s="62"/>
       <c r="E33" s="45"/>
       <c r="F33" s="61"/>
       <c r="G33" s="61"/>
-      <c r="H33" s="68"/>
+      <c r="H33" s="69"/>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C34" s="31" t="s">
         <v>342</v>
       </c>
-      <c r="D34" s="59" t="s">
+      <c r="D34" s="62" t="s">
         <v>343</v>
       </c>
       <c r="E34" s="45"/>
@@ -12576,7 +12562,7 @@
       <c r="G34" s="61" t="s">
         <v>567</v>
       </c>
-      <c r="H34" s="68" t="s">
+      <c r="H34" s="69" t="s">
         <v>509</v>
       </c>
     </row>
@@ -12584,17 +12570,17 @@
       <c r="C35" s="31" t="s">
         <v>345</v>
       </c>
-      <c r="D35" s="59"/>
+      <c r="D35" s="62"/>
       <c r="E35" s="45"/>
       <c r="F35" s="61"/>
       <c r="G35" s="61"/>
-      <c r="H35" s="68"/>
+      <c r="H35" s="69"/>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C36" s="31" t="s">
         <v>347</v>
       </c>
-      <c r="D36" s="59" t="s">
+      <c r="D36" s="62" t="s">
         <v>348</v>
       </c>
       <c r="E36" s="45"/>
@@ -12604,7 +12590,7 @@
       <c r="G36" s="61" t="s">
         <v>567</v>
       </c>
-      <c r="H36" s="68" t="s">
+      <c r="H36" s="69" t="s">
         <v>520</v>
       </c>
     </row>
@@ -12612,17 +12598,17 @@
       <c r="C37" s="32" t="s">
         <v>350</v>
       </c>
-      <c r="D37" s="62"/>
+      <c r="D37" s="64"/>
       <c r="E37" s="50"/>
-      <c r="F37" s="64"/>
-      <c r="G37" s="64"/>
-      <c r="H37" s="70"/>
+      <c r="F37" s="66"/>
+      <c r="G37" s="66"/>
+      <c r="H37" s="68"/>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C38" s="30" t="s">
         <v>365</v>
       </c>
-      <c r="D38" s="67" t="s">
+      <c r="D38" s="63" t="s">
         <v>366</v>
       </c>
       <c r="E38" s="49"/>
@@ -12632,7 +12618,7 @@
       <c r="G38" s="65" t="s">
         <v>369</v>
       </c>
-      <c r="H38" s="69" t="s">
+      <c r="H38" s="67" t="s">
         <v>514</v>
       </c>
     </row>
@@ -12640,27 +12626,27 @@
       <c r="C39" s="31" t="s">
         <v>376</v>
       </c>
-      <c r="D39" s="59"/>
+      <c r="D39" s="62"/>
       <c r="E39" s="45"/>
       <c r="F39" s="61"/>
       <c r="G39" s="61"/>
-      <c r="H39" s="68"/>
+      <c r="H39" s="69"/>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C40" s="31" t="s">
         <v>382</v>
       </c>
-      <c r="D40" s="59"/>
+      <c r="D40" s="62"/>
       <c r="E40" s="45"/>
       <c r="F40" s="61"/>
       <c r="G40" s="61"/>
-      <c r="H40" s="68"/>
+      <c r="H40" s="69"/>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C41" s="31" t="s">
         <v>370</v>
       </c>
-      <c r="D41" s="59" t="s">
+      <c r="D41" s="62" t="s">
         <v>371</v>
       </c>
       <c r="E41" s="45"/>
@@ -12670,7 +12656,7 @@
       <c r="G41" s="61" t="s">
         <v>369</v>
       </c>
-      <c r="H41" s="68" t="s">
+      <c r="H41" s="69" t="s">
         <v>513</v>
       </c>
     </row>
@@ -12678,27 +12664,27 @@
       <c r="C42" s="31" t="s">
         <v>378</v>
       </c>
-      <c r="D42" s="59"/>
+      <c r="D42" s="62"/>
       <c r="E42" s="45"/>
       <c r="F42" s="61"/>
       <c r="G42" s="61"/>
-      <c r="H42" s="68"/>
+      <c r="H42" s="69"/>
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C43" s="31" t="s">
         <v>384</v>
       </c>
-      <c r="D43" s="59"/>
+      <c r="D43" s="62"/>
       <c r="E43" s="45"/>
       <c r="F43" s="61"/>
       <c r="G43" s="61"/>
-      <c r="H43" s="68"/>
+      <c r="H43" s="69"/>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C44" s="31" t="s">
         <v>373</v>
       </c>
-      <c r="D44" s="59" t="s">
+      <c r="D44" s="62" t="s">
         <v>374</v>
       </c>
       <c r="E44" s="45"/>
@@ -12708,7 +12694,7 @@
       <c r="G44" s="61" t="s">
         <v>369</v>
       </c>
-      <c r="H44" s="68" t="s">
+      <c r="H44" s="69" t="s">
         <v>522</v>
       </c>
     </row>
@@ -12716,27 +12702,27 @@
       <c r="C45" s="31" t="s">
         <v>380</v>
       </c>
-      <c r="D45" s="59"/>
+      <c r="D45" s="62"/>
       <c r="E45" s="45"/>
       <c r="F45" s="61"/>
       <c r="G45" s="61"/>
-      <c r="H45" s="68"/>
+      <c r="H45" s="69"/>
     </row>
     <row r="46" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C46" s="31" t="s">
         <v>386</v>
       </c>
-      <c r="D46" s="59"/>
+      <c r="D46" s="62"/>
       <c r="E46" s="45"/>
       <c r="F46" s="61"/>
       <c r="G46" s="61"/>
-      <c r="H46" s="68"/>
+      <c r="H46" s="69"/>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C47" s="30" t="s">
         <v>464</v>
       </c>
-      <c r="D47" s="67" t="s">
+      <c r="D47" s="63" t="s">
         <v>465</v>
       </c>
       <c r="E47" s="49"/>
@@ -12744,7 +12730,7 @@
       <c r="G47" s="65" t="s">
         <v>584</v>
       </c>
-      <c r="H47" s="69" t="s">
+      <c r="H47" s="67" t="s">
         <v>585</v>
       </c>
     </row>
@@ -12752,11 +12738,11 @@
       <c r="C48" s="32" t="s">
         <v>467</v>
       </c>
-      <c r="D48" s="62"/>
+      <c r="D48" s="64"/>
       <c r="E48" s="50"/>
-      <c r="F48" s="64"/>
-      <c r="G48" s="64"/>
-      <c r="H48" s="70"/>
+      <c r="F48" s="66"/>
+      <c r="G48" s="66"/>
+      <c r="H48" s="68"/>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C49" s="31" t="s">
@@ -12787,7 +12773,7 @@
         <v>683</v>
       </c>
       <c r="H50" s="54" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.25">
@@ -13537,25 +13523,27 @@
       <c r="C98" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="D98" s="67" t="s">
+      <c r="D98" s="63" t="s">
         <v>38</v>
       </c>
       <c r="E98" s="65">
         <v>1</v>
       </c>
-      <c r="F98" s="65"/>
+      <c r="F98" s="65" t="s">
+        <v>81</v>
+      </c>
       <c r="G98" s="65" t="s">
         <v>18</v>
       </c>
       <c r="H98" s="52" t="s">
-        <v>749</v>
+        <v>754</v>
       </c>
     </row>
     <row r="99" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C99" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="D99" s="59"/>
+      <c r="D99" s="62"/>
       <c r="E99" s="61"/>
       <c r="F99" s="61"/>
       <c r="G99" s="61"/>
@@ -13567,7 +13555,7 @@
       <c r="C100" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="D100" s="59"/>
+      <c r="D100" s="62"/>
       <c r="E100" s="61"/>
       <c r="F100" s="61"/>
       <c r="G100" s="61"/>
@@ -13579,7 +13567,7 @@
       <c r="C101" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="D101" s="59" t="s">
+      <c r="D101" s="62" t="s">
         <v>48</v>
       </c>
       <c r="E101" s="61">
@@ -13590,14 +13578,14 @@
         <v>18</v>
       </c>
       <c r="H101" s="39" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="102" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C102" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="D102" s="59"/>
+      <c r="D102" s="62"/>
       <c r="E102" s="61"/>
       <c r="F102" s="61"/>
       <c r="G102" s="61"/>
@@ -13609,13 +13597,15 @@
       <c r="C103" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="D103" s="59" t="s">
+      <c r="D103" s="62" t="s">
         <v>53</v>
       </c>
       <c r="E103" s="61">
         <v>1</v>
       </c>
-      <c r="F103" s="61"/>
+      <c r="F103" s="61" t="s">
+        <v>81</v>
+      </c>
       <c r="G103" s="61" t="s">
         <v>18</v>
       </c>
@@ -13627,7 +13617,7 @@
       <c r="C104" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="D104" s="59"/>
+      <c r="D104" s="62"/>
       <c r="E104" s="61"/>
       <c r="F104" s="61"/>
       <c r="G104" s="61"/>
@@ -13639,7 +13629,7 @@
       <c r="C105" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="D105" s="59" t="s">
+      <c r="D105" s="62" t="s">
         <v>78</v>
       </c>
       <c r="E105" s="61">
@@ -13657,7 +13647,7 @@
       <c r="C106" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="D106" s="59"/>
+      <c r="D106" s="62"/>
       <c r="E106" s="61"/>
       <c r="F106" s="61"/>
       <c r="G106" s="61"/>
@@ -13669,7 +13659,7 @@
       <c r="C107" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="D107" s="59" t="s">
+      <c r="D107" s="62" t="s">
         <v>71</v>
       </c>
       <c r="E107" s="61">
@@ -13687,7 +13677,7 @@
       <c r="C108" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="D108" s="59"/>
+      <c r="D108" s="62"/>
       <c r="E108" s="61"/>
       <c r="F108" s="61"/>
       <c r="G108" s="61"/>
@@ -13699,7 +13689,7 @@
       <c r="C109" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="D109" s="59" t="s">
+      <c r="D109" s="62" t="s">
         <v>105</v>
       </c>
       <c r="E109" s="61">
@@ -13717,7 +13707,7 @@
       <c r="C110" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="D110" s="59"/>
+      <c r="D110" s="62"/>
       <c r="E110" s="61"/>
       <c r="F110" s="61"/>
       <c r="G110" s="61"/>
@@ -13729,7 +13719,7 @@
       <c r="C111" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="D111" s="59" t="s">
+      <c r="D111" s="62" t="s">
         <v>171</v>
       </c>
       <c r="E111" s="61">
@@ -13747,7 +13737,7 @@
       <c r="C112" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="D112" s="59"/>
+      <c r="D112" s="62"/>
       <c r="E112" s="61"/>
       <c r="F112" s="61"/>
       <c r="G112" s="61"/>
@@ -13759,7 +13749,7 @@
       <c r="C113" s="31" t="s">
         <v>176</v>
       </c>
-      <c r="D113" s="59"/>
+      <c r="D113" s="62"/>
       <c r="E113" s="61"/>
       <c r="F113" s="61"/>
       <c r="G113" s="61"/>
@@ -13771,7 +13761,7 @@
       <c r="C114" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="D114" s="59" t="s">
+      <c r="D114" s="62" t="s">
         <v>204</v>
       </c>
       <c r="E114" s="61">
@@ -13789,7 +13779,7 @@
       <c r="C115" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="D115" s="59"/>
+      <c r="D115" s="62"/>
       <c r="E115" s="61"/>
       <c r="F115" s="61"/>
       <c r="G115" s="61"/>
@@ -13801,7 +13791,7 @@
       <c r="C116" s="31" t="s">
         <v>299</v>
       </c>
-      <c r="D116" s="59" t="s">
+      <c r="D116" s="62" t="s">
         <v>300</v>
       </c>
       <c r="E116" s="61">
@@ -13821,7 +13811,7 @@
       <c r="C117" s="31" t="s">
         <v>302</v>
       </c>
-      <c r="D117" s="59"/>
+      <c r="D117" s="62"/>
       <c r="E117" s="61"/>
       <c r="F117" s="61"/>
       <c r="G117" s="61"/>
@@ -13833,13 +13823,15 @@
       <c r="C118" s="31" t="s">
         <v>304</v>
       </c>
-      <c r="D118" s="59" t="s">
+      <c r="D118" s="62" t="s">
         <v>305</v>
       </c>
       <c r="E118" s="61">
         <v>1</v>
       </c>
-      <c r="F118" s="61"/>
+      <c r="F118" s="61" t="s">
+        <v>81</v>
+      </c>
       <c r="G118" s="61" t="s">
         <v>18</v>
       </c>
@@ -13851,7 +13843,7 @@
       <c r="C119" s="31" t="s">
         <v>309</v>
       </c>
-      <c r="D119" s="59"/>
+      <c r="D119" s="62"/>
       <c r="E119" s="61"/>
       <c r="F119" s="61"/>
       <c r="G119" s="61"/>
@@ -13863,7 +13855,7 @@
       <c r="C120" s="31" t="s">
         <v>307</v>
       </c>
-      <c r="D120" s="59"/>
+      <c r="D120" s="62"/>
       <c r="E120" s="61"/>
       <c r="F120" s="61"/>
       <c r="G120" s="61"/>
@@ -13875,7 +13867,7 @@
       <c r="C121" s="31" t="s">
         <v>311</v>
       </c>
-      <c r="D121" s="59"/>
+      <c r="D121" s="62"/>
       <c r="E121" s="61"/>
       <c r="F121" s="61"/>
       <c r="G121" s="61"/>
@@ -13887,13 +13879,15 @@
       <c r="C122" s="31" t="s">
         <v>317</v>
       </c>
-      <c r="D122" s="59" t="s">
+      <c r="D122" s="62" t="s">
         <v>318</v>
       </c>
       <c r="E122" s="61">
         <v>1</v>
       </c>
-      <c r="F122" s="61"/>
+      <c r="F122" s="61" t="s">
+        <v>81</v>
+      </c>
       <c r="G122" s="61" t="s">
         <v>18</v>
       </c>
@@ -13905,7 +13899,7 @@
       <c r="C123" s="31" t="s">
         <v>320</v>
       </c>
-      <c r="D123" s="59"/>
+      <c r="D123" s="62"/>
       <c r="E123" s="61"/>
       <c r="F123" s="61"/>
       <c r="G123" s="61"/>
@@ -13917,13 +13911,15 @@
       <c r="C124" s="31" t="s">
         <v>322</v>
       </c>
-      <c r="D124" s="66" t="s">
+      <c r="D124" s="70" t="s">
         <v>323</v>
       </c>
       <c r="E124" s="61">
         <v>1</v>
       </c>
-      <c r="F124" s="61"/>
+      <c r="F124" s="61" t="s">
+        <v>81</v>
+      </c>
       <c r="G124" s="61" t="s">
         <v>18</v>
       </c>
@@ -13935,7 +13931,7 @@
       <c r="C125" s="31" t="s">
         <v>325</v>
       </c>
-      <c r="D125" s="66"/>
+      <c r="D125" s="70"/>
       <c r="E125" s="61"/>
       <c r="F125" s="61"/>
       <c r="G125" s="61"/>
@@ -13947,13 +13943,15 @@
       <c r="C126" s="31" t="s">
         <v>327</v>
       </c>
-      <c r="D126" s="59" t="s">
+      <c r="D126" s="62" t="s">
         <v>328</v>
       </c>
       <c r="E126" s="61">
         <v>1</v>
       </c>
-      <c r="F126" s="61"/>
+      <c r="F126" s="61" t="s">
+        <v>81</v>
+      </c>
       <c r="G126" s="61" t="s">
         <v>18</v>
       </c>
@@ -13965,7 +13963,7 @@
       <c r="C127" s="31" t="s">
         <v>330</v>
       </c>
-      <c r="D127" s="59"/>
+      <c r="D127" s="62"/>
       <c r="E127" s="61"/>
       <c r="F127" s="61"/>
       <c r="G127" s="61"/>
@@ -13977,13 +13975,15 @@
       <c r="C128" s="31" t="s">
         <v>332</v>
       </c>
-      <c r="D128" s="59" t="s">
+      <c r="D128" s="62" t="s">
         <v>333</v>
       </c>
       <c r="E128" s="61">
         <v>1</v>
       </c>
-      <c r="F128" s="61"/>
+      <c r="F128" s="61" t="s">
+        <v>81</v>
+      </c>
       <c r="G128" s="61" t="s">
         <v>18</v>
       </c>
@@ -13995,7 +13995,7 @@
       <c r="C129" s="31" t="s">
         <v>335</v>
       </c>
-      <c r="D129" s="59"/>
+      <c r="D129" s="62"/>
       <c r="E129" s="61"/>
       <c r="F129" s="61"/>
       <c r="G129" s="61"/>
@@ -14007,13 +14007,15 @@
       <c r="C130" s="31" t="s">
         <v>337</v>
       </c>
-      <c r="D130" s="59" t="s">
+      <c r="D130" s="62" t="s">
         <v>338</v>
       </c>
       <c r="E130" s="61">
         <v>1</v>
       </c>
-      <c r="F130" s="61"/>
+      <c r="F130" s="61" t="s">
+        <v>81</v>
+      </c>
       <c r="G130" s="61" t="s">
         <v>18</v>
       </c>
@@ -14025,7 +14027,7 @@
       <c r="C131" s="31" t="s">
         <v>340</v>
       </c>
-      <c r="D131" s="59"/>
+      <c r="D131" s="62"/>
       <c r="E131" s="61"/>
       <c r="F131" s="61"/>
       <c r="G131" s="61"/>
@@ -14037,7 +14039,7 @@
       <c r="C132" s="31" t="s">
         <v>342</v>
       </c>
-      <c r="D132" s="59" t="s">
+      <c r="D132" s="62" t="s">
         <v>343</v>
       </c>
       <c r="E132" s="61">
@@ -14055,7 +14057,7 @@
       <c r="C133" s="31" t="s">
         <v>345</v>
       </c>
-      <c r="D133" s="59"/>
+      <c r="D133" s="62"/>
       <c r="E133" s="61"/>
       <c r="F133" s="61"/>
       <c r="G133" s="61"/>
@@ -14067,13 +14069,15 @@
       <c r="C134" s="31" t="s">
         <v>347</v>
       </c>
-      <c r="D134" s="59" t="s">
+      <c r="D134" s="62" t="s">
         <v>348</v>
       </c>
       <c r="E134" s="61">
         <v>1</v>
       </c>
-      <c r="F134" s="61"/>
+      <c r="F134" s="61" t="s">
+        <v>81</v>
+      </c>
       <c r="G134" s="61" t="s">
         <v>18</v>
       </c>
@@ -14085,7 +14089,7 @@
       <c r="C135" s="31" t="s">
         <v>350</v>
       </c>
-      <c r="D135" s="59"/>
+      <c r="D135" s="62"/>
       <c r="E135" s="61"/>
       <c r="F135" s="61"/>
       <c r="G135" s="61"/>
@@ -14097,7 +14101,7 @@
       <c r="C136" s="31" t="s">
         <v>360</v>
       </c>
-      <c r="D136" s="59" t="s">
+      <c r="D136" s="62" t="s">
         <v>361</v>
       </c>
       <c r="E136" s="61">
@@ -14115,7 +14119,7 @@
       <c r="C137" s="31" t="s">
         <v>363</v>
       </c>
-      <c r="D137" s="59"/>
+      <c r="D137" s="62"/>
       <c r="E137" s="61"/>
       <c r="F137" s="61"/>
       <c r="G137" s="61"/>
@@ -14127,7 +14131,7 @@
       <c r="C138" s="31" t="s">
         <v>365</v>
       </c>
-      <c r="D138" s="59" t="s">
+      <c r="D138" s="62" t="s">
         <v>366</v>
       </c>
       <c r="E138" s="61">
@@ -14145,7 +14149,7 @@
       <c r="C139" s="31" t="s">
         <v>376</v>
       </c>
-      <c r="D139" s="59"/>
+      <c r="D139" s="62"/>
       <c r="E139" s="61"/>
       <c r="F139" s="61"/>
       <c r="G139" s="61"/>
@@ -14157,7 +14161,7 @@
       <c r="C140" s="31" t="s">
         <v>382</v>
       </c>
-      <c r="D140" s="59"/>
+      <c r="D140" s="62"/>
       <c r="E140" s="61"/>
       <c r="F140" s="61"/>
       <c r="G140" s="61"/>
@@ -14169,7 +14173,7 @@
       <c r="C141" s="31" t="s">
         <v>370</v>
       </c>
-      <c r="D141" s="59" t="s">
+      <c r="D141" s="62" t="s">
         <v>371</v>
       </c>
       <c r="E141" s="61">
@@ -14189,7 +14193,7 @@
       <c r="C142" s="31" t="s">
         <v>378</v>
       </c>
-      <c r="D142" s="59"/>
+      <c r="D142" s="62"/>
       <c r="E142" s="61"/>
       <c r="F142" s="61"/>
       <c r="G142" s="61"/>
@@ -14201,7 +14205,7 @@
       <c r="C143" s="31" t="s">
         <v>384</v>
       </c>
-      <c r="D143" s="59"/>
+      <c r="D143" s="62"/>
       <c r="E143" s="61"/>
       <c r="F143" s="61"/>
       <c r="G143" s="61"/>
@@ -14214,7 +14218,7 @@
       <c r="C144" s="31" t="s">
         <v>373</v>
       </c>
-      <c r="D144" s="59" t="s">
+      <c r="D144" s="62" t="s">
         <v>374</v>
       </c>
       <c r="E144" s="61">
@@ -14235,7 +14239,7 @@
       <c r="C145" s="31" t="s">
         <v>380</v>
       </c>
-      <c r="D145" s="59"/>
+      <c r="D145" s="62"/>
       <c r="E145" s="61"/>
       <c r="F145" s="61"/>
       <c r="G145" s="61"/>
@@ -14248,7 +14252,7 @@
       <c r="C146" s="31" t="s">
         <v>386</v>
       </c>
-      <c r="D146" s="59"/>
+      <c r="D146" s="62"/>
       <c r="E146" s="61"/>
       <c r="F146" s="61"/>
       <c r="G146" s="61"/>
@@ -14260,7 +14264,7 @@
       <c r="C147" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="D147" s="59" t="s">
+      <c r="D147" s="62" t="s">
         <v>65</v>
       </c>
       <c r="E147" s="61">
@@ -14278,7 +14282,7 @@
       <c r="C148" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="D148" s="59"/>
+      <c r="D148" s="62"/>
       <c r="E148" s="61"/>
       <c r="F148" s="61"/>
       <c r="G148" s="61"/>
@@ -14290,7 +14294,7 @@
       <c r="C149" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="D149" s="59" t="s">
+      <c r="D149" s="62" t="s">
         <v>110</v>
       </c>
       <c r="E149" s="61">
@@ -14308,7 +14312,7 @@
       <c r="C150" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="D150" s="59"/>
+      <c r="D150" s="62"/>
       <c r="E150" s="61"/>
       <c r="F150" s="61"/>
       <c r="G150" s="61"/>
@@ -14320,7 +14324,7 @@
       <c r="C151" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="D151" s="59"/>
+      <c r="D151" s="62"/>
       <c r="E151" s="61"/>
       <c r="F151" s="61"/>
       <c r="G151" s="61"/>
@@ -14332,7 +14336,7 @@
       <c r="C152" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="D152" s="59" t="s">
+      <c r="D152" s="62" t="s">
         <v>119</v>
       </c>
       <c r="E152" s="61">
@@ -14350,7 +14354,7 @@
       <c r="C153" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="D153" s="59"/>
+      <c r="D153" s="62"/>
       <c r="E153" s="61"/>
       <c r="F153" s="61"/>
       <c r="G153" s="61"/>
@@ -14362,7 +14366,7 @@
       <c r="C154" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="D154" s="59" t="s">
+      <c r="D154" s="62" t="s">
         <v>124</v>
       </c>
       <c r="E154" s="61">
@@ -14380,7 +14384,7 @@
       <c r="C155" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="D155" s="59"/>
+      <c r="D155" s="62"/>
       <c r="E155" s="61"/>
       <c r="F155" s="61"/>
       <c r="G155" s="61"/>
@@ -14392,7 +14396,7 @@
       <c r="C156" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="D156" s="59"/>
+      <c r="D156" s="62"/>
       <c r="E156" s="61"/>
       <c r="F156" s="61"/>
       <c r="G156" s="61"/>
@@ -14404,7 +14408,7 @@
       <c r="C157" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="D157" s="59" t="s">
+      <c r="D157" s="62" t="s">
         <v>131</v>
       </c>
       <c r="E157" s="61">
@@ -14422,7 +14426,7 @@
       <c r="C158" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="D158" s="59"/>
+      <c r="D158" s="62"/>
       <c r="E158" s="61"/>
       <c r="F158" s="61"/>
       <c r="G158" s="61"/>
@@ -14434,7 +14438,7 @@
       <c r="C159" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="D159" s="59"/>
+      <c r="D159" s="62"/>
       <c r="E159" s="61"/>
       <c r="F159" s="61"/>
       <c r="G159" s="61"/>
@@ -14446,25 +14450,27 @@
       <c r="C160" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="D160" s="59" t="s">
+      <c r="D160" s="62" t="s">
         <v>159</v>
       </c>
       <c r="E160" s="61">
         <v>5</v>
       </c>
-      <c r="F160" s="61"/>
+      <c r="F160" s="61">
+        <v>5</v>
+      </c>
       <c r="G160" s="61" t="s">
         <v>18</v>
       </c>
       <c r="H160" s="39" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="161" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C161" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D161" s="59"/>
+      <c r="D161" s="62"/>
       <c r="E161" s="61"/>
       <c r="F161" s="61"/>
       <c r="G161" s="61"/>
@@ -14476,13 +14482,15 @@
       <c r="C162" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="D162" s="59" t="s">
+      <c r="D162" s="62" t="s">
         <v>164</v>
       </c>
       <c r="E162" s="61">
         <v>5</v>
       </c>
-      <c r="F162" s="61"/>
+      <c r="F162" s="61">
+        <v>5</v>
+      </c>
       <c r="G162" s="61" t="s">
         <v>18</v>
       </c>
@@ -14494,7 +14502,7 @@
       <c r="C163" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="D163" s="59"/>
+      <c r="D163" s="62"/>
       <c r="E163" s="61"/>
       <c r="F163" s="61"/>
       <c r="G163" s="61"/>
@@ -14506,7 +14514,7 @@
       <c r="C164" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="D164" s="59"/>
+      <c r="D164" s="62"/>
       <c r="E164" s="61"/>
       <c r="F164" s="61"/>
       <c r="G164" s="61"/>
@@ -14518,13 +14526,15 @@
       <c r="C165" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="D165" s="59" t="s">
+      <c r="D165" s="62" t="s">
         <v>179</v>
       </c>
       <c r="E165" s="61">
         <v>5</v>
       </c>
-      <c r="F165" s="61"/>
+      <c r="F165" s="61">
+        <v>5</v>
+      </c>
       <c r="G165" s="61" t="s">
         <v>18</v>
       </c>
@@ -14536,7 +14546,7 @@
       <c r="C166" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="D166" s="59"/>
+      <c r="D166" s="62"/>
       <c r="E166" s="61"/>
       <c r="F166" s="61"/>
       <c r="G166" s="61"/>
@@ -14548,7 +14558,7 @@
       <c r="C167" s="31" t="s">
         <v>183</v>
       </c>
-      <c r="D167" s="59"/>
+      <c r="D167" s="62"/>
       <c r="E167" s="61"/>
       <c r="F167" s="61"/>
       <c r="G167" s="61"/>
@@ -14560,13 +14570,15 @@
       <c r="C168" s="31" t="s">
         <v>185</v>
       </c>
-      <c r="D168" s="59" t="s">
+      <c r="D168" s="62" t="s">
         <v>186</v>
       </c>
       <c r="E168" s="61">
         <v>5</v>
       </c>
-      <c r="F168" s="61"/>
+      <c r="F168" s="61">
+        <v>5</v>
+      </c>
       <c r="G168" s="61" t="s">
         <v>18</v>
       </c>
@@ -14578,7 +14590,7 @@
       <c r="C169" s="31" t="s">
         <v>188</v>
       </c>
-      <c r="D169" s="59"/>
+      <c r="D169" s="62"/>
       <c r="E169" s="61"/>
       <c r="F169" s="61"/>
       <c r="G169" s="61"/>
@@ -14590,13 +14602,15 @@
       <c r="C170" s="31" t="s">
         <v>194</v>
       </c>
-      <c r="D170" s="59" t="s">
+      <c r="D170" s="62" t="s">
         <v>195</v>
       </c>
       <c r="E170" s="61">
         <v>5</v>
       </c>
-      <c r="F170" s="61"/>
+      <c r="F170" s="61">
+        <v>5</v>
+      </c>
       <c r="G170" s="61" t="s">
         <v>18</v>
       </c>
@@ -14608,7 +14622,7 @@
       <c r="C171" s="31" t="s">
         <v>197</v>
       </c>
-      <c r="D171" s="59"/>
+      <c r="D171" s="62"/>
       <c r="E171" s="61"/>
       <c r="F171" s="61"/>
       <c r="G171" s="61"/>
@@ -14620,13 +14634,15 @@
       <c r="C172" s="31" t="s">
         <v>199</v>
       </c>
-      <c r="D172" s="59" t="s">
+      <c r="D172" s="62" t="s">
         <v>200</v>
       </c>
       <c r="E172" s="61">
         <v>5</v>
       </c>
-      <c r="F172" s="61"/>
+      <c r="F172" s="61">
+        <v>5</v>
+      </c>
       <c r="G172" s="61" t="s">
         <v>18</v>
       </c>
@@ -14638,7 +14654,7 @@
       <c r="C173" s="31" t="s">
         <v>202</v>
       </c>
-      <c r="D173" s="59"/>
+      <c r="D173" s="62"/>
       <c r="E173" s="61"/>
       <c r="F173" s="61"/>
       <c r="G173" s="61"/>
@@ -14650,13 +14666,15 @@
       <c r="C174" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="D174" s="59" t="s">
+      <c r="D174" s="62" t="s">
         <v>211</v>
       </c>
       <c r="E174" s="61">
         <v>5</v>
       </c>
-      <c r="F174" s="61"/>
+      <c r="F174" s="61">
+        <v>5</v>
+      </c>
       <c r="G174" s="61" t="s">
         <v>18</v>
       </c>
@@ -14668,7 +14686,7 @@
       <c r="C175" s="31" t="s">
         <v>213</v>
       </c>
-      <c r="D175" s="59"/>
+      <c r="D175" s="62"/>
       <c r="E175" s="61"/>
       <c r="F175" s="61"/>
       <c r="G175" s="61"/>
@@ -14680,7 +14698,7 @@
       <c r="C176" s="31" t="s">
         <v>215</v>
       </c>
-      <c r="D176" s="59"/>
+      <c r="D176" s="62"/>
       <c r="E176" s="61"/>
       <c r="F176" s="61"/>
       <c r="G176" s="61"/>
@@ -14692,13 +14710,15 @@
       <c r="C177" s="31" t="s">
         <v>222</v>
       </c>
-      <c r="D177" s="59" t="s">
+      <c r="D177" s="62" t="s">
         <v>223</v>
       </c>
       <c r="E177" s="61">
         <v>5</v>
       </c>
-      <c r="F177" s="61"/>
+      <c r="F177" s="61">
+        <v>5</v>
+      </c>
       <c r="G177" s="61" t="s">
         <v>18</v>
       </c>
@@ -14710,7 +14730,7 @@
       <c r="C178" s="31" t="s">
         <v>225</v>
       </c>
-      <c r="D178" s="59"/>
+      <c r="D178" s="62"/>
       <c r="E178" s="61"/>
       <c r="F178" s="61"/>
       <c r="G178" s="61"/>
@@ -14722,13 +14742,15 @@
       <c r="C179" s="31" t="s">
         <v>227</v>
       </c>
-      <c r="D179" s="59" t="s">
+      <c r="D179" s="62" t="s">
         <v>228</v>
       </c>
       <c r="E179" s="61">
         <v>5</v>
       </c>
-      <c r="F179" s="61"/>
+      <c r="F179" s="61">
+        <v>5</v>
+      </c>
       <c r="G179" s="61" t="s">
         <v>18</v>
       </c>
@@ -14740,7 +14762,7 @@
       <c r="C180" s="31" t="s">
         <v>230</v>
       </c>
-      <c r="D180" s="59"/>
+      <c r="D180" s="62"/>
       <c r="E180" s="61"/>
       <c r="F180" s="61"/>
       <c r="G180" s="61"/>
@@ -14752,7 +14774,7 @@
       <c r="C181" s="31" t="s">
         <v>232</v>
       </c>
-      <c r="D181" s="59"/>
+      <c r="D181" s="62"/>
       <c r="E181" s="61"/>
       <c r="F181" s="61"/>
       <c r="G181" s="61"/>
@@ -14770,6 +14792,9 @@
       <c r="E182" s="34">
         <v>4</v>
       </c>
+      <c r="F182" s="34">
+        <v>4</v>
+      </c>
       <c r="G182" s="34" t="s">
         <v>18</v>
       </c>
@@ -14787,6 +14812,9 @@
       <c r="E183" s="34">
         <v>4</v>
       </c>
+      <c r="F183" s="34">
+        <v>4</v>
+      </c>
       <c r="G183" s="34" t="s">
         <v>18</v>
       </c>
@@ -14804,6 +14832,9 @@
       <c r="E184" s="34">
         <v>4</v>
       </c>
+      <c r="F184" s="34">
+        <v>4</v>
+      </c>
       <c r="G184" s="34" t="s">
         <v>18</v>
       </c>
@@ -14821,6 +14852,9 @@
       <c r="E185" s="34">
         <v>4</v>
       </c>
+      <c r="F185" s="34">
+        <v>4</v>
+      </c>
       <c r="G185" s="34" t="s">
         <v>18</v>
       </c>
@@ -14832,7 +14866,7 @@
       <c r="C186" s="31" t="s">
         <v>454</v>
       </c>
-      <c r="D186" s="59" t="s">
+      <c r="D186" s="62" t="s">
         <v>582</v>
       </c>
       <c r="E186" s="61">
@@ -14850,7 +14884,7 @@
       <c r="C187" s="31" t="s">
         <v>457</v>
       </c>
-      <c r="D187" s="59"/>
+      <c r="D187" s="62"/>
       <c r="E187" s="61"/>
       <c r="F187" s="61"/>
       <c r="G187" s="61"/>
@@ -14862,7 +14896,7 @@
       <c r="C188" s="31" t="s">
         <v>459</v>
       </c>
-      <c r="D188" s="59" t="s">
+      <c r="D188" s="62" t="s">
         <v>460</v>
       </c>
       <c r="E188" s="61">
@@ -14880,7 +14914,7 @@
       <c r="C189" s="31" t="s">
         <v>462</v>
       </c>
-      <c r="D189" s="59"/>
+      <c r="D189" s="62"/>
       <c r="E189" s="61"/>
       <c r="F189" s="61"/>
       <c r="G189" s="61"/>
@@ -14898,6 +14932,9 @@
       <c r="E190" s="34">
         <v>4</v>
       </c>
+      <c r="F190" s="34">
+        <v>4</v>
+      </c>
       <c r="G190" s="34" t="s">
         <v>18</v>
       </c>
@@ -14915,6 +14952,9 @@
       <c r="E191" s="34">
         <v>4</v>
       </c>
+      <c r="F191" s="34">
+        <v>4</v>
+      </c>
       <c r="G191" s="34" t="s">
         <v>18</v>
       </c>
@@ -14932,6 +14972,9 @@
       <c r="E192" s="34">
         <v>4</v>
       </c>
+      <c r="F192" s="34">
+        <v>4</v>
+      </c>
       <c r="G192" s="34" t="s">
         <v>18</v>
       </c>
@@ -14943,13 +14986,15 @@
       <c r="C193" s="31" t="s">
         <v>477</v>
       </c>
-      <c r="D193" s="59" t="s">
+      <c r="D193" s="62" t="s">
         <v>478</v>
       </c>
       <c r="E193" s="61">
         <v>5</v>
       </c>
-      <c r="F193" s="61"/>
+      <c r="F193" s="61">
+        <v>5</v>
+      </c>
       <c r="G193" s="61" t="s">
         <v>18</v>
       </c>
@@ -14962,7 +15007,7 @@
       <c r="C194" s="31" t="s">
         <v>480</v>
       </c>
-      <c r="D194" s="59"/>
+      <c r="D194" s="62"/>
       <c r="E194" s="61"/>
       <c r="F194" s="61"/>
       <c r="G194" s="61"/>
@@ -14975,12 +15020,10 @@
       <c r="C195" s="31" t="s">
         <v>464</v>
       </c>
-      <c r="D195" s="59" t="s">
-        <v>755</v>
-      </c>
-      <c r="E195" s="60" t="s">
+      <c r="D195" s="62" t="s">
         <v>753</v>
       </c>
+      <c r="E195" s="72"/>
       <c r="F195" s="61"/>
       <c r="G195" s="61" t="s">
         <v>18</v>
@@ -14992,8 +15035,8 @@
       <c r="C196" t="s">
         <v>467</v>
       </c>
-      <c r="D196" s="59"/>
-      <c r="E196" s="60"/>
+      <c r="D196" s="62"/>
+      <c r="E196" s="72"/>
       <c r="F196" s="61"/>
       <c r="G196" s="61"/>
       <c r="H196" s="56"/>
@@ -15003,12 +15046,10 @@
       <c r="C197" t="s">
         <v>495</v>
       </c>
-      <c r="D197" s="59" t="s">
-        <v>754</v>
-      </c>
-      <c r="E197" s="60" t="s">
-        <v>753</v>
-      </c>
+      <c r="D197" s="62" t="s">
+        <v>752</v>
+      </c>
+      <c r="E197" s="72"/>
       <c r="F197" s="61"/>
       <c r="G197" s="61" t="s">
         <v>18</v>
@@ -15020,27 +15061,250 @@
       <c r="C198" s="58" t="s">
         <v>498</v>
       </c>
-      <c r="D198" s="62"/>
-      <c r="E198" s="63"/>
-      <c r="F198" s="64"/>
-      <c r="G198" s="64"/>
+      <c r="D198" s="64"/>
+      <c r="E198" s="73"/>
+      <c r="F198" s="66"/>
+      <c r="G198" s="66"/>
       <c r="H198" s="57"/>
     </row>
     <row r="200" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F200" s="34">
         <f>COUNTBLANK(F2:F194)</f>
-        <v>124</v>
+        <v>98</v>
       </c>
     </row>
     <row r="201" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F201" s="34">
         <f>COUNTA(F2:F194)</f>
-        <v>69</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q1" xr:uid="{20647E0C-146B-49B2-BC4C-D733C2BD2881}"/>
   <mergeCells count="247">
+    <mergeCell ref="D195:D196"/>
+    <mergeCell ref="E195:E196"/>
+    <mergeCell ref="F195:F196"/>
+    <mergeCell ref="G195:G196"/>
+    <mergeCell ref="D197:D198"/>
+    <mergeCell ref="E197:E198"/>
+    <mergeCell ref="F197:F198"/>
+    <mergeCell ref="G197:G198"/>
+    <mergeCell ref="E144:E146"/>
+    <mergeCell ref="E147:E148"/>
+    <mergeCell ref="E149:E151"/>
+    <mergeCell ref="E152:E153"/>
+    <mergeCell ref="E154:E156"/>
+    <mergeCell ref="E157:E159"/>
+    <mergeCell ref="E160:E161"/>
+    <mergeCell ref="E162:E164"/>
+    <mergeCell ref="E165:E167"/>
+    <mergeCell ref="D152:D153"/>
+    <mergeCell ref="F152:F153"/>
+    <mergeCell ref="G152:G153"/>
+    <mergeCell ref="D154:D156"/>
+    <mergeCell ref="F154:F156"/>
+    <mergeCell ref="G154:G156"/>
+    <mergeCell ref="D147:D148"/>
+    <mergeCell ref="E124:E125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="E128:E129"/>
+    <mergeCell ref="E130:E131"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="E134:E135"/>
+    <mergeCell ref="E136:E137"/>
+    <mergeCell ref="E138:E140"/>
+    <mergeCell ref="E141:E143"/>
+    <mergeCell ref="D138:D140"/>
+    <mergeCell ref="F138:F140"/>
+    <mergeCell ref="G138:G140"/>
+    <mergeCell ref="D141:D143"/>
+    <mergeCell ref="F141:F143"/>
+    <mergeCell ref="G141:G143"/>
+    <mergeCell ref="F98:F100"/>
+    <mergeCell ref="F103:F104"/>
+    <mergeCell ref="G103:G104"/>
+    <mergeCell ref="F105:F106"/>
+    <mergeCell ref="G105:G106"/>
+    <mergeCell ref="F107:F108"/>
+    <mergeCell ref="G107:G108"/>
+    <mergeCell ref="F109:F110"/>
+    <mergeCell ref="G109:G110"/>
+    <mergeCell ref="D118:D121"/>
+    <mergeCell ref="D122:D123"/>
+    <mergeCell ref="D124:D125"/>
+    <mergeCell ref="D126:D127"/>
+    <mergeCell ref="D128:D129"/>
+    <mergeCell ref="D130:D131"/>
+    <mergeCell ref="D132:D133"/>
+    <mergeCell ref="G136:G137"/>
+    <mergeCell ref="F116:F117"/>
+    <mergeCell ref="G128:G129"/>
+    <mergeCell ref="G130:G131"/>
+    <mergeCell ref="G132:G133"/>
+    <mergeCell ref="F136:F137"/>
+    <mergeCell ref="G134:G135"/>
+    <mergeCell ref="D134:D135"/>
+    <mergeCell ref="D136:D137"/>
+    <mergeCell ref="D116:D117"/>
+    <mergeCell ref="F122:F123"/>
+    <mergeCell ref="F124:F125"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="F128:F129"/>
+    <mergeCell ref="F130:F131"/>
+    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="F134:F135"/>
+    <mergeCell ref="G116:G117"/>
+    <mergeCell ref="F118:F121"/>
+    <mergeCell ref="G118:G121"/>
+    <mergeCell ref="G122:G123"/>
+    <mergeCell ref="G124:G125"/>
+    <mergeCell ref="G126:G127"/>
+    <mergeCell ref="E116:E117"/>
+    <mergeCell ref="E118:E121"/>
+    <mergeCell ref="E122:E123"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="D98:D100"/>
+    <mergeCell ref="D103:D104"/>
+    <mergeCell ref="D105:D106"/>
+    <mergeCell ref="D111:D113"/>
+    <mergeCell ref="D114:D115"/>
+    <mergeCell ref="G111:G113"/>
+    <mergeCell ref="D107:D108"/>
+    <mergeCell ref="D109:D110"/>
+    <mergeCell ref="G98:G100"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="G114:G115"/>
+    <mergeCell ref="F111:F113"/>
+    <mergeCell ref="E98:E100"/>
+    <mergeCell ref="E101:E102"/>
+    <mergeCell ref="E103:E104"/>
+    <mergeCell ref="E105:E106"/>
+    <mergeCell ref="E107:E108"/>
+    <mergeCell ref="E109:E110"/>
+    <mergeCell ref="E111:E113"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="G41:G43"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="F147:F148"/>
+    <mergeCell ref="G147:G148"/>
+    <mergeCell ref="D149:D151"/>
+    <mergeCell ref="F149:F151"/>
+    <mergeCell ref="G149:G151"/>
+    <mergeCell ref="D162:D164"/>
+    <mergeCell ref="F162:F164"/>
+    <mergeCell ref="G162:G164"/>
+    <mergeCell ref="D165:D167"/>
+    <mergeCell ref="F165:F167"/>
+    <mergeCell ref="G165:G167"/>
+    <mergeCell ref="D157:D159"/>
+    <mergeCell ref="F157:F159"/>
+    <mergeCell ref="G157:G159"/>
+    <mergeCell ref="D160:D161"/>
+    <mergeCell ref="F160:F161"/>
+    <mergeCell ref="G160:G161"/>
+    <mergeCell ref="D172:D173"/>
+    <mergeCell ref="F172:F173"/>
+    <mergeCell ref="G172:G173"/>
+    <mergeCell ref="D174:D176"/>
+    <mergeCell ref="F174:F176"/>
+    <mergeCell ref="G174:G176"/>
+    <mergeCell ref="D168:D169"/>
+    <mergeCell ref="F168:F169"/>
+    <mergeCell ref="G168:G169"/>
+    <mergeCell ref="D170:D171"/>
+    <mergeCell ref="F170:F171"/>
+    <mergeCell ref="G170:G171"/>
+    <mergeCell ref="E168:E169"/>
+    <mergeCell ref="E170:E171"/>
+    <mergeCell ref="E172:E173"/>
+    <mergeCell ref="E174:E176"/>
+    <mergeCell ref="D193:D194"/>
+    <mergeCell ref="F193:F194"/>
+    <mergeCell ref="G193:G194"/>
+    <mergeCell ref="D177:D178"/>
+    <mergeCell ref="F177:F178"/>
+    <mergeCell ref="G177:G178"/>
+    <mergeCell ref="D179:D181"/>
+    <mergeCell ref="F179:F181"/>
+    <mergeCell ref="G179:G181"/>
+    <mergeCell ref="D186:D187"/>
+    <mergeCell ref="D188:D189"/>
+    <mergeCell ref="G186:G187"/>
+    <mergeCell ref="G188:G189"/>
+    <mergeCell ref="F186:F187"/>
+    <mergeCell ref="F188:F189"/>
+    <mergeCell ref="E177:E178"/>
+    <mergeCell ref="E179:E181"/>
+    <mergeCell ref="E186:E187"/>
+    <mergeCell ref="E188:E189"/>
+    <mergeCell ref="E193:E194"/>
     <mergeCell ref="P5:P6"/>
     <mergeCell ref="N5:N6"/>
     <mergeCell ref="O5:O6"/>
@@ -15065,229 +15329,6 @@
     <mergeCell ref="D34:D35"/>
     <mergeCell ref="F34:F35"/>
     <mergeCell ref="G34:G35"/>
-    <mergeCell ref="D193:D194"/>
-    <mergeCell ref="F193:F194"/>
-    <mergeCell ref="G193:G194"/>
-    <mergeCell ref="D177:D178"/>
-    <mergeCell ref="F177:F178"/>
-    <mergeCell ref="G177:G178"/>
-    <mergeCell ref="D179:D181"/>
-    <mergeCell ref="F179:F181"/>
-    <mergeCell ref="G179:G181"/>
-    <mergeCell ref="D186:D187"/>
-    <mergeCell ref="D188:D189"/>
-    <mergeCell ref="G186:G187"/>
-    <mergeCell ref="G188:G189"/>
-    <mergeCell ref="F186:F187"/>
-    <mergeCell ref="F188:F189"/>
-    <mergeCell ref="E177:E178"/>
-    <mergeCell ref="E179:E181"/>
-    <mergeCell ref="E186:E187"/>
-    <mergeCell ref="E188:E189"/>
-    <mergeCell ref="E193:E194"/>
-    <mergeCell ref="D172:D173"/>
-    <mergeCell ref="F172:F173"/>
-    <mergeCell ref="G172:G173"/>
-    <mergeCell ref="D174:D176"/>
-    <mergeCell ref="F174:F176"/>
-    <mergeCell ref="G174:G176"/>
-    <mergeCell ref="D168:D169"/>
-    <mergeCell ref="F168:F169"/>
-    <mergeCell ref="G168:G169"/>
-    <mergeCell ref="D170:D171"/>
-    <mergeCell ref="F170:F171"/>
-    <mergeCell ref="G170:G171"/>
-    <mergeCell ref="E168:E169"/>
-    <mergeCell ref="E170:E171"/>
-    <mergeCell ref="E172:E173"/>
-    <mergeCell ref="E174:E176"/>
-    <mergeCell ref="F147:F148"/>
-    <mergeCell ref="G147:G148"/>
-    <mergeCell ref="D149:D151"/>
-    <mergeCell ref="F149:F151"/>
-    <mergeCell ref="G149:G151"/>
-    <mergeCell ref="D162:D164"/>
-    <mergeCell ref="F162:F164"/>
-    <mergeCell ref="G162:G164"/>
-    <mergeCell ref="D165:D167"/>
-    <mergeCell ref="F165:F167"/>
-    <mergeCell ref="G165:G167"/>
-    <mergeCell ref="D157:D159"/>
-    <mergeCell ref="F157:F159"/>
-    <mergeCell ref="G157:G159"/>
-    <mergeCell ref="D160:D161"/>
-    <mergeCell ref="F160:F161"/>
-    <mergeCell ref="G160:G161"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="G41:G43"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="D98:D100"/>
-    <mergeCell ref="D103:D104"/>
-    <mergeCell ref="D105:D106"/>
-    <mergeCell ref="D111:D113"/>
-    <mergeCell ref="D114:D115"/>
-    <mergeCell ref="G111:G113"/>
-    <mergeCell ref="D107:D108"/>
-    <mergeCell ref="D109:D110"/>
-    <mergeCell ref="G98:G100"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="G114:G115"/>
-    <mergeCell ref="F111:F113"/>
-    <mergeCell ref="E98:E100"/>
-    <mergeCell ref="E101:E102"/>
-    <mergeCell ref="E103:E104"/>
-    <mergeCell ref="E105:E106"/>
-    <mergeCell ref="E107:E108"/>
-    <mergeCell ref="E109:E110"/>
-    <mergeCell ref="E111:E113"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="G128:G129"/>
-    <mergeCell ref="G130:G131"/>
-    <mergeCell ref="G132:G133"/>
-    <mergeCell ref="F136:F137"/>
-    <mergeCell ref="G134:G135"/>
-    <mergeCell ref="D134:D135"/>
-    <mergeCell ref="D136:D137"/>
-    <mergeCell ref="D116:D117"/>
-    <mergeCell ref="F122:F123"/>
-    <mergeCell ref="F124:F125"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="F128:F129"/>
-    <mergeCell ref="F130:F131"/>
-    <mergeCell ref="F132:F133"/>
-    <mergeCell ref="F134:F135"/>
-    <mergeCell ref="G116:G117"/>
-    <mergeCell ref="F118:F121"/>
-    <mergeCell ref="G118:G121"/>
-    <mergeCell ref="G122:G123"/>
-    <mergeCell ref="G124:G125"/>
-    <mergeCell ref="G126:G127"/>
-    <mergeCell ref="E116:E117"/>
-    <mergeCell ref="E118:E121"/>
-    <mergeCell ref="E122:E123"/>
-    <mergeCell ref="D138:D140"/>
-    <mergeCell ref="F138:F140"/>
-    <mergeCell ref="G138:G140"/>
-    <mergeCell ref="D141:D143"/>
-    <mergeCell ref="F141:F143"/>
-    <mergeCell ref="G141:G143"/>
-    <mergeCell ref="F98:F100"/>
-    <mergeCell ref="F103:F104"/>
-    <mergeCell ref="G103:G104"/>
-    <mergeCell ref="F105:F106"/>
-    <mergeCell ref="G105:G106"/>
-    <mergeCell ref="F107:F108"/>
-    <mergeCell ref="G107:G108"/>
-    <mergeCell ref="F109:F110"/>
-    <mergeCell ref="G109:G110"/>
-    <mergeCell ref="D118:D121"/>
-    <mergeCell ref="D122:D123"/>
-    <mergeCell ref="D124:D125"/>
-    <mergeCell ref="D126:D127"/>
-    <mergeCell ref="D128:D129"/>
-    <mergeCell ref="D130:D131"/>
-    <mergeCell ref="D132:D133"/>
-    <mergeCell ref="G136:G137"/>
-    <mergeCell ref="F116:F117"/>
-    <mergeCell ref="E124:E125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="E128:E129"/>
-    <mergeCell ref="E130:E131"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="E134:E135"/>
-    <mergeCell ref="E136:E137"/>
-    <mergeCell ref="E138:E140"/>
-    <mergeCell ref="E141:E143"/>
-    <mergeCell ref="D195:D196"/>
-    <mergeCell ref="E195:E196"/>
-    <mergeCell ref="F195:F196"/>
-    <mergeCell ref="G195:G196"/>
-    <mergeCell ref="D197:D198"/>
-    <mergeCell ref="E197:E198"/>
-    <mergeCell ref="F197:F198"/>
-    <mergeCell ref="G197:G198"/>
-    <mergeCell ref="E144:E146"/>
-    <mergeCell ref="E147:E148"/>
-    <mergeCell ref="E149:E151"/>
-    <mergeCell ref="E152:E153"/>
-    <mergeCell ref="E154:E156"/>
-    <mergeCell ref="E157:E159"/>
-    <mergeCell ref="E160:E161"/>
-    <mergeCell ref="E162:E164"/>
-    <mergeCell ref="E165:E167"/>
-    <mergeCell ref="D152:D153"/>
-    <mergeCell ref="F152:F153"/>
-    <mergeCell ref="G152:G153"/>
-    <mergeCell ref="D154:D156"/>
-    <mergeCell ref="F154:F156"/>
-    <mergeCell ref="G154:G156"/>
-    <mergeCell ref="D147:D148"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -17924,6 +17965,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEAE28352B96D64C95AA0D5E2FA62FAD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed183881d36ac1b5d7d67982eda510d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d161086-4829-409f-9f75-5bde88dcb151" xmlns:ns3="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="685f4fda20cf913d28bf77c13cd653dd" ns2:_="" ns3:_="">
     <xsd:import namespace="3d161086-4829-409f-9f75-5bde88dcb151"/>
@@ -18146,15 +18196,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -18167,6 +18208,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C74AB5E7-5C87-4FF7-BF80-AB0EB6BD1D32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18185,27 +18234,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MLO_CETACEANS_TRACK SRID update added to release_001.sql
First version of V_MAP_UNIFIED_SECCHI_OBSERVATION done, still incomplete and not working
Frist version of V_UNIFIED_SECCHI done, still incomplete and not working
</commit_message>
<xml_diff>
--- a/analysis/MEDS_Tables.xlsx
+++ b/analysis/MEDS_Tables.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="919" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE91FA86-5292-4546-B304-E1A88F591476}"/>
+  <xr:revisionPtr revIDLastSave="943" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{37DB9835-8754-47EC-B2C6-2601E6E47759}"/>
   <bookViews>
-    <workbookView xWindow="-16005" yWindow="-21705" windowWidth="38625" windowHeight="21825" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16005" yWindow="-21705" windowWidth="38625" windowHeight="21825" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meds_tables" sheetId="1" r:id="rId1"/>
     <sheet name="csv" sheetId="6" r:id="rId2"/>
     <sheet name="tasks" sheetId="10" r:id="rId3"/>
-    <sheet name="indexes candidates" sheetId="11" r:id="rId4"/>
-    <sheet name="test cases" sheetId="12" r:id="rId5"/>
-    <sheet name="test plan" sheetId="13" r:id="rId6"/>
-    <sheet name="location" sheetId="14" r:id="rId7"/>
-    <sheet name="form" sheetId="7" r:id="rId8"/>
-    <sheet name="serd" sheetId="8" r:id="rId9"/>
-    <sheet name="output" sheetId="9" r:id="rId10"/>
-    <sheet name="enhancements" sheetId="4" r:id="rId11"/>
+    <sheet name="unified secchi" sheetId="15" r:id="rId4"/>
+    <sheet name="indexes candidates" sheetId="11" r:id="rId5"/>
+    <sheet name="test cases" sheetId="12" r:id="rId6"/>
+    <sheet name="test plan" sheetId="13" r:id="rId7"/>
+    <sheet name="location" sheetId="14" r:id="rId8"/>
+    <sheet name="form" sheetId="7" r:id="rId9"/>
+    <sheet name="serd" sheetId="8" r:id="rId10"/>
+    <sheet name="output" sheetId="9" r:id="rId11"/>
+    <sheet name="enhancements" sheetId="4" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">meds_tables!$A$1:$X$1</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3202" uniqueCount="757">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3257" uniqueCount="783">
   <si>
     <t>Table</t>
   </si>
@@ -2610,6 +2611,84 @@
   </si>
   <si>
     <t xml:space="preserve">CETACEANS </t>
+  </si>
+  <si>
+    <t>UNIFIED SECCHI DATA</t>
+  </si>
+  <si>
+    <t>ARCHIVED</t>
+  </si>
+  <si>
+    <t>CLOUD</t>
+  </si>
+  <si>
+    <t>COUNTRY_CODE</t>
+  </si>
+  <si>
+    <t>CRUISE_IDENTIFIER</t>
+  </si>
+  <si>
+    <t>DATA_TYPE</t>
+  </si>
+  <si>
+    <t>DIFFUSE_ATTN_COE</t>
+  </si>
+  <si>
+    <t>GENERAL_AREA</t>
+  </si>
+  <si>
+    <t>GMT</t>
+  </si>
+  <si>
+    <t>HORIZONTAL_VISABILITY</t>
+  </si>
+  <si>
+    <t>MEDS_JOB_NUMBER</t>
+  </si>
+  <si>
+    <t>MEDS_OBSERVATION_NUMBER</t>
+  </si>
+  <si>
+    <t>MONTH</t>
+  </si>
+  <si>
+    <t>PHOTIC_DEPTH</t>
+  </si>
+  <si>
+    <t>RECORD_NUMBER</t>
+  </si>
+  <si>
+    <t>REFERENCE</t>
+  </si>
+  <si>
+    <t>SEA_STATE</t>
+  </si>
+  <si>
+    <t>SECCHI_DEPTH</t>
+  </si>
+  <si>
+    <t>SHIP_CODE</t>
+  </si>
+  <si>
+    <t>SRC</t>
+  </si>
+  <si>
+    <t>STN_IDENTIFIER</t>
+  </si>
+  <si>
+    <t>SUN_ANGLE</t>
+  </si>
+  <si>
+    <t>WATER_COLOUR_NAME</t>
+  </si>
+  <si>
+    <t>WATER_COLOUR_H631A</t>
+  </si>
+  <si>
+    <t>WEATHER</t>
+  </si>
+  <si>
+    <t>? MEDS_CRUISE_NUMBER</t>
   </si>
 </sst>
 </file>
@@ -3347,7 +3426,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3484,35 +3563,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3521,18 +3601,19 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -11254,6 +11335,513 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A026136A-3463-4F46-9920-D2EEED3E1AFC}">
+  <dimension ref="A1:X17"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:W17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" customWidth="1"/>
+    <col min="4" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="66.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>565</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>365</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>514</v>
+      </c>
+      <c r="D2" s="16">
+        <v>101901</v>
+      </c>
+      <c r="E2" s="19"/>
+      <c r="I2" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>568</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>569</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>513</v>
+      </c>
+      <c r="D3" s="14">
+        <v>100167</v>
+      </c>
+      <c r="E3" s="20"/>
+      <c r="I3">
+        <v>5676</v>
+      </c>
+      <c r="J3" t="s">
+        <v>573</v>
+      </c>
+      <c r="K3">
+        <v>100167</v>
+      </c>
+      <c r="L3" t="s">
+        <v>576</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>5</v>
+      </c>
+      <c r="O3" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>373</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>374</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>522</v>
+      </c>
+      <c r="D4" s="16">
+        <v>102341</v>
+      </c>
+      <c r="E4" s="19"/>
+      <c r="I4">
+        <v>6830</v>
+      </c>
+      <c r="J4" t="s">
+        <v>574</v>
+      </c>
+      <c r="K4">
+        <v>101901</v>
+      </c>
+      <c r="L4" t="s">
+        <v>576</v>
+      </c>
+      <c r="M4">
+        <v>78</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+      <c r="O4" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>514</v>
+      </c>
+      <c r="D5" s="14">
+        <v>101901</v>
+      </c>
+      <c r="E5" s="20"/>
+      <c r="I5">
+        <v>7114</v>
+      </c>
+      <c r="J5" t="s">
+        <v>575</v>
+      </c>
+      <c r="K5">
+        <v>102341</v>
+      </c>
+      <c r="L5" t="s">
+        <v>576</v>
+      </c>
+      <c r="M5">
+        <v>19</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>371</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>513</v>
+      </c>
+      <c r="D6" s="16">
+        <v>100167</v>
+      </c>
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>380</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>522</v>
+      </c>
+      <c r="D7" s="14">
+        <v>102341</v>
+      </c>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>382</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>514</v>
+      </c>
+      <c r="D8" s="16">
+        <v>101901</v>
+      </c>
+      <c r="E8" s="19"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>384</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>513</v>
+      </c>
+      <c r="D9" s="14">
+        <v>100167</v>
+      </c>
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>386</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>374</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>522</v>
+      </c>
+      <c r="D10" s="16">
+        <v>102341</v>
+      </c>
+      <c r="E10" s="19"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B14" s="42"/>
+      <c r="C14" s="42">
+        <v>44358</v>
+      </c>
+      <c r="D14" t="s">
+        <v>585</v>
+      </c>
+      <c r="E14">
+        <v>102341</v>
+      </c>
+      <c r="F14">
+        <v>3628</v>
+      </c>
+      <c r="G14">
+        <v>19</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>3</v>
+      </c>
+      <c r="K14">
+        <v>131</v>
+      </c>
+      <c r="L14">
+        <v>129</v>
+      </c>
+      <c r="M14">
+        <v>145</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>75</v>
+      </c>
+      <c r="Q14">
+        <v>2021</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="T14" t="s">
+        <v>586</v>
+      </c>
+      <c r="U14">
+        <v>47.615000000000002</v>
+      </c>
+      <c r="V14">
+        <v>-5.5083000000000002</v>
+      </c>
+      <c r="W14">
+        <v>96304</v>
+      </c>
+      <c r="X14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B15" s="42"/>
+      <c r="C15" s="42">
+        <v>44358</v>
+      </c>
+      <c r="D15" t="s">
+        <v>585</v>
+      </c>
+      <c r="E15">
+        <v>102623</v>
+      </c>
+      <c r="F15">
+        <v>3372</v>
+      </c>
+      <c r="G15">
+        <v>19</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="K15">
+        <v>131</v>
+      </c>
+      <c r="L15">
+        <v>129</v>
+      </c>
+      <c r="M15">
+        <v>145</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>75</v>
+      </c>
+      <c r="Q15">
+        <v>2021</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="T15" t="s">
+        <v>586</v>
+      </c>
+      <c r="U15">
+        <v>47.615000000000002</v>
+      </c>
+      <c r="V15">
+        <v>-5.5083000000000002</v>
+      </c>
+      <c r="W15">
+        <v>97931</v>
+      </c>
+      <c r="X15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B16" s="42">
+        <v>44385</v>
+      </c>
+      <c r="C16" t="s">
+        <v>585</v>
+      </c>
+      <c r="D16">
+        <v>102341</v>
+      </c>
+      <c r="E16">
+        <v>3628</v>
+      </c>
+      <c r="F16">
+        <v>19</v>
+      </c>
+      <c r="G16">
+        <v>41</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <v>448</v>
+      </c>
+      <c r="K16">
+        <v>444</v>
+      </c>
+      <c r="L16">
+        <v>181</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>59</v>
+      </c>
+      <c r="P16">
+        <v>2021</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="S16" t="s">
+        <v>587</v>
+      </c>
+      <c r="T16">
+        <v>55.76</v>
+      </c>
+      <c r="U16">
+        <v>-9.3633000000000006</v>
+      </c>
+      <c r="V16">
+        <v>96304</v>
+      </c>
+      <c r="W16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B17" s="42">
+        <v>44385</v>
+      </c>
+      <c r="C17" t="s">
+        <v>585</v>
+      </c>
+      <c r="D17">
+        <v>102623</v>
+      </c>
+      <c r="E17">
+        <v>3372</v>
+      </c>
+      <c r="F17">
+        <v>19</v>
+      </c>
+      <c r="G17">
+        <v>41</v>
+      </c>
+      <c r="I17">
+        <v>3</v>
+      </c>
+      <c r="J17">
+        <v>448</v>
+      </c>
+      <c r="K17">
+        <v>444</v>
+      </c>
+      <c r="L17">
+        <v>181</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>59</v>
+      </c>
+      <c r="P17">
+        <v>2021</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="S17" t="s">
+        <v>587</v>
+      </c>
+      <c r="T17">
+        <v>55.76</v>
+      </c>
+      <c r="U17">
+        <v>-9.3633000000000006</v>
+      </c>
+      <c r="V17">
+        <v>97971</v>
+      </c>
+      <c r="W17">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6DDA247-F6AE-445A-B41C-F6181C9C037C}">
   <dimension ref="A1:C44"/>
   <sheetViews>
@@ -11630,7 +12218,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABE3366-981D-4444-A865-F5BA56B32FED}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -12061,7 +12649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8FA477-9B46-4053-B7AD-310B8B9F2B30}">
   <dimension ref="B1:P203"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
     </sheetView>
@@ -12114,17 +12702,17 @@
       <c r="C2" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="69" t="s">
         <v>38</v>
       </c>
       <c r="E2" s="49"/>
-      <c r="F2" s="68" t="s">
+      <c r="F2" s="71" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="68" t="s">
+      <c r="G2" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="72" t="s">
+      <c r="H2" s="73" t="s">
         <v>564</v>
       </c>
     </row>
@@ -12132,73 +12720,73 @@
       <c r="C3" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="62"/>
+      <c r="D3" s="68"/>
       <c r="E3" s="45"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="71"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="64"/>
     </row>
     <row r="4" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="62"/>
+      <c r="D4" s="68"/>
       <c r="E4" s="45"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="71"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="64"/>
     </row>
     <row r="5" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="62" t="s">
+      <c r="D5" s="68" t="s">
         <v>53</v>
       </c>
       <c r="E5" s="45"/>
-      <c r="F5" s="64" t="s">
+      <c r="F5" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="64" t="s">
+      <c r="G5" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="71" t="s">
+      <c r="H5" s="64" t="s">
         <v>519</v>
       </c>
       <c r="M5" s="36"/>
-      <c r="N5" s="76"/>
-      <c r="O5" s="64"/>
-      <c r="P5" s="75"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="65"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C6" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="62"/>
+      <c r="D6" s="68"/>
       <c r="E6" s="45"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="71"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="64"/>
       <c r="M6" s="36"/>
-      <c r="N6" s="76"/>
-      <c r="O6" s="64"/>
-      <c r="P6" s="75"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="67"/>
+      <c r="P6" s="65"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C7" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="62" t="s">
+      <c r="D7" s="68" t="s">
         <v>78</v>
       </c>
       <c r="E7" s="45"/>
-      <c r="F7" s="64" t="s">
+      <c r="F7" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G7" s="64" t="s">
+      <c r="G7" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="71" t="s">
+      <c r="H7" s="64" t="s">
         <v>80</v>
       </c>
     </row>
@@ -12206,27 +12794,27 @@
       <c r="C8" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="62"/>
+      <c r="D8" s="68"/>
       <c r="E8" s="45"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="71"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="64"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C9" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="D9" s="62" t="s">
+      <c r="D9" s="68" t="s">
         <v>171</v>
       </c>
       <c r="E9" s="45"/>
-      <c r="F9" s="64" t="s">
+      <c r="F9" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G9" s="64" t="s">
+      <c r="G9" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="H9" s="71" t="s">
+      <c r="H9" s="64" t="s">
         <v>523</v>
       </c>
     </row>
@@ -12234,37 +12822,37 @@
       <c r="C10" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="D10" s="62"/>
+      <c r="D10" s="68"/>
       <c r="E10" s="45"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="71"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="64"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C11" s="31" t="s">
         <v>176</v>
       </c>
-      <c r="D11" s="62"/>
+      <c r="D11" s="68"/>
       <c r="E11" s="45"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="71"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="64"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C12" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="D12" s="62" t="s">
+      <c r="D12" s="68" t="s">
         <v>204</v>
       </c>
       <c r="E12" s="45"/>
-      <c r="F12" s="64" t="s">
+      <c r="F12" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G12" s="64" t="s">
+      <c r="G12" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="71" t="s">
+      <c r="H12" s="64" t="s">
         <v>515</v>
       </c>
     </row>
@@ -12272,27 +12860,27 @@
       <c r="C13" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="D13" s="62"/>
+      <c r="D13" s="68"/>
       <c r="E13" s="45"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="71"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="64"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C14" s="31" t="s">
         <v>360</v>
       </c>
-      <c r="D14" s="62" t="s">
+      <c r="D14" s="68" t="s">
         <v>361</v>
       </c>
       <c r="E14" s="45"/>
-      <c r="F14" s="64" t="s">
+      <c r="F14" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G14" s="64" t="s">
+      <c r="G14" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="71" t="s">
+      <c r="H14" s="64" t="s">
         <v>518</v>
       </c>
     </row>
@@ -12300,27 +12888,27 @@
       <c r="C15" s="32" t="s">
         <v>363</v>
       </c>
-      <c r="D15" s="65"/>
+      <c r="D15" s="70"/>
       <c r="E15" s="50"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="73"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="74"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C16" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="70" t="s">
+      <c r="D16" s="69" t="s">
         <v>71</v>
       </c>
       <c r="E16" s="49"/>
-      <c r="F16" s="68" t="s">
+      <c r="F16" s="71" t="s">
         <v>81</v>
       </c>
-      <c r="G16" s="68" t="s">
+      <c r="G16" s="71" t="s">
         <v>567</v>
       </c>
-      <c r="H16" s="72" t="s">
+      <c r="H16" s="73" t="s">
         <v>73</v>
       </c>
     </row>
@@ -12328,27 +12916,27 @@
       <c r="C17" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="62"/>
+      <c r="D17" s="68"/>
       <c r="E17" s="45"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="71"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="64"/>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C18" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="62" t="s">
+      <c r="D18" s="68" t="s">
         <v>105</v>
       </c>
       <c r="E18" s="45"/>
-      <c r="F18" s="64" t="s">
+      <c r="F18" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G18" s="64" t="s">
+      <c r="G18" s="67" t="s">
         <v>567</v>
       </c>
-      <c r="H18" s="71" t="s">
+      <c r="H18" s="64" t="s">
         <v>524</v>
       </c>
     </row>
@@ -12356,27 +12944,27 @@
       <c r="C19" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="62"/>
+      <c r="D19" s="68"/>
       <c r="E19" s="45"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="64"/>
-      <c r="H19" s="71"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="64"/>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C20" s="31" t="s">
         <v>299</v>
       </c>
-      <c r="D20" s="62" t="s">
+      <c r="D20" s="68" t="s">
         <v>300</v>
       </c>
       <c r="E20" s="45"/>
-      <c r="F20" s="64" t="s">
+      <c r="F20" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G20" s="64" t="s">
+      <c r="G20" s="67" t="s">
         <v>567</v>
       </c>
-      <c r="H20" s="71" t="s">
+      <c r="H20" s="64" t="s">
         <v>516</v>
       </c>
     </row>
@@ -12384,27 +12972,27 @@
       <c r="C21" s="31" t="s">
         <v>302</v>
       </c>
-      <c r="D21" s="62"/>
+      <c r="D21" s="68"/>
       <c r="E21" s="45"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="71"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="64"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C22" s="31" t="s">
         <v>304</v>
       </c>
-      <c r="D22" s="62" t="s">
+      <c r="D22" s="68" t="s">
         <v>305</v>
       </c>
       <c r="E22" s="45"/>
-      <c r="F22" s="64" t="s">
+      <c r="F22" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G22" s="64" t="s">
+      <c r="G22" s="67" t="s">
         <v>567</v>
       </c>
-      <c r="H22" s="71" t="s">
+      <c r="H22" s="64" t="s">
         <v>521</v>
       </c>
     </row>
@@ -12412,11 +13000,11 @@
       <c r="C23" s="31" t="s">
         <v>309</v>
       </c>
-      <c r="D23" s="62"/>
+      <c r="D23" s="68"/>
       <c r="E23" s="45"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="71"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="64"/>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C24" s="31" t="s">
@@ -12432,7 +13020,7 @@
       <c r="G24" s="60" t="s">
         <v>567</v>
       </c>
-      <c r="H24" s="77" t="s">
+      <c r="H24" s="62" t="s">
         <v>521</v>
       </c>
     </row>
@@ -12440,17 +13028,17 @@
       <c r="C25" s="31" t="s">
         <v>317</v>
       </c>
-      <c r="D25" s="62" t="s">
+      <c r="D25" s="68" t="s">
         <v>318</v>
       </c>
       <c r="E25" s="45"/>
-      <c r="F25" s="64" t="s">
+      <c r="F25" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G25" s="64" t="s">
+      <c r="G25" s="67" t="s">
         <v>567</v>
       </c>
-      <c r="H25" s="71" t="s">
+      <c r="H25" s="64" t="s">
         <v>512</v>
       </c>
     </row>
@@ -12458,27 +13046,27 @@
       <c r="C26" s="31" t="s">
         <v>320</v>
       </c>
-      <c r="D26" s="62"/>
+      <c r="D26" s="68"/>
       <c r="E26" s="45"/>
-      <c r="F26" s="64"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="71"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="64"/>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C27" s="31" t="s">
         <v>322</v>
       </c>
-      <c r="D27" s="69" t="s">
+      <c r="D27" s="75" t="s">
         <v>323</v>
       </c>
       <c r="E27" s="48"/>
-      <c r="F27" s="74" t="s">
+      <c r="F27" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="G27" s="64" t="s">
+      <c r="G27" s="67" t="s">
         <v>567</v>
       </c>
-      <c r="H27" s="71" t="s">
+      <c r="H27" s="64" t="s">
         <v>517</v>
       </c>
     </row>
@@ -12486,27 +13074,27 @@
       <c r="C28" s="31" t="s">
         <v>325</v>
       </c>
-      <c r="D28" s="69"/>
+      <c r="D28" s="75"/>
       <c r="E28" s="48"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="71"/>
+      <c r="F28" s="76"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="64"/>
     </row>
     <row r="29" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C29" s="31" t="s">
         <v>327</v>
       </c>
-      <c r="D29" s="62" t="s">
+      <c r="D29" s="68" t="s">
         <v>328</v>
       </c>
       <c r="E29" s="45"/>
-      <c r="F29" s="64" t="s">
+      <c r="F29" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G29" s="64" t="s">
+      <c r="G29" s="67" t="s">
         <v>567</v>
       </c>
-      <c r="H29" s="71" t="s">
+      <c r="H29" s="64" t="s">
         <v>508</v>
       </c>
     </row>
@@ -12514,27 +13102,27 @@
       <c r="C30" s="31" t="s">
         <v>330</v>
       </c>
-      <c r="D30" s="62"/>
+      <c r="D30" s="68"/>
       <c r="E30" s="45"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="71"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="64"/>
     </row>
     <row r="31" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C31" s="31" t="s">
         <v>332</v>
       </c>
-      <c r="D31" s="62" t="s">
+      <c r="D31" s="68" t="s">
         <v>333</v>
       </c>
       <c r="E31" s="45"/>
-      <c r="F31" s="64" t="s">
+      <c r="F31" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G31" s="64" t="s">
+      <c r="G31" s="67" t="s">
         <v>567</v>
       </c>
-      <c r="H31" s="71" t="s">
+      <c r="H31" s="64" t="s">
         <v>510</v>
       </c>
     </row>
@@ -12542,27 +13130,27 @@
       <c r="C32" s="31" t="s">
         <v>335</v>
       </c>
-      <c r="D32" s="62"/>
+      <c r="D32" s="68"/>
       <c r="E32" s="45"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="71"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="64"/>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C33" s="31" t="s">
         <v>337</v>
       </c>
-      <c r="D33" s="62" t="s">
+      <c r="D33" s="68" t="s">
         <v>338</v>
       </c>
       <c r="E33" s="45"/>
-      <c r="F33" s="64" t="s">
+      <c r="F33" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G33" s="64" t="s">
+      <c r="G33" s="67" t="s">
         <v>567</v>
       </c>
-      <c r="H33" s="71" t="s">
+      <c r="H33" s="64" t="s">
         <v>511</v>
       </c>
     </row>
@@ -12570,27 +13158,27 @@
       <c r="C34" s="31" t="s">
         <v>340</v>
       </c>
-      <c r="D34" s="62"/>
+      <c r="D34" s="68"/>
       <c r="E34" s="45"/>
-      <c r="F34" s="64"/>
-      <c r="G34" s="64"/>
-      <c r="H34" s="71"/>
+      <c r="F34" s="67"/>
+      <c r="G34" s="67"/>
+      <c r="H34" s="64"/>
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C35" s="31" t="s">
         <v>342</v>
       </c>
-      <c r="D35" s="62" t="s">
+      <c r="D35" s="68" t="s">
         <v>343</v>
       </c>
       <c r="E35" s="45"/>
-      <c r="F35" s="64" t="s">
+      <c r="F35" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G35" s="64" t="s">
+      <c r="G35" s="67" t="s">
         <v>567</v>
       </c>
-      <c r="H35" s="71" t="s">
+      <c r="H35" s="64" t="s">
         <v>509</v>
       </c>
     </row>
@@ -12598,27 +13186,27 @@
       <c r="C36" s="31" t="s">
         <v>345</v>
       </c>
-      <c r="D36" s="62"/>
+      <c r="D36" s="68"/>
       <c r="E36" s="45"/>
-      <c r="F36" s="64"/>
-      <c r="G36" s="64"/>
-      <c r="H36" s="71"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="67"/>
+      <c r="H36" s="64"/>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C37" s="31" t="s">
         <v>347</v>
       </c>
-      <c r="D37" s="62" t="s">
+      <c r="D37" s="68" t="s">
         <v>348</v>
       </c>
       <c r="E37" s="45"/>
-      <c r="F37" s="64" t="s">
+      <c r="F37" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G37" s="64" t="s">
+      <c r="G37" s="67" t="s">
         <v>567</v>
       </c>
-      <c r="H37" s="71" t="s">
+      <c r="H37" s="64" t="s">
         <v>520</v>
       </c>
     </row>
@@ -12626,27 +13214,27 @@
       <c r="C38" s="32" t="s">
         <v>350</v>
       </c>
-      <c r="D38" s="65"/>
+      <c r="D38" s="70"/>
       <c r="E38" s="50"/>
-      <c r="F38" s="67"/>
-      <c r="G38" s="67"/>
-      <c r="H38" s="73"/>
+      <c r="F38" s="72"/>
+      <c r="G38" s="72"/>
+      <c r="H38" s="74"/>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C39" s="30" t="s">
         <v>365</v>
       </c>
-      <c r="D39" s="70" t="s">
+      <c r="D39" s="69" t="s">
         <v>366</v>
       </c>
       <c r="E39" s="49"/>
-      <c r="F39" s="68" t="s">
+      <c r="F39" s="71" t="s">
         <v>81</v>
       </c>
-      <c r="G39" s="68" t="s">
+      <c r="G39" s="71" t="s">
         <v>369</v>
       </c>
-      <c r="H39" s="72" t="s">
+      <c r="H39" s="73" t="s">
         <v>514</v>
       </c>
     </row>
@@ -12654,37 +13242,37 @@
       <c r="C40" s="31" t="s">
         <v>376</v>
       </c>
-      <c r="D40" s="62"/>
+      <c r="D40" s="68"/>
       <c r="E40" s="45"/>
-      <c r="F40" s="64"/>
-      <c r="G40" s="64"/>
-      <c r="H40" s="71"/>
+      <c r="F40" s="67"/>
+      <c r="G40" s="67"/>
+      <c r="H40" s="64"/>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C41" s="31" t="s">
         <v>382</v>
       </c>
-      <c r="D41" s="62"/>
+      <c r="D41" s="68"/>
       <c r="E41" s="45"/>
-      <c r="F41" s="64"/>
-      <c r="G41" s="64"/>
-      <c r="H41" s="71"/>
+      <c r="F41" s="67"/>
+      <c r="G41" s="67"/>
+      <c r="H41" s="64"/>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C42" s="31" t="s">
         <v>370</v>
       </c>
-      <c r="D42" s="62" t="s">
+      <c r="D42" s="68" t="s">
         <v>371</v>
       </c>
       <c r="E42" s="45"/>
-      <c r="F42" s="64" t="s">
+      <c r="F42" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G42" s="64" t="s">
+      <c r="G42" s="67" t="s">
         <v>369</v>
       </c>
-      <c r="H42" s="71" t="s">
+      <c r="H42" s="64" t="s">
         <v>513</v>
       </c>
     </row>
@@ -12692,37 +13280,37 @@
       <c r="C43" s="31" t="s">
         <v>378</v>
       </c>
-      <c r="D43" s="62"/>
+      <c r="D43" s="68"/>
       <c r="E43" s="45"/>
-      <c r="F43" s="64"/>
-      <c r="G43" s="64"/>
-      <c r="H43" s="71"/>
+      <c r="F43" s="67"/>
+      <c r="G43" s="67"/>
+      <c r="H43" s="64"/>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C44" s="31" t="s">
         <v>384</v>
       </c>
-      <c r="D44" s="62"/>
+      <c r="D44" s="68"/>
       <c r="E44" s="45"/>
-      <c r="F44" s="64"/>
-      <c r="G44" s="64"/>
-      <c r="H44" s="71"/>
+      <c r="F44" s="67"/>
+      <c r="G44" s="67"/>
+      <c r="H44" s="64"/>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C45" s="31" t="s">
         <v>373</v>
       </c>
-      <c r="D45" s="62" t="s">
+      <c r="D45" s="68" t="s">
         <v>374</v>
       </c>
       <c r="E45" s="45"/>
-      <c r="F45" s="64" t="s">
+      <c r="F45" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G45" s="64" t="s">
+      <c r="G45" s="67" t="s">
         <v>369</v>
       </c>
-      <c r="H45" s="71" t="s">
+      <c r="H45" s="64" t="s">
         <v>522</v>
       </c>
     </row>
@@ -12730,35 +13318,35 @@
       <c r="C46" s="31" t="s">
         <v>380</v>
       </c>
-      <c r="D46" s="62"/>
+      <c r="D46" s="68"/>
       <c r="E46" s="45"/>
-      <c r="F46" s="64"/>
-      <c r="G46" s="64"/>
-      <c r="H46" s="71"/>
+      <c r="F46" s="67"/>
+      <c r="G46" s="67"/>
+      <c r="H46" s="64"/>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C47" s="31" t="s">
         <v>386</v>
       </c>
-      <c r="D47" s="62"/>
+      <c r="D47" s="68"/>
       <c r="E47" s="45"/>
-      <c r="F47" s="64"/>
-      <c r="G47" s="64"/>
-      <c r="H47" s="71"/>
+      <c r="F47" s="67"/>
+      <c r="G47" s="67"/>
+      <c r="H47" s="64"/>
     </row>
     <row r="48" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C48" s="30" t="s">
         <v>464</v>
       </c>
-      <c r="D48" s="70" t="s">
+      <c r="D48" s="69" t="s">
         <v>465</v>
       </c>
       <c r="E48" s="49"/>
-      <c r="F48" s="68"/>
-      <c r="G48" s="68" t="s">
+      <c r="F48" s="71"/>
+      <c r="G48" s="71" t="s">
         <v>583</v>
       </c>
-      <c r="H48" s="72" t="s">
+      <c r="H48" s="73" t="s">
         <v>584</v>
       </c>
     </row>
@@ -12766,11 +13354,11 @@
       <c r="C49" s="32" t="s">
         <v>467</v>
       </c>
-      <c r="D49" s="65"/>
+      <c r="D49" s="70"/>
       <c r="E49" s="50"/>
-      <c r="F49" s="67"/>
-      <c r="G49" s="67"/>
-      <c r="H49" s="73"/>
+      <c r="F49" s="72"/>
+      <c r="G49" s="72"/>
+      <c r="H49" s="74"/>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C50" s="31" t="s">
@@ -12901,7 +13489,7 @@
       </c>
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C58" s="78" t="s">
+      <c r="C58" s="63" t="s">
         <v>755</v>
       </c>
       <c r="D58" s="61"/>
@@ -13568,16 +14156,16 @@
       <c r="C100" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="D100" s="70" t="s">
+      <c r="D100" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="E100" s="68">
+      <c r="E100" s="71">
         <v>1</v>
       </c>
-      <c r="F100" s="68" t="s">
+      <c r="F100" s="71" t="s">
         <v>81</v>
       </c>
-      <c r="G100" s="68" t="s">
+      <c r="G100" s="71" t="s">
         <v>18</v>
       </c>
       <c r="H100" s="52"/>
@@ -13586,10 +14174,10 @@
       <c r="C101" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="D101" s="62"/>
-      <c r="E101" s="64"/>
-      <c r="F101" s="64"/>
-      <c r="G101" s="64"/>
+      <c r="D101" s="68"/>
+      <c r="E101" s="67"/>
+      <c r="F101" s="67"/>
+      <c r="G101" s="67"/>
       <c r="H101" s="56" t="s">
         <v>33</v>
       </c>
@@ -13598,10 +14186,10 @@
       <c r="C102" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="D102" s="62"/>
-      <c r="E102" s="64"/>
-      <c r="F102" s="64"/>
-      <c r="G102" s="64"/>
+      <c r="D102" s="68"/>
+      <c r="E102" s="67"/>
+      <c r="F102" s="67"/>
+      <c r="G102" s="67"/>
       <c r="H102" s="56" t="s">
         <v>33</v>
       </c>
@@ -13610,19 +14198,19 @@
       <c r="C103" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="D103" s="62" t="s">
+      <c r="D103" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="E103" s="64">
+      <c r="E103" s="67">
         <v>1</v>
       </c>
-      <c r="F103" s="64" t="s">
+      <c r="F103" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G103" s="64" t="s">
+      <c r="G103" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="H103" s="71" t="s">
+      <c r="H103" s="64" t="s">
         <v>753</v>
       </c>
     </row>
@@ -13630,26 +14218,26 @@
       <c r="C104" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="D104" s="62"/>
-      <c r="E104" s="64"/>
-      <c r="F104" s="64"/>
-      <c r="G104" s="64"/>
-      <c r="H104" s="71"/>
+      <c r="D104" s="68"/>
+      <c r="E104" s="67"/>
+      <c r="F104" s="67"/>
+      <c r="G104" s="67"/>
+      <c r="H104" s="64"/>
     </row>
     <row r="105" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C105" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="D105" s="62" t="s">
+      <c r="D105" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="E105" s="64">
+      <c r="E105" s="67">
         <v>1</v>
       </c>
-      <c r="F105" s="64" t="s">
+      <c r="F105" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G105" s="64" t="s">
+      <c r="G105" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H105" s="56" t="s">
@@ -13660,10 +14248,10 @@
       <c r="C106" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="D106" s="62"/>
-      <c r="E106" s="64"/>
-      <c r="F106" s="64"/>
-      <c r="G106" s="64"/>
+      <c r="D106" s="68"/>
+      <c r="E106" s="67"/>
+      <c r="F106" s="67"/>
+      <c r="G106" s="67"/>
       <c r="H106" s="56" t="s">
         <v>33</v>
       </c>
@@ -13672,16 +14260,16 @@
       <c r="C107" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="D107" s="62" t="s">
+      <c r="D107" s="68" t="s">
         <v>78</v>
       </c>
-      <c r="E107" s="64">
+      <c r="E107" s="67">
         <v>1</v>
       </c>
-      <c r="F107" s="64" t="s">
+      <c r="F107" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G107" s="64" t="s">
+      <c r="G107" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H107" s="56" t="s">
@@ -13692,10 +14280,10 @@
       <c r="C108" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="D108" s="62"/>
-      <c r="E108" s="64"/>
-      <c r="F108" s="64"/>
-      <c r="G108" s="64"/>
+      <c r="D108" s="68"/>
+      <c r="E108" s="67"/>
+      <c r="F108" s="67"/>
+      <c r="G108" s="67"/>
       <c r="H108" s="56" t="s">
         <v>33</v>
       </c>
@@ -13704,16 +14292,16 @@
       <c r="C109" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="D109" s="62" t="s">
+      <c r="D109" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="E109" s="64">
+      <c r="E109" s="67">
         <v>1</v>
       </c>
-      <c r="F109" s="64" t="s">
+      <c r="F109" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G109" s="64" t="s">
+      <c r="G109" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H109" s="56" t="s">
@@ -13724,10 +14312,10 @@
       <c r="C110" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="D110" s="62"/>
-      <c r="E110" s="64"/>
-      <c r="F110" s="64"/>
-      <c r="G110" s="64"/>
+      <c r="D110" s="68"/>
+      <c r="E110" s="67"/>
+      <c r="F110" s="67"/>
+      <c r="G110" s="67"/>
       <c r="H110" s="56" t="s">
         <v>33</v>
       </c>
@@ -13736,16 +14324,16 @@
       <c r="C111" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="D111" s="62" t="s">
+      <c r="D111" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="E111" s="64">
+      <c r="E111" s="67">
         <v>1</v>
       </c>
-      <c r="F111" s="64" t="s">
+      <c r="F111" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G111" s="64" t="s">
+      <c r="G111" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H111" s="56" t="s">
@@ -13756,10 +14344,10 @@
       <c r="C112" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="D112" s="62"/>
-      <c r="E112" s="64"/>
-      <c r="F112" s="64"/>
-      <c r="G112" s="64"/>
+      <c r="D112" s="68"/>
+      <c r="E112" s="67"/>
+      <c r="F112" s="67"/>
+      <c r="G112" s="67"/>
       <c r="H112" s="56" t="s">
         <v>33</v>
       </c>
@@ -13768,16 +14356,16 @@
       <c r="C113" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="D113" s="62" t="s">
+      <c r="D113" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="E113" s="64">
+      <c r="E113" s="67">
         <v>3</v>
       </c>
-      <c r="F113" s="64" t="s">
+      <c r="F113" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G113" s="64" t="s">
+      <c r="G113" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H113" s="56" t="s">
@@ -13788,10 +14376,10 @@
       <c r="C114" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="D114" s="62"/>
-      <c r="E114" s="64"/>
-      <c r="F114" s="64"/>
-      <c r="G114" s="64"/>
+      <c r="D114" s="68"/>
+      <c r="E114" s="67"/>
+      <c r="F114" s="67"/>
+      <c r="G114" s="67"/>
       <c r="H114" s="56" t="s">
         <v>33</v>
       </c>
@@ -13800,10 +14388,10 @@
       <c r="C115" s="31" t="s">
         <v>176</v>
       </c>
-      <c r="D115" s="62"/>
-      <c r="E115" s="64"/>
-      <c r="F115" s="64"/>
-      <c r="G115" s="64"/>
+      <c r="D115" s="68"/>
+      <c r="E115" s="67"/>
+      <c r="F115" s="67"/>
+      <c r="G115" s="67"/>
       <c r="H115" s="56" t="s">
         <v>33</v>
       </c>
@@ -13812,16 +14400,16 @@
       <c r="C116" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="D116" s="62" t="s">
+      <c r="D116" s="68" t="s">
         <v>204</v>
       </c>
-      <c r="E116" s="64">
+      <c r="E116" s="67">
         <v>3</v>
       </c>
-      <c r="F116" s="64" t="s">
+      <c r="F116" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G116" s="64" t="s">
+      <c r="G116" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H116" s="56" t="s">
@@ -13832,10 +14420,10 @@
       <c r="C117" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="D117" s="62"/>
-      <c r="E117" s="64"/>
-      <c r="F117" s="64"/>
-      <c r="G117" s="64"/>
+      <c r="D117" s="68"/>
+      <c r="E117" s="67"/>
+      <c r="F117" s="67"/>
+      <c r="G117" s="67"/>
       <c r="H117" s="56" t="s">
         <v>33</v>
       </c>
@@ -13844,16 +14432,16 @@
       <c r="C118" s="31" t="s">
         <v>299</v>
       </c>
-      <c r="D118" s="62" t="s">
+      <c r="D118" s="68" t="s">
         <v>300</v>
       </c>
-      <c r="E118" s="64">
+      <c r="E118" s="67">
         <v>1</v>
       </c>
-      <c r="F118" s="64" t="s">
+      <c r="F118" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G118" s="64" t="s">
+      <c r="G118" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H118" s="56" t="s">
@@ -13864,10 +14452,10 @@
       <c r="C119" s="31" t="s">
         <v>302</v>
       </c>
-      <c r="D119" s="62"/>
-      <c r="E119" s="64"/>
-      <c r="F119" s="64"/>
-      <c r="G119" s="64"/>
+      <c r="D119" s="68"/>
+      <c r="E119" s="67"/>
+      <c r="F119" s="67"/>
+      <c r="G119" s="67"/>
       <c r="H119" s="56" t="s">
         <v>33</v>
       </c>
@@ -13876,16 +14464,16 @@
       <c r="C120" s="31" t="s">
         <v>304</v>
       </c>
-      <c r="D120" s="62" t="s">
+      <c r="D120" s="68" t="s">
         <v>305</v>
       </c>
-      <c r="E120" s="64">
+      <c r="E120" s="67">
         <v>1</v>
       </c>
-      <c r="F120" s="64" t="s">
+      <c r="F120" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G120" s="64" t="s">
+      <c r="G120" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H120" s="56" t="s">
@@ -13896,10 +14484,10 @@
       <c r="C121" s="31" t="s">
         <v>309</v>
       </c>
-      <c r="D121" s="62"/>
-      <c r="E121" s="64"/>
-      <c r="F121" s="64"/>
-      <c r="G121" s="64"/>
+      <c r="D121" s="68"/>
+      <c r="E121" s="67"/>
+      <c r="F121" s="67"/>
+      <c r="G121" s="67"/>
       <c r="H121" s="56" t="s">
         <v>33</v>
       </c>
@@ -13908,10 +14496,10 @@
       <c r="C122" s="31" t="s">
         <v>307</v>
       </c>
-      <c r="D122" s="62"/>
-      <c r="E122" s="64"/>
-      <c r="F122" s="64"/>
-      <c r="G122" s="64"/>
+      <c r="D122" s="68"/>
+      <c r="E122" s="67"/>
+      <c r="F122" s="67"/>
+      <c r="G122" s="67"/>
       <c r="H122" s="56" t="s">
         <v>33</v>
       </c>
@@ -13920,10 +14508,10 @@
       <c r="C123" s="31" t="s">
         <v>311</v>
       </c>
-      <c r="D123" s="62"/>
-      <c r="E123" s="64"/>
-      <c r="F123" s="64"/>
-      <c r="G123" s="64"/>
+      <c r="D123" s="68"/>
+      <c r="E123" s="67"/>
+      <c r="F123" s="67"/>
+      <c r="G123" s="67"/>
       <c r="H123" s="56" t="s">
         <v>33</v>
       </c>
@@ -13932,16 +14520,16 @@
       <c r="C124" s="31" t="s">
         <v>317</v>
       </c>
-      <c r="D124" s="62" t="s">
+      <c r="D124" s="68" t="s">
         <v>318</v>
       </c>
-      <c r="E124" s="64">
+      <c r="E124" s="67">
         <v>1</v>
       </c>
-      <c r="F124" s="64" t="s">
+      <c r="F124" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G124" s="64" t="s">
+      <c r="G124" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H124" s="56" t="s">
@@ -13952,10 +14540,10 @@
       <c r="C125" s="31" t="s">
         <v>320</v>
       </c>
-      <c r="D125" s="62"/>
-      <c r="E125" s="64"/>
-      <c r="F125" s="64"/>
-      <c r="G125" s="64"/>
+      <c r="D125" s="68"/>
+      <c r="E125" s="67"/>
+      <c r="F125" s="67"/>
+      <c r="G125" s="67"/>
       <c r="H125" s="56" t="s">
         <v>33</v>
       </c>
@@ -13964,16 +14552,16 @@
       <c r="C126" s="31" t="s">
         <v>322</v>
       </c>
-      <c r="D126" s="69" t="s">
+      <c r="D126" s="75" t="s">
         <v>323</v>
       </c>
-      <c r="E126" s="64">
+      <c r="E126" s="67">
         <v>1</v>
       </c>
-      <c r="F126" s="64" t="s">
+      <c r="F126" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G126" s="64" t="s">
+      <c r="G126" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H126" s="56" t="s">
@@ -13984,10 +14572,10 @@
       <c r="C127" s="31" t="s">
         <v>325</v>
       </c>
-      <c r="D127" s="69"/>
-      <c r="E127" s="64"/>
-      <c r="F127" s="64"/>
-      <c r="G127" s="64"/>
+      <c r="D127" s="75"/>
+      <c r="E127" s="67"/>
+      <c r="F127" s="67"/>
+      <c r="G127" s="67"/>
       <c r="H127" s="56" t="s">
         <v>33</v>
       </c>
@@ -13996,16 +14584,16 @@
       <c r="C128" s="31" t="s">
         <v>327</v>
       </c>
-      <c r="D128" s="62" t="s">
+      <c r="D128" s="68" t="s">
         <v>328</v>
       </c>
-      <c r="E128" s="64">
+      <c r="E128" s="67">
         <v>1</v>
       </c>
-      <c r="F128" s="64" t="s">
+      <c r="F128" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G128" s="64" t="s">
+      <c r="G128" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H128" s="56" t="s">
@@ -14016,10 +14604,10 @@
       <c r="C129" s="31" t="s">
         <v>330</v>
       </c>
-      <c r="D129" s="62"/>
-      <c r="E129" s="64"/>
-      <c r="F129" s="64"/>
-      <c r="G129" s="64"/>
+      <c r="D129" s="68"/>
+      <c r="E129" s="67"/>
+      <c r="F129" s="67"/>
+      <c r="G129" s="67"/>
       <c r="H129" s="56" t="s">
         <v>33</v>
       </c>
@@ -14028,16 +14616,16 @@
       <c r="C130" s="31" t="s">
         <v>332</v>
       </c>
-      <c r="D130" s="62" t="s">
+      <c r="D130" s="68" t="s">
         <v>333</v>
       </c>
-      <c r="E130" s="64">
+      <c r="E130" s="67">
         <v>1</v>
       </c>
-      <c r="F130" s="64" t="s">
+      <c r="F130" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G130" s="64" t="s">
+      <c r="G130" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H130" s="56" t="s">
@@ -14048,10 +14636,10 @@
       <c r="C131" s="31" t="s">
         <v>335</v>
       </c>
-      <c r="D131" s="62"/>
-      <c r="E131" s="64"/>
-      <c r="F131" s="64"/>
-      <c r="G131" s="64"/>
+      <c r="D131" s="68"/>
+      <c r="E131" s="67"/>
+      <c r="F131" s="67"/>
+      <c r="G131" s="67"/>
       <c r="H131" s="56" t="s">
         <v>33</v>
       </c>
@@ -14060,16 +14648,16 @@
       <c r="C132" s="31" t="s">
         <v>337</v>
       </c>
-      <c r="D132" s="62" t="s">
+      <c r="D132" s="68" t="s">
         <v>338</v>
       </c>
-      <c r="E132" s="64">
+      <c r="E132" s="67">
         <v>1</v>
       </c>
-      <c r="F132" s="64" t="s">
+      <c r="F132" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G132" s="64" t="s">
+      <c r="G132" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H132" s="56" t="s">
@@ -14080,10 +14668,10 @@
       <c r="C133" s="31" t="s">
         <v>340</v>
       </c>
-      <c r="D133" s="62"/>
-      <c r="E133" s="64"/>
-      <c r="F133" s="64"/>
-      <c r="G133" s="64"/>
+      <c r="D133" s="68"/>
+      <c r="E133" s="67"/>
+      <c r="F133" s="67"/>
+      <c r="G133" s="67"/>
       <c r="H133" s="56" t="s">
         <v>33</v>
       </c>
@@ -14092,16 +14680,16 @@
       <c r="C134" s="31" t="s">
         <v>342</v>
       </c>
-      <c r="D134" s="62" t="s">
+      <c r="D134" s="68" t="s">
         <v>343</v>
       </c>
-      <c r="E134" s="64">
+      <c r="E134" s="67">
         <v>1</v>
       </c>
-      <c r="F134" s="64" t="s">
+      <c r="F134" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G134" s="64" t="s">
+      <c r="G134" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H134" s="56" t="s">
@@ -14112,10 +14700,10 @@
       <c r="C135" s="31" t="s">
         <v>345</v>
       </c>
-      <c r="D135" s="62"/>
-      <c r="E135" s="64"/>
-      <c r="F135" s="64"/>
-      <c r="G135" s="64"/>
+      <c r="D135" s="68"/>
+      <c r="E135" s="67"/>
+      <c r="F135" s="67"/>
+      <c r="G135" s="67"/>
       <c r="H135" s="56" t="s">
         <v>33</v>
       </c>
@@ -14124,16 +14712,16 @@
       <c r="C136" s="31" t="s">
         <v>347</v>
       </c>
-      <c r="D136" s="62" t="s">
+      <c r="D136" s="68" t="s">
         <v>348</v>
       </c>
-      <c r="E136" s="64">
+      <c r="E136" s="67">
         <v>1</v>
       </c>
-      <c r="F136" s="64" t="s">
+      <c r="F136" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G136" s="64" t="s">
+      <c r="G136" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H136" s="56" t="s">
@@ -14144,10 +14732,10 @@
       <c r="C137" s="31" t="s">
         <v>350</v>
       </c>
-      <c r="D137" s="62"/>
-      <c r="E137" s="64"/>
-      <c r="F137" s="64"/>
-      <c r="G137" s="64"/>
+      <c r="D137" s="68"/>
+      <c r="E137" s="67"/>
+      <c r="F137" s="67"/>
+      <c r="G137" s="67"/>
       <c r="H137" s="56" t="s">
         <v>33</v>
       </c>
@@ -14156,16 +14744,16 @@
       <c r="C138" s="31" t="s">
         <v>360</v>
       </c>
-      <c r="D138" s="62" t="s">
+      <c r="D138" s="68" t="s">
         <v>361</v>
       </c>
-      <c r="E138" s="64">
+      <c r="E138" s="67">
         <v>2</v>
       </c>
-      <c r="F138" s="64" t="s">
+      <c r="F138" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G138" s="64" t="s">
+      <c r="G138" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H138" s="56" t="s">
@@ -14176,10 +14764,10 @@
       <c r="C139" s="31" t="s">
         <v>363</v>
       </c>
-      <c r="D139" s="62"/>
-      <c r="E139" s="64"/>
-      <c r="F139" s="64"/>
-      <c r="G139" s="64"/>
+      <c r="D139" s="68"/>
+      <c r="E139" s="67"/>
+      <c r="F139" s="67"/>
+      <c r="G139" s="67"/>
       <c r="H139" s="56" t="s">
         <v>33</v>
       </c>
@@ -14188,14 +14776,14 @@
       <c r="C140" s="31" t="s">
         <v>365</v>
       </c>
-      <c r="D140" s="62" t="s">
+      <c r="D140" s="68" t="s">
         <v>366</v>
       </c>
-      <c r="E140" s="64">
+      <c r="E140" s="67">
         <v>1</v>
       </c>
-      <c r="F140" s="64"/>
-      <c r="G140" s="64" t="s">
+      <c r="F140" s="67"/>
+      <c r="G140" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H140" s="56" t="s">
@@ -14206,10 +14794,10 @@
       <c r="C141" s="31" t="s">
         <v>376</v>
       </c>
-      <c r="D141" s="62"/>
-      <c r="E141" s="64"/>
-      <c r="F141" s="64"/>
-      <c r="G141" s="64"/>
+      <c r="D141" s="68"/>
+      <c r="E141" s="67"/>
+      <c r="F141" s="67"/>
+      <c r="G141" s="67"/>
       <c r="H141" s="56" t="s">
         <v>33</v>
       </c>
@@ -14218,10 +14806,10 @@
       <c r="C142" s="31" t="s">
         <v>382</v>
       </c>
-      <c r="D142" s="62"/>
-      <c r="E142" s="64"/>
-      <c r="F142" s="64"/>
-      <c r="G142" s="64"/>
+      <c r="D142" s="68"/>
+      <c r="E142" s="67"/>
+      <c r="F142" s="67"/>
+      <c r="G142" s="67"/>
       <c r="H142" s="56" t="s">
         <v>33</v>
       </c>
@@ -14230,14 +14818,14 @@
       <c r="C143" s="31" t="s">
         <v>370</v>
       </c>
-      <c r="D143" s="62" t="s">
+      <c r="D143" s="68" t="s">
         <v>371</v>
       </c>
-      <c r="E143" s="64">
+      <c r="E143" s="67">
         <v>1</v>
       </c>
-      <c r="F143" s="64"/>
-      <c r="G143" s="64" t="s">
+      <c r="F143" s="67"/>
+      <c r="G143" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H143" s="56" t="s">
@@ -14248,10 +14836,10 @@
       <c r="C144" s="31" t="s">
         <v>378</v>
       </c>
-      <c r="D144" s="62"/>
-      <c r="E144" s="64"/>
-      <c r="F144" s="64"/>
-      <c r="G144" s="64"/>
+      <c r="D144" s="68"/>
+      <c r="E144" s="67"/>
+      <c r="F144" s="67"/>
+      <c r="G144" s="67"/>
       <c r="H144" s="56" t="s">
         <v>33</v>
       </c>
@@ -14260,10 +14848,10 @@
       <c r="C145" s="31" t="s">
         <v>384</v>
       </c>
-      <c r="D145" s="62"/>
-      <c r="E145" s="64"/>
-      <c r="F145" s="64"/>
-      <c r="G145" s="64"/>
+      <c r="D145" s="68"/>
+      <c r="E145" s="67"/>
+      <c r="F145" s="67"/>
+      <c r="G145" s="67"/>
       <c r="H145" s="56" t="s">
         <v>33</v>
       </c>
@@ -14273,14 +14861,14 @@
       <c r="C146" s="31" t="s">
         <v>373</v>
       </c>
-      <c r="D146" s="62" t="s">
+      <c r="D146" s="68" t="s">
         <v>374</v>
       </c>
-      <c r="E146" s="64">
+      <c r="E146" s="67">
         <v>1</v>
       </c>
-      <c r="F146" s="64"/>
-      <c r="G146" s="64" t="s">
+      <c r="F146" s="67"/>
+      <c r="G146" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H146" s="56" t="s">
@@ -14292,10 +14880,10 @@
       <c r="C147" s="31" t="s">
         <v>380</v>
       </c>
-      <c r="D147" s="62"/>
-      <c r="E147" s="64"/>
-      <c r="F147" s="64"/>
-      <c r="G147" s="64"/>
+      <c r="D147" s="68"/>
+      <c r="E147" s="67"/>
+      <c r="F147" s="67"/>
+      <c r="G147" s="67"/>
       <c r="H147" s="56" t="s">
         <v>33</v>
       </c>
@@ -14305,10 +14893,10 @@
       <c r="C148" s="31" t="s">
         <v>386</v>
       </c>
-      <c r="D148" s="62"/>
-      <c r="E148" s="64"/>
-      <c r="F148" s="64"/>
-      <c r="G148" s="64"/>
+      <c r="D148" s="68"/>
+      <c r="E148" s="67"/>
+      <c r="F148" s="67"/>
+      <c r="G148" s="67"/>
       <c r="H148" s="56" t="s">
         <v>33</v>
       </c>
@@ -14317,14 +14905,14 @@
       <c r="C149" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="D149" s="62" t="s">
+      <c r="D149" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="E149" s="64">
+      <c r="E149" s="67">
         <v>4</v>
       </c>
-      <c r="F149" s="64"/>
-      <c r="G149" s="64" t="s">
+      <c r="F149" s="67"/>
+      <c r="G149" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H149" s="56" t="s">
@@ -14335,10 +14923,10 @@
       <c r="C150" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="D150" s="62"/>
-      <c r="E150" s="64"/>
-      <c r="F150" s="64"/>
-      <c r="G150" s="64"/>
+      <c r="D150" s="68"/>
+      <c r="E150" s="67"/>
+      <c r="F150" s="67"/>
+      <c r="G150" s="67"/>
       <c r="H150" s="56" t="s">
         <v>33</v>
       </c>
@@ -14347,19 +14935,19 @@
       <c r="C151" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="D151" s="62" t="s">
+      <c r="D151" s="68" t="s">
         <v>110</v>
       </c>
-      <c r="E151" s="64">
+      <c r="E151" s="67">
         <v>3</v>
       </c>
-      <c r="F151" s="64" t="s">
+      <c r="F151" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G151" s="64" t="s">
+      <c r="G151" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="H151" s="71" t="s">
+      <c r="H151" s="64" t="s">
         <v>750</v>
       </c>
     </row>
@@ -14367,36 +14955,36 @@
       <c r="C152" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="D152" s="62"/>
-      <c r="E152" s="64"/>
-      <c r="F152" s="64"/>
-      <c r="G152" s="64"/>
-      <c r="H152" s="71"/>
+      <c r="D152" s="68"/>
+      <c r="E152" s="67"/>
+      <c r="F152" s="67"/>
+      <c r="G152" s="67"/>
+      <c r="H152" s="64"/>
     </row>
     <row r="153" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C153" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="D153" s="62"/>
-      <c r="E153" s="64"/>
-      <c r="F153" s="64"/>
-      <c r="G153" s="64"/>
-      <c r="H153" s="71"/>
+      <c r="D153" s="68"/>
+      <c r="E153" s="67"/>
+      <c r="F153" s="67"/>
+      <c r="G153" s="67"/>
+      <c r="H153" s="64"/>
     </row>
     <row r="154" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C154" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="D154" s="62" t="s">
+      <c r="D154" s="68" t="s">
         <v>119</v>
       </c>
-      <c r="E154" s="64">
+      <c r="E154" s="67">
         <v>3</v>
       </c>
-      <c r="F154" s="64" t="s">
+      <c r="F154" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G154" s="64" t="s">
+      <c r="G154" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H154" s="56" t="s">
@@ -14407,10 +14995,10 @@
       <c r="C155" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="D155" s="62"/>
-      <c r="E155" s="64"/>
-      <c r="F155" s="64"/>
-      <c r="G155" s="64"/>
+      <c r="D155" s="68"/>
+      <c r="E155" s="67"/>
+      <c r="F155" s="67"/>
+      <c r="G155" s="67"/>
       <c r="H155" s="56" t="s">
         <v>33</v>
       </c>
@@ -14419,19 +15007,19 @@
       <c r="C156" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="D156" s="62" t="s">
+      <c r="D156" s="68" t="s">
         <v>124</v>
       </c>
-      <c r="E156" s="64">
+      <c r="E156" s="67">
         <v>3</v>
       </c>
-      <c r="F156" s="64" t="s">
+      <c r="F156" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G156" s="64" t="s">
+      <c r="G156" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="H156" s="71" t="s">
+      <c r="H156" s="64" t="s">
         <v>754</v>
       </c>
     </row>
@@ -14439,36 +15027,36 @@
       <c r="C157" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="D157" s="62"/>
-      <c r="E157" s="64"/>
-      <c r="F157" s="64"/>
-      <c r="G157" s="64"/>
-      <c r="H157" s="71"/>
+      <c r="D157" s="68"/>
+      <c r="E157" s="67"/>
+      <c r="F157" s="67"/>
+      <c r="G157" s="67"/>
+      <c r="H157" s="64"/>
     </row>
     <row r="158" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C158" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="D158" s="62"/>
-      <c r="E158" s="64"/>
-      <c r="F158" s="64"/>
-      <c r="G158" s="64"/>
-      <c r="H158" s="71"/>
+      <c r="D158" s="68"/>
+      <c r="E158" s="67"/>
+      <c r="F158" s="67"/>
+      <c r="G158" s="67"/>
+      <c r="H158" s="64"/>
     </row>
     <row r="159" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C159" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="D159" s="62" t="s">
+      <c r="D159" s="68" t="s">
         <v>131</v>
       </c>
-      <c r="E159" s="64">
+      <c r="E159" s="67">
         <v>3</v>
       </c>
-      <c r="F159" s="64" t="s">
+      <c r="F159" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G159" s="64" t="s">
+      <c r="G159" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H159" s="56" t="s">
@@ -14479,10 +15067,10 @@
       <c r="C160" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="D160" s="62"/>
-      <c r="E160" s="64"/>
-      <c r="F160" s="64"/>
-      <c r="G160" s="64"/>
+      <c r="D160" s="68"/>
+      <c r="E160" s="67"/>
+      <c r="F160" s="67"/>
+      <c r="G160" s="67"/>
       <c r="H160" s="56" t="s">
         <v>33</v>
       </c>
@@ -14491,10 +15079,10 @@
       <c r="C161" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="D161" s="62"/>
-      <c r="E161" s="64"/>
-      <c r="F161" s="64"/>
-      <c r="G161" s="64"/>
+      <c r="D161" s="68"/>
+      <c r="E161" s="67"/>
+      <c r="F161" s="67"/>
+      <c r="G161" s="67"/>
       <c r="H161" s="56" t="s">
         <v>33</v>
       </c>
@@ -14503,16 +15091,16 @@
       <c r="C162" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="D162" s="62" t="s">
+      <c r="D162" s="68" t="s">
         <v>159</v>
       </c>
-      <c r="E162" s="64">
+      <c r="E162" s="67">
         <v>5</v>
       </c>
-      <c r="F162" s="64">
+      <c r="F162" s="67">
         <v>5</v>
       </c>
-      <c r="G162" s="64" t="s">
+      <c r="G162" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H162" s="39" t="s">
@@ -14523,10 +15111,10 @@
       <c r="C163" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D163" s="62"/>
-      <c r="E163" s="64"/>
-      <c r="F163" s="64"/>
-      <c r="G163" s="64"/>
+      <c r="D163" s="68"/>
+      <c r="E163" s="67"/>
+      <c r="F163" s="67"/>
+      <c r="G163" s="67"/>
       <c r="H163" s="56" t="s">
         <v>33</v>
       </c>
@@ -14535,16 +15123,16 @@
       <c r="C164" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="D164" s="62" t="s">
+      <c r="D164" s="68" t="s">
         <v>164</v>
       </c>
-      <c r="E164" s="64">
+      <c r="E164" s="67">
         <v>5</v>
       </c>
-      <c r="F164" s="64">
+      <c r="F164" s="67">
         <v>5</v>
       </c>
-      <c r="G164" s="64" t="s">
+      <c r="G164" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H164" s="56" t="s">
@@ -14555,10 +15143,10 @@
       <c r="C165" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="D165" s="62"/>
-      <c r="E165" s="64"/>
-      <c r="F165" s="64"/>
-      <c r="G165" s="64"/>
+      <c r="D165" s="68"/>
+      <c r="E165" s="67"/>
+      <c r="F165" s="67"/>
+      <c r="G165" s="67"/>
       <c r="H165" s="56" t="s">
         <v>33</v>
       </c>
@@ -14567,10 +15155,10 @@
       <c r="C166" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="D166" s="62"/>
-      <c r="E166" s="64"/>
-      <c r="F166" s="64"/>
-      <c r="G166" s="64"/>
+      <c r="D166" s="68"/>
+      <c r="E166" s="67"/>
+      <c r="F166" s="67"/>
+      <c r="G166" s="67"/>
       <c r="H166" s="56" t="s">
         <v>33</v>
       </c>
@@ -14579,16 +15167,16 @@
       <c r="C167" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="D167" s="62" t="s">
+      <c r="D167" s="68" t="s">
         <v>179</v>
       </c>
-      <c r="E167" s="64">
+      <c r="E167" s="67">
         <v>5</v>
       </c>
-      <c r="F167" s="64">
+      <c r="F167" s="67">
         <v>5</v>
       </c>
-      <c r="G167" s="64" t="s">
+      <c r="G167" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H167" s="56" t="s">
@@ -14599,10 +15187,10 @@
       <c r="C168" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="D168" s="62"/>
-      <c r="E168" s="64"/>
-      <c r="F168" s="64"/>
-      <c r="G168" s="64"/>
+      <c r="D168" s="68"/>
+      <c r="E168" s="67"/>
+      <c r="F168" s="67"/>
+      <c r="G168" s="67"/>
       <c r="H168" s="56" t="s">
         <v>33</v>
       </c>
@@ -14611,10 +15199,10 @@
       <c r="C169" s="31" t="s">
         <v>183</v>
       </c>
-      <c r="D169" s="62"/>
-      <c r="E169" s="64"/>
-      <c r="F169" s="64"/>
-      <c r="G169" s="64"/>
+      <c r="D169" s="68"/>
+      <c r="E169" s="67"/>
+      <c r="F169" s="67"/>
+      <c r="G169" s="67"/>
       <c r="H169" s="56" t="s">
         <v>33</v>
       </c>
@@ -14623,16 +15211,16 @@
       <c r="C170" s="31" t="s">
         <v>185</v>
       </c>
-      <c r="D170" s="62" t="s">
+      <c r="D170" s="68" t="s">
         <v>186</v>
       </c>
-      <c r="E170" s="64">
+      <c r="E170" s="67">
         <v>5</v>
       </c>
-      <c r="F170" s="64">
+      <c r="F170" s="67">
         <v>5</v>
       </c>
-      <c r="G170" s="64" t="s">
+      <c r="G170" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H170" s="56" t="s">
@@ -14643,10 +15231,10 @@
       <c r="C171" s="31" t="s">
         <v>188</v>
       </c>
-      <c r="D171" s="62"/>
-      <c r="E171" s="64"/>
-      <c r="F171" s="64"/>
-      <c r="G171" s="64"/>
+      <c r="D171" s="68"/>
+      <c r="E171" s="67"/>
+      <c r="F171" s="67"/>
+      <c r="G171" s="67"/>
       <c r="H171" s="56" t="s">
         <v>33</v>
       </c>
@@ -14655,16 +15243,16 @@
       <c r="C172" s="31" t="s">
         <v>194</v>
       </c>
-      <c r="D172" s="62" t="s">
+      <c r="D172" s="68" t="s">
         <v>195</v>
       </c>
-      <c r="E172" s="64">
+      <c r="E172" s="67">
         <v>5</v>
       </c>
-      <c r="F172" s="64">
+      <c r="F172" s="67">
         <v>5</v>
       </c>
-      <c r="G172" s="64" t="s">
+      <c r="G172" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H172" s="56" t="s">
@@ -14675,10 +15263,10 @@
       <c r="C173" s="31" t="s">
         <v>197</v>
       </c>
-      <c r="D173" s="62"/>
-      <c r="E173" s="64"/>
-      <c r="F173" s="64"/>
-      <c r="G173" s="64"/>
+      <c r="D173" s="68"/>
+      <c r="E173" s="67"/>
+      <c r="F173" s="67"/>
+      <c r="G173" s="67"/>
       <c r="H173" s="56" t="s">
         <v>33</v>
       </c>
@@ -14687,16 +15275,16 @@
       <c r="C174" s="31" t="s">
         <v>199</v>
       </c>
-      <c r="D174" s="62" t="s">
+      <c r="D174" s="68" t="s">
         <v>200</v>
       </c>
-      <c r="E174" s="64">
+      <c r="E174" s="67">
         <v>5</v>
       </c>
-      <c r="F174" s="64">
+      <c r="F174" s="67">
         <v>5</v>
       </c>
-      <c r="G174" s="64" t="s">
+      <c r="G174" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H174" s="56" t="s">
@@ -14707,10 +15295,10 @@
       <c r="C175" s="31" t="s">
         <v>202</v>
       </c>
-      <c r="D175" s="62"/>
-      <c r="E175" s="64"/>
-      <c r="F175" s="64"/>
-      <c r="G175" s="64"/>
+      <c r="D175" s="68"/>
+      <c r="E175" s="67"/>
+      <c r="F175" s="67"/>
+      <c r="G175" s="67"/>
       <c r="H175" s="56" t="s">
         <v>33</v>
       </c>
@@ -14719,16 +15307,16 @@
       <c r="C176" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="D176" s="62" t="s">
+      <c r="D176" s="68" t="s">
         <v>211</v>
       </c>
-      <c r="E176" s="64">
+      <c r="E176" s="67">
         <v>5</v>
       </c>
-      <c r="F176" s="64">
+      <c r="F176" s="67">
         <v>5</v>
       </c>
-      <c r="G176" s="64" t="s">
+      <c r="G176" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H176" s="56" t="s">
@@ -14739,10 +15327,10 @@
       <c r="C177" s="31" t="s">
         <v>213</v>
       </c>
-      <c r="D177" s="62"/>
-      <c r="E177" s="64"/>
-      <c r="F177" s="64"/>
-      <c r="G177" s="64"/>
+      <c r="D177" s="68"/>
+      <c r="E177" s="67"/>
+      <c r="F177" s="67"/>
+      <c r="G177" s="67"/>
       <c r="H177" s="56" t="s">
         <v>33</v>
       </c>
@@ -14751,10 +15339,10 @@
       <c r="C178" s="31" t="s">
         <v>215</v>
       </c>
-      <c r="D178" s="62"/>
-      <c r="E178" s="64"/>
-      <c r="F178" s="64"/>
-      <c r="G178" s="64"/>
+      <c r="D178" s="68"/>
+      <c r="E178" s="67"/>
+      <c r="F178" s="67"/>
+      <c r="G178" s="67"/>
       <c r="H178" s="56" t="s">
         <v>33</v>
       </c>
@@ -14763,16 +15351,16 @@
       <c r="C179" s="31" t="s">
         <v>222</v>
       </c>
-      <c r="D179" s="62" t="s">
+      <c r="D179" s="68" t="s">
         <v>223</v>
       </c>
-      <c r="E179" s="64">
+      <c r="E179" s="67">
         <v>5</v>
       </c>
-      <c r="F179" s="64">
+      <c r="F179" s="67">
         <v>5</v>
       </c>
-      <c r="G179" s="64" t="s">
+      <c r="G179" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H179" s="56" t="s">
@@ -14783,10 +15371,10 @@
       <c r="C180" s="31" t="s">
         <v>225</v>
       </c>
-      <c r="D180" s="62"/>
-      <c r="E180" s="64"/>
-      <c r="F180" s="64"/>
-      <c r="G180" s="64"/>
+      <c r="D180" s="68"/>
+      <c r="E180" s="67"/>
+      <c r="F180" s="67"/>
+      <c r="G180" s="67"/>
       <c r="H180" s="56" t="s">
         <v>33</v>
       </c>
@@ -14795,16 +15383,16 @@
       <c r="C181" s="31" t="s">
         <v>227</v>
       </c>
-      <c r="D181" s="62" t="s">
+      <c r="D181" s="68" t="s">
         <v>228</v>
       </c>
-      <c r="E181" s="64">
+      <c r="E181" s="67">
         <v>5</v>
       </c>
-      <c r="F181" s="64">
+      <c r="F181" s="67">
         <v>5</v>
       </c>
-      <c r="G181" s="64" t="s">
+      <c r="G181" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H181" s="56" t="s">
@@ -14815,10 +15403,10 @@
       <c r="C182" s="31" t="s">
         <v>230</v>
       </c>
-      <c r="D182" s="62"/>
-      <c r="E182" s="64"/>
-      <c r="F182" s="64"/>
-      <c r="G182" s="64"/>
+      <c r="D182" s="68"/>
+      <c r="E182" s="67"/>
+      <c r="F182" s="67"/>
+      <c r="G182" s="67"/>
       <c r="H182" s="56" t="s">
         <v>33</v>
       </c>
@@ -14827,10 +15415,10 @@
       <c r="C183" s="31" t="s">
         <v>232</v>
       </c>
-      <c r="D183" s="62"/>
-      <c r="E183" s="64"/>
-      <c r="F183" s="64"/>
-      <c r="G183" s="64"/>
+      <c r="D183" s="68"/>
+      <c r="E183" s="67"/>
+      <c r="F183" s="67"/>
+      <c r="G183" s="67"/>
       <c r="H183" s="56" t="s">
         <v>33</v>
       </c>
@@ -14919,16 +15507,16 @@
       <c r="C188" s="31" t="s">
         <v>454</v>
       </c>
-      <c r="D188" s="62" t="s">
+      <c r="D188" s="68" t="s">
         <v>581</v>
       </c>
-      <c r="E188" s="64">
+      <c r="E188" s="67">
         <v>3</v>
       </c>
-      <c r="F188" s="64" t="s">
+      <c r="F188" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G188" s="64" t="s">
+      <c r="G188" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H188" s="56" t="s">
@@ -14939,10 +15527,10 @@
       <c r="C189" s="31" t="s">
         <v>457</v>
       </c>
-      <c r="D189" s="62"/>
-      <c r="E189" s="64"/>
-      <c r="F189" s="64"/>
-      <c r="G189" s="64"/>
+      <c r="D189" s="68"/>
+      <c r="E189" s="67"/>
+      <c r="F189" s="67"/>
+      <c r="G189" s="67"/>
       <c r="H189" s="56" t="s">
         <v>33</v>
       </c>
@@ -14951,16 +15539,16 @@
       <c r="C190" s="31" t="s">
         <v>459</v>
       </c>
-      <c r="D190" s="62" t="s">
+      <c r="D190" s="68" t="s">
         <v>460</v>
       </c>
-      <c r="E190" s="64">
+      <c r="E190" s="67">
         <v>3</v>
       </c>
-      <c r="F190" s="64" t="s">
+      <c r="F190" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G190" s="64" t="s">
+      <c r="G190" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H190" s="56" t="s">
@@ -14971,10 +15559,10 @@
       <c r="C191" s="31" t="s">
         <v>462</v>
       </c>
-      <c r="D191" s="62"/>
-      <c r="E191" s="64"/>
-      <c r="F191" s="64"/>
-      <c r="G191" s="64"/>
+      <c r="D191" s="68"/>
+      <c r="E191" s="67"/>
+      <c r="F191" s="67"/>
+      <c r="G191" s="67"/>
       <c r="H191" s="56" t="s">
         <v>33</v>
       </c>
@@ -15043,16 +15631,16 @@
       <c r="C195" s="31" t="s">
         <v>477</v>
       </c>
-      <c r="D195" s="62" t="s">
+      <c r="D195" s="68" t="s">
         <v>478</v>
       </c>
-      <c r="E195" s="64">
+      <c r="E195" s="67">
         <v>5</v>
       </c>
-      <c r="F195" s="64">
+      <c r="F195" s="67">
         <v>5</v>
       </c>
-      <c r="G195" s="64" t="s">
+      <c r="G195" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H195" s="56" t="s">
@@ -15064,10 +15652,10 @@
       <c r="C196" s="31" t="s">
         <v>480</v>
       </c>
-      <c r="D196" s="62"/>
-      <c r="E196" s="64"/>
-      <c r="F196" s="64"/>
-      <c r="G196" s="64"/>
+      <c r="D196" s="68"/>
+      <c r="E196" s="67"/>
+      <c r="F196" s="67"/>
+      <c r="G196" s="67"/>
       <c r="H196" s="56" t="s">
         <v>33</v>
       </c>
@@ -15077,12 +15665,12 @@
       <c r="C197" s="31" t="s">
         <v>464</v>
       </c>
-      <c r="D197" s="62" t="s">
+      <c r="D197" s="68" t="s">
         <v>749</v>
       </c>
-      <c r="E197" s="63"/>
-      <c r="F197" s="64"/>
-      <c r="G197" s="64" t="s">
+      <c r="E197" s="77"/>
+      <c r="F197" s="67"/>
+      <c r="G197" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H197" s="56"/>
@@ -15092,10 +15680,10 @@
       <c r="C198" t="s">
         <v>467</v>
       </c>
-      <c r="D198" s="62"/>
-      <c r="E198" s="63"/>
-      <c r="F198" s="64"/>
-      <c r="G198" s="64"/>
+      <c r="D198" s="68"/>
+      <c r="E198" s="77"/>
+      <c r="F198" s="67"/>
+      <c r="G198" s="67"/>
       <c r="H198" s="56"/>
     </row>
     <row r="199" spans="2:8" x14ac:dyDescent="0.25">
@@ -15103,12 +15691,12 @@
       <c r="C199" t="s">
         <v>495</v>
       </c>
-      <c r="D199" s="62" t="s">
+      <c r="D199" s="68" t="s">
         <v>748</v>
       </c>
-      <c r="E199" s="63"/>
-      <c r="F199" s="64"/>
-      <c r="G199" s="64" t="s">
+      <c r="E199" s="77"/>
+      <c r="F199" s="67"/>
+      <c r="G199" s="67" t="s">
         <v>18</v>
       </c>
       <c r="H199" s="56"/>
@@ -15118,10 +15706,10 @@
       <c r="C200" s="58" t="s">
         <v>498</v>
       </c>
-      <c r="D200" s="65"/>
-      <c r="E200" s="66"/>
-      <c r="F200" s="67"/>
-      <c r="G200" s="67"/>
+      <c r="D200" s="70"/>
+      <c r="E200" s="78"/>
+      <c r="F200" s="72"/>
+      <c r="G200" s="72"/>
       <c r="H200" s="57"/>
     </row>
     <row r="202" spans="2:8" x14ac:dyDescent="0.25">
@@ -15139,6 +15727,232 @@
   </sheetData>
   <autoFilter ref="A1:Q1" xr:uid="{20647E0C-146B-49B2-BC4C-D733C2BD2881}"/>
   <mergeCells count="250">
+    <mergeCell ref="D197:D198"/>
+    <mergeCell ref="E197:E198"/>
+    <mergeCell ref="F197:F198"/>
+    <mergeCell ref="G197:G198"/>
+    <mergeCell ref="D199:D200"/>
+    <mergeCell ref="E199:E200"/>
+    <mergeCell ref="F199:F200"/>
+    <mergeCell ref="G199:G200"/>
+    <mergeCell ref="E146:E148"/>
+    <mergeCell ref="E149:E150"/>
+    <mergeCell ref="E151:E153"/>
+    <mergeCell ref="E154:E155"/>
+    <mergeCell ref="E156:E158"/>
+    <mergeCell ref="E159:E161"/>
+    <mergeCell ref="E162:E163"/>
+    <mergeCell ref="E164:E166"/>
+    <mergeCell ref="E167:E169"/>
+    <mergeCell ref="D154:D155"/>
+    <mergeCell ref="F154:F155"/>
+    <mergeCell ref="G154:G155"/>
+    <mergeCell ref="D156:D158"/>
+    <mergeCell ref="F156:F158"/>
+    <mergeCell ref="G156:G158"/>
+    <mergeCell ref="D149:D150"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="E128:E129"/>
+    <mergeCell ref="E130:E131"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="E134:E135"/>
+    <mergeCell ref="E136:E137"/>
+    <mergeCell ref="E138:E139"/>
+    <mergeCell ref="E140:E142"/>
+    <mergeCell ref="E143:E145"/>
+    <mergeCell ref="D140:D142"/>
+    <mergeCell ref="F140:F142"/>
+    <mergeCell ref="G140:G142"/>
+    <mergeCell ref="D143:D145"/>
+    <mergeCell ref="F143:F145"/>
+    <mergeCell ref="G143:G145"/>
+    <mergeCell ref="F100:F102"/>
+    <mergeCell ref="F105:F106"/>
+    <mergeCell ref="G105:G106"/>
+    <mergeCell ref="F107:F108"/>
+    <mergeCell ref="G107:G108"/>
+    <mergeCell ref="F109:F110"/>
+    <mergeCell ref="G109:G110"/>
+    <mergeCell ref="F111:F112"/>
+    <mergeCell ref="G111:G112"/>
+    <mergeCell ref="D120:D123"/>
+    <mergeCell ref="D124:D125"/>
+    <mergeCell ref="D126:D127"/>
+    <mergeCell ref="D128:D129"/>
+    <mergeCell ref="D130:D131"/>
+    <mergeCell ref="D132:D133"/>
+    <mergeCell ref="D134:D135"/>
+    <mergeCell ref="G138:G139"/>
+    <mergeCell ref="F118:F119"/>
+    <mergeCell ref="G130:G131"/>
+    <mergeCell ref="G132:G133"/>
+    <mergeCell ref="G134:G135"/>
+    <mergeCell ref="F138:F139"/>
+    <mergeCell ref="G136:G137"/>
+    <mergeCell ref="D136:D137"/>
+    <mergeCell ref="D138:D139"/>
+    <mergeCell ref="D118:D119"/>
+    <mergeCell ref="F124:F125"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="F128:F129"/>
+    <mergeCell ref="F130:F131"/>
+    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="F134:F135"/>
+    <mergeCell ref="F136:F137"/>
+    <mergeCell ref="G118:G119"/>
+    <mergeCell ref="F120:F123"/>
+    <mergeCell ref="G120:G123"/>
+    <mergeCell ref="G124:G125"/>
+    <mergeCell ref="G126:G127"/>
+    <mergeCell ref="G128:G129"/>
+    <mergeCell ref="E118:E119"/>
+    <mergeCell ref="E120:E123"/>
+    <mergeCell ref="E124:E125"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="D45:D47"/>
+    <mergeCell ref="D100:D102"/>
+    <mergeCell ref="D105:D106"/>
+    <mergeCell ref="D107:D108"/>
+    <mergeCell ref="D113:D115"/>
+    <mergeCell ref="D116:D117"/>
+    <mergeCell ref="G113:G115"/>
+    <mergeCell ref="D109:D110"/>
+    <mergeCell ref="D111:D112"/>
+    <mergeCell ref="G100:G102"/>
+    <mergeCell ref="F116:F117"/>
+    <mergeCell ref="G116:G117"/>
+    <mergeCell ref="F113:F115"/>
+    <mergeCell ref="E100:E102"/>
+    <mergeCell ref="E103:E104"/>
+    <mergeCell ref="E105:E106"/>
+    <mergeCell ref="E107:E108"/>
+    <mergeCell ref="E109:E110"/>
+    <mergeCell ref="E111:E112"/>
+    <mergeCell ref="E113:E115"/>
+    <mergeCell ref="E116:E117"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="G39:G41"/>
+    <mergeCell ref="H39:H41"/>
+    <mergeCell ref="F42:F44"/>
+    <mergeCell ref="G42:G44"/>
+    <mergeCell ref="F45:F47"/>
+    <mergeCell ref="G45:G47"/>
+    <mergeCell ref="H42:H44"/>
+    <mergeCell ref="H45:H47"/>
+    <mergeCell ref="F149:F150"/>
+    <mergeCell ref="G149:G150"/>
+    <mergeCell ref="D151:D153"/>
+    <mergeCell ref="F151:F153"/>
+    <mergeCell ref="G151:G153"/>
+    <mergeCell ref="D164:D166"/>
+    <mergeCell ref="F164:F166"/>
+    <mergeCell ref="G164:G166"/>
+    <mergeCell ref="D167:D169"/>
+    <mergeCell ref="F167:F169"/>
+    <mergeCell ref="G167:G169"/>
+    <mergeCell ref="D159:D161"/>
+    <mergeCell ref="F159:F161"/>
+    <mergeCell ref="G159:G161"/>
+    <mergeCell ref="D162:D163"/>
+    <mergeCell ref="F162:F163"/>
+    <mergeCell ref="G162:G163"/>
+    <mergeCell ref="F174:F175"/>
+    <mergeCell ref="G174:G175"/>
+    <mergeCell ref="D176:D178"/>
+    <mergeCell ref="F176:F178"/>
+    <mergeCell ref="G176:G178"/>
+    <mergeCell ref="D170:D171"/>
+    <mergeCell ref="F170:F171"/>
+    <mergeCell ref="G170:G171"/>
+    <mergeCell ref="D172:D173"/>
+    <mergeCell ref="F172:F173"/>
+    <mergeCell ref="G172:G173"/>
+    <mergeCell ref="E170:E171"/>
+    <mergeCell ref="E172:E173"/>
+    <mergeCell ref="E174:E175"/>
+    <mergeCell ref="E176:E178"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="D195:D196"/>
+    <mergeCell ref="F195:F196"/>
+    <mergeCell ref="G195:G196"/>
+    <mergeCell ref="D179:D180"/>
+    <mergeCell ref="F179:F180"/>
+    <mergeCell ref="G179:G180"/>
+    <mergeCell ref="D181:D183"/>
+    <mergeCell ref="F181:F183"/>
+    <mergeCell ref="G181:G183"/>
+    <mergeCell ref="D188:D189"/>
+    <mergeCell ref="D190:D191"/>
+    <mergeCell ref="G188:G189"/>
+    <mergeCell ref="G190:G191"/>
+    <mergeCell ref="F188:F189"/>
+    <mergeCell ref="F190:F191"/>
+    <mergeCell ref="E179:E180"/>
+    <mergeCell ref="E181:E183"/>
+    <mergeCell ref="E188:E189"/>
+    <mergeCell ref="E190:E191"/>
+    <mergeCell ref="E195:E196"/>
+    <mergeCell ref="D174:D175"/>
     <mergeCell ref="H151:H153"/>
     <mergeCell ref="H156:H158"/>
     <mergeCell ref="H103:H104"/>
@@ -15163,232 +15977,6 @@
     <mergeCell ref="F33:F34"/>
     <mergeCell ref="G33:G34"/>
     <mergeCell ref="H33:H34"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="D195:D196"/>
-    <mergeCell ref="F195:F196"/>
-    <mergeCell ref="G195:G196"/>
-    <mergeCell ref="D179:D180"/>
-    <mergeCell ref="F179:F180"/>
-    <mergeCell ref="G179:G180"/>
-    <mergeCell ref="D181:D183"/>
-    <mergeCell ref="F181:F183"/>
-    <mergeCell ref="G181:G183"/>
-    <mergeCell ref="D188:D189"/>
-    <mergeCell ref="D190:D191"/>
-    <mergeCell ref="G188:G189"/>
-    <mergeCell ref="G190:G191"/>
-    <mergeCell ref="F188:F189"/>
-    <mergeCell ref="F190:F191"/>
-    <mergeCell ref="E179:E180"/>
-    <mergeCell ref="E181:E183"/>
-    <mergeCell ref="E188:E189"/>
-    <mergeCell ref="E190:E191"/>
-    <mergeCell ref="E195:E196"/>
-    <mergeCell ref="D174:D175"/>
-    <mergeCell ref="F174:F175"/>
-    <mergeCell ref="G174:G175"/>
-    <mergeCell ref="D176:D178"/>
-    <mergeCell ref="F176:F178"/>
-    <mergeCell ref="G176:G178"/>
-    <mergeCell ref="D170:D171"/>
-    <mergeCell ref="F170:F171"/>
-    <mergeCell ref="G170:G171"/>
-    <mergeCell ref="D172:D173"/>
-    <mergeCell ref="F172:F173"/>
-    <mergeCell ref="G172:G173"/>
-    <mergeCell ref="E170:E171"/>
-    <mergeCell ref="E172:E173"/>
-    <mergeCell ref="E174:E175"/>
-    <mergeCell ref="E176:E178"/>
-    <mergeCell ref="F149:F150"/>
-    <mergeCell ref="G149:G150"/>
-    <mergeCell ref="D151:D153"/>
-    <mergeCell ref="F151:F153"/>
-    <mergeCell ref="G151:G153"/>
-    <mergeCell ref="D164:D166"/>
-    <mergeCell ref="F164:F166"/>
-    <mergeCell ref="G164:G166"/>
-    <mergeCell ref="D167:D169"/>
-    <mergeCell ref="F167:F169"/>
-    <mergeCell ref="G167:G169"/>
-    <mergeCell ref="D159:D161"/>
-    <mergeCell ref="F159:F161"/>
-    <mergeCell ref="G159:G161"/>
-    <mergeCell ref="D162:D163"/>
-    <mergeCell ref="F162:F163"/>
-    <mergeCell ref="G162:G163"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="G39:G41"/>
-    <mergeCell ref="H39:H41"/>
-    <mergeCell ref="F42:F44"/>
-    <mergeCell ref="G42:G44"/>
-    <mergeCell ref="F45:F47"/>
-    <mergeCell ref="G45:G47"/>
-    <mergeCell ref="H42:H44"/>
-    <mergeCell ref="H45:H47"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="D45:D47"/>
-    <mergeCell ref="D100:D102"/>
-    <mergeCell ref="D105:D106"/>
-    <mergeCell ref="D107:D108"/>
-    <mergeCell ref="D113:D115"/>
-    <mergeCell ref="D116:D117"/>
-    <mergeCell ref="G113:G115"/>
-    <mergeCell ref="D109:D110"/>
-    <mergeCell ref="D111:D112"/>
-    <mergeCell ref="G100:G102"/>
-    <mergeCell ref="F116:F117"/>
-    <mergeCell ref="G116:G117"/>
-    <mergeCell ref="F113:F115"/>
-    <mergeCell ref="E100:E102"/>
-    <mergeCell ref="E103:E104"/>
-    <mergeCell ref="E105:E106"/>
-    <mergeCell ref="E107:E108"/>
-    <mergeCell ref="E109:E110"/>
-    <mergeCell ref="E111:E112"/>
-    <mergeCell ref="E113:E115"/>
-    <mergeCell ref="E116:E117"/>
-    <mergeCell ref="G130:G131"/>
-    <mergeCell ref="G132:G133"/>
-    <mergeCell ref="G134:G135"/>
-    <mergeCell ref="F138:F139"/>
-    <mergeCell ref="G136:G137"/>
-    <mergeCell ref="D136:D137"/>
-    <mergeCell ref="D138:D139"/>
-    <mergeCell ref="D118:D119"/>
-    <mergeCell ref="F124:F125"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="F128:F129"/>
-    <mergeCell ref="F130:F131"/>
-    <mergeCell ref="F132:F133"/>
-    <mergeCell ref="F134:F135"/>
-    <mergeCell ref="F136:F137"/>
-    <mergeCell ref="G118:G119"/>
-    <mergeCell ref="F120:F123"/>
-    <mergeCell ref="G120:G123"/>
-    <mergeCell ref="G124:G125"/>
-    <mergeCell ref="G126:G127"/>
-    <mergeCell ref="G128:G129"/>
-    <mergeCell ref="E118:E119"/>
-    <mergeCell ref="E120:E123"/>
-    <mergeCell ref="E124:E125"/>
-    <mergeCell ref="D140:D142"/>
-    <mergeCell ref="F140:F142"/>
-    <mergeCell ref="G140:G142"/>
-    <mergeCell ref="D143:D145"/>
-    <mergeCell ref="F143:F145"/>
-    <mergeCell ref="G143:G145"/>
-    <mergeCell ref="F100:F102"/>
-    <mergeCell ref="F105:F106"/>
-    <mergeCell ref="G105:G106"/>
-    <mergeCell ref="F107:F108"/>
-    <mergeCell ref="G107:G108"/>
-    <mergeCell ref="F109:F110"/>
-    <mergeCell ref="G109:G110"/>
-    <mergeCell ref="F111:F112"/>
-    <mergeCell ref="G111:G112"/>
-    <mergeCell ref="D120:D123"/>
-    <mergeCell ref="D124:D125"/>
-    <mergeCell ref="D126:D127"/>
-    <mergeCell ref="D128:D129"/>
-    <mergeCell ref="D130:D131"/>
-    <mergeCell ref="D132:D133"/>
-    <mergeCell ref="D134:D135"/>
-    <mergeCell ref="G138:G139"/>
-    <mergeCell ref="F118:F119"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="E128:E129"/>
-    <mergeCell ref="E130:E131"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="E134:E135"/>
-    <mergeCell ref="E136:E137"/>
-    <mergeCell ref="E138:E139"/>
-    <mergeCell ref="E140:E142"/>
-    <mergeCell ref="E143:E145"/>
-    <mergeCell ref="D197:D198"/>
-    <mergeCell ref="E197:E198"/>
-    <mergeCell ref="F197:F198"/>
-    <mergeCell ref="G197:G198"/>
-    <mergeCell ref="D199:D200"/>
-    <mergeCell ref="E199:E200"/>
-    <mergeCell ref="F199:F200"/>
-    <mergeCell ref="G199:G200"/>
-    <mergeCell ref="E146:E148"/>
-    <mergeCell ref="E149:E150"/>
-    <mergeCell ref="E151:E153"/>
-    <mergeCell ref="E154:E155"/>
-    <mergeCell ref="E156:E158"/>
-    <mergeCell ref="E159:E161"/>
-    <mergeCell ref="E162:E163"/>
-    <mergeCell ref="E164:E166"/>
-    <mergeCell ref="E167:E169"/>
-    <mergeCell ref="D154:D155"/>
-    <mergeCell ref="F154:F155"/>
-    <mergeCell ref="G154:G155"/>
-    <mergeCell ref="D156:D158"/>
-    <mergeCell ref="F156:F158"/>
-    <mergeCell ref="G156:G158"/>
-    <mergeCell ref="D149:D150"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -15396,6 +15984,256 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA6FC159-35F6-4366-8175-846334DBAE0D}">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="29" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="80" t="s">
+        <v>757</v>
+      </c>
+      <c r="B1" s="80" t="s">
+        <v>464</v>
+      </c>
+      <c r="C1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="79" t="s">
+        <v>758</v>
+      </c>
+      <c r="B2" s="79" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="79" t="s">
+        <v>759</v>
+      </c>
+      <c r="B3" s="79" t="s">
+        <v>759</v>
+      </c>
+      <c r="C3" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="79" t="s">
+        <v>760</v>
+      </c>
+      <c r="B4" s="79"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="79" t="s">
+        <v>761</v>
+      </c>
+      <c r="B5" s="79" t="s">
+        <v>761</v>
+      </c>
+      <c r="C5" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="79" t="s">
+        <v>762</v>
+      </c>
+      <c r="B6" s="79"/>
+      <c r="C6" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="79" t="s">
+        <v>763</v>
+      </c>
+      <c r="B7" s="79" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="79" t="s">
+        <v>764</v>
+      </c>
+      <c r="B8" s="79" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="79" t="s">
+        <v>765</v>
+      </c>
+      <c r="B9" s="79" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="79" t="s">
+        <v>766</v>
+      </c>
+      <c r="B10" s="79" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="79" t="s">
+        <v>767</v>
+      </c>
+      <c r="B11" s="79" t="s">
+        <v>767</v>
+      </c>
+      <c r="C11" s="79" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="79" t="s">
+        <v>768</v>
+      </c>
+      <c r="B12" s="79" t="s">
+        <v>768</v>
+      </c>
+      <c r="C12" s="79" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="79" t="s">
+        <v>769</v>
+      </c>
+      <c r="B13" s="79" t="s">
+        <v>769</v>
+      </c>
+      <c r="C13" s="79" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="79" t="s">
+        <v>770</v>
+      </c>
+      <c r="B14" s="79" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="79" t="s">
+        <v>771</v>
+      </c>
+      <c r="B15" s="79" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="79" t="s">
+        <v>772</v>
+      </c>
+      <c r="B16" s="79" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="79" t="s">
+        <v>773</v>
+      </c>
+      <c r="B17" s="79" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="79" t="s">
+        <v>774</v>
+      </c>
+      <c r="B18" s="79" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="79" t="s">
+        <v>598</v>
+      </c>
+      <c r="B19" s="79" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="79" t="s">
+        <v>775</v>
+      </c>
+      <c r="B20" s="79"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="79" t="s">
+        <v>776</v>
+      </c>
+      <c r="B21" s="79"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="79" t="s">
+        <v>777</v>
+      </c>
+      <c r="B22" s="79" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="79" t="s">
+        <v>778</v>
+      </c>
+      <c r="B23" s="79" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="79" t="s">
+        <v>505</v>
+      </c>
+      <c r="B24" s="79" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="79" t="s">
+        <v>779</v>
+      </c>
+      <c r="B25" s="79" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="79" t="s">
+        <v>781</v>
+      </c>
+      <c r="B26" s="79" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="79"/>
+      <c r="B27" s="79"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="79"/>
+      <c r="B28" s="79"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="79"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C5067C9-23D2-4ADE-8DCB-648ED12E8246}">
   <dimension ref="A2:D14"/>
   <sheetViews>
@@ -15559,7 +16397,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FEA6E34-2715-4365-861D-18E53AC7F8C2}">
   <dimension ref="A1:M10"/>
   <sheetViews>
@@ -15699,7 +16537,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71B37C7A-27BB-4B6C-AB7C-FA91261DBC1C}">
   <dimension ref="A1:D52"/>
   <sheetViews>
@@ -16299,7 +17137,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0658980E-FDBF-4B6D-A13D-5531F4808D66}">
   <dimension ref="A1:O54"/>
   <sheetViews>
@@ -17078,7 +17916,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA06BA7C-CD17-4C21-9F28-C604AE25C8B9}">
   <dimension ref="A1:F25"/>
   <sheetViews>
@@ -17129,7 +17967,7 @@
       <c r="D2" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="64">
+      <c r="E2" s="67">
         <v>101332</v>
       </c>
     </row>
@@ -17146,7 +17984,7 @@
       <c r="D3" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="64"/>
+      <c r="E3" s="67"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -17161,7 +17999,7 @@
       <c r="D4" t="s">
         <v>524</v>
       </c>
-      <c r="E4" s="64">
+      <c r="E4" s="67">
         <v>99343</v>
       </c>
     </row>
@@ -17178,7 +18016,7 @@
       <c r="D5" t="s">
         <v>524</v>
       </c>
-      <c r="E5" s="64"/>
+      <c r="E5" s="67"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -17193,7 +18031,7 @@
       <c r="D6" t="s">
         <v>516</v>
       </c>
-      <c r="E6" s="64">
+      <c r="E6" s="67">
         <v>102453</v>
       </c>
     </row>
@@ -17210,7 +18048,7 @@
       <c r="D7" t="s">
         <v>516</v>
       </c>
-      <c r="E7" s="64"/>
+      <c r="E7" s="67"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -17225,7 +18063,7 @@
       <c r="D8" t="s">
         <v>521</v>
       </c>
-      <c r="E8" s="64">
+      <c r="E8" s="67">
         <v>102447</v>
       </c>
     </row>
@@ -17242,7 +18080,7 @@
       <c r="D9" t="s">
         <v>521</v>
       </c>
-      <c r="E9" s="64"/>
+      <c r="E9" s="67"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -17257,7 +18095,7 @@
       <c r="D10" t="s">
         <v>521</v>
       </c>
-      <c r="E10" s="64"/>
+      <c r="E10" s="67"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -17272,7 +18110,7 @@
       <c r="D11" t="s">
         <v>521</v>
       </c>
-      <c r="E11" s="64"/>
+      <c r="E11" s="67"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -17287,7 +18125,7 @@
       <c r="D12" t="s">
         <v>512</v>
       </c>
-      <c r="E12" s="64">
+      <c r="E12" s="67">
         <v>101221</v>
       </c>
     </row>
@@ -17304,7 +18142,7 @@
       <c r="D13" t="s">
         <v>512</v>
       </c>
-      <c r="E13" s="64"/>
+      <c r="E13" s="67"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -17319,7 +18157,7 @@
       <c r="D14" t="s">
         <v>517</v>
       </c>
-      <c r="E14" s="64">
+      <c r="E14" s="67">
         <v>102455</v>
       </c>
     </row>
@@ -17336,7 +18174,7 @@
       <c r="D15" t="s">
         <v>517</v>
       </c>
-      <c r="E15" s="64"/>
+      <c r="E15" s="67"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -17351,7 +18189,7 @@
       <c r="D16" t="s">
         <v>508</v>
       </c>
-      <c r="E16" s="64">
+      <c r="E16" s="67">
         <v>1013824</v>
       </c>
     </row>
@@ -17368,7 +18206,7 @@
       <c r="D17" t="s">
         <v>508</v>
       </c>
-      <c r="E17" s="64"/>
+      <c r="E17" s="67"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -17383,7 +18221,7 @@
       <c r="D18" t="s">
         <v>510</v>
       </c>
-      <c r="E18" s="64">
+      <c r="E18" s="67">
         <v>102445</v>
       </c>
     </row>
@@ -17400,7 +18238,7 @@
       <c r="D19" t="s">
         <v>510</v>
       </c>
-      <c r="E19" s="64"/>
+      <c r="E19" s="67"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -17415,7 +18253,7 @@
       <c r="D20" t="s">
         <v>511</v>
       </c>
-      <c r="E20" s="64">
+      <c r="E20" s="67">
         <v>101557</v>
       </c>
     </row>
@@ -17432,7 +18270,7 @@
       <c r="D21" t="s">
         <v>511</v>
       </c>
-      <c r="E21" s="64"/>
+      <c r="E21" s="67"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -17447,7 +18285,7 @@
       <c r="D22" t="s">
         <v>509</v>
       </c>
-      <c r="E22" s="64">
+      <c r="E22" s="67">
         <v>101339</v>
       </c>
     </row>
@@ -17464,7 +18302,7 @@
       <c r="D23" t="s">
         <v>509</v>
       </c>
-      <c r="E23" s="64"/>
+      <c r="E23" s="67"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -17479,7 +18317,7 @@
       <c r="D24" t="s">
         <v>520</v>
       </c>
-      <c r="E24" s="64">
+      <c r="E24" s="67">
         <v>102391</v>
       </c>
     </row>
@@ -17496,7 +18334,7 @@
       <c r="D25" t="s">
         <v>520</v>
       </c>
-      <c r="E25" s="64"/>
+      <c r="E25" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -17517,514 +18355,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A026136A-3463-4F46-9920-D2EEED3E1AFC}">
-  <dimension ref="A1:X17"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:W17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.85546875" customWidth="1"/>
-    <col min="4" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="66.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>565</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>365</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>366</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>514</v>
-      </c>
-      <c r="D2" s="16">
-        <v>101901</v>
-      </c>
-      <c r="E2" s="19"/>
-      <c r="I2" s="7" t="s">
-        <v>570</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>572</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>571</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>568</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>569</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>370</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>371</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>513</v>
-      </c>
-      <c r="D3" s="14">
-        <v>100167</v>
-      </c>
-      <c r="E3" s="20"/>
-      <c r="I3">
-        <v>5676</v>
-      </c>
-      <c r="J3" t="s">
-        <v>573</v>
-      </c>
-      <c r="K3">
-        <v>100167</v>
-      </c>
-      <c r="L3" t="s">
-        <v>576</v>
-      </c>
-      <c r="M3">
-        <v>4</v>
-      </c>
-      <c r="N3">
-        <v>5</v>
-      </c>
-      <c r="O3" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>373</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>374</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>522</v>
-      </c>
-      <c r="D4" s="16">
-        <v>102341</v>
-      </c>
-      <c r="E4" s="19"/>
-      <c r="I4">
-        <v>6830</v>
-      </c>
-      <c r="J4" t="s">
-        <v>574</v>
-      </c>
-      <c r="K4">
-        <v>101901</v>
-      </c>
-      <c r="L4" t="s">
-        <v>576</v>
-      </c>
-      <c r="M4">
-        <v>78</v>
-      </c>
-      <c r="N4">
-        <v>4</v>
-      </c>
-      <c r="O4" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>376</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>366</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>514</v>
-      </c>
-      <c r="D5" s="14">
-        <v>101901</v>
-      </c>
-      <c r="E5" s="20"/>
-      <c r="I5">
-        <v>7114</v>
-      </c>
-      <c r="J5" t="s">
-        <v>575</v>
-      </c>
-      <c r="K5">
-        <v>102341</v>
-      </c>
-      <c r="L5" t="s">
-        <v>576</v>
-      </c>
-      <c r="M5">
-        <v>19</v>
-      </c>
-      <c r="N5">
-        <v>2</v>
-      </c>
-      <c r="O5" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>378</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>371</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>513</v>
-      </c>
-      <c r="D6" s="16">
-        <v>100167</v>
-      </c>
-      <c r="E6" s="19"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>380</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>522</v>
-      </c>
-      <c r="D7" s="14">
-        <v>102341</v>
-      </c>
-      <c r="E7" s="20"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>382</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>366</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>514</v>
-      </c>
-      <c r="D8" s="16">
-        <v>101901</v>
-      </c>
-      <c r="E8" s="19"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>384</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>371</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>513</v>
-      </c>
-      <c r="D9" s="14">
-        <v>100167</v>
-      </c>
-      <c r="E9" s="20"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>386</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>374</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>522</v>
-      </c>
-      <c r="D10" s="16">
-        <v>102341</v>
-      </c>
-      <c r="E10" s="19"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B14" s="42"/>
-      <c r="C14" s="42">
-        <v>44358</v>
-      </c>
-      <c r="D14" t="s">
-        <v>585</v>
-      </c>
-      <c r="E14">
-        <v>102341</v>
-      </c>
-      <c r="F14">
-        <v>3628</v>
-      </c>
-      <c r="G14">
-        <v>19</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="J14">
-        <v>3</v>
-      </c>
-      <c r="K14">
-        <v>131</v>
-      </c>
-      <c r="L14">
-        <v>129</v>
-      </c>
-      <c r="M14">
-        <v>145</v>
-      </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
-      <c r="O14">
-        <v>75</v>
-      </c>
-      <c r="Q14">
-        <v>2021</v>
-      </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
-      <c r="T14" t="s">
-        <v>586</v>
-      </c>
-      <c r="U14">
-        <v>47.615000000000002</v>
-      </c>
-      <c r="V14">
-        <v>-5.5083000000000002</v>
-      </c>
-      <c r="W14">
-        <v>96304</v>
-      </c>
-      <c r="X14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B15" s="42"/>
-      <c r="C15" s="42">
-        <v>44358</v>
-      </c>
-      <c r="D15" t="s">
-        <v>585</v>
-      </c>
-      <c r="E15">
-        <v>102623</v>
-      </c>
-      <c r="F15">
-        <v>3372</v>
-      </c>
-      <c r="G15">
-        <v>19</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>3</v>
-      </c>
-      <c r="K15">
-        <v>131</v>
-      </c>
-      <c r="L15">
-        <v>129</v>
-      </c>
-      <c r="M15">
-        <v>145</v>
-      </c>
-      <c r="N15">
-        <v>1</v>
-      </c>
-      <c r="O15">
-        <v>75</v>
-      </c>
-      <c r="Q15">
-        <v>2021</v>
-      </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
-      <c r="T15" t="s">
-        <v>586</v>
-      </c>
-      <c r="U15">
-        <v>47.615000000000002</v>
-      </c>
-      <c r="V15">
-        <v>-5.5083000000000002</v>
-      </c>
-      <c r="W15">
-        <v>97931</v>
-      </c>
-      <c r="X15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B16" s="42">
-        <v>44385</v>
-      </c>
-      <c r="C16" t="s">
-        <v>585</v>
-      </c>
-      <c r="D16">
-        <v>102341</v>
-      </c>
-      <c r="E16">
-        <v>3628</v>
-      </c>
-      <c r="F16">
-        <v>19</v>
-      </c>
-      <c r="G16">
-        <v>41</v>
-      </c>
-      <c r="I16">
-        <v>3</v>
-      </c>
-      <c r="J16">
-        <v>448</v>
-      </c>
-      <c r="K16">
-        <v>444</v>
-      </c>
-      <c r="L16">
-        <v>181</v>
-      </c>
-      <c r="M16">
-        <v>1</v>
-      </c>
-      <c r="N16">
-        <v>59</v>
-      </c>
-      <c r="P16">
-        <v>2021</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="S16" t="s">
-        <v>587</v>
-      </c>
-      <c r="T16">
-        <v>55.76</v>
-      </c>
-      <c r="U16">
-        <v>-9.3633000000000006</v>
-      </c>
-      <c r="V16">
-        <v>96304</v>
-      </c>
-      <c r="W16">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B17" s="42">
-        <v>44385</v>
-      </c>
-      <c r="C17" t="s">
-        <v>585</v>
-      </c>
-      <c r="D17">
-        <v>102623</v>
-      </c>
-      <c r="E17">
-        <v>3372</v>
-      </c>
-      <c r="F17">
-        <v>19</v>
-      </c>
-      <c r="G17">
-        <v>41</v>
-      </c>
-      <c r="I17">
-        <v>3</v>
-      </c>
-      <c r="J17">
-        <v>448</v>
-      </c>
-      <c r="K17">
-        <v>444</v>
-      </c>
-      <c r="L17">
-        <v>181</v>
-      </c>
-      <c r="M17">
-        <v>1</v>
-      </c>
-      <c r="N17">
-        <v>59</v>
-      </c>
-      <c r="P17">
-        <v>2021</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="S17" t="s">
-        <v>587</v>
-      </c>
-      <c r="T17">
-        <v>55.76</v>
-      </c>
-      <c r="U17">
-        <v>-9.3633000000000006</v>
-      </c>
-      <c r="V17">
-        <v>97971</v>
-      </c>
-      <c r="W17">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEAE28352B96D64C95AA0D5E2FA62FAD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed183881d36ac1b5d7d67982eda510d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d161086-4829-409f-9f75-5bde88dcb151" xmlns:ns3="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="685f4fda20cf913d28bf77c13cd653dd" ns2:_="" ns3:_="">
     <xsd:import namespace="3d161086-4829-409f-9f75-5bde88dcb151"/>
@@ -18247,15 +18587,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -18268,6 +18599,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C74AB5E7-5C87-4FF7-BF80-AB0EB6BD1D32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18286,27 +18625,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2FFB1F-984F-402F-9296-7A081636DDF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>